<commit_message>
Adding to the list of tests
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="168">
   <si>
     <t>Test Number</t>
   </si>
@@ -490,6 +490,36 @@
   </si>
   <si>
     <t>Dashboard Perspective</t>
+  </si>
+  <si>
+    <t>Cannot create a synoptic with a name of greather than 40 characters</t>
+  </si>
+  <si>
+    <t>All synoptics can be loaded on a remote instrument (especially long ones)</t>
+  </si>
+  <si>
+    <t>All configs can be viewed via their config name PV from a remote system</t>
+  </si>
+  <si>
+    <t>A block can be created with run control</t>
+  </si>
+  <si>
+    <t>A block can be created with logging</t>
+  </si>
+  <si>
+    <t>Run control can be turned off for a block in the config</t>
+  </si>
+  <si>
+    <t>Logging can be turned off for a block</t>
+  </si>
+  <si>
+    <t>Run control can be reinstated for a block via the config editor</t>
+  </si>
+  <si>
+    <t>Logging can be reinstated for a block via the config editor</t>
+  </si>
+  <si>
+    <t>Verify that config changes are pushed to the repo</t>
   </si>
 </sst>
 </file>
@@ -936,9 +966,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H134"/>
+  <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1747,7 +1779,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
-        <f t="shared" ref="A66:A129" si="1">IF(ISNUMBER(A65),A65+1,1)</f>
+        <f t="shared" ref="A66:A139" si="1">IF(ISNUMBER(A65),A65+1,1)</f>
         <v>65</v>
       </c>
       <c r="D66" s="7" t="s">
@@ -2054,7 +2086,7 @@
         <v>97</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>111</v>
+        <v>161</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2066,10 +2098,10 @@
         <v>97</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -2078,7 +2110,7 @@
         <v>97</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2090,10 +2122,10 @@
         <v>97</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -2102,10 +2134,10 @@
         <v>97</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -2114,7 +2146,7 @@
         <v>97</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>116</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2126,7 +2158,7 @@
         <v>97</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2138,7 +2170,7 @@
         <v>97</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2150,7 +2182,7 @@
         <v>97</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2162,7 +2194,7 @@
         <v>97</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2174,31 +2206,31 @@
         <v>97</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2207,10 +2239,10 @@
         <v>103</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2219,10 +2251,10 @@
         <v>104</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2231,10 +2263,10 @@
         <v>105</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2243,73 +2275,73 @@
         <v>106</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -2318,10 +2350,10 @@
         <v>89</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -2330,10 +2362,10 @@
         <v>89</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -2342,10 +2374,10 @@
         <v>89</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -2354,127 +2386,127 @@
         <v>89</v>
       </c>
       <c r="E116" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="5">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E117" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="5">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119" s="5">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="D119" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A120" s="5">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="5">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A122" s="5">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="D122" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A123" s="5">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A124" s="5">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="D124" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E124" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="5">
-        <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
-      <c r="D117" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E117" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A118" s="5">
-        <f t="shared" si="1"/>
-        <v>117</v>
-      </c>
-      <c r="D118" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E118" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="5">
-        <f t="shared" si="1"/>
-        <v>118</v>
-      </c>
-      <c r="D119" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E119" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="5">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E120" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="5">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E121" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A122" s="5">
-        <f t="shared" si="1"/>
-        <v>121</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E122" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="5">
-        <f t="shared" si="1"/>
-        <v>122</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E123" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="5">
-        <f t="shared" si="1"/>
-        <v>123</v>
-      </c>
-      <c r="D124" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E124" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
       <c r="D126" s="7" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="E126" s="7" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2483,93 +2515,213 @@
         <v>126</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="D128" s="7" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="E128" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="E129" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
-        <f t="shared" ref="A130:A134" si="2">IF(ISNUMBER(A129),A129+1,1)</f>
+        <f t="shared" si="1"/>
         <v>129</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="D131" s="7" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="D132" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E132" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="5">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="D133" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E133" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="5">
+        <f t="shared" si="1"/>
+        <v>133</v>
+      </c>
+      <c r="D134" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E134" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="5">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+      <c r="D135" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E135" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="5">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
+      <c r="D136" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E136" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A137" s="5">
+        <f t="shared" si="1"/>
+        <v>136</v>
+      </c>
+      <c r="D137" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E137" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="5">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+      <c r="D138" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E138" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="5">
+        <f t="shared" si="1"/>
+        <v>138</v>
+      </c>
+      <c r="D139" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E139" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A140" s="5">
+        <f t="shared" ref="A140:A144" si="2">IF(ISNUMBER(A139),A139+1,1)</f>
+        <v>139</v>
+      </c>
+      <c r="D140" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E140" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A141" s="5">
         <f t="shared" si="2"/>
-        <v>131</v>
-      </c>
-      <c r="D132" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D141" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E132" s="7" t="s">
+      <c r="E141" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A142" s="5">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
+      <c r="D142" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E142" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A133" s="5">
+    <row r="143" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A143" s="5">
         <f t="shared" si="2"/>
-        <v>132</v>
-      </c>
-      <c r="D133" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D143" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E133" s="7" t="s">
+      <c r="E143" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A134" s="5">
+    <row r="144" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A144" s="5">
         <f t="shared" si="2"/>
-        <v>133</v>
-      </c>
-      <c r="D134" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D144" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E134" s="7" t="s">
+      <c r="E144" s="7" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ticket 1635: added a manual system test to verify default log settings for block
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="231">
   <si>
     <t>Test Number</t>
   </si>
@@ -704,6 +704,12 @@
   </si>
   <si>
     <t>Value returned as "*** diconnected ***"</t>
+  </si>
+  <si>
+    <t>15-30</t>
+  </si>
+  <si>
+    <t>Default log settings for block is enabled and 30 s rate</t>
   </si>
 </sst>
 </file>
@@ -862,14 +868,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1214,16 +1220,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1032"/>
+  <dimension ref="A1:N1033"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I77" sqref="I77"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" customWidth="1"/>
@@ -1238,10 +1244,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="57">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>222</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -3153,11 +3159,11 @@
         <v>10</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:B131" si="3">IF(A67=A66,B66+1,1)</f>
+        <f t="shared" ref="B67:B132" si="3">IF(A67=A66,B66+1,1)</f>
         <v>2</v>
       </c>
       <c r="C67" s="3" t="str">
-        <f t="shared" ref="C67:C131" si="4">CONCATENATE(A67,"-",B67)</f>
+        <f t="shared" ref="C67:C132" si="4">CONCATENATE(A67,"-",B67)</f>
         <v>10-2</v>
       </c>
       <c r="D67" s="5"/>
@@ -3177,7 +3183,7 @@
     </row>
     <row r="68" spans="1:13" ht="15">
       <c r="A68">
-        <f t="shared" ref="A68:A132" si="5">A67</f>
+        <f t="shared" ref="A68:A133" si="5">A67</f>
         <v>10</v>
       </c>
       <c r="B68">
@@ -4611,41 +4617,37 @@
       <c r="L118" s="8"/>
       <c r="M118" s="6"/>
     </row>
-    <row r="119" spans="1:13" ht="15">
+    <row r="119" spans="1:13" ht="30">
       <c r="A119">
-        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="B119">
-        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="C119" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>15-30</v>
-      </c>
-      <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="7"/>
-      <c r="G119" s="7"/>
-      <c r="H119" s="7" t="s">
+      <c r="C119" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D119" s="9"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+      <c r="H119" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="I119" s="1" t="s">
-        <v>141</v>
+      <c r="I119" s="8" t="s">
+        <v>230</v>
       </c>
       <c r="J119" s="8"/>
-      <c r="K119" s="7"/>
+      <c r="K119" s="9"/>
       <c r="L119" s="8"/>
       <c r="M119" s="6"/>
     </row>
-    <row r="120" spans="1:13" ht="30">
+    <row r="120" spans="1:13" ht="15">
       <c r="A120">
-        <f t="shared" si="5"/>
+        <f>A118</f>
         <v>15</v>
       </c>
       <c r="B120">
-        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="C120" s="3" t="str">
@@ -4660,14 +4662,14 @@
         <v>111</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J120" s="8"/>
       <c r="K120" s="7"/>
-      <c r="L120" s="1"/>
+      <c r="L120" s="8"/>
       <c r="M120" s="6"/>
     </row>
-    <row r="121" spans="1:13" ht="15">
+    <row r="121" spans="1:13" ht="30">
       <c r="A121">
         <f t="shared" si="5"/>
         <v>15</v>
@@ -4688,14 +4690,14 @@
         <v>111</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J121" s="8"/>
       <c r="K121" s="7"/>
-      <c r="L121" s="8"/>
+      <c r="L121" s="1"/>
       <c r="M121" s="6"/>
     </row>
-    <row r="122" spans="1:13" ht="30">
+    <row r="122" spans="1:13" ht="15">
       <c r="A122">
         <f t="shared" si="5"/>
         <v>15</v>
@@ -4716,7 +4718,7 @@
         <v>111</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J122" s="8"/>
       <c r="K122" s="7"/>
@@ -4744,14 +4746,14 @@
         <v>111</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J123" s="8"/>
       <c r="K123" s="7"/>
       <c r="L123" s="8"/>
       <c r="M123" s="6"/>
     </row>
-    <row r="124" spans="1:13" ht="15">
+    <row r="124" spans="1:13" ht="30">
       <c r="A124">
         <f t="shared" si="5"/>
         <v>15</v>
@@ -4772,7 +4774,7 @@
         <v>111</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J124" s="8"/>
       <c r="K124" s="7"/>
@@ -4800,7 +4802,7 @@
         <v>111</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J125" s="8"/>
       <c r="K125" s="7"/>
@@ -4828,7 +4830,7 @@
         <v>111</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J126" s="8"/>
       <c r="K126" s="7"/>
@@ -4856,7 +4858,7 @@
         <v>111</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J127" s="8"/>
       <c r="K127" s="7"/>
@@ -4884,7 +4886,7 @@
         <v>111</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J128" s="8"/>
       <c r="K128" s="7"/>
@@ -4912,7 +4914,7 @@
         <v>111</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J129" s="8"/>
       <c r="K129" s="7"/>
@@ -4940,7 +4942,7 @@
         <v>111</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J130" s="8"/>
       <c r="K130" s="7"/>
@@ -4968,7 +4970,7 @@
         <v>111</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J131" s="8"/>
       <c r="K131" s="7"/>
@@ -4981,11 +4983,11 @@
         <v>15</v>
       </c>
       <c r="B132">
-        <f t="shared" ref="B132:B195" si="8">IF(A132=A131,B131+1,1)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="C132" s="3" t="str">
-        <f t="shared" ref="C132:C195" si="9">CONCATENATE(A132,"-",B132)</f>
+        <f t="shared" si="4"/>
         <v>15-43</v>
       </c>
       <c r="D132" s="5"/>
@@ -4996,7 +4998,7 @@
         <v>111</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J132" s="8"/>
       <c r="K132" s="7"/>
@@ -5005,15 +5007,15 @@
     </row>
     <row r="133" spans="1:13" ht="15">
       <c r="A133">
-        <f t="shared" ref="A133:A196" si="10">A132</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="B133">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="B133:B196" si="8">IF(A133=A132,B132+1,1)</f>
         <v>44</v>
       </c>
       <c r="C133" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="C133:C196" si="9">CONCATENATE(A133,"-",B133)</f>
         <v>15-44</v>
       </c>
       <c r="D133" s="5"/>
@@ -5024,7 +5026,7 @@
         <v>111</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J133" s="8"/>
       <c r="K133" s="7"/>
@@ -5033,7 +5035,7 @@
     </row>
     <row r="134" spans="1:13" ht="15">
       <c r="A134">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="A134:A197" si="10">A133</f>
         <v>15</v>
       </c>
       <c r="B134">
@@ -5052,14 +5054,14 @@
         <v>111</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J134" s="8"/>
       <c r="K134" s="7"/>
       <c r="L134" s="8"/>
       <c r="M134" s="6"/>
     </row>
-    <row r="135" spans="1:13" ht="120">
+    <row r="135" spans="1:13" ht="15">
       <c r="A135">
         <f t="shared" si="10"/>
         <v>15</v>
@@ -5080,14 +5082,14 @@
         <v>111</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J135" s="8"/>
       <c r="K135" s="7"/>
-      <c r="L135" s="1"/>
+      <c r="L135" s="8"/>
       <c r="M135" s="6"/>
     </row>
-    <row r="136" spans="1:13" ht="30">
+    <row r="136" spans="1:13" ht="120">
       <c r="A136">
         <f t="shared" si="10"/>
         <v>15</v>
@@ -5108,14 +5110,14 @@
         <v>111</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J136" s="8"/>
-      <c r="K136" s="5"/>
-      <c r="L136" s="16"/>
+      <c r="K136" s="7"/>
+      <c r="L136" s="1"/>
       <c r="M136" s="6"/>
     </row>
-    <row r="137" spans="1:13" ht="45">
+    <row r="137" spans="1:13" ht="30">
       <c r="A137">
         <f t="shared" si="10"/>
         <v>15</v>
@@ -5133,17 +5135,17 @@
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
       <c r="H137" s="7" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J137" s="8"/>
-      <c r="K137" s="7"/>
-      <c r="L137" s="8"/>
+      <c r="K137" s="5"/>
+      <c r="L137" s="16"/>
       <c r="M137" s="6"/>
     </row>
-    <row r="138" spans="1:13" ht="30">
+    <row r="138" spans="1:13" ht="45">
       <c r="A138">
         <f t="shared" si="10"/>
         <v>15</v>
@@ -5164,14 +5166,14 @@
         <v>159</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J138" s="8"/>
       <c r="K138" s="7"/>
-      <c r="L138" s="1"/>
+      <c r="L138" s="8"/>
       <c r="M138" s="6"/>
     </row>
-    <row r="139" spans="1:13" ht="15">
+    <row r="139" spans="1:13" ht="30">
       <c r="A139">
         <f t="shared" si="10"/>
         <v>15</v>
@@ -5192,14 +5194,14 @@
         <v>159</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J139" s="8"/>
       <c r="K139" s="7"/>
-      <c r="L139" s="8"/>
+      <c r="L139" s="1"/>
       <c r="M139" s="6"/>
     </row>
-    <row r="140" spans="1:13" ht="30">
+    <row r="140" spans="1:13" ht="15">
       <c r="A140">
         <f t="shared" si="10"/>
         <v>15</v>
@@ -5220,36 +5222,35 @@
         <v>159</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J140" s="8"/>
       <c r="K140" s="7"/>
       <c r="L140" s="8"/>
       <c r="M140" s="6"/>
     </row>
-    <row r="141" spans="1:13" ht="15">
+    <row r="141" spans="1:13" ht="30">
       <c r="A141">
-        <v>16</v>
+        <f t="shared" si="10"/>
+        <v>15</v>
       </c>
       <c r="B141">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C141" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-1</v>
+        <v>15-52</v>
       </c>
       <c r="D141" s="5"/>
       <c r="E141" s="5"/>
-      <c r="F141" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="F141" s="7"/>
       <c r="G141" s="7"/>
       <c r="H141" s="7" t="s">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J141" s="8"/>
       <c r="K141" s="7"/>
@@ -5258,16 +5259,15 @@
     </row>
     <row r="142" spans="1:13" ht="15">
       <c r="A142">
-        <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="B142">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C142" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-2</v>
+        <v>16-1</v>
       </c>
       <c r="D142" s="5"/>
       <c r="E142" s="5"/>
@@ -5279,7 +5279,7 @@
         <v>100</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J142" s="8"/>
       <c r="K142" s="7"/>
@@ -5293,11 +5293,11 @@
       </c>
       <c r="B143">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C143" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-3</v>
+        <v>16-2</v>
       </c>
       <c r="D143" s="5"/>
       <c r="E143" s="5"/>
@@ -5309,11 +5309,12 @@
         <v>100</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J143" s="8"/>
       <c r="K143" s="7"/>
-      <c r="L143" s="11"/>
+      <c r="L143" s="8"/>
+      <c r="M143" s="6"/>
     </row>
     <row r="144" spans="1:13" ht="15">
       <c r="A144">
@@ -5322,11 +5323,11 @@
       </c>
       <c r="B144">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C144" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-4</v>
+        <v>16-3</v>
       </c>
       <c r="D144" s="5"/>
       <c r="E144" s="5"/>
@@ -5338,12 +5339,11 @@
         <v>100</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J144" s="8"/>
       <c r="K144" s="7"/>
-      <c r="L144" s="8"/>
-      <c r="M144" s="6"/>
+      <c r="L144" s="11"/>
     </row>
     <row r="145" spans="1:13" ht="15">
       <c r="A145">
@@ -5352,23 +5352,23 @@
       </c>
       <c r="B145">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C145" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-5</v>
+        <v>16-4</v>
       </c>
       <c r="D145" s="5"/>
       <c r="E145" s="5"/>
-      <c r="F145" s="7"/>
-      <c r="G145" s="7" t="s">
+      <c r="F145" s="7" t="s">
         <v>65</v>
       </c>
+      <c r="G145" s="7"/>
       <c r="H145" s="7" t="s">
         <v>100</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J145" s="8"/>
       <c r="K145" s="7"/>
@@ -5382,11 +5382,11 @@
       </c>
       <c r="B146">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C146" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-6</v>
+        <v>16-5</v>
       </c>
       <c r="D146" s="5"/>
       <c r="E146" s="5"/>
@@ -5398,7 +5398,7 @@
         <v>100</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J146" s="8"/>
       <c r="K146" s="7"/>
@@ -5412,11 +5412,11 @@
       </c>
       <c r="B147">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C147" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-7</v>
+        <v>16-6</v>
       </c>
       <c r="D147" s="5"/>
       <c r="E147" s="5"/>
@@ -5428,7 +5428,7 @@
         <v>100</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J147" s="8"/>
       <c r="K147" s="7"/>
@@ -5442,11 +5442,11 @@
       </c>
       <c r="B148">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C148" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-8</v>
+        <v>16-7</v>
       </c>
       <c r="D148" s="5"/>
       <c r="E148" s="5"/>
@@ -5458,24 +5458,25 @@
         <v>100</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J148" s="8"/>
       <c r="K148" s="7"/>
       <c r="L148" s="8"/>
-    </row>
-    <row r="149" spans="1:13" ht="30">
+      <c r="M148" s="6"/>
+    </row>
+    <row r="149" spans="1:13" ht="15">
       <c r="A149">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="B149">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C149" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-9</v>
+        <v>16-8</v>
       </c>
       <c r="D149" s="5"/>
       <c r="E149" s="5"/>
@@ -5487,25 +5488,24 @@
         <v>100</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J149" s="8"/>
       <c r="K149" s="7"/>
-      <c r="L149" s="1"/>
-      <c r="M149" s="6"/>
-    </row>
-    <row r="150" spans="1:13" ht="45">
+      <c r="L149" s="8"/>
+    </row>
+    <row r="150" spans="1:13" ht="30">
       <c r="A150">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="B150">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C150" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-10</v>
+        <v>16-9</v>
       </c>
       <c r="D150" s="5"/>
       <c r="E150" s="5"/>
@@ -5517,25 +5517,25 @@
         <v>100</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J150" s="8"/>
       <c r="K150" s="7"/>
-      <c r="L150" s="8"/>
+      <c r="L150" s="1"/>
       <c r="M150" s="6"/>
     </row>
-    <row r="151" spans="1:13" ht="30">
+    <row r="151" spans="1:13" ht="45">
       <c r="A151">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="B151">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C151" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-11</v>
+        <v>16-10</v>
       </c>
       <c r="D151" s="5"/>
       <c r="E151" s="5"/>
@@ -5547,25 +5547,25 @@
         <v>100</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J151" s="8"/>
       <c r="K151" s="7"/>
       <c r="L151" s="8"/>
       <c r="M151" s="6"/>
     </row>
-    <row r="152" spans="1:13" ht="45">
+    <row r="152" spans="1:13" ht="30">
       <c r="A152">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="B152">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C152" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-12</v>
+        <v>16-11</v>
       </c>
       <c r="D152" s="5"/>
       <c r="E152" s="5"/>
@@ -5577,7 +5577,7 @@
         <v>100</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J152" s="8"/>
       <c r="K152" s="7"/>
@@ -5591,11 +5591,11 @@
       </c>
       <c r="B153">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C153" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-13</v>
+        <v>16-12</v>
       </c>
       <c r="D153" s="5"/>
       <c r="E153" s="5"/>
@@ -5607,25 +5607,25 @@
         <v>100</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J153" s="8"/>
       <c r="K153" s="7"/>
       <c r="L153" s="8"/>
       <c r="M153" s="6"/>
     </row>
-    <row r="154" spans="1:13" ht="60">
+    <row r="154" spans="1:13" ht="45">
       <c r="A154">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="B154">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C154" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-14</v>
+        <v>16-13</v>
       </c>
       <c r="D154" s="5"/>
       <c r="E154" s="5"/>
@@ -5637,25 +5637,25 @@
         <v>100</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J154" s="8"/>
       <c r="K154" s="7"/>
       <c r="L154" s="8"/>
       <c r="M154" s="6"/>
     </row>
-    <row r="155" spans="1:13" ht="15">
+    <row r="155" spans="1:13" ht="60">
       <c r="A155">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="B155">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C155" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-15</v>
+        <v>16-14</v>
       </c>
       <c r="D155" s="5"/>
       <c r="E155" s="5"/>
@@ -5667,7 +5667,7 @@
         <v>100</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J155" s="8"/>
       <c r="K155" s="7"/>
@@ -5681,11 +5681,11 @@
       </c>
       <c r="B156">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C156" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-16</v>
+        <v>16-15</v>
       </c>
       <c r="D156" s="5"/>
       <c r="E156" s="5"/>
@@ -5697,41 +5697,41 @@
         <v>100</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J156" s="8"/>
       <c r="K156" s="7"/>
       <c r="L156" s="8"/>
       <c r="M156" s="6"/>
     </row>
-    <row r="157" spans="1:13" ht="30">
+    <row r="157" spans="1:13" ht="15">
       <c r="A157">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="B157">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C157" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-17</v>
+        <v>16-16</v>
       </c>
       <c r="D157" s="5"/>
       <c r="E157" s="5"/>
-      <c r="F157" s="7" t="s">
+      <c r="F157" s="7"/>
+      <c r="G157" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G157" s="7"/>
       <c r="H157" s="7" t="s">
         <v>100</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J157" s="8"/>
       <c r="K157" s="7"/>
-      <c r="L157" s="1"/>
+      <c r="L157" s="8"/>
       <c r="M157" s="6"/>
     </row>
     <row r="158" spans="1:13" ht="30">
@@ -5741,27 +5741,27 @@
       </c>
       <c r="B158">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C158" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-18</v>
+        <v>16-17</v>
       </c>
       <c r="D158" s="5"/>
       <c r="E158" s="5"/>
-      <c r="F158" s="7"/>
-      <c r="G158" s="7" t="s">
-        <v>181</v>
-      </c>
+      <c r="F158" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G158" s="7"/>
       <c r="H158" s="7" t="s">
         <v>100</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J158" s="8"/>
       <c r="K158" s="7"/>
-      <c r="L158" s="8"/>
+      <c r="L158" s="1"/>
       <c r="M158" s="6"/>
     </row>
     <row r="159" spans="1:13" ht="30">
@@ -5771,23 +5771,23 @@
       </c>
       <c r="B159">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C159" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-19</v>
+        <v>16-18</v>
       </c>
       <c r="D159" s="5"/>
       <c r="E159" s="5"/>
       <c r="F159" s="7"/>
       <c r="G159" s="7" t="s">
-        <v>65</v>
+        <v>181</v>
       </c>
       <c r="H159" s="7" t="s">
-        <v>183</v>
+        <v>100</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J159" s="8"/>
       <c r="K159" s="7"/>
@@ -5801,11 +5801,11 @@
       </c>
       <c r="B160">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C160" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-20</v>
+        <v>16-19</v>
       </c>
       <c r="D160" s="5"/>
       <c r="E160" s="5"/>
@@ -5817,25 +5817,25 @@
         <v>183</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J160" s="8"/>
       <c r="K160" s="7"/>
       <c r="L160" s="8"/>
       <c r="M160" s="6"/>
     </row>
-    <row r="161" spans="1:13" ht="15">
+    <row r="161" spans="1:13" ht="30">
       <c r="A161">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="B161">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C161" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-21</v>
+        <v>16-20</v>
       </c>
       <c r="D161" s="5"/>
       <c r="E161" s="5"/>
@@ -5847,7 +5847,7 @@
         <v>183</v>
       </c>
       <c r="I161" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J161" s="8"/>
       <c r="K161" s="7"/>
@@ -5861,11 +5861,11 @@
       </c>
       <c r="B162">
         <f t="shared" si="8"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C162" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>16-22</v>
+        <v>16-21</v>
       </c>
       <c r="D162" s="5"/>
       <c r="E162" s="5"/>
@@ -5877,7 +5877,7 @@
         <v>183</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J162" s="8"/>
       <c r="K162" s="7"/>
@@ -5886,15 +5886,16 @@
     </row>
     <row r="163" spans="1:13" ht="15">
       <c r="A163">
-        <v>17</v>
+        <f t="shared" si="10"/>
+        <v>16</v>
       </c>
       <c r="B163">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C163" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>17-1</v>
+        <v>16-22</v>
       </c>
       <c r="D163" s="5"/>
       <c r="E163" s="5"/>
@@ -5903,27 +5904,27 @@
         <v>65</v>
       </c>
       <c r="H163" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J163" s="8"/>
       <c r="K163" s="7"/>
-      <c r="L163" s="11"/>
-    </row>
-    <row r="164" spans="1:13" ht="30">
+      <c r="L163" s="8"/>
+      <c r="M163" s="6"/>
+    </row>
+    <row r="164" spans="1:13" ht="15">
       <c r="A164">
-        <f t="shared" si="10"/>
         <v>17</v>
       </c>
       <c r="B164">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C164" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>17-2</v>
+        <v>17-1</v>
       </c>
       <c r="D164" s="5"/>
       <c r="E164" s="5"/>
@@ -5935,25 +5936,24 @@
         <v>188</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J164" s="8"/>
       <c r="K164" s="7"/>
-      <c r="L164" s="1"/>
-      <c r="M164" s="6"/>
-    </row>
-    <row r="165" spans="1:13" ht="15">
+      <c r="L164" s="11"/>
+    </row>
+    <row r="165" spans="1:13" ht="30">
       <c r="A165">
         <f t="shared" si="10"/>
         <v>17</v>
       </c>
       <c r="B165">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C165" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>17-3</v>
+        <v>17-2</v>
       </c>
       <c r="D165" s="5"/>
       <c r="E165" s="5"/>
@@ -5965,11 +5965,11 @@
         <v>188</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J165" s="8"/>
       <c r="K165" s="7"/>
-      <c r="L165" s="8"/>
+      <c r="L165" s="1"/>
       <c r="M165" s="6"/>
     </row>
     <row r="166" spans="1:13" ht="15">
@@ -5979,11 +5979,11 @@
       </c>
       <c r="B166">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C166" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>17-4</v>
+        <v>17-3</v>
       </c>
       <c r="D166" s="5"/>
       <c r="E166" s="5"/>
@@ -5995,7 +5995,7 @@
         <v>188</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J166" s="8"/>
       <c r="K166" s="7"/>
@@ -6004,15 +6004,16 @@
     </row>
     <row r="167" spans="1:13" ht="15">
       <c r="A167">
-        <v>18</v>
+        <f t="shared" si="10"/>
+        <v>17</v>
       </c>
       <c r="B167">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C167" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>18-1</v>
+        <v>17-4</v>
       </c>
       <c r="D167" s="5"/>
       <c r="E167" s="5"/>
@@ -6021,27 +6022,27 @@
         <v>65</v>
       </c>
       <c r="H167" s="7" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J167" s="8"/>
       <c r="K167" s="7"/>
-      <c r="L167" s="11"/>
+      <c r="L167" s="8"/>
+      <c r="M167" s="6"/>
     </row>
     <row r="168" spans="1:13" ht="15">
       <c r="A168">
-        <f t="shared" si="10"/>
         <v>18</v>
       </c>
       <c r="B168">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C168" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>18-2</v>
+        <v>18-1</v>
       </c>
       <c r="D168" s="5"/>
       <c r="E168" s="5"/>
@@ -6053,12 +6054,11 @@
         <v>193</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J168" s="8"/>
       <c r="K168" s="7"/>
-      <c r="L168" s="8"/>
-      <c r="M168" s="6"/>
+      <c r="L168" s="11"/>
     </row>
     <row r="169" spans="1:13" ht="15">
       <c r="A169">
@@ -6067,11 +6067,11 @@
       </c>
       <c r="B169">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C169" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>18-3</v>
+        <v>18-2</v>
       </c>
       <c r="D169" s="5"/>
       <c r="E169" s="5"/>
@@ -6083,24 +6083,25 @@
         <v>193</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J169" s="8"/>
       <c r="K169" s="7"/>
       <c r="L169" s="8"/>
       <c r="M169" s="6"/>
     </row>
-    <row r="170" spans="1:13" ht="30">
+    <row r="170" spans="1:13" ht="15">
       <c r="A170">
-        <v>19</v>
+        <f t="shared" si="10"/>
+        <v>18</v>
       </c>
       <c r="B170">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C170" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>19-1</v>
+        <v>18-3</v>
       </c>
       <c r="D170" s="5"/>
       <c r="E170" s="5"/>
@@ -6109,10 +6110,10 @@
         <v>65</v>
       </c>
       <c r="H170" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J170" s="8"/>
       <c r="K170" s="7"/>
@@ -6121,16 +6122,15 @@
     </row>
     <row r="171" spans="1:13" ht="30">
       <c r="A171">
-        <f t="shared" si="10"/>
         <v>19</v>
       </c>
       <c r="B171">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C171" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>19-2</v>
+        <v>19-1</v>
       </c>
       <c r="D171" s="5"/>
       <c r="E171" s="5"/>
@@ -6142,11 +6142,12 @@
         <v>197</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J171" s="8"/>
       <c r="K171" s="7"/>
-      <c r="L171" s="17"/>
+      <c r="L171" s="8"/>
+      <c r="M171" s="6"/>
     </row>
     <row r="172" spans="1:13" ht="30">
       <c r="A172">
@@ -6155,11 +6156,11 @@
       </c>
       <c r="B172">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C172" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>19-3</v>
+        <v>19-2</v>
       </c>
       <c r="D172" s="5"/>
       <c r="E172" s="5"/>
@@ -6171,25 +6172,24 @@
         <v>197</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J172" s="8"/>
       <c r="K172" s="7"/>
       <c r="L172" s="18"/>
-      <c r="M172" s="6"/>
-    </row>
-    <row r="173" spans="1:13" ht="45">
+    </row>
+    <row r="173" spans="1:13" ht="30">
       <c r="A173">
         <f t="shared" si="10"/>
         <v>19</v>
       </c>
       <c r="B173">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C173" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>19-4</v>
+        <v>19-3</v>
       </c>
       <c r="D173" s="5"/>
       <c r="E173" s="5"/>
@@ -6201,25 +6201,25 @@
         <v>197</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J173" s="8"/>
       <c r="K173" s="7"/>
-      <c r="L173" s="18"/>
+      <c r="L173" s="19"/>
       <c r="M173" s="6"/>
     </row>
-    <row r="174" spans="1:13" ht="30">
+    <row r="174" spans="1:13" ht="45">
       <c r="A174">
         <f t="shared" si="10"/>
         <v>19</v>
       </c>
       <c r="B174">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C174" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>19-5</v>
+        <v>19-4</v>
       </c>
       <c r="D174" s="5"/>
       <c r="E174" s="5"/>
@@ -6231,7 +6231,7 @@
         <v>197</v>
       </c>
       <c r="I174" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J174" s="8"/>
       <c r="K174" s="7"/>
@@ -6240,45 +6240,45 @@
     </row>
     <row r="175" spans="1:13" ht="30">
       <c r="A175">
-        <v>20</v>
+        <f t="shared" si="10"/>
+        <v>19</v>
       </c>
       <c r="B175">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C175" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>20-1</v>
+        <v>19-5</v>
       </c>
       <c r="D175" s="5"/>
       <c r="E175" s="5"/>
       <c r="F175" s="7"/>
       <c r="G175" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H175" s="7" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="I175" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J175" s="8"/>
       <c r="K175" s="7"/>
-      <c r="L175" s="8"/>
+      <c r="L175" s="20"/>
       <c r="M175" s="6"/>
     </row>
-    <row r="176" spans="1:13" ht="45">
+    <row r="176" spans="1:13" ht="30">
       <c r="A176">
-        <f t="shared" si="10"/>
         <v>20</v>
       </c>
       <c r="B176">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C176" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>20-2</v>
+        <v>20-1</v>
       </c>
       <c r="D176" s="5"/>
       <c r="E176" s="5"/>
@@ -6290,84 +6290,84 @@
         <v>203</v>
       </c>
       <c r="I176" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J176" s="8"/>
       <c r="K176" s="7"/>
       <c r="L176" s="8"/>
       <c r="M176" s="6"/>
     </row>
-    <row r="177" spans="1:13" ht="26.25">
+    <row r="177" spans="1:13" ht="45">
       <c r="A177">
-        <v>21</v>
+        <f t="shared" si="10"/>
+        <v>20</v>
       </c>
       <c r="B177">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C177" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-1</v>
-      </c>
-      <c r="D177" s="15"/>
-      <c r="E177" s="15"/>
-      <c r="F177" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G177" s="15"/>
-      <c r="H177" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I177" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="J177" s="12"/>
-      <c r="K177" s="10"/>
-      <c r="L177" s="12"/>
+        <v>20-2</v>
+      </c>
+      <c r="D177" s="5"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="7"/>
+      <c r="G177" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H177" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="I177" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J177" s="8"/>
+      <c r="K177" s="7"/>
+      <c r="L177" s="8"/>
       <c r="M177" s="6"/>
     </row>
     <row r="178" spans="1:13" ht="26.25">
       <c r="A178">
-        <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="B178">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C178" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-2</v>
+        <v>21-1</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15"/>
-      <c r="F178" s="15"/>
-      <c r="G178" s="10" t="s">
+      <c r="F178" s="7" t="s">
         <v>65</v>
       </c>
+      <c r="G178" s="15"/>
       <c r="H178" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I178" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J178" s="12"/>
       <c r="K178" s="10"/>
       <c r="L178" s="12"/>
       <c r="M178" s="6"/>
     </row>
-    <row r="179" spans="1:13" ht="39">
+    <row r="179" spans="1:13" ht="26.25">
       <c r="A179">
         <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="B179">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C179" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-3</v>
+        <v>21-2</v>
       </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15"/>
@@ -6379,11 +6379,11 @@
         <v>15</v>
       </c>
       <c r="I179" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J179" s="12"/>
       <c r="K179" s="10"/>
-      <c r="L179" s="11"/>
+      <c r="L179" s="12"/>
       <c r="M179" s="6"/>
     </row>
     <row r="180" spans="1:13" ht="39">
@@ -6393,11 +6393,11 @@
       </c>
       <c r="B180">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C180" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-4</v>
+        <v>21-3</v>
       </c>
       <c r="D180" s="15"/>
       <c r="E180" s="15"/>
@@ -6408,26 +6408,26 @@
       <c r="H180" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I180" s="12" t="s">
-        <v>209</v>
+      <c r="I180" s="11" t="s">
+        <v>208</v>
       </c>
       <c r="J180" s="12"/>
       <c r="K180" s="10"/>
-      <c r="L180" s="12"/>
+      <c r="L180" s="11"/>
       <c r="M180" s="6"/>
     </row>
-    <row r="181" spans="1:13" ht="51.75">
+    <row r="181" spans="1:13" ht="39">
       <c r="A181">
         <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="B181">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C181" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-5</v>
+        <v>21-4</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15"/>
@@ -6439,25 +6439,25 @@
         <v>15</v>
       </c>
       <c r="I181" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J181" s="12"/>
       <c r="K181" s="10"/>
       <c r="L181" s="12"/>
       <c r="M181" s="6"/>
     </row>
-    <row r="182" spans="1:13" ht="26.25">
+    <row r="182" spans="1:13" ht="51.75">
       <c r="A182">
         <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="B182">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C182" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-6</v>
+        <v>21-5</v>
       </c>
       <c r="D182" s="15"/>
       <c r="E182" s="15"/>
@@ -6469,27 +6469,41 @@
         <v>15</v>
       </c>
       <c r="I182" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J182" s="12"/>
       <c r="K182" s="10"/>
       <c r="L182" s="12"/>
       <c r="M182" s="6"/>
     </row>
-    <row r="183" spans="1:13" ht="15">
+    <row r="183" spans="1:13" ht="26.25">
       <c r="A183">
         <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="B183">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C183" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-7</v>
-      </c>
-      <c r="L183" s="6"/>
+        <v>21-6</v>
+      </c>
+      <c r="D183" s="15"/>
+      <c r="E183" s="15"/>
+      <c r="F183" s="15"/>
+      <c r="G183" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H183" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I183" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="J183" s="12"/>
+      <c r="K183" s="10"/>
+      <c r="L183" s="12"/>
       <c r="M183" s="6"/>
     </row>
     <row r="184" spans="1:13" ht="15">
@@ -6499,11 +6513,11 @@
       </c>
       <c r="B184">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C184" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-8</v>
+        <v>21-7</v>
       </c>
       <c r="L184" s="6"/>
       <c r="M184" s="6"/>
@@ -6515,11 +6529,11 @@
       </c>
       <c r="B185">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C185" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-9</v>
+        <v>21-8</v>
       </c>
       <c r="L185" s="6"/>
       <c r="M185" s="6"/>
@@ -6531,11 +6545,11 @@
       </c>
       <c r="B186">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C186" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-10</v>
+        <v>21-9</v>
       </c>
       <c r="L186" s="6"/>
       <c r="M186" s="6"/>
@@ -6547,11 +6561,11 @@
       </c>
       <c r="B187">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C187" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-11</v>
+        <v>21-10</v>
       </c>
       <c r="L187" s="6"/>
       <c r="M187" s="6"/>
@@ -6563,11 +6577,11 @@
       </c>
       <c r="B188">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C188" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-12</v>
+        <v>21-11</v>
       </c>
       <c r="L188" s="6"/>
       <c r="M188" s="6"/>
@@ -6579,11 +6593,11 @@
       </c>
       <c r="B189">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C189" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-13</v>
+        <v>21-12</v>
       </c>
       <c r="L189" s="6"/>
       <c r="M189" s="6"/>
@@ -6595,11 +6609,11 @@
       </c>
       <c r="B190">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C190" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-14</v>
+        <v>21-13</v>
       </c>
       <c r="L190" s="6"/>
       <c r="M190" s="6"/>
@@ -6611,11 +6625,11 @@
       </c>
       <c r="B191">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C191" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-15</v>
+        <v>21-14</v>
       </c>
       <c r="L191" s="6"/>
       <c r="M191" s="6"/>
@@ -6627,11 +6641,11 @@
       </c>
       <c r="B192">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C192" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-16</v>
+        <v>21-15</v>
       </c>
       <c r="L192" s="6"/>
       <c r="M192" s="6"/>
@@ -6643,11 +6657,11 @@
       </c>
       <c r="B193">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C193" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-17</v>
+        <v>21-16</v>
       </c>
       <c r="L193" s="6"/>
       <c r="M193" s="6"/>
@@ -6659,11 +6673,11 @@
       </c>
       <c r="B194">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C194" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-18</v>
+        <v>21-17</v>
       </c>
       <c r="L194" s="6"/>
       <c r="M194" s="6"/>
@@ -6675,11 +6689,11 @@
       </c>
       <c r="B195">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C195" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>21-19</v>
+        <v>21-18</v>
       </c>
       <c r="L195" s="6"/>
       <c r="M195" s="6"/>
@@ -6690,44 +6704,44 @@
         <v>21</v>
       </c>
       <c r="B196">
-        <f t="shared" ref="B196:B259" si="11">IF(A196=A195,B195+1,1)</f>
-        <v>20</v>
+        <f t="shared" si="8"/>
+        <v>19</v>
       </c>
       <c r="C196" s="3" t="str">
-        <f t="shared" ref="C196:C259" si="12">CONCATENATE(A196,"-",B196)</f>
-        <v>21-20</v>
+        <f t="shared" si="9"/>
+        <v>21-19</v>
       </c>
       <c r="L196" s="6"/>
       <c r="M196" s="6"/>
     </row>
     <row r="197" spans="1:13" ht="15">
       <c r="A197">
-        <f t="shared" ref="A197:A260" si="13">A196</f>
+        <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="B197">
+        <f t="shared" ref="B197:B260" si="11">IF(A197=A196,B196+1,1)</f>
+        <v>20</v>
+      </c>
+      <c r="C197" s="3" t="str">
+        <f t="shared" ref="C197:C260" si="12">CONCATENATE(A197,"-",B197)</f>
+        <v>21-20</v>
+      </c>
+      <c r="L197" s="6"/>
+      <c r="M197" s="6"/>
+    </row>
+    <row r="198" spans="1:13" ht="15">
+      <c r="A198">
+        <f t="shared" ref="A198:A261" si="13">A197</f>
+        <v>21</v>
+      </c>
+      <c r="B198">
         <f t="shared" si="11"/>
         <v>21</v>
       </c>
-      <c r="C197" s="3" t="str">
+      <c r="C198" s="3" t="str">
         <f t="shared" si="12"/>
         <v>21-21</v>
-      </c>
-      <c r="L197" s="6"/>
-      <c r="M197" s="6"/>
-    </row>
-    <row r="198" spans="1:13" ht="15">
-      <c r="A198">
-        <f t="shared" si="13"/>
-        <v>21</v>
-      </c>
-      <c r="B198">
-        <f t="shared" si="11"/>
-        <v>22</v>
-      </c>
-      <c r="C198" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>21-22</v>
       </c>
       <c r="L198" s="6"/>
       <c r="M198" s="6"/>
@@ -6739,11 +6753,11 @@
       </c>
       <c r="B199">
         <f t="shared" si="11"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C199" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-23</v>
+        <v>21-22</v>
       </c>
       <c r="L199" s="6"/>
       <c r="M199" s="6"/>
@@ -6755,11 +6769,11 @@
       </c>
       <c r="B200">
         <f t="shared" si="11"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C200" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-24</v>
+        <v>21-23</v>
       </c>
       <c r="L200" s="6"/>
       <c r="M200" s="6"/>
@@ -6771,11 +6785,11 @@
       </c>
       <c r="B201">
         <f t="shared" si="11"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C201" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-25</v>
+        <v>21-24</v>
       </c>
       <c r="L201" s="6"/>
       <c r="M201" s="6"/>
@@ -6787,11 +6801,11 @@
       </c>
       <c r="B202">
         <f t="shared" si="11"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C202" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-26</v>
+        <v>21-25</v>
       </c>
       <c r="L202" s="6"/>
       <c r="M202" s="6"/>
@@ -6803,11 +6817,11 @@
       </c>
       <c r="B203">
         <f t="shared" si="11"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C203" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-27</v>
+        <v>21-26</v>
       </c>
       <c r="L203" s="6"/>
       <c r="M203" s="6"/>
@@ -6819,11 +6833,11 @@
       </c>
       <c r="B204">
         <f t="shared" si="11"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C204" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-28</v>
+        <v>21-27</v>
       </c>
       <c r="L204" s="6"/>
       <c r="M204" s="6"/>
@@ -6835,11 +6849,11 @@
       </c>
       <c r="B205">
         <f t="shared" si="11"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C205" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-29</v>
+        <v>21-28</v>
       </c>
       <c r="L205" s="6"/>
       <c r="M205" s="6"/>
@@ -6851,11 +6865,11 @@
       </c>
       <c r="B206">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C206" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-30</v>
+        <v>21-29</v>
       </c>
       <c r="L206" s="6"/>
       <c r="M206" s="6"/>
@@ -6867,11 +6881,11 @@
       </c>
       <c r="B207">
         <f t="shared" si="11"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C207" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-31</v>
+        <v>21-30</v>
       </c>
       <c r="L207" s="6"/>
       <c r="M207" s="6"/>
@@ -6883,11 +6897,11 @@
       </c>
       <c r="B208">
         <f t="shared" si="11"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C208" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-32</v>
+        <v>21-31</v>
       </c>
       <c r="L208" s="6"/>
       <c r="M208" s="6"/>
@@ -6899,11 +6913,11 @@
       </c>
       <c r="B209">
         <f t="shared" si="11"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C209" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-33</v>
+        <v>21-32</v>
       </c>
       <c r="L209" s="6"/>
       <c r="M209" s="6"/>
@@ -6915,11 +6929,11 @@
       </c>
       <c r="B210">
         <f t="shared" si="11"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C210" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-34</v>
+        <v>21-33</v>
       </c>
       <c r="L210" s="6"/>
       <c r="M210" s="6"/>
@@ -6931,11 +6945,11 @@
       </c>
       <c r="B211">
         <f t="shared" si="11"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C211" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-35</v>
+        <v>21-34</v>
       </c>
       <c r="L211" s="6"/>
       <c r="M211" s="6"/>
@@ -6947,11 +6961,11 @@
       </c>
       <c r="B212">
         <f t="shared" si="11"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C212" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-36</v>
+        <v>21-35</v>
       </c>
       <c r="L212" s="6"/>
       <c r="M212" s="6"/>
@@ -6963,11 +6977,11 @@
       </c>
       <c r="B213">
         <f t="shared" si="11"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C213" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-37</v>
+        <v>21-36</v>
       </c>
       <c r="L213" s="6"/>
       <c r="M213" s="6"/>
@@ -6979,11 +6993,11 @@
       </c>
       <c r="B214">
         <f t="shared" si="11"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C214" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-38</v>
+        <v>21-37</v>
       </c>
       <c r="L214" s="6"/>
       <c r="M214" s="6"/>
@@ -6995,11 +7009,11 @@
       </c>
       <c r="B215">
         <f t="shared" si="11"/>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C215" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-39</v>
+        <v>21-38</v>
       </c>
       <c r="L215" s="6"/>
       <c r="M215" s="6"/>
@@ -7011,11 +7025,11 @@
       </c>
       <c r="B216">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C216" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-40</v>
+        <v>21-39</v>
       </c>
       <c r="L216" s="6"/>
       <c r="M216" s="6"/>
@@ -7027,11 +7041,11 @@
       </c>
       <c r="B217">
         <f t="shared" si="11"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C217" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-41</v>
+        <v>21-40</v>
       </c>
       <c r="L217" s="6"/>
       <c r="M217" s="6"/>
@@ -7043,11 +7057,11 @@
       </c>
       <c r="B218">
         <f t="shared" si="11"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C218" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-42</v>
+        <v>21-41</v>
       </c>
       <c r="L218" s="6"/>
       <c r="M218" s="6"/>
@@ -7059,11 +7073,11 @@
       </c>
       <c r="B219">
         <f t="shared" si="11"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C219" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-43</v>
+        <v>21-42</v>
       </c>
       <c r="L219" s="6"/>
       <c r="M219" s="6"/>
@@ -7075,11 +7089,11 @@
       </c>
       <c r="B220">
         <f t="shared" si="11"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C220" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-44</v>
+        <v>21-43</v>
       </c>
       <c r="L220" s="6"/>
       <c r="M220" s="6"/>
@@ -7091,11 +7105,11 @@
       </c>
       <c r="B221">
         <f t="shared" si="11"/>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C221" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-45</v>
+        <v>21-44</v>
       </c>
       <c r="L221" s="6"/>
       <c r="M221" s="6"/>
@@ -7107,11 +7121,11 @@
       </c>
       <c r="B222">
         <f t="shared" si="11"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C222" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-46</v>
+        <v>21-45</v>
       </c>
       <c r="L222" s="6"/>
       <c r="M222" s="6"/>
@@ -7123,11 +7137,11 @@
       </c>
       <c r="B223">
         <f t="shared" si="11"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C223" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-47</v>
+        <v>21-46</v>
       </c>
       <c r="L223" s="6"/>
       <c r="M223" s="6"/>
@@ -7139,11 +7153,11 @@
       </c>
       <c r="B224">
         <f t="shared" si="11"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C224" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-48</v>
+        <v>21-47</v>
       </c>
       <c r="L224" s="6"/>
       <c r="M224" s="6"/>
@@ -7155,11 +7169,11 @@
       </c>
       <c r="B225">
         <f t="shared" si="11"/>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C225" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-49</v>
+        <v>21-48</v>
       </c>
       <c r="L225" s="6"/>
       <c r="M225" s="6"/>
@@ -7171,11 +7185,11 @@
       </c>
       <c r="B226">
         <f t="shared" si="11"/>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C226" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-50</v>
+        <v>21-49</v>
       </c>
       <c r="L226" s="6"/>
       <c r="M226" s="6"/>
@@ -7187,11 +7201,11 @@
       </c>
       <c r="B227">
         <f t="shared" si="11"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C227" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-51</v>
+        <v>21-50</v>
       </c>
       <c r="L227" s="6"/>
       <c r="M227" s="6"/>
@@ -7203,11 +7217,11 @@
       </c>
       <c r="B228">
         <f t="shared" si="11"/>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C228" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-52</v>
+        <v>21-51</v>
       </c>
       <c r="L228" s="6"/>
       <c r="M228" s="6"/>
@@ -7219,11 +7233,11 @@
       </c>
       <c r="B229">
         <f t="shared" si="11"/>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C229" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-53</v>
+        <v>21-52</v>
       </c>
       <c r="L229" s="6"/>
       <c r="M229" s="6"/>
@@ -7235,11 +7249,11 @@
       </c>
       <c r="B230">
         <f t="shared" si="11"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C230" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-54</v>
+        <v>21-53</v>
       </c>
       <c r="L230" s="6"/>
       <c r="M230" s="6"/>
@@ -7251,11 +7265,11 @@
       </c>
       <c r="B231">
         <f t="shared" si="11"/>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C231" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-55</v>
+        <v>21-54</v>
       </c>
       <c r="L231" s="6"/>
       <c r="M231" s="6"/>
@@ -7267,11 +7281,11 @@
       </c>
       <c r="B232">
         <f t="shared" si="11"/>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C232" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-56</v>
+        <v>21-55</v>
       </c>
       <c r="L232" s="6"/>
       <c r="M232" s="6"/>
@@ -7283,11 +7297,11 @@
       </c>
       <c r="B233">
         <f t="shared" si="11"/>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C233" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-57</v>
+        <v>21-56</v>
       </c>
       <c r="L233" s="6"/>
       <c r="M233" s="6"/>
@@ -7299,11 +7313,11 @@
       </c>
       <c r="B234">
         <f t="shared" si="11"/>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C234" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-58</v>
+        <v>21-57</v>
       </c>
       <c r="L234" s="6"/>
       <c r="M234" s="6"/>
@@ -7315,11 +7329,11 @@
       </c>
       <c r="B235">
         <f t="shared" si="11"/>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C235" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-59</v>
+        <v>21-58</v>
       </c>
       <c r="L235" s="6"/>
       <c r="M235" s="6"/>
@@ -7331,11 +7345,11 @@
       </c>
       <c r="B236">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C236" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-60</v>
+        <v>21-59</v>
       </c>
       <c r="L236" s="6"/>
       <c r="M236" s="6"/>
@@ -7347,11 +7361,11 @@
       </c>
       <c r="B237">
         <f t="shared" si="11"/>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C237" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-61</v>
+        <v>21-60</v>
       </c>
       <c r="L237" s="6"/>
       <c r="M237" s="6"/>
@@ -7363,11 +7377,11 @@
       </c>
       <c r="B238">
         <f t="shared" si="11"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C238" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-62</v>
+        <v>21-61</v>
       </c>
       <c r="L238" s="6"/>
       <c r="M238" s="6"/>
@@ -7379,11 +7393,11 @@
       </c>
       <c r="B239">
         <f t="shared" si="11"/>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C239" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-63</v>
+        <v>21-62</v>
       </c>
       <c r="L239" s="6"/>
       <c r="M239" s="6"/>
@@ -7395,11 +7409,11 @@
       </c>
       <c r="B240">
         <f t="shared" si="11"/>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C240" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-64</v>
+        <v>21-63</v>
       </c>
       <c r="L240" s="6"/>
       <c r="M240" s="6"/>
@@ -7411,11 +7425,11 @@
       </c>
       <c r="B241">
         <f t="shared" si="11"/>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C241" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-65</v>
+        <v>21-64</v>
       </c>
       <c r="L241" s="6"/>
       <c r="M241" s="6"/>
@@ -7427,11 +7441,11 @@
       </c>
       <c r="B242">
         <f t="shared" si="11"/>
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C242" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-66</v>
+        <v>21-65</v>
       </c>
       <c r="L242" s="6"/>
       <c r="M242" s="6"/>
@@ -7443,11 +7457,11 @@
       </c>
       <c r="B243">
         <f t="shared" si="11"/>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C243" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-67</v>
+        <v>21-66</v>
       </c>
       <c r="L243" s="6"/>
       <c r="M243" s="6"/>
@@ -7459,11 +7473,11 @@
       </c>
       <c r="B244">
         <f t="shared" si="11"/>
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C244" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-68</v>
+        <v>21-67</v>
       </c>
       <c r="L244" s="6"/>
       <c r="M244" s="6"/>
@@ -7475,11 +7489,11 @@
       </c>
       <c r="B245">
         <f t="shared" si="11"/>
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C245" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-69</v>
+        <v>21-68</v>
       </c>
       <c r="L245" s="6"/>
       <c r="M245" s="6"/>
@@ -7491,11 +7505,11 @@
       </c>
       <c r="B246">
         <f t="shared" si="11"/>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C246" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-70</v>
+        <v>21-69</v>
       </c>
       <c r="L246" s="6"/>
       <c r="M246" s="6"/>
@@ -7507,11 +7521,11 @@
       </c>
       <c r="B247">
         <f t="shared" si="11"/>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C247" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-71</v>
+        <v>21-70</v>
       </c>
       <c r="L247" s="6"/>
       <c r="M247" s="6"/>
@@ -7523,11 +7537,11 @@
       </c>
       <c r="B248">
         <f t="shared" si="11"/>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C248" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-72</v>
+        <v>21-71</v>
       </c>
       <c r="L248" s="6"/>
       <c r="M248" s="6"/>
@@ -7539,11 +7553,11 @@
       </c>
       <c r="B249">
         <f t="shared" si="11"/>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C249" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-73</v>
+        <v>21-72</v>
       </c>
       <c r="L249" s="6"/>
       <c r="M249" s="6"/>
@@ -7555,11 +7569,11 @@
       </c>
       <c r="B250">
         <f t="shared" si="11"/>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C250" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-74</v>
+        <v>21-73</v>
       </c>
       <c r="L250" s="6"/>
       <c r="M250" s="6"/>
@@ -7571,11 +7585,11 @@
       </c>
       <c r="B251">
         <f t="shared" si="11"/>
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C251" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-75</v>
+        <v>21-74</v>
       </c>
       <c r="L251" s="6"/>
       <c r="M251" s="6"/>
@@ -7587,11 +7601,11 @@
       </c>
       <c r="B252">
         <f t="shared" si="11"/>
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C252" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-76</v>
+        <v>21-75</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
@@ -7603,11 +7617,11 @@
       </c>
       <c r="B253">
         <f t="shared" si="11"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C253" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-77</v>
+        <v>21-76</v>
       </c>
       <c r="L253" s="6"/>
       <c r="M253" s="6"/>
@@ -7619,11 +7633,11 @@
       </c>
       <c r="B254">
         <f t="shared" si="11"/>
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C254" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-78</v>
+        <v>21-77</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
@@ -7635,11 +7649,11 @@
       </c>
       <c r="B255">
         <f t="shared" si="11"/>
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C255" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-79</v>
+        <v>21-78</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
@@ -7651,11 +7665,11 @@
       </c>
       <c r="B256">
         <f t="shared" si="11"/>
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C256" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-80</v>
+        <v>21-79</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
@@ -7667,11 +7681,11 @@
       </c>
       <c r="B257">
         <f t="shared" si="11"/>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C257" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-81</v>
+        <v>21-80</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
@@ -7683,11 +7697,11 @@
       </c>
       <c r="B258">
         <f t="shared" si="11"/>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C258" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-82</v>
+        <v>21-81</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
@@ -7699,11 +7713,11 @@
       </c>
       <c r="B259">
         <f t="shared" si="11"/>
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C259" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>21-83</v>
+        <v>21-82</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
@@ -7714,44 +7728,44 @@
         <v>21</v>
       </c>
       <c r="B260">
-        <f t="shared" ref="B260:B323" si="14">IF(A260=A259,B259+1,1)</f>
-        <v>84</v>
+        <f t="shared" si="11"/>
+        <v>83</v>
       </c>
       <c r="C260" s="3" t="str">
-        <f t="shared" ref="C260:C323" si="15">CONCATENATE(A260,"-",B260)</f>
-        <v>21-84</v>
+        <f t="shared" si="12"/>
+        <v>21-83</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
     </row>
     <row r="261" spans="1:13" ht="15">
       <c r="A261">
-        <f t="shared" ref="A261:A324" si="16">A260</f>
+        <f t="shared" si="13"/>
         <v>21</v>
       </c>
       <c r="B261">
+        <f t="shared" ref="B261:B324" si="14">IF(A261=A260,B260+1,1)</f>
+        <v>84</v>
+      </c>
+      <c r="C261" s="3" t="str">
+        <f t="shared" ref="C261:C324" si="15">CONCATENATE(A261,"-",B261)</f>
+        <v>21-84</v>
+      </c>
+      <c r="L261" s="6"/>
+      <c r="M261" s="6"/>
+    </row>
+    <row r="262" spans="1:13" ht="15">
+      <c r="A262">
+        <f t="shared" ref="A262:A325" si="16">A261</f>
+        <v>21</v>
+      </c>
+      <c r="B262">
         <f t="shared" si="14"/>
         <v>85</v>
       </c>
-      <c r="C261" s="3" t="str">
+      <c r="C262" s="3" t="str">
         <f t="shared" si="15"/>
         <v>21-85</v>
-      </c>
-      <c r="L261" s="6"/>
-      <c r="M261" s="6"/>
-    </row>
-    <row r="262" spans="1:13" ht="15">
-      <c r="A262">
-        <f t="shared" si="16"/>
-        <v>21</v>
-      </c>
-      <c r="B262">
-        <f t="shared" si="14"/>
-        <v>86</v>
-      </c>
-      <c r="C262" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v>21-86</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
@@ -7763,11 +7777,11 @@
       </c>
       <c r="B263">
         <f t="shared" si="14"/>
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C263" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-87</v>
+        <v>21-86</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
@@ -7779,11 +7793,11 @@
       </c>
       <c r="B264">
         <f t="shared" si="14"/>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C264" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-88</v>
+        <v>21-87</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
@@ -7795,11 +7809,11 @@
       </c>
       <c r="B265">
         <f t="shared" si="14"/>
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C265" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-89</v>
+        <v>21-88</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
@@ -7811,11 +7825,11 @@
       </c>
       <c r="B266">
         <f t="shared" si="14"/>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C266" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-90</v>
+        <v>21-89</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
@@ -7827,11 +7841,11 @@
       </c>
       <c r="B267">
         <f t="shared" si="14"/>
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C267" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-91</v>
+        <v>21-90</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
@@ -7843,11 +7857,11 @@
       </c>
       <c r="B268">
         <f t="shared" si="14"/>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C268" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-92</v>
+        <v>21-91</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
@@ -7859,11 +7873,11 @@
       </c>
       <c r="B269">
         <f t="shared" si="14"/>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C269" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-93</v>
+        <v>21-92</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
@@ -7875,11 +7889,11 @@
       </c>
       <c r="B270">
         <f t="shared" si="14"/>
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C270" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-94</v>
+        <v>21-93</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
@@ -7891,11 +7905,11 @@
       </c>
       <c r="B271">
         <f t="shared" si="14"/>
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C271" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-95</v>
+        <v>21-94</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
@@ -7907,11 +7921,11 @@
       </c>
       <c r="B272">
         <f t="shared" si="14"/>
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C272" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-96</v>
+        <v>21-95</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
@@ -7923,11 +7937,11 @@
       </c>
       <c r="B273">
         <f t="shared" si="14"/>
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C273" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-97</v>
+        <v>21-96</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
@@ -7939,11 +7953,11 @@
       </c>
       <c r="B274">
         <f t="shared" si="14"/>
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C274" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-98</v>
+        <v>21-97</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
@@ -7955,11 +7969,11 @@
       </c>
       <c r="B275">
         <f t="shared" si="14"/>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C275" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-99</v>
+        <v>21-98</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
@@ -7971,11 +7985,11 @@
       </c>
       <c r="B276">
         <f t="shared" si="14"/>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C276" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-100</v>
+        <v>21-99</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
@@ -7987,11 +8001,11 @@
       </c>
       <c r="B277">
         <f t="shared" si="14"/>
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C277" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-101</v>
+        <v>21-100</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
@@ -8003,11 +8017,11 @@
       </c>
       <c r="B278">
         <f t="shared" si="14"/>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C278" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-102</v>
+        <v>21-101</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
@@ -8019,11 +8033,11 @@
       </c>
       <c r="B279">
         <f t="shared" si="14"/>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C279" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-103</v>
+        <v>21-102</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
@@ -8035,11 +8049,11 @@
       </c>
       <c r="B280">
         <f t="shared" si="14"/>
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C280" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-104</v>
+        <v>21-103</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
@@ -8051,11 +8065,11 @@
       </c>
       <c r="B281">
         <f t="shared" si="14"/>
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C281" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-105</v>
+        <v>21-104</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
@@ -8067,11 +8081,11 @@
       </c>
       <c r="B282">
         <f t="shared" si="14"/>
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C282" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-106</v>
+        <v>21-105</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
@@ -8083,11 +8097,11 @@
       </c>
       <c r="B283">
         <f t="shared" si="14"/>
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C283" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-107</v>
+        <v>21-106</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
@@ -8099,11 +8113,11 @@
       </c>
       <c r="B284">
         <f t="shared" si="14"/>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C284" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-108</v>
+        <v>21-107</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
@@ -8115,11 +8129,11 @@
       </c>
       <c r="B285">
         <f t="shared" si="14"/>
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C285" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-109</v>
+        <v>21-108</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
@@ -8131,11 +8145,11 @@
       </c>
       <c r="B286">
         <f t="shared" si="14"/>
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C286" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-110</v>
+        <v>21-109</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
@@ -8147,11 +8161,11 @@
       </c>
       <c r="B287">
         <f t="shared" si="14"/>
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C287" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-111</v>
+        <v>21-110</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
@@ -8163,11 +8177,11 @@
       </c>
       <c r="B288">
         <f t="shared" si="14"/>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C288" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-112</v>
+        <v>21-111</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
@@ -8179,11 +8193,11 @@
       </c>
       <c r="B289">
         <f t="shared" si="14"/>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C289" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-113</v>
+        <v>21-112</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
@@ -8195,11 +8209,11 @@
       </c>
       <c r="B290">
         <f t="shared" si="14"/>
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C290" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-114</v>
+        <v>21-113</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
@@ -8211,11 +8225,11 @@
       </c>
       <c r="B291">
         <f t="shared" si="14"/>
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C291" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-115</v>
+        <v>21-114</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
@@ -8227,11 +8241,11 @@
       </c>
       <c r="B292">
         <f t="shared" si="14"/>
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C292" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-116</v>
+        <v>21-115</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
@@ -8243,11 +8257,11 @@
       </c>
       <c r="B293">
         <f t="shared" si="14"/>
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C293" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-117</v>
+        <v>21-116</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
@@ -8259,11 +8273,11 @@
       </c>
       <c r="B294">
         <f t="shared" si="14"/>
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C294" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-118</v>
+        <v>21-117</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
@@ -8275,11 +8289,11 @@
       </c>
       <c r="B295">
         <f t="shared" si="14"/>
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C295" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-119</v>
+        <v>21-118</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
@@ -8291,11 +8305,11 @@
       </c>
       <c r="B296">
         <f t="shared" si="14"/>
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C296" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-120</v>
+        <v>21-119</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
@@ -8307,11 +8321,11 @@
       </c>
       <c r="B297">
         <f t="shared" si="14"/>
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C297" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-121</v>
+        <v>21-120</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
@@ -8323,11 +8337,11 @@
       </c>
       <c r="B298">
         <f t="shared" si="14"/>
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C298" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-122</v>
+        <v>21-121</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
@@ -8339,11 +8353,11 @@
       </c>
       <c r="B299">
         <f t="shared" si="14"/>
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C299" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-123</v>
+        <v>21-122</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
@@ -8355,11 +8369,11 @@
       </c>
       <c r="B300">
         <f t="shared" si="14"/>
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C300" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-124</v>
+        <v>21-123</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
@@ -8371,11 +8385,11 @@
       </c>
       <c r="B301">
         <f t="shared" si="14"/>
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C301" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-125</v>
+        <v>21-124</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
@@ -8387,11 +8401,11 @@
       </c>
       <c r="B302">
         <f t="shared" si="14"/>
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C302" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-126</v>
+        <v>21-125</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
@@ -8403,11 +8417,11 @@
       </c>
       <c r="B303">
         <f t="shared" si="14"/>
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C303" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-127</v>
+        <v>21-126</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
@@ -8419,11 +8433,11 @@
       </c>
       <c r="B304">
         <f t="shared" si="14"/>
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C304" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-128</v>
+        <v>21-127</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
@@ -8435,11 +8449,11 @@
       </c>
       <c r="B305">
         <f t="shared" si="14"/>
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C305" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-129</v>
+        <v>21-128</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
@@ -8451,11 +8465,11 @@
       </c>
       <c r="B306">
         <f t="shared" si="14"/>
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C306" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-130</v>
+        <v>21-129</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
@@ -8467,11 +8481,11 @@
       </c>
       <c r="B307">
         <f t="shared" si="14"/>
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C307" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-131</v>
+        <v>21-130</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
@@ -8483,11 +8497,11 @@
       </c>
       <c r="B308">
         <f t="shared" si="14"/>
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C308" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-132</v>
+        <v>21-131</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
@@ -8499,11 +8513,11 @@
       </c>
       <c r="B309">
         <f t="shared" si="14"/>
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C309" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-133</v>
+        <v>21-132</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
@@ -8515,11 +8529,11 @@
       </c>
       <c r="B310">
         <f t="shared" si="14"/>
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C310" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-134</v>
+        <v>21-133</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
@@ -8531,11 +8545,11 @@
       </c>
       <c r="B311">
         <f t="shared" si="14"/>
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C311" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-135</v>
+        <v>21-134</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
@@ -8547,11 +8561,11 @@
       </c>
       <c r="B312">
         <f t="shared" si="14"/>
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C312" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-136</v>
+        <v>21-135</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
@@ -8563,11 +8577,11 @@
       </c>
       <c r="B313">
         <f t="shared" si="14"/>
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C313" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-137</v>
+        <v>21-136</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
@@ -8579,11 +8593,11 @@
       </c>
       <c r="B314">
         <f t="shared" si="14"/>
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C314" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-138</v>
+        <v>21-137</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
@@ -8595,11 +8609,11 @@
       </c>
       <c r="B315">
         <f t="shared" si="14"/>
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C315" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-139</v>
+        <v>21-138</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
@@ -8611,11 +8625,11 @@
       </c>
       <c r="B316">
         <f t="shared" si="14"/>
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C316" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-140</v>
+        <v>21-139</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
@@ -8627,11 +8641,11 @@
       </c>
       <c r="B317">
         <f t="shared" si="14"/>
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C317" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-141</v>
+        <v>21-140</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
@@ -8643,11 +8657,11 @@
       </c>
       <c r="B318">
         <f t="shared" si="14"/>
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C318" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-142</v>
+        <v>21-141</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
@@ -8659,11 +8673,11 @@
       </c>
       <c r="B319">
         <f t="shared" si="14"/>
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C319" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-143</v>
+        <v>21-142</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
@@ -8675,11 +8689,11 @@
       </c>
       <c r="B320">
         <f t="shared" si="14"/>
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C320" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-144</v>
+        <v>21-143</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
@@ -8691,11 +8705,11 @@
       </c>
       <c r="B321">
         <f t="shared" si="14"/>
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C321" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-145</v>
+        <v>21-144</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
@@ -8707,11 +8721,11 @@
       </c>
       <c r="B322">
         <f t="shared" si="14"/>
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C322" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-146</v>
+        <v>21-145</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
@@ -8723,11 +8737,11 @@
       </c>
       <c r="B323">
         <f t="shared" si="14"/>
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C323" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>21-147</v>
+        <v>21-146</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
@@ -8738,44 +8752,44 @@
         <v>21</v>
       </c>
       <c r="B324">
-        <f t="shared" ref="B324:B345" si="17">IF(A324=A323,B323+1,1)</f>
-        <v>148</v>
+        <f t="shared" si="14"/>
+        <v>147</v>
       </c>
       <c r="C324" s="3" t="str">
-        <f t="shared" ref="C324:C345" si="18">CONCATENATE(A324,"-",B324)</f>
-        <v>21-148</v>
+        <f t="shared" si="15"/>
+        <v>21-147</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
     </row>
     <row r="325" spans="1:13" ht="15">
       <c r="A325">
-        <f t="shared" ref="A325:A345" si="19">A324</f>
+        <f t="shared" si="16"/>
         <v>21</v>
       </c>
       <c r="B325">
+        <f t="shared" ref="B325:B346" si="17">IF(A325=A324,B324+1,1)</f>
+        <v>148</v>
+      </c>
+      <c r="C325" s="3" t="str">
+        <f t="shared" ref="C325:C346" si="18">CONCATENATE(A325,"-",B325)</f>
+        <v>21-148</v>
+      </c>
+      <c r="L325" s="6"/>
+      <c r="M325" s="6"/>
+    </row>
+    <row r="326" spans="1:13" ht="15">
+      <c r="A326">
+        <f t="shared" ref="A326:A346" si="19">A325</f>
+        <v>21</v>
+      </c>
+      <c r="B326">
         <f t="shared" si="17"/>
         <v>149</v>
       </c>
-      <c r="C325" s="3" t="str">
+      <c r="C326" s="3" t="str">
         <f t="shared" si="18"/>
         <v>21-149</v>
-      </c>
-      <c r="L325" s="6"/>
-      <c r="M325" s="6"/>
-    </row>
-    <row r="326" spans="1:13" ht="15">
-      <c r="A326">
-        <f t="shared" si="19"/>
-        <v>21</v>
-      </c>
-      <c r="B326">
-        <f t="shared" si="17"/>
-        <v>150</v>
-      </c>
-      <c r="C326" s="3" t="str">
-        <f t="shared" si="18"/>
-        <v>21-150</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
@@ -8787,11 +8801,11 @@
       </c>
       <c r="B327">
         <f t="shared" si="17"/>
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C327" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-151</v>
+        <v>21-150</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
@@ -8803,11 +8817,11 @@
       </c>
       <c r="B328">
         <f t="shared" si="17"/>
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C328" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-152</v>
+        <v>21-151</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
@@ -8819,11 +8833,11 @@
       </c>
       <c r="B329">
         <f t="shared" si="17"/>
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C329" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-153</v>
+        <v>21-152</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
@@ -8835,11 +8849,11 @@
       </c>
       <c r="B330">
         <f t="shared" si="17"/>
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C330" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-154</v>
+        <v>21-153</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
@@ -8851,11 +8865,11 @@
       </c>
       <c r="B331">
         <f t="shared" si="17"/>
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C331" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-155</v>
+        <v>21-154</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
@@ -8867,11 +8881,11 @@
       </c>
       <c r="B332">
         <f t="shared" si="17"/>
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C332" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-156</v>
+        <v>21-155</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
@@ -8883,11 +8897,11 @@
       </c>
       <c r="B333">
         <f t="shared" si="17"/>
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C333" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-157</v>
+        <v>21-156</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
@@ -8899,11 +8913,11 @@
       </c>
       <c r="B334">
         <f t="shared" si="17"/>
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C334" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-158</v>
+        <v>21-157</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
@@ -8915,11 +8929,11 @@
       </c>
       <c r="B335">
         <f t="shared" si="17"/>
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C335" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-159</v>
+        <v>21-158</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
@@ -8931,11 +8945,11 @@
       </c>
       <c r="B336">
         <f t="shared" si="17"/>
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C336" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-160</v>
+        <v>21-159</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
@@ -8947,11 +8961,11 @@
       </c>
       <c r="B337">
         <f t="shared" si="17"/>
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C337" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-161</v>
+        <v>21-160</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
@@ -8963,11 +8977,11 @@
       </c>
       <c r="B338">
         <f t="shared" si="17"/>
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C338" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-162</v>
+        <v>21-161</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
@@ -8979,11 +8993,11 @@
       </c>
       <c r="B339">
         <f t="shared" si="17"/>
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C339" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-163</v>
+        <v>21-162</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
@@ -8995,11 +9009,11 @@
       </c>
       <c r="B340">
         <f t="shared" si="17"/>
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C340" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-164</v>
+        <v>21-163</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
@@ -9011,11 +9025,11 @@
       </c>
       <c r="B341">
         <f t="shared" si="17"/>
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C341" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-165</v>
+        <v>21-164</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
@@ -9027,11 +9041,11 @@
       </c>
       <c r="B342">
         <f t="shared" si="17"/>
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C342" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-166</v>
+        <v>21-165</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
@@ -9043,11 +9057,11 @@
       </c>
       <c r="B343">
         <f t="shared" si="17"/>
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C343" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-167</v>
+        <v>21-166</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
@@ -9059,11 +9073,11 @@
       </c>
       <c r="B344">
         <f t="shared" si="17"/>
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C344" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-168</v>
+        <v>21-167</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
@@ -9075,16 +9089,28 @@
       </c>
       <c r="B345">
         <f t="shared" si="17"/>
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C345" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>21-169</v>
+        <v>21-168</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
     </row>
-    <row r="346" spans="1:13" ht="12.75">
+    <row r="346" spans="1:13" ht="15">
+      <c r="A346">
+        <f t="shared" si="19"/>
+        <v>21</v>
+      </c>
+      <c r="B346">
+        <f t="shared" si="17"/>
+        <v>169</v>
+      </c>
+      <c r="C346" s="3" t="str">
+        <f t="shared" si="18"/>
+        <v>21-169</v>
+      </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
     </row>
@@ -11832,21 +11858,25 @@
       <c r="L1032" s="6"/>
       <c r="M1032" s="6"/>
     </row>
+    <row r="1033" spans="12:13" ht="12.75">
+      <c r="L1033" s="6"/>
+      <c r="M1033" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L171:L174"/>
+    <mergeCell ref="L172:L175"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:K182">
+  <conditionalFormatting sqref="K2:K183">
     <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K182">
+  <conditionalFormatting sqref="K2:K183">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K182">
+  <conditionalFormatting sqref="K2:K183">
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add instrument list tests to manual system tests spreadsheet
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="262">
   <si>
     <t>Test Number</t>
   </si>
@@ -782,6 +782,27 @@
   </si>
   <si>
     <t>The gui is filtering out requests to refresh the message view but this means the last refresh may not be caught hence the check on the last message.</t>
+  </si>
+  <si>
+    <t>Local host name appears at the top of the instrument list when on a host machine</t>
+  </si>
+  <si>
+    <t>Instrument List</t>
+  </si>
+  <si>
+    <t>When on an instrument machine for an instrument in CS:INSTLIST, the instrument name only appears once and it is at the top of the list</t>
+  </si>
+  <si>
+    <t>List of supported instruments appears in the instrument list</t>
+  </si>
+  <si>
+    <t>Can switch from local host to other instrument</t>
+  </si>
+  <si>
+    <t>Can switch between two listed instruments</t>
+  </si>
+  <si>
+    <t>Can switch to a custom instrument not on the list</t>
   </si>
 </sst>
 </file>
@@ -838,7 +859,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -898,11 +919,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -946,14 +1013,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="54">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1710,132 +1803,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2136,8 +2103,8 @@
   <dimension ref="A1:N1052"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H208" sqref="H208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -7163,7 +7130,7 @@
       </c>
       <c r="J174" s="8"/>
       <c r="K174" s="7"/>
-      <c r="L174" s="18"/>
+      <c r="L174" s="19"/>
     </row>
     <row r="175" spans="1:13" ht="30">
       <c r="A175">
@@ -7192,7 +7159,7 @@
       </c>
       <c r="J175" s="8"/>
       <c r="K175" s="7"/>
-      <c r="L175" s="19"/>
+      <c r="L175" s="20"/>
       <c r="M175" s="6"/>
     </row>
     <row r="176" spans="1:13" ht="45">
@@ -7222,7 +7189,7 @@
       </c>
       <c r="J176" s="8"/>
       <c r="K176" s="7"/>
-      <c r="L176" s="19"/>
+      <c r="L176" s="20"/>
       <c r="M176" s="6"/>
     </row>
     <row r="177" spans="1:13" ht="30">
@@ -7252,7 +7219,7 @@
       </c>
       <c r="J177" s="8"/>
       <c r="K177" s="7"/>
-      <c r="L177" s="20"/>
+      <c r="L177" s="21"/>
       <c r="M177" s="6"/>
     </row>
     <row r="178" spans="1:13" ht="30">
@@ -8013,75 +7980,109 @@
         <f t="shared" si="12"/>
         <v>23</v>
       </c>
-      <c r="C202" s="3" t="str">
-        <f t="shared" ref="C202" si="28">CONCATENATE(A202,"-",B202)</f>
+      <c r="C202" s="22" t="str">
+        <f t="shared" ref="C202:C203" si="28">CONCATENATE(A202,"-",B202)</f>
         <v>21-23</v>
       </c>
-      <c r="D202" s="15"/>
-      <c r="E202" s="15"/>
-      <c r="F202" s="15"/>
-      <c r="G202" s="10" t="s">
+      <c r="D202" s="23"/>
+      <c r="E202" s="23"/>
+      <c r="F202" s="23"/>
+      <c r="G202" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="H202" s="10" t="s">
+      <c r="H202" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="I202" s="12" t="s">
+      <c r="I202" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="J202" s="12"/>
-      <c r="K202" s="10"/>
-      <c r="L202" s="12" t="s">
+      <c r="J202" s="18"/>
+      <c r="K202" s="24"/>
+      <c r="L202" s="18" t="s">
         <v>231</v>
       </c>
       <c r="M202" s="6"/>
     </row>
-    <row r="203" spans="1:13" ht="15">
+    <row r="203" spans="1:13" ht="26.25">
       <c r="A203">
         <v>22</v>
       </c>
       <c r="B203">
-        <v>24</v>
-      </c>
-      <c r="C203" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>22-24</v>
-      </c>
-      <c r="G203" s="21"/>
-      <c r="H203" s="21"/>
-      <c r="L203" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="C203" s="26" t="str">
+        <f>CONCATENATE(A203,"-",B203)</f>
+        <v>22-1</v>
+      </c>
+      <c r="D203" s="27"/>
+      <c r="E203" s="27"/>
+      <c r="F203" s="27"/>
+      <c r="G203" s="28"/>
+      <c r="H203" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="I203" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="J203" s="27"/>
+      <c r="K203" s="27"/>
+      <c r="L203" s="30"/>
       <c r="M203" s="6"/>
     </row>
-    <row r="204" spans="1:13" ht="15">
+    <row r="204" spans="1:13" ht="39">
       <c r="A204">
         <f>A203</f>
         <v>22</v>
       </c>
       <c r="B204">
         <f>IF(A204=A203,B203+1,1)</f>
-        <v>25</v>
-      </c>
-      <c r="C204" s="3" t="str">
+        <v>2</v>
+      </c>
+      <c r="C204" s="26" t="str">
         <f t="shared" si="13"/>
-        <v>22-25</v>
-      </c>
-      <c r="L204" s="6"/>
+        <v>22-2</v>
+      </c>
+      <c r="D204" s="27"/>
+      <c r="E204" s="27"/>
+      <c r="F204" s="27"/>
+      <c r="G204" s="27"/>
+      <c r="H204" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="I204" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="J204" s="27"/>
+      <c r="K204" s="27"/>
+      <c r="L204" s="30"/>
       <c r="M204" s="6"/>
     </row>
-    <row r="205" spans="1:13" ht="15">
+    <row r="205" spans="1:13" ht="26.25">
       <c r="A205">
         <f t="shared" si="14"/>
         <v>22</v>
       </c>
       <c r="B205">
         <f t="shared" si="12"/>
-        <v>26</v>
-      </c>
-      <c r="C205" s="3" t="str">
+        <v>3</v>
+      </c>
+      <c r="C205" s="26" t="str">
         <f t="shared" si="13"/>
-        <v>22-26</v>
-      </c>
-      <c r="L205" s="6"/>
+        <v>22-3</v>
+      </c>
+      <c r="D205" s="27"/>
+      <c r="E205" s="27"/>
+      <c r="F205" s="27"/>
+      <c r="G205" s="27"/>
+      <c r="H205" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="I205" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="J205" s="27"/>
+      <c r="K205" s="27"/>
+      <c r="L205" s="30"/>
       <c r="M205" s="6"/>
     </row>
     <row r="206" spans="1:13" ht="15">
@@ -8091,13 +8092,25 @@
       </c>
       <c r="B206">
         <f t="shared" si="12"/>
-        <v>27</v>
-      </c>
-      <c r="C206" s="3" t="str">
+        <v>4</v>
+      </c>
+      <c r="C206" s="26" t="str">
         <f t="shared" si="13"/>
-        <v>22-27</v>
-      </c>
-      <c r="L206" s="6"/>
+        <v>22-4</v>
+      </c>
+      <c r="D206" s="27"/>
+      <c r="E206" s="27"/>
+      <c r="F206" s="27"/>
+      <c r="G206" s="27"/>
+      <c r="H206" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="I206" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="J206" s="27"/>
+      <c r="K206" s="27"/>
+      <c r="L206" s="30"/>
       <c r="M206" s="6"/>
     </row>
     <row r="207" spans="1:13" ht="15">
@@ -8107,13 +8120,25 @@
       </c>
       <c r="B207">
         <f t="shared" si="12"/>
-        <v>28</v>
-      </c>
-      <c r="C207" s="3" t="str">
+        <v>5</v>
+      </c>
+      <c r="C207" s="26" t="str">
         <f t="shared" si="13"/>
-        <v>22-28</v>
-      </c>
-      <c r="L207" s="6"/>
+        <v>22-5</v>
+      </c>
+      <c r="D207" s="27"/>
+      <c r="E207" s="27"/>
+      <c r="F207" s="27"/>
+      <c r="G207" s="27"/>
+      <c r="H207" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="I207" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="J207" s="27"/>
+      <c r="K207" s="27"/>
+      <c r="L207" s="30"/>
       <c r="M207" s="6"/>
     </row>
     <row r="208" spans="1:13" ht="15">
@@ -8123,43 +8148,56 @@
       </c>
       <c r="B208">
         <f t="shared" si="12"/>
-        <v>29</v>
-      </c>
-      <c r="C208" s="3" t="str">
+        <v>6</v>
+      </c>
+      <c r="C208" s="26" t="str">
         <f t="shared" si="13"/>
-        <v>22-29</v>
-      </c>
-      <c r="L208" s="6"/>
+        <v>22-6</v>
+      </c>
+      <c r="D208" s="27"/>
+      <c r="E208" s="27"/>
+      <c r="F208" s="27"/>
+      <c r="G208" s="27"/>
+      <c r="H208" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="I208" s="29" t="s">
+        <v>261</v>
+      </c>
+      <c r="J208" s="27"/>
+      <c r="K208" s="27"/>
+      <c r="L208" s="30"/>
       <c r="M208" s="6"/>
     </row>
     <row r="209" spans="1:13" ht="15">
       <c r="A209">
-        <f t="shared" si="14"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B209">
         <f t="shared" si="12"/>
-        <v>30</v>
-      </c>
-      <c r="C209" s="3" t="str">
+        <v>1</v>
+      </c>
+      <c r="C209" s="25" t="str">
         <f t="shared" si="13"/>
-        <v>22-30</v>
-      </c>
+        <v>23-1</v>
+      </c>
+      <c r="H209" s="33"/>
+      <c r="I209" s="31"/>
       <c r="L209" s="6"/>
       <c r="M209" s="6"/>
     </row>
     <row r="210" spans="1:13" ht="15">
       <c r="A210">
         <f t="shared" si="14"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B210">
         <f t="shared" si="12"/>
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C210" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>22-31</v>
+        <v>23-2</v>
       </c>
       <c r="L210" s="6"/>
       <c r="M210" s="6"/>
@@ -8167,15 +8205,15 @@
     <row r="211" spans="1:13" ht="15">
       <c r="A211">
         <f t="shared" si="14"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B211">
         <f t="shared" si="12"/>
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C211" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>22-32</v>
+        <v>23-3</v>
       </c>
       <c r="L211" s="6"/>
       <c r="M211" s="6"/>
@@ -8183,15 +8221,15 @@
     <row r="212" spans="1:13" ht="15">
       <c r="A212">
         <f t="shared" si="14"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B212">
         <f t="shared" si="12"/>
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C212" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>22-33</v>
+        <v>23-4</v>
       </c>
       <c r="L212" s="6"/>
       <c r="M212" s="6"/>
@@ -8199,15 +8237,15 @@
     <row r="213" spans="1:13" ht="15">
       <c r="A213">
         <f t="shared" si="14"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B213">
         <f t="shared" si="12"/>
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C213" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>22-34</v>
+        <v>23-5</v>
       </c>
       <c r="L213" s="6"/>
       <c r="M213" s="6"/>
@@ -8215,15 +8253,15 @@
     <row r="214" spans="1:13" ht="15">
       <c r="A214">
         <f t="shared" si="14"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B214">
         <f t="shared" si="12"/>
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C214" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>22-35</v>
+        <v>23-6</v>
       </c>
       <c r="L214" s="6"/>
       <c r="M214" s="6"/>
@@ -8231,15 +8269,15 @@
     <row r="215" spans="1:13" ht="15">
       <c r="A215">
         <f t="shared" si="14"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B215">
         <f t="shared" si="12"/>
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C215" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>22-36</v>
+        <v>23-7</v>
       </c>
       <c r="L215" s="6"/>
       <c r="M215" s="6"/>
@@ -8247,15 +8285,15 @@
     <row r="216" spans="1:13" ht="15">
       <c r="A216">
         <f t="shared" si="14"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B216">
         <f t="shared" ref="B216:B279" si="29">IF(A216=A215,B215+1,1)</f>
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C216" s="3" t="str">
         <f t="shared" ref="C216:C279" si="30">CONCATENATE(A216,"-",B216)</f>
-        <v>22-37</v>
+        <v>23-8</v>
       </c>
       <c r="L216" s="6"/>
       <c r="M216" s="6"/>
@@ -8263,15 +8301,15 @@
     <row r="217" spans="1:13" ht="15">
       <c r="A217">
         <f t="shared" ref="A217:A280" si="31">A216</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B217">
         <f t="shared" si="29"/>
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C217" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-38</v>
+        <v>23-9</v>
       </c>
       <c r="L217" s="6"/>
       <c r="M217" s="6"/>
@@ -8279,15 +8317,15 @@
     <row r="218" spans="1:13" ht="15">
       <c r="A218">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B218">
         <f t="shared" si="29"/>
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C218" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-39</v>
+        <v>23-10</v>
       </c>
       <c r="L218" s="6"/>
       <c r="M218" s="6"/>
@@ -8295,15 +8333,15 @@
     <row r="219" spans="1:13" ht="15">
       <c r="A219">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B219">
         <f t="shared" si="29"/>
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C219" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-40</v>
+        <v>23-11</v>
       </c>
       <c r="L219" s="6"/>
       <c r="M219" s="6"/>
@@ -8311,15 +8349,15 @@
     <row r="220" spans="1:13" ht="15">
       <c r="A220">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B220">
         <f t="shared" si="29"/>
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C220" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-41</v>
+        <v>23-12</v>
       </c>
       <c r="L220" s="6"/>
       <c r="M220" s="6"/>
@@ -8327,15 +8365,15 @@
     <row r="221" spans="1:13" ht="15">
       <c r="A221">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B221">
         <f t="shared" si="29"/>
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="C221" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-42</v>
+        <v>23-13</v>
       </c>
       <c r="L221" s="6"/>
       <c r="M221" s="6"/>
@@ -8343,15 +8381,15 @@
     <row r="222" spans="1:13" ht="15">
       <c r="A222">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B222">
         <f t="shared" si="29"/>
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="C222" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-43</v>
+        <v>23-14</v>
       </c>
       <c r="L222" s="6"/>
       <c r="M222" s="6"/>
@@ -8359,15 +8397,15 @@
     <row r="223" spans="1:13" ht="15">
       <c r="A223">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B223">
         <f t="shared" si="29"/>
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="C223" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-44</v>
+        <v>23-15</v>
       </c>
       <c r="L223" s="6"/>
       <c r="M223" s="6"/>
@@ -8375,15 +8413,15 @@
     <row r="224" spans="1:13" ht="15">
       <c r="A224">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B224">
         <f t="shared" si="29"/>
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="C224" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-45</v>
+        <v>23-16</v>
       </c>
       <c r="L224" s="6"/>
       <c r="M224" s="6"/>
@@ -8391,15 +8429,15 @@
     <row r="225" spans="1:13" ht="15">
       <c r="A225">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B225">
         <f t="shared" si="29"/>
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="C225" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-46</v>
+        <v>23-17</v>
       </c>
       <c r="L225" s="6"/>
       <c r="M225" s="6"/>
@@ -8407,15 +8445,15 @@
     <row r="226" spans="1:13" ht="15">
       <c r="A226">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B226">
         <f t="shared" si="29"/>
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="C226" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-47</v>
+        <v>23-18</v>
       </c>
       <c r="L226" s="6"/>
       <c r="M226" s="6"/>
@@ -8423,15 +8461,15 @@
     <row r="227" spans="1:13" ht="15">
       <c r="A227">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B227">
         <f t="shared" si="29"/>
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C227" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-48</v>
+        <v>23-19</v>
       </c>
       <c r="L227" s="6"/>
       <c r="M227" s="6"/>
@@ -8439,15 +8477,15 @@
     <row r="228" spans="1:13" ht="15">
       <c r="A228">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B228">
         <f t="shared" si="29"/>
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="C228" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-49</v>
+        <v>23-20</v>
       </c>
       <c r="L228" s="6"/>
       <c r="M228" s="6"/>
@@ -8455,15 +8493,15 @@
     <row r="229" spans="1:13" ht="15">
       <c r="A229">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B229">
         <f t="shared" si="29"/>
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="C229" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-50</v>
+        <v>23-21</v>
       </c>
       <c r="L229" s="6"/>
       <c r="M229" s="6"/>
@@ -8471,15 +8509,15 @@
     <row r="230" spans="1:13" ht="15">
       <c r="A230">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B230">
         <f t="shared" si="29"/>
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C230" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-51</v>
+        <v>23-22</v>
       </c>
       <c r="L230" s="6"/>
       <c r="M230" s="6"/>
@@ -8487,15 +8525,15 @@
     <row r="231" spans="1:13" ht="15">
       <c r="A231">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B231">
         <f t="shared" si="29"/>
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="C231" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-52</v>
+        <v>23-23</v>
       </c>
       <c r="L231" s="6"/>
       <c r="M231" s="6"/>
@@ -8503,15 +8541,15 @@
     <row r="232" spans="1:13" ht="15">
       <c r="A232">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B232">
         <f t="shared" si="29"/>
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C232" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-53</v>
+        <v>23-24</v>
       </c>
       <c r="L232" s="6"/>
       <c r="M232" s="6"/>
@@ -8519,15 +8557,15 @@
     <row r="233" spans="1:13" ht="15">
       <c r="A233">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B233">
         <f t="shared" si="29"/>
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="C233" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-54</v>
+        <v>23-25</v>
       </c>
       <c r="L233" s="6"/>
       <c r="M233" s="6"/>
@@ -8535,15 +8573,15 @@
     <row r="234" spans="1:13" ht="15">
       <c r="A234">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B234">
         <f t="shared" si="29"/>
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="C234" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-55</v>
+        <v>23-26</v>
       </c>
       <c r="L234" s="6"/>
       <c r="M234" s="6"/>
@@ -8551,15 +8589,15 @@
     <row r="235" spans="1:13" ht="15">
       <c r="A235">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B235">
         <f t="shared" si="29"/>
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C235" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-56</v>
+        <v>23-27</v>
       </c>
       <c r="L235" s="6"/>
       <c r="M235" s="6"/>
@@ -8567,15 +8605,15 @@
     <row r="236" spans="1:13" ht="15">
       <c r="A236">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B236">
         <f t="shared" si="29"/>
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="C236" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-57</v>
+        <v>23-28</v>
       </c>
       <c r="L236" s="6"/>
       <c r="M236" s="6"/>
@@ -8583,15 +8621,15 @@
     <row r="237" spans="1:13" ht="15">
       <c r="A237">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B237">
         <f t="shared" si="29"/>
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="C237" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-58</v>
+        <v>23-29</v>
       </c>
       <c r="L237" s="6"/>
       <c r="M237" s="6"/>
@@ -8599,15 +8637,15 @@
     <row r="238" spans="1:13" ht="15">
       <c r="A238">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B238">
         <f t="shared" si="29"/>
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C238" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-59</v>
+        <v>23-30</v>
       </c>
       <c r="L238" s="6"/>
       <c r="M238" s="6"/>
@@ -8615,15 +8653,15 @@
     <row r="239" spans="1:13" ht="15">
       <c r="A239">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B239">
         <f t="shared" si="29"/>
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C239" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-60</v>
+        <v>23-31</v>
       </c>
       <c r="L239" s="6"/>
       <c r="M239" s="6"/>
@@ -8631,15 +8669,15 @@
     <row r="240" spans="1:13" ht="15">
       <c r="A240">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B240">
         <f t="shared" si="29"/>
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="C240" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-61</v>
+        <v>23-32</v>
       </c>
       <c r="L240" s="6"/>
       <c r="M240" s="6"/>
@@ -8647,15 +8685,15 @@
     <row r="241" spans="1:13" ht="15">
       <c r="A241">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B241">
         <f t="shared" si="29"/>
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="C241" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-62</v>
+        <v>23-33</v>
       </c>
       <c r="L241" s="6"/>
       <c r="M241" s="6"/>
@@ -8663,15 +8701,15 @@
     <row r="242" spans="1:13" ht="15">
       <c r="A242">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B242">
         <f t="shared" si="29"/>
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="C242" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-63</v>
+        <v>23-34</v>
       </c>
       <c r="L242" s="6"/>
       <c r="M242" s="6"/>
@@ -8679,15 +8717,15 @@
     <row r="243" spans="1:13" ht="15">
       <c r="A243">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B243">
         <f t="shared" si="29"/>
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="C243" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-64</v>
+        <v>23-35</v>
       </c>
       <c r="L243" s="6"/>
       <c r="M243" s="6"/>
@@ -8695,15 +8733,15 @@
     <row r="244" spans="1:13" ht="15">
       <c r="A244">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B244">
         <f t="shared" si="29"/>
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="C244" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-65</v>
+        <v>23-36</v>
       </c>
       <c r="L244" s="6"/>
       <c r="M244" s="6"/>
@@ -8711,15 +8749,15 @@
     <row r="245" spans="1:13" ht="15">
       <c r="A245">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B245">
         <f t="shared" si="29"/>
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C245" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-66</v>
+        <v>23-37</v>
       </c>
       <c r="L245" s="6"/>
       <c r="M245" s="6"/>
@@ -8727,15 +8765,15 @@
     <row r="246" spans="1:13" ht="15">
       <c r="A246">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B246">
         <f t="shared" si="29"/>
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="C246" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-67</v>
+        <v>23-38</v>
       </c>
       <c r="L246" s="6"/>
       <c r="M246" s="6"/>
@@ -8743,15 +8781,15 @@
     <row r="247" spans="1:13" ht="15">
       <c r="A247">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B247">
         <f t="shared" si="29"/>
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C247" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-68</v>
+        <v>23-39</v>
       </c>
       <c r="L247" s="6"/>
       <c r="M247" s="6"/>
@@ -8759,15 +8797,15 @@
     <row r="248" spans="1:13" ht="15">
       <c r="A248">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B248">
         <f t="shared" si="29"/>
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="C248" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-69</v>
+        <v>23-40</v>
       </c>
       <c r="L248" s="6"/>
       <c r="M248" s="6"/>
@@ -8775,15 +8813,15 @@
     <row r="249" spans="1:13" ht="15">
       <c r="A249">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B249">
         <f t="shared" si="29"/>
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="C249" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-70</v>
+        <v>23-41</v>
       </c>
       <c r="L249" s="6"/>
       <c r="M249" s="6"/>
@@ -8791,15 +8829,15 @@
     <row r="250" spans="1:13" ht="15">
       <c r="A250">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B250">
         <f t="shared" si="29"/>
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="C250" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-71</v>
+        <v>23-42</v>
       </c>
       <c r="L250" s="6"/>
       <c r="M250" s="6"/>
@@ -8807,15 +8845,15 @@
     <row r="251" spans="1:13" ht="15">
       <c r="A251">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B251">
         <f t="shared" si="29"/>
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="C251" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-72</v>
+        <v>23-43</v>
       </c>
       <c r="L251" s="6"/>
       <c r="M251" s="6"/>
@@ -8823,15 +8861,15 @@
     <row r="252" spans="1:13" ht="15">
       <c r="A252">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B252">
         <f t="shared" si="29"/>
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="C252" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-73</v>
+        <v>23-44</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
@@ -8839,15 +8877,15 @@
     <row r="253" spans="1:13" ht="15">
       <c r="A253">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B253">
         <f t="shared" si="29"/>
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="C253" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-74</v>
+        <v>23-45</v>
       </c>
       <c r="L253" s="6"/>
       <c r="M253" s="6"/>
@@ -8855,15 +8893,15 @@
     <row r="254" spans="1:13" ht="15">
       <c r="A254">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B254">
         <f t="shared" si="29"/>
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C254" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-75</v>
+        <v>23-46</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
@@ -8871,15 +8909,15 @@
     <row r="255" spans="1:13" ht="15">
       <c r="A255">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B255">
         <f t="shared" si="29"/>
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="C255" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-76</v>
+        <v>23-47</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
@@ -8887,15 +8925,15 @@
     <row r="256" spans="1:13" ht="15">
       <c r="A256">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B256">
         <f t="shared" si="29"/>
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="C256" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-77</v>
+        <v>23-48</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
@@ -8903,15 +8941,15 @@
     <row r="257" spans="1:13" ht="15">
       <c r="A257">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B257">
         <f t="shared" si="29"/>
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="C257" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-78</v>
+        <v>23-49</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
@@ -8919,15 +8957,15 @@
     <row r="258" spans="1:13" ht="15">
       <c r="A258">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B258">
         <f t="shared" si="29"/>
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="C258" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-79</v>
+        <v>23-50</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
@@ -8935,15 +8973,15 @@
     <row r="259" spans="1:13" ht="15">
       <c r="A259">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B259">
         <f t="shared" si="29"/>
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="C259" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-80</v>
+        <v>23-51</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
@@ -8951,15 +8989,15 @@
     <row r="260" spans="1:13" ht="15">
       <c r="A260">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B260">
         <f t="shared" si="29"/>
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C260" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-81</v>
+        <v>23-52</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
@@ -8967,15 +9005,15 @@
     <row r="261" spans="1:13" ht="15">
       <c r="A261">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B261">
         <f t="shared" si="29"/>
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="C261" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-82</v>
+        <v>23-53</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
@@ -8983,15 +9021,15 @@
     <row r="262" spans="1:13" ht="15">
       <c r="A262">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B262">
         <f t="shared" si="29"/>
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="C262" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-83</v>
+        <v>23-54</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
@@ -8999,15 +9037,15 @@
     <row r="263" spans="1:13" ht="15">
       <c r="A263">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B263">
         <f t="shared" si="29"/>
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="C263" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-84</v>
+        <v>23-55</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
@@ -9015,15 +9053,15 @@
     <row r="264" spans="1:13" ht="15">
       <c r="A264">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B264">
         <f t="shared" si="29"/>
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="C264" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-85</v>
+        <v>23-56</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
@@ -9031,15 +9069,15 @@
     <row r="265" spans="1:13" ht="15">
       <c r="A265">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B265">
         <f t="shared" si="29"/>
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C265" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-86</v>
+        <v>23-57</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
@@ -9047,15 +9085,15 @@
     <row r="266" spans="1:13" ht="15">
       <c r="A266">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B266">
         <f t="shared" si="29"/>
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="C266" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-87</v>
+        <v>23-58</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
@@ -9063,15 +9101,15 @@
     <row r="267" spans="1:13" ht="15">
       <c r="A267">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B267">
         <f t="shared" si="29"/>
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="C267" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-88</v>
+        <v>23-59</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
@@ -9079,15 +9117,15 @@
     <row r="268" spans="1:13" ht="15">
       <c r="A268">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B268">
         <f t="shared" si="29"/>
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="C268" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-89</v>
+        <v>23-60</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
@@ -9095,15 +9133,15 @@
     <row r="269" spans="1:13" ht="15">
       <c r="A269">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B269">
         <f t="shared" si="29"/>
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="C269" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-90</v>
+        <v>23-61</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
@@ -9111,15 +9149,15 @@
     <row r="270" spans="1:13" ht="15">
       <c r="A270">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B270">
         <f t="shared" si="29"/>
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="C270" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-91</v>
+        <v>23-62</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
@@ -9127,15 +9165,15 @@
     <row r="271" spans="1:13" ht="15">
       <c r="A271">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B271">
         <f t="shared" si="29"/>
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="C271" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-92</v>
+        <v>23-63</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
@@ -9143,15 +9181,15 @@
     <row r="272" spans="1:13" ht="15">
       <c r="A272">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B272">
         <f t="shared" si="29"/>
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="C272" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-93</v>
+        <v>23-64</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
@@ -9159,15 +9197,15 @@
     <row r="273" spans="1:13" ht="15">
       <c r="A273">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B273">
         <f t="shared" si="29"/>
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="C273" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-94</v>
+        <v>23-65</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
@@ -9175,15 +9213,15 @@
     <row r="274" spans="1:13" ht="15">
       <c r="A274">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B274">
         <f t="shared" si="29"/>
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="C274" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-95</v>
+        <v>23-66</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
@@ -9191,15 +9229,15 @@
     <row r="275" spans="1:13" ht="15">
       <c r="A275">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B275">
         <f t="shared" si="29"/>
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C275" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-96</v>
+        <v>23-67</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
@@ -9207,15 +9245,15 @@
     <row r="276" spans="1:13" ht="15">
       <c r="A276">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B276">
         <f t="shared" si="29"/>
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="C276" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-97</v>
+        <v>23-68</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
@@ -9223,15 +9261,15 @@
     <row r="277" spans="1:13" ht="15">
       <c r="A277">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B277">
         <f t="shared" si="29"/>
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="C277" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-98</v>
+        <v>23-69</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
@@ -9239,15 +9277,15 @@
     <row r="278" spans="1:13" ht="15">
       <c r="A278">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B278">
         <f t="shared" si="29"/>
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="C278" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-99</v>
+        <v>23-70</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
@@ -9255,15 +9293,15 @@
     <row r="279" spans="1:13" ht="15">
       <c r="A279">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B279">
         <f t="shared" si="29"/>
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="C279" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>22-100</v>
+        <v>23-71</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
@@ -9271,15 +9309,15 @@
     <row r="280" spans="1:13" ht="15">
       <c r="A280">
         <f t="shared" si="31"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B280">
         <f t="shared" ref="B280:B343" si="32">IF(A280=A279,B279+1,1)</f>
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="C280" s="3" t="str">
         <f t="shared" ref="C280:C343" si="33">CONCATENATE(A280,"-",B280)</f>
-        <v>22-101</v>
+        <v>23-72</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
@@ -9287,15 +9325,15 @@
     <row r="281" spans="1:13" ht="15">
       <c r="A281">
         <f t="shared" ref="A281:A344" si="34">A280</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B281">
         <f t="shared" si="32"/>
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C281" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-102</v>
+        <v>23-73</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
@@ -9303,15 +9341,15 @@
     <row r="282" spans="1:13" ht="15">
       <c r="A282">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B282">
         <f t="shared" si="32"/>
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="C282" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-103</v>
+        <v>23-74</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
@@ -9319,15 +9357,15 @@
     <row r="283" spans="1:13" ht="15">
       <c r="A283">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B283">
         <f t="shared" si="32"/>
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C283" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-104</v>
+        <v>23-75</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
@@ -9335,15 +9373,15 @@
     <row r="284" spans="1:13" ht="15">
       <c r="A284">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B284">
         <f t="shared" si="32"/>
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="C284" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-105</v>
+        <v>23-76</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
@@ -9351,15 +9389,15 @@
     <row r="285" spans="1:13" ht="15">
       <c r="A285">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B285">
         <f t="shared" si="32"/>
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="C285" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-106</v>
+        <v>23-77</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
@@ -9367,15 +9405,15 @@
     <row r="286" spans="1:13" ht="15">
       <c r="A286">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B286">
         <f t="shared" si="32"/>
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="C286" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-107</v>
+        <v>23-78</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
@@ -9383,15 +9421,15 @@
     <row r="287" spans="1:13" ht="15">
       <c r="A287">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B287">
         <f t="shared" si="32"/>
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="C287" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-108</v>
+        <v>23-79</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
@@ -9399,15 +9437,15 @@
     <row r="288" spans="1:13" ht="15">
       <c r="A288">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B288">
         <f t="shared" si="32"/>
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="C288" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-109</v>
+        <v>23-80</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
@@ -9415,15 +9453,15 @@
     <row r="289" spans="1:13" ht="15">
       <c r="A289">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B289">
         <f t="shared" si="32"/>
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="C289" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-110</v>
+        <v>23-81</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
@@ -9431,15 +9469,15 @@
     <row r="290" spans="1:13" ht="15">
       <c r="A290">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B290">
         <f t="shared" si="32"/>
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="C290" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-111</v>
+        <v>23-82</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
@@ -9447,15 +9485,15 @@
     <row r="291" spans="1:13" ht="15">
       <c r="A291">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B291">
         <f t="shared" si="32"/>
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="C291" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-112</v>
+        <v>23-83</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
@@ -9463,15 +9501,15 @@
     <row r="292" spans="1:13" ht="15">
       <c r="A292">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B292">
         <f t="shared" si="32"/>
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="C292" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-113</v>
+        <v>23-84</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
@@ -9479,15 +9517,15 @@
     <row r="293" spans="1:13" ht="15">
       <c r="A293">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B293">
         <f t="shared" si="32"/>
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="C293" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-114</v>
+        <v>23-85</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
@@ -9495,15 +9533,15 @@
     <row r="294" spans="1:13" ht="15">
       <c r="A294">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B294">
         <f t="shared" si="32"/>
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="C294" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-115</v>
+        <v>23-86</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
@@ -9511,15 +9549,15 @@
     <row r="295" spans="1:13" ht="15">
       <c r="A295">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B295">
         <f t="shared" si="32"/>
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="C295" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-116</v>
+        <v>23-87</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
@@ -9527,15 +9565,15 @@
     <row r="296" spans="1:13" ht="15">
       <c r="A296">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B296">
         <f t="shared" si="32"/>
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="C296" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-117</v>
+        <v>23-88</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
@@ -9543,15 +9581,15 @@
     <row r="297" spans="1:13" ht="15">
       <c r="A297">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B297">
         <f t="shared" si="32"/>
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C297" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-118</v>
+        <v>23-89</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
@@ -9559,15 +9597,15 @@
     <row r="298" spans="1:13" ht="15">
       <c r="A298">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B298">
         <f t="shared" si="32"/>
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="C298" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-119</v>
+        <v>23-90</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
@@ -9575,15 +9613,15 @@
     <row r="299" spans="1:13" ht="15">
       <c r="A299">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B299">
         <f t="shared" si="32"/>
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C299" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-120</v>
+        <v>23-91</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
@@ -9591,15 +9629,15 @@
     <row r="300" spans="1:13" ht="15">
       <c r="A300">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B300">
         <f t="shared" si="32"/>
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="C300" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-121</v>
+        <v>23-92</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
@@ -9607,15 +9645,15 @@
     <row r="301" spans="1:13" ht="15">
       <c r="A301">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B301">
         <f t="shared" si="32"/>
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="C301" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-122</v>
+        <v>23-93</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
@@ -9623,15 +9661,15 @@
     <row r="302" spans="1:13" ht="15">
       <c r="A302">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B302">
         <f t="shared" si="32"/>
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="C302" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-123</v>
+        <v>23-94</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
@@ -9639,15 +9677,15 @@
     <row r="303" spans="1:13" ht="15">
       <c r="A303">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B303">
         <f t="shared" si="32"/>
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C303" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-124</v>
+        <v>23-95</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
@@ -9655,15 +9693,15 @@
     <row r="304" spans="1:13" ht="15">
       <c r="A304">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B304">
         <f t="shared" si="32"/>
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="C304" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-125</v>
+        <v>23-96</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
@@ -9671,15 +9709,15 @@
     <row r="305" spans="1:13" ht="15">
       <c r="A305">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B305">
         <f t="shared" si="32"/>
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="C305" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-126</v>
+        <v>23-97</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
@@ -9687,15 +9725,15 @@
     <row r="306" spans="1:13" ht="15">
       <c r="A306">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B306">
         <f t="shared" si="32"/>
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="C306" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-127</v>
+        <v>23-98</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
@@ -9703,15 +9741,15 @@
     <row r="307" spans="1:13" ht="15">
       <c r="A307">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B307">
         <f t="shared" si="32"/>
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="C307" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-128</v>
+        <v>23-99</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
@@ -9719,15 +9757,15 @@
     <row r="308" spans="1:13" ht="15">
       <c r="A308">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B308">
         <f t="shared" si="32"/>
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="C308" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-129</v>
+        <v>23-100</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
@@ -9735,15 +9773,15 @@
     <row r="309" spans="1:13" ht="15">
       <c r="A309">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B309">
         <f t="shared" si="32"/>
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="C309" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-130</v>
+        <v>23-101</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
@@ -9751,15 +9789,15 @@
     <row r="310" spans="1:13" ht="15">
       <c r="A310">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B310">
         <f t="shared" si="32"/>
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C310" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-131</v>
+        <v>23-102</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
@@ -9767,15 +9805,15 @@
     <row r="311" spans="1:13" ht="15">
       <c r="A311">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B311">
         <f t="shared" si="32"/>
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="C311" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-132</v>
+        <v>23-103</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
@@ -9783,15 +9821,15 @@
     <row r="312" spans="1:13" ht="15">
       <c r="A312">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B312">
         <f t="shared" si="32"/>
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="C312" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-133</v>
+        <v>23-104</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
@@ -9799,15 +9837,15 @@
     <row r="313" spans="1:13" ht="15">
       <c r="A313">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B313">
         <f t="shared" si="32"/>
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C313" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-134</v>
+        <v>23-105</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
@@ -9815,15 +9853,15 @@
     <row r="314" spans="1:13" ht="15">
       <c r="A314">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B314">
         <f t="shared" si="32"/>
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="C314" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-135</v>
+        <v>23-106</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
@@ -9831,15 +9869,15 @@
     <row r="315" spans="1:13" ht="15">
       <c r="A315">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B315">
         <f t="shared" si="32"/>
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="C315" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-136</v>
+        <v>23-107</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
@@ -9847,15 +9885,15 @@
     <row r="316" spans="1:13" ht="15">
       <c r="A316">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B316">
         <f t="shared" si="32"/>
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="C316" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-137</v>
+        <v>23-108</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
@@ -9863,15 +9901,15 @@
     <row r="317" spans="1:13" ht="15">
       <c r="A317">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B317">
         <f t="shared" si="32"/>
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="C317" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-138</v>
+        <v>23-109</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
@@ -9879,15 +9917,15 @@
     <row r="318" spans="1:13" ht="15">
       <c r="A318">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B318">
         <f t="shared" si="32"/>
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="C318" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-139</v>
+        <v>23-110</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
@@ -9895,15 +9933,15 @@
     <row r="319" spans="1:13" ht="15">
       <c r="A319">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B319">
         <f t="shared" si="32"/>
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="C319" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-140</v>
+        <v>23-111</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
@@ -9911,15 +9949,15 @@
     <row r="320" spans="1:13" ht="15">
       <c r="A320">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B320">
         <f t="shared" si="32"/>
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="C320" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-141</v>
+        <v>23-112</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
@@ -9927,15 +9965,15 @@
     <row r="321" spans="1:13" ht="15">
       <c r="A321">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B321">
         <f t="shared" si="32"/>
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="C321" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-142</v>
+        <v>23-113</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
@@ -9943,15 +9981,15 @@
     <row r="322" spans="1:13" ht="15">
       <c r="A322">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B322">
         <f t="shared" si="32"/>
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="C322" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-143</v>
+        <v>23-114</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
@@ -9959,15 +9997,15 @@
     <row r="323" spans="1:13" ht="15">
       <c r="A323">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B323">
         <f t="shared" si="32"/>
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="C323" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-144</v>
+        <v>23-115</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
@@ -9975,15 +10013,15 @@
     <row r="324" spans="1:13" ht="15">
       <c r="A324">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B324">
         <f t="shared" si="32"/>
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="C324" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-145</v>
+        <v>23-116</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
@@ -9991,15 +10029,15 @@
     <row r="325" spans="1:13" ht="15">
       <c r="A325">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B325">
         <f t="shared" si="32"/>
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="C325" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-146</v>
+        <v>23-117</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
@@ -10007,15 +10045,15 @@
     <row r="326" spans="1:13" ht="15">
       <c r="A326">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B326">
         <f t="shared" si="32"/>
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="C326" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-147</v>
+        <v>23-118</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
@@ -10023,15 +10061,15 @@
     <row r="327" spans="1:13" ht="15">
       <c r="A327">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B327">
         <f t="shared" si="32"/>
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="C327" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-148</v>
+        <v>23-119</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
@@ -10039,15 +10077,15 @@
     <row r="328" spans="1:13" ht="15">
       <c r="A328">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B328">
         <f t="shared" si="32"/>
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="C328" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-149</v>
+        <v>23-120</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
@@ -10055,15 +10093,15 @@
     <row r="329" spans="1:13" ht="15">
       <c r="A329">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B329">
         <f t="shared" si="32"/>
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="C329" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-150</v>
+        <v>23-121</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
@@ -10071,15 +10109,15 @@
     <row r="330" spans="1:13" ht="15">
       <c r="A330">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B330">
         <f t="shared" si="32"/>
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="C330" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-151</v>
+        <v>23-122</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
@@ -10087,15 +10125,15 @@
     <row r="331" spans="1:13" ht="15">
       <c r="A331">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B331">
         <f t="shared" si="32"/>
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="C331" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-152</v>
+        <v>23-123</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
@@ -10103,15 +10141,15 @@
     <row r="332" spans="1:13" ht="15">
       <c r="A332">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B332">
         <f t="shared" si="32"/>
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="C332" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-153</v>
+        <v>23-124</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
@@ -10119,15 +10157,15 @@
     <row r="333" spans="1:13" ht="15">
       <c r="A333">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B333">
         <f t="shared" si="32"/>
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="C333" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-154</v>
+        <v>23-125</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
@@ -10135,15 +10173,15 @@
     <row r="334" spans="1:13" ht="15">
       <c r="A334">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B334">
         <f t="shared" si="32"/>
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="C334" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-155</v>
+        <v>23-126</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
@@ -10151,15 +10189,15 @@
     <row r="335" spans="1:13" ht="15">
       <c r="A335">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B335">
         <f t="shared" si="32"/>
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="C335" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-156</v>
+        <v>23-127</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
@@ -10167,15 +10205,15 @@
     <row r="336" spans="1:13" ht="15">
       <c r="A336">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B336">
         <f t="shared" si="32"/>
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="C336" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-157</v>
+        <v>23-128</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
@@ -10183,15 +10221,15 @@
     <row r="337" spans="1:13" ht="15">
       <c r="A337">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B337">
         <f t="shared" si="32"/>
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="C337" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-158</v>
+        <v>23-129</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
@@ -10199,15 +10237,15 @@
     <row r="338" spans="1:13" ht="15">
       <c r="A338">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B338">
         <f t="shared" si="32"/>
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="C338" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-159</v>
+        <v>23-130</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
@@ -10215,15 +10253,15 @@
     <row r="339" spans="1:13" ht="15">
       <c r="A339">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B339">
         <f t="shared" si="32"/>
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="C339" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-160</v>
+        <v>23-131</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
@@ -10231,15 +10269,15 @@
     <row r="340" spans="1:13" ht="15">
       <c r="A340">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B340">
         <f t="shared" si="32"/>
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C340" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-161</v>
+        <v>23-132</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
@@ -10247,15 +10285,15 @@
     <row r="341" spans="1:13" ht="15">
       <c r="A341">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B341">
         <f t="shared" si="32"/>
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="C341" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-162</v>
+        <v>23-133</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
@@ -10263,15 +10301,15 @@
     <row r="342" spans="1:13" ht="15">
       <c r="A342">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B342">
         <f t="shared" si="32"/>
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C342" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-163</v>
+        <v>23-134</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
@@ -10279,15 +10317,15 @@
     <row r="343" spans="1:13" ht="15">
       <c r="A343">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B343">
         <f t="shared" si="32"/>
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="C343" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>22-164</v>
+        <v>23-135</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
@@ -10295,15 +10333,15 @@
     <row r="344" spans="1:13" ht="15">
       <c r="A344">
         <f t="shared" si="34"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B344">
         <f t="shared" ref="B344:B365" si="35">IF(A344=A343,B343+1,1)</f>
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="C344" s="3" t="str">
         <f t="shared" ref="C344:C365" si="36">CONCATENATE(A344,"-",B344)</f>
-        <v>22-165</v>
+        <v>23-136</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
@@ -10311,15 +10349,15 @@
     <row r="345" spans="1:13" ht="15">
       <c r="A345">
         <f t="shared" ref="A345:A365" si="37">A344</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B345">
         <f t="shared" si="35"/>
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="C345" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-166</v>
+        <v>23-137</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
@@ -10327,15 +10365,15 @@
     <row r="346" spans="1:13" ht="15">
       <c r="A346">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B346">
         <f t="shared" si="35"/>
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="C346" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-167</v>
+        <v>23-138</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
@@ -10343,15 +10381,15 @@
     <row r="347" spans="1:13" ht="15">
       <c r="A347">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B347">
         <f t="shared" si="35"/>
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="C347" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-168</v>
+        <v>23-139</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
@@ -10359,15 +10397,15 @@
     <row r="348" spans="1:13" ht="15">
       <c r="A348">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B348">
         <f t="shared" si="35"/>
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="C348" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-169</v>
+        <v>23-140</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
@@ -10375,15 +10413,15 @@
     <row r="349" spans="1:13" ht="15">
       <c r="A349">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B349">
         <f t="shared" si="35"/>
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="C349" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-170</v>
+        <v>23-141</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
@@ -10391,15 +10429,15 @@
     <row r="350" spans="1:13" ht="15">
       <c r="A350">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B350">
         <f t="shared" si="35"/>
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="C350" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-171</v>
+        <v>23-142</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
@@ -10407,15 +10445,15 @@
     <row r="351" spans="1:13" ht="15">
       <c r="A351">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B351">
         <f t="shared" si="35"/>
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="C351" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-172</v>
+        <v>23-143</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
@@ -10423,15 +10461,15 @@
     <row r="352" spans="1:13" ht="15">
       <c r="A352">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B352">
         <f t="shared" si="35"/>
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="C352" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-173</v>
+        <v>23-144</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
@@ -10439,15 +10477,15 @@
     <row r="353" spans="1:13" ht="15">
       <c r="A353">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B353">
         <f t="shared" si="35"/>
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="C353" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-174</v>
+        <v>23-145</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
@@ -10455,15 +10493,15 @@
     <row r="354" spans="1:13" ht="15">
       <c r="A354">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B354">
         <f t="shared" si="35"/>
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="C354" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-175</v>
+        <v>23-146</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
@@ -10471,15 +10509,15 @@
     <row r="355" spans="1:13" ht="15">
       <c r="A355">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B355">
         <f t="shared" si="35"/>
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="C355" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-176</v>
+        <v>23-147</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
@@ -10487,15 +10525,15 @@
     <row r="356" spans="1:13" ht="15">
       <c r="A356">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B356">
         <f t="shared" si="35"/>
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="C356" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-177</v>
+        <v>23-148</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
@@ -10503,15 +10541,15 @@
     <row r="357" spans="1:13" ht="15">
       <c r="A357">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B357">
         <f t="shared" si="35"/>
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="C357" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-178</v>
+        <v>23-149</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
@@ -10519,15 +10557,15 @@
     <row r="358" spans="1:13" ht="15">
       <c r="A358">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B358">
         <f t="shared" si="35"/>
-        <v>179</v>
+        <v>150</v>
       </c>
       <c r="C358" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-179</v>
+        <v>23-150</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
@@ -10535,15 +10573,15 @@
     <row r="359" spans="1:13" ht="15">
       <c r="A359">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B359">
         <f t="shared" si="35"/>
-        <v>180</v>
+        <v>151</v>
       </c>
       <c r="C359" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-180</v>
+        <v>23-151</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
@@ -10551,15 +10589,15 @@
     <row r="360" spans="1:13" ht="15">
       <c r="A360">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B360">
         <f t="shared" si="35"/>
-        <v>181</v>
+        <v>152</v>
       </c>
       <c r="C360" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-181</v>
+        <v>23-152</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
@@ -10567,15 +10605,15 @@
     <row r="361" spans="1:13" ht="15">
       <c r="A361">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B361">
         <f t="shared" si="35"/>
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="C361" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-182</v>
+        <v>23-153</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
@@ -10583,15 +10621,15 @@
     <row r="362" spans="1:13" ht="15">
       <c r="A362">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B362">
         <f t="shared" si="35"/>
-        <v>183</v>
+        <v>154</v>
       </c>
       <c r="C362" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-183</v>
+        <v>23-154</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
@@ -10599,15 +10637,15 @@
     <row r="363" spans="1:13" ht="15">
       <c r="A363">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B363">
         <f t="shared" si="35"/>
-        <v>184</v>
+        <v>155</v>
       </c>
       <c r="C363" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-184</v>
+        <v>23-155</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
@@ -10615,15 +10653,15 @@
     <row r="364" spans="1:13" ht="15">
       <c r="A364">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B364">
         <f t="shared" si="35"/>
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="C364" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-185</v>
+        <v>23-156</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
@@ -10631,15 +10669,15 @@
     <row r="365" spans="1:13" ht="15">
       <c r="A365">
         <f t="shared" si="37"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B365">
         <f t="shared" si="35"/>
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="C365" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>22-186</v>
+        <v>23-157</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
@@ -13397,17 +13435,17 @@
     <mergeCell ref="L174:L177"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K185">
-    <cfRule type="containsBlanks" dxfId="56" priority="58">
+    <cfRule type="containsBlanks" dxfId="53" priority="58">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K185">
-    <cfRule type="containsText" dxfId="55" priority="59" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K185">
-    <cfRule type="containsText" dxfId="54" priority="60" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="51" priority="60" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added manual tests for #1667
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="277">
   <si>
     <t>Test Number</t>
   </si>
@@ -821,6 +821,33 @@
   </si>
   <si>
     <t>Contents of Experiment Setup sub-tabs are enabled when instrument is NOT running</t>
+  </si>
+  <si>
+    <t>Config Version Control</t>
+  </si>
+  <si>
+    <t>New configurations get added to the local repository if on a branch named after your system</t>
+  </si>
+  <si>
+    <t>Config changes get committed to the local repository if on a branch named after your system</t>
+  </si>
+  <si>
+    <t>Config changes get pushed to remote repository if on a branch named after your system</t>
+  </si>
+  <si>
+    <t>Config changes do not get committed if on a branch starting with ND that is not your system name</t>
+  </si>
+  <si>
+    <t>Configs starting with rcptt_ are not added to a repo</t>
+  </si>
+  <si>
+    <t>Read-only access</t>
+  </si>
+  <si>
+    <t>Current configuration can be viewed on instruments where you do not have write access</t>
+  </si>
+  <si>
+    <t>Right-click edit block does not work on read-only instruments</t>
   </si>
 </sst>
 </file>
@@ -890,7 +917,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -966,15 +993,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -988,19 +1006,21 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1049,9 +1069,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1063,11 +1080,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1083,19 +1096,113 @@
     <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="60">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2152,8 +2259,8 @@
   <dimension ref="A1:N1056"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
+      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I220" sqref="I220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3346,35 +3453,35 @@
       <c r="L41" s="8"/>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="1:13" s="32" customFormat="1" ht="45">
-      <c r="A42" s="32">
+    <row r="42" spans="1:13" s="29" customFormat="1" ht="45">
+      <c r="A42" s="29">
         <f>A40</f>
         <v>6</v>
       </c>
-      <c r="B42" s="32">
+      <c r="B42" s="29">
         <f>IF(A42=A41,B41+1,1)</f>
         <v>14</v>
       </c>
-      <c r="C42" s="31" t="str">
+      <c r="C42" s="28" t="str">
         <f t="shared" si="1"/>
         <v>6-14</v>
       </c>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34" t="s">
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="I42" s="35" t="s">
+      <c r="I42" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="J42" s="35"/>
-      <c r="K42" s="34"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="36"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="33"/>
     </row>
     <row r="43" spans="1:13" ht="45">
       <c r="A43">
@@ -3395,7 +3502,7 @@
       <c r="G43" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="31" t="s">
         <v>46</v>
       </c>
       <c r="I43" s="1" t="s">
@@ -3425,7 +3532,7 @@
       <c r="G44" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H44" s="34" t="s">
+      <c r="H44" s="31" t="s">
         <v>46</v>
       </c>
       <c r="I44" s="1" t="s">
@@ -3455,7 +3562,7 @@
       <c r="G45" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H45" s="34" t="s">
+      <c r="H45" s="31" t="s">
         <v>46</v>
       </c>
       <c r="I45" s="1" t="s">
@@ -3485,7 +3592,7 @@
       <c r="G46" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H46" s="34" t="s">
+      <c r="H46" s="31" t="s">
         <v>46</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -3515,7 +3622,7 @@
       <c r="G47" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H47" s="34" t="s">
+      <c r="H47" s="31" t="s">
         <v>46</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -3535,7 +3642,7 @@
         <f>IF(A48=A47,B47+1,1)</f>
         <v>20</v>
       </c>
-      <c r="C48" s="37" t="str">
+      <c r="C48" s="34" t="str">
         <f>CONCATENATE(A48,"-",B48)</f>
         <v>6-20</v>
       </c>
@@ -3545,7 +3652,7 @@
         <v>47</v>
       </c>
       <c r="G48" s="9"/>
-      <c r="H48" s="34" t="s">
+      <c r="H48" s="31" t="s">
         <v>46</v>
       </c>
       <c r="I48" s="8" t="s">
@@ -3577,7 +3684,7 @@
         <v>47</v>
       </c>
       <c r="G49" s="9"/>
-      <c r="H49" s="34" t="s">
+      <c r="H49" s="31" t="s">
         <v>46</v>
       </c>
       <c r="I49" s="8" t="s">
@@ -6387,7 +6494,7 @@
       <c r="H147" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="I147" s="41" t="s">
+      <c r="I147" s="35" t="s">
         <v>265</v>
       </c>
       <c r="J147" s="8"/>
@@ -7314,7 +7421,7 @@
       </c>
       <c r="J178" s="8"/>
       <c r="K178" s="7"/>
-      <c r="L178" s="38"/>
+      <c r="L178" s="40"/>
     </row>
     <row r="179" spans="1:13" ht="30">
       <c r="A179">
@@ -7343,7 +7450,7 @@
       </c>
       <c r="J179" s="8"/>
       <c r="K179" s="7"/>
-      <c r="L179" s="39"/>
+      <c r="L179" s="41"/>
       <c r="M179" s="6"/>
     </row>
     <row r="180" spans="1:13" ht="45">
@@ -7373,7 +7480,7 @@
       </c>
       <c r="J180" s="8"/>
       <c r="K180" s="7"/>
-      <c r="L180" s="39"/>
+      <c r="L180" s="41"/>
       <c r="M180" s="6"/>
     </row>
     <row r="181" spans="1:13" ht="30">
@@ -7403,7 +7510,7 @@
       </c>
       <c r="J181" s="8"/>
       <c r="K181" s="7"/>
-      <c r="L181" s="40"/>
+      <c r="L181" s="42"/>
       <c r="M181" s="6"/>
     </row>
     <row r="182" spans="1:13" ht="30">
@@ -8194,23 +8301,23 @@
       <c r="B207">
         <v>1</v>
       </c>
-      <c r="C207" s="23" t="str">
+      <c r="C207" s="22" t="str">
         <f>CONCATENATE(A207,"-",B207)</f>
         <v>22-1</v>
       </c>
-      <c r="D207" s="24"/>
-      <c r="E207" s="24"/>
-      <c r="F207" s="24"/>
-      <c r="G207" s="25"/>
-      <c r="H207" s="25" t="s">
+      <c r="D207" s="23"/>
+      <c r="E207" s="23"/>
+      <c r="F207" s="23"/>
+      <c r="G207" s="24"/>
+      <c r="H207" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="I207" s="26" t="s">
+      <c r="I207" s="25" t="s">
         <v>250</v>
       </c>
-      <c r="J207" s="24"/>
-      <c r="K207" s="24"/>
-      <c r="L207" s="27"/>
+      <c r="J207" s="23"/>
+      <c r="K207" s="21"/>
+      <c r="L207" s="26"/>
       <c r="M207" s="6"/>
     </row>
     <row r="208" spans="1:13" ht="39">
@@ -8222,23 +8329,23 @@
         <f>IF(A208=A207,B207+1,1)</f>
         <v>2</v>
       </c>
-      <c r="C208" s="23" t="str">
+      <c r="C208" s="22" t="str">
         <f t="shared" si="12"/>
         <v>22-2</v>
       </c>
-      <c r="D208" s="24"/>
-      <c r="E208" s="24"/>
-      <c r="F208" s="24"/>
-      <c r="G208" s="24"/>
-      <c r="H208" s="25" t="s">
+      <c r="D208" s="23"/>
+      <c r="E208" s="23"/>
+      <c r="F208" s="23"/>
+      <c r="G208" s="23"/>
+      <c r="H208" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="I208" s="26" t="s">
+      <c r="I208" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="J208" s="24"/>
-      <c r="K208" s="24"/>
-      <c r="L208" s="27"/>
+      <c r="J208" s="23"/>
+      <c r="K208" s="21"/>
+      <c r="L208" s="26"/>
       <c r="M208" s="6"/>
     </row>
     <row r="209" spans="1:13" ht="26.25">
@@ -8250,23 +8357,23 @@
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="C209" s="23" t="str">
+      <c r="C209" s="22" t="str">
         <f t="shared" si="12"/>
         <v>22-3</v>
       </c>
-      <c r="D209" s="24"/>
-      <c r="E209" s="24"/>
-      <c r="F209" s="24"/>
-      <c r="G209" s="24"/>
-      <c r="H209" s="25" t="s">
+      <c r="D209" s="23"/>
+      <c r="E209" s="23"/>
+      <c r="F209" s="23"/>
+      <c r="G209" s="23"/>
+      <c r="H209" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="I209" s="26" t="s">
+      <c r="I209" s="25" t="s">
         <v>253</v>
       </c>
-      <c r="J209" s="24"/>
-      <c r="K209" s="24"/>
-      <c r="L209" s="27"/>
+      <c r="J209" s="23"/>
+      <c r="K209" s="21"/>
+      <c r="L209" s="26"/>
       <c r="M209" s="6"/>
     </row>
     <row r="210" spans="1:13" ht="15">
@@ -8278,23 +8385,23 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="C210" s="23" t="str">
+      <c r="C210" s="22" t="str">
         <f t="shared" si="12"/>
         <v>22-4</v>
       </c>
-      <c r="D210" s="24"/>
-      <c r="E210" s="24"/>
-      <c r="F210" s="24"/>
-      <c r="G210" s="24"/>
-      <c r="H210" s="25" t="s">
+      <c r="D210" s="23"/>
+      <c r="E210" s="23"/>
+      <c r="F210" s="23"/>
+      <c r="G210" s="23"/>
+      <c r="H210" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="I210" s="26" t="s">
+      <c r="I210" s="25" t="s">
         <v>254</v>
       </c>
-      <c r="J210" s="24"/>
-      <c r="K210" s="24"/>
-      <c r="L210" s="27"/>
+      <c r="J210" s="23"/>
+      <c r="K210" s="21"/>
+      <c r="L210" s="26"/>
       <c r="M210" s="6"/>
     </row>
     <row r="211" spans="1:13" ht="15">
@@ -8306,23 +8413,23 @@
         <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="C211" s="23" t="str">
+      <c r="C211" s="22" t="str">
         <f t="shared" si="12"/>
         <v>22-5</v>
       </c>
-      <c r="D211" s="24"/>
-      <c r="E211" s="24"/>
-      <c r="F211" s="24"/>
-      <c r="G211" s="24"/>
-      <c r="H211" s="25" t="s">
+      <c r="D211" s="23"/>
+      <c r="E211" s="23"/>
+      <c r="F211" s="23"/>
+      <c r="G211" s="23"/>
+      <c r="H211" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="I211" s="26" t="s">
+      <c r="I211" s="25" t="s">
         <v>255</v>
       </c>
-      <c r="J211" s="24"/>
-      <c r="K211" s="24"/>
-      <c r="L211" s="27"/>
+      <c r="J211" s="23"/>
+      <c r="K211" s="21"/>
+      <c r="L211" s="26"/>
       <c r="M211" s="6"/>
     </row>
     <row r="212" spans="1:13" ht="15">
@@ -8334,26 +8441,26 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="C212" s="23" t="str">
+      <c r="C212" s="22" t="str">
         <f t="shared" si="12"/>
         <v>22-6</v>
       </c>
-      <c r="D212" s="24"/>
-      <c r="E212" s="24"/>
-      <c r="F212" s="24"/>
-      <c r="G212" s="24"/>
-      <c r="H212" s="29" t="s">
+      <c r="D212" s="37"/>
+      <c r="E212" s="37"/>
+      <c r="F212" s="37"/>
+      <c r="G212" s="37"/>
+      <c r="H212" s="27" t="s">
         <v>251</v>
       </c>
-      <c r="I212" s="26" t="s">
+      <c r="I212" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="J212" s="24"/>
-      <c r="K212" s="24"/>
-      <c r="L212" s="27"/>
+      <c r="J212" s="37"/>
+      <c r="K212" s="21"/>
+      <c r="L212" s="39"/>
       <c r="M212" s="6"/>
     </row>
-    <row r="213" spans="1:13" ht="15">
+    <row r="213" spans="1:13" ht="26.25">
       <c r="A213">
         <v>23</v>
       </c>
@@ -8361,16 +8468,28 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="C213" s="22" t="str">
+      <c r="C213" s="36" t="str">
         <f t="shared" si="12"/>
         <v>23-1</v>
       </c>
-      <c r="H213" s="30"/>
-      <c r="I213" s="28"/>
-      <c r="L213" s="6"/>
+      <c r="D213" s="23"/>
+      <c r="E213" s="23"/>
+      <c r="F213" s="23"/>
+      <c r="G213" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H213" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="I213" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="J213" s="23"/>
+      <c r="K213" s="21"/>
+      <c r="L213" s="26"/>
       <c r="M213" s="6"/>
     </row>
-    <row r="214" spans="1:13" ht="15">
+    <row r="214" spans="1:13" ht="26.25">
       <c r="A214">
         <f t="shared" si="13"/>
         <v>23</v>
@@ -8383,10 +8502,24 @@
         <f t="shared" si="12"/>
         <v>23-2</v>
       </c>
-      <c r="L214" s="6"/>
+      <c r="D214" s="23"/>
+      <c r="E214" s="23"/>
+      <c r="F214" s="23"/>
+      <c r="G214" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H214" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="I214" s="25" t="s">
+        <v>270</v>
+      </c>
+      <c r="J214" s="23"/>
+      <c r="K214" s="21"/>
+      <c r="L214" s="26"/>
       <c r="M214" s="6"/>
     </row>
-    <row r="215" spans="1:13" ht="15">
+    <row r="215" spans="1:13" ht="26.25">
       <c r="A215">
         <f t="shared" si="13"/>
         <v>23</v>
@@ -8399,10 +8532,24 @@
         <f t="shared" si="12"/>
         <v>23-3</v>
       </c>
-      <c r="L215" s="6"/>
+      <c r="D215" s="23"/>
+      <c r="E215" s="23"/>
+      <c r="F215" s="23"/>
+      <c r="G215" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H215" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="I215" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="J215" s="23"/>
+      <c r="K215" s="21"/>
+      <c r="L215" s="26"/>
       <c r="M215" s="6"/>
     </row>
-    <row r="216" spans="1:13" ht="15">
+    <row r="216" spans="1:13" ht="39">
       <c r="A216">
         <f t="shared" si="13"/>
         <v>23</v>
@@ -8415,7 +8562,21 @@
         <f t="shared" si="12"/>
         <v>23-4</v>
       </c>
-      <c r="L216" s="6"/>
+      <c r="D216" s="23"/>
+      <c r="E216" s="23"/>
+      <c r="F216" s="23"/>
+      <c r="G216" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H216" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="I216" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="J216" s="23"/>
+      <c r="K216" s="21"/>
+      <c r="L216" s="26"/>
       <c r="M216" s="6"/>
     </row>
     <row r="217" spans="1:13" ht="15">
@@ -8431,2437 +8592,2478 @@
         <f t="shared" si="12"/>
         <v>23-5</v>
       </c>
-      <c r="L217" s="6"/>
+      <c r="D217" s="23"/>
+      <c r="E217" s="23"/>
+      <c r="F217" s="23"/>
+      <c r="G217" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H217" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="I217" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="J217" s="23"/>
+      <c r="K217" s="21"/>
+      <c r="L217" s="26"/>
       <c r="M217" s="6"/>
     </row>
-    <row r="218" spans="1:13" ht="15">
+    <row r="218" spans="1:13" ht="26.25">
       <c r="A218">
-        <f t="shared" si="13"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B218">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C218" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>23-6</v>
-      </c>
-      <c r="L218" s="6"/>
+        <v>24-1</v>
+      </c>
+      <c r="D218" s="23"/>
+      <c r="E218" s="23"/>
+      <c r="F218" s="23"/>
+      <c r="G218" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H218" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="I218" s="25" t="s">
+        <v>275</v>
+      </c>
+      <c r="J218" s="23"/>
+      <c r="K218" s="21"/>
+      <c r="L218" s="26"/>
       <c r="M218" s="6"/>
     </row>
-    <row r="219" spans="1:13" ht="15">
+    <row r="219" spans="1:13" ht="26.25">
       <c r="A219">
         <f t="shared" si="13"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B219">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C219" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>23-7</v>
-      </c>
-      <c r="L219" s="6"/>
+        <f t="shared" ref="C219" si="28">CONCATENATE(A219,"-",B219)</f>
+        <v>24-2</v>
+      </c>
+      <c r="D219" s="23"/>
+      <c r="E219" s="23"/>
+      <c r="F219" s="23"/>
+      <c r="G219" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H219" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="I219" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="J219" s="23"/>
+      <c r="K219" s="21"/>
+      <c r="L219" s="26"/>
       <c r="M219" s="6"/>
     </row>
     <row r="220" spans="1:13" ht="15">
       <c r="A220">
         <f t="shared" si="13"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B220">
-        <f t="shared" ref="B220:B283" si="28">IF(A220=A219,B219+1,1)</f>
-        <v>8</v>
+        <f t="shared" ref="B220:B283" si="29">IF(A220=A219,B219+1,1)</f>
+        <v>3</v>
       </c>
       <c r="C220" s="3" t="str">
-        <f t="shared" ref="C220:C283" si="29">CONCATENATE(A220,"-",B220)</f>
-        <v>23-8</v>
+        <f t="shared" ref="C220:C283" si="30">CONCATENATE(A220,"-",B220)</f>
+        <v>24-3</v>
       </c>
       <c r="L220" s="6"/>
       <c r="M220" s="6"/>
     </row>
     <row r="221" spans="1:13" ht="15">
       <c r="A221">
-        <f t="shared" ref="A221:A284" si="30">A220</f>
-        <v>23</v>
+        <f t="shared" ref="A221:A284" si="31">A220</f>
+        <v>24</v>
       </c>
       <c r="B221">
-        <f t="shared" si="28"/>
-        <v>9</v>
+        <f t="shared" si="29"/>
+        <v>4</v>
       </c>
       <c r="C221" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-9</v>
+        <f t="shared" si="30"/>
+        <v>24-4</v>
       </c>
       <c r="L221" s="6"/>
       <c r="M221" s="6"/>
     </row>
     <row r="222" spans="1:13" ht="15">
       <c r="A222">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B222">
+        <f t="shared" si="29"/>
+        <v>5</v>
+      </c>
+      <c r="C222" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B222">
-        <f t="shared" si="28"/>
-        <v>10</v>
-      </c>
-      <c r="C222" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-10</v>
+        <v>24-5</v>
       </c>
       <c r="L222" s="6"/>
       <c r="M222" s="6"/>
     </row>
     <row r="223" spans="1:13" ht="15">
       <c r="A223">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B223">
+        <f t="shared" si="29"/>
+        <v>6</v>
+      </c>
+      <c r="C223" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B223">
-        <f t="shared" si="28"/>
-        <v>11</v>
-      </c>
-      <c r="C223" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-11</v>
+        <v>24-6</v>
       </c>
       <c r="L223" s="6"/>
       <c r="M223" s="6"/>
     </row>
     <row r="224" spans="1:13" ht="15">
       <c r="A224">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B224">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="C224" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B224">
-        <f t="shared" si="28"/>
-        <v>12</v>
-      </c>
-      <c r="C224" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-12</v>
+        <v>24-7</v>
       </c>
       <c r="L224" s="6"/>
       <c r="M224" s="6"/>
     </row>
     <row r="225" spans="1:13" ht="15">
       <c r="A225">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B225">
+        <f t="shared" si="29"/>
+        <v>8</v>
+      </c>
+      <c r="C225" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B225">
-        <f t="shared" si="28"/>
-        <v>13</v>
-      </c>
-      <c r="C225" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-13</v>
+        <v>24-8</v>
       </c>
       <c r="L225" s="6"/>
       <c r="M225" s="6"/>
     </row>
     <row r="226" spans="1:13" ht="15">
       <c r="A226">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B226">
+        <f t="shared" si="29"/>
+        <v>9</v>
+      </c>
+      <c r="C226" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B226">
-        <f t="shared" si="28"/>
-        <v>14</v>
-      </c>
-      <c r="C226" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-14</v>
+        <v>24-9</v>
       </c>
       <c r="L226" s="6"/>
       <c r="M226" s="6"/>
     </row>
     <row r="227" spans="1:13" ht="15">
       <c r="A227">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B227">
+        <f t="shared" si="29"/>
+        <v>10</v>
+      </c>
+      <c r="C227" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B227">
-        <f t="shared" si="28"/>
-        <v>15</v>
-      </c>
-      <c r="C227" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-15</v>
+        <v>24-10</v>
       </c>
       <c r="L227" s="6"/>
       <c r="M227" s="6"/>
     </row>
     <row r="228" spans="1:13" ht="15">
       <c r="A228">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B228">
+        <f t="shared" si="29"/>
+        <v>11</v>
+      </c>
+      <c r="C228" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B228">
-        <f t="shared" si="28"/>
-        <v>16</v>
-      </c>
-      <c r="C228" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-16</v>
+        <v>24-11</v>
       </c>
       <c r="L228" s="6"/>
       <c r="M228" s="6"/>
     </row>
     <row r="229" spans="1:13" ht="15">
       <c r="A229">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B229">
+        <f t="shared" si="29"/>
+        <v>12</v>
+      </c>
+      <c r="C229" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B229">
-        <f t="shared" si="28"/>
-        <v>17</v>
-      </c>
-      <c r="C229" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-17</v>
+        <v>24-12</v>
       </c>
       <c r="L229" s="6"/>
       <c r="M229" s="6"/>
     </row>
     <row r="230" spans="1:13" ht="15">
       <c r="A230">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B230">
+        <f t="shared" si="29"/>
+        <v>13</v>
+      </c>
+      <c r="C230" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B230">
-        <f t="shared" si="28"/>
-        <v>18</v>
-      </c>
-      <c r="C230" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-18</v>
+        <v>24-13</v>
       </c>
       <c r="L230" s="6"/>
       <c r="M230" s="6"/>
     </row>
     <row r="231" spans="1:13" ht="15">
       <c r="A231">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B231">
+        <f t="shared" si="29"/>
+        <v>14</v>
+      </c>
+      <c r="C231" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B231">
-        <f t="shared" si="28"/>
-        <v>19</v>
-      </c>
-      <c r="C231" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-19</v>
+        <v>24-14</v>
       </c>
       <c r="L231" s="6"/>
       <c r="M231" s="6"/>
     </row>
     <row r="232" spans="1:13" ht="15">
       <c r="A232">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B232">
+        <f t="shared" si="29"/>
+        <v>15</v>
+      </c>
+      <c r="C232" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B232">
-        <f t="shared" si="28"/>
-        <v>20</v>
-      </c>
-      <c r="C232" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-20</v>
+        <v>24-15</v>
       </c>
       <c r="L232" s="6"/>
       <c r="M232" s="6"/>
     </row>
     <row r="233" spans="1:13" ht="15">
       <c r="A233">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B233">
+        <f t="shared" si="29"/>
+        <v>16</v>
+      </c>
+      <c r="C233" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B233">
-        <f t="shared" si="28"/>
-        <v>21</v>
-      </c>
-      <c r="C233" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-21</v>
+        <v>24-16</v>
       </c>
       <c r="L233" s="6"/>
       <c r="M233" s="6"/>
     </row>
     <row r="234" spans="1:13" ht="15">
       <c r="A234">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B234">
+        <f t="shared" si="29"/>
+        <v>17</v>
+      </c>
+      <c r="C234" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B234">
-        <f t="shared" si="28"/>
-        <v>22</v>
-      </c>
-      <c r="C234" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-22</v>
+        <v>24-17</v>
       </c>
       <c r="L234" s="6"/>
       <c r="M234" s="6"/>
     </row>
     <row r="235" spans="1:13" ht="15">
       <c r="A235">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B235">
+        <f t="shared" si="29"/>
+        <v>18</v>
+      </c>
+      <c r="C235" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B235">
-        <f t="shared" si="28"/>
-        <v>23</v>
-      </c>
-      <c r="C235" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-23</v>
+        <v>24-18</v>
       </c>
       <c r="L235" s="6"/>
       <c r="M235" s="6"/>
     </row>
     <row r="236" spans="1:13" ht="15">
       <c r="A236">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B236">
+        <f t="shared" si="29"/>
+        <v>19</v>
+      </c>
+      <c r="C236" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B236">
-        <f t="shared" si="28"/>
-        <v>24</v>
-      </c>
-      <c r="C236" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-24</v>
+        <v>24-19</v>
       </c>
       <c r="L236" s="6"/>
       <c r="M236" s="6"/>
     </row>
     <row r="237" spans="1:13" ht="15">
       <c r="A237">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B237">
+        <f t="shared" si="29"/>
+        <v>20</v>
+      </c>
+      <c r="C237" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B237">
-        <f t="shared" si="28"/>
-        <v>25</v>
-      </c>
-      <c r="C237" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-25</v>
+        <v>24-20</v>
       </c>
       <c r="L237" s="6"/>
       <c r="M237" s="6"/>
     </row>
     <row r="238" spans="1:13" ht="15">
       <c r="A238">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B238">
+        <f t="shared" si="29"/>
+        <v>21</v>
+      </c>
+      <c r="C238" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B238">
-        <f t="shared" si="28"/>
-        <v>26</v>
-      </c>
-      <c r="C238" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-26</v>
+        <v>24-21</v>
       </c>
       <c r="L238" s="6"/>
       <c r="M238" s="6"/>
     </row>
     <row r="239" spans="1:13" ht="15">
       <c r="A239">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B239">
+        <f t="shared" si="29"/>
+        <v>22</v>
+      </c>
+      <c r="C239" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B239">
-        <f t="shared" si="28"/>
-        <v>27</v>
-      </c>
-      <c r="C239" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-27</v>
+        <v>24-22</v>
       </c>
       <c r="L239" s="6"/>
       <c r="M239" s="6"/>
     </row>
     <row r="240" spans="1:13" ht="15">
       <c r="A240">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B240">
+        <f t="shared" si="29"/>
+        <v>23</v>
+      </c>
+      <c r="C240" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B240">
-        <f t="shared" si="28"/>
-        <v>28</v>
-      </c>
-      <c r="C240" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-28</v>
+        <v>24-23</v>
       </c>
       <c r="L240" s="6"/>
       <c r="M240" s="6"/>
     </row>
     <row r="241" spans="1:13" ht="15">
       <c r="A241">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B241">
+        <f t="shared" si="29"/>
+        <v>24</v>
+      </c>
+      <c r="C241" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B241">
-        <f t="shared" si="28"/>
-        <v>29</v>
-      </c>
-      <c r="C241" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-29</v>
+        <v>24-24</v>
       </c>
       <c r="L241" s="6"/>
       <c r="M241" s="6"/>
     </row>
     <row r="242" spans="1:13" ht="15">
       <c r="A242">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B242">
+        <f t="shared" si="29"/>
+        <v>25</v>
+      </c>
+      <c r="C242" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B242">
-        <f t="shared" si="28"/>
-        <v>30</v>
-      </c>
-      <c r="C242" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-30</v>
+        <v>24-25</v>
       </c>
       <c r="L242" s="6"/>
       <c r="M242" s="6"/>
     </row>
     <row r="243" spans="1:13" ht="15">
       <c r="A243">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B243">
+        <f t="shared" si="29"/>
+        <v>26</v>
+      </c>
+      <c r="C243" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B243">
-        <f t="shared" si="28"/>
-        <v>31</v>
-      </c>
-      <c r="C243" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-31</v>
+        <v>24-26</v>
       </c>
       <c r="L243" s="6"/>
       <c r="M243" s="6"/>
     </row>
     <row r="244" spans="1:13" ht="15">
       <c r="A244">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B244">
+        <f t="shared" si="29"/>
+        <v>27</v>
+      </c>
+      <c r="C244" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B244">
-        <f t="shared" si="28"/>
-        <v>32</v>
-      </c>
-      <c r="C244" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-32</v>
+        <v>24-27</v>
       </c>
       <c r="L244" s="6"/>
       <c r="M244" s="6"/>
     </row>
     <row r="245" spans="1:13" ht="15">
       <c r="A245">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B245">
+        <f t="shared" si="29"/>
+        <v>28</v>
+      </c>
+      <c r="C245" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B245">
-        <f t="shared" si="28"/>
-        <v>33</v>
-      </c>
-      <c r="C245" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-33</v>
+        <v>24-28</v>
       </c>
       <c r="L245" s="6"/>
       <c r="M245" s="6"/>
     </row>
     <row r="246" spans="1:13" ht="15">
       <c r="A246">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B246">
+        <f t="shared" si="29"/>
+        <v>29</v>
+      </c>
+      <c r="C246" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B246">
-        <f t="shared" si="28"/>
-        <v>34</v>
-      </c>
-      <c r="C246" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-34</v>
+        <v>24-29</v>
       </c>
       <c r="L246" s="6"/>
       <c r="M246" s="6"/>
     </row>
     <row r="247" spans="1:13" ht="15">
       <c r="A247">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B247">
+        <f t="shared" si="29"/>
+        <v>30</v>
+      </c>
+      <c r="C247" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B247">
-        <f t="shared" si="28"/>
-        <v>35</v>
-      </c>
-      <c r="C247" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-35</v>
+        <v>24-30</v>
       </c>
       <c r="L247" s="6"/>
       <c r="M247" s="6"/>
     </row>
     <row r="248" spans="1:13" ht="15">
       <c r="A248">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B248">
+        <f t="shared" si="29"/>
+        <v>31</v>
+      </c>
+      <c r="C248" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B248">
-        <f t="shared" si="28"/>
-        <v>36</v>
-      </c>
-      <c r="C248" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-36</v>
+        <v>24-31</v>
       </c>
       <c r="L248" s="6"/>
       <c r="M248" s="6"/>
     </row>
     <row r="249" spans="1:13" ht="15">
       <c r="A249">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B249">
+        <f t="shared" si="29"/>
+        <v>32</v>
+      </c>
+      <c r="C249" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B249">
-        <f t="shared" si="28"/>
-        <v>37</v>
-      </c>
-      <c r="C249" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-37</v>
+        <v>24-32</v>
       </c>
       <c r="L249" s="6"/>
       <c r="M249" s="6"/>
     </row>
     <row r="250" spans="1:13" ht="15">
       <c r="A250">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B250">
+        <f t="shared" si="29"/>
+        <v>33</v>
+      </c>
+      <c r="C250" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B250">
-        <f t="shared" si="28"/>
-        <v>38</v>
-      </c>
-      <c r="C250" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-38</v>
+        <v>24-33</v>
       </c>
       <c r="L250" s="6"/>
       <c r="M250" s="6"/>
     </row>
     <row r="251" spans="1:13" ht="15">
       <c r="A251">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B251">
+        <f t="shared" si="29"/>
+        <v>34</v>
+      </c>
+      <c r="C251" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B251">
-        <f t="shared" si="28"/>
-        <v>39</v>
-      </c>
-      <c r="C251" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-39</v>
+        <v>24-34</v>
       </c>
       <c r="L251" s="6"/>
       <c r="M251" s="6"/>
     </row>
     <row r="252" spans="1:13" ht="15">
       <c r="A252">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B252">
+        <f t="shared" si="29"/>
+        <v>35</v>
+      </c>
+      <c r="C252" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B252">
-        <f t="shared" si="28"/>
-        <v>40</v>
-      </c>
-      <c r="C252" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-40</v>
+        <v>24-35</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
     </row>
     <row r="253" spans="1:13" ht="15">
       <c r="A253">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B253">
+        <f t="shared" si="29"/>
+        <v>36</v>
+      </c>
+      <c r="C253" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B253">
-        <f t="shared" si="28"/>
-        <v>41</v>
-      </c>
-      <c r="C253" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-41</v>
+        <v>24-36</v>
       </c>
       <c r="L253" s="6"/>
       <c r="M253" s="6"/>
     </row>
     <row r="254" spans="1:13" ht="15">
       <c r="A254">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B254">
+        <f t="shared" si="29"/>
+        <v>37</v>
+      </c>
+      <c r="C254" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B254">
-        <f t="shared" si="28"/>
-        <v>42</v>
-      </c>
-      <c r="C254" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-42</v>
+        <v>24-37</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
     </row>
     <row r="255" spans="1:13" ht="15">
       <c r="A255">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B255">
+        <f t="shared" si="29"/>
+        <v>38</v>
+      </c>
+      <c r="C255" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B255">
-        <f t="shared" si="28"/>
-        <v>43</v>
-      </c>
-      <c r="C255" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-43</v>
+        <v>24-38</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
     </row>
     <row r="256" spans="1:13" ht="15">
       <c r="A256">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B256">
+        <f t="shared" si="29"/>
+        <v>39</v>
+      </c>
+      <c r="C256" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B256">
-        <f t="shared" si="28"/>
-        <v>44</v>
-      </c>
-      <c r="C256" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-44</v>
+        <v>24-39</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
     </row>
     <row r="257" spans="1:13" ht="15">
       <c r="A257">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B257">
+        <f t="shared" si="29"/>
+        <v>40</v>
+      </c>
+      <c r="C257" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B257">
-        <f t="shared" si="28"/>
-        <v>45</v>
-      </c>
-      <c r="C257" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-45</v>
+        <v>24-40</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
     </row>
     <row r="258" spans="1:13" ht="15">
       <c r="A258">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B258">
+        <f t="shared" si="29"/>
+        <v>41</v>
+      </c>
+      <c r="C258" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B258">
-        <f t="shared" si="28"/>
-        <v>46</v>
-      </c>
-      <c r="C258" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-46</v>
+        <v>24-41</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
     </row>
     <row r="259" spans="1:13" ht="15">
       <c r="A259">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B259">
+        <f t="shared" si="29"/>
+        <v>42</v>
+      </c>
+      <c r="C259" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B259">
-        <f t="shared" si="28"/>
-        <v>47</v>
-      </c>
-      <c r="C259" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-47</v>
+        <v>24-42</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
     </row>
     <row r="260" spans="1:13" ht="15">
       <c r="A260">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B260">
+        <f t="shared" si="29"/>
+        <v>43</v>
+      </c>
+      <c r="C260" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B260">
-        <f t="shared" si="28"/>
-        <v>48</v>
-      </c>
-      <c r="C260" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-48</v>
+        <v>24-43</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
     </row>
     <row r="261" spans="1:13" ht="15">
       <c r="A261">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B261">
+        <f t="shared" si="29"/>
+        <v>44</v>
+      </c>
+      <c r="C261" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B261">
-        <f t="shared" si="28"/>
-        <v>49</v>
-      </c>
-      <c r="C261" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-49</v>
+        <v>24-44</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
     </row>
     <row r="262" spans="1:13" ht="15">
       <c r="A262">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B262">
+        <f t="shared" si="29"/>
+        <v>45</v>
+      </c>
+      <c r="C262" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B262">
-        <f t="shared" si="28"/>
-        <v>50</v>
-      </c>
-      <c r="C262" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-50</v>
+        <v>24-45</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
     </row>
     <row r="263" spans="1:13" ht="15">
       <c r="A263">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B263">
+        <f t="shared" si="29"/>
+        <v>46</v>
+      </c>
+      <c r="C263" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B263">
-        <f t="shared" si="28"/>
-        <v>51</v>
-      </c>
-      <c r="C263" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-51</v>
+        <v>24-46</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
     </row>
     <row r="264" spans="1:13" ht="15">
       <c r="A264">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B264">
+        <f t="shared" si="29"/>
+        <v>47</v>
+      </c>
+      <c r="C264" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B264">
-        <f t="shared" si="28"/>
-        <v>52</v>
-      </c>
-      <c r="C264" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-52</v>
+        <v>24-47</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
     </row>
     <row r="265" spans="1:13" ht="15">
       <c r="A265">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B265">
+        <f t="shared" si="29"/>
+        <v>48</v>
+      </c>
+      <c r="C265" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B265">
-        <f t="shared" si="28"/>
-        <v>53</v>
-      </c>
-      <c r="C265" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-53</v>
+        <v>24-48</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
     </row>
     <row r="266" spans="1:13" ht="15">
       <c r="A266">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B266">
+        <f t="shared" si="29"/>
+        <v>49</v>
+      </c>
+      <c r="C266" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B266">
-        <f t="shared" si="28"/>
-        <v>54</v>
-      </c>
-      <c r="C266" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-54</v>
+        <v>24-49</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
     </row>
     <row r="267" spans="1:13" ht="15">
       <c r="A267">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B267">
+        <f t="shared" si="29"/>
+        <v>50</v>
+      </c>
+      <c r="C267" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B267">
-        <f t="shared" si="28"/>
-        <v>55</v>
-      </c>
-      <c r="C267" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-55</v>
+        <v>24-50</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
     </row>
     <row r="268" spans="1:13" ht="15">
       <c r="A268">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B268">
+        <f t="shared" si="29"/>
+        <v>51</v>
+      </c>
+      <c r="C268" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B268">
-        <f t="shared" si="28"/>
-        <v>56</v>
-      </c>
-      <c r="C268" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-56</v>
+        <v>24-51</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
     </row>
     <row r="269" spans="1:13" ht="15">
       <c r="A269">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B269">
+        <f t="shared" si="29"/>
+        <v>52</v>
+      </c>
+      <c r="C269" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B269">
-        <f t="shared" si="28"/>
-        <v>57</v>
-      </c>
-      <c r="C269" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-57</v>
+        <v>24-52</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
     </row>
     <row r="270" spans="1:13" ht="15">
       <c r="A270">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B270">
+        <f t="shared" si="29"/>
+        <v>53</v>
+      </c>
+      <c r="C270" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B270">
-        <f t="shared" si="28"/>
-        <v>58</v>
-      </c>
-      <c r="C270" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-58</v>
+        <v>24-53</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
     </row>
     <row r="271" spans="1:13" ht="15">
       <c r="A271">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B271">
+        <f t="shared" si="29"/>
+        <v>54</v>
+      </c>
+      <c r="C271" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B271">
-        <f t="shared" si="28"/>
-        <v>59</v>
-      </c>
-      <c r="C271" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-59</v>
+        <v>24-54</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
     </row>
     <row r="272" spans="1:13" ht="15">
       <c r="A272">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B272">
+        <f t="shared" si="29"/>
+        <v>55</v>
+      </c>
+      <c r="C272" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B272">
-        <f t="shared" si="28"/>
-        <v>60</v>
-      </c>
-      <c r="C272" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-60</v>
+        <v>24-55</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
     </row>
     <row r="273" spans="1:13" ht="15">
       <c r="A273">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B273">
+        <f t="shared" si="29"/>
+        <v>56</v>
+      </c>
+      <c r="C273" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B273">
-        <f t="shared" si="28"/>
-        <v>61</v>
-      </c>
-      <c r="C273" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-61</v>
+        <v>24-56</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
     </row>
     <row r="274" spans="1:13" ht="15">
       <c r="A274">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B274">
+        <f t="shared" si="29"/>
+        <v>57</v>
+      </c>
+      <c r="C274" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B274">
-        <f t="shared" si="28"/>
-        <v>62</v>
-      </c>
-      <c r="C274" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-62</v>
+        <v>24-57</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
     </row>
     <row r="275" spans="1:13" ht="15">
       <c r="A275">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B275">
+        <f t="shared" si="29"/>
+        <v>58</v>
+      </c>
+      <c r="C275" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B275">
-        <f t="shared" si="28"/>
-        <v>63</v>
-      </c>
-      <c r="C275" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-63</v>
+        <v>24-58</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
     </row>
     <row r="276" spans="1:13" ht="15">
       <c r="A276">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B276">
+        <f t="shared" si="29"/>
+        <v>59</v>
+      </c>
+      <c r="C276" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B276">
-        <f t="shared" si="28"/>
-        <v>64</v>
-      </c>
-      <c r="C276" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-64</v>
+        <v>24-59</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
     </row>
     <row r="277" spans="1:13" ht="15">
       <c r="A277">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B277">
+        <f t="shared" si="29"/>
+        <v>60</v>
+      </c>
+      <c r="C277" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B277">
-        <f t="shared" si="28"/>
-        <v>65</v>
-      </c>
-      <c r="C277" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-65</v>
+        <v>24-60</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
     </row>
     <row r="278" spans="1:13" ht="15">
       <c r="A278">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B278">
+        <f t="shared" si="29"/>
+        <v>61</v>
+      </c>
+      <c r="C278" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B278">
-        <f t="shared" si="28"/>
-        <v>66</v>
-      </c>
-      <c r="C278" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-66</v>
+        <v>24-61</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
     </row>
     <row r="279" spans="1:13" ht="15">
       <c r="A279">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B279">
+        <f t="shared" si="29"/>
+        <v>62</v>
+      </c>
+      <c r="C279" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B279">
-        <f t="shared" si="28"/>
-        <v>67</v>
-      </c>
-      <c r="C279" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-67</v>
+        <v>24-62</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
     </row>
     <row r="280" spans="1:13" ht="15">
       <c r="A280">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B280">
+        <f t="shared" si="29"/>
+        <v>63</v>
+      </c>
+      <c r="C280" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B280">
-        <f t="shared" si="28"/>
-        <v>68</v>
-      </c>
-      <c r="C280" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-68</v>
+        <v>24-63</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
     </row>
     <row r="281" spans="1:13" ht="15">
       <c r="A281">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B281">
+        <f t="shared" si="29"/>
+        <v>64</v>
+      </c>
+      <c r="C281" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B281">
-        <f t="shared" si="28"/>
-        <v>69</v>
-      </c>
-      <c r="C281" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-69</v>
+        <v>24-64</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
     </row>
     <row r="282" spans="1:13" ht="15">
       <c r="A282">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B282">
+        <f t="shared" si="29"/>
+        <v>65</v>
+      </c>
+      <c r="C282" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B282">
-        <f t="shared" si="28"/>
-        <v>70</v>
-      </c>
-      <c r="C282" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-70</v>
+        <v>24-65</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
     </row>
     <row r="283" spans="1:13" ht="15">
       <c r="A283">
+        <f t="shared" si="31"/>
+        <v>24</v>
+      </c>
+      <c r="B283">
+        <f t="shared" si="29"/>
+        <v>66</v>
+      </c>
+      <c r="C283" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>23</v>
-      </c>
-      <c r="B283">
-        <f t="shared" si="28"/>
-        <v>71</v>
-      </c>
-      <c r="C283" s="3" t="str">
-        <f t="shared" si="29"/>
-        <v>23-71</v>
+        <v>24-66</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
     </row>
     <row r="284" spans="1:13" ht="15">
       <c r="A284">
-        <f t="shared" si="30"/>
-        <v>23</v>
+        <f t="shared" si="31"/>
+        <v>24</v>
       </c>
       <c r="B284">
-        <f t="shared" ref="B284:B347" si="31">IF(A284=A283,B283+1,1)</f>
-        <v>72</v>
+        <f t="shared" ref="B284:B347" si="32">IF(A284=A283,B283+1,1)</f>
+        <v>67</v>
       </c>
       <c r="C284" s="3" t="str">
-        <f t="shared" ref="C284:C347" si="32">CONCATENATE(A284,"-",B284)</f>
-        <v>23-72</v>
+        <f t="shared" ref="C284:C347" si="33">CONCATENATE(A284,"-",B284)</f>
+        <v>24-67</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
     </row>
     <row r="285" spans="1:13" ht="15">
       <c r="A285">
-        <f t="shared" ref="A285:A348" si="33">A284</f>
-        <v>23</v>
+        <f t="shared" ref="A285:A348" si="34">A284</f>
+        <v>24</v>
       </c>
       <c r="B285">
-        <f t="shared" si="31"/>
-        <v>73</v>
+        <f t="shared" si="32"/>
+        <v>68</v>
       </c>
       <c r="C285" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-73</v>
+        <f t="shared" si="33"/>
+        <v>24-68</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
     </row>
     <row r="286" spans="1:13" ht="15">
       <c r="A286">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B286">
+        <f t="shared" si="32"/>
+        <v>69</v>
+      </c>
+      <c r="C286" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B286">
-        <f t="shared" si="31"/>
-        <v>74</v>
-      </c>
-      <c r="C286" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-74</v>
+        <v>24-69</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
     </row>
     <row r="287" spans="1:13" ht="15">
       <c r="A287">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B287">
+        <f t="shared" si="32"/>
+        <v>70</v>
+      </c>
+      <c r="C287" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B287">
-        <f t="shared" si="31"/>
-        <v>75</v>
-      </c>
-      <c r="C287" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-75</v>
+        <v>24-70</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
     </row>
     <row r="288" spans="1:13" ht="15">
       <c r="A288">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B288">
+        <f t="shared" si="32"/>
+        <v>71</v>
+      </c>
+      <c r="C288" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B288">
-        <f t="shared" si="31"/>
-        <v>76</v>
-      </c>
-      <c r="C288" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-76</v>
+        <v>24-71</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
     </row>
     <row r="289" spans="1:13" ht="15">
       <c r="A289">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B289">
+        <f t="shared" si="32"/>
+        <v>72</v>
+      </c>
+      <c r="C289" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B289">
-        <f t="shared" si="31"/>
-        <v>77</v>
-      </c>
-      <c r="C289" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-77</v>
+        <v>24-72</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
     </row>
     <row r="290" spans="1:13" ht="15">
       <c r="A290">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B290">
+        <f t="shared" si="32"/>
+        <v>73</v>
+      </c>
+      <c r="C290" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B290">
-        <f t="shared" si="31"/>
-        <v>78</v>
-      </c>
-      <c r="C290" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-78</v>
+        <v>24-73</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
     </row>
     <row r="291" spans="1:13" ht="15">
       <c r="A291">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B291">
+        <f t="shared" si="32"/>
+        <v>74</v>
+      </c>
+      <c r="C291" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B291">
-        <f t="shared" si="31"/>
-        <v>79</v>
-      </c>
-      <c r="C291" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-79</v>
+        <v>24-74</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
     </row>
     <row r="292" spans="1:13" ht="15">
       <c r="A292">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B292">
+        <f t="shared" si="32"/>
+        <v>75</v>
+      </c>
+      <c r="C292" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B292">
-        <f t="shared" si="31"/>
-        <v>80</v>
-      </c>
-      <c r="C292" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-80</v>
+        <v>24-75</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
     </row>
     <row r="293" spans="1:13" ht="15">
       <c r="A293">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B293">
+        <f t="shared" si="32"/>
+        <v>76</v>
+      </c>
+      <c r="C293" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B293">
-        <f t="shared" si="31"/>
-        <v>81</v>
-      </c>
-      <c r="C293" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-81</v>
+        <v>24-76</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
     </row>
     <row r="294" spans="1:13" ht="15">
       <c r="A294">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B294">
+        <f t="shared" si="32"/>
+        <v>77</v>
+      </c>
+      <c r="C294" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B294">
-        <f t="shared" si="31"/>
-        <v>82</v>
-      </c>
-      <c r="C294" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-82</v>
+        <v>24-77</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
     </row>
     <row r="295" spans="1:13" ht="15">
       <c r="A295">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B295">
+        <f t="shared" si="32"/>
+        <v>78</v>
+      </c>
+      <c r="C295" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B295">
-        <f t="shared" si="31"/>
-        <v>83</v>
-      </c>
-      <c r="C295" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-83</v>
+        <v>24-78</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
     </row>
     <row r="296" spans="1:13" ht="15">
       <c r="A296">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B296">
+        <f t="shared" si="32"/>
+        <v>79</v>
+      </c>
+      <c r="C296" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B296">
-        <f t="shared" si="31"/>
-        <v>84</v>
-      </c>
-      <c r="C296" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-84</v>
+        <v>24-79</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
     </row>
     <row r="297" spans="1:13" ht="15">
       <c r="A297">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B297">
+        <f t="shared" si="32"/>
+        <v>80</v>
+      </c>
+      <c r="C297" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B297">
-        <f t="shared" si="31"/>
-        <v>85</v>
-      </c>
-      <c r="C297" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-85</v>
+        <v>24-80</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
     </row>
     <row r="298" spans="1:13" ht="15">
       <c r="A298">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B298">
+        <f t="shared" si="32"/>
+        <v>81</v>
+      </c>
+      <c r="C298" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B298">
-        <f t="shared" si="31"/>
-        <v>86</v>
-      </c>
-      <c r="C298" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-86</v>
+        <v>24-81</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
     </row>
     <row r="299" spans="1:13" ht="15">
       <c r="A299">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B299">
+        <f t="shared" si="32"/>
+        <v>82</v>
+      </c>
+      <c r="C299" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B299">
-        <f t="shared" si="31"/>
-        <v>87</v>
-      </c>
-      <c r="C299" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-87</v>
+        <v>24-82</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
     </row>
     <row r="300" spans="1:13" ht="15">
       <c r="A300">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B300">
+        <f t="shared" si="32"/>
+        <v>83</v>
+      </c>
+      <c r="C300" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B300">
-        <f t="shared" si="31"/>
-        <v>88</v>
-      </c>
-      <c r="C300" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-88</v>
+        <v>24-83</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
     </row>
     <row r="301" spans="1:13" ht="15">
       <c r="A301">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B301">
+        <f t="shared" si="32"/>
+        <v>84</v>
+      </c>
+      <c r="C301" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B301">
-        <f t="shared" si="31"/>
-        <v>89</v>
-      </c>
-      <c r="C301" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-89</v>
+        <v>24-84</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
     </row>
     <row r="302" spans="1:13" ht="15">
       <c r="A302">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B302">
+        <f t="shared" si="32"/>
+        <v>85</v>
+      </c>
+      <c r="C302" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B302">
-        <f t="shared" si="31"/>
-        <v>90</v>
-      </c>
-      <c r="C302" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-90</v>
+        <v>24-85</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
     </row>
     <row r="303" spans="1:13" ht="15">
       <c r="A303">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B303">
+        <f t="shared" si="32"/>
+        <v>86</v>
+      </c>
+      <c r="C303" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B303">
-        <f t="shared" si="31"/>
-        <v>91</v>
-      </c>
-      <c r="C303" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-91</v>
+        <v>24-86</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
     </row>
     <row r="304" spans="1:13" ht="15">
       <c r="A304">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B304">
+        <f t="shared" si="32"/>
+        <v>87</v>
+      </c>
+      <c r="C304" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B304">
-        <f t="shared" si="31"/>
-        <v>92</v>
-      </c>
-      <c r="C304" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-92</v>
+        <v>24-87</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
     </row>
     <row r="305" spans="1:13" ht="15">
       <c r="A305">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B305">
+        <f t="shared" si="32"/>
+        <v>88</v>
+      </c>
+      <c r="C305" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B305">
-        <f t="shared" si="31"/>
-        <v>93</v>
-      </c>
-      <c r="C305" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-93</v>
+        <v>24-88</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
     </row>
     <row r="306" spans="1:13" ht="15">
       <c r="A306">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B306">
+        <f t="shared" si="32"/>
+        <v>89</v>
+      </c>
+      <c r="C306" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B306">
-        <f t="shared" si="31"/>
-        <v>94</v>
-      </c>
-      <c r="C306" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-94</v>
+        <v>24-89</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
     </row>
     <row r="307" spans="1:13" ht="15">
       <c r="A307">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B307">
+        <f t="shared" si="32"/>
+        <v>90</v>
+      </c>
+      <c r="C307" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B307">
-        <f t="shared" si="31"/>
-        <v>95</v>
-      </c>
-      <c r="C307" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-95</v>
+        <v>24-90</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
     </row>
     <row r="308" spans="1:13" ht="15">
       <c r="A308">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B308">
+        <f t="shared" si="32"/>
+        <v>91</v>
+      </c>
+      <c r="C308" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B308">
-        <f t="shared" si="31"/>
-        <v>96</v>
-      </c>
-      <c r="C308" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-96</v>
+        <v>24-91</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
     </row>
     <row r="309" spans="1:13" ht="15">
       <c r="A309">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B309">
+        <f t="shared" si="32"/>
+        <v>92</v>
+      </c>
+      <c r="C309" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B309">
-        <f t="shared" si="31"/>
-        <v>97</v>
-      </c>
-      <c r="C309" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-97</v>
+        <v>24-92</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
     </row>
     <row r="310" spans="1:13" ht="15">
       <c r="A310">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B310">
+        <f t="shared" si="32"/>
+        <v>93</v>
+      </c>
+      <c r="C310" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B310">
-        <f t="shared" si="31"/>
-        <v>98</v>
-      </c>
-      <c r="C310" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-98</v>
+        <v>24-93</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
     </row>
     <row r="311" spans="1:13" ht="15">
       <c r="A311">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B311">
+        <f t="shared" si="32"/>
+        <v>94</v>
+      </c>
+      <c r="C311" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B311">
-        <f t="shared" si="31"/>
-        <v>99</v>
-      </c>
-      <c r="C311" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-99</v>
+        <v>24-94</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
     </row>
     <row r="312" spans="1:13" ht="15">
       <c r="A312">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B312">
+        <f t="shared" si="32"/>
+        <v>95</v>
+      </c>
+      <c r="C312" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B312">
-        <f t="shared" si="31"/>
-        <v>100</v>
-      </c>
-      <c r="C312" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-100</v>
+        <v>24-95</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
     </row>
     <row r="313" spans="1:13" ht="15">
       <c r="A313">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B313">
+        <f t="shared" si="32"/>
+        <v>96</v>
+      </c>
+      <c r="C313" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B313">
-        <f t="shared" si="31"/>
-        <v>101</v>
-      </c>
-      <c r="C313" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-101</v>
+        <v>24-96</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
     </row>
     <row r="314" spans="1:13" ht="15">
       <c r="A314">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B314">
+        <f t="shared" si="32"/>
+        <v>97</v>
+      </c>
+      <c r="C314" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B314">
-        <f t="shared" si="31"/>
-        <v>102</v>
-      </c>
-      <c r="C314" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-102</v>
+        <v>24-97</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
     </row>
     <row r="315" spans="1:13" ht="15">
       <c r="A315">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B315">
+        <f t="shared" si="32"/>
+        <v>98</v>
+      </c>
+      <c r="C315" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B315">
-        <f t="shared" si="31"/>
-        <v>103</v>
-      </c>
-      <c r="C315" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-103</v>
+        <v>24-98</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
     </row>
     <row r="316" spans="1:13" ht="15">
       <c r="A316">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B316">
+        <f t="shared" si="32"/>
+        <v>99</v>
+      </c>
+      <c r="C316" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B316">
-        <f t="shared" si="31"/>
-        <v>104</v>
-      </c>
-      <c r="C316" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-104</v>
+        <v>24-99</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
     </row>
     <row r="317" spans="1:13" ht="15">
       <c r="A317">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B317">
+        <f t="shared" si="32"/>
+        <v>100</v>
+      </c>
+      <c r="C317" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B317">
-        <f t="shared" si="31"/>
-        <v>105</v>
-      </c>
-      <c r="C317" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-105</v>
+        <v>24-100</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
     </row>
     <row r="318" spans="1:13" ht="15">
       <c r="A318">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B318">
+        <f t="shared" si="32"/>
+        <v>101</v>
+      </c>
+      <c r="C318" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B318">
-        <f t="shared" si="31"/>
-        <v>106</v>
-      </c>
-      <c r="C318" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-106</v>
+        <v>24-101</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
     </row>
     <row r="319" spans="1:13" ht="15">
       <c r="A319">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B319">
+        <f t="shared" si="32"/>
+        <v>102</v>
+      </c>
+      <c r="C319" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B319">
-        <f t="shared" si="31"/>
-        <v>107</v>
-      </c>
-      <c r="C319" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-107</v>
+        <v>24-102</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
     </row>
     <row r="320" spans="1:13" ht="15">
       <c r="A320">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B320">
+        <f t="shared" si="32"/>
+        <v>103</v>
+      </c>
+      <c r="C320" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B320">
-        <f t="shared" si="31"/>
-        <v>108</v>
-      </c>
-      <c r="C320" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-108</v>
+        <v>24-103</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
     </row>
     <row r="321" spans="1:13" ht="15">
       <c r="A321">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B321">
+        <f t="shared" si="32"/>
+        <v>104</v>
+      </c>
+      <c r="C321" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B321">
-        <f t="shared" si="31"/>
-        <v>109</v>
-      </c>
-      <c r="C321" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-109</v>
+        <v>24-104</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
     </row>
     <row r="322" spans="1:13" ht="15">
       <c r="A322">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B322">
+        <f t="shared" si="32"/>
+        <v>105</v>
+      </c>
+      <c r="C322" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B322">
-        <f t="shared" si="31"/>
-        <v>110</v>
-      </c>
-      <c r="C322" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-110</v>
+        <v>24-105</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
     </row>
     <row r="323" spans="1:13" ht="15">
       <c r="A323">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B323">
+        <f t="shared" si="32"/>
+        <v>106</v>
+      </c>
+      <c r="C323" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B323">
-        <f t="shared" si="31"/>
-        <v>111</v>
-      </c>
-      <c r="C323" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-111</v>
+        <v>24-106</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
     </row>
     <row r="324" spans="1:13" ht="15">
       <c r="A324">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B324">
+        <f t="shared" si="32"/>
+        <v>107</v>
+      </c>
+      <c r="C324" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B324">
-        <f t="shared" si="31"/>
-        <v>112</v>
-      </c>
-      <c r="C324" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-112</v>
+        <v>24-107</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
     </row>
     <row r="325" spans="1:13" ht="15">
       <c r="A325">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B325">
+        <f t="shared" si="32"/>
+        <v>108</v>
+      </c>
+      <c r="C325" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B325">
-        <f t="shared" si="31"/>
-        <v>113</v>
-      </c>
-      <c r="C325" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-113</v>
+        <v>24-108</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
     </row>
     <row r="326" spans="1:13" ht="15">
       <c r="A326">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B326">
+        <f t="shared" si="32"/>
+        <v>109</v>
+      </c>
+      <c r="C326" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B326">
-        <f t="shared" si="31"/>
-        <v>114</v>
-      </c>
-      <c r="C326" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-114</v>
+        <v>24-109</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
     </row>
     <row r="327" spans="1:13" ht="15">
       <c r="A327">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B327">
+        <f t="shared" si="32"/>
+        <v>110</v>
+      </c>
+      <c r="C327" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B327">
-        <f t="shared" si="31"/>
-        <v>115</v>
-      </c>
-      <c r="C327" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-115</v>
+        <v>24-110</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
     </row>
     <row r="328" spans="1:13" ht="15">
       <c r="A328">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B328">
+        <f t="shared" si="32"/>
+        <v>111</v>
+      </c>
+      <c r="C328" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B328">
-        <f t="shared" si="31"/>
-        <v>116</v>
-      </c>
-      <c r="C328" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-116</v>
+        <v>24-111</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
     </row>
     <row r="329" spans="1:13" ht="15">
       <c r="A329">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B329">
+        <f t="shared" si="32"/>
+        <v>112</v>
+      </c>
+      <c r="C329" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B329">
-        <f t="shared" si="31"/>
-        <v>117</v>
-      </c>
-      <c r="C329" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-117</v>
+        <v>24-112</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
     </row>
     <row r="330" spans="1:13" ht="15">
       <c r="A330">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B330">
+        <f t="shared" si="32"/>
+        <v>113</v>
+      </c>
+      <c r="C330" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B330">
-        <f t="shared" si="31"/>
-        <v>118</v>
-      </c>
-      <c r="C330" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-118</v>
+        <v>24-113</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
     </row>
     <row r="331" spans="1:13" ht="15">
       <c r="A331">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B331">
+        <f t="shared" si="32"/>
+        <v>114</v>
+      </c>
+      <c r="C331" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B331">
-        <f t="shared" si="31"/>
-        <v>119</v>
-      </c>
-      <c r="C331" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-119</v>
+        <v>24-114</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
     </row>
     <row r="332" spans="1:13" ht="15">
       <c r="A332">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B332">
+        <f t="shared" si="32"/>
+        <v>115</v>
+      </c>
+      <c r="C332" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B332">
-        <f t="shared" si="31"/>
-        <v>120</v>
-      </c>
-      <c r="C332" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-120</v>
+        <v>24-115</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
     </row>
     <row r="333" spans="1:13" ht="15">
       <c r="A333">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B333">
+        <f t="shared" si="32"/>
+        <v>116</v>
+      </c>
+      <c r="C333" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B333">
-        <f t="shared" si="31"/>
-        <v>121</v>
-      </c>
-      <c r="C333" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-121</v>
+        <v>24-116</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
     </row>
     <row r="334" spans="1:13" ht="15">
       <c r="A334">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B334">
+        <f t="shared" si="32"/>
+        <v>117</v>
+      </c>
+      <c r="C334" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B334">
-        <f t="shared" si="31"/>
-        <v>122</v>
-      </c>
-      <c r="C334" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-122</v>
+        <v>24-117</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
     </row>
     <row r="335" spans="1:13" ht="15">
       <c r="A335">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B335">
+        <f t="shared" si="32"/>
+        <v>118</v>
+      </c>
+      <c r="C335" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B335">
-        <f t="shared" si="31"/>
-        <v>123</v>
-      </c>
-      <c r="C335" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-123</v>
+        <v>24-118</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
     </row>
     <row r="336" spans="1:13" ht="15">
       <c r="A336">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B336">
+        <f t="shared" si="32"/>
+        <v>119</v>
+      </c>
+      <c r="C336" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B336">
-        <f t="shared" si="31"/>
-        <v>124</v>
-      </c>
-      <c r="C336" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-124</v>
+        <v>24-119</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
     </row>
     <row r="337" spans="1:13" ht="15">
       <c r="A337">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B337">
+        <f t="shared" si="32"/>
+        <v>120</v>
+      </c>
+      <c r="C337" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B337">
-        <f t="shared" si="31"/>
-        <v>125</v>
-      </c>
-      <c r="C337" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-125</v>
+        <v>24-120</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
     </row>
     <row r="338" spans="1:13" ht="15">
       <c r="A338">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B338">
+        <f t="shared" si="32"/>
+        <v>121</v>
+      </c>
+      <c r="C338" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B338">
-        <f t="shared" si="31"/>
-        <v>126</v>
-      </c>
-      <c r="C338" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-126</v>
+        <v>24-121</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
     </row>
     <row r="339" spans="1:13" ht="15">
       <c r="A339">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B339">
+        <f t="shared" si="32"/>
+        <v>122</v>
+      </c>
+      <c r="C339" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B339">
-        <f t="shared" si="31"/>
-        <v>127</v>
-      </c>
-      <c r="C339" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-127</v>
+        <v>24-122</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
     </row>
     <row r="340" spans="1:13" ht="15">
       <c r="A340">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B340">
+        <f t="shared" si="32"/>
+        <v>123</v>
+      </c>
+      <c r="C340" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B340">
-        <f t="shared" si="31"/>
-        <v>128</v>
-      </c>
-      <c r="C340" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-128</v>
+        <v>24-123</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
     </row>
     <row r="341" spans="1:13" ht="15">
       <c r="A341">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B341">
+        <f t="shared" si="32"/>
+        <v>124</v>
+      </c>
+      <c r="C341" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B341">
-        <f t="shared" si="31"/>
-        <v>129</v>
-      </c>
-      <c r="C341" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-129</v>
+        <v>24-124</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
     </row>
     <row r="342" spans="1:13" ht="15">
       <c r="A342">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B342">
+        <f t="shared" si="32"/>
+        <v>125</v>
+      </c>
+      <c r="C342" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B342">
-        <f t="shared" si="31"/>
-        <v>130</v>
-      </c>
-      <c r="C342" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-130</v>
+        <v>24-125</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
     </row>
     <row r="343" spans="1:13" ht="15">
       <c r="A343">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B343">
+        <f t="shared" si="32"/>
+        <v>126</v>
+      </c>
+      <c r="C343" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B343">
-        <f t="shared" si="31"/>
-        <v>131</v>
-      </c>
-      <c r="C343" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-131</v>
+        <v>24-126</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
     </row>
     <row r="344" spans="1:13" ht="15">
       <c r="A344">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B344">
+        <f t="shared" si="32"/>
+        <v>127</v>
+      </c>
+      <c r="C344" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B344">
-        <f t="shared" si="31"/>
-        <v>132</v>
-      </c>
-      <c r="C344" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-132</v>
+        <v>24-127</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
     </row>
     <row r="345" spans="1:13" ht="15">
       <c r="A345">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B345">
+        <f t="shared" si="32"/>
+        <v>128</v>
+      </c>
+      <c r="C345" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B345">
-        <f t="shared" si="31"/>
-        <v>133</v>
-      </c>
-      <c r="C345" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-133</v>
+        <v>24-128</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
     </row>
     <row r="346" spans="1:13" ht="15">
       <c r="A346">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B346">
+        <f t="shared" si="32"/>
+        <v>129</v>
+      </c>
+      <c r="C346" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B346">
-        <f t="shared" si="31"/>
-        <v>134</v>
-      </c>
-      <c r="C346" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-134</v>
+        <v>24-129</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
     </row>
     <row r="347" spans="1:13" ht="15">
       <c r="A347">
+        <f t="shared" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="B347">
+        <f t="shared" si="32"/>
+        <v>130</v>
+      </c>
+      <c r="C347" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>23</v>
-      </c>
-      <c r="B347">
-        <f t="shared" si="31"/>
-        <v>135</v>
-      </c>
-      <c r="C347" s="3" t="str">
-        <f t="shared" si="32"/>
-        <v>23-135</v>
+        <v>24-130</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
     </row>
     <row r="348" spans="1:13" ht="15">
       <c r="A348">
-        <f t="shared" si="33"/>
-        <v>23</v>
+        <f t="shared" si="34"/>
+        <v>24</v>
       </c>
       <c r="B348">
-        <f t="shared" ref="B348:B369" si="34">IF(A348=A347,B347+1,1)</f>
-        <v>136</v>
+        <f t="shared" ref="B348:B369" si="35">IF(A348=A347,B347+1,1)</f>
+        <v>131</v>
       </c>
       <c r="C348" s="3" t="str">
-        <f t="shared" ref="C348:C369" si="35">CONCATENATE(A348,"-",B348)</f>
-        <v>23-136</v>
+        <f t="shared" ref="C348:C369" si="36">CONCATENATE(A348,"-",B348)</f>
+        <v>24-131</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
     </row>
     <row r="349" spans="1:13" ht="15">
       <c r="A349">
-        <f t="shared" ref="A349:A369" si="36">A348</f>
-        <v>23</v>
+        <f t="shared" ref="A349:A369" si="37">A348</f>
+        <v>24</v>
       </c>
       <c r="B349">
-        <f t="shared" si="34"/>
-        <v>137</v>
+        <f t="shared" si="35"/>
+        <v>132</v>
       </c>
       <c r="C349" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-137</v>
+        <f t="shared" si="36"/>
+        <v>24-132</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
     </row>
     <row r="350" spans="1:13" ht="15">
       <c r="A350">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B350">
+        <f t="shared" si="35"/>
+        <v>133</v>
+      </c>
+      <c r="C350" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B350">
-        <f t="shared" si="34"/>
-        <v>138</v>
-      </c>
-      <c r="C350" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-138</v>
+        <v>24-133</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
     </row>
     <row r="351" spans="1:13" ht="15">
       <c r="A351">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B351">
+        <f t="shared" si="35"/>
+        <v>134</v>
+      </c>
+      <c r="C351" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B351">
-        <f t="shared" si="34"/>
-        <v>139</v>
-      </c>
-      <c r="C351" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-139</v>
+        <v>24-134</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
     </row>
     <row r="352" spans="1:13" ht="15">
       <c r="A352">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B352">
+        <f t="shared" si="35"/>
+        <v>135</v>
+      </c>
+      <c r="C352" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B352">
-        <f t="shared" si="34"/>
-        <v>140</v>
-      </c>
-      <c r="C352" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-140</v>
+        <v>24-135</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
     </row>
     <row r="353" spans="1:13" ht="15">
       <c r="A353">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B353">
+        <f t="shared" si="35"/>
+        <v>136</v>
+      </c>
+      <c r="C353" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B353">
-        <f t="shared" si="34"/>
-        <v>141</v>
-      </c>
-      <c r="C353" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-141</v>
+        <v>24-136</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
     </row>
     <row r="354" spans="1:13" ht="15">
       <c r="A354">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B354">
+        <f t="shared" si="35"/>
+        <v>137</v>
+      </c>
+      <c r="C354" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B354">
-        <f t="shared" si="34"/>
-        <v>142</v>
-      </c>
-      <c r="C354" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-142</v>
+        <v>24-137</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
     </row>
     <row r="355" spans="1:13" ht="15">
       <c r="A355">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B355">
+        <f t="shared" si="35"/>
+        <v>138</v>
+      </c>
+      <c r="C355" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B355">
-        <f t="shared" si="34"/>
-        <v>143</v>
-      </c>
-      <c r="C355" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-143</v>
+        <v>24-138</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
     </row>
     <row r="356" spans="1:13" ht="15">
       <c r="A356">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B356">
+        <f t="shared" si="35"/>
+        <v>139</v>
+      </c>
+      <c r="C356" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B356">
-        <f t="shared" si="34"/>
-        <v>144</v>
-      </c>
-      <c r="C356" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-144</v>
+        <v>24-139</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
     </row>
     <row r="357" spans="1:13" ht="15">
       <c r="A357">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B357">
+        <f t="shared" si="35"/>
+        <v>140</v>
+      </c>
+      <c r="C357" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B357">
-        <f t="shared" si="34"/>
-        <v>145</v>
-      </c>
-      <c r="C357" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-145</v>
+        <v>24-140</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
     </row>
     <row r="358" spans="1:13" ht="15">
       <c r="A358">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B358">
+        <f t="shared" si="35"/>
+        <v>141</v>
+      </c>
+      <c r="C358" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B358">
-        <f t="shared" si="34"/>
-        <v>146</v>
-      </c>
-      <c r="C358" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-146</v>
+        <v>24-141</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
     </row>
     <row r="359" spans="1:13" ht="15">
       <c r="A359">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B359">
+        <f t="shared" si="35"/>
+        <v>142</v>
+      </c>
+      <c r="C359" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B359">
-        <f t="shared" si="34"/>
-        <v>147</v>
-      </c>
-      <c r="C359" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-147</v>
+        <v>24-142</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
     </row>
     <row r="360" spans="1:13" ht="15">
       <c r="A360">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B360">
+        <f t="shared" si="35"/>
+        <v>143</v>
+      </c>
+      <c r="C360" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B360">
-        <f t="shared" si="34"/>
-        <v>148</v>
-      </c>
-      <c r="C360" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-148</v>
+        <v>24-143</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
     </row>
     <row r="361" spans="1:13" ht="15">
       <c r="A361">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B361">
+        <f t="shared" si="35"/>
+        <v>144</v>
+      </c>
+      <c r="C361" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B361">
-        <f t="shared" si="34"/>
-        <v>149</v>
-      </c>
-      <c r="C361" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-149</v>
+        <v>24-144</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
     </row>
     <row r="362" spans="1:13" ht="15">
       <c r="A362">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B362">
+        <f t="shared" si="35"/>
+        <v>145</v>
+      </c>
+      <c r="C362" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B362">
-        <f t="shared" si="34"/>
-        <v>150</v>
-      </c>
-      <c r="C362" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-150</v>
+        <v>24-145</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
     </row>
     <row r="363" spans="1:13" ht="15">
       <c r="A363">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B363">
+        <f t="shared" si="35"/>
+        <v>146</v>
+      </c>
+      <c r="C363" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B363">
-        <f t="shared" si="34"/>
-        <v>151</v>
-      </c>
-      <c r="C363" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-151</v>
+        <v>24-146</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
     </row>
     <row r="364" spans="1:13" ht="15">
       <c r="A364">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B364">
+        <f t="shared" si="35"/>
+        <v>147</v>
+      </c>
+      <c r="C364" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B364">
-        <f t="shared" si="34"/>
-        <v>152</v>
-      </c>
-      <c r="C364" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-152</v>
+        <v>24-147</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
     </row>
     <row r="365" spans="1:13" ht="15">
       <c r="A365">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B365">
+        <f t="shared" si="35"/>
+        <v>148</v>
+      </c>
+      <c r="C365" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B365">
-        <f t="shared" si="34"/>
-        <v>153</v>
-      </c>
-      <c r="C365" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-153</v>
+        <v>24-148</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
     </row>
     <row r="366" spans="1:13" ht="15">
       <c r="A366">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B366">
+        <f t="shared" si="35"/>
+        <v>149</v>
+      </c>
+      <c r="C366" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B366">
-        <f t="shared" si="34"/>
-        <v>154</v>
-      </c>
-      <c r="C366" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-154</v>
+        <v>24-149</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
     </row>
     <row r="367" spans="1:13" ht="15">
       <c r="A367">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B367">
+        <f t="shared" si="35"/>
+        <v>150</v>
+      </c>
+      <c r="C367" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B367">
-        <f t="shared" si="34"/>
-        <v>155</v>
-      </c>
-      <c r="C367" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-155</v>
+        <v>24-150</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
     </row>
     <row r="368" spans="1:13" ht="15">
       <c r="A368">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B368">
+        <f t="shared" si="35"/>
+        <v>151</v>
+      </c>
+      <c r="C368" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B368">
-        <f t="shared" si="34"/>
-        <v>156</v>
-      </c>
-      <c r="C368" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-156</v>
+        <v>24-151</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
     </row>
     <row r="369" spans="1:13" ht="15">
       <c r="A369">
+        <f t="shared" si="37"/>
+        <v>24</v>
+      </c>
+      <c r="B369">
+        <f t="shared" si="35"/>
+        <v>152</v>
+      </c>
+      <c r="C369" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>23</v>
-      </c>
-      <c r="B369">
-        <f t="shared" si="34"/>
-        <v>157</v>
-      </c>
-      <c r="C369" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>23-157</v>
+        <v>24-152</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
@@ -13619,272 +13821,272 @@
     <mergeCell ref="L178:L181"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K189">
-    <cfRule type="containsBlanks" dxfId="53" priority="58">
+    <cfRule type="containsBlanks" dxfId="59" priority="58">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K189">
-    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K189">
-    <cfRule type="containsText" dxfId="51" priority="60" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K190">
-    <cfRule type="containsBlanks" dxfId="50" priority="55">
+    <cfRule type="containsBlanks" dxfId="56" priority="55">
       <formula>LEN(TRIM(K190))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K190">
-    <cfRule type="containsText" dxfId="49" priority="56" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K190))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K190">
-    <cfRule type="containsText" dxfId="48" priority="57" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K190))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K191">
-    <cfRule type="containsBlanks" dxfId="47" priority="49">
+    <cfRule type="containsBlanks" dxfId="53" priority="49">
       <formula>LEN(TRIM(K191))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K191">
-    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K191))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K191">
-    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K191))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K192">
-    <cfRule type="containsBlanks" dxfId="44" priority="46">
+    <cfRule type="containsBlanks" dxfId="50" priority="46">
       <formula>LEN(TRIM(K192))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K192">
-    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K192))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K192">
-    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K192))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K193">
-    <cfRule type="containsBlanks" dxfId="41" priority="43">
+    <cfRule type="containsBlanks" dxfId="47" priority="43">
       <formula>LEN(TRIM(K193))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K193">
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K193))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K193">
-    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K193))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K195">
-    <cfRule type="containsBlanks" dxfId="38" priority="40">
+    <cfRule type="containsBlanks" dxfId="44" priority="40">
       <formula>LEN(TRIM(K195))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K197">
-    <cfRule type="containsBlanks" dxfId="37" priority="37">
+    <cfRule type="containsBlanks" dxfId="43" priority="37">
       <formula>LEN(TRIM(K197))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K199">
-    <cfRule type="containsBlanks" dxfId="36" priority="34">
+    <cfRule type="containsBlanks" dxfId="42" priority="34">
       <formula>LEN(TRIM(K199))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsBlanks" dxfId="35" priority="31">
+    <cfRule type="containsBlanks" dxfId="41" priority="31">
       <formula>LEN(TRIM(K200))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsBlanks" dxfId="34" priority="28">
+    <cfRule type="containsBlanks" dxfId="40" priority="28">
       <formula>LEN(TRIM(K202))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="33" priority="25">
+    <cfRule type="containsBlanks" dxfId="39" priority="25">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="32" priority="22">
+  <conditionalFormatting sqref="K206:K219">
+    <cfRule type="containsBlanks" dxfId="38" priority="22">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K196">
-    <cfRule type="containsBlanks" dxfId="31" priority="16">
+    <cfRule type="containsBlanks" dxfId="37" priority="16">
       <formula>LEN(TRIM(K196))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K195">
-    <cfRule type="containsText" dxfId="30" priority="41" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K195))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K195">
-    <cfRule type="containsText" dxfId="29" priority="42" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="35" priority="42" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K195))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K198">
-    <cfRule type="containsBlanks" dxfId="28" priority="13">
+    <cfRule type="containsBlanks" dxfId="34" priority="13">
       <formula>LEN(TRIM(K198))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K197">
-    <cfRule type="containsText" dxfId="27" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="33" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K197))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K197">
-    <cfRule type="containsText" dxfId="26" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="32" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K197))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K194">
-    <cfRule type="containsBlanks" dxfId="25" priority="10">
+    <cfRule type="containsBlanks" dxfId="31" priority="10">
       <formula>LEN(TRIM(K194))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K199">
-    <cfRule type="containsText" dxfId="24" priority="35" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K199))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K199">
-    <cfRule type="containsText" dxfId="23" priority="36" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K199))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsBlanks" dxfId="22" priority="7">
+    <cfRule type="containsBlanks" dxfId="28" priority="7">
       <formula>LEN(TRIM(K201))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="21" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="20" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="26" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsBlanks" dxfId="19" priority="4">
+    <cfRule type="containsBlanks" dxfId="25" priority="4">
       <formula>LEN(TRIM(K203))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="18" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="24" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="17" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="23" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="16" priority="1">
+    <cfRule type="containsBlanks" dxfId="22" priority="1">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="14" priority="27" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="20" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K206:K219">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="12" priority="24" operator="containsText" text="fail">
+  <conditionalFormatting sqref="K206:K219">
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K196">
-    <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K196))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K196">
-    <cfRule type="containsText" dxfId="10" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K196))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K198">
-    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K198))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K198">
-    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K198))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K194">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K194))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K194">
-    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K194))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added manual system test to check rcptt synoptics not added to version control
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="278">
   <si>
     <t>Test Number</t>
   </si>
@@ -848,6 +848,9 @@
   </si>
   <si>
     <t>Edit a config (not current) by setting some IOC macros. Load the config. Verify the new macro values are displayed in the config and that they are applied to the respective IOCs</t>
+  </si>
+  <si>
+    <t>Synoptics starting with rcptt_ are not added to a repo</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1121,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="60">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2172,11 +2259,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1057"/>
+  <dimension ref="A1:N1058"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I103" sqref="I103"/>
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I223" sqref="I223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4292,11 +4379,11 @@
         <v>10</v>
       </c>
       <c r="B72">
-        <f t="shared" ref="B72:B138" si="6">IF(A72=A71,B71+1,1)</f>
+        <f t="shared" ref="B72:B104" si="6">IF(A72=A71,B71+1,1)</f>
         <v>2</v>
       </c>
       <c r="C72" s="3" t="str">
-        <f t="shared" ref="C72:C138" si="7">CONCATENATE(A72,"-",B72)</f>
+        <f t="shared" ref="C72:C104" si="7">CONCATENATE(A72,"-",B72)</f>
         <v>10-2</v>
       </c>
       <c r="D72" s="5"/>
@@ -6455,11 +6542,11 @@
         <v>16</v>
       </c>
       <c r="B149">
-        <f t="shared" ref="B139:B220" si="16">IF(A149=A148,B148+1,1)</f>
+        <f t="shared" ref="B149:B221" si="16">IF(A149=A148,B148+1,1)</f>
         <v>1</v>
       </c>
       <c r="C149" s="3" t="str">
-        <f t="shared" ref="C139:C219" si="17">CONCATENATE(A149,"-",B149)</f>
+        <f t="shared" ref="C149:C220" si="17">CONCATENATE(A149,"-",B149)</f>
         <v>16-1</v>
       </c>
       <c r="D149" s="5"/>
@@ -6481,7 +6568,7 @@
     </row>
     <row r="150" spans="1:13" ht="15">
       <c r="A150">
-        <f t="shared" ref="A140:A221" si="18">A149</f>
+        <f t="shared" ref="A150:A222" si="18">A149</f>
         <v>16</v>
       </c>
       <c r="B150">
@@ -8562,12 +8649,11 @@
         <v>24</v>
       </c>
       <c r="B219">
-        <f t="shared" si="16"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C219" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v>24-1</v>
+        <f t="shared" ref="C219" si="33">CONCATENATE(A219,"-",B219)</f>
+        <v>24-6</v>
       </c>
       <c r="D219" s="23"/>
       <c r="E219" s="23"/>
@@ -8576,10 +8662,10 @@
         <v>63</v>
       </c>
       <c r="H219" s="24" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I219" s="25" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="J219" s="23"/>
       <c r="K219" s="21"/>
@@ -8588,16 +8674,15 @@
     </row>
     <row r="220" spans="1:13" ht="26.25">
       <c r="A220">
-        <f t="shared" si="18"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B220">
-        <f t="shared" si="16"/>
-        <v>2</v>
+        <f>IF(A220=A218,B218+1,1)</f>
+        <v>1</v>
       </c>
       <c r="C220" s="3" t="str">
-        <f t="shared" ref="C220" si="33">CONCATENATE(A220,"-",B220)</f>
-        <v>24-2</v>
+        <f t="shared" si="17"/>
+        <v>25-1</v>
       </c>
       <c r="D220" s="23"/>
       <c r="E220" s="23"/>
@@ -8609,2414 +8694,2440 @@
         <v>272</v>
       </c>
       <c r="I220" s="25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J220" s="23"/>
       <c r="K220" s="21"/>
       <c r="L220" s="26"/>
       <c r="M220" s="6"/>
     </row>
-    <row r="221" spans="1:13" ht="15">
+    <row r="221" spans="1:13" ht="26.25">
       <c r="A221">
         <f t="shared" si="18"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B221">
-        <f t="shared" ref="B221:B284" si="34">IF(A221=A220,B220+1,1)</f>
-        <v>3</v>
+        <f t="shared" si="16"/>
+        <v>2</v>
       </c>
       <c r="C221" s="3" t="str">
-        <f t="shared" ref="C221:C284" si="35">CONCATENATE(A221,"-",B221)</f>
-        <v>24-3</v>
-      </c>
-      <c r="L221" s="6"/>
+        <f t="shared" ref="C221" si="34">CONCATENATE(A221,"-",B221)</f>
+        <v>25-2</v>
+      </c>
+      <c r="D221" s="23"/>
+      <c r="E221" s="23"/>
+      <c r="F221" s="23"/>
+      <c r="G221" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H221" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="I221" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="J221" s="23"/>
+      <c r="K221" s="21"/>
+      <c r="L221" s="26"/>
       <c r="M221" s="6"/>
     </row>
     <row r="222" spans="1:13" ht="15">
       <c r="A222">
-        <f t="shared" ref="A222:A285" si="36">A221</f>
-        <v>24</v>
+        <f t="shared" si="18"/>
+        <v>25</v>
       </c>
       <c r="B222">
-        <f t="shared" si="34"/>
-        <v>4</v>
+        <f t="shared" ref="B222:B285" si="35">IF(A222=A221,B221+1,1)</f>
+        <v>3</v>
       </c>
       <c r="C222" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-4</v>
+        <f t="shared" ref="C222:C285" si="36">CONCATENATE(A222,"-",B222)</f>
+        <v>25-3</v>
       </c>
       <c r="L222" s="6"/>
       <c r="M222" s="6"/>
     </row>
     <row r="223" spans="1:13" ht="15">
       <c r="A223">
+        <f t="shared" ref="A223:A286" si="37">A222</f>
+        <v>25</v>
+      </c>
+      <c r="B223">
+        <f t="shared" si="35"/>
+        <v>4</v>
+      </c>
+      <c r="C223" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B223">
-        <f t="shared" si="34"/>
-        <v>5</v>
-      </c>
-      <c r="C223" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-5</v>
+        <v>25-4</v>
       </c>
       <c r="L223" s="6"/>
       <c r="M223" s="6"/>
     </row>
     <row r="224" spans="1:13" ht="15">
       <c r="A224">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B224">
+        <f t="shared" si="35"/>
+        <v>5</v>
+      </c>
+      <c r="C224" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B224">
-        <f t="shared" si="34"/>
-        <v>6</v>
-      </c>
-      <c r="C224" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-6</v>
+        <v>25-5</v>
       </c>
       <c r="L224" s="6"/>
       <c r="M224" s="6"/>
     </row>
     <row r="225" spans="1:13" ht="15">
       <c r="A225">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B225">
+        <f t="shared" si="35"/>
+        <v>6</v>
+      </c>
+      <c r="C225" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B225">
-        <f t="shared" si="34"/>
-        <v>7</v>
-      </c>
-      <c r="C225" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-7</v>
+        <v>25-6</v>
       </c>
       <c r="L225" s="6"/>
       <c r="M225" s="6"/>
     </row>
     <row r="226" spans="1:13" ht="15">
       <c r="A226">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B226">
+        <f t="shared" si="35"/>
+        <v>7</v>
+      </c>
+      <c r="C226" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B226">
-        <f t="shared" si="34"/>
-        <v>8</v>
-      </c>
-      <c r="C226" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-8</v>
+        <v>25-7</v>
       </c>
       <c r="L226" s="6"/>
       <c r="M226" s="6"/>
     </row>
     <row r="227" spans="1:13" ht="15">
       <c r="A227">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B227">
+        <f t="shared" si="35"/>
+        <v>8</v>
+      </c>
+      <c r="C227" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B227">
-        <f t="shared" si="34"/>
-        <v>9</v>
-      </c>
-      <c r="C227" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-9</v>
+        <v>25-8</v>
       </c>
       <c r="L227" s="6"/>
       <c r="M227" s="6"/>
     </row>
     <row r="228" spans="1:13" ht="15">
       <c r="A228">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B228">
+        <f t="shared" si="35"/>
+        <v>9</v>
+      </c>
+      <c r="C228" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B228">
-        <f t="shared" si="34"/>
-        <v>10</v>
-      </c>
-      <c r="C228" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-10</v>
+        <v>25-9</v>
       </c>
       <c r="L228" s="6"/>
       <c r="M228" s="6"/>
     </row>
     <row r="229" spans="1:13" ht="15">
       <c r="A229">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B229">
+        <f t="shared" si="35"/>
+        <v>10</v>
+      </c>
+      <c r="C229" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B229">
-        <f t="shared" si="34"/>
-        <v>11</v>
-      </c>
-      <c r="C229" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-11</v>
+        <v>25-10</v>
       </c>
       <c r="L229" s="6"/>
       <c r="M229" s="6"/>
     </row>
     <row r="230" spans="1:13" ht="15">
       <c r="A230">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B230">
+        <f t="shared" si="35"/>
+        <v>11</v>
+      </c>
+      <c r="C230" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B230">
-        <f t="shared" si="34"/>
-        <v>12</v>
-      </c>
-      <c r="C230" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-12</v>
+        <v>25-11</v>
       </c>
       <c r="L230" s="6"/>
       <c r="M230" s="6"/>
     </row>
     <row r="231" spans="1:13" ht="15">
       <c r="A231">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B231">
+        <f t="shared" si="35"/>
+        <v>12</v>
+      </c>
+      <c r="C231" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B231">
-        <f t="shared" si="34"/>
-        <v>13</v>
-      </c>
-      <c r="C231" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-13</v>
+        <v>25-12</v>
       </c>
       <c r="L231" s="6"/>
       <c r="M231" s="6"/>
     </row>
     <row r="232" spans="1:13" ht="15">
       <c r="A232">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B232">
+        <f t="shared" si="35"/>
+        <v>13</v>
+      </c>
+      <c r="C232" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B232">
-        <f t="shared" si="34"/>
-        <v>14</v>
-      </c>
-      <c r="C232" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-14</v>
+        <v>25-13</v>
       </c>
       <c r="L232" s="6"/>
       <c r="M232" s="6"/>
     </row>
     <row r="233" spans="1:13" ht="15">
       <c r="A233">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B233">
+        <f t="shared" si="35"/>
+        <v>14</v>
+      </c>
+      <c r="C233" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B233">
-        <f t="shared" si="34"/>
-        <v>15</v>
-      </c>
-      <c r="C233" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-15</v>
+        <v>25-14</v>
       </c>
       <c r="L233" s="6"/>
       <c r="M233" s="6"/>
     </row>
     <row r="234" spans="1:13" ht="15">
       <c r="A234">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B234">
+        <f t="shared" si="35"/>
+        <v>15</v>
+      </c>
+      <c r="C234" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B234">
-        <f t="shared" si="34"/>
-        <v>16</v>
-      </c>
-      <c r="C234" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-16</v>
+        <v>25-15</v>
       </c>
       <c r="L234" s="6"/>
       <c r="M234" s="6"/>
     </row>
     <row r="235" spans="1:13" ht="15">
       <c r="A235">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B235">
+        <f t="shared" si="35"/>
+        <v>16</v>
+      </c>
+      <c r="C235" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B235">
-        <f t="shared" si="34"/>
-        <v>17</v>
-      </c>
-      <c r="C235" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-17</v>
+        <v>25-16</v>
       </c>
       <c r="L235" s="6"/>
       <c r="M235" s="6"/>
     </row>
     <row r="236" spans="1:13" ht="15">
       <c r="A236">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B236">
+        <f t="shared" si="35"/>
+        <v>17</v>
+      </c>
+      <c r="C236" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B236">
-        <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="C236" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-18</v>
+        <v>25-17</v>
       </c>
       <c r="L236" s="6"/>
       <c r="M236" s="6"/>
     </row>
     <row r="237" spans="1:13" ht="15">
       <c r="A237">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B237">
+        <f t="shared" si="35"/>
+        <v>18</v>
+      </c>
+      <c r="C237" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B237">
-        <f t="shared" si="34"/>
-        <v>19</v>
-      </c>
-      <c r="C237" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-19</v>
+        <v>25-18</v>
       </c>
       <c r="L237" s="6"/>
       <c r="M237" s="6"/>
     </row>
     <row r="238" spans="1:13" ht="15">
       <c r="A238">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B238">
+        <f t="shared" si="35"/>
+        <v>19</v>
+      </c>
+      <c r="C238" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B238">
-        <f t="shared" si="34"/>
-        <v>20</v>
-      </c>
-      <c r="C238" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-20</v>
+        <v>25-19</v>
       </c>
       <c r="L238" s="6"/>
       <c r="M238" s="6"/>
     </row>
     <row r="239" spans="1:13" ht="15">
       <c r="A239">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B239">
+        <f t="shared" si="35"/>
+        <v>20</v>
+      </c>
+      <c r="C239" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B239">
-        <f t="shared" si="34"/>
-        <v>21</v>
-      </c>
-      <c r="C239" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-21</v>
+        <v>25-20</v>
       </c>
       <c r="L239" s="6"/>
       <c r="M239" s="6"/>
     </row>
     <row r="240" spans="1:13" ht="15">
       <c r="A240">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B240">
+        <f t="shared" si="35"/>
+        <v>21</v>
+      </c>
+      <c r="C240" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B240">
-        <f t="shared" si="34"/>
-        <v>22</v>
-      </c>
-      <c r="C240" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-22</v>
+        <v>25-21</v>
       </c>
       <c r="L240" s="6"/>
       <c r="M240" s="6"/>
     </row>
     <row r="241" spans="1:13" ht="15">
       <c r="A241">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B241">
+        <f t="shared" si="35"/>
+        <v>22</v>
+      </c>
+      <c r="C241" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B241">
-        <f t="shared" si="34"/>
-        <v>23</v>
-      </c>
-      <c r="C241" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-23</v>
+        <v>25-22</v>
       </c>
       <c r="L241" s="6"/>
       <c r="M241" s="6"/>
     </row>
     <row r="242" spans="1:13" ht="15">
       <c r="A242">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B242">
+        <f t="shared" si="35"/>
+        <v>23</v>
+      </c>
+      <c r="C242" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B242">
-        <f t="shared" si="34"/>
-        <v>24</v>
-      </c>
-      <c r="C242" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-24</v>
+        <v>25-23</v>
       </c>
       <c r="L242" s="6"/>
       <c r="M242" s="6"/>
     </row>
     <row r="243" spans="1:13" ht="15">
       <c r="A243">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B243">
+        <f t="shared" si="35"/>
+        <v>24</v>
+      </c>
+      <c r="C243" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B243">
-        <f t="shared" si="34"/>
-        <v>25</v>
-      </c>
-      <c r="C243" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-25</v>
+        <v>25-24</v>
       </c>
       <c r="L243" s="6"/>
       <c r="M243" s="6"/>
     </row>
     <row r="244" spans="1:13" ht="15">
       <c r="A244">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B244">
+        <f t="shared" si="35"/>
+        <v>25</v>
+      </c>
+      <c r="C244" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B244">
-        <f t="shared" si="34"/>
-        <v>26</v>
-      </c>
-      <c r="C244" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-26</v>
+        <v>25-25</v>
       </c>
       <c r="L244" s="6"/>
       <c r="M244" s="6"/>
     </row>
     <row r="245" spans="1:13" ht="15">
       <c r="A245">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B245">
+        <f t="shared" si="35"/>
+        <v>26</v>
+      </c>
+      <c r="C245" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B245">
-        <f t="shared" si="34"/>
-        <v>27</v>
-      </c>
-      <c r="C245" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-27</v>
+        <v>25-26</v>
       </c>
       <c r="L245" s="6"/>
       <c r="M245" s="6"/>
     </row>
     <row r="246" spans="1:13" ht="15">
       <c r="A246">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B246">
+        <f t="shared" si="35"/>
+        <v>27</v>
+      </c>
+      <c r="C246" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B246">
-        <f t="shared" si="34"/>
-        <v>28</v>
-      </c>
-      <c r="C246" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-28</v>
+        <v>25-27</v>
       </c>
       <c r="L246" s="6"/>
       <c r="M246" s="6"/>
     </row>
     <row r="247" spans="1:13" ht="15">
       <c r="A247">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B247">
+        <f t="shared" si="35"/>
+        <v>28</v>
+      </c>
+      <c r="C247" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B247">
-        <f t="shared" si="34"/>
-        <v>29</v>
-      </c>
-      <c r="C247" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-29</v>
+        <v>25-28</v>
       </c>
       <c r="L247" s="6"/>
       <c r="M247" s="6"/>
     </row>
     <row r="248" spans="1:13" ht="15">
       <c r="A248">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B248">
+        <f t="shared" si="35"/>
+        <v>29</v>
+      </c>
+      <c r="C248" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B248">
-        <f t="shared" si="34"/>
-        <v>30</v>
-      </c>
-      <c r="C248" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-30</v>
+        <v>25-29</v>
       </c>
       <c r="L248" s="6"/>
       <c r="M248" s="6"/>
     </row>
     <row r="249" spans="1:13" ht="15">
       <c r="A249">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B249">
+        <f t="shared" si="35"/>
+        <v>30</v>
+      </c>
+      <c r="C249" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B249">
-        <f t="shared" si="34"/>
-        <v>31</v>
-      </c>
-      <c r="C249" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-31</v>
+        <v>25-30</v>
       </c>
       <c r="L249" s="6"/>
       <c r="M249" s="6"/>
     </row>
     <row r="250" spans="1:13" ht="15">
       <c r="A250">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B250">
+        <f t="shared" si="35"/>
+        <v>31</v>
+      </c>
+      <c r="C250" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B250">
-        <f t="shared" si="34"/>
-        <v>32</v>
-      </c>
-      <c r="C250" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-32</v>
+        <v>25-31</v>
       </c>
       <c r="L250" s="6"/>
       <c r="M250" s="6"/>
     </row>
     <row r="251" spans="1:13" ht="15">
       <c r="A251">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B251">
+        <f t="shared" si="35"/>
+        <v>32</v>
+      </c>
+      <c r="C251" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B251">
-        <f t="shared" si="34"/>
-        <v>33</v>
-      </c>
-      <c r="C251" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-33</v>
+        <v>25-32</v>
       </c>
       <c r="L251" s="6"/>
       <c r="M251" s="6"/>
     </row>
     <row r="252" spans="1:13" ht="15">
       <c r="A252">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B252">
+        <f t="shared" si="35"/>
+        <v>33</v>
+      </c>
+      <c r="C252" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B252">
-        <f t="shared" si="34"/>
-        <v>34</v>
-      </c>
-      <c r="C252" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-34</v>
+        <v>25-33</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
     </row>
     <row r="253" spans="1:13" ht="15">
       <c r="A253">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B253">
+        <f t="shared" si="35"/>
+        <v>34</v>
+      </c>
+      <c r="C253" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B253">
-        <f t="shared" si="34"/>
-        <v>35</v>
-      </c>
-      <c r="C253" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-35</v>
+        <v>25-34</v>
       </c>
       <c r="L253" s="6"/>
       <c r="M253" s="6"/>
     </row>
     <row r="254" spans="1:13" ht="15">
       <c r="A254">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B254">
+        <f t="shared" si="35"/>
+        <v>35</v>
+      </c>
+      <c r="C254" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B254">
-        <f t="shared" si="34"/>
-        <v>36</v>
-      </c>
-      <c r="C254" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-36</v>
+        <v>25-35</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
     </row>
     <row r="255" spans="1:13" ht="15">
       <c r="A255">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B255">
+        <f t="shared" si="35"/>
+        <v>36</v>
+      </c>
+      <c r="C255" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B255">
-        <f t="shared" si="34"/>
-        <v>37</v>
-      </c>
-      <c r="C255" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-37</v>
+        <v>25-36</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
     </row>
     <row r="256" spans="1:13" ht="15">
       <c r="A256">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B256">
+        <f t="shared" si="35"/>
+        <v>37</v>
+      </c>
+      <c r="C256" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B256">
-        <f t="shared" si="34"/>
-        <v>38</v>
-      </c>
-      <c r="C256" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-38</v>
+        <v>25-37</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
     </row>
     <row r="257" spans="1:13" ht="15">
       <c r="A257">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B257">
+        <f t="shared" si="35"/>
+        <v>38</v>
+      </c>
+      <c r="C257" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B257">
-        <f t="shared" si="34"/>
-        <v>39</v>
-      </c>
-      <c r="C257" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-39</v>
+        <v>25-38</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
     </row>
     <row r="258" spans="1:13" ht="15">
       <c r="A258">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B258">
+        <f t="shared" si="35"/>
+        <v>39</v>
+      </c>
+      <c r="C258" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B258">
-        <f t="shared" si="34"/>
-        <v>40</v>
-      </c>
-      <c r="C258" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-40</v>
+        <v>25-39</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
     </row>
     <row r="259" spans="1:13" ht="15">
       <c r="A259">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B259">
+        <f t="shared" si="35"/>
+        <v>40</v>
+      </c>
+      <c r="C259" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B259">
-        <f t="shared" si="34"/>
-        <v>41</v>
-      </c>
-      <c r="C259" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-41</v>
+        <v>25-40</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
     </row>
     <row r="260" spans="1:13" ht="15">
       <c r="A260">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B260">
+        <f t="shared" si="35"/>
+        <v>41</v>
+      </c>
+      <c r="C260" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B260">
-        <f t="shared" si="34"/>
-        <v>42</v>
-      </c>
-      <c r="C260" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-42</v>
+        <v>25-41</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
     </row>
     <row r="261" spans="1:13" ht="15">
       <c r="A261">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B261">
+        <f t="shared" si="35"/>
+        <v>42</v>
+      </c>
+      <c r="C261" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B261">
-        <f t="shared" si="34"/>
-        <v>43</v>
-      </c>
-      <c r="C261" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-43</v>
+        <v>25-42</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
     </row>
     <row r="262" spans="1:13" ht="15">
       <c r="A262">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B262">
+        <f t="shared" si="35"/>
+        <v>43</v>
+      </c>
+      <c r="C262" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B262">
-        <f t="shared" si="34"/>
-        <v>44</v>
-      </c>
-      <c r="C262" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-44</v>
+        <v>25-43</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
     </row>
     <row r="263" spans="1:13" ht="15">
       <c r="A263">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B263">
+        <f t="shared" si="35"/>
+        <v>44</v>
+      </c>
+      <c r="C263" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B263">
-        <f t="shared" si="34"/>
-        <v>45</v>
-      </c>
-      <c r="C263" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-45</v>
+        <v>25-44</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
     </row>
     <row r="264" spans="1:13" ht="15">
       <c r="A264">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B264">
+        <f t="shared" si="35"/>
+        <v>45</v>
+      </c>
+      <c r="C264" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B264">
-        <f t="shared" si="34"/>
-        <v>46</v>
-      </c>
-      <c r="C264" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-46</v>
+        <v>25-45</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
     </row>
     <row r="265" spans="1:13" ht="15">
       <c r="A265">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B265">
+        <f t="shared" si="35"/>
+        <v>46</v>
+      </c>
+      <c r="C265" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B265">
-        <f t="shared" si="34"/>
-        <v>47</v>
-      </c>
-      <c r="C265" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-47</v>
+        <v>25-46</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
     </row>
     <row r="266" spans="1:13" ht="15">
       <c r="A266">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B266">
+        <f t="shared" si="35"/>
+        <v>47</v>
+      </c>
+      <c r="C266" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B266">
-        <f t="shared" si="34"/>
-        <v>48</v>
-      </c>
-      <c r="C266" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-48</v>
+        <v>25-47</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
     </row>
     <row r="267" spans="1:13" ht="15">
       <c r="A267">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B267">
+        <f t="shared" si="35"/>
+        <v>48</v>
+      </c>
+      <c r="C267" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B267">
-        <f t="shared" si="34"/>
-        <v>49</v>
-      </c>
-      <c r="C267" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-49</v>
+        <v>25-48</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
     </row>
     <row r="268" spans="1:13" ht="15">
       <c r="A268">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B268">
+        <f t="shared" si="35"/>
+        <v>49</v>
+      </c>
+      <c r="C268" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B268">
-        <f t="shared" si="34"/>
-        <v>50</v>
-      </c>
-      <c r="C268" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-50</v>
+        <v>25-49</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
     </row>
     <row r="269" spans="1:13" ht="15">
       <c r="A269">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B269">
+        <f t="shared" si="35"/>
+        <v>50</v>
+      </c>
+      <c r="C269" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B269">
-        <f t="shared" si="34"/>
-        <v>51</v>
-      </c>
-      <c r="C269" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-51</v>
+        <v>25-50</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
     </row>
     <row r="270" spans="1:13" ht="15">
       <c r="A270">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B270">
+        <f t="shared" si="35"/>
+        <v>51</v>
+      </c>
+      <c r="C270" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B270">
-        <f t="shared" si="34"/>
-        <v>52</v>
-      </c>
-      <c r="C270" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-52</v>
+        <v>25-51</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
     </row>
     <row r="271" spans="1:13" ht="15">
       <c r="A271">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B271">
+        <f t="shared" si="35"/>
+        <v>52</v>
+      </c>
+      <c r="C271" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B271">
-        <f t="shared" si="34"/>
-        <v>53</v>
-      </c>
-      <c r="C271" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-53</v>
+        <v>25-52</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
     </row>
     <row r="272" spans="1:13" ht="15">
       <c r="A272">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B272">
+        <f t="shared" si="35"/>
+        <v>53</v>
+      </c>
+      <c r="C272" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B272">
-        <f t="shared" si="34"/>
-        <v>54</v>
-      </c>
-      <c r="C272" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-54</v>
+        <v>25-53</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
     </row>
     <row r="273" spans="1:13" ht="15">
       <c r="A273">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B273">
+        <f t="shared" si="35"/>
+        <v>54</v>
+      </c>
+      <c r="C273" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B273">
-        <f t="shared" si="34"/>
-        <v>55</v>
-      </c>
-      <c r="C273" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-55</v>
+        <v>25-54</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
     </row>
     <row r="274" spans="1:13" ht="15">
       <c r="A274">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B274">
+        <f t="shared" si="35"/>
+        <v>55</v>
+      </c>
+      <c r="C274" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B274">
-        <f t="shared" si="34"/>
-        <v>56</v>
-      </c>
-      <c r="C274" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-56</v>
+        <v>25-55</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
     </row>
     <row r="275" spans="1:13" ht="15">
       <c r="A275">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B275">
+        <f t="shared" si="35"/>
+        <v>56</v>
+      </c>
+      <c r="C275" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B275">
-        <f t="shared" si="34"/>
-        <v>57</v>
-      </c>
-      <c r="C275" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-57</v>
+        <v>25-56</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
     </row>
     <row r="276" spans="1:13" ht="15">
       <c r="A276">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B276">
+        <f t="shared" si="35"/>
+        <v>57</v>
+      </c>
+      <c r="C276" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B276">
-        <f t="shared" si="34"/>
-        <v>58</v>
-      </c>
-      <c r="C276" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-58</v>
+        <v>25-57</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
     </row>
     <row r="277" spans="1:13" ht="15">
       <c r="A277">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B277">
+        <f t="shared" si="35"/>
+        <v>58</v>
+      </c>
+      <c r="C277" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B277">
-        <f t="shared" si="34"/>
-        <v>59</v>
-      </c>
-      <c r="C277" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-59</v>
+        <v>25-58</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
     </row>
     <row r="278" spans="1:13" ht="15">
       <c r="A278">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B278">
+        <f t="shared" si="35"/>
+        <v>59</v>
+      </c>
+      <c r="C278" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B278">
-        <f t="shared" si="34"/>
-        <v>60</v>
-      </c>
-      <c r="C278" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-60</v>
+        <v>25-59</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
     </row>
     <row r="279" spans="1:13" ht="15">
       <c r="A279">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B279">
+        <f t="shared" si="35"/>
+        <v>60</v>
+      </c>
+      <c r="C279" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B279">
-        <f t="shared" si="34"/>
-        <v>61</v>
-      </c>
-      <c r="C279" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-61</v>
+        <v>25-60</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
     </row>
     <row r="280" spans="1:13" ht="15">
       <c r="A280">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B280">
+        <f t="shared" si="35"/>
+        <v>61</v>
+      </c>
+      <c r="C280" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B280">
-        <f t="shared" si="34"/>
-        <v>62</v>
-      </c>
-      <c r="C280" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-62</v>
+        <v>25-61</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
     </row>
     <row r="281" spans="1:13" ht="15">
       <c r="A281">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B281">
+        <f t="shared" si="35"/>
+        <v>62</v>
+      </c>
+      <c r="C281" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B281">
-        <f t="shared" si="34"/>
-        <v>63</v>
-      </c>
-      <c r="C281" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-63</v>
+        <v>25-62</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
     </row>
     <row r="282" spans="1:13" ht="15">
       <c r="A282">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B282">
+        <f t="shared" si="35"/>
+        <v>63</v>
+      </c>
+      <c r="C282" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B282">
-        <f t="shared" si="34"/>
-        <v>64</v>
-      </c>
-      <c r="C282" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-64</v>
+        <v>25-63</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
     </row>
     <row r="283" spans="1:13" ht="15">
       <c r="A283">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B283">
+        <f t="shared" si="35"/>
+        <v>64</v>
+      </c>
+      <c r="C283" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B283">
-        <f t="shared" si="34"/>
-        <v>65</v>
-      </c>
-      <c r="C283" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-65</v>
+        <v>25-64</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
     </row>
     <row r="284" spans="1:13" ht="15">
       <c r="A284">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B284">
+        <f t="shared" si="35"/>
+        <v>65</v>
+      </c>
+      <c r="C284" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B284">
-        <f t="shared" si="34"/>
-        <v>66</v>
-      </c>
-      <c r="C284" s="3" t="str">
-        <f t="shared" si="35"/>
-        <v>24-66</v>
+        <v>25-65</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
     </row>
     <row r="285" spans="1:13" ht="15">
       <c r="A285">
+        <f t="shared" si="37"/>
+        <v>25</v>
+      </c>
+      <c r="B285">
+        <f t="shared" si="35"/>
+        <v>66</v>
+      </c>
+      <c r="C285" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>24</v>
-      </c>
-      <c r="B285">
-        <f t="shared" ref="B285:B348" si="37">IF(A285=A284,B284+1,1)</f>
-        <v>67</v>
-      </c>
-      <c r="C285" s="3" t="str">
-        <f t="shared" ref="C285:C348" si="38">CONCATENATE(A285,"-",B285)</f>
-        <v>24-67</v>
+        <v>25-66</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
     </row>
     <row r="286" spans="1:13" ht="15">
       <c r="A286">
-        <f t="shared" ref="A286:A349" si="39">A285</f>
-        <v>24</v>
+        <f t="shared" si="37"/>
+        <v>25</v>
       </c>
       <c r="B286">
-        <f t="shared" si="37"/>
-        <v>68</v>
+        <f t="shared" ref="B286:B349" si="38">IF(A286=A285,B285+1,1)</f>
+        <v>67</v>
       </c>
       <c r="C286" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-68</v>
+        <f t="shared" ref="C286:C349" si="39">CONCATENATE(A286,"-",B286)</f>
+        <v>25-67</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
     </row>
     <row r="287" spans="1:13" ht="15">
       <c r="A287">
+        <f t="shared" ref="A287:A350" si="40">A286</f>
+        <v>25</v>
+      </c>
+      <c r="B287">
+        <f t="shared" si="38"/>
+        <v>68</v>
+      </c>
+      <c r="C287" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B287">
-        <f t="shared" si="37"/>
-        <v>69</v>
-      </c>
-      <c r="C287" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-69</v>
+        <v>25-68</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
     </row>
     <row r="288" spans="1:13" ht="15">
       <c r="A288">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B288">
+        <f t="shared" si="38"/>
+        <v>69</v>
+      </c>
+      <c r="C288" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B288">
-        <f t="shared" si="37"/>
-        <v>70</v>
-      </c>
-      <c r="C288" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-70</v>
+        <v>25-69</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
     </row>
     <row r="289" spans="1:13" ht="15">
       <c r="A289">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B289">
+        <f t="shared" si="38"/>
+        <v>70</v>
+      </c>
+      <c r="C289" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B289">
-        <f t="shared" si="37"/>
-        <v>71</v>
-      </c>
-      <c r="C289" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-71</v>
+        <v>25-70</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
     </row>
     <row r="290" spans="1:13" ht="15">
       <c r="A290">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B290">
+        <f t="shared" si="38"/>
+        <v>71</v>
+      </c>
+      <c r="C290" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B290">
-        <f t="shared" si="37"/>
-        <v>72</v>
-      </c>
-      <c r="C290" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-72</v>
+        <v>25-71</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
     </row>
     <row r="291" spans="1:13" ht="15">
       <c r="A291">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B291">
+        <f t="shared" si="38"/>
+        <v>72</v>
+      </c>
+      <c r="C291" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B291">
-        <f t="shared" si="37"/>
-        <v>73</v>
-      </c>
-      <c r="C291" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-73</v>
+        <v>25-72</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
     </row>
     <row r="292" spans="1:13" ht="15">
       <c r="A292">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B292">
+        <f t="shared" si="38"/>
+        <v>73</v>
+      </c>
+      <c r="C292" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B292">
-        <f t="shared" si="37"/>
-        <v>74</v>
-      </c>
-      <c r="C292" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-74</v>
+        <v>25-73</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
     </row>
     <row r="293" spans="1:13" ht="15">
       <c r="A293">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B293">
+        <f t="shared" si="38"/>
+        <v>74</v>
+      </c>
+      <c r="C293" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B293">
-        <f t="shared" si="37"/>
-        <v>75</v>
-      </c>
-      <c r="C293" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-75</v>
+        <v>25-74</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
     </row>
     <row r="294" spans="1:13" ht="15">
       <c r="A294">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B294">
+        <f t="shared" si="38"/>
+        <v>75</v>
+      </c>
+      <c r="C294" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B294">
-        <f t="shared" si="37"/>
-        <v>76</v>
-      </c>
-      <c r="C294" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-76</v>
+        <v>25-75</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
     </row>
     <row r="295" spans="1:13" ht="15">
       <c r="A295">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B295">
+        <f t="shared" si="38"/>
+        <v>76</v>
+      </c>
+      <c r="C295" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B295">
-        <f t="shared" si="37"/>
-        <v>77</v>
-      </c>
-      <c r="C295" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-77</v>
+        <v>25-76</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
     </row>
     <row r="296" spans="1:13" ht="15">
       <c r="A296">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B296">
+        <f t="shared" si="38"/>
+        <v>77</v>
+      </c>
+      <c r="C296" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B296">
-        <f t="shared" si="37"/>
-        <v>78</v>
-      </c>
-      <c r="C296" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-78</v>
+        <v>25-77</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
     </row>
     <row r="297" spans="1:13" ht="15">
       <c r="A297">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B297">
+        <f t="shared" si="38"/>
+        <v>78</v>
+      </c>
+      <c r="C297" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B297">
-        <f t="shared" si="37"/>
-        <v>79</v>
-      </c>
-      <c r="C297" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-79</v>
+        <v>25-78</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
     </row>
     <row r="298" spans="1:13" ht="15">
       <c r="A298">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B298">
+        <f t="shared" si="38"/>
+        <v>79</v>
+      </c>
+      <c r="C298" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B298">
-        <f t="shared" si="37"/>
-        <v>80</v>
-      </c>
-      <c r="C298" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-80</v>
+        <v>25-79</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
     </row>
     <row r="299" spans="1:13" ht="15">
       <c r="A299">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B299">
+        <f t="shared" si="38"/>
+        <v>80</v>
+      </c>
+      <c r="C299" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B299">
-        <f t="shared" si="37"/>
-        <v>81</v>
-      </c>
-      <c r="C299" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-81</v>
+        <v>25-80</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
     </row>
     <row r="300" spans="1:13" ht="15">
       <c r="A300">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B300">
+        <f t="shared" si="38"/>
+        <v>81</v>
+      </c>
+      <c r="C300" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B300">
-        <f t="shared" si="37"/>
-        <v>82</v>
-      </c>
-      <c r="C300" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-82</v>
+        <v>25-81</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
     </row>
     <row r="301" spans="1:13" ht="15">
       <c r="A301">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B301">
+        <f t="shared" si="38"/>
+        <v>82</v>
+      </c>
+      <c r="C301" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B301">
-        <f t="shared" si="37"/>
-        <v>83</v>
-      </c>
-      <c r="C301" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-83</v>
+        <v>25-82</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
     </row>
     <row r="302" spans="1:13" ht="15">
       <c r="A302">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B302">
+        <f t="shared" si="38"/>
+        <v>83</v>
+      </c>
+      <c r="C302" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B302">
-        <f t="shared" si="37"/>
-        <v>84</v>
-      </c>
-      <c r="C302" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-84</v>
+        <v>25-83</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
     </row>
     <row r="303" spans="1:13" ht="15">
       <c r="A303">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B303">
+        <f t="shared" si="38"/>
+        <v>84</v>
+      </c>
+      <c r="C303" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B303">
-        <f t="shared" si="37"/>
-        <v>85</v>
-      </c>
-      <c r="C303" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-85</v>
+        <v>25-84</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
     </row>
     <row r="304" spans="1:13" ht="15">
       <c r="A304">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B304">
+        <f t="shared" si="38"/>
+        <v>85</v>
+      </c>
+      <c r="C304" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B304">
-        <f t="shared" si="37"/>
-        <v>86</v>
-      </c>
-      <c r="C304" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-86</v>
+        <v>25-85</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
     </row>
     <row r="305" spans="1:13" ht="15">
       <c r="A305">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B305">
+        <f t="shared" si="38"/>
+        <v>86</v>
+      </c>
+      <c r="C305" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B305">
-        <f t="shared" si="37"/>
-        <v>87</v>
-      </c>
-      <c r="C305" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-87</v>
+        <v>25-86</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
     </row>
     <row r="306" spans="1:13" ht="15">
       <c r="A306">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B306">
+        <f t="shared" si="38"/>
+        <v>87</v>
+      </c>
+      <c r="C306" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B306">
-        <f t="shared" si="37"/>
-        <v>88</v>
-      </c>
-      <c r="C306" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-88</v>
+        <v>25-87</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
     </row>
     <row r="307" spans="1:13" ht="15">
       <c r="A307">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B307">
+        <f t="shared" si="38"/>
+        <v>88</v>
+      </c>
+      <c r="C307" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B307">
-        <f t="shared" si="37"/>
-        <v>89</v>
-      </c>
-      <c r="C307" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-89</v>
+        <v>25-88</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
     </row>
     <row r="308" spans="1:13" ht="15">
       <c r="A308">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B308">
+        <f t="shared" si="38"/>
+        <v>89</v>
+      </c>
+      <c r="C308" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B308">
-        <f t="shared" si="37"/>
-        <v>90</v>
-      </c>
-      <c r="C308" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-90</v>
+        <v>25-89</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
     </row>
     <row r="309" spans="1:13" ht="15">
       <c r="A309">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B309">
+        <f t="shared" si="38"/>
+        <v>90</v>
+      </c>
+      <c r="C309" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B309">
-        <f t="shared" si="37"/>
-        <v>91</v>
-      </c>
-      <c r="C309" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-91</v>
+        <v>25-90</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
     </row>
     <row r="310" spans="1:13" ht="15">
       <c r="A310">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B310">
+        <f t="shared" si="38"/>
+        <v>91</v>
+      </c>
+      <c r="C310" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B310">
-        <f t="shared" si="37"/>
-        <v>92</v>
-      </c>
-      <c r="C310" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-92</v>
+        <v>25-91</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
     </row>
     <row r="311" spans="1:13" ht="15">
       <c r="A311">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B311">
+        <f t="shared" si="38"/>
+        <v>92</v>
+      </c>
+      <c r="C311" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B311">
-        <f t="shared" si="37"/>
-        <v>93</v>
-      </c>
-      <c r="C311" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-93</v>
+        <v>25-92</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
     </row>
     <row r="312" spans="1:13" ht="15">
       <c r="A312">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B312">
+        <f t="shared" si="38"/>
+        <v>93</v>
+      </c>
+      <c r="C312" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B312">
-        <f t="shared" si="37"/>
-        <v>94</v>
-      </c>
-      <c r="C312" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-94</v>
+        <v>25-93</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
     </row>
     <row r="313" spans="1:13" ht="15">
       <c r="A313">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B313">
+        <f t="shared" si="38"/>
+        <v>94</v>
+      </c>
+      <c r="C313" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B313">
-        <f t="shared" si="37"/>
-        <v>95</v>
-      </c>
-      <c r="C313" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-95</v>
+        <v>25-94</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
     </row>
     <row r="314" spans="1:13" ht="15">
       <c r="A314">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B314">
+        <f t="shared" si="38"/>
+        <v>95</v>
+      </c>
+      <c r="C314" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B314">
-        <f t="shared" si="37"/>
-        <v>96</v>
-      </c>
-      <c r="C314" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-96</v>
+        <v>25-95</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
     </row>
     <row r="315" spans="1:13" ht="15">
       <c r="A315">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B315">
+        <f t="shared" si="38"/>
+        <v>96</v>
+      </c>
+      <c r="C315" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B315">
-        <f t="shared" si="37"/>
-        <v>97</v>
-      </c>
-      <c r="C315" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-97</v>
+        <v>25-96</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
     </row>
     <row r="316" spans="1:13" ht="15">
       <c r="A316">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B316">
+        <f t="shared" si="38"/>
+        <v>97</v>
+      </c>
+      <c r="C316" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B316">
-        <f t="shared" si="37"/>
-        <v>98</v>
-      </c>
-      <c r="C316" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-98</v>
+        <v>25-97</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
     </row>
     <row r="317" spans="1:13" ht="15">
       <c r="A317">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B317">
+        <f t="shared" si="38"/>
+        <v>98</v>
+      </c>
+      <c r="C317" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B317">
-        <f t="shared" si="37"/>
-        <v>99</v>
-      </c>
-      <c r="C317" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-99</v>
+        <v>25-98</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
     </row>
     <row r="318" spans="1:13" ht="15">
       <c r="A318">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B318">
+        <f t="shared" si="38"/>
+        <v>99</v>
+      </c>
+      <c r="C318" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B318">
-        <f t="shared" si="37"/>
-        <v>100</v>
-      </c>
-      <c r="C318" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-100</v>
+        <v>25-99</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
     </row>
     <row r="319" spans="1:13" ht="15">
       <c r="A319">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B319">
+        <f t="shared" si="38"/>
+        <v>100</v>
+      </c>
+      <c r="C319" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B319">
-        <f t="shared" si="37"/>
-        <v>101</v>
-      </c>
-      <c r="C319" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-101</v>
+        <v>25-100</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
     </row>
     <row r="320" spans="1:13" ht="15">
       <c r="A320">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B320">
+        <f t="shared" si="38"/>
+        <v>101</v>
+      </c>
+      <c r="C320" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B320">
-        <f t="shared" si="37"/>
-        <v>102</v>
-      </c>
-      <c r="C320" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-102</v>
+        <v>25-101</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
     </row>
     <row r="321" spans="1:13" ht="15">
       <c r="A321">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B321">
+        <f t="shared" si="38"/>
+        <v>102</v>
+      </c>
+      <c r="C321" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B321">
-        <f t="shared" si="37"/>
-        <v>103</v>
-      </c>
-      <c r="C321" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-103</v>
+        <v>25-102</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
     </row>
     <row r="322" spans="1:13" ht="15">
       <c r="A322">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B322">
+        <f t="shared" si="38"/>
+        <v>103</v>
+      </c>
+      <c r="C322" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B322">
-        <f t="shared" si="37"/>
-        <v>104</v>
-      </c>
-      <c r="C322" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-104</v>
+        <v>25-103</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
     </row>
     <row r="323" spans="1:13" ht="15">
       <c r="A323">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B323">
+        <f t="shared" si="38"/>
+        <v>104</v>
+      </c>
+      <c r="C323" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B323">
-        <f t="shared" si="37"/>
-        <v>105</v>
-      </c>
-      <c r="C323" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-105</v>
+        <v>25-104</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
     </row>
     <row r="324" spans="1:13" ht="15">
       <c r="A324">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B324">
+        <f t="shared" si="38"/>
+        <v>105</v>
+      </c>
+      <c r="C324" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B324">
-        <f t="shared" si="37"/>
-        <v>106</v>
-      </c>
-      <c r="C324" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-106</v>
+        <v>25-105</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
     </row>
     <row r="325" spans="1:13" ht="15">
       <c r="A325">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B325">
+        <f t="shared" si="38"/>
+        <v>106</v>
+      </c>
+      <c r="C325" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B325">
-        <f t="shared" si="37"/>
-        <v>107</v>
-      </c>
-      <c r="C325" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-107</v>
+        <v>25-106</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
     </row>
     <row r="326" spans="1:13" ht="15">
       <c r="A326">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B326">
+        <f t="shared" si="38"/>
+        <v>107</v>
+      </c>
+      <c r="C326" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B326">
-        <f t="shared" si="37"/>
-        <v>108</v>
-      </c>
-      <c r="C326" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-108</v>
+        <v>25-107</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
     </row>
     <row r="327" spans="1:13" ht="15">
       <c r="A327">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B327">
+        <f t="shared" si="38"/>
+        <v>108</v>
+      </c>
+      <c r="C327" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B327">
-        <f t="shared" si="37"/>
-        <v>109</v>
-      </c>
-      <c r="C327" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-109</v>
+        <v>25-108</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
     </row>
     <row r="328" spans="1:13" ht="15">
       <c r="A328">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B328">
+        <f t="shared" si="38"/>
+        <v>109</v>
+      </c>
+      <c r="C328" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B328">
-        <f t="shared" si="37"/>
-        <v>110</v>
-      </c>
-      <c r="C328" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-110</v>
+        <v>25-109</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
     </row>
     <row r="329" spans="1:13" ht="15">
       <c r="A329">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B329">
+        <f t="shared" si="38"/>
+        <v>110</v>
+      </c>
+      <c r="C329" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B329">
-        <f t="shared" si="37"/>
-        <v>111</v>
-      </c>
-      <c r="C329" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-111</v>
+        <v>25-110</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
     </row>
     <row r="330" spans="1:13" ht="15">
       <c r="A330">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B330">
+        <f t="shared" si="38"/>
+        <v>111</v>
+      </c>
+      <c r="C330" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B330">
-        <f t="shared" si="37"/>
-        <v>112</v>
-      </c>
-      <c r="C330" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-112</v>
+        <v>25-111</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
     </row>
     <row r="331" spans="1:13" ht="15">
       <c r="A331">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B331">
+        <f t="shared" si="38"/>
+        <v>112</v>
+      </c>
+      <c r="C331" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B331">
-        <f t="shared" si="37"/>
-        <v>113</v>
-      </c>
-      <c r="C331" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-113</v>
+        <v>25-112</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
     </row>
     <row r="332" spans="1:13" ht="15">
       <c r="A332">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B332">
+        <f t="shared" si="38"/>
+        <v>113</v>
+      </c>
+      <c r="C332" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B332">
-        <f t="shared" si="37"/>
-        <v>114</v>
-      </c>
-      <c r="C332" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-114</v>
+        <v>25-113</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
     </row>
     <row r="333" spans="1:13" ht="15">
       <c r="A333">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B333">
+        <f t="shared" si="38"/>
+        <v>114</v>
+      </c>
+      <c r="C333" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B333">
-        <f t="shared" si="37"/>
-        <v>115</v>
-      </c>
-      <c r="C333" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-115</v>
+        <v>25-114</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
     </row>
     <row r="334" spans="1:13" ht="15">
       <c r="A334">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B334">
+        <f t="shared" si="38"/>
+        <v>115</v>
+      </c>
+      <c r="C334" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B334">
-        <f t="shared" si="37"/>
-        <v>116</v>
-      </c>
-      <c r="C334" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-116</v>
+        <v>25-115</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
     </row>
     <row r="335" spans="1:13" ht="15">
       <c r="A335">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B335">
+        <f t="shared" si="38"/>
+        <v>116</v>
+      </c>
+      <c r="C335" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B335">
-        <f t="shared" si="37"/>
-        <v>117</v>
-      </c>
-      <c r="C335" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-117</v>
+        <v>25-116</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
     </row>
     <row r="336" spans="1:13" ht="15">
       <c r="A336">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B336">
+        <f t="shared" si="38"/>
+        <v>117</v>
+      </c>
+      <c r="C336" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B336">
-        <f t="shared" si="37"/>
-        <v>118</v>
-      </c>
-      <c r="C336" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-118</v>
+        <v>25-117</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
     </row>
     <row r="337" spans="1:13" ht="15">
       <c r="A337">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B337">
+        <f t="shared" si="38"/>
+        <v>118</v>
+      </c>
+      <c r="C337" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B337">
-        <f t="shared" si="37"/>
-        <v>119</v>
-      </c>
-      <c r="C337" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-119</v>
+        <v>25-118</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
     </row>
     <row r="338" spans="1:13" ht="15">
       <c r="A338">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B338">
+        <f t="shared" si="38"/>
+        <v>119</v>
+      </c>
+      <c r="C338" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B338">
-        <f t="shared" si="37"/>
-        <v>120</v>
-      </c>
-      <c r="C338" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-120</v>
+        <v>25-119</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
     </row>
     <row r="339" spans="1:13" ht="15">
       <c r="A339">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B339">
+        <f t="shared" si="38"/>
+        <v>120</v>
+      </c>
+      <c r="C339" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B339">
-        <f t="shared" si="37"/>
-        <v>121</v>
-      </c>
-      <c r="C339" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-121</v>
+        <v>25-120</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
     </row>
     <row r="340" spans="1:13" ht="15">
       <c r="A340">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B340">
+        <f t="shared" si="38"/>
+        <v>121</v>
+      </c>
+      <c r="C340" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B340">
-        <f t="shared" si="37"/>
-        <v>122</v>
-      </c>
-      <c r="C340" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-122</v>
+        <v>25-121</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
     </row>
     <row r="341" spans="1:13" ht="15">
       <c r="A341">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B341">
+        <f t="shared" si="38"/>
+        <v>122</v>
+      </c>
+      <c r="C341" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B341">
-        <f t="shared" si="37"/>
-        <v>123</v>
-      </c>
-      <c r="C341" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-123</v>
+        <v>25-122</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
     </row>
     <row r="342" spans="1:13" ht="15">
       <c r="A342">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B342">
+        <f t="shared" si="38"/>
+        <v>123</v>
+      </c>
+      <c r="C342" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B342">
-        <f t="shared" si="37"/>
-        <v>124</v>
-      </c>
-      <c r="C342" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-124</v>
+        <v>25-123</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
     </row>
     <row r="343" spans="1:13" ht="15">
       <c r="A343">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B343">
+        <f t="shared" si="38"/>
+        <v>124</v>
+      </c>
+      <c r="C343" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B343">
-        <f t="shared" si="37"/>
-        <v>125</v>
-      </c>
-      <c r="C343" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-125</v>
+        <v>25-124</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
     </row>
     <row r="344" spans="1:13" ht="15">
       <c r="A344">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B344">
+        <f t="shared" si="38"/>
+        <v>125</v>
+      </c>
+      <c r="C344" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B344">
-        <f t="shared" si="37"/>
-        <v>126</v>
-      </c>
-      <c r="C344" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-126</v>
+        <v>25-125</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
     </row>
     <row r="345" spans="1:13" ht="15">
       <c r="A345">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B345">
+        <f t="shared" si="38"/>
+        <v>126</v>
+      </c>
+      <c r="C345" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B345">
-        <f t="shared" si="37"/>
-        <v>127</v>
-      </c>
-      <c r="C345" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-127</v>
+        <v>25-126</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
     </row>
     <row r="346" spans="1:13" ht="15">
       <c r="A346">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B346">
+        <f t="shared" si="38"/>
+        <v>127</v>
+      </c>
+      <c r="C346" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B346">
-        <f t="shared" si="37"/>
-        <v>128</v>
-      </c>
-      <c r="C346" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-128</v>
+        <v>25-127</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
     </row>
     <row r="347" spans="1:13" ht="15">
       <c r="A347">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B347">
+        <f t="shared" si="38"/>
+        <v>128</v>
+      </c>
+      <c r="C347" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B347">
-        <f t="shared" si="37"/>
-        <v>129</v>
-      </c>
-      <c r="C347" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-129</v>
+        <v>25-128</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
     </row>
     <row r="348" spans="1:13" ht="15">
       <c r="A348">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B348">
+        <f t="shared" si="38"/>
+        <v>129</v>
+      </c>
+      <c r="C348" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B348">
-        <f t="shared" si="37"/>
-        <v>130</v>
-      </c>
-      <c r="C348" s="3" t="str">
-        <f t="shared" si="38"/>
-        <v>24-130</v>
+        <v>25-129</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
     </row>
     <row r="349" spans="1:13" ht="15">
       <c r="A349">
+        <f t="shared" si="40"/>
+        <v>25</v>
+      </c>
+      <c r="B349">
+        <f t="shared" si="38"/>
+        <v>130</v>
+      </c>
+      <c r="C349" s="3" t="str">
         <f t="shared" si="39"/>
-        <v>24</v>
-      </c>
-      <c r="B349">
-        <f t="shared" ref="B349:B370" si="40">IF(A349=A348,B348+1,1)</f>
-        <v>131</v>
-      </c>
-      <c r="C349" s="3" t="str">
-        <f t="shared" ref="C349:C370" si="41">CONCATENATE(A349,"-",B349)</f>
-        <v>24-131</v>
+        <v>25-130</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
     </row>
     <row r="350" spans="1:13" ht="15">
       <c r="A350">
-        <f t="shared" ref="A350:A370" si="42">A349</f>
-        <v>24</v>
+        <f t="shared" si="40"/>
+        <v>25</v>
       </c>
       <c r="B350">
-        <f t="shared" si="40"/>
-        <v>132</v>
+        <f t="shared" ref="B350:B371" si="41">IF(A350=A349,B349+1,1)</f>
+        <v>131</v>
       </c>
       <c r="C350" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-132</v>
+        <f t="shared" ref="C350:C371" si="42">CONCATENATE(A350,"-",B350)</f>
+        <v>25-131</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
     </row>
     <row r="351" spans="1:13" ht="15">
       <c r="A351">
+        <f t="shared" ref="A351:A371" si="43">A350</f>
+        <v>25</v>
+      </c>
+      <c r="B351">
+        <f t="shared" si="41"/>
+        <v>132</v>
+      </c>
+      <c r="C351" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B351">
-        <f t="shared" si="40"/>
-        <v>133</v>
-      </c>
-      <c r="C351" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-133</v>
+        <v>25-132</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
     </row>
     <row r="352" spans="1:13" ht="15">
       <c r="A352">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B352">
+        <f t="shared" si="41"/>
+        <v>133</v>
+      </c>
+      <c r="C352" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B352">
-        <f t="shared" si="40"/>
-        <v>134</v>
-      </c>
-      <c r="C352" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-134</v>
+        <v>25-133</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
     </row>
     <row r="353" spans="1:13" ht="15">
       <c r="A353">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B353">
+        <f t="shared" si="41"/>
+        <v>134</v>
+      </c>
+      <c r="C353" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B353">
-        <f t="shared" si="40"/>
-        <v>135</v>
-      </c>
-      <c r="C353" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-135</v>
+        <v>25-134</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
     </row>
     <row r="354" spans="1:13" ht="15">
       <c r="A354">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B354">
+        <f t="shared" si="41"/>
+        <v>135</v>
+      </c>
+      <c r="C354" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B354">
-        <f t="shared" si="40"/>
-        <v>136</v>
-      </c>
-      <c r="C354" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-136</v>
+        <v>25-135</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
     </row>
     <row r="355" spans="1:13" ht="15">
       <c r="A355">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B355">
+        <f t="shared" si="41"/>
+        <v>136</v>
+      </c>
+      <c r="C355" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B355">
-        <f t="shared" si="40"/>
-        <v>137</v>
-      </c>
-      <c r="C355" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-137</v>
+        <v>25-136</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
     </row>
     <row r="356" spans="1:13" ht="15">
       <c r="A356">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B356">
+        <f t="shared" si="41"/>
+        <v>137</v>
+      </c>
+      <c r="C356" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B356">
-        <f t="shared" si="40"/>
-        <v>138</v>
-      </c>
-      <c r="C356" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-138</v>
+        <v>25-137</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
     </row>
     <row r="357" spans="1:13" ht="15">
       <c r="A357">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B357">
+        <f t="shared" si="41"/>
+        <v>138</v>
+      </c>
+      <c r="C357" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B357">
-        <f t="shared" si="40"/>
-        <v>139</v>
-      </c>
-      <c r="C357" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-139</v>
+        <v>25-138</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
     </row>
     <row r="358" spans="1:13" ht="15">
       <c r="A358">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B358">
+        <f t="shared" si="41"/>
+        <v>139</v>
+      </c>
+      <c r="C358" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B358">
-        <f t="shared" si="40"/>
-        <v>140</v>
-      </c>
-      <c r="C358" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-140</v>
+        <v>25-139</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
     </row>
     <row r="359" spans="1:13" ht="15">
       <c r="A359">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B359">
+        <f t="shared" si="41"/>
+        <v>140</v>
+      </c>
+      <c r="C359" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B359">
-        <f t="shared" si="40"/>
-        <v>141</v>
-      </c>
-      <c r="C359" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-141</v>
+        <v>25-140</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
     </row>
     <row r="360" spans="1:13" ht="15">
       <c r="A360">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B360">
+        <f t="shared" si="41"/>
+        <v>141</v>
+      </c>
+      <c r="C360" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B360">
-        <f t="shared" si="40"/>
-        <v>142</v>
-      </c>
-      <c r="C360" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-142</v>
+        <v>25-141</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
     </row>
     <row r="361" spans="1:13" ht="15">
       <c r="A361">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B361">
+        <f t="shared" si="41"/>
+        <v>142</v>
+      </c>
+      <c r="C361" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B361">
-        <f t="shared" si="40"/>
-        <v>143</v>
-      </c>
-      <c r="C361" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-143</v>
+        <v>25-142</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
     </row>
     <row r="362" spans="1:13" ht="15">
       <c r="A362">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B362">
+        <f t="shared" si="41"/>
+        <v>143</v>
+      </c>
+      <c r="C362" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B362">
-        <f t="shared" si="40"/>
-        <v>144</v>
-      </c>
-      <c r="C362" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-144</v>
+        <v>25-143</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
     </row>
     <row r="363" spans="1:13" ht="15">
       <c r="A363">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B363">
+        <f t="shared" si="41"/>
+        <v>144</v>
+      </c>
+      <c r="C363" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B363">
-        <f t="shared" si="40"/>
-        <v>145</v>
-      </c>
-      <c r="C363" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-145</v>
+        <v>25-144</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
     </row>
     <row r="364" spans="1:13" ht="15">
       <c r="A364">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B364">
+        <f t="shared" si="41"/>
+        <v>145</v>
+      </c>
+      <c r="C364" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B364">
-        <f t="shared" si="40"/>
-        <v>146</v>
-      </c>
-      <c r="C364" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-146</v>
+        <v>25-145</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
     </row>
     <row r="365" spans="1:13" ht="15">
       <c r="A365">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B365">
+        <f t="shared" si="41"/>
+        <v>146</v>
+      </c>
+      <c r="C365" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B365">
-        <f t="shared" si="40"/>
-        <v>147</v>
-      </c>
-      <c r="C365" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-147</v>
+        <v>25-146</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
     </row>
     <row r="366" spans="1:13" ht="15">
       <c r="A366">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B366">
+        <f t="shared" si="41"/>
+        <v>147</v>
+      </c>
+      <c r="C366" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B366">
-        <f t="shared" si="40"/>
-        <v>148</v>
-      </c>
-      <c r="C366" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-148</v>
+        <v>25-147</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
     </row>
     <row r="367" spans="1:13" ht="15">
       <c r="A367">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B367">
+        <f t="shared" si="41"/>
+        <v>148</v>
+      </c>
+      <c r="C367" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B367">
-        <f t="shared" si="40"/>
-        <v>149</v>
-      </c>
-      <c r="C367" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-149</v>
+        <v>25-148</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
     </row>
     <row r="368" spans="1:13" ht="15">
       <c r="A368">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B368">
+        <f t="shared" si="41"/>
+        <v>149</v>
+      </c>
+      <c r="C368" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B368">
-        <f t="shared" si="40"/>
-        <v>150</v>
-      </c>
-      <c r="C368" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-150</v>
+        <v>25-149</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
     </row>
     <row r="369" spans="1:13" ht="15">
       <c r="A369">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B369">
+        <f t="shared" si="41"/>
+        <v>150</v>
+      </c>
+      <c r="C369" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B369">
-        <f t="shared" si="40"/>
-        <v>151</v>
-      </c>
-      <c r="C369" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-151</v>
+        <v>25-150</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
     </row>
     <row r="370" spans="1:13" ht="15">
       <c r="A370">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B370">
+        <f t="shared" si="41"/>
+        <v>151</v>
+      </c>
+      <c r="C370" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="B370">
-        <f t="shared" si="40"/>
-        <v>152</v>
-      </c>
-      <c r="C370" s="3" t="str">
-        <f t="shared" si="41"/>
-        <v>24-152</v>
+        <v>25-151</v>
       </c>
       <c r="L370" s="6"/>
       <c r="M370" s="6"/>
     </row>
-    <row r="371" spans="1:13" ht="12.75">
+    <row r="371" spans="1:13" ht="15">
+      <c r="A371">
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="B371">
+        <f t="shared" si="41"/>
+        <v>152</v>
+      </c>
+      <c r="C371" s="3" t="str">
+        <f t="shared" si="42"/>
+        <v>25-152</v>
+      </c>
       <c r="L371" s="6"/>
       <c r="M371" s="6"/>
     </row>
@@ -13763,279 +13874,298 @@
     <row r="1057" spans="12:13" ht="12.75">
       <c r="L1057" s="6"/>
       <c r="M1057" s="6"/>
+    </row>
+    <row r="1058" spans="12:13" ht="12.75">
+      <c r="L1058" s="6"/>
+      <c r="M1058" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="L179:L182"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K190">
-    <cfRule type="containsBlanks" dxfId="53" priority="58">
+    <cfRule type="containsBlanks" dxfId="59" priority="61">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K190">
-    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="58" priority="62" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K190">
-    <cfRule type="containsText" dxfId="51" priority="60" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="57" priority="63" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K191">
-    <cfRule type="containsBlanks" dxfId="50" priority="55">
+    <cfRule type="containsBlanks" dxfId="56" priority="58">
       <formula>LEN(TRIM(K191))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K191">
-    <cfRule type="containsText" dxfId="49" priority="56" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="55" priority="59" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K191))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K191">
-    <cfRule type="containsText" dxfId="48" priority="57" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="54" priority="60" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K191))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K192">
-    <cfRule type="containsBlanks" dxfId="47" priority="49">
+    <cfRule type="containsBlanks" dxfId="53" priority="52">
       <formula>LEN(TRIM(K192))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K192">
-    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K192))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K192">
-    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K192))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K193">
-    <cfRule type="containsBlanks" dxfId="44" priority="46">
+    <cfRule type="containsBlanks" dxfId="50" priority="49">
       <formula>LEN(TRIM(K193))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K193">
-    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K193))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K193">
-    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K193))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K194">
-    <cfRule type="containsBlanks" dxfId="41" priority="43">
+    <cfRule type="containsBlanks" dxfId="47" priority="46">
       <formula>LEN(TRIM(K194))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K194">
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K194))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K194">
-    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K194))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K196">
-    <cfRule type="containsBlanks" dxfId="38" priority="40">
+    <cfRule type="containsBlanks" dxfId="44" priority="43">
       <formula>LEN(TRIM(K196))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K198">
-    <cfRule type="containsBlanks" dxfId="37" priority="37">
+    <cfRule type="containsBlanks" dxfId="43" priority="40">
       <formula>LEN(TRIM(K198))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsBlanks" dxfId="36" priority="34">
+    <cfRule type="containsBlanks" dxfId="42" priority="37">
       <formula>LEN(TRIM(K200))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsBlanks" dxfId="35" priority="31">
+    <cfRule type="containsBlanks" dxfId="41" priority="34">
       <formula>LEN(TRIM(K201))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsBlanks" dxfId="34" priority="28">
+    <cfRule type="containsBlanks" dxfId="40" priority="31">
       <formula>LEN(TRIM(K203))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="33" priority="25">
+    <cfRule type="containsBlanks" dxfId="39" priority="28">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K207:K220">
-    <cfRule type="containsBlanks" dxfId="32" priority="22">
+  <conditionalFormatting sqref="K207:K218 K220:K221">
+    <cfRule type="containsBlanks" dxfId="38" priority="25">
       <formula>LEN(TRIM(K207))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K197">
-    <cfRule type="containsBlanks" dxfId="31" priority="16">
+    <cfRule type="containsBlanks" dxfId="37" priority="19">
       <formula>LEN(TRIM(K197))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K196">
-    <cfRule type="containsText" dxfId="30" priority="41" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="36" priority="44" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K196))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K196">
-    <cfRule type="containsText" dxfId="29" priority="42" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="35" priority="45" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K196))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K199">
-    <cfRule type="containsBlanks" dxfId="28" priority="13">
+    <cfRule type="containsBlanks" dxfId="34" priority="16">
       <formula>LEN(TRIM(K199))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K198">
-    <cfRule type="containsText" dxfId="27" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="33" priority="41" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K198))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K198">
-    <cfRule type="containsText" dxfId="26" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="32" priority="42" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K198))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K195">
-    <cfRule type="containsBlanks" dxfId="25" priority="10">
+    <cfRule type="containsBlanks" dxfId="31" priority="13">
       <formula>LEN(TRIM(K195))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="24" priority="35" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="30" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="23" priority="36" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="29" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsBlanks" dxfId="22" priority="7">
+    <cfRule type="containsBlanks" dxfId="28" priority="10">
       <formula>LEN(TRIM(K202))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="21" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="27" priority="35" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="20" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="26" priority="36" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="19" priority="4">
+    <cfRule type="containsBlanks" dxfId="25" priority="7">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="18" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="24" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="17" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="23" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="16" priority="1">
+    <cfRule type="containsBlanks" dxfId="22" priority="4">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="21" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="14" priority="27" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="20" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K207:K220">
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K207:K218 K220:K221">
+    <cfRule type="containsText" dxfId="19" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K207:K220">
-    <cfRule type="containsText" dxfId="12" priority="24" operator="containsText" text="fail">
+  <conditionalFormatting sqref="K207:K218 K220:K221">
+    <cfRule type="containsText" dxfId="18" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K197">
-    <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K197))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K197">
-    <cfRule type="containsText" dxfId="10" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K197))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K199">
-    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K199))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K199">
-    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K199))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K195">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K195))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K195">
-    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K195))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K219">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
+      <formula>LEN(TRIM(K219))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K219">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K219))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K219">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K219))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add tests for editing a block from the blocks dashboard
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="294">
   <si>
     <t>Test Number</t>
   </si>
@@ -893,6 +893,12 @@
   </si>
   <si>
     <t>Create a new configuration. Click `save as`. Try adding spaces (start, middle and end of name) and special characters. Name should only support alpha-numeric characters and underscores. Error appears otherwise and config cannot be saved</t>
+  </si>
+  <si>
+    <t>Create a block. Right click on it in the blocks dashboard and select `Edit block`. Change the block. Click cancel. Verify the changes are not applied</t>
+  </si>
+  <si>
+    <t>Create a block. Right click on it in the blocks dashboard and select `Edit block`. Change the block. Click ok. Verify the changes are applied</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1084,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1167,8 +1173,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1190,11 +1194,184 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="69">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2290,11 +2467,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1066"/>
+  <dimension ref="A1:N1068"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H156" sqref="H156"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J216" sqref="J216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -6707,14 +6884,14 @@
         <f t="shared" si="21"/>
         <v>15-54</v>
       </c>
-      <c r="D153" s="43"/>
-      <c r="E153" s="43"/>
-      <c r="F153" s="43"/>
-      <c r="G153" s="43"/>
-      <c r="H153" s="43" t="s">
+      <c r="D153" s="41"/>
+      <c r="E153" s="41"/>
+      <c r="F153" s="41"/>
+      <c r="G153" s="41"/>
+      <c r="H153" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="I153" s="44" t="s">
+      <c r="I153" s="42" t="s">
         <v>158</v>
       </c>
       <c r="J153" s="8"/>
@@ -6735,17 +6912,17 @@
         <f t="shared" si="21"/>
         <v>15-55</v>
       </c>
-      <c r="D154" s="48"/>
-      <c r="E154" s="48"/>
-      <c r="F154" s="48"/>
-      <c r="G154" s="48"/>
-      <c r="H154" s="48" t="s">
+      <c r="D154" s="46"/>
+      <c r="E154" s="46"/>
+      <c r="F154" s="46"/>
+      <c r="G154" s="46"/>
+      <c r="H154" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="I154" s="49" t="s">
+      <c r="I154" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="J154" s="42"/>
+      <c r="J154" s="40"/>
       <c r="K154" s="7"/>
       <c r="L154" s="8"/>
       <c r="M154" s="6"/>
@@ -6763,17 +6940,17 @@
         <f t="shared" si="21"/>
         <v>15-56</v>
       </c>
-      <c r="D155" s="48"/>
-      <c r="E155" s="48"/>
-      <c r="F155" s="48"/>
-      <c r="G155" s="48"/>
-      <c r="H155" s="48" t="s">
+      <c r="D155" s="46"/>
+      <c r="E155" s="46"/>
+      <c r="F155" s="46"/>
+      <c r="G155" s="46"/>
+      <c r="H155" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="I155" s="50" t="s">
+      <c r="I155" s="48" t="s">
         <v>263</v>
       </c>
-      <c r="J155" s="42"/>
+      <c r="J155" s="40"/>
       <c r="K155" s="9"/>
       <c r="L155" s="8"/>
       <c r="M155" s="6"/>
@@ -6791,17 +6968,17 @@
         <f t="shared" ref="C156" si="24">CONCATENATE(A156,"-",B156)</f>
         <v>15-57</v>
       </c>
-      <c r="D156" s="48"/>
-      <c r="E156" s="48"/>
-      <c r="F156" s="48"/>
-      <c r="G156" s="48"/>
-      <c r="H156" s="48" t="s">
+      <c r="D156" s="46"/>
+      <c r="E156" s="46"/>
+      <c r="F156" s="46"/>
+      <c r="G156" s="46"/>
+      <c r="H156" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="I156" s="50" t="s">
+      <c r="I156" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="J156" s="42"/>
+      <c r="J156" s="40"/>
       <c r="K156" s="9"/>
       <c r="L156" s="8"/>
       <c r="M156" s="6"/>
@@ -6815,52 +6992,52 @@
         <v>1</v>
       </c>
       <c r="C157" s="22" t="str">
-        <f t="shared" ref="C157:C228" si="25">CONCATENATE(A157,"-",B157)</f>
+        <f t="shared" ref="C157:C230" si="25">CONCATENATE(A157,"-",B157)</f>
         <v>16-1</v>
       </c>
-      <c r="D157" s="48"/>
-      <c r="E157" s="48"/>
-      <c r="F157" s="48" t="s">
+      <c r="D157" s="46"/>
+      <c r="E157" s="46"/>
+      <c r="F157" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G157" s="48"/>
-      <c r="H157" s="48" t="s">
+      <c r="G157" s="46"/>
+      <c r="H157" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="I157" s="49" t="s">
+      <c r="I157" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="J157" s="42"/>
+      <c r="J157" s="40"/>
       <c r="K157" s="7"/>
       <c r="L157" s="8"/>
       <c r="M157" s="6"/>
     </row>
     <row r="158" spans="1:13" ht="15">
       <c r="A158">
-        <f t="shared" ref="A158:A230" si="26">A157</f>
+        <f t="shared" ref="A158:A232" si="26">A157</f>
         <v>16</v>
       </c>
       <c r="B158">
-        <f t="shared" ref="B158:B229" si="27">IF(A158=A157,B157+1,1)</f>
+        <f t="shared" ref="B158:B231" si="27">IF(A158=A157,B157+1,1)</f>
         <v>2</v>
       </c>
       <c r="C158" s="22" t="str">
         <f t="shared" si="25"/>
         <v>16-2</v>
       </c>
-      <c r="D158" s="48"/>
-      <c r="E158" s="48"/>
-      <c r="F158" s="48" t="s">
+      <c r="D158" s="46"/>
+      <c r="E158" s="46"/>
+      <c r="F158" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G158" s="48"/>
-      <c r="H158" s="48" t="s">
+      <c r="G158" s="46"/>
+      <c r="H158" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="I158" s="49" t="s">
+      <c r="I158" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="J158" s="42"/>
+      <c r="J158" s="40"/>
       <c r="K158" s="7"/>
       <c r="L158" s="8"/>
       <c r="M158" s="6"/>
@@ -6878,19 +7055,19 @@
         <f t="shared" si="25"/>
         <v>16-3</v>
       </c>
-      <c r="D159" s="48"/>
-      <c r="E159" s="48"/>
-      <c r="F159" s="48" t="s">
+      <c r="D159" s="46"/>
+      <c r="E159" s="46"/>
+      <c r="F159" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G159" s="48"/>
-      <c r="H159" s="48" t="s">
+      <c r="G159" s="46"/>
+      <c r="H159" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="I159" s="49" t="s">
+      <c r="I159" s="47" t="s">
         <v>162</v>
       </c>
-      <c r="J159" s="42"/>
+      <c r="J159" s="40"/>
       <c r="K159" s="7"/>
       <c r="L159" s="11"/>
     </row>
@@ -6907,19 +7084,19 @@
         <f t="shared" si="25"/>
         <v>16-4</v>
       </c>
-      <c r="D160" s="48"/>
-      <c r="E160" s="48"/>
-      <c r="F160" s="48" t="s">
+      <c r="D160" s="46"/>
+      <c r="E160" s="46"/>
+      <c r="F160" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G160" s="48"/>
-      <c r="H160" s="48" t="s">
+      <c r="G160" s="46"/>
+      <c r="H160" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="I160" s="49" t="s">
+      <c r="I160" s="47" t="s">
         <v>163</v>
       </c>
-      <c r="J160" s="42"/>
+      <c r="J160" s="40"/>
       <c r="K160" s="7"/>
       <c r="L160" s="8"/>
       <c r="M160" s="6"/>
@@ -6937,19 +7114,19 @@
         <f t="shared" si="25"/>
         <v>16-5</v>
       </c>
-      <c r="D161" s="48"/>
-      <c r="E161" s="48"/>
-      <c r="F161" s="48"/>
-      <c r="G161" s="48" t="s">
+      <c r="D161" s="46"/>
+      <c r="E161" s="46"/>
+      <c r="F161" s="46"/>
+      <c r="G161" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="H161" s="48" t="s">
+      <c r="H161" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="I161" s="49" t="s">
+      <c r="I161" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="J161" s="42"/>
+      <c r="J161" s="40"/>
       <c r="K161" s="7"/>
       <c r="L161" s="8"/>
       <c r="M161" s="6"/>
@@ -6967,19 +7144,19 @@
         <f t="shared" si="25"/>
         <v>16-6</v>
       </c>
-      <c r="D162" s="48"/>
-      <c r="E162" s="48"/>
-      <c r="F162" s="48"/>
-      <c r="G162" s="48" t="s">
+      <c r="D162" s="46"/>
+      <c r="E162" s="46"/>
+      <c r="F162" s="46"/>
+      <c r="G162" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="H162" s="48" t="s">
+      <c r="H162" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="I162" s="49" t="s">
+      <c r="I162" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="J162" s="42"/>
+      <c r="J162" s="40"/>
       <c r="K162" s="7"/>
       <c r="L162" s="8"/>
       <c r="M162" s="6"/>
@@ -6993,20 +7170,20 @@
         <f t="shared" si="27"/>
         <v>7</v>
       </c>
-      <c r="C163" s="45" t="str">
+      <c r="C163" s="43" t="str">
         <f t="shared" si="25"/>
         <v>16-7</v>
       </c>
-      <c r="D163" s="46"/>
-      <c r="E163" s="46"/>
-      <c r="F163" s="46"/>
-      <c r="G163" s="46" t="s">
+      <c r="D163" s="44"/>
+      <c r="E163" s="44"/>
+      <c r="F163" s="44"/>
+      <c r="G163" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="H163" s="46" t="s">
+      <c r="H163" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="I163" s="47" t="s">
+      <c r="I163" s="45" t="s">
         <v>166</v>
       </c>
       <c r="J163" s="8"/>
@@ -7725,7 +7902,7 @@
       </c>
       <c r="J187" s="8"/>
       <c r="K187" s="7"/>
-      <c r="L187" s="39"/>
+      <c r="L187" s="49"/>
     </row>
     <row r="188" spans="1:13" ht="30">
       <c r="A188">
@@ -7754,7 +7931,7 @@
       </c>
       <c r="J188" s="8"/>
       <c r="K188" s="7"/>
-      <c r="L188" s="40"/>
+      <c r="L188" s="50"/>
       <c r="M188" s="6"/>
     </row>
     <row r="189" spans="1:13" ht="45">
@@ -7784,7 +7961,7 @@
       </c>
       <c r="J189" s="8"/>
       <c r="K189" s="7"/>
-      <c r="L189" s="40"/>
+      <c r="L189" s="50"/>
       <c r="M189" s="6"/>
     </row>
     <row r="190" spans="1:13" ht="30">
@@ -7814,7 +7991,7 @@
       </c>
       <c r="J190" s="8"/>
       <c r="K190" s="7"/>
-      <c r="L190" s="41"/>
+      <c r="L190" s="51"/>
       <c r="M190" s="6"/>
     </row>
     <row r="191" spans="1:13" ht="30">
@@ -8598,100 +8775,100 @@
       </c>
       <c r="M215" s="6"/>
     </row>
-    <row r="216" spans="1:13" ht="26.25">
+    <row r="216" spans="1:13" ht="51.75">
       <c r="A216">
-        <v>22</v>
+        <f t="shared" ref="A216:A217" si="42">A214</f>
+        <v>21</v>
       </c>
       <c r="B216">
-        <v>1</v>
-      </c>
-      <c r="C216" s="22" t="str">
-        <f>CONCATENATE(A216,"-",B216)</f>
-        <v>22-1</v>
-      </c>
-      <c r="D216" s="23"/>
-      <c r="E216" s="23"/>
-      <c r="F216" s="23"/>
-      <c r="G216" s="24"/>
-      <c r="H216" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="I216" s="25" t="s">
-        <v>248</v>
-      </c>
-      <c r="J216" s="23"/>
+        <f t="shared" ref="B216:B217" si="43">IF(A216=A215,B215+1,1)</f>
+        <v>24</v>
+      </c>
+      <c r="C216" s="19" t="str">
+        <f t="shared" ref="C216:C217" si="44">CONCATENATE(A216,"-",B216)</f>
+        <v>21-24</v>
+      </c>
+      <c r="D216" s="20"/>
+      <c r="E216" s="20"/>
+      <c r="F216" s="20"/>
+      <c r="G216" s="21"/>
+      <c r="H216" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I216" s="39" t="s">
+        <v>292</v>
+      </c>
+      <c r="J216" s="39"/>
       <c r="K216" s="21"/>
-      <c r="L216" s="26"/>
+      <c r="L216" s="39"/>
       <c r="M216" s="6"/>
     </row>
     <row r="217" spans="1:13" ht="39">
       <c r="A217">
-        <f>A216</f>
-        <v>22</v>
+        <f t="shared" si="42"/>
+        <v>21</v>
       </c>
       <c r="B217">
-        <f>IF(A217=A216,B216+1,1)</f>
-        <v>2</v>
-      </c>
-      <c r="C217" s="22" t="str">
-        <f t="shared" si="25"/>
-        <v>22-2</v>
-      </c>
-      <c r="D217" s="23"/>
-      <c r="E217" s="23"/>
-      <c r="F217" s="23"/>
-      <c r="G217" s="23"/>
-      <c r="H217" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="I217" s="25" t="s">
-        <v>250</v>
-      </c>
-      <c r="J217" s="23"/>
+        <f t="shared" si="43"/>
+        <v>25</v>
+      </c>
+      <c r="C217" s="19" t="str">
+        <f t="shared" si="44"/>
+        <v>21-25</v>
+      </c>
+      <c r="D217" s="20"/>
+      <c r="E217" s="20"/>
+      <c r="F217" s="20"/>
+      <c r="G217" s="21"/>
+      <c r="H217" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I217" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="J217" s="39"/>
       <c r="K217" s="21"/>
-      <c r="L217" s="26"/>
+      <c r="L217" s="39"/>
       <c r="M217" s="6"/>
     </row>
     <row r="218" spans="1:13" ht="26.25">
       <c r="A218">
-        <f t="shared" si="26"/>
         <v>22</v>
       </c>
       <c r="B218">
-        <f t="shared" si="27"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C218" s="22" t="str">
-        <f t="shared" si="25"/>
-        <v>22-3</v>
+        <f>CONCATENATE(A218,"-",B218)</f>
+        <v>22-1</v>
       </c>
       <c r="D218" s="23"/>
       <c r="E218" s="23"/>
       <c r="F218" s="23"/>
-      <c r="G218" s="23"/>
+      <c r="G218" s="24"/>
       <c r="H218" s="24" t="s">
         <v>249</v>
       </c>
       <c r="I218" s="25" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J218" s="23"/>
       <c r="K218" s="21"/>
       <c r="L218" s="26"/>
       <c r="M218" s="6"/>
     </row>
-    <row r="219" spans="1:13" ht="15">
+    <row r="219" spans="1:13" ht="39">
       <c r="A219">
-        <f t="shared" si="26"/>
+        <f>A218</f>
         <v>22</v>
       </c>
       <c r="B219">
-        <f t="shared" si="27"/>
-        <v>4</v>
+        <f>IF(A219=A218,B218+1,1)</f>
+        <v>2</v>
       </c>
       <c r="C219" s="22" t="str">
         <f t="shared" si="25"/>
-        <v>22-4</v>
+        <v>22-2</v>
       </c>
       <c r="D219" s="23"/>
       <c r="E219" s="23"/>
@@ -8701,25 +8878,25 @@
         <v>249</v>
       </c>
       <c r="I219" s="25" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J219" s="23"/>
       <c r="K219" s="21"/>
       <c r="L219" s="26"/>
       <c r="M219" s="6"/>
     </row>
-    <row r="220" spans="1:13" ht="15">
+    <row r="220" spans="1:13" ht="26.25">
       <c r="A220">
         <f t="shared" si="26"/>
         <v>22</v>
       </c>
       <c r="B220">
         <f t="shared" si="27"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C220" s="22" t="str">
         <f t="shared" si="25"/>
-        <v>22-5</v>
+        <v>22-3</v>
       </c>
       <c r="D220" s="23"/>
       <c r="E220" s="23"/>
@@ -8729,7 +8906,7 @@
         <v>249</v>
       </c>
       <c r="I220" s="25" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J220" s="23"/>
       <c r="K220" s="21"/>
@@ -8743,98 +8920,94 @@
       </c>
       <c r="B221">
         <f t="shared" si="27"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C221" s="22" t="str">
         <f t="shared" si="25"/>
-        <v>22-6</v>
-      </c>
-      <c r="D221" s="36"/>
-      <c r="E221" s="36"/>
-      <c r="F221" s="36"/>
-      <c r="G221" s="36"/>
-      <c r="H221" s="27" t="s">
+        <v>22-4</v>
+      </c>
+      <c r="D221" s="23"/>
+      <c r="E221" s="23"/>
+      <c r="F221" s="23"/>
+      <c r="G221" s="23"/>
+      <c r="H221" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="I221" s="37" t="s">
-        <v>254</v>
-      </c>
-      <c r="J221" s="36"/>
+      <c r="I221" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="J221" s="23"/>
       <c r="K221" s="21"/>
-      <c r="L221" s="38"/>
+      <c r="L221" s="26"/>
       <c r="M221" s="6"/>
     </row>
-    <row r="222" spans="1:13" ht="26.25">
+    <row r="222" spans="1:13" ht="15">
       <c r="A222">
-        <v>23</v>
+        <f t="shared" si="26"/>
+        <v>22</v>
       </c>
       <c r="B222">
         <f t="shared" si="27"/>
-        <v>1</v>
-      </c>
-      <c r="C222" s="35" t="str">
+        <v>5</v>
+      </c>
+      <c r="C222" s="22" t="str">
         <f t="shared" si="25"/>
-        <v>23-1</v>
+        <v>22-5</v>
       </c>
       <c r="D222" s="23"/>
       <c r="E222" s="23"/>
       <c r="F222" s="23"/>
-      <c r="G222" s="23" t="s">
-        <v>63</v>
-      </c>
+      <c r="G222" s="23"/>
       <c r="H222" s="24" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="I222" s="25" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="J222" s="23"/>
       <c r="K222" s="21"/>
       <c r="L222" s="26"/>
       <c r="M222" s="6"/>
     </row>
-    <row r="223" spans="1:13" ht="26.25">
+    <row r="223" spans="1:13" ht="15">
       <c r="A223">
         <f t="shared" si="26"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B223">
         <f t="shared" si="27"/>
-        <v>2</v>
-      </c>
-      <c r="C223" s="3" t="str">
+        <v>6</v>
+      </c>
+      <c r="C223" s="22" t="str">
         <f t="shared" si="25"/>
-        <v>23-2</v>
-      </c>
-      <c r="D223" s="23"/>
-      <c r="E223" s="23"/>
-      <c r="F223" s="23"/>
-      <c r="G223" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="H223" s="24" t="s">
-        <v>266</v>
-      </c>
-      <c r="I223" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="J223" s="23"/>
+        <v>22-6</v>
+      </c>
+      <c r="D223" s="36"/>
+      <c r="E223" s="36"/>
+      <c r="F223" s="36"/>
+      <c r="G223" s="36"/>
+      <c r="H223" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="I223" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="J223" s="36"/>
       <c r="K223" s="21"/>
-      <c r="L223" s="26"/>
+      <c r="L223" s="38"/>
       <c r="M223" s="6"/>
     </row>
     <row r="224" spans="1:13" ht="26.25">
       <c r="A224">
-        <f t="shared" si="26"/>
         <v>23</v>
       </c>
       <c r="B224">
         <f t="shared" si="27"/>
-        <v>3</v>
-      </c>
-      <c r="C224" s="3" t="str">
+        <v>1</v>
+      </c>
+      <c r="C224" s="35" t="str">
         <f t="shared" si="25"/>
-        <v>23-3</v>
+        <v>23-1</v>
       </c>
       <c r="D224" s="23"/>
       <c r="E224" s="23"/>
@@ -8846,25 +9019,25 @@
         <v>266</v>
       </c>
       <c r="I224" s="25" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J224" s="23"/>
       <c r="K224" s="21"/>
       <c r="L224" s="26"/>
       <c r="M224" s="6"/>
     </row>
-    <row r="225" spans="1:13" ht="39">
+    <row r="225" spans="1:13" ht="26.25">
       <c r="A225">
         <f t="shared" si="26"/>
         <v>23</v>
       </c>
       <c r="B225">
         <f t="shared" si="27"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C225" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>23-4</v>
+        <v>23-2</v>
       </c>
       <c r="D225" s="23"/>
       <c r="E225" s="23"/>
@@ -8876,25 +9049,25 @@
         <v>266</v>
       </c>
       <c r="I225" s="25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J225" s="23"/>
       <c r="K225" s="21"/>
       <c r="L225" s="26"/>
       <c r="M225" s="6"/>
     </row>
-    <row r="226" spans="1:13" ht="15">
+    <row r="226" spans="1:13" ht="26.25">
       <c r="A226">
         <f t="shared" si="26"/>
         <v>23</v>
       </c>
       <c r="B226">
         <f t="shared" si="27"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C226" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>23-5</v>
+        <v>23-3</v>
       </c>
       <c r="D226" s="23"/>
       <c r="E226" s="23"/>
@@ -8906,23 +9079,25 @@
         <v>266</v>
       </c>
       <c r="I226" s="25" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J226" s="23"/>
       <c r="K226" s="21"/>
       <c r="L226" s="26"/>
       <c r="M226" s="6"/>
     </row>
-    <row r="227" spans="1:13" ht="26.25">
+    <row r="227" spans="1:13" ht="39">
       <c r="A227">
-        <v>24</v>
+        <f t="shared" si="26"/>
+        <v>23</v>
       </c>
       <c r="B227">
-        <v>6</v>
+        <f t="shared" si="27"/>
+        <v>4</v>
       </c>
       <c r="C227" s="3" t="str">
-        <f t="shared" ref="C227" si="42">CONCATENATE(A227,"-",B227)</f>
-        <v>24-6</v>
+        <f t="shared" si="25"/>
+        <v>23-4</v>
       </c>
       <c r="D227" s="23"/>
       <c r="E227" s="23"/>
@@ -8934,24 +9109,25 @@
         <v>266</v>
       </c>
       <c r="I227" s="25" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="J227" s="23"/>
       <c r="K227" s="21"/>
       <c r="L227" s="26"/>
       <c r="M227" s="6"/>
     </row>
-    <row r="228" spans="1:13" ht="26.25">
+    <row r="228" spans="1:13" ht="15">
       <c r="A228">
-        <v>25</v>
+        <f t="shared" si="26"/>
+        <v>23</v>
       </c>
       <c r="B228">
-        <f>IF(A228=A226,B226+1,1)</f>
-        <v>1</v>
+        <f t="shared" si="27"/>
+        <v>5</v>
       </c>
       <c r="C228" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>25-1</v>
+        <v>23-5</v>
       </c>
       <c r="D228" s="23"/>
       <c r="E228" s="23"/>
@@ -8960,10 +9136,10 @@
         <v>63</v>
       </c>
       <c r="H228" s="24" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I228" s="25" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J228" s="23"/>
       <c r="K228" s="21"/>
@@ -8972,16 +9148,14 @@
     </row>
     <row r="229" spans="1:13" ht="26.25">
       <c r="A229">
-        <f t="shared" si="26"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B229">
-        <f t="shared" si="27"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C229" s="3" t="str">
-        <f t="shared" ref="C229" si="43">CONCATENATE(A229,"-",B229)</f>
-        <v>25-2</v>
+        <f t="shared" ref="C229" si="45">CONCATENATE(A229,"-",B229)</f>
+        <v>24-6</v>
       </c>
       <c r="D229" s="23"/>
       <c r="E229" s="23"/>
@@ -8990,1068 +9164,1095 @@
         <v>63</v>
       </c>
       <c r="H229" s="24" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I229" s="25" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="J229" s="23"/>
       <c r="K229" s="21"/>
       <c r="L229" s="26"/>
       <c r="M229" s="6"/>
     </row>
-    <row r="230" spans="1:13" ht="15">
+    <row r="230" spans="1:13" ht="26.25">
       <c r="A230">
+        <v>25</v>
+      </c>
+      <c r="B230">
+        <f>IF(A230=A228,B228+1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C230" s="3" t="str">
+        <f t="shared" si="25"/>
+        <v>25-1</v>
+      </c>
+      <c r="D230" s="23"/>
+      <c r="E230" s="23"/>
+      <c r="F230" s="23"/>
+      <c r="G230" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H230" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="I230" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="J230" s="23"/>
+      <c r="K230" s="21"/>
+      <c r="L230" s="26"/>
+      <c r="M230" s="6"/>
+    </row>
+    <row r="231" spans="1:13" ht="26.25">
+      <c r="A231">
         <f t="shared" si="26"/>
         <v>25</v>
       </c>
-      <c r="B230">
-        <f t="shared" ref="B230:B293" si="44">IF(A230=A229,B229+1,1)</f>
-        <v>3</v>
-      </c>
-      <c r="C230" s="3" t="str">
-        <f t="shared" ref="C230:C293" si="45">CONCATENATE(A230,"-",B230)</f>
-        <v>25-3</v>
-      </c>
-      <c r="L230" s="6"/>
-      <c r="M230" s="6"/>
-    </row>
-    <row r="231" spans="1:13" ht="15">
-      <c r="A231">
-        <f t="shared" ref="A231:A294" si="46">A230</f>
-        <v>25</v>
-      </c>
       <c r="B231">
-        <f t="shared" si="44"/>
-        <v>4</v>
+        <f t="shared" si="27"/>
+        <v>2</v>
       </c>
       <c r="C231" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-4</v>
-      </c>
-      <c r="L231" s="6"/>
+        <f t="shared" ref="C231" si="46">CONCATENATE(A231,"-",B231)</f>
+        <v>25-2</v>
+      </c>
+      <c r="D231" s="23"/>
+      <c r="E231" s="23"/>
+      <c r="F231" s="23"/>
+      <c r="G231" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H231" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="I231" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="J231" s="23"/>
+      <c r="K231" s="21"/>
+      <c r="L231" s="26"/>
       <c r="M231" s="6"/>
     </row>
     <row r="232" spans="1:13" ht="15">
       <c r="A232">
-        <f t="shared" si="46"/>
+        <f t="shared" si="26"/>
         <v>25</v>
       </c>
       <c r="B232">
-        <f t="shared" si="44"/>
-        <v>5</v>
+        <f t="shared" ref="B232:B295" si="47">IF(A232=A231,B231+1,1)</f>
+        <v>3</v>
       </c>
       <c r="C232" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-5</v>
+        <f t="shared" ref="C232:C295" si="48">CONCATENATE(A232,"-",B232)</f>
+        <v>25-3</v>
       </c>
       <c r="L232" s="6"/>
       <c r="M232" s="6"/>
     </row>
     <row r="233" spans="1:13" ht="15">
       <c r="A233">
-        <f t="shared" si="46"/>
+        <f t="shared" ref="A233:A296" si="49">A232</f>
         <v>25</v>
       </c>
       <c r="B233">
-        <f t="shared" si="44"/>
-        <v>6</v>
+        <f t="shared" si="47"/>
+        <v>4</v>
       </c>
       <c r="C233" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-6</v>
+        <f t="shared" si="48"/>
+        <v>25-4</v>
       </c>
       <c r="L233" s="6"/>
       <c r="M233" s="6"/>
     </row>
     <row r="234" spans="1:13" ht="15">
       <c r="A234">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B234">
-        <f t="shared" si="44"/>
-        <v>7</v>
+        <f t="shared" si="47"/>
+        <v>5</v>
       </c>
       <c r="C234" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-7</v>
+        <f t="shared" si="48"/>
+        <v>25-5</v>
       </c>
       <c r="L234" s="6"/>
       <c r="M234" s="6"/>
     </row>
     <row r="235" spans="1:13" ht="15">
       <c r="A235">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B235">
-        <f t="shared" si="44"/>
-        <v>8</v>
+        <f t="shared" si="47"/>
+        <v>6</v>
       </c>
       <c r="C235" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-8</v>
+        <f t="shared" si="48"/>
+        <v>25-6</v>
       </c>
       <c r="L235" s="6"/>
       <c r="M235" s="6"/>
     </row>
     <row r="236" spans="1:13" ht="15">
       <c r="A236">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B236">
-        <f t="shared" si="44"/>
-        <v>9</v>
+        <f t="shared" si="47"/>
+        <v>7</v>
       </c>
       <c r="C236" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-9</v>
+        <f t="shared" si="48"/>
+        <v>25-7</v>
       </c>
       <c r="L236" s="6"/>
       <c r="M236" s="6"/>
     </row>
     <row r="237" spans="1:13" ht="15">
       <c r="A237">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B237">
-        <f t="shared" si="44"/>
-        <v>10</v>
+        <f t="shared" si="47"/>
+        <v>8</v>
       </c>
       <c r="C237" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-10</v>
+        <f t="shared" si="48"/>
+        <v>25-8</v>
       </c>
       <c r="L237" s="6"/>
       <c r="M237" s="6"/>
     </row>
     <row r="238" spans="1:13" ht="15">
       <c r="A238">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B238">
-        <f t="shared" si="44"/>
-        <v>11</v>
+        <f t="shared" si="47"/>
+        <v>9</v>
       </c>
       <c r="C238" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-11</v>
+        <f t="shared" si="48"/>
+        <v>25-9</v>
       </c>
       <c r="L238" s="6"/>
       <c r="M238" s="6"/>
     </row>
     <row r="239" spans="1:13" ht="15">
       <c r="A239">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B239">
-        <f t="shared" si="44"/>
-        <v>12</v>
+        <f t="shared" si="47"/>
+        <v>10</v>
       </c>
       <c r="C239" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-12</v>
+        <f t="shared" si="48"/>
+        <v>25-10</v>
       </c>
       <c r="L239" s="6"/>
       <c r="M239" s="6"/>
     </row>
     <row r="240" spans="1:13" ht="15">
       <c r="A240">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B240">
-        <f t="shared" si="44"/>
-        <v>13</v>
+        <f t="shared" si="47"/>
+        <v>11</v>
       </c>
       <c r="C240" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-13</v>
+        <f t="shared" si="48"/>
+        <v>25-11</v>
       </c>
       <c r="L240" s="6"/>
       <c r="M240" s="6"/>
     </row>
     <row r="241" spans="1:13" ht="15">
       <c r="A241">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B241">
-        <f t="shared" si="44"/>
-        <v>14</v>
+        <f t="shared" si="47"/>
+        <v>12</v>
       </c>
       <c r="C241" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-14</v>
+        <f t="shared" si="48"/>
+        <v>25-12</v>
       </c>
       <c r="L241" s="6"/>
       <c r="M241" s="6"/>
     </row>
     <row r="242" spans="1:13" ht="15">
       <c r="A242">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B242">
-        <f t="shared" si="44"/>
-        <v>15</v>
+        <f t="shared" si="47"/>
+        <v>13</v>
       </c>
       <c r="C242" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-15</v>
+        <f t="shared" si="48"/>
+        <v>25-13</v>
       </c>
       <c r="L242" s="6"/>
       <c r="M242" s="6"/>
     </row>
     <row r="243" spans="1:13" ht="15">
       <c r="A243">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B243">
-        <f t="shared" si="44"/>
-        <v>16</v>
+        <f t="shared" si="47"/>
+        <v>14</v>
       </c>
       <c r="C243" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-16</v>
+        <f t="shared" si="48"/>
+        <v>25-14</v>
       </c>
       <c r="L243" s="6"/>
       <c r="M243" s="6"/>
     </row>
     <row r="244" spans="1:13" ht="15">
       <c r="A244">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B244">
-        <f t="shared" si="44"/>
-        <v>17</v>
+        <f t="shared" si="47"/>
+        <v>15</v>
       </c>
       <c r="C244" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-17</v>
+        <f t="shared" si="48"/>
+        <v>25-15</v>
       </c>
       <c r="L244" s="6"/>
       <c r="M244" s="6"/>
     </row>
     <row r="245" spans="1:13" ht="15">
       <c r="A245">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B245">
-        <f t="shared" si="44"/>
-        <v>18</v>
+        <f t="shared" si="47"/>
+        <v>16</v>
       </c>
       <c r="C245" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-18</v>
+        <f t="shared" si="48"/>
+        <v>25-16</v>
       </c>
       <c r="L245" s="6"/>
       <c r="M245" s="6"/>
     </row>
     <row r="246" spans="1:13" ht="15">
       <c r="A246">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B246">
-        <f t="shared" si="44"/>
-        <v>19</v>
+        <f t="shared" si="47"/>
+        <v>17</v>
       </c>
       <c r="C246" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-19</v>
+        <f t="shared" si="48"/>
+        <v>25-17</v>
       </c>
       <c r="L246" s="6"/>
       <c r="M246" s="6"/>
     </row>
     <row r="247" spans="1:13" ht="15">
       <c r="A247">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B247">
-        <f t="shared" si="44"/>
-        <v>20</v>
+        <f t="shared" si="47"/>
+        <v>18</v>
       </c>
       <c r="C247" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-20</v>
+        <f t="shared" si="48"/>
+        <v>25-18</v>
       </c>
       <c r="L247" s="6"/>
       <c r="M247" s="6"/>
     </row>
     <row r="248" spans="1:13" ht="15">
       <c r="A248">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B248">
-        <f t="shared" si="44"/>
-        <v>21</v>
+        <f t="shared" si="47"/>
+        <v>19</v>
       </c>
       <c r="C248" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-21</v>
+        <f t="shared" si="48"/>
+        <v>25-19</v>
       </c>
       <c r="L248" s="6"/>
       <c r="M248" s="6"/>
     </row>
     <row r="249" spans="1:13" ht="15">
       <c r="A249">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B249">
-        <f t="shared" si="44"/>
-        <v>22</v>
+        <f t="shared" si="47"/>
+        <v>20</v>
       </c>
       <c r="C249" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-22</v>
+        <f t="shared" si="48"/>
+        <v>25-20</v>
       </c>
       <c r="L249" s="6"/>
       <c r="M249" s="6"/>
     </row>
     <row r="250" spans="1:13" ht="15">
       <c r="A250">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B250">
-        <f t="shared" si="44"/>
-        <v>23</v>
+        <f t="shared" si="47"/>
+        <v>21</v>
       </c>
       <c r="C250" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-23</v>
+        <f t="shared" si="48"/>
+        <v>25-21</v>
       </c>
       <c r="L250" s="6"/>
       <c r="M250" s="6"/>
     </row>
     <row r="251" spans="1:13" ht="15">
       <c r="A251">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B251">
-        <f t="shared" si="44"/>
-        <v>24</v>
+        <f t="shared" si="47"/>
+        <v>22</v>
       </c>
       <c r="C251" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-24</v>
+        <f t="shared" si="48"/>
+        <v>25-22</v>
       </c>
       <c r="L251" s="6"/>
       <c r="M251" s="6"/>
     </row>
     <row r="252" spans="1:13" ht="15">
       <c r="A252">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B252">
-        <f t="shared" si="44"/>
-        <v>25</v>
+        <f t="shared" si="47"/>
+        <v>23</v>
       </c>
       <c r="C252" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-25</v>
+        <f t="shared" si="48"/>
+        <v>25-23</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
     </row>
     <row r="253" spans="1:13" ht="15">
       <c r="A253">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B253">
-        <f t="shared" si="44"/>
-        <v>26</v>
+        <f t="shared" si="47"/>
+        <v>24</v>
       </c>
       <c r="C253" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-26</v>
+        <f t="shared" si="48"/>
+        <v>25-24</v>
       </c>
       <c r="L253" s="6"/>
       <c r="M253" s="6"/>
     </row>
     <row r="254" spans="1:13" ht="15">
       <c r="A254">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B254">
-        <f t="shared" si="44"/>
-        <v>27</v>
+        <f t="shared" si="47"/>
+        <v>25</v>
       </c>
       <c r="C254" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-27</v>
+        <f t="shared" si="48"/>
+        <v>25-25</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
     </row>
     <row r="255" spans="1:13" ht="15">
       <c r="A255">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B255">
-        <f t="shared" si="44"/>
-        <v>28</v>
+        <f t="shared" si="47"/>
+        <v>26</v>
       </c>
       <c r="C255" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-28</v>
+        <f t="shared" si="48"/>
+        <v>25-26</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
     </row>
     <row r="256" spans="1:13" ht="15">
       <c r="A256">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B256">
-        <f t="shared" si="44"/>
-        <v>29</v>
+        <f t="shared" si="47"/>
+        <v>27</v>
       </c>
       <c r="C256" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-29</v>
+        <f t="shared" si="48"/>
+        <v>25-27</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
     </row>
     <row r="257" spans="1:13" ht="15">
       <c r="A257">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B257">
-        <f t="shared" si="44"/>
-        <v>30</v>
+        <f t="shared" si="47"/>
+        <v>28</v>
       </c>
       <c r="C257" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-30</v>
+        <f t="shared" si="48"/>
+        <v>25-28</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
     </row>
     <row r="258" spans="1:13" ht="15">
       <c r="A258">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B258">
-        <f t="shared" si="44"/>
-        <v>31</v>
+        <f t="shared" si="47"/>
+        <v>29</v>
       </c>
       <c r="C258" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-31</v>
+        <f t="shared" si="48"/>
+        <v>25-29</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
     </row>
     <row r="259" spans="1:13" ht="15">
       <c r="A259">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B259">
-        <f t="shared" si="44"/>
-        <v>32</v>
+        <f t="shared" si="47"/>
+        <v>30</v>
       </c>
       <c r="C259" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-32</v>
+        <f t="shared" si="48"/>
+        <v>25-30</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
     </row>
     <row r="260" spans="1:13" ht="15">
       <c r="A260">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B260">
-        <f t="shared" si="44"/>
-        <v>33</v>
+        <f t="shared" si="47"/>
+        <v>31</v>
       </c>
       <c r="C260" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-33</v>
+        <f t="shared" si="48"/>
+        <v>25-31</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
     </row>
     <row r="261" spans="1:13" ht="15">
       <c r="A261">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B261">
-        <f t="shared" si="44"/>
-        <v>34</v>
+        <f t="shared" si="47"/>
+        <v>32</v>
       </c>
       <c r="C261" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-34</v>
+        <f t="shared" si="48"/>
+        <v>25-32</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
     </row>
     <row r="262" spans="1:13" ht="15">
       <c r="A262">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B262">
-        <f t="shared" si="44"/>
-        <v>35</v>
+        <f t="shared" si="47"/>
+        <v>33</v>
       </c>
       <c r="C262" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-35</v>
+        <f t="shared" si="48"/>
+        <v>25-33</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
     </row>
     <row r="263" spans="1:13" ht="15">
       <c r="A263">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B263">
-        <f t="shared" si="44"/>
-        <v>36</v>
+        <f t="shared" si="47"/>
+        <v>34</v>
       </c>
       <c r="C263" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-36</v>
+        <f t="shared" si="48"/>
+        <v>25-34</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
     </row>
     <row r="264" spans="1:13" ht="15">
       <c r="A264">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B264">
-        <f t="shared" si="44"/>
-        <v>37</v>
+        <f t="shared" si="47"/>
+        <v>35</v>
       </c>
       <c r="C264" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-37</v>
+        <f t="shared" si="48"/>
+        <v>25-35</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
     </row>
     <row r="265" spans="1:13" ht="15">
       <c r="A265">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B265">
-        <f t="shared" si="44"/>
-        <v>38</v>
+        <f t="shared" si="47"/>
+        <v>36</v>
       </c>
       <c r="C265" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-38</v>
+        <f t="shared" si="48"/>
+        <v>25-36</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
     </row>
     <row r="266" spans="1:13" ht="15">
       <c r="A266">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B266">
-        <f t="shared" si="44"/>
-        <v>39</v>
+        <f t="shared" si="47"/>
+        <v>37</v>
       </c>
       <c r="C266" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-39</v>
+        <f t="shared" si="48"/>
+        <v>25-37</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
     </row>
     <row r="267" spans="1:13" ht="15">
       <c r="A267">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B267">
-        <f t="shared" si="44"/>
-        <v>40</v>
+        <f t="shared" si="47"/>
+        <v>38</v>
       </c>
       <c r="C267" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-40</v>
+        <f t="shared" si="48"/>
+        <v>25-38</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
     </row>
     <row r="268" spans="1:13" ht="15">
       <c r="A268">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B268">
-        <f t="shared" si="44"/>
-        <v>41</v>
+        <f t="shared" si="47"/>
+        <v>39</v>
       </c>
       <c r="C268" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-41</v>
+        <f t="shared" si="48"/>
+        <v>25-39</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
     </row>
     <row r="269" spans="1:13" ht="15">
       <c r="A269">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B269">
-        <f t="shared" si="44"/>
-        <v>42</v>
+        <f t="shared" si="47"/>
+        <v>40</v>
       </c>
       <c r="C269" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-42</v>
+        <f t="shared" si="48"/>
+        <v>25-40</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
     </row>
     <row r="270" spans="1:13" ht="15">
       <c r="A270">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B270">
-        <f t="shared" si="44"/>
-        <v>43</v>
+        <f t="shared" si="47"/>
+        <v>41</v>
       </c>
       <c r="C270" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-43</v>
+        <f t="shared" si="48"/>
+        <v>25-41</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
     </row>
     <row r="271" spans="1:13" ht="15">
       <c r="A271">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B271">
-        <f t="shared" si="44"/>
-        <v>44</v>
+        <f t="shared" si="47"/>
+        <v>42</v>
       </c>
       <c r="C271" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-44</v>
+        <f t="shared" si="48"/>
+        <v>25-42</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
     </row>
     <row r="272" spans="1:13" ht="15">
       <c r="A272">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B272">
-        <f t="shared" si="44"/>
-        <v>45</v>
+        <f t="shared" si="47"/>
+        <v>43</v>
       </c>
       <c r="C272" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-45</v>
+        <f t="shared" si="48"/>
+        <v>25-43</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
     </row>
     <row r="273" spans="1:13" ht="15">
       <c r="A273">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B273">
-        <f t="shared" si="44"/>
-        <v>46</v>
+        <f t="shared" si="47"/>
+        <v>44</v>
       </c>
       <c r="C273" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-46</v>
+        <f t="shared" si="48"/>
+        <v>25-44</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
     </row>
     <row r="274" spans="1:13" ht="15">
       <c r="A274">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B274">
-        <f t="shared" si="44"/>
-        <v>47</v>
+        <f t="shared" si="47"/>
+        <v>45</v>
       </c>
       <c r="C274" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-47</v>
+        <f t="shared" si="48"/>
+        <v>25-45</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
     </row>
     <row r="275" spans="1:13" ht="15">
       <c r="A275">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B275">
-        <f t="shared" si="44"/>
-        <v>48</v>
+        <f t="shared" si="47"/>
+        <v>46</v>
       </c>
       <c r="C275" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-48</v>
+        <f t="shared" si="48"/>
+        <v>25-46</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
     </row>
     <row r="276" spans="1:13" ht="15">
       <c r="A276">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B276">
-        <f t="shared" si="44"/>
-        <v>49</v>
+        <f t="shared" si="47"/>
+        <v>47</v>
       </c>
       <c r="C276" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-49</v>
+        <f t="shared" si="48"/>
+        <v>25-47</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
     </row>
     <row r="277" spans="1:13" ht="15">
       <c r="A277">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B277">
-        <f t="shared" si="44"/>
-        <v>50</v>
+        <f t="shared" si="47"/>
+        <v>48</v>
       </c>
       <c r="C277" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-50</v>
+        <f t="shared" si="48"/>
+        <v>25-48</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
     </row>
     <row r="278" spans="1:13" ht="15">
       <c r="A278">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B278">
-        <f t="shared" si="44"/>
-        <v>51</v>
+        <f t="shared" si="47"/>
+        <v>49</v>
       </c>
       <c r="C278" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-51</v>
+        <f t="shared" si="48"/>
+        <v>25-49</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
     </row>
     <row r="279" spans="1:13" ht="15">
       <c r="A279">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B279">
-        <f t="shared" si="44"/>
-        <v>52</v>
+        <f t="shared" si="47"/>
+        <v>50</v>
       </c>
       <c r="C279" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-52</v>
+        <f t="shared" si="48"/>
+        <v>25-50</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
     </row>
     <row r="280" spans="1:13" ht="15">
       <c r="A280">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B280">
-        <f t="shared" si="44"/>
-        <v>53</v>
+        <f t="shared" si="47"/>
+        <v>51</v>
       </c>
       <c r="C280" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-53</v>
+        <f t="shared" si="48"/>
+        <v>25-51</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
     </row>
     <row r="281" spans="1:13" ht="15">
       <c r="A281">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B281">
-        <f t="shared" si="44"/>
-        <v>54</v>
+        <f t="shared" si="47"/>
+        <v>52</v>
       </c>
       <c r="C281" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-54</v>
+        <f t="shared" si="48"/>
+        <v>25-52</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
     </row>
     <row r="282" spans="1:13" ht="15">
       <c r="A282">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B282">
-        <f t="shared" si="44"/>
-        <v>55</v>
+        <f t="shared" si="47"/>
+        <v>53</v>
       </c>
       <c r="C282" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-55</v>
+        <f t="shared" si="48"/>
+        <v>25-53</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
     </row>
     <row r="283" spans="1:13" ht="15">
       <c r="A283">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B283">
-        <f t="shared" si="44"/>
-        <v>56</v>
+        <f t="shared" si="47"/>
+        <v>54</v>
       </c>
       <c r="C283" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-56</v>
+        <f t="shared" si="48"/>
+        <v>25-54</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
     </row>
     <row r="284" spans="1:13" ht="15">
       <c r="A284">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B284">
-        <f t="shared" si="44"/>
-        <v>57</v>
+        <f t="shared" si="47"/>
+        <v>55</v>
       </c>
       <c r="C284" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-57</v>
+        <f t="shared" si="48"/>
+        <v>25-55</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
     </row>
     <row r="285" spans="1:13" ht="15">
       <c r="A285">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B285">
-        <f t="shared" si="44"/>
-        <v>58</v>
+        <f t="shared" si="47"/>
+        <v>56</v>
       </c>
       <c r="C285" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-58</v>
+        <f t="shared" si="48"/>
+        <v>25-56</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
     </row>
     <row r="286" spans="1:13" ht="15">
       <c r="A286">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B286">
-        <f t="shared" si="44"/>
-        <v>59</v>
+        <f t="shared" si="47"/>
+        <v>57</v>
       </c>
       <c r="C286" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-59</v>
+        <f t="shared" si="48"/>
+        <v>25-57</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
     </row>
     <row r="287" spans="1:13" ht="15">
       <c r="A287">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B287">
-        <f t="shared" si="44"/>
-        <v>60</v>
+        <f t="shared" si="47"/>
+        <v>58</v>
       </c>
       <c r="C287" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-60</v>
+        <f t="shared" si="48"/>
+        <v>25-58</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
     </row>
     <row r="288" spans="1:13" ht="15">
       <c r="A288">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B288">
-        <f t="shared" si="44"/>
-        <v>61</v>
+        <f t="shared" si="47"/>
+        <v>59</v>
       </c>
       <c r="C288" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-61</v>
+        <f t="shared" si="48"/>
+        <v>25-59</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
     </row>
     <row r="289" spans="1:13" ht="15">
       <c r="A289">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B289">
-        <f t="shared" si="44"/>
-        <v>62</v>
+        <f t="shared" si="47"/>
+        <v>60</v>
       </c>
       <c r="C289" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-62</v>
+        <f t="shared" si="48"/>
+        <v>25-60</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
     </row>
     <row r="290" spans="1:13" ht="15">
       <c r="A290">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B290">
-        <f t="shared" si="44"/>
-        <v>63</v>
+        <f t="shared" si="47"/>
+        <v>61</v>
       </c>
       <c r="C290" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-63</v>
+        <f t="shared" si="48"/>
+        <v>25-61</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
     </row>
     <row r="291" spans="1:13" ht="15">
       <c r="A291">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B291">
-        <f t="shared" si="44"/>
-        <v>64</v>
+        <f t="shared" si="47"/>
+        <v>62</v>
       </c>
       <c r="C291" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-64</v>
+        <f t="shared" si="48"/>
+        <v>25-62</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
     </row>
     <row r="292" spans="1:13" ht="15">
       <c r="A292">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B292">
-        <f t="shared" si="44"/>
-        <v>65</v>
+        <f t="shared" si="47"/>
+        <v>63</v>
       </c>
       <c r="C292" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-65</v>
+        <f t="shared" si="48"/>
+        <v>25-63</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
     </row>
     <row r="293" spans="1:13" ht="15">
       <c r="A293">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B293">
-        <f t="shared" si="44"/>
-        <v>66</v>
+        <f t="shared" si="47"/>
+        <v>64</v>
       </c>
       <c r="C293" s="3" t="str">
-        <f t="shared" si="45"/>
-        <v>25-66</v>
+        <f t="shared" si="48"/>
+        <v>25-64</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
     </row>
     <row r="294" spans="1:13" ht="15">
       <c r="A294">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B294">
-        <f t="shared" ref="B294:B357" si="47">IF(A294=A293,B293+1,1)</f>
-        <v>67</v>
+        <f t="shared" si="47"/>
+        <v>65</v>
       </c>
       <c r="C294" s="3" t="str">
-        <f t="shared" ref="C294:C357" si="48">CONCATENATE(A294,"-",B294)</f>
-        <v>25-67</v>
+        <f t="shared" si="48"/>
+        <v>25-65</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
     </row>
     <row r="295" spans="1:13" ht="15">
       <c r="A295">
-        <f t="shared" ref="A295:A358" si="49">A294</f>
+        <f t="shared" si="49"/>
         <v>25</v>
       </c>
       <c r="B295">
         <f t="shared" si="47"/>
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C295" s="3" t="str">
         <f t="shared" si="48"/>
-        <v>25-68</v>
+        <v>25-66</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
@@ -10062,1020 +10263,1020 @@
         <v>25</v>
       </c>
       <c r="B296">
-        <f t="shared" si="47"/>
-        <v>69</v>
+        <f t="shared" ref="B296:B359" si="50">IF(A296=A295,B295+1,1)</f>
+        <v>67</v>
       </c>
       <c r="C296" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-69</v>
+        <f t="shared" ref="C296:C359" si="51">CONCATENATE(A296,"-",B296)</f>
+        <v>25-67</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
     </row>
     <row r="297" spans="1:13" ht="15">
       <c r="A297">
-        <f t="shared" si="49"/>
+        <f t="shared" ref="A297:A360" si="52">A296</f>
         <v>25</v>
       </c>
       <c r="B297">
-        <f t="shared" si="47"/>
-        <v>70</v>
+        <f t="shared" si="50"/>
+        <v>68</v>
       </c>
       <c r="C297" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-70</v>
+        <f t="shared" si="51"/>
+        <v>25-68</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
     </row>
     <row r="298" spans="1:13" ht="15">
       <c r="A298">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B298">
-        <f t="shared" si="47"/>
-        <v>71</v>
+        <f t="shared" si="50"/>
+        <v>69</v>
       </c>
       <c r="C298" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-71</v>
+        <f t="shared" si="51"/>
+        <v>25-69</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
     </row>
     <row r="299" spans="1:13" ht="15">
       <c r="A299">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B299">
-        <f t="shared" si="47"/>
-        <v>72</v>
+        <f t="shared" si="50"/>
+        <v>70</v>
       </c>
       <c r="C299" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-72</v>
+        <f t="shared" si="51"/>
+        <v>25-70</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
     </row>
     <row r="300" spans="1:13" ht="15">
       <c r="A300">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B300">
-        <f t="shared" si="47"/>
-        <v>73</v>
+        <f t="shared" si="50"/>
+        <v>71</v>
       </c>
       <c r="C300" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-73</v>
+        <f t="shared" si="51"/>
+        <v>25-71</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
     </row>
     <row r="301" spans="1:13" ht="15">
       <c r="A301">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B301">
-        <f t="shared" si="47"/>
-        <v>74</v>
+        <f t="shared" si="50"/>
+        <v>72</v>
       </c>
       <c r="C301" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-74</v>
+        <f t="shared" si="51"/>
+        <v>25-72</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
     </row>
     <row r="302" spans="1:13" ht="15">
       <c r="A302">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B302">
-        <f t="shared" si="47"/>
-        <v>75</v>
+        <f t="shared" si="50"/>
+        <v>73</v>
       </c>
       <c r="C302" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-75</v>
+        <f t="shared" si="51"/>
+        <v>25-73</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
     </row>
     <row r="303" spans="1:13" ht="15">
       <c r="A303">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B303">
-        <f t="shared" si="47"/>
-        <v>76</v>
+        <f t="shared" si="50"/>
+        <v>74</v>
       </c>
       <c r="C303" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-76</v>
+        <f t="shared" si="51"/>
+        <v>25-74</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
     </row>
     <row r="304" spans="1:13" ht="15">
       <c r="A304">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B304">
-        <f t="shared" si="47"/>
-        <v>77</v>
+        <f t="shared" si="50"/>
+        <v>75</v>
       </c>
       <c r="C304" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-77</v>
+        <f t="shared" si="51"/>
+        <v>25-75</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
     </row>
     <row r="305" spans="1:13" ht="15">
       <c r="A305">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B305">
-        <f t="shared" si="47"/>
-        <v>78</v>
+        <f t="shared" si="50"/>
+        <v>76</v>
       </c>
       <c r="C305" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-78</v>
+        <f t="shared" si="51"/>
+        <v>25-76</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
     </row>
     <row r="306" spans="1:13" ht="15">
       <c r="A306">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B306">
-        <f t="shared" si="47"/>
-        <v>79</v>
+        <f t="shared" si="50"/>
+        <v>77</v>
       </c>
       <c r="C306" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-79</v>
+        <f t="shared" si="51"/>
+        <v>25-77</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
     </row>
     <row r="307" spans="1:13" ht="15">
       <c r="A307">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B307">
-        <f t="shared" si="47"/>
-        <v>80</v>
+        <f t="shared" si="50"/>
+        <v>78</v>
       </c>
       <c r="C307" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-80</v>
+        <f t="shared" si="51"/>
+        <v>25-78</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
     </row>
     <row r="308" spans="1:13" ht="15">
       <c r="A308">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B308">
-        <f t="shared" si="47"/>
-        <v>81</v>
+        <f t="shared" si="50"/>
+        <v>79</v>
       </c>
       <c r="C308" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-81</v>
+        <f t="shared" si="51"/>
+        <v>25-79</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
     </row>
     <row r="309" spans="1:13" ht="15">
       <c r="A309">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B309">
-        <f t="shared" si="47"/>
-        <v>82</v>
+        <f t="shared" si="50"/>
+        <v>80</v>
       </c>
       <c r="C309" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-82</v>
+        <f t="shared" si="51"/>
+        <v>25-80</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
     </row>
     <row r="310" spans="1:13" ht="15">
       <c r="A310">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B310">
-        <f t="shared" si="47"/>
-        <v>83</v>
+        <f t="shared" si="50"/>
+        <v>81</v>
       </c>
       <c r="C310" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-83</v>
+        <f t="shared" si="51"/>
+        <v>25-81</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
     </row>
     <row r="311" spans="1:13" ht="15">
       <c r="A311">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B311">
-        <f t="shared" si="47"/>
-        <v>84</v>
+        <f t="shared" si="50"/>
+        <v>82</v>
       </c>
       <c r="C311" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-84</v>
+        <f t="shared" si="51"/>
+        <v>25-82</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
     </row>
     <row r="312" spans="1:13" ht="15">
       <c r="A312">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B312">
-        <f t="shared" si="47"/>
-        <v>85</v>
+        <f t="shared" si="50"/>
+        <v>83</v>
       </c>
       <c r="C312" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-85</v>
+        <f t="shared" si="51"/>
+        <v>25-83</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
     </row>
     <row r="313" spans="1:13" ht="15">
       <c r="A313">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B313">
-        <f t="shared" si="47"/>
-        <v>86</v>
+        <f t="shared" si="50"/>
+        <v>84</v>
       </c>
       <c r="C313" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-86</v>
+        <f t="shared" si="51"/>
+        <v>25-84</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
     </row>
     <row r="314" spans="1:13" ht="15">
       <c r="A314">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B314">
-        <f t="shared" si="47"/>
-        <v>87</v>
+        <f t="shared" si="50"/>
+        <v>85</v>
       </c>
       <c r="C314" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-87</v>
+        <f t="shared" si="51"/>
+        <v>25-85</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
     </row>
     <row r="315" spans="1:13" ht="15">
       <c r="A315">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B315">
-        <f t="shared" si="47"/>
-        <v>88</v>
+        <f t="shared" si="50"/>
+        <v>86</v>
       </c>
       <c r="C315" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-88</v>
+        <f t="shared" si="51"/>
+        <v>25-86</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
     </row>
     <row r="316" spans="1:13" ht="15">
       <c r="A316">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B316">
-        <f t="shared" si="47"/>
-        <v>89</v>
+        <f t="shared" si="50"/>
+        <v>87</v>
       </c>
       <c r="C316" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-89</v>
+        <f t="shared" si="51"/>
+        <v>25-87</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
     </row>
     <row r="317" spans="1:13" ht="15">
       <c r="A317">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B317">
-        <f t="shared" si="47"/>
-        <v>90</v>
+        <f t="shared" si="50"/>
+        <v>88</v>
       </c>
       <c r="C317" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-90</v>
+        <f t="shared" si="51"/>
+        <v>25-88</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
     </row>
     <row r="318" spans="1:13" ht="15">
       <c r="A318">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B318">
-        <f t="shared" si="47"/>
-        <v>91</v>
+        <f t="shared" si="50"/>
+        <v>89</v>
       </c>
       <c r="C318" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-91</v>
+        <f t="shared" si="51"/>
+        <v>25-89</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
     </row>
     <row r="319" spans="1:13" ht="15">
       <c r="A319">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B319">
-        <f t="shared" si="47"/>
-        <v>92</v>
+        <f t="shared" si="50"/>
+        <v>90</v>
       </c>
       <c r="C319" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-92</v>
+        <f t="shared" si="51"/>
+        <v>25-90</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
     </row>
     <row r="320" spans="1:13" ht="15">
       <c r="A320">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B320">
-        <f t="shared" si="47"/>
-        <v>93</v>
+        <f t="shared" si="50"/>
+        <v>91</v>
       </c>
       <c r="C320" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-93</v>
+        <f t="shared" si="51"/>
+        <v>25-91</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
     </row>
     <row r="321" spans="1:13" ht="15">
       <c r="A321">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B321">
-        <f t="shared" si="47"/>
-        <v>94</v>
+        <f t="shared" si="50"/>
+        <v>92</v>
       </c>
       <c r="C321" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-94</v>
+        <f t="shared" si="51"/>
+        <v>25-92</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
     </row>
     <row r="322" spans="1:13" ht="15">
       <c r="A322">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B322">
-        <f t="shared" si="47"/>
-        <v>95</v>
+        <f t="shared" si="50"/>
+        <v>93</v>
       </c>
       <c r="C322" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-95</v>
+        <f t="shared" si="51"/>
+        <v>25-93</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
     </row>
     <row r="323" spans="1:13" ht="15">
       <c r="A323">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B323">
-        <f t="shared" si="47"/>
-        <v>96</v>
+        <f t="shared" si="50"/>
+        <v>94</v>
       </c>
       <c r="C323" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-96</v>
+        <f t="shared" si="51"/>
+        <v>25-94</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
     </row>
     <row r="324" spans="1:13" ht="15">
       <c r="A324">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B324">
-        <f t="shared" si="47"/>
-        <v>97</v>
+        <f t="shared" si="50"/>
+        <v>95</v>
       </c>
       <c r="C324" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-97</v>
+        <f t="shared" si="51"/>
+        <v>25-95</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
     </row>
     <row r="325" spans="1:13" ht="15">
       <c r="A325">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B325">
-        <f t="shared" si="47"/>
-        <v>98</v>
+        <f t="shared" si="50"/>
+        <v>96</v>
       </c>
       <c r="C325" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-98</v>
+        <f t="shared" si="51"/>
+        <v>25-96</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
     </row>
     <row r="326" spans="1:13" ht="15">
       <c r="A326">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B326">
-        <f t="shared" si="47"/>
-        <v>99</v>
+        <f t="shared" si="50"/>
+        <v>97</v>
       </c>
       <c r="C326" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-99</v>
+        <f t="shared" si="51"/>
+        <v>25-97</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
     </row>
     <row r="327" spans="1:13" ht="15">
       <c r="A327">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B327">
-        <f t="shared" si="47"/>
-        <v>100</v>
+        <f t="shared" si="50"/>
+        <v>98</v>
       </c>
       <c r="C327" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-100</v>
+        <f t="shared" si="51"/>
+        <v>25-98</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
     </row>
     <row r="328" spans="1:13" ht="15">
       <c r="A328">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B328">
-        <f t="shared" si="47"/>
-        <v>101</v>
+        <f t="shared" si="50"/>
+        <v>99</v>
       </c>
       <c r="C328" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-101</v>
+        <f t="shared" si="51"/>
+        <v>25-99</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
     </row>
     <row r="329" spans="1:13" ht="15">
       <c r="A329">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B329">
-        <f t="shared" si="47"/>
-        <v>102</v>
+        <f t="shared" si="50"/>
+        <v>100</v>
       </c>
       <c r="C329" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-102</v>
+        <f t="shared" si="51"/>
+        <v>25-100</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
     </row>
     <row r="330" spans="1:13" ht="15">
       <c r="A330">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B330">
-        <f t="shared" si="47"/>
-        <v>103</v>
+        <f t="shared" si="50"/>
+        <v>101</v>
       </c>
       <c r="C330" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-103</v>
+        <f t="shared" si="51"/>
+        <v>25-101</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
     </row>
     <row r="331" spans="1:13" ht="15">
       <c r="A331">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B331">
-        <f t="shared" si="47"/>
-        <v>104</v>
+        <f t="shared" si="50"/>
+        <v>102</v>
       </c>
       <c r="C331" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-104</v>
+        <f t="shared" si="51"/>
+        <v>25-102</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
     </row>
     <row r="332" spans="1:13" ht="15">
       <c r="A332">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B332">
-        <f t="shared" si="47"/>
-        <v>105</v>
+        <f t="shared" si="50"/>
+        <v>103</v>
       </c>
       <c r="C332" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-105</v>
+        <f t="shared" si="51"/>
+        <v>25-103</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
     </row>
     <row r="333" spans="1:13" ht="15">
       <c r="A333">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B333">
-        <f t="shared" si="47"/>
-        <v>106</v>
+        <f t="shared" si="50"/>
+        <v>104</v>
       </c>
       <c r="C333" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-106</v>
+        <f t="shared" si="51"/>
+        <v>25-104</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
     </row>
     <row r="334" spans="1:13" ht="15">
       <c r="A334">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B334">
-        <f t="shared" si="47"/>
-        <v>107</v>
+        <f t="shared" si="50"/>
+        <v>105</v>
       </c>
       <c r="C334" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-107</v>
+        <f t="shared" si="51"/>
+        <v>25-105</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
     </row>
     <row r="335" spans="1:13" ht="15">
       <c r="A335">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B335">
-        <f t="shared" si="47"/>
-        <v>108</v>
+        <f t="shared" si="50"/>
+        <v>106</v>
       </c>
       <c r="C335" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-108</v>
+        <f t="shared" si="51"/>
+        <v>25-106</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
     </row>
     <row r="336" spans="1:13" ht="15">
       <c r="A336">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B336">
-        <f t="shared" si="47"/>
-        <v>109</v>
+        <f t="shared" si="50"/>
+        <v>107</v>
       </c>
       <c r="C336" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-109</v>
+        <f t="shared" si="51"/>
+        <v>25-107</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
     </row>
     <row r="337" spans="1:13" ht="15">
       <c r="A337">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B337">
-        <f t="shared" si="47"/>
-        <v>110</v>
+        <f t="shared" si="50"/>
+        <v>108</v>
       </c>
       <c r="C337" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-110</v>
+        <f t="shared" si="51"/>
+        <v>25-108</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
     </row>
     <row r="338" spans="1:13" ht="15">
       <c r="A338">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B338">
-        <f t="shared" si="47"/>
-        <v>111</v>
+        <f t="shared" si="50"/>
+        <v>109</v>
       </c>
       <c r="C338" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-111</v>
+        <f t="shared" si="51"/>
+        <v>25-109</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
     </row>
     <row r="339" spans="1:13" ht="15">
       <c r="A339">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B339">
-        <f t="shared" si="47"/>
-        <v>112</v>
+        <f t="shared" si="50"/>
+        <v>110</v>
       </c>
       <c r="C339" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-112</v>
+        <f t="shared" si="51"/>
+        <v>25-110</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
     </row>
     <row r="340" spans="1:13" ht="15">
       <c r="A340">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B340">
-        <f t="shared" si="47"/>
-        <v>113</v>
+        <f t="shared" si="50"/>
+        <v>111</v>
       </c>
       <c r="C340" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-113</v>
+        <f t="shared" si="51"/>
+        <v>25-111</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
     </row>
     <row r="341" spans="1:13" ht="15">
       <c r="A341">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B341">
-        <f t="shared" si="47"/>
-        <v>114</v>
+        <f t="shared" si="50"/>
+        <v>112</v>
       </c>
       <c r="C341" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-114</v>
+        <f t="shared" si="51"/>
+        <v>25-112</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
     </row>
     <row r="342" spans="1:13" ht="15">
       <c r="A342">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B342">
-        <f t="shared" si="47"/>
-        <v>115</v>
+        <f t="shared" si="50"/>
+        <v>113</v>
       </c>
       <c r="C342" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-115</v>
+        <f t="shared" si="51"/>
+        <v>25-113</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
     </row>
     <row r="343" spans="1:13" ht="15">
       <c r="A343">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B343">
-        <f t="shared" si="47"/>
-        <v>116</v>
+        <f t="shared" si="50"/>
+        <v>114</v>
       </c>
       <c r="C343" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-116</v>
+        <f t="shared" si="51"/>
+        <v>25-114</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
     </row>
     <row r="344" spans="1:13" ht="15">
       <c r="A344">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B344">
-        <f t="shared" si="47"/>
-        <v>117</v>
+        <f t="shared" si="50"/>
+        <v>115</v>
       </c>
       <c r="C344" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-117</v>
+        <f t="shared" si="51"/>
+        <v>25-115</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
     </row>
     <row r="345" spans="1:13" ht="15">
       <c r="A345">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B345">
-        <f t="shared" si="47"/>
-        <v>118</v>
+        <f t="shared" si="50"/>
+        <v>116</v>
       </c>
       <c r="C345" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-118</v>
+        <f t="shared" si="51"/>
+        <v>25-116</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
     </row>
     <row r="346" spans="1:13" ht="15">
       <c r="A346">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B346">
-        <f t="shared" si="47"/>
-        <v>119</v>
+        <f t="shared" si="50"/>
+        <v>117</v>
       </c>
       <c r="C346" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-119</v>
+        <f t="shared" si="51"/>
+        <v>25-117</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
     </row>
     <row r="347" spans="1:13" ht="15">
       <c r="A347">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B347">
-        <f t="shared" si="47"/>
-        <v>120</v>
+        <f t="shared" si="50"/>
+        <v>118</v>
       </c>
       <c r="C347" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-120</v>
+        <f t="shared" si="51"/>
+        <v>25-118</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
     </row>
     <row r="348" spans="1:13" ht="15">
       <c r="A348">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B348">
-        <f t="shared" si="47"/>
-        <v>121</v>
+        <f t="shared" si="50"/>
+        <v>119</v>
       </c>
       <c r="C348" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-121</v>
+        <f t="shared" si="51"/>
+        <v>25-119</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
     </row>
     <row r="349" spans="1:13" ht="15">
       <c r="A349">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B349">
-        <f t="shared" si="47"/>
-        <v>122</v>
+        <f t="shared" si="50"/>
+        <v>120</v>
       </c>
       <c r="C349" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-122</v>
+        <f t="shared" si="51"/>
+        <v>25-120</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
     </row>
     <row r="350" spans="1:13" ht="15">
       <c r="A350">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B350">
-        <f t="shared" si="47"/>
-        <v>123</v>
+        <f t="shared" si="50"/>
+        <v>121</v>
       </c>
       <c r="C350" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-123</v>
+        <f t="shared" si="51"/>
+        <v>25-121</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
     </row>
     <row r="351" spans="1:13" ht="15">
       <c r="A351">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B351">
-        <f t="shared" si="47"/>
-        <v>124</v>
+        <f t="shared" si="50"/>
+        <v>122</v>
       </c>
       <c r="C351" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-124</v>
+        <f t="shared" si="51"/>
+        <v>25-122</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
     </row>
     <row r="352" spans="1:13" ht="15">
       <c r="A352">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B352">
-        <f t="shared" si="47"/>
-        <v>125</v>
+        <f t="shared" si="50"/>
+        <v>123</v>
       </c>
       <c r="C352" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-125</v>
+        <f t="shared" si="51"/>
+        <v>25-123</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
     </row>
     <row r="353" spans="1:13" ht="15">
       <c r="A353">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B353">
-        <f t="shared" si="47"/>
-        <v>126</v>
+        <f t="shared" si="50"/>
+        <v>124</v>
       </c>
       <c r="C353" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-126</v>
+        <f t="shared" si="51"/>
+        <v>25-124</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
     </row>
     <row r="354" spans="1:13" ht="15">
       <c r="A354">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B354">
-        <f t="shared" si="47"/>
-        <v>127</v>
+        <f t="shared" si="50"/>
+        <v>125</v>
       </c>
       <c r="C354" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-127</v>
+        <f t="shared" si="51"/>
+        <v>25-125</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
     </row>
     <row r="355" spans="1:13" ht="15">
       <c r="A355">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B355">
-        <f t="shared" si="47"/>
-        <v>128</v>
+        <f t="shared" si="50"/>
+        <v>126</v>
       </c>
       <c r="C355" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-128</v>
+        <f t="shared" si="51"/>
+        <v>25-126</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
     </row>
     <row r="356" spans="1:13" ht="15">
       <c r="A356">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B356">
-        <f t="shared" si="47"/>
-        <v>129</v>
+        <f t="shared" si="50"/>
+        <v>127</v>
       </c>
       <c r="C356" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-129</v>
+        <f t="shared" si="51"/>
+        <v>25-127</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
     </row>
     <row r="357" spans="1:13" ht="15">
       <c r="A357">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B357">
-        <f t="shared" si="47"/>
-        <v>130</v>
+        <f t="shared" si="50"/>
+        <v>128</v>
       </c>
       <c r="C357" s="3" t="str">
-        <f t="shared" si="48"/>
-        <v>25-130</v>
+        <f t="shared" si="51"/>
+        <v>25-128</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
     </row>
     <row r="358" spans="1:13" ht="15">
       <c r="A358">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B358">
-        <f t="shared" ref="B358:B379" si="50">IF(A358=A357,B357+1,1)</f>
-        <v>131</v>
+        <f t="shared" si="50"/>
+        <v>129</v>
       </c>
       <c r="C358" s="3" t="str">
-        <f t="shared" ref="C358:C379" si="51">CONCATENATE(A358,"-",B358)</f>
-        <v>25-131</v>
+        <f t="shared" si="51"/>
+        <v>25-129</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
     </row>
     <row r="359" spans="1:13" ht="15">
       <c r="A359">
-        <f t="shared" ref="A359:A379" si="52">A358</f>
+        <f t="shared" si="52"/>
         <v>25</v>
       </c>
       <c r="B359">
         <f t="shared" si="50"/>
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C359" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>25-132</v>
+        <v>25-130</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
@@ -11086,325 +11287,349 @@
         <v>25</v>
       </c>
       <c r="B360">
-        <f t="shared" si="50"/>
-        <v>133</v>
+        <f t="shared" ref="B360:B381" si="53">IF(A360=A359,B359+1,1)</f>
+        <v>131</v>
       </c>
       <c r="C360" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-133</v>
+        <f t="shared" ref="C360:C381" si="54">CONCATENATE(A360,"-",B360)</f>
+        <v>25-131</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
     </row>
     <row r="361" spans="1:13" ht="15">
       <c r="A361">
-        <f t="shared" si="52"/>
+        <f t="shared" ref="A361:A381" si="55">A360</f>
         <v>25</v>
       </c>
       <c r="B361">
-        <f t="shared" si="50"/>
-        <v>134</v>
+        <f t="shared" si="53"/>
+        <v>132</v>
       </c>
       <c r="C361" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-134</v>
+        <f t="shared" si="54"/>
+        <v>25-132</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
     </row>
     <row r="362" spans="1:13" ht="15">
       <c r="A362">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B362">
-        <f t="shared" si="50"/>
-        <v>135</v>
+        <f t="shared" si="53"/>
+        <v>133</v>
       </c>
       <c r="C362" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-135</v>
+        <f t="shared" si="54"/>
+        <v>25-133</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
     </row>
     <row r="363" spans="1:13" ht="15">
       <c r="A363">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B363">
-        <f t="shared" si="50"/>
-        <v>136</v>
+        <f t="shared" si="53"/>
+        <v>134</v>
       </c>
       <c r="C363" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-136</v>
+        <f t="shared" si="54"/>
+        <v>25-134</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
     </row>
     <row r="364" spans="1:13" ht="15">
       <c r="A364">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B364">
-        <f t="shared" si="50"/>
-        <v>137</v>
+        <f t="shared" si="53"/>
+        <v>135</v>
       </c>
       <c r="C364" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-137</v>
+        <f t="shared" si="54"/>
+        <v>25-135</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
     </row>
     <row r="365" spans="1:13" ht="15">
       <c r="A365">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B365">
-        <f t="shared" si="50"/>
-        <v>138</v>
+        <f t="shared" si="53"/>
+        <v>136</v>
       </c>
       <c r="C365" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-138</v>
+        <f t="shared" si="54"/>
+        <v>25-136</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
     </row>
     <row r="366" spans="1:13" ht="15">
       <c r="A366">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B366">
-        <f t="shared" si="50"/>
-        <v>139</v>
+        <f t="shared" si="53"/>
+        <v>137</v>
       </c>
       <c r="C366" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-139</v>
+        <f t="shared" si="54"/>
+        <v>25-137</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
     </row>
     <row r="367" spans="1:13" ht="15">
       <c r="A367">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B367">
-        <f t="shared" si="50"/>
-        <v>140</v>
+        <f t="shared" si="53"/>
+        <v>138</v>
       </c>
       <c r="C367" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-140</v>
+        <f t="shared" si="54"/>
+        <v>25-138</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
     </row>
     <row r="368" spans="1:13" ht="15">
       <c r="A368">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B368">
-        <f t="shared" si="50"/>
-        <v>141</v>
+        <f t="shared" si="53"/>
+        <v>139</v>
       </c>
       <c r="C368" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-141</v>
+        <f t="shared" si="54"/>
+        <v>25-139</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
     </row>
     <row r="369" spans="1:13" ht="15">
       <c r="A369">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B369">
-        <f t="shared" si="50"/>
-        <v>142</v>
+        <f t="shared" si="53"/>
+        <v>140</v>
       </c>
       <c r="C369" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-142</v>
+        <f t="shared" si="54"/>
+        <v>25-140</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
     </row>
     <row r="370" spans="1:13" ht="15">
       <c r="A370">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B370">
-        <f t="shared" si="50"/>
-        <v>143</v>
+        <f t="shared" si="53"/>
+        <v>141</v>
       </c>
       <c r="C370" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-143</v>
+        <f t="shared" si="54"/>
+        <v>25-141</v>
       </c>
       <c r="L370" s="6"/>
       <c r="M370" s="6"/>
     </row>
     <row r="371" spans="1:13" ht="15">
       <c r="A371">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B371">
-        <f t="shared" si="50"/>
-        <v>144</v>
+        <f t="shared" si="53"/>
+        <v>142</v>
       </c>
       <c r="C371" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-144</v>
+        <f t="shared" si="54"/>
+        <v>25-142</v>
       </c>
       <c r="L371" s="6"/>
       <c r="M371" s="6"/>
     </row>
     <row r="372" spans="1:13" ht="15">
       <c r="A372">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B372">
-        <f t="shared" si="50"/>
-        <v>145</v>
+        <f t="shared" si="53"/>
+        <v>143</v>
       </c>
       <c r="C372" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-145</v>
+        <f t="shared" si="54"/>
+        <v>25-143</v>
       </c>
       <c r="L372" s="6"/>
       <c r="M372" s="6"/>
     </row>
     <row r="373" spans="1:13" ht="15">
       <c r="A373">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B373">
-        <f t="shared" si="50"/>
-        <v>146</v>
+        <f t="shared" si="53"/>
+        <v>144</v>
       </c>
       <c r="C373" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-146</v>
+        <f t="shared" si="54"/>
+        <v>25-144</v>
       </c>
       <c r="L373" s="6"/>
       <c r="M373" s="6"/>
     </row>
     <row r="374" spans="1:13" ht="15">
       <c r="A374">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B374">
-        <f t="shared" si="50"/>
-        <v>147</v>
+        <f t="shared" si="53"/>
+        <v>145</v>
       </c>
       <c r="C374" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-147</v>
+        <f t="shared" si="54"/>
+        <v>25-145</v>
       </c>
       <c r="L374" s="6"/>
       <c r="M374" s="6"/>
     </row>
     <row r="375" spans="1:13" ht="15">
       <c r="A375">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B375">
-        <f t="shared" si="50"/>
-        <v>148</v>
+        <f t="shared" si="53"/>
+        <v>146</v>
       </c>
       <c r="C375" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-148</v>
+        <f t="shared" si="54"/>
+        <v>25-146</v>
       </c>
       <c r="L375" s="6"/>
       <c r="M375" s="6"/>
     </row>
     <row r="376" spans="1:13" ht="15">
       <c r="A376">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B376">
-        <f t="shared" si="50"/>
-        <v>149</v>
+        <f t="shared" si="53"/>
+        <v>147</v>
       </c>
       <c r="C376" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-149</v>
+        <f t="shared" si="54"/>
+        <v>25-147</v>
       </c>
       <c r="L376" s="6"/>
       <c r="M376" s="6"/>
     </row>
     <row r="377" spans="1:13" ht="15">
       <c r="A377">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B377">
-        <f t="shared" si="50"/>
-        <v>150</v>
+        <f t="shared" si="53"/>
+        <v>148</v>
       </c>
       <c r="C377" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-150</v>
+        <f t="shared" si="54"/>
+        <v>25-148</v>
       </c>
       <c r="L377" s="6"/>
       <c r="M377" s="6"/>
     </row>
     <row r="378" spans="1:13" ht="15">
       <c r="A378">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B378">
-        <f t="shared" si="50"/>
-        <v>151</v>
+        <f t="shared" si="53"/>
+        <v>149</v>
       </c>
       <c r="C378" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-151</v>
+        <f t="shared" si="54"/>
+        <v>25-149</v>
       </c>
       <c r="L378" s="6"/>
       <c r="M378" s="6"/>
     </row>
     <row r="379" spans="1:13" ht="15">
       <c r="A379">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>25</v>
       </c>
       <c r="B379">
-        <f t="shared" si="50"/>
-        <v>152</v>
+        <f t="shared" si="53"/>
+        <v>150</v>
       </c>
       <c r="C379" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>25-152</v>
+        <f t="shared" si="54"/>
+        <v>25-150</v>
       </c>
       <c r="L379" s="6"/>
       <c r="M379" s="6"/>
     </row>
-    <row r="380" spans="1:13" ht="12.75">
+    <row r="380" spans="1:13" ht="15">
+      <c r="A380">
+        <f t="shared" si="55"/>
+        <v>25</v>
+      </c>
+      <c r="B380">
+        <f t="shared" si="53"/>
+        <v>151</v>
+      </c>
+      <c r="C380" s="3" t="str">
+        <f t="shared" si="54"/>
+        <v>25-151</v>
+      </c>
       <c r="L380" s="6"/>
       <c r="M380" s="6"/>
     </row>
-    <row r="381" spans="1:13" ht="12.75">
+    <row r="381" spans="1:13" ht="15">
+      <c r="A381">
+        <f t="shared" si="55"/>
+        <v>25</v>
+      </c>
+      <c r="B381">
+        <f t="shared" si="53"/>
+        <v>152</v>
+      </c>
+      <c r="C381" s="3" t="str">
+        <f t="shared" si="54"/>
+        <v>25-152</v>
+      </c>
       <c r="L381" s="6"/>
       <c r="M381" s="6"/>
     </row>
@@ -14147,294 +14372,332 @@
     <row r="1066" spans="12:13" ht="12.75">
       <c r="L1066" s="6"/>
       <c r="M1066" s="6"/>
+    </row>
+    <row r="1067" spans="12:13" ht="12.75">
+      <c r="L1067" s="6"/>
+      <c r="M1067" s="6"/>
+    </row>
+    <row r="1068" spans="12:13" ht="12.75">
+      <c r="L1068" s="6"/>
+      <c r="M1068" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="L187:L190"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K198">
-    <cfRule type="containsBlanks" dxfId="56" priority="61">
+    <cfRule type="containsBlanks" dxfId="68" priority="67">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K198">
-    <cfRule type="containsText" dxfId="55" priority="62" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K198">
-    <cfRule type="containsText" dxfId="54" priority="63" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K199">
-    <cfRule type="containsBlanks" dxfId="53" priority="58">
+    <cfRule type="containsBlanks" dxfId="65" priority="64">
       <formula>LEN(TRIM(K199))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K199">
-    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K199))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K199">
-    <cfRule type="containsText" dxfId="51" priority="60" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K199))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsBlanks" dxfId="50" priority="52">
+    <cfRule type="containsBlanks" dxfId="62" priority="58">
       <formula>LEN(TRIM(K200))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="61" priority="59" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="48" priority="54" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="60" priority="60" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsBlanks" dxfId="47" priority="49">
+    <cfRule type="containsBlanks" dxfId="59" priority="55">
       <formula>LEN(TRIM(K201))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="58" priority="56" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="57" priority="57" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsBlanks" dxfId="44" priority="46">
+    <cfRule type="containsBlanks" dxfId="56" priority="52">
       <formula>LEN(TRIM(K202))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="41" priority="43">
+    <cfRule type="containsBlanks" dxfId="53" priority="49">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="40" priority="40">
+    <cfRule type="containsBlanks" dxfId="52" priority="46">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsBlanks" dxfId="39" priority="37">
+    <cfRule type="containsBlanks" dxfId="51" priority="43">
       <formula>LEN(TRIM(K208))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsBlanks" dxfId="38" priority="34">
+    <cfRule type="containsBlanks" dxfId="50" priority="40">
       <formula>LEN(TRIM(K209))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsBlanks" dxfId="37" priority="31">
+    <cfRule type="containsBlanks" dxfId="49" priority="37">
       <formula>LEN(TRIM(K211))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsBlanks" dxfId="36" priority="28">
+    <cfRule type="containsBlanks" dxfId="48" priority="34">
       <formula>LEN(TRIM(K213))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K215:K226 K228:K229">
-    <cfRule type="containsBlanks" dxfId="35" priority="25">
+  <conditionalFormatting sqref="K215 K230:K231 K218:K228">
+    <cfRule type="containsBlanks" dxfId="47" priority="31">
       <formula>LEN(TRIM(K215))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="34" priority="19">
+    <cfRule type="containsBlanks" dxfId="46" priority="25">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="33" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="32" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="44" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsBlanks" dxfId="31" priority="16">
+    <cfRule type="containsBlanks" dxfId="43" priority="22">
       <formula>LEN(TRIM(K207))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="30" priority="41" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="42" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="29" priority="42" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="41" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsBlanks" dxfId="28" priority="13">
+    <cfRule type="containsBlanks" dxfId="40" priority="19">
       <formula>LEN(TRIM(K203))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="27" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="39" priority="44" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="26" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="38" priority="45" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsBlanks" dxfId="25" priority="10">
+    <cfRule type="containsBlanks" dxfId="37" priority="16">
       <formula>LEN(TRIM(K210))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="24" priority="35" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="23" priority="36" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="35" priority="42" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsBlanks" dxfId="22" priority="7">
+    <cfRule type="containsBlanks" dxfId="34" priority="13">
       <formula>LEN(TRIM(K212))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="21" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="33" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="20" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="32" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsBlanks" dxfId="19" priority="4">
+    <cfRule type="containsBlanks" dxfId="31" priority="10">
       <formula>LEN(TRIM(K214))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="18" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="17" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K215:K226 K228:K229">
-    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K215 K230:K231 K218:K228">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K215:K226 K228:K229">
-    <cfRule type="containsText" dxfId="15" priority="27" operator="containsText" text="fail">
+  <conditionalFormatting sqref="K215 K230:K231 K218:K228">
+    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="14" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="13" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="24" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="11" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K227">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
-      <formula>LEN(TRIM(K227))=0</formula>
+  <conditionalFormatting sqref="K229">
+    <cfRule type="containsBlanks" dxfId="14" priority="7">
+      <formula>LEN(TRIM(K229))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K227">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K227))))</formula>
+  <conditionalFormatting sqref="K229">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K229))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K227">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K227))))</formula>
+  <conditionalFormatting sqref="K229">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K229))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K216">
+    <cfRule type="containsBlanks" dxfId="11" priority="4">
+      <formula>LEN(TRIM(K216))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K216">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K216))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K216">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K216))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K217">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
+      <formula>LEN(TRIM(K217))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K217">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K217))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K217">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added manual test for #369
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="300">
   <si>
     <t>Test Number</t>
   </si>
@@ -911,6 +911,12 @@
   </si>
   <si>
     <t>Switch to a different instrument. Repeat above</t>
+  </si>
+  <si>
+    <t>General perspectives</t>
+  </si>
+  <si>
+    <t>Confirm that you can switch perspectives with the function keys</t>
   </si>
 </sst>
 </file>
@@ -1215,12 +1221,40 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="72">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF4C7C3"/>
           <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
         </patternFill>
       </fill>
       <border>
@@ -1261,34 +1295,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFCE8B2"/>
           <bgColor rgb="FFFCE8B2"/>
         </patternFill>
@@ -1317,50 +1323,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
         </patternFill>
       </fill>
       <border>
@@ -2566,8 +2530,8 @@
   <dimension ref="A1:N1069"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I235" sqref="I235"/>
+      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I241" sqref="I241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -7110,7 +7074,7 @@
     </row>
     <row r="158" spans="1:13" ht="15">
       <c r="A158">
-        <f t="shared" ref="A158:A233" si="26">A157</f>
+        <f t="shared" ref="A158:A232" si="26">A157</f>
         <v>16</v>
       </c>
       <c r="B158">
@@ -9414,20 +9378,31 @@
       <c r="L234" s="26"/>
       <c r="M234" s="6"/>
     </row>
-    <row r="235" spans="1:13" ht="15">
+    <row r="235" spans="1:13" ht="26.25">
       <c r="A235">
         <f t="shared" si="51"/>
         <v>26</v>
       </c>
       <c r="B235">
-        <f t="shared" si="49"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C235" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-3</v>
-      </c>
-      <c r="L235" s="6"/>
+        <v>26-1</v>
+      </c>
+      <c r="D235" s="23"/>
+      <c r="E235" s="23"/>
+      <c r="F235" s="23"/>
+      <c r="G235" s="23"/>
+      <c r="H235" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="I235" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="J235" s="23"/>
+      <c r="K235" s="21"/>
+      <c r="L235" s="26"/>
       <c r="M235" s="6"/>
     </row>
     <row r="236" spans="1:13" ht="15">
@@ -9437,11 +9412,11 @@
       </c>
       <c r="B236">
         <f t="shared" si="49"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C236" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-4</v>
+        <v>26-2</v>
       </c>
       <c r="L236" s="6"/>
       <c r="M236" s="6"/>
@@ -9453,11 +9428,11 @@
       </c>
       <c r="B237">
         <f t="shared" si="49"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C237" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-5</v>
+        <v>26-3</v>
       </c>
       <c r="L237" s="6"/>
       <c r="M237" s="6"/>
@@ -9469,11 +9444,11 @@
       </c>
       <c r="B238">
         <f t="shared" si="49"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C238" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-6</v>
+        <v>26-4</v>
       </c>
       <c r="L238" s="6"/>
       <c r="M238" s="6"/>
@@ -9485,11 +9460,11 @@
       </c>
       <c r="B239">
         <f t="shared" si="49"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C239" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-7</v>
+        <v>26-5</v>
       </c>
       <c r="L239" s="6"/>
       <c r="M239" s="6"/>
@@ -9501,11 +9476,11 @@
       </c>
       <c r="B240">
         <f t="shared" si="49"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C240" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-8</v>
+        <v>26-6</v>
       </c>
       <c r="L240" s="6"/>
       <c r="M240" s="6"/>
@@ -9517,11 +9492,11 @@
       </c>
       <c r="B241">
         <f t="shared" si="49"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C241" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-9</v>
+        <v>26-7</v>
       </c>
       <c r="L241" s="6"/>
       <c r="M241" s="6"/>
@@ -9533,11 +9508,11 @@
       </c>
       <c r="B242">
         <f t="shared" si="49"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C242" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-10</v>
+        <v>26-8</v>
       </c>
       <c r="L242" s="6"/>
       <c r="M242" s="6"/>
@@ -9549,11 +9524,11 @@
       </c>
       <c r="B243">
         <f t="shared" si="49"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C243" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-11</v>
+        <v>26-9</v>
       </c>
       <c r="L243" s="6"/>
       <c r="M243" s="6"/>
@@ -9565,11 +9540,11 @@
       </c>
       <c r="B244">
         <f t="shared" si="49"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C244" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-12</v>
+        <v>26-10</v>
       </c>
       <c r="L244" s="6"/>
       <c r="M244" s="6"/>
@@ -9581,11 +9556,11 @@
       </c>
       <c r="B245">
         <f t="shared" si="49"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C245" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-13</v>
+        <v>26-11</v>
       </c>
       <c r="L245" s="6"/>
       <c r="M245" s="6"/>
@@ -9597,11 +9572,11 @@
       </c>
       <c r="B246">
         <f t="shared" si="49"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C246" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-14</v>
+        <v>26-12</v>
       </c>
       <c r="L246" s="6"/>
       <c r="M246" s="6"/>
@@ -9613,11 +9588,11 @@
       </c>
       <c r="B247">
         <f t="shared" si="49"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C247" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-15</v>
+        <v>26-13</v>
       </c>
       <c r="L247" s="6"/>
       <c r="M247" s="6"/>
@@ -9629,11 +9604,11 @@
       </c>
       <c r="B248">
         <f t="shared" si="49"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C248" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-16</v>
+        <v>26-14</v>
       </c>
       <c r="L248" s="6"/>
       <c r="M248" s="6"/>
@@ -9645,11 +9620,11 @@
       </c>
       <c r="B249">
         <f t="shared" si="49"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C249" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-17</v>
+        <v>26-15</v>
       </c>
       <c r="L249" s="6"/>
       <c r="M249" s="6"/>
@@ -9661,11 +9636,11 @@
       </c>
       <c r="B250">
         <f t="shared" si="49"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C250" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-18</v>
+        <v>26-16</v>
       </c>
       <c r="L250" s="6"/>
       <c r="M250" s="6"/>
@@ -9677,11 +9652,11 @@
       </c>
       <c r="B251">
         <f t="shared" si="49"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C251" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-19</v>
+        <v>26-17</v>
       </c>
       <c r="L251" s="6"/>
       <c r="M251" s="6"/>
@@ -9693,11 +9668,11 @@
       </c>
       <c r="B252">
         <f t="shared" si="49"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C252" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-20</v>
+        <v>26-18</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
@@ -9709,11 +9684,11 @@
       </c>
       <c r="B253">
         <f t="shared" si="49"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C253" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-21</v>
+        <v>26-19</v>
       </c>
       <c r="L253" s="6"/>
       <c r="M253" s="6"/>
@@ -9725,11 +9700,11 @@
       </c>
       <c r="B254">
         <f t="shared" si="49"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C254" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-22</v>
+        <v>26-20</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
@@ -9741,11 +9716,11 @@
       </c>
       <c r="B255">
         <f t="shared" si="49"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C255" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-23</v>
+        <v>26-21</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
@@ -9757,11 +9732,11 @@
       </c>
       <c r="B256">
         <f t="shared" si="49"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C256" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-24</v>
+        <v>26-22</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
@@ -9773,11 +9748,11 @@
       </c>
       <c r="B257">
         <f t="shared" si="49"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C257" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-25</v>
+        <v>26-23</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
@@ -9789,11 +9764,11 @@
       </c>
       <c r="B258">
         <f t="shared" si="49"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C258" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-26</v>
+        <v>26-24</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
@@ -9805,11 +9780,11 @@
       </c>
       <c r="B259">
         <f t="shared" si="49"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C259" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-27</v>
+        <v>26-25</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
@@ -9821,11 +9796,11 @@
       </c>
       <c r="B260">
         <f t="shared" si="49"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C260" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-28</v>
+        <v>26-26</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
@@ -9837,11 +9812,11 @@
       </c>
       <c r="B261">
         <f t="shared" si="49"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C261" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-29</v>
+        <v>26-27</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
@@ -9853,11 +9828,11 @@
       </c>
       <c r="B262">
         <f t="shared" si="49"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C262" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-30</v>
+        <v>26-28</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
@@ -9869,11 +9844,11 @@
       </c>
       <c r="B263">
         <f t="shared" si="49"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C263" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-31</v>
+        <v>26-29</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
@@ -9885,11 +9860,11 @@
       </c>
       <c r="B264">
         <f t="shared" si="49"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C264" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-32</v>
+        <v>26-30</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
@@ -9901,11 +9876,11 @@
       </c>
       <c r="B265">
         <f t="shared" si="49"/>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C265" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-33</v>
+        <v>26-31</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
@@ -9917,11 +9892,11 @@
       </c>
       <c r="B266">
         <f t="shared" si="49"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C266" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-34</v>
+        <v>26-32</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
@@ -9933,11 +9908,11 @@
       </c>
       <c r="B267">
         <f t="shared" si="49"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C267" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-35</v>
+        <v>26-33</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
@@ -9949,11 +9924,11 @@
       </c>
       <c r="B268">
         <f t="shared" si="49"/>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C268" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-36</v>
+        <v>26-34</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
@@ -9965,11 +9940,11 @@
       </c>
       <c r="B269">
         <f t="shared" si="49"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C269" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-37</v>
+        <v>26-35</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
@@ -9981,11 +9956,11 @@
       </c>
       <c r="B270">
         <f t="shared" si="49"/>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C270" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-38</v>
+        <v>26-36</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
@@ -9997,11 +9972,11 @@
       </c>
       <c r="B271">
         <f t="shared" si="49"/>
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C271" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-39</v>
+        <v>26-37</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
@@ -10013,11 +9988,11 @@
       </c>
       <c r="B272">
         <f t="shared" si="49"/>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C272" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-40</v>
+        <v>26-38</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
@@ -10029,11 +10004,11 @@
       </c>
       <c r="B273">
         <f t="shared" si="49"/>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C273" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-41</v>
+        <v>26-39</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
@@ -10045,11 +10020,11 @@
       </c>
       <c r="B274">
         <f t="shared" si="49"/>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C274" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-42</v>
+        <v>26-40</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
@@ -10061,11 +10036,11 @@
       </c>
       <c r="B275">
         <f t="shared" si="49"/>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C275" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-43</v>
+        <v>26-41</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
@@ -10077,11 +10052,11 @@
       </c>
       <c r="B276">
         <f t="shared" si="49"/>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C276" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-44</v>
+        <v>26-42</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
@@ -10093,11 +10068,11 @@
       </c>
       <c r="B277">
         <f t="shared" si="49"/>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C277" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-45</v>
+        <v>26-43</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
@@ -10109,11 +10084,11 @@
       </c>
       <c r="B278">
         <f t="shared" si="49"/>
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C278" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-46</v>
+        <v>26-44</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
@@ -10125,11 +10100,11 @@
       </c>
       <c r="B279">
         <f t="shared" si="49"/>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C279" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-47</v>
+        <v>26-45</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
@@ -10141,11 +10116,11 @@
       </c>
       <c r="B280">
         <f t="shared" si="49"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C280" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-48</v>
+        <v>26-46</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
@@ -10157,11 +10132,11 @@
       </c>
       <c r="B281">
         <f t="shared" si="49"/>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C281" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-49</v>
+        <v>26-47</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
@@ -10173,11 +10148,11 @@
       </c>
       <c r="B282">
         <f t="shared" si="49"/>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C282" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-50</v>
+        <v>26-48</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
@@ -10189,11 +10164,11 @@
       </c>
       <c r="B283">
         <f t="shared" si="49"/>
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C283" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-51</v>
+        <v>26-49</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
@@ -10205,11 +10180,11 @@
       </c>
       <c r="B284">
         <f t="shared" si="49"/>
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C284" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-52</v>
+        <v>26-50</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
@@ -10221,11 +10196,11 @@
       </c>
       <c r="B285">
         <f t="shared" si="49"/>
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C285" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-53</v>
+        <v>26-51</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
@@ -10237,11 +10212,11 @@
       </c>
       <c r="B286">
         <f t="shared" si="49"/>
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C286" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-54</v>
+        <v>26-52</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
@@ -10253,11 +10228,11 @@
       </c>
       <c r="B287">
         <f t="shared" si="49"/>
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C287" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-55</v>
+        <v>26-53</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
@@ -10269,11 +10244,11 @@
       </c>
       <c r="B288">
         <f t="shared" si="49"/>
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C288" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-56</v>
+        <v>26-54</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
@@ -10285,11 +10260,11 @@
       </c>
       <c r="B289">
         <f t="shared" si="49"/>
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C289" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-57</v>
+        <v>26-55</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
@@ -10301,11 +10276,11 @@
       </c>
       <c r="B290">
         <f t="shared" si="49"/>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C290" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-58</v>
+        <v>26-56</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
@@ -10317,11 +10292,11 @@
       </c>
       <c r="B291">
         <f t="shared" si="49"/>
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C291" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-59</v>
+        <v>26-57</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
@@ -10333,11 +10308,11 @@
       </c>
       <c r="B292">
         <f t="shared" si="49"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C292" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-60</v>
+        <v>26-58</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
@@ -10349,11 +10324,11 @@
       </c>
       <c r="B293">
         <f t="shared" si="49"/>
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C293" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-61</v>
+        <v>26-59</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
@@ -10365,11 +10340,11 @@
       </c>
       <c r="B294">
         <f t="shared" si="49"/>
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C294" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-62</v>
+        <v>26-60</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
@@ -10381,11 +10356,11 @@
       </c>
       <c r="B295">
         <f t="shared" si="49"/>
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C295" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-63</v>
+        <v>26-61</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
@@ -10397,11 +10372,11 @@
       </c>
       <c r="B296">
         <f t="shared" si="49"/>
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C296" s="3" t="str">
         <f t="shared" si="50"/>
-        <v>26-64</v>
+        <v>26-62</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
@@ -10413,11 +10388,11 @@
       </c>
       <c r="B297">
         <f t="shared" ref="B297:B360" si="52">IF(A297=A296,B296+1,1)</f>
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C297" s="3" t="str">
         <f t="shared" ref="C297:C360" si="53">CONCATENATE(A297,"-",B297)</f>
-        <v>26-65</v>
+        <v>26-63</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
@@ -10429,11 +10404,11 @@
       </c>
       <c r="B298">
         <f t="shared" si="52"/>
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C298" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-66</v>
+        <v>26-64</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
@@ -10445,11 +10420,11 @@
       </c>
       <c r="B299">
         <f t="shared" si="52"/>
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C299" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-67</v>
+        <v>26-65</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
@@ -10461,11 +10436,11 @@
       </c>
       <c r="B300">
         <f t="shared" si="52"/>
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C300" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-68</v>
+        <v>26-66</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
@@ -10477,11 +10452,11 @@
       </c>
       <c r="B301">
         <f t="shared" si="52"/>
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C301" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-69</v>
+        <v>26-67</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
@@ -10493,11 +10468,11 @@
       </c>
       <c r="B302">
         <f t="shared" si="52"/>
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C302" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-70</v>
+        <v>26-68</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
@@ -10509,11 +10484,11 @@
       </c>
       <c r="B303">
         <f t="shared" si="52"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C303" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-71</v>
+        <v>26-69</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
@@ -10525,11 +10500,11 @@
       </c>
       <c r="B304">
         <f t="shared" si="52"/>
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C304" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-72</v>
+        <v>26-70</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
@@ -10541,11 +10516,11 @@
       </c>
       <c r="B305">
         <f t="shared" si="52"/>
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C305" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-73</v>
+        <v>26-71</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
@@ -10557,11 +10532,11 @@
       </c>
       <c r="B306">
         <f t="shared" si="52"/>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C306" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-74</v>
+        <v>26-72</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
@@ -10573,11 +10548,11 @@
       </c>
       <c r="B307">
         <f t="shared" si="52"/>
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C307" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-75</v>
+        <v>26-73</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
@@ -10589,11 +10564,11 @@
       </c>
       <c r="B308">
         <f t="shared" si="52"/>
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C308" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-76</v>
+        <v>26-74</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
@@ -10605,11 +10580,11 @@
       </c>
       <c r="B309">
         <f t="shared" si="52"/>
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C309" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-77</v>
+        <v>26-75</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
@@ -10621,11 +10596,11 @@
       </c>
       <c r="B310">
         <f t="shared" si="52"/>
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C310" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-78</v>
+        <v>26-76</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
@@ -10637,11 +10612,11 @@
       </c>
       <c r="B311">
         <f t="shared" si="52"/>
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C311" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-79</v>
+        <v>26-77</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
@@ -10653,11 +10628,11 @@
       </c>
       <c r="B312">
         <f t="shared" si="52"/>
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C312" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-80</v>
+        <v>26-78</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
@@ -10669,11 +10644,11 @@
       </c>
       <c r="B313">
         <f t="shared" si="52"/>
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C313" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-81</v>
+        <v>26-79</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
@@ -10685,11 +10660,11 @@
       </c>
       <c r="B314">
         <f t="shared" si="52"/>
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C314" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-82</v>
+        <v>26-80</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
@@ -10701,11 +10676,11 @@
       </c>
       <c r="B315">
         <f t="shared" si="52"/>
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C315" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-83</v>
+        <v>26-81</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
@@ -10717,11 +10692,11 @@
       </c>
       <c r="B316">
         <f t="shared" si="52"/>
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C316" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-84</v>
+        <v>26-82</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
@@ -10733,11 +10708,11 @@
       </c>
       <c r="B317">
         <f t="shared" si="52"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C317" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-85</v>
+        <v>26-83</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
@@ -10749,11 +10724,11 @@
       </c>
       <c r="B318">
         <f t="shared" si="52"/>
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C318" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-86</v>
+        <v>26-84</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
@@ -10765,11 +10740,11 @@
       </c>
       <c r="B319">
         <f t="shared" si="52"/>
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C319" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-87</v>
+        <v>26-85</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
@@ -10781,11 +10756,11 @@
       </c>
       <c r="B320">
         <f t="shared" si="52"/>
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C320" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-88</v>
+        <v>26-86</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
@@ -10797,11 +10772,11 @@
       </c>
       <c r="B321">
         <f t="shared" si="52"/>
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C321" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-89</v>
+        <v>26-87</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
@@ -10813,11 +10788,11 @@
       </c>
       <c r="B322">
         <f t="shared" si="52"/>
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C322" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-90</v>
+        <v>26-88</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
@@ -10829,11 +10804,11 @@
       </c>
       <c r="B323">
         <f t="shared" si="52"/>
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C323" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-91</v>
+        <v>26-89</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
@@ -10845,11 +10820,11 @@
       </c>
       <c r="B324">
         <f t="shared" si="52"/>
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C324" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-92</v>
+        <v>26-90</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
@@ -10861,11 +10836,11 @@
       </c>
       <c r="B325">
         <f t="shared" si="52"/>
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C325" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-93</v>
+        <v>26-91</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
@@ -10877,11 +10852,11 @@
       </c>
       <c r="B326">
         <f t="shared" si="52"/>
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C326" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-94</v>
+        <v>26-92</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
@@ -10893,11 +10868,11 @@
       </c>
       <c r="B327">
         <f t="shared" si="52"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C327" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-95</v>
+        <v>26-93</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
@@ -10909,11 +10884,11 @@
       </c>
       <c r="B328">
         <f t="shared" si="52"/>
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C328" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-96</v>
+        <v>26-94</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
@@ -10925,11 +10900,11 @@
       </c>
       <c r="B329">
         <f t="shared" si="52"/>
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C329" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-97</v>
+        <v>26-95</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
@@ -10941,11 +10916,11 @@
       </c>
       <c r="B330">
         <f t="shared" si="52"/>
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C330" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-98</v>
+        <v>26-96</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
@@ -10957,11 +10932,11 @@
       </c>
       <c r="B331">
         <f t="shared" si="52"/>
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C331" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-99</v>
+        <v>26-97</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
@@ -10973,11 +10948,11 @@
       </c>
       <c r="B332">
         <f t="shared" si="52"/>
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C332" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-100</v>
+        <v>26-98</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
@@ -10989,11 +10964,11 @@
       </c>
       <c r="B333">
         <f t="shared" si="52"/>
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C333" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-101</v>
+        <v>26-99</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
@@ -11005,11 +10980,11 @@
       </c>
       <c r="B334">
         <f t="shared" si="52"/>
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C334" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-102</v>
+        <v>26-100</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
@@ -11021,11 +10996,11 @@
       </c>
       <c r="B335">
         <f t="shared" si="52"/>
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C335" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-103</v>
+        <v>26-101</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
@@ -11037,11 +11012,11 @@
       </c>
       <c r="B336">
         <f t="shared" si="52"/>
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C336" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-104</v>
+        <v>26-102</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
@@ -11053,11 +11028,11 @@
       </c>
       <c r="B337">
         <f t="shared" si="52"/>
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C337" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-105</v>
+        <v>26-103</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
@@ -11069,11 +11044,11 @@
       </c>
       <c r="B338">
         <f t="shared" si="52"/>
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C338" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-106</v>
+        <v>26-104</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
@@ -11085,11 +11060,11 @@
       </c>
       <c r="B339">
         <f t="shared" si="52"/>
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C339" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-107</v>
+        <v>26-105</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
@@ -11101,11 +11076,11 @@
       </c>
       <c r="B340">
         <f t="shared" si="52"/>
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C340" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-108</v>
+        <v>26-106</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
@@ -11117,11 +11092,11 @@
       </c>
       <c r="B341">
         <f t="shared" si="52"/>
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C341" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-109</v>
+        <v>26-107</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
@@ -11133,11 +11108,11 @@
       </c>
       <c r="B342">
         <f t="shared" si="52"/>
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C342" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-110</v>
+        <v>26-108</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
@@ -11149,11 +11124,11 @@
       </c>
       <c r="B343">
         <f t="shared" si="52"/>
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C343" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-111</v>
+        <v>26-109</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
@@ -11165,11 +11140,11 @@
       </c>
       <c r="B344">
         <f t="shared" si="52"/>
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C344" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-112</v>
+        <v>26-110</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
@@ -11181,11 +11156,11 @@
       </c>
       <c r="B345">
         <f t="shared" si="52"/>
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C345" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-113</v>
+        <v>26-111</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
@@ -11197,11 +11172,11 @@
       </c>
       <c r="B346">
         <f t="shared" si="52"/>
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C346" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-114</v>
+        <v>26-112</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
@@ -11213,11 +11188,11 @@
       </c>
       <c r="B347">
         <f t="shared" si="52"/>
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C347" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-115</v>
+        <v>26-113</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
@@ -11229,11 +11204,11 @@
       </c>
       <c r="B348">
         <f t="shared" si="52"/>
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C348" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-116</v>
+        <v>26-114</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
@@ -11245,11 +11220,11 @@
       </c>
       <c r="B349">
         <f t="shared" si="52"/>
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C349" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-117</v>
+        <v>26-115</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
@@ -11261,11 +11236,11 @@
       </c>
       <c r="B350">
         <f t="shared" si="52"/>
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C350" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-118</v>
+        <v>26-116</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
@@ -11277,11 +11252,11 @@
       </c>
       <c r="B351">
         <f t="shared" si="52"/>
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C351" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-119</v>
+        <v>26-117</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
@@ -11293,11 +11268,11 @@
       </c>
       <c r="B352">
         <f t="shared" si="52"/>
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C352" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-120</v>
+        <v>26-118</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
@@ -11309,11 +11284,11 @@
       </c>
       <c r="B353">
         <f t="shared" si="52"/>
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C353" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-121</v>
+        <v>26-119</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
@@ -11325,11 +11300,11 @@
       </c>
       <c r="B354">
         <f t="shared" si="52"/>
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C354" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-122</v>
+        <v>26-120</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
@@ -11341,11 +11316,11 @@
       </c>
       <c r="B355">
         <f t="shared" si="52"/>
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C355" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-123</v>
+        <v>26-121</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
@@ -11357,11 +11332,11 @@
       </c>
       <c r="B356">
         <f t="shared" si="52"/>
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C356" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-124</v>
+        <v>26-122</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
@@ -11373,11 +11348,11 @@
       </c>
       <c r="B357">
         <f t="shared" si="52"/>
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C357" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-125</v>
+        <v>26-123</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
@@ -11389,11 +11364,11 @@
       </c>
       <c r="B358">
         <f t="shared" si="52"/>
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C358" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-126</v>
+        <v>26-124</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
@@ -11405,11 +11380,11 @@
       </c>
       <c r="B359">
         <f t="shared" si="52"/>
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C359" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-127</v>
+        <v>26-125</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
@@ -11421,11 +11396,11 @@
       </c>
       <c r="B360">
         <f t="shared" si="52"/>
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C360" s="3" t="str">
         <f t="shared" si="53"/>
-        <v>26-128</v>
+        <v>26-126</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
@@ -11437,11 +11412,11 @@
       </c>
       <c r="B361">
         <f t="shared" ref="B361:B382" si="55">IF(A361=A360,B360+1,1)</f>
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C361" s="3" t="str">
         <f t="shared" ref="C361:C382" si="56">CONCATENATE(A361,"-",B361)</f>
-        <v>26-129</v>
+        <v>26-127</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
@@ -11453,11 +11428,11 @@
       </c>
       <c r="B362">
         <f t="shared" si="55"/>
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C362" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-130</v>
+        <v>26-128</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
@@ -11469,11 +11444,11 @@
       </c>
       <c r="B363">
         <f t="shared" si="55"/>
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C363" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-131</v>
+        <v>26-129</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
@@ -11485,11 +11460,11 @@
       </c>
       <c r="B364">
         <f t="shared" si="55"/>
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C364" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-132</v>
+        <v>26-130</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
@@ -11501,11 +11476,11 @@
       </c>
       <c r="B365">
         <f t="shared" si="55"/>
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C365" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-133</v>
+        <v>26-131</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
@@ -11517,11 +11492,11 @@
       </c>
       <c r="B366">
         <f t="shared" si="55"/>
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C366" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-134</v>
+        <v>26-132</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
@@ -11533,11 +11508,11 @@
       </c>
       <c r="B367">
         <f t="shared" si="55"/>
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C367" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-135</v>
+        <v>26-133</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
@@ -11549,11 +11524,11 @@
       </c>
       <c r="B368">
         <f t="shared" si="55"/>
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C368" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-136</v>
+        <v>26-134</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
@@ -11565,11 +11540,11 @@
       </c>
       <c r="B369">
         <f t="shared" si="55"/>
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C369" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-137</v>
+        <v>26-135</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
@@ -11581,11 +11556,11 @@
       </c>
       <c r="B370">
         <f t="shared" si="55"/>
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C370" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-138</v>
+        <v>26-136</v>
       </c>
       <c r="L370" s="6"/>
       <c r="M370" s="6"/>
@@ -11597,11 +11572,11 @@
       </c>
       <c r="B371">
         <f t="shared" si="55"/>
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C371" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-139</v>
+        <v>26-137</v>
       </c>
       <c r="L371" s="6"/>
       <c r="M371" s="6"/>
@@ -11613,11 +11588,11 @@
       </c>
       <c r="B372">
         <f t="shared" si="55"/>
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C372" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-140</v>
+        <v>26-138</v>
       </c>
       <c r="L372" s="6"/>
       <c r="M372" s="6"/>
@@ -11629,11 +11604,11 @@
       </c>
       <c r="B373">
         <f t="shared" si="55"/>
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C373" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-141</v>
+        <v>26-139</v>
       </c>
       <c r="L373" s="6"/>
       <c r="M373" s="6"/>
@@ -11645,11 +11620,11 @@
       </c>
       <c r="B374">
         <f t="shared" si="55"/>
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C374" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-142</v>
+        <v>26-140</v>
       </c>
       <c r="L374" s="6"/>
       <c r="M374" s="6"/>
@@ -11661,11 +11636,11 @@
       </c>
       <c r="B375">
         <f t="shared" si="55"/>
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C375" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-143</v>
+        <v>26-141</v>
       </c>
       <c r="L375" s="6"/>
       <c r="M375" s="6"/>
@@ -11677,11 +11652,11 @@
       </c>
       <c r="B376">
         <f t="shared" si="55"/>
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C376" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-144</v>
+        <v>26-142</v>
       </c>
       <c r="L376" s="6"/>
       <c r="M376" s="6"/>
@@ -11693,11 +11668,11 @@
       </c>
       <c r="B377">
         <f t="shared" si="55"/>
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C377" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-145</v>
+        <v>26-143</v>
       </c>
       <c r="L377" s="6"/>
       <c r="M377" s="6"/>
@@ -11709,11 +11684,11 @@
       </c>
       <c r="B378">
         <f t="shared" si="55"/>
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C378" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-146</v>
+        <v>26-144</v>
       </c>
       <c r="L378" s="6"/>
       <c r="M378" s="6"/>
@@ -11725,11 +11700,11 @@
       </c>
       <c r="B379">
         <f t="shared" si="55"/>
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C379" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-147</v>
+        <v>26-145</v>
       </c>
       <c r="L379" s="6"/>
       <c r="M379" s="6"/>
@@ -11741,11 +11716,11 @@
       </c>
       <c r="B380">
         <f t="shared" si="55"/>
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C380" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-148</v>
+        <v>26-146</v>
       </c>
       <c r="L380" s="6"/>
       <c r="M380" s="6"/>
@@ -11757,11 +11732,11 @@
       </c>
       <c r="B381">
         <f t="shared" si="55"/>
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C381" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-149</v>
+        <v>26-147</v>
       </c>
       <c r="L381" s="6"/>
       <c r="M381" s="6"/>
@@ -11773,11 +11748,11 @@
       </c>
       <c r="B382">
         <f t="shared" si="55"/>
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C382" s="3" t="str">
         <f t="shared" si="56"/>
-        <v>26-150</v>
+        <v>26-148</v>
       </c>
       <c r="L382" s="6"/>
       <c r="M382" s="6"/>
@@ -14535,347 +14510,347 @@
     <mergeCell ref="L188:L191"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsBlanks" dxfId="74" priority="73">
+    <cfRule type="containsBlanks" dxfId="71" priority="73">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="70" priority="74" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsText" dxfId="72" priority="75" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="69" priority="75" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsBlanks" dxfId="71" priority="70">
+    <cfRule type="containsBlanks" dxfId="68" priority="70">
       <formula>LEN(TRIM(K200))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsBlanks" dxfId="68" priority="64">
+    <cfRule type="containsBlanks" dxfId="65" priority="64">
       <formula>LEN(TRIM(K201))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsBlanks" dxfId="65" priority="61">
+    <cfRule type="containsBlanks" dxfId="62" priority="61">
       <formula>LEN(TRIM(K202))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="64" priority="62" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="63" priority="63" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsBlanks" dxfId="62" priority="58">
+    <cfRule type="containsBlanks" dxfId="59" priority="58">
       <formula>LEN(TRIM(K203))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="61" priority="59" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="60" priority="60" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="59" priority="55">
+    <cfRule type="containsBlanks" dxfId="56" priority="55">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsBlanks" dxfId="58" priority="52">
+    <cfRule type="containsBlanks" dxfId="55" priority="52">
       <formula>LEN(TRIM(K207))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsBlanks" dxfId="57" priority="49">
+    <cfRule type="containsBlanks" dxfId="54" priority="49">
       <formula>LEN(TRIM(K209))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsBlanks" dxfId="56" priority="46">
+    <cfRule type="containsBlanks" dxfId="53" priority="46">
       <formula>LEN(TRIM(K210))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsBlanks" dxfId="55" priority="43">
+    <cfRule type="containsBlanks" dxfId="52" priority="43">
       <formula>LEN(TRIM(K212))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsBlanks" dxfId="54" priority="40">
+    <cfRule type="containsBlanks" dxfId="51" priority="40">
       <formula>LEN(TRIM(K214))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K231:K232 K219:K229">
-    <cfRule type="containsBlanks" dxfId="53" priority="37">
+    <cfRule type="containsBlanks" dxfId="50" priority="37">
       <formula>LEN(TRIM(K216))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="52" priority="31">
+    <cfRule type="containsBlanks" dxfId="49" priority="31">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="51" priority="56" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="48" priority="56" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="50" priority="57" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="47" priority="57" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsBlanks" dxfId="49" priority="28">
+    <cfRule type="containsBlanks" dxfId="46" priority="28">
       <formula>LEN(TRIM(K208))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="48" priority="53" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="45" priority="53" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="47" priority="54" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="44" priority="54" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="46" priority="25">
+    <cfRule type="containsBlanks" dxfId="43" priority="25">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="42" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="44" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="41" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsBlanks" dxfId="43" priority="22">
+    <cfRule type="containsBlanks" dxfId="40" priority="22">
       <formula>LEN(TRIM(K211))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="42" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="39" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="41" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="38" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsBlanks" dxfId="40" priority="19">
+    <cfRule type="containsBlanks" dxfId="37" priority="19">
       <formula>LEN(TRIM(K213))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="39" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="36" priority="44" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="38" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="35" priority="45" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsBlanks" dxfId="37" priority="16">
+    <cfRule type="containsBlanks" dxfId="34" priority="16">
       <formula>LEN(TRIM(K215))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="33" priority="41" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="35" priority="42" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="32" priority="42" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K231:K232 K219:K229">
-    <cfRule type="containsText" dxfId="34" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K231:K232 K219:K229">
-    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="30" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="30" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="26" priority="23" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="24" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="21" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K230">
-    <cfRule type="containsBlanks" dxfId="20" priority="13">
+    <cfRule type="containsBlanks" dxfId="17" priority="13">
       <formula>LEN(TRIM(K230))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K230">
-    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K230))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K230">
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K230))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsBlanks" dxfId="17" priority="10">
+    <cfRule type="containsBlanks" dxfId="14" priority="10">
       <formula>LEN(TRIM(K217))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsBlanks" dxfId="14" priority="7">
+    <cfRule type="containsBlanks" dxfId="11" priority="7">
       <formula>LEN(TRIM(K218))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K233">
-    <cfRule type="containsBlanks" dxfId="11" priority="4">
+    <cfRule type="containsBlanks" dxfId="8" priority="4">
       <formula>LEN(TRIM(K233))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K233">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K233))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K233">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K233))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K234">
+  <conditionalFormatting sqref="K234:K235">
     <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(K234))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K234">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K234:K235">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K234))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K234">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="fail">
+  <conditionalFormatting sqref="K234:K235">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K234))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added manual tests for #370
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="302">
   <si>
     <t>Test Number</t>
   </si>
@@ -917,6 +917,12 @@
   </si>
   <si>
     <t>Confirm that you can switch perspectives with the function keys</t>
+  </si>
+  <si>
+    <t>Create a hidden block. Right click on any group and confirm that you can switch between showing and hiding the block.</t>
+  </si>
+  <si>
+    <t>Create a hidden block. Right click on the block and confirm that you can switch between showing and hiding the block.</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1215,13 +1221,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
+  <dxfs count="75">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2230,6 +2239,48 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2527,11 +2578,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1069"/>
+  <dimension ref="A1:N1071"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I241" sqref="I241"/>
+      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I220" sqref="I220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -7052,7 +7103,7 @@
         <v>1</v>
       </c>
       <c r="C157" s="22" t="str">
-        <f t="shared" ref="C157:C231" si="25">CONCATENATE(A157,"-",B157)</f>
+        <f t="shared" ref="C157:C233" si="25">CONCATENATE(A157,"-",B157)</f>
         <v>16-1</v>
       </c>
       <c r="D157" s="46"/>
@@ -7074,11 +7125,11 @@
     </row>
     <row r="158" spans="1:13" ht="15">
       <c r="A158">
-        <f t="shared" ref="A158:A232" si="26">A157</f>
+        <f t="shared" ref="A158:A234" si="26">A157</f>
         <v>16</v>
       </c>
       <c r="B158">
-        <f t="shared" ref="B158:B232" si="27">IF(A158=A157,B157+1,1)</f>
+        <f t="shared" ref="B158:B234" si="27">IF(A158=A157,B157+1,1)</f>
         <v>2</v>
       </c>
       <c r="C158" s="22" t="str">
@@ -7992,7 +8043,7 @@
       </c>
       <c r="J188" s="8"/>
       <c r="K188" s="7"/>
-      <c r="L188" s="49"/>
+      <c r="L188" s="50"/>
     </row>
     <row r="189" spans="1:13" ht="30">
       <c r="A189">
@@ -8021,7 +8072,7 @@
       </c>
       <c r="J189" s="8"/>
       <c r="K189" s="7"/>
-      <c r="L189" s="50"/>
+      <c r="L189" s="51"/>
       <c r="M189" s="6"/>
     </row>
     <row r="190" spans="1:13" ht="45">
@@ -8051,7 +8102,7 @@
       </c>
       <c r="J190" s="8"/>
       <c r="K190" s="7"/>
-      <c r="L190" s="50"/>
+      <c r="L190" s="51"/>
       <c r="M190" s="6"/>
     </row>
     <row r="191" spans="1:13" ht="30">
@@ -8081,7 +8132,7 @@
       </c>
       <c r="J191" s="8"/>
       <c r="K191" s="7"/>
-      <c r="L191" s="51"/>
+      <c r="L191" s="52"/>
       <c r="M191" s="6"/>
     </row>
     <row r="192" spans="1:13" ht="30">
@@ -8867,15 +8918,15 @@
     </row>
     <row r="217" spans="1:13" ht="51.75">
       <c r="A217">
-        <f t="shared" ref="A217:A218" si="44">A215</f>
+        <f t="shared" ref="A217" si="44">A215</f>
         <v>21</v>
       </c>
       <c r="B217">
-        <f t="shared" ref="B217:B218" si="45">IF(A217=A216,B216+1,1)</f>
+        <f t="shared" ref="B217" si="45">IF(A217=A216,B216+1,1)</f>
         <v>24</v>
       </c>
       <c r="C217" s="19" t="str">
-        <f t="shared" ref="C217:C218" si="46">CONCATENATE(A217,"-",B217)</f>
+        <f t="shared" ref="C217:C219" si="46">CONCATENATE(A217,"-",B217)</f>
         <v>21-24</v>
       </c>
       <c r="D217" s="20"/>
@@ -8895,11 +8946,11 @@
     </row>
     <row r="218" spans="1:13" ht="39">
       <c r="A218">
-        <f t="shared" si="44"/>
+        <f>A216</f>
         <v>21</v>
       </c>
       <c r="B218">
-        <f t="shared" si="45"/>
+        <f>IF(A218=A217,B217+1,1)</f>
         <v>25</v>
       </c>
       <c r="C218" s="19" t="str">
@@ -8921,100 +8972,100 @@
       <c r="L218" s="39"/>
       <c r="M218" s="6"/>
     </row>
-    <row r="219" spans="1:13" ht="26.25">
+    <row r="219" spans="1:13" ht="39">
       <c r="A219">
-        <v>22</v>
+        <f>A216</f>
+        <v>21</v>
       </c>
       <c r="B219">
-        <v>1</v>
-      </c>
-      <c r="C219" s="22" t="str">
-        <f>CONCATENATE(A219,"-",B219)</f>
-        <v>22-1</v>
-      </c>
-      <c r="D219" s="23"/>
-      <c r="E219" s="23"/>
-      <c r="F219" s="23"/>
-      <c r="G219" s="24"/>
-      <c r="H219" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="I219" s="25" t="s">
-        <v>248</v>
-      </c>
-      <c r="J219" s="23"/>
+        <f>IF(A219=A217,B217+1,1)</f>
+        <v>25</v>
+      </c>
+      <c r="C219" s="19" t="str">
+        <f t="shared" si="46"/>
+        <v>21-25</v>
+      </c>
+      <c r="D219" s="20"/>
+      <c r="E219" s="20"/>
+      <c r="F219" s="20"/>
+      <c r="G219" s="21"/>
+      <c r="H219" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I219" s="49" t="s">
+        <v>300</v>
+      </c>
+      <c r="J219" s="49"/>
       <c r="K219" s="21"/>
-      <c r="L219" s="26"/>
+      <c r="L219" s="49"/>
       <c r="M219" s="6"/>
     </row>
     <row r="220" spans="1:13" ht="39">
       <c r="A220">
-        <f>A219</f>
-        <v>22</v>
+        <f>A217</f>
+        <v>21</v>
       </c>
       <c r="B220">
-        <f>IF(A220=A219,B219+1,1)</f>
-        <v>2</v>
-      </c>
-      <c r="C220" s="22" t="str">
-        <f t="shared" si="25"/>
-        <v>22-2</v>
-      </c>
-      <c r="D220" s="23"/>
-      <c r="E220" s="23"/>
-      <c r="F220" s="23"/>
-      <c r="G220" s="23"/>
-      <c r="H220" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="I220" s="25" t="s">
-        <v>250</v>
-      </c>
-      <c r="J220" s="23"/>
+        <f>IF(A220=A218,B218+1,1)</f>
+        <v>26</v>
+      </c>
+      <c r="C220" s="19" t="str">
+        <f t="shared" ref="C220" si="47">CONCATENATE(A220,"-",B220)</f>
+        <v>21-26</v>
+      </c>
+      <c r="D220" s="20"/>
+      <c r="E220" s="20"/>
+      <c r="F220" s="20"/>
+      <c r="G220" s="21"/>
+      <c r="H220" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I220" s="49" t="s">
+        <v>301</v>
+      </c>
+      <c r="J220" s="49"/>
       <c r="K220" s="21"/>
-      <c r="L220" s="26"/>
+      <c r="L220" s="49"/>
       <c r="M220" s="6"/>
     </row>
     <row r="221" spans="1:13" ht="26.25">
       <c r="A221">
-        <f t="shared" si="26"/>
         <v>22</v>
       </c>
       <c r="B221">
-        <f t="shared" si="27"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C221" s="22" t="str">
-        <f t="shared" si="25"/>
-        <v>22-3</v>
+        <f>CONCATENATE(A221,"-",B221)</f>
+        <v>22-1</v>
       </c>
       <c r="D221" s="23"/>
       <c r="E221" s="23"/>
       <c r="F221" s="23"/>
-      <c r="G221" s="23"/>
+      <c r="G221" s="24"/>
       <c r="H221" s="24" t="s">
         <v>249</v>
       </c>
       <c r="I221" s="25" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J221" s="23"/>
       <c r="K221" s="21"/>
       <c r="L221" s="26"/>
       <c r="M221" s="6"/>
     </row>
-    <row r="222" spans="1:13" ht="15">
+    <row r="222" spans="1:13" ht="39">
       <c r="A222">
-        <f t="shared" si="26"/>
+        <f>A221</f>
         <v>22</v>
       </c>
       <c r="B222">
-        <f t="shared" si="27"/>
-        <v>4</v>
+        <f>IF(A222=A221,B221+1,1)</f>
+        <v>2</v>
       </c>
       <c r="C222" s="22" t="str">
         <f t="shared" si="25"/>
-        <v>22-4</v>
+        <v>22-2</v>
       </c>
       <c r="D222" s="23"/>
       <c r="E222" s="23"/>
@@ -9024,25 +9075,25 @@
         <v>249</v>
       </c>
       <c r="I222" s="25" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J222" s="23"/>
       <c r="K222" s="21"/>
       <c r="L222" s="26"/>
       <c r="M222" s="6"/>
     </row>
-    <row r="223" spans="1:13" ht="15">
+    <row r="223" spans="1:13" ht="26.25">
       <c r="A223">
         <f t="shared" si="26"/>
         <v>22</v>
       </c>
       <c r="B223">
         <f t="shared" si="27"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C223" s="22" t="str">
         <f t="shared" si="25"/>
-        <v>22-5</v>
+        <v>22-3</v>
       </c>
       <c r="D223" s="23"/>
       <c r="E223" s="23"/>
@@ -9052,7 +9103,7 @@
         <v>249</v>
       </c>
       <c r="I223" s="25" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J223" s="23"/>
       <c r="K223" s="21"/>
@@ -9066,98 +9117,94 @@
       </c>
       <c r="B224">
         <f t="shared" si="27"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C224" s="22" t="str">
         <f t="shared" si="25"/>
-        <v>22-6</v>
-      </c>
-      <c r="D224" s="36"/>
-      <c r="E224" s="36"/>
-      <c r="F224" s="36"/>
-      <c r="G224" s="36"/>
-      <c r="H224" s="27" t="s">
+        <v>22-4</v>
+      </c>
+      <c r="D224" s="23"/>
+      <c r="E224" s="23"/>
+      <c r="F224" s="23"/>
+      <c r="G224" s="23"/>
+      <c r="H224" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="I224" s="37" t="s">
-        <v>254</v>
-      </c>
-      <c r="J224" s="36"/>
+      <c r="I224" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="J224" s="23"/>
       <c r="K224" s="21"/>
-      <c r="L224" s="38"/>
+      <c r="L224" s="26"/>
       <c r="M224" s="6"/>
     </row>
-    <row r="225" spans="1:13" ht="26.25">
+    <row r="225" spans="1:13" ht="15">
       <c r="A225">
-        <v>23</v>
+        <f t="shared" si="26"/>
+        <v>22</v>
       </c>
       <c r="B225">
         <f t="shared" si="27"/>
-        <v>1</v>
-      </c>
-      <c r="C225" s="35" t="str">
+        <v>5</v>
+      </c>
+      <c r="C225" s="22" t="str">
         <f t="shared" si="25"/>
-        <v>23-1</v>
+        <v>22-5</v>
       </c>
       <c r="D225" s="23"/>
       <c r="E225" s="23"/>
       <c r="F225" s="23"/>
-      <c r="G225" s="23" t="s">
-        <v>63</v>
-      </c>
+      <c r="G225" s="23"/>
       <c r="H225" s="24" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="I225" s="25" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="J225" s="23"/>
       <c r="K225" s="21"/>
       <c r="L225" s="26"/>
       <c r="M225" s="6"/>
     </row>
-    <row r="226" spans="1:13" ht="26.25">
+    <row r="226" spans="1:13" ht="15">
       <c r="A226">
         <f t="shared" si="26"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B226">
         <f t="shared" si="27"/>
-        <v>2</v>
-      </c>
-      <c r="C226" s="3" t="str">
+        <v>6</v>
+      </c>
+      <c r="C226" s="22" t="str">
         <f t="shared" si="25"/>
-        <v>23-2</v>
-      </c>
-      <c r="D226" s="23"/>
-      <c r="E226" s="23"/>
-      <c r="F226" s="23"/>
-      <c r="G226" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="H226" s="24" t="s">
-        <v>266</v>
-      </c>
-      <c r="I226" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="J226" s="23"/>
+        <v>22-6</v>
+      </c>
+      <c r="D226" s="36"/>
+      <c r="E226" s="36"/>
+      <c r="F226" s="36"/>
+      <c r="G226" s="36"/>
+      <c r="H226" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="I226" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="J226" s="36"/>
       <c r="K226" s="21"/>
-      <c r="L226" s="26"/>
+      <c r="L226" s="38"/>
       <c r="M226" s="6"/>
     </row>
     <row r="227" spans="1:13" ht="26.25">
       <c r="A227">
-        <f t="shared" si="26"/>
         <v>23</v>
       </c>
       <c r="B227">
         <f t="shared" si="27"/>
-        <v>3</v>
-      </c>
-      <c r="C227" s="3" t="str">
+        <v>1</v>
+      </c>
+      <c r="C227" s="35" t="str">
         <f t="shared" si="25"/>
-        <v>23-3</v>
+        <v>23-1</v>
       </c>
       <c r="D227" s="23"/>
       <c r="E227" s="23"/>
@@ -9169,25 +9216,25 @@
         <v>266</v>
       </c>
       <c r="I227" s="25" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J227" s="23"/>
       <c r="K227" s="21"/>
       <c r="L227" s="26"/>
       <c r="M227" s="6"/>
     </row>
-    <row r="228" spans="1:13" ht="39">
+    <row r="228" spans="1:13" ht="26.25">
       <c r="A228">
         <f t="shared" si="26"/>
         <v>23</v>
       </c>
       <c r="B228">
         <f t="shared" si="27"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C228" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>23-4</v>
+        <v>23-2</v>
       </c>
       <c r="D228" s="23"/>
       <c r="E228" s="23"/>
@@ -9199,25 +9246,25 @@
         <v>266</v>
       </c>
       <c r="I228" s="25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J228" s="23"/>
       <c r="K228" s="21"/>
       <c r="L228" s="26"/>
       <c r="M228" s="6"/>
     </row>
-    <row r="229" spans="1:13" ht="15">
+    <row r="229" spans="1:13" ht="26.25">
       <c r="A229">
         <f t="shared" si="26"/>
         <v>23</v>
       </c>
       <c r="B229">
         <f t="shared" si="27"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C229" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>23-5</v>
+        <v>23-3</v>
       </c>
       <c r="D229" s="23"/>
       <c r="E229" s="23"/>
@@ -9229,23 +9276,25 @@
         <v>266</v>
       </c>
       <c r="I229" s="25" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J229" s="23"/>
       <c r="K229" s="21"/>
       <c r="L229" s="26"/>
       <c r="M229" s="6"/>
     </row>
-    <row r="230" spans="1:13" ht="26.25">
+    <row r="230" spans="1:13" ht="39">
       <c r="A230">
-        <v>24</v>
+        <f t="shared" si="26"/>
+        <v>23</v>
       </c>
       <c r="B230">
-        <v>6</v>
+        <f t="shared" si="27"/>
+        <v>4</v>
       </c>
       <c r="C230" s="3" t="str">
-        <f t="shared" ref="C230" si="47">CONCATENATE(A230,"-",B230)</f>
-        <v>24-6</v>
+        <f t="shared" si="25"/>
+        <v>23-4</v>
       </c>
       <c r="D230" s="23"/>
       <c r="E230" s="23"/>
@@ -9257,24 +9306,25 @@
         <v>266</v>
       </c>
       <c r="I230" s="25" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="J230" s="23"/>
       <c r="K230" s="21"/>
       <c r="L230" s="26"/>
       <c r="M230" s="6"/>
     </row>
-    <row r="231" spans="1:13" ht="26.25">
+    <row r="231" spans="1:13" ht="15">
       <c r="A231">
-        <v>25</v>
+        <f t="shared" si="26"/>
+        <v>23</v>
       </c>
       <c r="B231">
-        <f>IF(A231=A229,B229+1,1)</f>
-        <v>1</v>
+        <f t="shared" si="27"/>
+        <v>5</v>
       </c>
       <c r="C231" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>25-1</v>
+        <v>23-5</v>
       </c>
       <c r="D231" s="23"/>
       <c r="E231" s="23"/>
@@ -9283,10 +9333,10 @@
         <v>63</v>
       </c>
       <c r="H231" s="24" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I231" s="25" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J231" s="23"/>
       <c r="K231" s="21"/>
@@ -9295,16 +9345,14 @@
     </row>
     <row r="232" spans="1:13" ht="26.25">
       <c r="A232">
-        <f t="shared" si="26"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B232">
-        <f t="shared" si="27"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C232" s="3" t="str">
         <f t="shared" ref="C232" si="48">CONCATENATE(A232,"-",B232)</f>
-        <v>25-2</v>
+        <v>24-6</v>
       </c>
       <c r="D232" s="23"/>
       <c r="E232" s="23"/>
@@ -9313,81 +9361,85 @@
         <v>63</v>
       </c>
       <c r="H232" s="24" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I232" s="25" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="J232" s="23"/>
       <c r="K232" s="21"/>
       <c r="L232" s="26"/>
       <c r="M232" s="6"/>
     </row>
-    <row r="233" spans="1:13" ht="39">
+    <row r="233" spans="1:13" ht="26.25">
       <c r="A233">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B233">
-        <f t="shared" ref="B233:B296" si="49">IF(A233=A232,B232+1,1)</f>
+        <f>IF(A233=A231,B231+1,1)</f>
         <v>1</v>
       </c>
       <c r="C233" s="3" t="str">
-        <f t="shared" ref="C233:C296" si="50">CONCATENATE(A233,"-",B233)</f>
-        <v>26-1</v>
+        <f t="shared" si="25"/>
+        <v>25-1</v>
       </c>
       <c r="D233" s="23"/>
       <c r="E233" s="23"/>
       <c r="F233" s="23"/>
-      <c r="G233" s="23"/>
+      <c r="G233" s="23" t="s">
+        <v>63</v>
+      </c>
       <c r="H233" s="24" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="I233" s="25" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="J233" s="23"/>
       <c r="K233" s="21"/>
       <c r="L233" s="26"/>
       <c r="M233" s="6"/>
     </row>
-    <row r="234" spans="1:13" ht="15">
+    <row r="234" spans="1:13" ht="26.25">
       <c r="A234">
-        <f t="shared" ref="A234:A297" si="51">A233</f>
-        <v>26</v>
+        <f t="shared" si="26"/>
+        <v>25</v>
       </c>
       <c r="B234">
-        <f t="shared" si="49"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="C234" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-2</v>
+        <f t="shared" ref="C234" si="49">CONCATENATE(A234,"-",B234)</f>
+        <v>25-2</v>
       </c>
       <c r="D234" s="23"/>
       <c r="E234" s="23"/>
       <c r="F234" s="23"/>
-      <c r="G234" s="23"/>
+      <c r="G234" s="23" t="s">
+        <v>63</v>
+      </c>
       <c r="H234" s="24" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="I234" s="25" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="J234" s="23"/>
       <c r="K234" s="21"/>
       <c r="L234" s="26"/>
       <c r="M234" s="6"/>
     </row>
-    <row r="235" spans="1:13" ht="26.25">
+    <row r="235" spans="1:13" ht="39">
       <c r="A235">
-        <f t="shared" si="51"/>
         <v>26</v>
       </c>
       <c r="B235">
+        <f t="shared" ref="B235:B298" si="50">IF(A235=A234,B234+1,1)</f>
         <v>1</v>
       </c>
       <c r="C235" s="3" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" ref="C235:C298" si="51">CONCATENATE(A235,"-",B235)</f>
         <v>26-1</v>
       </c>
       <c r="D235" s="23"/>
@@ -9395,10 +9447,10 @@
       <c r="F235" s="23"/>
       <c r="G235" s="23"/>
       <c r="H235" s="24" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I235" s="25" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J235" s="23"/>
       <c r="K235" s="21"/>
@@ -9407,2361 +9459,2408 @@
     </row>
     <row r="236" spans="1:13" ht="15">
       <c r="A236">
+        <f t="shared" ref="A236:A299" si="52">A235</f>
+        <v>26</v>
+      </c>
+      <c r="B236">
+        <f t="shared" si="50"/>
+        <v>2</v>
+      </c>
+      <c r="C236" s="3" t="str">
         <f t="shared" si="51"/>
+        <v>26-2</v>
+      </c>
+      <c r="D236" s="23"/>
+      <c r="E236" s="23"/>
+      <c r="F236" s="23"/>
+      <c r="G236" s="23"/>
+      <c r="H236" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="I236" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="J236" s="23"/>
+      <c r="K236" s="21"/>
+      <c r="L236" s="26"/>
+      <c r="M236" s="6"/>
+    </row>
+    <row r="237" spans="1:13" ht="26.25">
+      <c r="A237">
+        <f t="shared" si="52"/>
         <v>26</v>
       </c>
-      <c r="B236">
-        <f t="shared" si="49"/>
-        <v>2</v>
-      </c>
-      <c r="C236" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-2</v>
-      </c>
-      <c r="L236" s="6"/>
-      <c r="M236" s="6"/>
-    </row>
-    <row r="237" spans="1:13" ht="15">
-      <c r="A237">
+      <c r="B237">
+        <v>1</v>
+      </c>
+      <c r="C237" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B237">
-        <f t="shared" si="49"/>
-        <v>3</v>
-      </c>
-      <c r="C237" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-3</v>
-      </c>
-      <c r="L237" s="6"/>
+        <v>26-1</v>
+      </c>
+      <c r="D237" s="23"/>
+      <c r="E237" s="23"/>
+      <c r="F237" s="23"/>
+      <c r="G237" s="23"/>
+      <c r="H237" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="I237" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="J237" s="23"/>
+      <c r="K237" s="21"/>
+      <c r="L237" s="26"/>
       <c r="M237" s="6"/>
     </row>
     <row r="238" spans="1:13" ht="15">
       <c r="A238">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B238">
+        <f t="shared" si="50"/>
+        <v>2</v>
+      </c>
+      <c r="C238" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B238">
-        <f t="shared" si="49"/>
-        <v>4</v>
-      </c>
-      <c r="C238" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-4</v>
+        <v>26-2</v>
       </c>
       <c r="L238" s="6"/>
       <c r="M238" s="6"/>
     </row>
     <row r="239" spans="1:13" ht="15">
       <c r="A239">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B239">
+        <f t="shared" si="50"/>
+        <v>3</v>
+      </c>
+      <c r="C239" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B239">
-        <f t="shared" si="49"/>
-        <v>5</v>
-      </c>
-      <c r="C239" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-5</v>
+        <v>26-3</v>
       </c>
       <c r="L239" s="6"/>
       <c r="M239" s="6"/>
     </row>
     <row r="240" spans="1:13" ht="15">
       <c r="A240">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B240">
+        <f t="shared" si="50"/>
+        <v>4</v>
+      </c>
+      <c r="C240" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B240">
-        <f t="shared" si="49"/>
-        <v>6</v>
-      </c>
-      <c r="C240" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-6</v>
+        <v>26-4</v>
       </c>
       <c r="L240" s="6"/>
       <c r="M240" s="6"/>
     </row>
     <row r="241" spans="1:13" ht="15">
       <c r="A241">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B241">
+        <f t="shared" si="50"/>
+        <v>5</v>
+      </c>
+      <c r="C241" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B241">
-        <f t="shared" si="49"/>
-        <v>7</v>
-      </c>
-      <c r="C241" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-7</v>
+        <v>26-5</v>
       </c>
       <c r="L241" s="6"/>
       <c r="M241" s="6"/>
     </row>
     <row r="242" spans="1:13" ht="15">
       <c r="A242">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B242">
+        <f t="shared" si="50"/>
+        <v>6</v>
+      </c>
+      <c r="C242" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B242">
-        <f t="shared" si="49"/>
-        <v>8</v>
-      </c>
-      <c r="C242" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-8</v>
+        <v>26-6</v>
       </c>
       <c r="L242" s="6"/>
       <c r="M242" s="6"/>
     </row>
     <row r="243" spans="1:13" ht="15">
       <c r="A243">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B243">
+        <f t="shared" si="50"/>
+        <v>7</v>
+      </c>
+      <c r="C243" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B243">
-        <f t="shared" si="49"/>
-        <v>9</v>
-      </c>
-      <c r="C243" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-9</v>
+        <v>26-7</v>
       </c>
       <c r="L243" s="6"/>
       <c r="M243" s="6"/>
     </row>
     <row r="244" spans="1:13" ht="15">
       <c r="A244">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B244">
+        <f t="shared" si="50"/>
+        <v>8</v>
+      </c>
+      <c r="C244" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B244">
-        <f t="shared" si="49"/>
-        <v>10</v>
-      </c>
-      <c r="C244" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-10</v>
+        <v>26-8</v>
       </c>
       <c r="L244" s="6"/>
       <c r="M244" s="6"/>
     </row>
     <row r="245" spans="1:13" ht="15">
       <c r="A245">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B245">
+        <f t="shared" si="50"/>
+        <v>9</v>
+      </c>
+      <c r="C245" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B245">
-        <f t="shared" si="49"/>
-        <v>11</v>
-      </c>
-      <c r="C245" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-11</v>
+        <v>26-9</v>
       </c>
       <c r="L245" s="6"/>
       <c r="M245" s="6"/>
     </row>
     <row r="246" spans="1:13" ht="15">
       <c r="A246">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B246">
+        <f t="shared" si="50"/>
+        <v>10</v>
+      </c>
+      <c r="C246" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B246">
-        <f t="shared" si="49"/>
-        <v>12</v>
-      </c>
-      <c r="C246" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-12</v>
+        <v>26-10</v>
       </c>
       <c r="L246" s="6"/>
       <c r="M246" s="6"/>
     </row>
     <row r="247" spans="1:13" ht="15">
       <c r="A247">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B247">
+        <f t="shared" si="50"/>
+        <v>11</v>
+      </c>
+      <c r="C247" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B247">
-        <f t="shared" si="49"/>
-        <v>13</v>
-      </c>
-      <c r="C247" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-13</v>
+        <v>26-11</v>
       </c>
       <c r="L247" s="6"/>
       <c r="M247" s="6"/>
     </row>
     <row r="248" spans="1:13" ht="15">
       <c r="A248">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B248">
+        <f t="shared" si="50"/>
+        <v>12</v>
+      </c>
+      <c r="C248" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B248">
-        <f t="shared" si="49"/>
-        <v>14</v>
-      </c>
-      <c r="C248" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-14</v>
+        <v>26-12</v>
       </c>
       <c r="L248" s="6"/>
       <c r="M248" s="6"/>
     </row>
     <row r="249" spans="1:13" ht="15">
       <c r="A249">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B249">
+        <f t="shared" si="50"/>
+        <v>13</v>
+      </c>
+      <c r="C249" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B249">
-        <f t="shared" si="49"/>
-        <v>15</v>
-      </c>
-      <c r="C249" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-15</v>
+        <v>26-13</v>
       </c>
       <c r="L249" s="6"/>
       <c r="M249" s="6"/>
     </row>
     <row r="250" spans="1:13" ht="15">
       <c r="A250">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B250">
+        <f t="shared" si="50"/>
+        <v>14</v>
+      </c>
+      <c r="C250" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B250">
-        <f t="shared" si="49"/>
-        <v>16</v>
-      </c>
-      <c r="C250" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-16</v>
+        <v>26-14</v>
       </c>
       <c r="L250" s="6"/>
       <c r="M250" s="6"/>
     </row>
     <row r="251" spans="1:13" ht="15">
       <c r="A251">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B251">
+        <f t="shared" si="50"/>
+        <v>15</v>
+      </c>
+      <c r="C251" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B251">
-        <f t="shared" si="49"/>
-        <v>17</v>
-      </c>
-      <c r="C251" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-17</v>
+        <v>26-15</v>
       </c>
       <c r="L251" s="6"/>
       <c r="M251" s="6"/>
     </row>
     <row r="252" spans="1:13" ht="15">
       <c r="A252">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B252">
+        <f t="shared" si="50"/>
+        <v>16</v>
+      </c>
+      <c r="C252" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B252">
-        <f t="shared" si="49"/>
-        <v>18</v>
-      </c>
-      <c r="C252" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-18</v>
+        <v>26-16</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
     </row>
     <row r="253" spans="1:13" ht="15">
       <c r="A253">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B253">
+        <f t="shared" si="50"/>
+        <v>17</v>
+      </c>
+      <c r="C253" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B253">
-        <f t="shared" si="49"/>
-        <v>19</v>
-      </c>
-      <c r="C253" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-19</v>
+        <v>26-17</v>
       </c>
       <c r="L253" s="6"/>
       <c r="M253" s="6"/>
     </row>
     <row r="254" spans="1:13" ht="15">
       <c r="A254">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B254">
+        <f t="shared" si="50"/>
+        <v>18</v>
+      </c>
+      <c r="C254" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B254">
-        <f t="shared" si="49"/>
-        <v>20</v>
-      </c>
-      <c r="C254" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-20</v>
+        <v>26-18</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
     </row>
     <row r="255" spans="1:13" ht="15">
       <c r="A255">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B255">
+        <f t="shared" si="50"/>
+        <v>19</v>
+      </c>
+      <c r="C255" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B255">
-        <f t="shared" si="49"/>
-        <v>21</v>
-      </c>
-      <c r="C255" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-21</v>
+        <v>26-19</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
     </row>
     <row r="256" spans="1:13" ht="15">
       <c r="A256">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B256">
+        <f t="shared" si="50"/>
+        <v>20</v>
+      </c>
+      <c r="C256" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B256">
-        <f t="shared" si="49"/>
-        <v>22</v>
-      </c>
-      <c r="C256" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-22</v>
+        <v>26-20</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
     </row>
     <row r="257" spans="1:13" ht="15">
       <c r="A257">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B257">
+        <f t="shared" si="50"/>
+        <v>21</v>
+      </c>
+      <c r="C257" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B257">
-        <f t="shared" si="49"/>
-        <v>23</v>
-      </c>
-      <c r="C257" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-23</v>
+        <v>26-21</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
     </row>
     <row r="258" spans="1:13" ht="15">
       <c r="A258">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B258">
+        <f t="shared" si="50"/>
+        <v>22</v>
+      </c>
+      <c r="C258" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B258">
-        <f t="shared" si="49"/>
-        <v>24</v>
-      </c>
-      <c r="C258" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-24</v>
+        <v>26-22</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
     </row>
     <row r="259" spans="1:13" ht="15">
       <c r="A259">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B259">
+        <f t="shared" si="50"/>
+        <v>23</v>
+      </c>
+      <c r="C259" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B259">
-        <f t="shared" si="49"/>
-        <v>25</v>
-      </c>
-      <c r="C259" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-25</v>
+        <v>26-23</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
     </row>
     <row r="260" spans="1:13" ht="15">
       <c r="A260">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B260">
+        <f t="shared" si="50"/>
+        <v>24</v>
+      </c>
+      <c r="C260" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B260">
-        <f t="shared" si="49"/>
-        <v>26</v>
-      </c>
-      <c r="C260" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-26</v>
+        <v>26-24</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
     </row>
     <row r="261" spans="1:13" ht="15">
       <c r="A261">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B261">
+        <f t="shared" si="50"/>
+        <v>25</v>
+      </c>
+      <c r="C261" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B261">
-        <f t="shared" si="49"/>
-        <v>27</v>
-      </c>
-      <c r="C261" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-27</v>
+        <v>26-25</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
     </row>
     <row r="262" spans="1:13" ht="15">
       <c r="A262">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B262">
+        <f t="shared" si="50"/>
+        <v>26</v>
+      </c>
+      <c r="C262" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B262">
-        <f t="shared" si="49"/>
-        <v>28</v>
-      </c>
-      <c r="C262" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-28</v>
+        <v>26-26</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
     </row>
     <row r="263" spans="1:13" ht="15">
       <c r="A263">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B263">
+        <f t="shared" si="50"/>
+        <v>27</v>
+      </c>
+      <c r="C263" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B263">
-        <f t="shared" si="49"/>
-        <v>29</v>
-      </c>
-      <c r="C263" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-29</v>
+        <v>26-27</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
     </row>
     <row r="264" spans="1:13" ht="15">
       <c r="A264">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B264">
+        <f t="shared" si="50"/>
+        <v>28</v>
+      </c>
+      <c r="C264" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B264">
-        <f t="shared" si="49"/>
-        <v>30</v>
-      </c>
-      <c r="C264" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-30</v>
+        <v>26-28</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
     </row>
     <row r="265" spans="1:13" ht="15">
       <c r="A265">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B265">
+        <f t="shared" si="50"/>
+        <v>29</v>
+      </c>
+      <c r="C265" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B265">
-        <f t="shared" si="49"/>
-        <v>31</v>
-      </c>
-      <c r="C265" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-31</v>
+        <v>26-29</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
     </row>
     <row r="266" spans="1:13" ht="15">
       <c r="A266">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B266">
+        <f t="shared" si="50"/>
+        <v>30</v>
+      </c>
+      <c r="C266" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B266">
-        <f t="shared" si="49"/>
-        <v>32</v>
-      </c>
-      <c r="C266" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-32</v>
+        <v>26-30</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
     </row>
     <row r="267" spans="1:13" ht="15">
       <c r="A267">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B267">
+        <f t="shared" si="50"/>
+        <v>31</v>
+      </c>
+      <c r="C267" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B267">
-        <f t="shared" si="49"/>
-        <v>33</v>
-      </c>
-      <c r="C267" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-33</v>
+        <v>26-31</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
     </row>
     <row r="268" spans="1:13" ht="15">
       <c r="A268">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B268">
+        <f t="shared" si="50"/>
+        <v>32</v>
+      </c>
+      <c r="C268" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B268">
-        <f t="shared" si="49"/>
-        <v>34</v>
-      </c>
-      <c r="C268" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-34</v>
+        <v>26-32</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
     </row>
     <row r="269" spans="1:13" ht="15">
       <c r="A269">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B269">
+        <f t="shared" si="50"/>
+        <v>33</v>
+      </c>
+      <c r="C269" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B269">
-        <f t="shared" si="49"/>
-        <v>35</v>
-      </c>
-      <c r="C269" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-35</v>
+        <v>26-33</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
     </row>
     <row r="270" spans="1:13" ht="15">
       <c r="A270">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B270">
+        <f t="shared" si="50"/>
+        <v>34</v>
+      </c>
+      <c r="C270" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B270">
-        <f t="shared" si="49"/>
-        <v>36</v>
-      </c>
-      <c r="C270" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-36</v>
+        <v>26-34</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
     </row>
     <row r="271" spans="1:13" ht="15">
       <c r="A271">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B271">
+        <f t="shared" si="50"/>
+        <v>35</v>
+      </c>
+      <c r="C271" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B271">
-        <f t="shared" si="49"/>
-        <v>37</v>
-      </c>
-      <c r="C271" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-37</v>
+        <v>26-35</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
     </row>
     <row r="272" spans="1:13" ht="15">
       <c r="A272">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B272">
+        <f t="shared" si="50"/>
+        <v>36</v>
+      </c>
+      <c r="C272" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B272">
-        <f t="shared" si="49"/>
-        <v>38</v>
-      </c>
-      <c r="C272" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-38</v>
+        <v>26-36</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
     </row>
     <row r="273" spans="1:13" ht="15">
       <c r="A273">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B273">
+        <f t="shared" si="50"/>
+        <v>37</v>
+      </c>
+      <c r="C273" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B273">
-        <f t="shared" si="49"/>
-        <v>39</v>
-      </c>
-      <c r="C273" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-39</v>
+        <v>26-37</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
     </row>
     <row r="274" spans="1:13" ht="15">
       <c r="A274">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B274">
+        <f t="shared" si="50"/>
+        <v>38</v>
+      </c>
+      <c r="C274" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B274">
-        <f t="shared" si="49"/>
-        <v>40</v>
-      </c>
-      <c r="C274" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-40</v>
+        <v>26-38</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
     </row>
     <row r="275" spans="1:13" ht="15">
       <c r="A275">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B275">
+        <f t="shared" si="50"/>
+        <v>39</v>
+      </c>
+      <c r="C275" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B275">
-        <f t="shared" si="49"/>
-        <v>41</v>
-      </c>
-      <c r="C275" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-41</v>
+        <v>26-39</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
     </row>
     <row r="276" spans="1:13" ht="15">
       <c r="A276">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B276">
+        <f t="shared" si="50"/>
+        <v>40</v>
+      </c>
+      <c r="C276" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B276">
-        <f t="shared" si="49"/>
-        <v>42</v>
-      </c>
-      <c r="C276" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-42</v>
+        <v>26-40</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
     </row>
     <row r="277" spans="1:13" ht="15">
       <c r="A277">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B277">
+        <f t="shared" si="50"/>
+        <v>41</v>
+      </c>
+      <c r="C277" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B277">
-        <f t="shared" si="49"/>
-        <v>43</v>
-      </c>
-      <c r="C277" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-43</v>
+        <v>26-41</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
     </row>
     <row r="278" spans="1:13" ht="15">
       <c r="A278">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B278">
+        <f t="shared" si="50"/>
+        <v>42</v>
+      </c>
+      <c r="C278" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B278">
-        <f t="shared" si="49"/>
-        <v>44</v>
-      </c>
-      <c r="C278" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-44</v>
+        <v>26-42</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
     </row>
     <row r="279" spans="1:13" ht="15">
       <c r="A279">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B279">
+        <f t="shared" si="50"/>
+        <v>43</v>
+      </c>
+      <c r="C279" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B279">
-        <f t="shared" si="49"/>
-        <v>45</v>
-      </c>
-      <c r="C279" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-45</v>
+        <v>26-43</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
     </row>
     <row r="280" spans="1:13" ht="15">
       <c r="A280">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B280">
+        <f t="shared" si="50"/>
+        <v>44</v>
+      </c>
+      <c r="C280" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B280">
-        <f t="shared" si="49"/>
-        <v>46</v>
-      </c>
-      <c r="C280" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-46</v>
+        <v>26-44</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
     </row>
     <row r="281" spans="1:13" ht="15">
       <c r="A281">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B281">
+        <f t="shared" si="50"/>
+        <v>45</v>
+      </c>
+      <c r="C281" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B281">
-        <f t="shared" si="49"/>
-        <v>47</v>
-      </c>
-      <c r="C281" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-47</v>
+        <v>26-45</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
     </row>
     <row r="282" spans="1:13" ht="15">
       <c r="A282">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B282">
+        <f t="shared" si="50"/>
+        <v>46</v>
+      </c>
+      <c r="C282" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B282">
-        <f t="shared" si="49"/>
-        <v>48</v>
-      </c>
-      <c r="C282" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-48</v>
+        <v>26-46</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
     </row>
     <row r="283" spans="1:13" ht="15">
       <c r="A283">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B283">
+        <f t="shared" si="50"/>
+        <v>47</v>
+      </c>
+      <c r="C283" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B283">
-        <f t="shared" si="49"/>
-        <v>49</v>
-      </c>
-      <c r="C283" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-49</v>
+        <v>26-47</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
     </row>
     <row r="284" spans="1:13" ht="15">
       <c r="A284">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B284">
+        <f t="shared" si="50"/>
+        <v>48</v>
+      </c>
+      <c r="C284" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B284">
-        <f t="shared" si="49"/>
-        <v>50</v>
-      </c>
-      <c r="C284" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-50</v>
+        <v>26-48</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
     </row>
     <row r="285" spans="1:13" ht="15">
       <c r="A285">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B285">
+        <f t="shared" si="50"/>
+        <v>49</v>
+      </c>
+      <c r="C285" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B285">
-        <f t="shared" si="49"/>
-        <v>51</v>
-      </c>
-      <c r="C285" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-51</v>
+        <v>26-49</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
     </row>
     <row r="286" spans="1:13" ht="15">
       <c r="A286">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B286">
+        <f t="shared" si="50"/>
+        <v>50</v>
+      </c>
+      <c r="C286" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B286">
-        <f t="shared" si="49"/>
-        <v>52</v>
-      </c>
-      <c r="C286" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-52</v>
+        <v>26-50</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
     </row>
     <row r="287" spans="1:13" ht="15">
       <c r="A287">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B287">
+        <f t="shared" si="50"/>
+        <v>51</v>
+      </c>
+      <c r="C287" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B287">
-        <f t="shared" si="49"/>
-        <v>53</v>
-      </c>
-      <c r="C287" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-53</v>
+        <v>26-51</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
     </row>
     <row r="288" spans="1:13" ht="15">
       <c r="A288">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B288">
+        <f t="shared" si="50"/>
+        <v>52</v>
+      </c>
+      <c r="C288" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B288">
-        <f t="shared" si="49"/>
-        <v>54</v>
-      </c>
-      <c r="C288" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-54</v>
+        <v>26-52</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
     </row>
     <row r="289" spans="1:13" ht="15">
       <c r="A289">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B289">
+        <f t="shared" si="50"/>
+        <v>53</v>
+      </c>
+      <c r="C289" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B289">
-        <f t="shared" si="49"/>
-        <v>55</v>
-      </c>
-      <c r="C289" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-55</v>
+        <v>26-53</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
     </row>
     <row r="290" spans="1:13" ht="15">
       <c r="A290">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B290">
+        <f t="shared" si="50"/>
+        <v>54</v>
+      </c>
+      <c r="C290" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B290">
-        <f t="shared" si="49"/>
-        <v>56</v>
-      </c>
-      <c r="C290" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-56</v>
+        <v>26-54</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
     </row>
     <row r="291" spans="1:13" ht="15">
       <c r="A291">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B291">
+        <f t="shared" si="50"/>
+        <v>55</v>
+      </c>
+      <c r="C291" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B291">
-        <f t="shared" si="49"/>
-        <v>57</v>
-      </c>
-      <c r="C291" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-57</v>
+        <v>26-55</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
     </row>
     <row r="292" spans="1:13" ht="15">
       <c r="A292">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B292">
+        <f t="shared" si="50"/>
+        <v>56</v>
+      </c>
+      <c r="C292" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B292">
-        <f t="shared" si="49"/>
-        <v>58</v>
-      </c>
-      <c r="C292" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-58</v>
+        <v>26-56</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
     </row>
     <row r="293" spans="1:13" ht="15">
       <c r="A293">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B293">
+        <f t="shared" si="50"/>
+        <v>57</v>
+      </c>
+      <c r="C293" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B293">
-        <f t="shared" si="49"/>
-        <v>59</v>
-      </c>
-      <c r="C293" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-59</v>
+        <v>26-57</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
     </row>
     <row r="294" spans="1:13" ht="15">
       <c r="A294">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B294">
+        <f t="shared" si="50"/>
+        <v>58</v>
+      </c>
+      <c r="C294" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B294">
-        <f t="shared" si="49"/>
-        <v>60</v>
-      </c>
-      <c r="C294" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-60</v>
+        <v>26-58</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
     </row>
     <row r="295" spans="1:13" ht="15">
       <c r="A295">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B295">
+        <f t="shared" si="50"/>
+        <v>59</v>
+      </c>
+      <c r="C295" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B295">
-        <f t="shared" si="49"/>
-        <v>61</v>
-      </c>
-      <c r="C295" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-61</v>
+        <v>26-59</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
     </row>
     <row r="296" spans="1:13" ht="15">
       <c r="A296">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B296">
+        <f t="shared" si="50"/>
+        <v>60</v>
+      </c>
+      <c r="C296" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B296">
-        <f t="shared" si="49"/>
-        <v>62</v>
-      </c>
-      <c r="C296" s="3" t="str">
-        <f t="shared" si="50"/>
-        <v>26-62</v>
+        <v>26-60</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
     </row>
     <row r="297" spans="1:13" ht="15">
       <c r="A297">
+        <f t="shared" si="52"/>
+        <v>26</v>
+      </c>
+      <c r="B297">
+        <f t="shared" si="50"/>
+        <v>61</v>
+      </c>
+      <c r="C297" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26</v>
-      </c>
-      <c r="B297">
-        <f t="shared" ref="B297:B360" si="52">IF(A297=A296,B296+1,1)</f>
-        <v>63</v>
-      </c>
-      <c r="C297" s="3" t="str">
-        <f t="shared" ref="C297:C360" si="53">CONCATENATE(A297,"-",B297)</f>
-        <v>26-63</v>
+        <v>26-61</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
     </row>
     <row r="298" spans="1:13" ht="15">
       <c r="A298">
-        <f t="shared" ref="A298:A361" si="54">A297</f>
+        <f t="shared" si="52"/>
         <v>26</v>
       </c>
       <c r="B298">
-        <f t="shared" si="52"/>
-        <v>64</v>
+        <f t="shared" si="50"/>
+        <v>62</v>
       </c>
       <c r="C298" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-64</v>
+        <f t="shared" si="51"/>
+        <v>26-62</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
     </row>
     <row r="299" spans="1:13" ht="15">
       <c r="A299">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v>26</v>
       </c>
       <c r="B299">
-        <f t="shared" si="52"/>
-        <v>65</v>
+        <f t="shared" ref="B299:B362" si="53">IF(A299=A298,B298+1,1)</f>
+        <v>63</v>
       </c>
       <c r="C299" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-65</v>
+        <f t="shared" ref="C299:C362" si="54">CONCATENATE(A299,"-",B299)</f>
+        <v>26-63</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
     </row>
     <row r="300" spans="1:13" ht="15">
       <c r="A300">
+        <f t="shared" ref="A300:A363" si="55">A299</f>
+        <v>26</v>
+      </c>
+      <c r="B300">
+        <f t="shared" si="53"/>
+        <v>64</v>
+      </c>
+      <c r="C300" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B300">
-        <f t="shared" si="52"/>
-        <v>66</v>
-      </c>
-      <c r="C300" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-66</v>
+        <v>26-64</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
     </row>
     <row r="301" spans="1:13" ht="15">
       <c r="A301">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B301">
+        <f t="shared" si="53"/>
+        <v>65</v>
+      </c>
+      <c r="C301" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B301">
-        <f t="shared" si="52"/>
-        <v>67</v>
-      </c>
-      <c r="C301" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-67</v>
+        <v>26-65</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
     </row>
     <row r="302" spans="1:13" ht="15">
       <c r="A302">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B302">
+        <f t="shared" si="53"/>
+        <v>66</v>
+      </c>
+      <c r="C302" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B302">
-        <f t="shared" si="52"/>
-        <v>68</v>
-      </c>
-      <c r="C302" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-68</v>
+        <v>26-66</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
     </row>
     <row r="303" spans="1:13" ht="15">
       <c r="A303">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B303">
+        <f t="shared" si="53"/>
+        <v>67</v>
+      </c>
+      <c r="C303" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B303">
-        <f t="shared" si="52"/>
-        <v>69</v>
-      </c>
-      <c r="C303" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-69</v>
+        <v>26-67</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
     </row>
     <row r="304" spans="1:13" ht="15">
       <c r="A304">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B304">
+        <f t="shared" si="53"/>
+        <v>68</v>
+      </c>
+      <c r="C304" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B304">
-        <f t="shared" si="52"/>
-        <v>70</v>
-      </c>
-      <c r="C304" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-70</v>
+        <v>26-68</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
     </row>
     <row r="305" spans="1:13" ht="15">
       <c r="A305">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B305">
+        <f t="shared" si="53"/>
+        <v>69</v>
+      </c>
+      <c r="C305" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B305">
-        <f t="shared" si="52"/>
-        <v>71</v>
-      </c>
-      <c r="C305" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-71</v>
+        <v>26-69</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
     </row>
     <row r="306" spans="1:13" ht="15">
       <c r="A306">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B306">
+        <f t="shared" si="53"/>
+        <v>70</v>
+      </c>
+      <c r="C306" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B306">
-        <f t="shared" si="52"/>
-        <v>72</v>
-      </c>
-      <c r="C306" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-72</v>
+        <v>26-70</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
     </row>
     <row r="307" spans="1:13" ht="15">
       <c r="A307">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B307">
+        <f t="shared" si="53"/>
+        <v>71</v>
+      </c>
+      <c r="C307" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B307">
-        <f t="shared" si="52"/>
-        <v>73</v>
-      </c>
-      <c r="C307" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-73</v>
+        <v>26-71</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
     </row>
     <row r="308" spans="1:13" ht="15">
       <c r="A308">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B308">
+        <f t="shared" si="53"/>
+        <v>72</v>
+      </c>
+      <c r="C308" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B308">
-        <f t="shared" si="52"/>
-        <v>74</v>
-      </c>
-      <c r="C308" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-74</v>
+        <v>26-72</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
     </row>
     <row r="309" spans="1:13" ht="15">
       <c r="A309">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B309">
+        <f t="shared" si="53"/>
+        <v>73</v>
+      </c>
+      <c r="C309" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B309">
-        <f t="shared" si="52"/>
-        <v>75</v>
-      </c>
-      <c r="C309" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-75</v>
+        <v>26-73</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
     </row>
     <row r="310" spans="1:13" ht="15">
       <c r="A310">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B310">
+        <f t="shared" si="53"/>
+        <v>74</v>
+      </c>
+      <c r="C310" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B310">
-        <f t="shared" si="52"/>
-        <v>76</v>
-      </c>
-      <c r="C310" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-76</v>
+        <v>26-74</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
     </row>
     <row r="311" spans="1:13" ht="15">
       <c r="A311">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B311">
+        <f t="shared" si="53"/>
+        <v>75</v>
+      </c>
+      <c r="C311" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B311">
-        <f t="shared" si="52"/>
-        <v>77</v>
-      </c>
-      <c r="C311" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-77</v>
+        <v>26-75</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
     </row>
     <row r="312" spans="1:13" ht="15">
       <c r="A312">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B312">
+        <f t="shared" si="53"/>
+        <v>76</v>
+      </c>
+      <c r="C312" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B312">
-        <f t="shared" si="52"/>
-        <v>78</v>
-      </c>
-      <c r="C312" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-78</v>
+        <v>26-76</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
     </row>
     <row r="313" spans="1:13" ht="15">
       <c r="A313">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B313">
+        <f t="shared" si="53"/>
+        <v>77</v>
+      </c>
+      <c r="C313" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B313">
-        <f t="shared" si="52"/>
-        <v>79</v>
-      </c>
-      <c r="C313" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-79</v>
+        <v>26-77</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
     </row>
     <row r="314" spans="1:13" ht="15">
       <c r="A314">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B314">
+        <f t="shared" si="53"/>
+        <v>78</v>
+      </c>
+      <c r="C314" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B314">
-        <f t="shared" si="52"/>
-        <v>80</v>
-      </c>
-      <c r="C314" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-80</v>
+        <v>26-78</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
     </row>
     <row r="315" spans="1:13" ht="15">
       <c r="A315">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B315">
+        <f t="shared" si="53"/>
+        <v>79</v>
+      </c>
+      <c r="C315" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B315">
-        <f t="shared" si="52"/>
-        <v>81</v>
-      </c>
-      <c r="C315" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-81</v>
+        <v>26-79</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
     </row>
     <row r="316" spans="1:13" ht="15">
       <c r="A316">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B316">
+        <f t="shared" si="53"/>
+        <v>80</v>
+      </c>
+      <c r="C316" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B316">
-        <f t="shared" si="52"/>
-        <v>82</v>
-      </c>
-      <c r="C316" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-82</v>
+        <v>26-80</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
     </row>
     <row r="317" spans="1:13" ht="15">
       <c r="A317">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B317">
+        <f t="shared" si="53"/>
+        <v>81</v>
+      </c>
+      <c r="C317" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B317">
-        <f t="shared" si="52"/>
-        <v>83</v>
-      </c>
-      <c r="C317" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-83</v>
+        <v>26-81</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
     </row>
     <row r="318" spans="1:13" ht="15">
       <c r="A318">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B318">
+        <f t="shared" si="53"/>
+        <v>82</v>
+      </c>
+      <c r="C318" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B318">
-        <f t="shared" si="52"/>
-        <v>84</v>
-      </c>
-      <c r="C318" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-84</v>
+        <v>26-82</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
     </row>
     <row r="319" spans="1:13" ht="15">
       <c r="A319">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B319">
+        <f t="shared" si="53"/>
+        <v>83</v>
+      </c>
+      <c r="C319" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B319">
-        <f t="shared" si="52"/>
-        <v>85</v>
-      </c>
-      <c r="C319" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-85</v>
+        <v>26-83</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
     </row>
     <row r="320" spans="1:13" ht="15">
       <c r="A320">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B320">
+        <f t="shared" si="53"/>
+        <v>84</v>
+      </c>
+      <c r="C320" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B320">
-        <f t="shared" si="52"/>
-        <v>86</v>
-      </c>
-      <c r="C320" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-86</v>
+        <v>26-84</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
     </row>
     <row r="321" spans="1:13" ht="15">
       <c r="A321">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B321">
+        <f t="shared" si="53"/>
+        <v>85</v>
+      </c>
+      <c r="C321" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B321">
-        <f t="shared" si="52"/>
-        <v>87</v>
-      </c>
-      <c r="C321" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-87</v>
+        <v>26-85</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
     </row>
     <row r="322" spans="1:13" ht="15">
       <c r="A322">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B322">
+        <f t="shared" si="53"/>
+        <v>86</v>
+      </c>
+      <c r="C322" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B322">
-        <f t="shared" si="52"/>
-        <v>88</v>
-      </c>
-      <c r="C322" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-88</v>
+        <v>26-86</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
     </row>
     <row r="323" spans="1:13" ht="15">
       <c r="A323">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B323">
+        <f t="shared" si="53"/>
+        <v>87</v>
+      </c>
+      <c r="C323" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B323">
-        <f t="shared" si="52"/>
-        <v>89</v>
-      </c>
-      <c r="C323" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-89</v>
+        <v>26-87</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
     </row>
     <row r="324" spans="1:13" ht="15">
       <c r="A324">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B324">
+        <f t="shared" si="53"/>
+        <v>88</v>
+      </c>
+      <c r="C324" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B324">
-        <f t="shared" si="52"/>
-        <v>90</v>
-      </c>
-      <c r="C324" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-90</v>
+        <v>26-88</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
     </row>
     <row r="325" spans="1:13" ht="15">
       <c r="A325">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B325">
+        <f t="shared" si="53"/>
+        <v>89</v>
+      </c>
+      <c r="C325" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B325">
-        <f t="shared" si="52"/>
-        <v>91</v>
-      </c>
-      <c r="C325" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-91</v>
+        <v>26-89</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
     </row>
     <row r="326" spans="1:13" ht="15">
       <c r="A326">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B326">
+        <f t="shared" si="53"/>
+        <v>90</v>
+      </c>
+      <c r="C326" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B326">
-        <f t="shared" si="52"/>
-        <v>92</v>
-      </c>
-      <c r="C326" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-92</v>
+        <v>26-90</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
     </row>
     <row r="327" spans="1:13" ht="15">
       <c r="A327">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B327">
+        <f t="shared" si="53"/>
+        <v>91</v>
+      </c>
+      <c r="C327" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B327">
-        <f t="shared" si="52"/>
-        <v>93</v>
-      </c>
-      <c r="C327" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-93</v>
+        <v>26-91</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
     </row>
     <row r="328" spans="1:13" ht="15">
       <c r="A328">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B328">
+        <f t="shared" si="53"/>
+        <v>92</v>
+      </c>
+      <c r="C328" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B328">
-        <f t="shared" si="52"/>
-        <v>94</v>
-      </c>
-      <c r="C328" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-94</v>
+        <v>26-92</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
     </row>
     <row r="329" spans="1:13" ht="15">
       <c r="A329">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B329">
+        <f t="shared" si="53"/>
+        <v>93</v>
+      </c>
+      <c r="C329" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B329">
-        <f t="shared" si="52"/>
-        <v>95</v>
-      </c>
-      <c r="C329" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-95</v>
+        <v>26-93</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
     </row>
     <row r="330" spans="1:13" ht="15">
       <c r="A330">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B330">
+        <f t="shared" si="53"/>
+        <v>94</v>
+      </c>
+      <c r="C330" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B330">
-        <f t="shared" si="52"/>
-        <v>96</v>
-      </c>
-      <c r="C330" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-96</v>
+        <v>26-94</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
     </row>
     <row r="331" spans="1:13" ht="15">
       <c r="A331">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B331">
+        <f t="shared" si="53"/>
+        <v>95</v>
+      </c>
+      <c r="C331" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B331">
-        <f t="shared" si="52"/>
-        <v>97</v>
-      </c>
-      <c r="C331" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-97</v>
+        <v>26-95</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
     </row>
     <row r="332" spans="1:13" ht="15">
       <c r="A332">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B332">
+        <f t="shared" si="53"/>
+        <v>96</v>
+      </c>
+      <c r="C332" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B332">
-        <f t="shared" si="52"/>
-        <v>98</v>
-      </c>
-      <c r="C332" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-98</v>
+        <v>26-96</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
     </row>
     <row r="333" spans="1:13" ht="15">
       <c r="A333">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B333">
+        <f t="shared" si="53"/>
+        <v>97</v>
+      </c>
+      <c r="C333" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B333">
-        <f t="shared" si="52"/>
-        <v>99</v>
-      </c>
-      <c r="C333" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-99</v>
+        <v>26-97</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
     </row>
     <row r="334" spans="1:13" ht="15">
       <c r="A334">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B334">
+        <f t="shared" si="53"/>
+        <v>98</v>
+      </c>
+      <c r="C334" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B334">
-        <f t="shared" si="52"/>
-        <v>100</v>
-      </c>
-      <c r="C334" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-100</v>
+        <v>26-98</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
     </row>
     <row r="335" spans="1:13" ht="15">
       <c r="A335">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B335">
+        <f t="shared" si="53"/>
+        <v>99</v>
+      </c>
+      <c r="C335" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B335">
-        <f t="shared" si="52"/>
-        <v>101</v>
-      </c>
-      <c r="C335" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-101</v>
+        <v>26-99</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
     </row>
     <row r="336" spans="1:13" ht="15">
       <c r="A336">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B336">
+        <f t="shared" si="53"/>
+        <v>100</v>
+      </c>
+      <c r="C336" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B336">
-        <f t="shared" si="52"/>
-        <v>102</v>
-      </c>
-      <c r="C336" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-102</v>
+        <v>26-100</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
     </row>
     <row r="337" spans="1:13" ht="15">
       <c r="A337">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B337">
+        <f t="shared" si="53"/>
+        <v>101</v>
+      </c>
+      <c r="C337" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B337">
-        <f t="shared" si="52"/>
-        <v>103</v>
-      </c>
-      <c r="C337" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-103</v>
+        <v>26-101</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
     </row>
     <row r="338" spans="1:13" ht="15">
       <c r="A338">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B338">
+        <f t="shared" si="53"/>
+        <v>102</v>
+      </c>
+      <c r="C338" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B338">
-        <f t="shared" si="52"/>
-        <v>104</v>
-      </c>
-      <c r="C338" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-104</v>
+        <v>26-102</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
     </row>
     <row r="339" spans="1:13" ht="15">
       <c r="A339">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B339">
+        <f t="shared" si="53"/>
+        <v>103</v>
+      </c>
+      <c r="C339" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B339">
-        <f t="shared" si="52"/>
-        <v>105</v>
-      </c>
-      <c r="C339" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-105</v>
+        <v>26-103</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
     </row>
     <row r="340" spans="1:13" ht="15">
       <c r="A340">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B340">
+        <f t="shared" si="53"/>
+        <v>104</v>
+      </c>
+      <c r="C340" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B340">
-        <f t="shared" si="52"/>
-        <v>106</v>
-      </c>
-      <c r="C340" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-106</v>
+        <v>26-104</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
     </row>
     <row r="341" spans="1:13" ht="15">
       <c r="A341">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B341">
+        <f t="shared" si="53"/>
+        <v>105</v>
+      </c>
+      <c r="C341" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B341">
-        <f t="shared" si="52"/>
-        <v>107</v>
-      </c>
-      <c r="C341" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-107</v>
+        <v>26-105</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
     </row>
     <row r="342" spans="1:13" ht="15">
       <c r="A342">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B342">
+        <f t="shared" si="53"/>
+        <v>106</v>
+      </c>
+      <c r="C342" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B342">
-        <f t="shared" si="52"/>
-        <v>108</v>
-      </c>
-      <c r="C342" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-108</v>
+        <v>26-106</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
     </row>
     <row r="343" spans="1:13" ht="15">
       <c r="A343">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B343">
+        <f t="shared" si="53"/>
+        <v>107</v>
+      </c>
+      <c r="C343" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B343">
-        <f t="shared" si="52"/>
-        <v>109</v>
-      </c>
-      <c r="C343" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-109</v>
+        <v>26-107</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
     </row>
     <row r="344" spans="1:13" ht="15">
       <c r="A344">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B344">
+        <f t="shared" si="53"/>
+        <v>108</v>
+      </c>
+      <c r="C344" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B344">
-        <f t="shared" si="52"/>
-        <v>110</v>
-      </c>
-      <c r="C344" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-110</v>
+        <v>26-108</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
     </row>
     <row r="345" spans="1:13" ht="15">
       <c r="A345">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B345">
+        <f t="shared" si="53"/>
+        <v>109</v>
+      </c>
+      <c r="C345" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B345">
-        <f t="shared" si="52"/>
-        <v>111</v>
-      </c>
-      <c r="C345" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-111</v>
+        <v>26-109</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
     </row>
     <row r="346" spans="1:13" ht="15">
       <c r="A346">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B346">
+        <f t="shared" si="53"/>
+        <v>110</v>
+      </c>
+      <c r="C346" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B346">
-        <f t="shared" si="52"/>
-        <v>112</v>
-      </c>
-      <c r="C346" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-112</v>
+        <v>26-110</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
     </row>
     <row r="347" spans="1:13" ht="15">
       <c r="A347">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B347">
+        <f t="shared" si="53"/>
+        <v>111</v>
+      </c>
+      <c r="C347" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B347">
-        <f t="shared" si="52"/>
-        <v>113</v>
-      </c>
-      <c r="C347" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-113</v>
+        <v>26-111</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
     </row>
     <row r="348" spans="1:13" ht="15">
       <c r="A348">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B348">
+        <f t="shared" si="53"/>
+        <v>112</v>
+      </c>
+      <c r="C348" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B348">
-        <f t="shared" si="52"/>
-        <v>114</v>
-      </c>
-      <c r="C348" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-114</v>
+        <v>26-112</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
     </row>
     <row r="349" spans="1:13" ht="15">
       <c r="A349">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B349">
+        <f t="shared" si="53"/>
+        <v>113</v>
+      </c>
+      <c r="C349" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B349">
-        <f t="shared" si="52"/>
-        <v>115</v>
-      </c>
-      <c r="C349" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-115</v>
+        <v>26-113</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
     </row>
     <row r="350" spans="1:13" ht="15">
       <c r="A350">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B350">
+        <f t="shared" si="53"/>
+        <v>114</v>
+      </c>
+      <c r="C350" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B350">
-        <f t="shared" si="52"/>
-        <v>116</v>
-      </c>
-      <c r="C350" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-116</v>
+        <v>26-114</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
     </row>
     <row r="351" spans="1:13" ht="15">
       <c r="A351">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B351">
+        <f t="shared" si="53"/>
+        <v>115</v>
+      </c>
+      <c r="C351" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B351">
-        <f t="shared" si="52"/>
-        <v>117</v>
-      </c>
-      <c r="C351" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-117</v>
+        <v>26-115</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
     </row>
     <row r="352" spans="1:13" ht="15">
       <c r="A352">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B352">
+        <f t="shared" si="53"/>
+        <v>116</v>
+      </c>
+      <c r="C352" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B352">
-        <f t="shared" si="52"/>
-        <v>118</v>
-      </c>
-      <c r="C352" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-118</v>
+        <v>26-116</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
     </row>
     <row r="353" spans="1:13" ht="15">
       <c r="A353">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B353">
+        <f t="shared" si="53"/>
+        <v>117</v>
+      </c>
+      <c r="C353" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B353">
-        <f t="shared" si="52"/>
-        <v>119</v>
-      </c>
-      <c r="C353" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-119</v>
+        <v>26-117</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
     </row>
     <row r="354" spans="1:13" ht="15">
       <c r="A354">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B354">
+        <f t="shared" si="53"/>
+        <v>118</v>
+      </c>
+      <c r="C354" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B354">
-        <f t="shared" si="52"/>
-        <v>120</v>
-      </c>
-      <c r="C354" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-120</v>
+        <v>26-118</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
     </row>
     <row r="355" spans="1:13" ht="15">
       <c r="A355">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B355">
+        <f t="shared" si="53"/>
+        <v>119</v>
+      </c>
+      <c r="C355" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B355">
-        <f t="shared" si="52"/>
-        <v>121</v>
-      </c>
-      <c r="C355" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-121</v>
+        <v>26-119</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
     </row>
     <row r="356" spans="1:13" ht="15">
       <c r="A356">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B356">
+        <f t="shared" si="53"/>
+        <v>120</v>
+      </c>
+      <c r="C356" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B356">
-        <f t="shared" si="52"/>
-        <v>122</v>
-      </c>
-      <c r="C356" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-122</v>
+        <v>26-120</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
     </row>
     <row r="357" spans="1:13" ht="15">
       <c r="A357">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B357">
+        <f t="shared" si="53"/>
+        <v>121</v>
+      </c>
+      <c r="C357" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B357">
-        <f t="shared" si="52"/>
-        <v>123</v>
-      </c>
-      <c r="C357" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-123</v>
+        <v>26-121</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
     </row>
     <row r="358" spans="1:13" ht="15">
       <c r="A358">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B358">
+        <f t="shared" si="53"/>
+        <v>122</v>
+      </c>
+      <c r="C358" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B358">
-        <f t="shared" si="52"/>
-        <v>124</v>
-      </c>
-      <c r="C358" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-124</v>
+        <v>26-122</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
     </row>
     <row r="359" spans="1:13" ht="15">
       <c r="A359">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B359">
+        <f t="shared" si="53"/>
+        <v>123</v>
+      </c>
+      <c r="C359" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B359">
-        <f t="shared" si="52"/>
-        <v>125</v>
-      </c>
-      <c r="C359" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-125</v>
+        <v>26-123</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
     </row>
     <row r="360" spans="1:13" ht="15">
       <c r="A360">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B360">
+        <f t="shared" si="53"/>
+        <v>124</v>
+      </c>
+      <c r="C360" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B360">
-        <f t="shared" si="52"/>
-        <v>126</v>
-      </c>
-      <c r="C360" s="3" t="str">
-        <f t="shared" si="53"/>
-        <v>26-126</v>
+        <v>26-124</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
     </row>
     <row r="361" spans="1:13" ht="15">
       <c r="A361">
+        <f t="shared" si="55"/>
+        <v>26</v>
+      </c>
+      <c r="B361">
+        <f t="shared" si="53"/>
+        <v>125</v>
+      </c>
+      <c r="C361" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26</v>
-      </c>
-      <c r="B361">
-        <f t="shared" ref="B361:B382" si="55">IF(A361=A360,B360+1,1)</f>
-        <v>127</v>
-      </c>
-      <c r="C361" s="3" t="str">
-        <f t="shared" ref="C361:C382" si="56">CONCATENATE(A361,"-",B361)</f>
-        <v>26-127</v>
+        <v>26-125</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
     </row>
     <row r="362" spans="1:13" ht="15">
       <c r="A362">
-        <f t="shared" ref="A362:A382" si="57">A361</f>
+        <f t="shared" si="55"/>
         <v>26</v>
       </c>
       <c r="B362">
-        <f t="shared" si="55"/>
-        <v>128</v>
+        <f t="shared" si="53"/>
+        <v>126</v>
       </c>
       <c r="C362" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-128</v>
+        <f t="shared" si="54"/>
+        <v>26-126</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
     </row>
     <row r="363" spans="1:13" ht="15">
       <c r="A363">
-        <f t="shared" si="57"/>
+        <f t="shared" si="55"/>
         <v>26</v>
       </c>
       <c r="B363">
-        <f t="shared" si="55"/>
-        <v>129</v>
+        <f t="shared" ref="B363:B384" si="56">IF(A363=A362,B362+1,1)</f>
+        <v>127</v>
       </c>
       <c r="C363" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-129</v>
+        <f t="shared" ref="C363:C384" si="57">CONCATENATE(A363,"-",B363)</f>
+        <v>26-127</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
     </row>
     <row r="364" spans="1:13" ht="15">
       <c r="A364">
+        <f t="shared" ref="A364:A384" si="58">A363</f>
+        <v>26</v>
+      </c>
+      <c r="B364">
+        <f t="shared" si="56"/>
+        <v>128</v>
+      </c>
+      <c r="C364" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B364">
-        <f t="shared" si="55"/>
-        <v>130</v>
-      </c>
-      <c r="C364" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-130</v>
+        <v>26-128</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
     </row>
     <row r="365" spans="1:13" ht="15">
       <c r="A365">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B365">
+        <f t="shared" si="56"/>
+        <v>129</v>
+      </c>
+      <c r="C365" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B365">
-        <f t="shared" si="55"/>
-        <v>131</v>
-      </c>
-      <c r="C365" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-131</v>
+        <v>26-129</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
     </row>
     <row r="366" spans="1:13" ht="15">
       <c r="A366">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B366">
+        <f t="shared" si="56"/>
+        <v>130</v>
+      </c>
+      <c r="C366" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B366">
-        <f t="shared" si="55"/>
-        <v>132</v>
-      </c>
-      <c r="C366" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-132</v>
+        <v>26-130</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
     </row>
     <row r="367" spans="1:13" ht="15">
       <c r="A367">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B367">
+        <f t="shared" si="56"/>
+        <v>131</v>
+      </c>
+      <c r="C367" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B367">
-        <f t="shared" si="55"/>
-        <v>133</v>
-      </c>
-      <c r="C367" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-133</v>
+        <v>26-131</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
     </row>
     <row r="368" spans="1:13" ht="15">
       <c r="A368">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B368">
+        <f t="shared" si="56"/>
+        <v>132</v>
+      </c>
+      <c r="C368" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B368">
-        <f t="shared" si="55"/>
-        <v>134</v>
-      </c>
-      <c r="C368" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-134</v>
+        <v>26-132</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
     </row>
     <row r="369" spans="1:13" ht="15">
       <c r="A369">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B369">
+        <f t="shared" si="56"/>
+        <v>133</v>
+      </c>
+      <c r="C369" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B369">
-        <f t="shared" si="55"/>
-        <v>135</v>
-      </c>
-      <c r="C369" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-135</v>
+        <v>26-133</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
     </row>
     <row r="370" spans="1:13" ht="15">
       <c r="A370">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B370">
+        <f t="shared" si="56"/>
+        <v>134</v>
+      </c>
+      <c r="C370" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B370">
-        <f t="shared" si="55"/>
-        <v>136</v>
-      </c>
-      <c r="C370" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-136</v>
+        <v>26-134</v>
       </c>
       <c r="L370" s="6"/>
       <c r="M370" s="6"/>
     </row>
     <row r="371" spans="1:13" ht="15">
       <c r="A371">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B371">
+        <f t="shared" si="56"/>
+        <v>135</v>
+      </c>
+      <c r="C371" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B371">
-        <f t="shared" si="55"/>
-        <v>137</v>
-      </c>
-      <c r="C371" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-137</v>
+        <v>26-135</v>
       </c>
       <c r="L371" s="6"/>
       <c r="M371" s="6"/>
     </row>
     <row r="372" spans="1:13" ht="15">
       <c r="A372">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B372">
+        <f t="shared" si="56"/>
+        <v>136</v>
+      </c>
+      <c r="C372" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B372">
-        <f t="shared" si="55"/>
-        <v>138</v>
-      </c>
-      <c r="C372" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-138</v>
+        <v>26-136</v>
       </c>
       <c r="L372" s="6"/>
       <c r="M372" s="6"/>
     </row>
     <row r="373" spans="1:13" ht="15">
       <c r="A373">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B373">
+        <f t="shared" si="56"/>
+        <v>137</v>
+      </c>
+      <c r="C373" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B373">
-        <f t="shared" si="55"/>
-        <v>139</v>
-      </c>
-      <c r="C373" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-139</v>
+        <v>26-137</v>
       </c>
       <c r="L373" s="6"/>
       <c r="M373" s="6"/>
     </row>
     <row r="374" spans="1:13" ht="15">
       <c r="A374">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B374">
+        <f t="shared" si="56"/>
+        <v>138</v>
+      </c>
+      <c r="C374" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B374">
-        <f t="shared" si="55"/>
-        <v>140</v>
-      </c>
-      <c r="C374" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-140</v>
+        <v>26-138</v>
       </c>
       <c r="L374" s="6"/>
       <c r="M374" s="6"/>
     </row>
     <row r="375" spans="1:13" ht="15">
       <c r="A375">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B375">
+        <f t="shared" si="56"/>
+        <v>139</v>
+      </c>
+      <c r="C375" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B375">
-        <f t="shared" si="55"/>
-        <v>141</v>
-      </c>
-      <c r="C375" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-141</v>
+        <v>26-139</v>
       </c>
       <c r="L375" s="6"/>
       <c r="M375" s="6"/>
     </row>
     <row r="376" spans="1:13" ht="15">
       <c r="A376">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B376">
+        <f t="shared" si="56"/>
+        <v>140</v>
+      </c>
+      <c r="C376" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B376">
-        <f t="shared" si="55"/>
-        <v>142</v>
-      </c>
-      <c r="C376" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-142</v>
+        <v>26-140</v>
       </c>
       <c r="L376" s="6"/>
       <c r="M376" s="6"/>
     </row>
     <row r="377" spans="1:13" ht="15">
       <c r="A377">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B377">
+        <f t="shared" si="56"/>
+        <v>141</v>
+      </c>
+      <c r="C377" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B377">
-        <f t="shared" si="55"/>
-        <v>143</v>
-      </c>
-      <c r="C377" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-143</v>
+        <v>26-141</v>
       </c>
       <c r="L377" s="6"/>
       <c r="M377" s="6"/>
     </row>
     <row r="378" spans="1:13" ht="15">
       <c r="A378">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B378">
+        <f t="shared" si="56"/>
+        <v>142</v>
+      </c>
+      <c r="C378" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B378">
-        <f t="shared" si="55"/>
-        <v>144</v>
-      </c>
-      <c r="C378" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-144</v>
+        <v>26-142</v>
       </c>
       <c r="L378" s="6"/>
       <c r="M378" s="6"/>
     </row>
     <row r="379" spans="1:13" ht="15">
       <c r="A379">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B379">
+        <f t="shared" si="56"/>
+        <v>143</v>
+      </c>
+      <c r="C379" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B379">
-        <f t="shared" si="55"/>
-        <v>145</v>
-      </c>
-      <c r="C379" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-145</v>
+        <v>26-143</v>
       </c>
       <c r="L379" s="6"/>
       <c r="M379" s="6"/>
     </row>
     <row r="380" spans="1:13" ht="15">
       <c r="A380">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B380">
+        <f t="shared" si="56"/>
+        <v>144</v>
+      </c>
+      <c r="C380" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B380">
-        <f t="shared" si="55"/>
-        <v>146</v>
-      </c>
-      <c r="C380" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-146</v>
+        <v>26-144</v>
       </c>
       <c r="L380" s="6"/>
       <c r="M380" s="6"/>
     </row>
     <row r="381" spans="1:13" ht="15">
       <c r="A381">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B381">
+        <f t="shared" si="56"/>
+        <v>145</v>
+      </c>
+      <c r="C381" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B381">
-        <f t="shared" si="55"/>
-        <v>147</v>
-      </c>
-      <c r="C381" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-147</v>
+        <v>26-145</v>
       </c>
       <c r="L381" s="6"/>
       <c r="M381" s="6"/>
     </row>
     <row r="382" spans="1:13" ht="15">
       <c r="A382">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B382">
+        <f t="shared" si="56"/>
+        <v>146</v>
+      </c>
+      <c r="C382" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26</v>
-      </c>
-      <c r="B382">
-        <f t="shared" si="55"/>
-        <v>148</v>
-      </c>
-      <c r="C382" s="3" t="str">
-        <f t="shared" si="56"/>
-        <v>26-148</v>
+        <v>26-146</v>
       </c>
       <c r="L382" s="6"/>
       <c r="M382" s="6"/>
     </row>
-    <row r="383" spans="1:13" ht="12.75">
+    <row r="383" spans="1:13" ht="15">
+      <c r="A383">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B383">
+        <f t="shared" si="56"/>
+        <v>147</v>
+      </c>
+      <c r="C383" s="3" t="str">
+        <f t="shared" si="57"/>
+        <v>26-147</v>
+      </c>
       <c r="L383" s="6"/>
       <c r="M383" s="6"/>
     </row>
-    <row r="384" spans="1:13" ht="12.75">
+    <row r="384" spans="1:13" ht="15">
+      <c r="A384">
+        <f t="shared" si="58"/>
+        <v>26</v>
+      </c>
+      <c r="B384">
+        <f t="shared" si="56"/>
+        <v>148</v>
+      </c>
+      <c r="C384" s="3" t="str">
+        <f t="shared" si="57"/>
+        <v>26-148</v>
+      </c>
       <c r="L384" s="6"/>
       <c r="M384" s="6"/>
     </row>
@@ -14504,6 +14603,14 @@
     <row r="1069" spans="12:13" ht="12.75">
       <c r="L1069" s="6"/>
       <c r="M1069" s="6"/>
+    </row>
+    <row r="1070" spans="12:13" ht="12.75">
+      <c r="L1070" s="6"/>
+      <c r="M1070" s="6"/>
+    </row>
+    <row r="1071" spans="12:13" ht="12.75">
+      <c r="L1071" s="6"/>
+      <c r="M1071" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14614,7 +14721,7 @@
       <formula>LEN(TRIM(K214))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K216 K231:K232 K219:K229">
+  <conditionalFormatting sqref="K216 K233:K234 K221:K231">
     <cfRule type="containsBlanks" dxfId="50" priority="37">
       <formula>LEN(TRIM(K216))=0</formula>
     </cfRule>
@@ -14709,12 +14816,12 @@
       <formula>NOT(ISERROR(SEARCH(("fail"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K216 K231:K232 K219:K229">
+  <conditionalFormatting sqref="K216 K233:K234 K221:K231">
     <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K216 K231:K232 K219:K229">
+  <conditionalFormatting sqref="K216 K233:K234 K221:K231">
     <cfRule type="containsText" dxfId="30" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K216))))</formula>
     </cfRule>
@@ -14779,19 +14886,19 @@
       <formula>NOT(ISERROR(SEARCH(("fail"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K230">
+  <conditionalFormatting sqref="K232">
     <cfRule type="containsBlanks" dxfId="17" priority="13">
-      <formula>LEN(TRIM(K230))=0</formula>
+      <formula>LEN(TRIM(K232))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K230">
+  <conditionalFormatting sqref="K232">
     <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K230))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K232))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K230">
+  <conditionalFormatting sqref="K232">
     <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K230))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K232))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
@@ -14809,49 +14916,49 @@
       <formula>NOT(ISERROR(SEARCH(("fail"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K218">
+  <conditionalFormatting sqref="K218:K220">
     <cfRule type="containsBlanks" dxfId="11" priority="7">
       <formula>LEN(TRIM(K218))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K218">
+  <conditionalFormatting sqref="K218:K220">
     <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K218">
+  <conditionalFormatting sqref="K218:K220">
     <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K233">
+  <conditionalFormatting sqref="K235">
     <cfRule type="containsBlanks" dxfId="8" priority="4">
-      <formula>LEN(TRIM(K233))=0</formula>
+      <formula>LEN(TRIM(K235))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K233">
+  <conditionalFormatting sqref="K235">
     <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K233))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K233">
+  <conditionalFormatting sqref="K235">
     <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K233))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K234:K235">
+  <conditionalFormatting sqref="K236:K237">
     <cfRule type="containsBlanks" dxfId="5" priority="1">
-      <formula>LEN(TRIM(K234))=0</formula>
+      <formula>LEN(TRIM(K236))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K234:K235">
+  <conditionalFormatting sqref="K236:K237">
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K234))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K234:K235">
+  <conditionalFormatting sqref="K236:K237">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K234))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated tests for #381
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="303">
   <si>
     <t>Test Number</t>
   </si>
@@ -913,16 +913,19 @@
     <t>Switch to a different instrument. Repeat above</t>
   </si>
   <si>
-    <t>General perspectives</t>
-  </si>
-  <si>
-    <t>Confirm that you can switch perspectives with the function keys</t>
-  </si>
-  <si>
     <t>Create a hidden block. Right click on any group and confirm that you can switch between showing and hiding the block.</t>
   </si>
   <si>
     <t>Create a hidden block. Right click on the block and confirm that you can switch between showing and hiding the block.</t>
+  </si>
+  <si>
+    <t>Confirm that you can switch perspectives with ALT + Shift + underlined key</t>
+  </si>
+  <si>
+    <t>Keyboard shortcuts</t>
+  </si>
+  <si>
+    <t>Confirm that you can access menu items with ALT + underlined key</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1233,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="72">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2239,48 +2242,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2581,8 +2542,8 @@
   <dimension ref="A1:N1071"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I220" sqref="I220"/>
+      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G250" sqref="G250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -8993,7 +8954,7 @@
         <v>15</v>
       </c>
       <c r="I219" s="49" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J219" s="49"/>
       <c r="K219" s="21"/>
@@ -9021,7 +8982,7 @@
         <v>15</v>
       </c>
       <c r="I220" s="49" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J220" s="49"/>
       <c r="K220" s="21"/>
@@ -9487,35 +9448,34 @@
     </row>
     <row r="237" spans="1:13" ht="26.25">
       <c r="A237">
-        <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B237">
         <v>1</v>
       </c>
       <c r="C237" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-1</v>
+        <v>27-1</v>
       </c>
       <c r="D237" s="23"/>
       <c r="E237" s="23"/>
       <c r="F237" s="23"/>
       <c r="G237" s="23"/>
       <c r="H237" s="24" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I237" s="25" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="J237" s="23"/>
       <c r="K237" s="21"/>
       <c r="L237" s="26"/>
       <c r="M237" s="6"/>
     </row>
-    <row r="238" spans="1:13" ht="15">
+    <row r="238" spans="1:13" ht="26.25">
       <c r="A238">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B238">
         <f t="shared" si="50"/>
@@ -9523,15 +9483,27 @@
       </c>
       <c r="C238" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-2</v>
-      </c>
-      <c r="L238" s="6"/>
+        <v>27-2</v>
+      </c>
+      <c r="D238" s="23"/>
+      <c r="E238" s="23"/>
+      <c r="F238" s="23"/>
+      <c r="G238" s="23"/>
+      <c r="H238" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="I238" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="J238" s="23"/>
+      <c r="K238" s="21"/>
+      <c r="L238" s="26"/>
       <c r="M238" s="6"/>
     </row>
     <row r="239" spans="1:13" ht="15">
       <c r="A239">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B239">
         <f t="shared" si="50"/>
@@ -9539,7 +9511,7 @@
       </c>
       <c r="C239" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-3</v>
+        <v>27-3</v>
       </c>
       <c r="L239" s="6"/>
       <c r="M239" s="6"/>
@@ -9547,7 +9519,7 @@
     <row r="240" spans="1:13" ht="15">
       <c r="A240">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B240">
         <f t="shared" si="50"/>
@@ -9555,7 +9527,7 @@
       </c>
       <c r="C240" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-4</v>
+        <v>27-4</v>
       </c>
       <c r="L240" s="6"/>
       <c r="M240" s="6"/>
@@ -9563,7 +9535,7 @@
     <row r="241" spans="1:13" ht="15">
       <c r="A241">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B241">
         <f t="shared" si="50"/>
@@ -9571,7 +9543,7 @@
       </c>
       <c r="C241" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-5</v>
+        <v>27-5</v>
       </c>
       <c r="L241" s="6"/>
       <c r="M241" s="6"/>
@@ -9579,7 +9551,7 @@
     <row r="242" spans="1:13" ht="15">
       <c r="A242">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B242">
         <f t="shared" si="50"/>
@@ -9587,7 +9559,7 @@
       </c>
       <c r="C242" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-6</v>
+        <v>27-6</v>
       </c>
       <c r="L242" s="6"/>
       <c r="M242" s="6"/>
@@ -9595,7 +9567,7 @@
     <row r="243" spans="1:13" ht="15">
       <c r="A243">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B243">
         <f t="shared" si="50"/>
@@ -9603,7 +9575,7 @@
       </c>
       <c r="C243" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-7</v>
+        <v>27-7</v>
       </c>
       <c r="L243" s="6"/>
       <c r="M243" s="6"/>
@@ -9611,7 +9583,7 @@
     <row r="244" spans="1:13" ht="15">
       <c r="A244">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B244">
         <f t="shared" si="50"/>
@@ -9619,7 +9591,7 @@
       </c>
       <c r="C244" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-8</v>
+        <v>27-8</v>
       </c>
       <c r="L244" s="6"/>
       <c r="M244" s="6"/>
@@ -9627,7 +9599,7 @@
     <row r="245" spans="1:13" ht="15">
       <c r="A245">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B245">
         <f t="shared" si="50"/>
@@ -9635,7 +9607,7 @@
       </c>
       <c r="C245" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-9</v>
+        <v>27-9</v>
       </c>
       <c r="L245" s="6"/>
       <c r="M245" s="6"/>
@@ -9643,7 +9615,7 @@
     <row r="246" spans="1:13" ht="15">
       <c r="A246">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B246">
         <f t="shared" si="50"/>
@@ -9651,7 +9623,7 @@
       </c>
       <c r="C246" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-10</v>
+        <v>27-10</v>
       </c>
       <c r="L246" s="6"/>
       <c r="M246" s="6"/>
@@ -9659,7 +9631,7 @@
     <row r="247" spans="1:13" ht="15">
       <c r="A247">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B247">
         <f t="shared" si="50"/>
@@ -9667,7 +9639,7 @@
       </c>
       <c r="C247" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-11</v>
+        <v>27-11</v>
       </c>
       <c r="L247" s="6"/>
       <c r="M247" s="6"/>
@@ -9675,7 +9647,7 @@
     <row r="248" spans="1:13" ht="15">
       <c r="A248">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B248">
         <f t="shared" si="50"/>
@@ -9683,7 +9655,7 @@
       </c>
       <c r="C248" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-12</v>
+        <v>27-12</v>
       </c>
       <c r="L248" s="6"/>
       <c r="M248" s="6"/>
@@ -9691,7 +9663,7 @@
     <row r="249" spans="1:13" ht="15">
       <c r="A249">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B249">
         <f t="shared" si="50"/>
@@ -9699,7 +9671,7 @@
       </c>
       <c r="C249" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-13</v>
+        <v>27-13</v>
       </c>
       <c r="L249" s="6"/>
       <c r="M249" s="6"/>
@@ -9707,7 +9679,7 @@
     <row r="250" spans="1:13" ht="15">
       <c r="A250">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B250">
         <f t="shared" si="50"/>
@@ -9715,7 +9687,7 @@
       </c>
       <c r="C250" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-14</v>
+        <v>27-14</v>
       </c>
       <c r="L250" s="6"/>
       <c r="M250" s="6"/>
@@ -9723,7 +9695,7 @@
     <row r="251" spans="1:13" ht="15">
       <c r="A251">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B251">
         <f t="shared" si="50"/>
@@ -9731,7 +9703,7 @@
       </c>
       <c r="C251" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-15</v>
+        <v>27-15</v>
       </c>
       <c r="L251" s="6"/>
       <c r="M251" s="6"/>
@@ -9739,7 +9711,7 @@
     <row r="252" spans="1:13" ht="15">
       <c r="A252">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B252">
         <f t="shared" si="50"/>
@@ -9747,7 +9719,7 @@
       </c>
       <c r="C252" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-16</v>
+        <v>27-16</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
@@ -9755,7 +9727,7 @@
     <row r="253" spans="1:13" ht="15">
       <c r="A253">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B253">
         <f t="shared" si="50"/>
@@ -9763,7 +9735,7 @@
       </c>
       <c r="C253" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-17</v>
+        <v>27-17</v>
       </c>
       <c r="L253" s="6"/>
       <c r="M253" s="6"/>
@@ -9771,7 +9743,7 @@
     <row r="254" spans="1:13" ht="15">
       <c r="A254">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B254">
         <f t="shared" si="50"/>
@@ -9779,7 +9751,7 @@
       </c>
       <c r="C254" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-18</v>
+        <v>27-18</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
@@ -9787,7 +9759,7 @@
     <row r="255" spans="1:13" ht="15">
       <c r="A255">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B255">
         <f t="shared" si="50"/>
@@ -9795,7 +9767,7 @@
       </c>
       <c r="C255" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-19</v>
+        <v>27-19</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
@@ -9803,7 +9775,7 @@
     <row r="256" spans="1:13" ht="15">
       <c r="A256">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B256">
         <f t="shared" si="50"/>
@@ -9811,7 +9783,7 @@
       </c>
       <c r="C256" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-20</v>
+        <v>27-20</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
@@ -9819,7 +9791,7 @@
     <row r="257" spans="1:13" ht="15">
       <c r="A257">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B257">
         <f t="shared" si="50"/>
@@ -9827,7 +9799,7 @@
       </c>
       <c r="C257" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-21</v>
+        <v>27-21</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
@@ -9835,7 +9807,7 @@
     <row r="258" spans="1:13" ht="15">
       <c r="A258">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B258">
         <f t="shared" si="50"/>
@@ -9843,7 +9815,7 @@
       </c>
       <c r="C258" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-22</v>
+        <v>27-22</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
@@ -9851,7 +9823,7 @@
     <row r="259" spans="1:13" ht="15">
       <c r="A259">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B259">
         <f t="shared" si="50"/>
@@ -9859,7 +9831,7 @@
       </c>
       <c r="C259" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-23</v>
+        <v>27-23</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
@@ -9867,7 +9839,7 @@
     <row r="260" spans="1:13" ht="15">
       <c r="A260">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B260">
         <f t="shared" si="50"/>
@@ -9875,7 +9847,7 @@
       </c>
       <c r="C260" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-24</v>
+        <v>27-24</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
@@ -9883,7 +9855,7 @@
     <row r="261" spans="1:13" ht="15">
       <c r="A261">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B261">
         <f t="shared" si="50"/>
@@ -9891,7 +9863,7 @@
       </c>
       <c r="C261" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-25</v>
+        <v>27-25</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
@@ -9899,7 +9871,7 @@
     <row r="262" spans="1:13" ht="15">
       <c r="A262">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B262">
         <f t="shared" si="50"/>
@@ -9907,7 +9879,7 @@
       </c>
       <c r="C262" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-26</v>
+        <v>27-26</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
@@ -9915,7 +9887,7 @@
     <row r="263" spans="1:13" ht="15">
       <c r="A263">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B263">
         <f t="shared" si="50"/>
@@ -9923,7 +9895,7 @@
       </c>
       <c r="C263" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-27</v>
+        <v>27-27</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
@@ -9931,7 +9903,7 @@
     <row r="264" spans="1:13" ht="15">
       <c r="A264">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B264">
         <f t="shared" si="50"/>
@@ -9939,7 +9911,7 @@
       </c>
       <c r="C264" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-28</v>
+        <v>27-28</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
@@ -9947,7 +9919,7 @@
     <row r="265" spans="1:13" ht="15">
       <c r="A265">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B265">
         <f t="shared" si="50"/>
@@ -9955,7 +9927,7 @@
       </c>
       <c r="C265" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-29</v>
+        <v>27-29</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
@@ -9963,7 +9935,7 @@
     <row r="266" spans="1:13" ht="15">
       <c r="A266">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B266">
         <f t="shared" si="50"/>
@@ -9971,7 +9943,7 @@
       </c>
       <c r="C266" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-30</v>
+        <v>27-30</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
@@ -9979,7 +9951,7 @@
     <row r="267" spans="1:13" ht="15">
       <c r="A267">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B267">
         <f t="shared" si="50"/>
@@ -9987,7 +9959,7 @@
       </c>
       <c r="C267" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-31</v>
+        <v>27-31</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
@@ -9995,7 +9967,7 @@
     <row r="268" spans="1:13" ht="15">
       <c r="A268">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B268">
         <f t="shared" si="50"/>
@@ -10003,7 +9975,7 @@
       </c>
       <c r="C268" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-32</v>
+        <v>27-32</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
@@ -10011,7 +9983,7 @@
     <row r="269" spans="1:13" ht="15">
       <c r="A269">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B269">
         <f t="shared" si="50"/>
@@ -10019,7 +9991,7 @@
       </c>
       <c r="C269" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-33</v>
+        <v>27-33</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
@@ -10027,7 +9999,7 @@
     <row r="270" spans="1:13" ht="15">
       <c r="A270">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B270">
         <f t="shared" si="50"/>
@@ -10035,7 +10007,7 @@
       </c>
       <c r="C270" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-34</v>
+        <v>27-34</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
@@ -10043,7 +10015,7 @@
     <row r="271" spans="1:13" ht="15">
       <c r="A271">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B271">
         <f t="shared" si="50"/>
@@ -10051,7 +10023,7 @@
       </c>
       <c r="C271" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-35</v>
+        <v>27-35</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
@@ -10059,7 +10031,7 @@
     <row r="272" spans="1:13" ht="15">
       <c r="A272">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B272">
         <f t="shared" si="50"/>
@@ -10067,7 +10039,7 @@
       </c>
       <c r="C272" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-36</v>
+        <v>27-36</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
@@ -10075,7 +10047,7 @@
     <row r="273" spans="1:13" ht="15">
       <c r="A273">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B273">
         <f t="shared" si="50"/>
@@ -10083,7 +10055,7 @@
       </c>
       <c r="C273" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-37</v>
+        <v>27-37</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
@@ -10091,7 +10063,7 @@
     <row r="274" spans="1:13" ht="15">
       <c r="A274">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B274">
         <f t="shared" si="50"/>
@@ -10099,7 +10071,7 @@
       </c>
       <c r="C274" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-38</v>
+        <v>27-38</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
@@ -10107,7 +10079,7 @@
     <row r="275" spans="1:13" ht="15">
       <c r="A275">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B275">
         <f t="shared" si="50"/>
@@ -10115,7 +10087,7 @@
       </c>
       <c r="C275" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-39</v>
+        <v>27-39</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
@@ -10123,7 +10095,7 @@
     <row r="276" spans="1:13" ht="15">
       <c r="A276">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B276">
         <f t="shared" si="50"/>
@@ -10131,7 +10103,7 @@
       </c>
       <c r="C276" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-40</v>
+        <v>27-40</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
@@ -10139,7 +10111,7 @@
     <row r="277" spans="1:13" ht="15">
       <c r="A277">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B277">
         <f t="shared" si="50"/>
@@ -10147,7 +10119,7 @@
       </c>
       <c r="C277" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-41</v>
+        <v>27-41</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
@@ -10155,7 +10127,7 @@
     <row r="278" spans="1:13" ht="15">
       <c r="A278">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B278">
         <f t="shared" si="50"/>
@@ -10163,7 +10135,7 @@
       </c>
       <c r="C278" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-42</v>
+        <v>27-42</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
@@ -10171,7 +10143,7 @@
     <row r="279" spans="1:13" ht="15">
       <c r="A279">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B279">
         <f t="shared" si="50"/>
@@ -10179,7 +10151,7 @@
       </c>
       <c r="C279" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-43</v>
+        <v>27-43</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
@@ -10187,7 +10159,7 @@
     <row r="280" spans="1:13" ht="15">
       <c r="A280">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B280">
         <f t="shared" si="50"/>
@@ -10195,7 +10167,7 @@
       </c>
       <c r="C280" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-44</v>
+        <v>27-44</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
@@ -10203,7 +10175,7 @@
     <row r="281" spans="1:13" ht="15">
       <c r="A281">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B281">
         <f t="shared" si="50"/>
@@ -10211,7 +10183,7 @@
       </c>
       <c r="C281" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-45</v>
+        <v>27-45</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
@@ -10219,7 +10191,7 @@
     <row r="282" spans="1:13" ht="15">
       <c r="A282">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B282">
         <f t="shared" si="50"/>
@@ -10227,7 +10199,7 @@
       </c>
       <c r="C282" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-46</v>
+        <v>27-46</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
@@ -10235,7 +10207,7 @@
     <row r="283" spans="1:13" ht="15">
       <c r="A283">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B283">
         <f t="shared" si="50"/>
@@ -10243,7 +10215,7 @@
       </c>
       <c r="C283" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-47</v>
+        <v>27-47</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
@@ -10251,7 +10223,7 @@
     <row r="284" spans="1:13" ht="15">
       <c r="A284">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B284">
         <f t="shared" si="50"/>
@@ -10259,7 +10231,7 @@
       </c>
       <c r="C284" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-48</v>
+        <v>27-48</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
@@ -10267,7 +10239,7 @@
     <row r="285" spans="1:13" ht="15">
       <c r="A285">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B285">
         <f t="shared" si="50"/>
@@ -10275,7 +10247,7 @@
       </c>
       <c r="C285" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-49</v>
+        <v>27-49</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
@@ -10283,7 +10255,7 @@
     <row r="286" spans="1:13" ht="15">
       <c r="A286">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B286">
         <f t="shared" si="50"/>
@@ -10291,7 +10263,7 @@
       </c>
       <c r="C286" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-50</v>
+        <v>27-50</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
@@ -10299,7 +10271,7 @@
     <row r="287" spans="1:13" ht="15">
       <c r="A287">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B287">
         <f t="shared" si="50"/>
@@ -10307,7 +10279,7 @@
       </c>
       <c r="C287" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-51</v>
+        <v>27-51</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
@@ -10315,7 +10287,7 @@
     <row r="288" spans="1:13" ht="15">
       <c r="A288">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B288">
         <f t="shared" si="50"/>
@@ -10323,7 +10295,7 @@
       </c>
       <c r="C288" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-52</v>
+        <v>27-52</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
@@ -10331,7 +10303,7 @@
     <row r="289" spans="1:13" ht="15">
       <c r="A289">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B289">
         <f t="shared" si="50"/>
@@ -10339,7 +10311,7 @@
       </c>
       <c r="C289" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-53</v>
+        <v>27-53</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
@@ -10347,7 +10319,7 @@
     <row r="290" spans="1:13" ht="15">
       <c r="A290">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B290">
         <f t="shared" si="50"/>
@@ -10355,7 +10327,7 @@
       </c>
       <c r="C290" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-54</v>
+        <v>27-54</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
@@ -10363,7 +10335,7 @@
     <row r="291" spans="1:13" ht="15">
       <c r="A291">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B291">
         <f t="shared" si="50"/>
@@ -10371,7 +10343,7 @@
       </c>
       <c r="C291" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-55</v>
+        <v>27-55</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
@@ -10379,7 +10351,7 @@
     <row r="292" spans="1:13" ht="15">
       <c r="A292">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B292">
         <f t="shared" si="50"/>
@@ -10387,7 +10359,7 @@
       </c>
       <c r="C292" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-56</v>
+        <v>27-56</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
@@ -10395,7 +10367,7 @@
     <row r="293" spans="1:13" ht="15">
       <c r="A293">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B293">
         <f t="shared" si="50"/>
@@ -10403,7 +10375,7 @@
       </c>
       <c r="C293" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-57</v>
+        <v>27-57</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
@@ -10411,7 +10383,7 @@
     <row r="294" spans="1:13" ht="15">
       <c r="A294">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B294">
         <f t="shared" si="50"/>
@@ -10419,7 +10391,7 @@
       </c>
       <c r="C294" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-58</v>
+        <v>27-58</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
@@ -10427,7 +10399,7 @@
     <row r="295" spans="1:13" ht="15">
       <c r="A295">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B295">
         <f t="shared" si="50"/>
@@ -10435,7 +10407,7 @@
       </c>
       <c r="C295" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-59</v>
+        <v>27-59</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
@@ -10443,7 +10415,7 @@
     <row r="296" spans="1:13" ht="15">
       <c r="A296">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B296">
         <f t="shared" si="50"/>
@@ -10451,7 +10423,7 @@
       </c>
       <c r="C296" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-60</v>
+        <v>27-60</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
@@ -10459,7 +10431,7 @@
     <row r="297" spans="1:13" ht="15">
       <c r="A297">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B297">
         <f t="shared" si="50"/>
@@ -10467,7 +10439,7 @@
       </c>
       <c r="C297" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-61</v>
+        <v>27-61</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
@@ -10475,7 +10447,7 @@
     <row r="298" spans="1:13" ht="15">
       <c r="A298">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B298">
         <f t="shared" si="50"/>
@@ -10483,7 +10455,7 @@
       </c>
       <c r="C298" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>26-62</v>
+        <v>27-62</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
@@ -10491,7 +10463,7 @@
     <row r="299" spans="1:13" ht="15">
       <c r="A299">
         <f t="shared" si="52"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B299">
         <f t="shared" ref="B299:B362" si="53">IF(A299=A298,B298+1,1)</f>
@@ -10499,7 +10471,7 @@
       </c>
       <c r="C299" s="3" t="str">
         <f t="shared" ref="C299:C362" si="54">CONCATENATE(A299,"-",B299)</f>
-        <v>26-63</v>
+        <v>27-63</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
@@ -10507,7 +10479,7 @@
     <row r="300" spans="1:13" ht="15">
       <c r="A300">
         <f t="shared" ref="A300:A363" si="55">A299</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B300">
         <f t="shared" si="53"/>
@@ -10515,7 +10487,7 @@
       </c>
       <c r="C300" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-64</v>
+        <v>27-64</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
@@ -10523,7 +10495,7 @@
     <row r="301" spans="1:13" ht="15">
       <c r="A301">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B301">
         <f t="shared" si="53"/>
@@ -10531,7 +10503,7 @@
       </c>
       <c r="C301" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-65</v>
+        <v>27-65</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
@@ -10539,7 +10511,7 @@
     <row r="302" spans="1:13" ht="15">
       <c r="A302">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B302">
         <f t="shared" si="53"/>
@@ -10547,7 +10519,7 @@
       </c>
       <c r="C302" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-66</v>
+        <v>27-66</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
@@ -10555,7 +10527,7 @@
     <row r="303" spans="1:13" ht="15">
       <c r="A303">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B303">
         <f t="shared" si="53"/>
@@ -10563,7 +10535,7 @@
       </c>
       <c r="C303" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-67</v>
+        <v>27-67</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
@@ -10571,7 +10543,7 @@
     <row r="304" spans="1:13" ht="15">
       <c r="A304">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B304">
         <f t="shared" si="53"/>
@@ -10579,7 +10551,7 @@
       </c>
       <c r="C304" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-68</v>
+        <v>27-68</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
@@ -10587,7 +10559,7 @@
     <row r="305" spans="1:13" ht="15">
       <c r="A305">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B305">
         <f t="shared" si="53"/>
@@ -10595,7 +10567,7 @@
       </c>
       <c r="C305" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-69</v>
+        <v>27-69</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
@@ -10603,7 +10575,7 @@
     <row r="306" spans="1:13" ht="15">
       <c r="A306">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B306">
         <f t="shared" si="53"/>
@@ -10611,7 +10583,7 @@
       </c>
       <c r="C306" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-70</v>
+        <v>27-70</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
@@ -10619,7 +10591,7 @@
     <row r="307" spans="1:13" ht="15">
       <c r="A307">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B307">
         <f t="shared" si="53"/>
@@ -10627,7 +10599,7 @@
       </c>
       <c r="C307" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-71</v>
+        <v>27-71</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
@@ -10635,7 +10607,7 @@
     <row r="308" spans="1:13" ht="15">
       <c r="A308">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B308">
         <f t="shared" si="53"/>
@@ -10643,7 +10615,7 @@
       </c>
       <c r="C308" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-72</v>
+        <v>27-72</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
@@ -10651,7 +10623,7 @@
     <row r="309" spans="1:13" ht="15">
       <c r="A309">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B309">
         <f t="shared" si="53"/>
@@ -10659,7 +10631,7 @@
       </c>
       <c r="C309" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-73</v>
+        <v>27-73</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
@@ -10667,7 +10639,7 @@
     <row r="310" spans="1:13" ht="15">
       <c r="A310">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B310">
         <f t="shared" si="53"/>
@@ -10675,7 +10647,7 @@
       </c>
       <c r="C310" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-74</v>
+        <v>27-74</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
@@ -10683,7 +10655,7 @@
     <row r="311" spans="1:13" ht="15">
       <c r="A311">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B311">
         <f t="shared" si="53"/>
@@ -10691,7 +10663,7 @@
       </c>
       <c r="C311" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-75</v>
+        <v>27-75</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
@@ -10699,7 +10671,7 @@
     <row r="312" spans="1:13" ht="15">
       <c r="A312">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B312">
         <f t="shared" si="53"/>
@@ -10707,7 +10679,7 @@
       </c>
       <c r="C312" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-76</v>
+        <v>27-76</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
@@ -10715,7 +10687,7 @@
     <row r="313" spans="1:13" ht="15">
       <c r="A313">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B313">
         <f t="shared" si="53"/>
@@ -10723,7 +10695,7 @@
       </c>
       <c r="C313" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-77</v>
+        <v>27-77</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
@@ -10731,7 +10703,7 @@
     <row r="314" spans="1:13" ht="15">
       <c r="A314">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B314">
         <f t="shared" si="53"/>
@@ -10739,7 +10711,7 @@
       </c>
       <c r="C314" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-78</v>
+        <v>27-78</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
@@ -10747,7 +10719,7 @@
     <row r="315" spans="1:13" ht="15">
       <c r="A315">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B315">
         <f t="shared" si="53"/>
@@ -10755,7 +10727,7 @@
       </c>
       <c r="C315" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-79</v>
+        <v>27-79</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
@@ -10763,7 +10735,7 @@
     <row r="316" spans="1:13" ht="15">
       <c r="A316">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B316">
         <f t="shared" si="53"/>
@@ -10771,7 +10743,7 @@
       </c>
       <c r="C316" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-80</v>
+        <v>27-80</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
@@ -10779,7 +10751,7 @@
     <row r="317" spans="1:13" ht="15">
       <c r="A317">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B317">
         <f t="shared" si="53"/>
@@ -10787,7 +10759,7 @@
       </c>
       <c r="C317" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-81</v>
+        <v>27-81</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
@@ -10795,7 +10767,7 @@
     <row r="318" spans="1:13" ht="15">
       <c r="A318">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B318">
         <f t="shared" si="53"/>
@@ -10803,7 +10775,7 @@
       </c>
       <c r="C318" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-82</v>
+        <v>27-82</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
@@ -10811,7 +10783,7 @@
     <row r="319" spans="1:13" ht="15">
       <c r="A319">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B319">
         <f t="shared" si="53"/>
@@ -10819,7 +10791,7 @@
       </c>
       <c r="C319" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-83</v>
+        <v>27-83</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
@@ -10827,7 +10799,7 @@
     <row r="320" spans="1:13" ht="15">
       <c r="A320">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B320">
         <f t="shared" si="53"/>
@@ -10835,7 +10807,7 @@
       </c>
       <c r="C320" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-84</v>
+        <v>27-84</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
@@ -10843,7 +10815,7 @@
     <row r="321" spans="1:13" ht="15">
       <c r="A321">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B321">
         <f t="shared" si="53"/>
@@ -10851,7 +10823,7 @@
       </c>
       <c r="C321" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-85</v>
+        <v>27-85</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
@@ -10859,7 +10831,7 @@
     <row r="322" spans="1:13" ht="15">
       <c r="A322">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B322">
         <f t="shared" si="53"/>
@@ -10867,7 +10839,7 @@
       </c>
       <c r="C322" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-86</v>
+        <v>27-86</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
@@ -10875,7 +10847,7 @@
     <row r="323" spans="1:13" ht="15">
       <c r="A323">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B323">
         <f t="shared" si="53"/>
@@ -10883,7 +10855,7 @@
       </c>
       <c r="C323" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-87</v>
+        <v>27-87</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
@@ -10891,7 +10863,7 @@
     <row r="324" spans="1:13" ht="15">
       <c r="A324">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B324">
         <f t="shared" si="53"/>
@@ -10899,7 +10871,7 @@
       </c>
       <c r="C324" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-88</v>
+        <v>27-88</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
@@ -10907,7 +10879,7 @@
     <row r="325" spans="1:13" ht="15">
       <c r="A325">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B325">
         <f t="shared" si="53"/>
@@ -10915,7 +10887,7 @@
       </c>
       <c r="C325" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-89</v>
+        <v>27-89</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
@@ -10923,7 +10895,7 @@
     <row r="326" spans="1:13" ht="15">
       <c r="A326">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B326">
         <f t="shared" si="53"/>
@@ -10931,7 +10903,7 @@
       </c>
       <c r="C326" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-90</v>
+        <v>27-90</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
@@ -10939,7 +10911,7 @@
     <row r="327" spans="1:13" ht="15">
       <c r="A327">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B327">
         <f t="shared" si="53"/>
@@ -10947,7 +10919,7 @@
       </c>
       <c r="C327" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-91</v>
+        <v>27-91</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
@@ -10955,7 +10927,7 @@
     <row r="328" spans="1:13" ht="15">
       <c r="A328">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B328">
         <f t="shared" si="53"/>
@@ -10963,7 +10935,7 @@
       </c>
       <c r="C328" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-92</v>
+        <v>27-92</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
@@ -10971,7 +10943,7 @@
     <row r="329" spans="1:13" ht="15">
       <c r="A329">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B329">
         <f t="shared" si="53"/>
@@ -10979,7 +10951,7 @@
       </c>
       <c r="C329" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-93</v>
+        <v>27-93</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
@@ -10987,7 +10959,7 @@
     <row r="330" spans="1:13" ht="15">
       <c r="A330">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B330">
         <f t="shared" si="53"/>
@@ -10995,7 +10967,7 @@
       </c>
       <c r="C330" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-94</v>
+        <v>27-94</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
@@ -11003,7 +10975,7 @@
     <row r="331" spans="1:13" ht="15">
       <c r="A331">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B331">
         <f t="shared" si="53"/>
@@ -11011,7 +10983,7 @@
       </c>
       <c r="C331" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-95</v>
+        <v>27-95</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
@@ -11019,7 +10991,7 @@
     <row r="332" spans="1:13" ht="15">
       <c r="A332">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B332">
         <f t="shared" si="53"/>
@@ -11027,7 +10999,7 @@
       </c>
       <c r="C332" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-96</v>
+        <v>27-96</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
@@ -11035,7 +11007,7 @@
     <row r="333" spans="1:13" ht="15">
       <c r="A333">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B333">
         <f t="shared" si="53"/>
@@ -11043,7 +11015,7 @@
       </c>
       <c r="C333" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-97</v>
+        <v>27-97</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
@@ -11051,7 +11023,7 @@
     <row r="334" spans="1:13" ht="15">
       <c r="A334">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B334">
         <f t="shared" si="53"/>
@@ -11059,7 +11031,7 @@
       </c>
       <c r="C334" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-98</v>
+        <v>27-98</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
@@ -11067,7 +11039,7 @@
     <row r="335" spans="1:13" ht="15">
       <c r="A335">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B335">
         <f t="shared" si="53"/>
@@ -11075,7 +11047,7 @@
       </c>
       <c r="C335" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-99</v>
+        <v>27-99</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
@@ -11083,7 +11055,7 @@
     <row r="336" spans="1:13" ht="15">
       <c r="A336">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B336">
         <f t="shared" si="53"/>
@@ -11091,7 +11063,7 @@
       </c>
       <c r="C336" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-100</v>
+        <v>27-100</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
@@ -11099,7 +11071,7 @@
     <row r="337" spans="1:13" ht="15">
       <c r="A337">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B337">
         <f t="shared" si="53"/>
@@ -11107,7 +11079,7 @@
       </c>
       <c r="C337" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-101</v>
+        <v>27-101</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
@@ -11115,7 +11087,7 @@
     <row r="338" spans="1:13" ht="15">
       <c r="A338">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B338">
         <f t="shared" si="53"/>
@@ -11123,7 +11095,7 @@
       </c>
       <c r="C338" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-102</v>
+        <v>27-102</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
@@ -11131,7 +11103,7 @@
     <row r="339" spans="1:13" ht="15">
       <c r="A339">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B339">
         <f t="shared" si="53"/>
@@ -11139,7 +11111,7 @@
       </c>
       <c r="C339" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-103</v>
+        <v>27-103</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
@@ -11147,7 +11119,7 @@
     <row r="340" spans="1:13" ht="15">
       <c r="A340">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B340">
         <f t="shared" si="53"/>
@@ -11155,7 +11127,7 @@
       </c>
       <c r="C340" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-104</v>
+        <v>27-104</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
@@ -11163,7 +11135,7 @@
     <row r="341" spans="1:13" ht="15">
       <c r="A341">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B341">
         <f t="shared" si="53"/>
@@ -11171,7 +11143,7 @@
       </c>
       <c r="C341" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-105</v>
+        <v>27-105</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
@@ -11179,7 +11151,7 @@
     <row r="342" spans="1:13" ht="15">
       <c r="A342">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B342">
         <f t="shared" si="53"/>
@@ -11187,7 +11159,7 @@
       </c>
       <c r="C342" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-106</v>
+        <v>27-106</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
@@ -11195,7 +11167,7 @@
     <row r="343" spans="1:13" ht="15">
       <c r="A343">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B343">
         <f t="shared" si="53"/>
@@ -11203,7 +11175,7 @@
       </c>
       <c r="C343" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-107</v>
+        <v>27-107</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
@@ -11211,7 +11183,7 @@
     <row r="344" spans="1:13" ht="15">
       <c r="A344">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B344">
         <f t="shared" si="53"/>
@@ -11219,7 +11191,7 @@
       </c>
       <c r="C344" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-108</v>
+        <v>27-108</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
@@ -11227,7 +11199,7 @@
     <row r="345" spans="1:13" ht="15">
       <c r="A345">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B345">
         <f t="shared" si="53"/>
@@ -11235,7 +11207,7 @@
       </c>
       <c r="C345" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-109</v>
+        <v>27-109</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
@@ -11243,7 +11215,7 @@
     <row r="346" spans="1:13" ht="15">
       <c r="A346">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B346">
         <f t="shared" si="53"/>
@@ -11251,7 +11223,7 @@
       </c>
       <c r="C346" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-110</v>
+        <v>27-110</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
@@ -11259,7 +11231,7 @@
     <row r="347" spans="1:13" ht="15">
       <c r="A347">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B347">
         <f t="shared" si="53"/>
@@ -11267,7 +11239,7 @@
       </c>
       <c r="C347" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-111</v>
+        <v>27-111</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
@@ -11275,7 +11247,7 @@
     <row r="348" spans="1:13" ht="15">
       <c r="A348">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B348">
         <f t="shared" si="53"/>
@@ -11283,7 +11255,7 @@
       </c>
       <c r="C348" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-112</v>
+        <v>27-112</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
@@ -11291,7 +11263,7 @@
     <row r="349" spans="1:13" ht="15">
       <c r="A349">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B349">
         <f t="shared" si="53"/>
@@ -11299,7 +11271,7 @@
       </c>
       <c r="C349" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-113</v>
+        <v>27-113</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
@@ -11307,7 +11279,7 @@
     <row r="350" spans="1:13" ht="15">
       <c r="A350">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B350">
         <f t="shared" si="53"/>
@@ -11315,7 +11287,7 @@
       </c>
       <c r="C350" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-114</v>
+        <v>27-114</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
@@ -11323,7 +11295,7 @@
     <row r="351" spans="1:13" ht="15">
       <c r="A351">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B351">
         <f t="shared" si="53"/>
@@ -11331,7 +11303,7 @@
       </c>
       <c r="C351" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-115</v>
+        <v>27-115</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
@@ -11339,7 +11311,7 @@
     <row r="352" spans="1:13" ht="15">
       <c r="A352">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B352">
         <f t="shared" si="53"/>
@@ -11347,7 +11319,7 @@
       </c>
       <c r="C352" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-116</v>
+        <v>27-116</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
@@ -11355,7 +11327,7 @@
     <row r="353" spans="1:13" ht="15">
       <c r="A353">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B353">
         <f t="shared" si="53"/>
@@ -11363,7 +11335,7 @@
       </c>
       <c r="C353" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-117</v>
+        <v>27-117</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
@@ -11371,7 +11343,7 @@
     <row r="354" spans="1:13" ht="15">
       <c r="A354">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B354">
         <f t="shared" si="53"/>
@@ -11379,7 +11351,7 @@
       </c>
       <c r="C354" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-118</v>
+        <v>27-118</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
@@ -11387,7 +11359,7 @@
     <row r="355" spans="1:13" ht="15">
       <c r="A355">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B355">
         <f t="shared" si="53"/>
@@ -11395,7 +11367,7 @@
       </c>
       <c r="C355" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-119</v>
+        <v>27-119</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
@@ -11403,7 +11375,7 @@
     <row r="356" spans="1:13" ht="15">
       <c r="A356">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B356">
         <f t="shared" si="53"/>
@@ -11411,7 +11383,7 @@
       </c>
       <c r="C356" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-120</v>
+        <v>27-120</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
@@ -11419,7 +11391,7 @@
     <row r="357" spans="1:13" ht="15">
       <c r="A357">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B357">
         <f t="shared" si="53"/>
@@ -11427,7 +11399,7 @@
       </c>
       <c r="C357" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-121</v>
+        <v>27-121</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
@@ -11435,7 +11407,7 @@
     <row r="358" spans="1:13" ht="15">
       <c r="A358">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B358">
         <f t="shared" si="53"/>
@@ -11443,7 +11415,7 @@
       </c>
       <c r="C358" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-122</v>
+        <v>27-122</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
@@ -11451,7 +11423,7 @@
     <row r="359" spans="1:13" ht="15">
       <c r="A359">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B359">
         <f t="shared" si="53"/>
@@ -11459,7 +11431,7 @@
       </c>
       <c r="C359" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-123</v>
+        <v>27-123</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
@@ -11467,7 +11439,7 @@
     <row r="360" spans="1:13" ht="15">
       <c r="A360">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B360">
         <f t="shared" si="53"/>
@@ -11475,7 +11447,7 @@
       </c>
       <c r="C360" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-124</v>
+        <v>27-124</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
@@ -11483,7 +11455,7 @@
     <row r="361" spans="1:13" ht="15">
       <c r="A361">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B361">
         <f t="shared" si="53"/>
@@ -11491,7 +11463,7 @@
       </c>
       <c r="C361" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-125</v>
+        <v>27-125</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
@@ -11499,7 +11471,7 @@
     <row r="362" spans="1:13" ht="15">
       <c r="A362">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B362">
         <f t="shared" si="53"/>
@@ -11507,7 +11479,7 @@
       </c>
       <c r="C362" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>26-126</v>
+        <v>27-126</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
@@ -11515,7 +11487,7 @@
     <row r="363" spans="1:13" ht="15">
       <c r="A363">
         <f t="shared" si="55"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B363">
         <f t="shared" ref="B363:B384" si="56">IF(A363=A362,B362+1,1)</f>
@@ -11523,7 +11495,7 @@
       </c>
       <c r="C363" s="3" t="str">
         <f t="shared" ref="C363:C384" si="57">CONCATENATE(A363,"-",B363)</f>
-        <v>26-127</v>
+        <v>27-127</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
@@ -11531,7 +11503,7 @@
     <row r="364" spans="1:13" ht="15">
       <c r="A364">
         <f t="shared" ref="A364:A384" si="58">A363</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B364">
         <f t="shared" si="56"/>
@@ -11539,7 +11511,7 @@
       </c>
       <c r="C364" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-128</v>
+        <v>27-128</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
@@ -11547,7 +11519,7 @@
     <row r="365" spans="1:13" ht="15">
       <c r="A365">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B365">
         <f t="shared" si="56"/>
@@ -11555,7 +11527,7 @@
       </c>
       <c r="C365" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-129</v>
+        <v>27-129</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
@@ -11563,7 +11535,7 @@
     <row r="366" spans="1:13" ht="15">
       <c r="A366">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B366">
         <f t="shared" si="56"/>
@@ -11571,7 +11543,7 @@
       </c>
       <c r="C366" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-130</v>
+        <v>27-130</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
@@ -11579,7 +11551,7 @@
     <row r="367" spans="1:13" ht="15">
       <c r="A367">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B367">
         <f t="shared" si="56"/>
@@ -11587,7 +11559,7 @@
       </c>
       <c r="C367" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-131</v>
+        <v>27-131</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
@@ -11595,7 +11567,7 @@
     <row r="368" spans="1:13" ht="15">
       <c r="A368">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B368">
         <f t="shared" si="56"/>
@@ -11603,7 +11575,7 @@
       </c>
       <c r="C368" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-132</v>
+        <v>27-132</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
@@ -11611,7 +11583,7 @@
     <row r="369" spans="1:13" ht="15">
       <c r="A369">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B369">
         <f t="shared" si="56"/>
@@ -11619,7 +11591,7 @@
       </c>
       <c r="C369" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-133</v>
+        <v>27-133</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
@@ -11627,7 +11599,7 @@
     <row r="370" spans="1:13" ht="15">
       <c r="A370">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B370">
         <f t="shared" si="56"/>
@@ -11635,7 +11607,7 @@
       </c>
       <c r="C370" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-134</v>
+        <v>27-134</v>
       </c>
       <c r="L370" s="6"/>
       <c r="M370" s="6"/>
@@ -11643,7 +11615,7 @@
     <row r="371" spans="1:13" ht="15">
       <c r="A371">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B371">
         <f t="shared" si="56"/>
@@ -11651,7 +11623,7 @@
       </c>
       <c r="C371" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-135</v>
+        <v>27-135</v>
       </c>
       <c r="L371" s="6"/>
       <c r="M371" s="6"/>
@@ -11659,7 +11631,7 @@
     <row r="372" spans="1:13" ht="15">
       <c r="A372">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B372">
         <f t="shared" si="56"/>
@@ -11667,7 +11639,7 @@
       </c>
       <c r="C372" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-136</v>
+        <v>27-136</v>
       </c>
       <c r="L372" s="6"/>
       <c r="M372" s="6"/>
@@ -11675,7 +11647,7 @@
     <row r="373" spans="1:13" ht="15">
       <c r="A373">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B373">
         <f t="shared" si="56"/>
@@ -11683,7 +11655,7 @@
       </c>
       <c r="C373" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-137</v>
+        <v>27-137</v>
       </c>
       <c r="L373" s="6"/>
       <c r="M373" s="6"/>
@@ -11691,7 +11663,7 @@
     <row r="374" spans="1:13" ht="15">
       <c r="A374">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B374">
         <f t="shared" si="56"/>
@@ -11699,7 +11671,7 @@
       </c>
       <c r="C374" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-138</v>
+        <v>27-138</v>
       </c>
       <c r="L374" s="6"/>
       <c r="M374" s="6"/>
@@ -11707,7 +11679,7 @@
     <row r="375" spans="1:13" ht="15">
       <c r="A375">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B375">
         <f t="shared" si="56"/>
@@ -11715,7 +11687,7 @@
       </c>
       <c r="C375" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-139</v>
+        <v>27-139</v>
       </c>
       <c r="L375" s="6"/>
       <c r="M375" s="6"/>
@@ -11723,7 +11695,7 @@
     <row r="376" spans="1:13" ht="15">
       <c r="A376">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B376">
         <f t="shared" si="56"/>
@@ -11731,7 +11703,7 @@
       </c>
       <c r="C376" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-140</v>
+        <v>27-140</v>
       </c>
       <c r="L376" s="6"/>
       <c r="M376" s="6"/>
@@ -11739,7 +11711,7 @@
     <row r="377" spans="1:13" ht="15">
       <c r="A377">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B377">
         <f t="shared" si="56"/>
@@ -11747,7 +11719,7 @@
       </c>
       <c r="C377" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-141</v>
+        <v>27-141</v>
       </c>
       <c r="L377" s="6"/>
       <c r="M377" s="6"/>
@@ -11755,7 +11727,7 @@
     <row r="378" spans="1:13" ht="15">
       <c r="A378">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B378">
         <f t="shared" si="56"/>
@@ -11763,7 +11735,7 @@
       </c>
       <c r="C378" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-142</v>
+        <v>27-142</v>
       </c>
       <c r="L378" s="6"/>
       <c r="M378" s="6"/>
@@ -11771,7 +11743,7 @@
     <row r="379" spans="1:13" ht="15">
       <c r="A379">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B379">
         <f t="shared" si="56"/>
@@ -11779,7 +11751,7 @@
       </c>
       <c r="C379" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-143</v>
+        <v>27-143</v>
       </c>
       <c r="L379" s="6"/>
       <c r="M379" s="6"/>
@@ -11787,7 +11759,7 @@
     <row r="380" spans="1:13" ht="15">
       <c r="A380">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B380">
         <f t="shared" si="56"/>
@@ -11795,7 +11767,7 @@
       </c>
       <c r="C380" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-144</v>
+        <v>27-144</v>
       </c>
       <c r="L380" s="6"/>
       <c r="M380" s="6"/>
@@ -11803,7 +11775,7 @@
     <row r="381" spans="1:13" ht="15">
       <c r="A381">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B381">
         <f t="shared" si="56"/>
@@ -11811,7 +11783,7 @@
       </c>
       <c r="C381" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-145</v>
+        <v>27-145</v>
       </c>
       <c r="L381" s="6"/>
       <c r="M381" s="6"/>
@@ -11819,7 +11791,7 @@
     <row r="382" spans="1:13" ht="15">
       <c r="A382">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B382">
         <f t="shared" si="56"/>
@@ -11827,7 +11799,7 @@
       </c>
       <c r="C382" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-146</v>
+        <v>27-146</v>
       </c>
       <c r="L382" s="6"/>
       <c r="M382" s="6"/>
@@ -11835,7 +11807,7 @@
     <row r="383" spans="1:13" ht="15">
       <c r="A383">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B383">
         <f t="shared" si="56"/>
@@ -11843,7 +11815,7 @@
       </c>
       <c r="C383" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-147</v>
+        <v>27-147</v>
       </c>
       <c r="L383" s="6"/>
       <c r="M383" s="6"/>
@@ -11851,7 +11823,7 @@
     <row r="384" spans="1:13" ht="15">
       <c r="A384">
         <f t="shared" si="58"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B384">
         <f t="shared" si="56"/>
@@ -11859,7 +11831,7 @@
       </c>
       <c r="C384" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>26-148</v>
+        <v>27-148</v>
       </c>
       <c r="L384" s="6"/>
       <c r="M384" s="6"/>
@@ -14946,17 +14918,17 @@
       <formula>NOT(ISERROR(SEARCH(("fail"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K236:K237">
+  <conditionalFormatting sqref="K236:K238">
     <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(K236))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K236:K237">
+  <conditionalFormatting sqref="K236:K238">
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K236:K237">
+  <conditionalFormatting sqref="K236:K238">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K236))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
added system test for ticket 1810
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="307">
   <si>
     <t>Test Number</t>
   </si>
@@ -926,6 +926,18 @@
   </si>
   <si>
     <t>Confirm that you can access menu items with ALT + underlined key</t>
+  </si>
+  <si>
+    <t>Device Screens</t>
+  </si>
+  <si>
+    <t>Confirm that you can add/edit/delete Device Screens</t>
+  </si>
+  <si>
+    <t>Confirm that device screens can not be saved if one or more items is not pointing at a target OPI.</t>
+  </si>
+  <si>
+    <t>If target is blank: Error message is shown naming the offending device screen &amp; ok button is disabled</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1229,11 +1241,28 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
+  <dxfs count="81">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1253,6 +1282,118 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
         </patternFill>
       </fill>
       <border>
@@ -2542,8 +2683,8 @@
   <dimension ref="A1:N1071"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G250" sqref="G250"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J232" sqref="J232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -9474,7 +9615,7 @@
     </row>
     <row r="238" spans="1:13" ht="26.25">
       <c r="A238">
-        <f t="shared" si="52"/>
+        <f>A237</f>
         <v>27</v>
       </c>
       <c r="B238">
@@ -9500,50 +9641,75 @@
       <c r="L238" s="26"/>
       <c r="M238" s="6"/>
     </row>
-    <row r="239" spans="1:13" ht="15">
+    <row r="239" spans="1:13" ht="26.25">
       <c r="A239">
-        <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B239">
         <f t="shared" si="50"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C239" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-3</v>
-      </c>
-      <c r="L239" s="6"/>
+        <v>28-1</v>
+      </c>
+      <c r="D239" s="23"/>
+      <c r="E239" s="23"/>
+      <c r="F239" s="23"/>
+      <c r="G239" s="23"/>
+      <c r="H239" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="I239" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="J239" s="23"/>
+      <c r="K239" s="21"/>
+      <c r="L239" s="26"/>
       <c r="M239" s="6"/>
     </row>
-    <row r="240" spans="1:13" ht="15">
+    <row r="240" spans="1:13" ht="26.25">
       <c r="A240">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B240">
         <f t="shared" si="50"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C240" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-4</v>
-      </c>
-      <c r="L240" s="6"/>
+        <v>28-2</v>
+      </c>
+      <c r="D240" s="23"/>
+      <c r="E240" s="23"/>
+      <c r="F240" s="23"/>
+      <c r="G240" s="23"/>
+      <c r="H240" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="I240" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="J240" s="53" t="s">
+        <v>306</v>
+      </c>
+      <c r="K240" s="21"/>
+      <c r="L240" s="26"/>
       <c r="M240" s="6"/>
     </row>
     <row r="241" spans="1:13" ht="15">
       <c r="A241">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B241">
         <f t="shared" si="50"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C241" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-5</v>
+        <v>28-3</v>
       </c>
       <c r="L241" s="6"/>
       <c r="M241" s="6"/>
@@ -9551,15 +9717,15 @@
     <row r="242" spans="1:13" ht="15">
       <c r="A242">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B242">
         <f t="shared" si="50"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C242" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-6</v>
+        <v>28-4</v>
       </c>
       <c r="L242" s="6"/>
       <c r="M242" s="6"/>
@@ -9567,15 +9733,15 @@
     <row r="243" spans="1:13" ht="15">
       <c r="A243">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B243">
         <f t="shared" si="50"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C243" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-7</v>
+        <v>28-5</v>
       </c>
       <c r="L243" s="6"/>
       <c r="M243" s="6"/>
@@ -9583,15 +9749,15 @@
     <row r="244" spans="1:13" ht="15">
       <c r="A244">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B244">
         <f t="shared" si="50"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C244" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-8</v>
+        <v>28-6</v>
       </c>
       <c r="L244" s="6"/>
       <c r="M244" s="6"/>
@@ -9599,15 +9765,15 @@
     <row r="245" spans="1:13" ht="15">
       <c r="A245">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B245">
         <f t="shared" si="50"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C245" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-9</v>
+        <v>28-7</v>
       </c>
       <c r="L245" s="6"/>
       <c r="M245" s="6"/>
@@ -9615,15 +9781,15 @@
     <row r="246" spans="1:13" ht="15">
       <c r="A246">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B246">
         <f t="shared" si="50"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C246" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-10</v>
+        <v>28-8</v>
       </c>
       <c r="L246" s="6"/>
       <c r="M246" s="6"/>
@@ -9631,15 +9797,15 @@
     <row r="247" spans="1:13" ht="15">
       <c r="A247">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B247">
         <f t="shared" si="50"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C247" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-11</v>
+        <v>28-9</v>
       </c>
       <c r="L247" s="6"/>
       <c r="M247" s="6"/>
@@ -9647,15 +9813,15 @@
     <row r="248" spans="1:13" ht="15">
       <c r="A248">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B248">
         <f t="shared" si="50"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C248" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-12</v>
+        <v>28-10</v>
       </c>
       <c r="L248" s="6"/>
       <c r="M248" s="6"/>
@@ -9663,15 +9829,15 @@
     <row r="249" spans="1:13" ht="15">
       <c r="A249">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B249">
         <f t="shared" si="50"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C249" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-13</v>
+        <v>28-11</v>
       </c>
       <c r="L249" s="6"/>
       <c r="M249" s="6"/>
@@ -9679,15 +9845,15 @@
     <row r="250" spans="1:13" ht="15">
       <c r="A250">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B250">
         <f t="shared" si="50"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C250" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-14</v>
+        <v>28-12</v>
       </c>
       <c r="L250" s="6"/>
       <c r="M250" s="6"/>
@@ -9695,15 +9861,15 @@
     <row r="251" spans="1:13" ht="15">
       <c r="A251">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B251">
         <f t="shared" si="50"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C251" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-15</v>
+        <v>28-13</v>
       </c>
       <c r="L251" s="6"/>
       <c r="M251" s="6"/>
@@ -9711,15 +9877,15 @@
     <row r="252" spans="1:13" ht="15">
       <c r="A252">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B252">
         <f t="shared" si="50"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C252" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-16</v>
+        <v>28-14</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
@@ -9727,15 +9893,15 @@
     <row r="253" spans="1:13" ht="15">
       <c r="A253">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B253">
         <f t="shared" si="50"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C253" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-17</v>
+        <v>28-15</v>
       </c>
       <c r="L253" s="6"/>
       <c r="M253" s="6"/>
@@ -9743,15 +9909,15 @@
     <row r="254" spans="1:13" ht="15">
       <c r="A254">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B254">
         <f t="shared" si="50"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C254" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-18</v>
+        <v>28-16</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
@@ -9759,15 +9925,15 @@
     <row r="255" spans="1:13" ht="15">
       <c r="A255">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B255">
         <f t="shared" si="50"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C255" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-19</v>
+        <v>28-17</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
@@ -9775,15 +9941,15 @@
     <row r="256" spans="1:13" ht="15">
       <c r="A256">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B256">
         <f t="shared" si="50"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C256" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-20</v>
+        <v>28-18</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
@@ -9791,15 +9957,15 @@
     <row r="257" spans="1:13" ht="15">
       <c r="A257">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B257">
         <f t="shared" si="50"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C257" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-21</v>
+        <v>28-19</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
@@ -9807,15 +9973,15 @@
     <row r="258" spans="1:13" ht="15">
       <c r="A258">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B258">
         <f t="shared" si="50"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C258" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-22</v>
+        <v>28-20</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
@@ -9823,15 +9989,15 @@
     <row r="259" spans="1:13" ht="15">
       <c r="A259">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B259">
         <f t="shared" si="50"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C259" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-23</v>
+        <v>28-21</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
@@ -9839,15 +10005,15 @@
     <row r="260" spans="1:13" ht="15">
       <c r="A260">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B260">
         <f t="shared" si="50"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C260" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-24</v>
+        <v>28-22</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
@@ -9855,15 +10021,15 @@
     <row r="261" spans="1:13" ht="15">
       <c r="A261">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B261">
         <f t="shared" si="50"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C261" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-25</v>
+        <v>28-23</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
@@ -9871,15 +10037,15 @@
     <row r="262" spans="1:13" ht="15">
       <c r="A262">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B262">
         <f t="shared" si="50"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C262" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-26</v>
+        <v>28-24</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
@@ -9887,15 +10053,15 @@
     <row r="263" spans="1:13" ht="15">
       <c r="A263">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B263">
         <f t="shared" si="50"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C263" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-27</v>
+        <v>28-25</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
@@ -9903,15 +10069,15 @@
     <row r="264" spans="1:13" ht="15">
       <c r="A264">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B264">
         <f t="shared" si="50"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C264" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-28</v>
+        <v>28-26</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
@@ -9919,15 +10085,15 @@
     <row r="265" spans="1:13" ht="15">
       <c r="A265">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B265">
         <f t="shared" si="50"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C265" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-29</v>
+        <v>28-27</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
@@ -9935,15 +10101,15 @@
     <row r="266" spans="1:13" ht="15">
       <c r="A266">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B266">
         <f t="shared" si="50"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C266" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-30</v>
+        <v>28-28</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
@@ -9951,15 +10117,15 @@
     <row r="267" spans="1:13" ht="15">
       <c r="A267">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B267">
         <f t="shared" si="50"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C267" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-31</v>
+        <v>28-29</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
@@ -9967,15 +10133,15 @@
     <row r="268" spans="1:13" ht="15">
       <c r="A268">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B268">
         <f t="shared" si="50"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C268" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-32</v>
+        <v>28-30</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
@@ -9983,15 +10149,15 @@
     <row r="269" spans="1:13" ht="15">
       <c r="A269">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B269">
         <f t="shared" si="50"/>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C269" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-33</v>
+        <v>28-31</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
@@ -9999,15 +10165,15 @@
     <row r="270" spans="1:13" ht="15">
       <c r="A270">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B270">
         <f t="shared" si="50"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C270" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-34</v>
+        <v>28-32</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
@@ -10015,15 +10181,15 @@
     <row r="271" spans="1:13" ht="15">
       <c r="A271">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B271">
         <f t="shared" si="50"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C271" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-35</v>
+        <v>28-33</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
@@ -10031,15 +10197,15 @@
     <row r="272" spans="1:13" ht="15">
       <c r="A272">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B272">
         <f t="shared" si="50"/>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C272" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-36</v>
+        <v>28-34</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
@@ -10047,15 +10213,15 @@
     <row r="273" spans="1:13" ht="15">
       <c r="A273">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B273">
         <f t="shared" si="50"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C273" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-37</v>
+        <v>28-35</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
@@ -10063,15 +10229,15 @@
     <row r="274" spans="1:13" ht="15">
       <c r="A274">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B274">
         <f t="shared" si="50"/>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C274" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-38</v>
+        <v>28-36</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
@@ -10079,15 +10245,15 @@
     <row r="275" spans="1:13" ht="15">
       <c r="A275">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B275">
         <f t="shared" si="50"/>
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C275" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-39</v>
+        <v>28-37</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
@@ -10095,15 +10261,15 @@
     <row r="276" spans="1:13" ht="15">
       <c r="A276">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B276">
         <f t="shared" si="50"/>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C276" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-40</v>
+        <v>28-38</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
@@ -10111,15 +10277,15 @@
     <row r="277" spans="1:13" ht="15">
       <c r="A277">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B277">
         <f t="shared" si="50"/>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C277" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-41</v>
+        <v>28-39</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
@@ -10127,15 +10293,15 @@
     <row r="278" spans="1:13" ht="15">
       <c r="A278">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B278">
         <f t="shared" si="50"/>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C278" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-42</v>
+        <v>28-40</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
@@ -10143,15 +10309,15 @@
     <row r="279" spans="1:13" ht="15">
       <c r="A279">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B279">
         <f t="shared" si="50"/>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C279" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-43</v>
+        <v>28-41</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
@@ -10159,15 +10325,15 @@
     <row r="280" spans="1:13" ht="15">
       <c r="A280">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B280">
         <f t="shared" si="50"/>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C280" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-44</v>
+        <v>28-42</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
@@ -10175,15 +10341,15 @@
     <row r="281" spans="1:13" ht="15">
       <c r="A281">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B281">
         <f t="shared" si="50"/>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C281" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-45</v>
+        <v>28-43</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
@@ -10191,15 +10357,15 @@
     <row r="282" spans="1:13" ht="15">
       <c r="A282">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B282">
         <f t="shared" si="50"/>
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C282" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-46</v>
+        <v>28-44</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
@@ -10207,15 +10373,15 @@
     <row r="283" spans="1:13" ht="15">
       <c r="A283">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B283">
         <f t="shared" si="50"/>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C283" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-47</v>
+        <v>28-45</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
@@ -10223,15 +10389,15 @@
     <row r="284" spans="1:13" ht="15">
       <c r="A284">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B284">
         <f t="shared" si="50"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C284" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-48</v>
+        <v>28-46</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
@@ -10239,15 +10405,15 @@
     <row r="285" spans="1:13" ht="15">
       <c r="A285">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B285">
         <f t="shared" si="50"/>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C285" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-49</v>
+        <v>28-47</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
@@ -10255,15 +10421,15 @@
     <row r="286" spans="1:13" ht="15">
       <c r="A286">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B286">
         <f t="shared" si="50"/>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C286" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-50</v>
+        <v>28-48</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
@@ -10271,15 +10437,15 @@
     <row r="287" spans="1:13" ht="15">
       <c r="A287">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B287">
         <f t="shared" si="50"/>
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C287" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-51</v>
+        <v>28-49</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
@@ -10287,15 +10453,15 @@
     <row r="288" spans="1:13" ht="15">
       <c r="A288">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B288">
         <f t="shared" si="50"/>
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C288" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-52</v>
+        <v>28-50</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
@@ -10303,15 +10469,15 @@
     <row r="289" spans="1:13" ht="15">
       <c r="A289">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B289">
         <f t="shared" si="50"/>
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C289" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-53</v>
+        <v>28-51</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
@@ -10319,15 +10485,15 @@
     <row r="290" spans="1:13" ht="15">
       <c r="A290">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B290">
         <f t="shared" si="50"/>
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C290" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-54</v>
+        <v>28-52</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
@@ -10335,15 +10501,15 @@
     <row r="291" spans="1:13" ht="15">
       <c r="A291">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B291">
         <f t="shared" si="50"/>
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C291" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-55</v>
+        <v>28-53</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
@@ -10351,15 +10517,15 @@
     <row r="292" spans="1:13" ht="15">
       <c r="A292">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B292">
         <f t="shared" si="50"/>
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C292" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-56</v>
+        <v>28-54</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
@@ -10367,15 +10533,15 @@
     <row r="293" spans="1:13" ht="15">
       <c r="A293">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B293">
         <f t="shared" si="50"/>
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C293" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-57</v>
+        <v>28-55</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
@@ -10383,15 +10549,15 @@
     <row r="294" spans="1:13" ht="15">
       <c r="A294">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B294">
         <f t="shared" si="50"/>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C294" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-58</v>
+        <v>28-56</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
@@ -10399,15 +10565,15 @@
     <row r="295" spans="1:13" ht="15">
       <c r="A295">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B295">
         <f t="shared" si="50"/>
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C295" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-59</v>
+        <v>28-57</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
@@ -10415,15 +10581,15 @@
     <row r="296" spans="1:13" ht="15">
       <c r="A296">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B296">
         <f t="shared" si="50"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C296" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-60</v>
+        <v>28-58</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
@@ -10431,15 +10597,15 @@
     <row r="297" spans="1:13" ht="15">
       <c r="A297">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B297">
         <f t="shared" si="50"/>
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C297" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-61</v>
+        <v>28-59</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
@@ -10447,15 +10613,15 @@
     <row r="298" spans="1:13" ht="15">
       <c r="A298">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B298">
         <f t="shared" si="50"/>
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C298" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>27-62</v>
+        <v>28-60</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
@@ -10463,15 +10629,15 @@
     <row r="299" spans="1:13" ht="15">
       <c r="A299">
         <f t="shared" si="52"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B299">
         <f t="shared" ref="B299:B362" si="53">IF(A299=A298,B298+1,1)</f>
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C299" s="3" t="str">
         <f t="shared" ref="C299:C362" si="54">CONCATENATE(A299,"-",B299)</f>
-        <v>27-63</v>
+        <v>28-61</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
@@ -10479,15 +10645,15 @@
     <row r="300" spans="1:13" ht="15">
       <c r="A300">
         <f t="shared" ref="A300:A363" si="55">A299</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B300">
         <f t="shared" si="53"/>
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C300" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-64</v>
+        <v>28-62</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
@@ -10495,15 +10661,15 @@
     <row r="301" spans="1:13" ht="15">
       <c r="A301">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B301">
         <f t="shared" si="53"/>
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C301" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-65</v>
+        <v>28-63</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
@@ -10511,15 +10677,15 @@
     <row r="302" spans="1:13" ht="15">
       <c r="A302">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B302">
         <f t="shared" si="53"/>
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C302" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-66</v>
+        <v>28-64</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
@@ -10527,15 +10693,15 @@
     <row r="303" spans="1:13" ht="15">
       <c r="A303">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B303">
         <f t="shared" si="53"/>
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C303" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-67</v>
+        <v>28-65</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
@@ -10543,15 +10709,15 @@
     <row r="304" spans="1:13" ht="15">
       <c r="A304">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B304">
         <f t="shared" si="53"/>
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C304" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-68</v>
+        <v>28-66</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
@@ -10559,15 +10725,15 @@
     <row r="305" spans="1:13" ht="15">
       <c r="A305">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B305">
         <f t="shared" si="53"/>
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C305" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-69</v>
+        <v>28-67</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
@@ -10575,15 +10741,15 @@
     <row r="306" spans="1:13" ht="15">
       <c r="A306">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B306">
         <f t="shared" si="53"/>
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C306" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-70</v>
+        <v>28-68</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
@@ -10591,15 +10757,15 @@
     <row r="307" spans="1:13" ht="15">
       <c r="A307">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B307">
         <f t="shared" si="53"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C307" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-71</v>
+        <v>28-69</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
@@ -10607,15 +10773,15 @@
     <row r="308" spans="1:13" ht="15">
       <c r="A308">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B308">
         <f t="shared" si="53"/>
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C308" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-72</v>
+        <v>28-70</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
@@ -10623,15 +10789,15 @@
     <row r="309" spans="1:13" ht="15">
       <c r="A309">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B309">
         <f t="shared" si="53"/>
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C309" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-73</v>
+        <v>28-71</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
@@ -10639,15 +10805,15 @@
     <row r="310" spans="1:13" ht="15">
       <c r="A310">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B310">
         <f t="shared" si="53"/>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C310" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-74</v>
+        <v>28-72</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
@@ -10655,15 +10821,15 @@
     <row r="311" spans="1:13" ht="15">
       <c r="A311">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B311">
         <f t="shared" si="53"/>
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C311" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-75</v>
+        <v>28-73</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
@@ -10671,15 +10837,15 @@
     <row r="312" spans="1:13" ht="15">
       <c r="A312">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B312">
         <f t="shared" si="53"/>
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C312" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-76</v>
+        <v>28-74</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
@@ -10687,15 +10853,15 @@
     <row r="313" spans="1:13" ht="15">
       <c r="A313">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B313">
         <f t="shared" si="53"/>
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C313" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-77</v>
+        <v>28-75</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
@@ -10703,15 +10869,15 @@
     <row r="314" spans="1:13" ht="15">
       <c r="A314">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B314">
         <f t="shared" si="53"/>
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C314" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-78</v>
+        <v>28-76</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
@@ -10719,15 +10885,15 @@
     <row r="315" spans="1:13" ht="15">
       <c r="A315">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B315">
         <f t="shared" si="53"/>
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C315" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-79</v>
+        <v>28-77</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
@@ -10735,15 +10901,15 @@
     <row r="316" spans="1:13" ht="15">
       <c r="A316">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B316">
         <f t="shared" si="53"/>
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C316" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-80</v>
+        <v>28-78</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
@@ -10751,15 +10917,15 @@
     <row r="317" spans="1:13" ht="15">
       <c r="A317">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B317">
         <f t="shared" si="53"/>
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C317" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-81</v>
+        <v>28-79</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
@@ -10767,15 +10933,15 @@
     <row r="318" spans="1:13" ht="15">
       <c r="A318">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B318">
         <f t="shared" si="53"/>
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C318" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-82</v>
+        <v>28-80</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
@@ -10783,15 +10949,15 @@
     <row r="319" spans="1:13" ht="15">
       <c r="A319">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B319">
         <f t="shared" si="53"/>
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C319" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-83</v>
+        <v>28-81</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
@@ -10799,15 +10965,15 @@
     <row r="320" spans="1:13" ht="15">
       <c r="A320">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B320">
         <f t="shared" si="53"/>
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C320" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-84</v>
+        <v>28-82</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
@@ -10815,15 +10981,15 @@
     <row r="321" spans="1:13" ht="15">
       <c r="A321">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B321">
         <f t="shared" si="53"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C321" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-85</v>
+        <v>28-83</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
@@ -10831,15 +10997,15 @@
     <row r="322" spans="1:13" ht="15">
       <c r="A322">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B322">
         <f t="shared" si="53"/>
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C322" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-86</v>
+        <v>28-84</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
@@ -10847,15 +11013,15 @@
     <row r="323" spans="1:13" ht="15">
       <c r="A323">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B323">
         <f t="shared" si="53"/>
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C323" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-87</v>
+        <v>28-85</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
@@ -10863,15 +11029,15 @@
     <row r="324" spans="1:13" ht="15">
       <c r="A324">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B324">
         <f t="shared" si="53"/>
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C324" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-88</v>
+        <v>28-86</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
@@ -10879,15 +11045,15 @@
     <row r="325" spans="1:13" ht="15">
       <c r="A325">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B325">
         <f t="shared" si="53"/>
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C325" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-89</v>
+        <v>28-87</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
@@ -10895,15 +11061,15 @@
     <row r="326" spans="1:13" ht="15">
       <c r="A326">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B326">
         <f t="shared" si="53"/>
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C326" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-90</v>
+        <v>28-88</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
@@ -10911,15 +11077,15 @@
     <row r="327" spans="1:13" ht="15">
       <c r="A327">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B327">
         <f t="shared" si="53"/>
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C327" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-91</v>
+        <v>28-89</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
@@ -10927,15 +11093,15 @@
     <row r="328" spans="1:13" ht="15">
       <c r="A328">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B328">
         <f t="shared" si="53"/>
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C328" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-92</v>
+        <v>28-90</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
@@ -10943,15 +11109,15 @@
     <row r="329" spans="1:13" ht="15">
       <c r="A329">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B329">
         <f t="shared" si="53"/>
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C329" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-93</v>
+        <v>28-91</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
@@ -10959,15 +11125,15 @@
     <row r="330" spans="1:13" ht="15">
       <c r="A330">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B330">
         <f t="shared" si="53"/>
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C330" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-94</v>
+        <v>28-92</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
@@ -10975,15 +11141,15 @@
     <row r="331" spans="1:13" ht="15">
       <c r="A331">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B331">
         <f t="shared" si="53"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C331" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-95</v>
+        <v>28-93</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
@@ -10991,15 +11157,15 @@
     <row r="332" spans="1:13" ht="15">
       <c r="A332">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B332">
         <f t="shared" si="53"/>
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C332" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-96</v>
+        <v>28-94</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
@@ -11007,15 +11173,15 @@
     <row r="333" spans="1:13" ht="15">
       <c r="A333">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B333">
         <f t="shared" si="53"/>
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C333" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-97</v>
+        <v>28-95</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
@@ -11023,15 +11189,15 @@
     <row r="334" spans="1:13" ht="15">
       <c r="A334">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B334">
         <f t="shared" si="53"/>
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C334" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-98</v>
+        <v>28-96</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
@@ -11039,15 +11205,15 @@
     <row r="335" spans="1:13" ht="15">
       <c r="A335">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B335">
         <f t="shared" si="53"/>
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C335" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-99</v>
+        <v>28-97</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
@@ -11055,15 +11221,15 @@
     <row r="336" spans="1:13" ht="15">
       <c r="A336">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B336">
         <f t="shared" si="53"/>
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C336" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-100</v>
+        <v>28-98</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
@@ -11071,15 +11237,15 @@
     <row r="337" spans="1:13" ht="15">
       <c r="A337">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B337">
         <f t="shared" si="53"/>
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C337" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-101</v>
+        <v>28-99</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
@@ -11087,15 +11253,15 @@
     <row r="338" spans="1:13" ht="15">
       <c r="A338">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B338">
         <f t="shared" si="53"/>
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C338" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-102</v>
+        <v>28-100</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
@@ -11103,15 +11269,15 @@
     <row r="339" spans="1:13" ht="15">
       <c r="A339">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B339">
         <f t="shared" si="53"/>
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C339" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-103</v>
+        <v>28-101</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
@@ -11119,15 +11285,15 @@
     <row r="340" spans="1:13" ht="15">
       <c r="A340">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B340">
         <f t="shared" si="53"/>
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C340" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-104</v>
+        <v>28-102</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
@@ -11135,15 +11301,15 @@
     <row r="341" spans="1:13" ht="15">
       <c r="A341">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B341">
         <f t="shared" si="53"/>
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C341" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-105</v>
+        <v>28-103</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
@@ -11151,15 +11317,15 @@
     <row r="342" spans="1:13" ht="15">
       <c r="A342">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B342">
         <f t="shared" si="53"/>
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C342" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-106</v>
+        <v>28-104</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
@@ -11167,15 +11333,15 @@
     <row r="343" spans="1:13" ht="15">
       <c r="A343">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B343">
         <f t="shared" si="53"/>
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C343" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-107</v>
+        <v>28-105</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
@@ -11183,15 +11349,15 @@
     <row r="344" spans="1:13" ht="15">
       <c r="A344">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B344">
         <f t="shared" si="53"/>
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C344" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-108</v>
+        <v>28-106</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
@@ -11199,15 +11365,15 @@
     <row r="345" spans="1:13" ht="15">
       <c r="A345">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B345">
         <f t="shared" si="53"/>
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C345" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-109</v>
+        <v>28-107</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
@@ -11215,15 +11381,15 @@
     <row r="346" spans="1:13" ht="15">
       <c r="A346">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B346">
         <f t="shared" si="53"/>
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C346" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-110</v>
+        <v>28-108</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
@@ -11231,15 +11397,15 @@
     <row r="347" spans="1:13" ht="15">
       <c r="A347">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B347">
         <f t="shared" si="53"/>
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C347" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-111</v>
+        <v>28-109</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
@@ -11247,15 +11413,15 @@
     <row r="348" spans="1:13" ht="15">
       <c r="A348">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B348">
         <f t="shared" si="53"/>
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C348" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-112</v>
+        <v>28-110</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
@@ -11263,15 +11429,15 @@
     <row r="349" spans="1:13" ht="15">
       <c r="A349">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B349">
         <f t="shared" si="53"/>
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C349" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-113</v>
+        <v>28-111</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
@@ -11279,15 +11445,15 @@
     <row r="350" spans="1:13" ht="15">
       <c r="A350">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B350">
         <f t="shared" si="53"/>
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C350" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-114</v>
+        <v>28-112</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
@@ -11295,15 +11461,15 @@
     <row r="351" spans="1:13" ht="15">
       <c r="A351">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B351">
         <f t="shared" si="53"/>
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C351" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-115</v>
+        <v>28-113</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
@@ -11311,15 +11477,15 @@
     <row r="352" spans="1:13" ht="15">
       <c r="A352">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B352">
         <f t="shared" si="53"/>
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C352" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-116</v>
+        <v>28-114</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
@@ -11327,15 +11493,15 @@
     <row r="353" spans="1:13" ht="15">
       <c r="A353">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B353">
         <f t="shared" si="53"/>
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C353" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-117</v>
+        <v>28-115</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
@@ -11343,15 +11509,15 @@
     <row r="354" spans="1:13" ht="15">
       <c r="A354">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B354">
         <f t="shared" si="53"/>
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C354" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-118</v>
+        <v>28-116</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
@@ -11359,15 +11525,15 @@
     <row r="355" spans="1:13" ht="15">
       <c r="A355">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B355">
         <f t="shared" si="53"/>
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C355" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-119</v>
+        <v>28-117</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
@@ -11375,15 +11541,15 @@
     <row r="356" spans="1:13" ht="15">
       <c r="A356">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B356">
         <f t="shared" si="53"/>
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C356" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-120</v>
+        <v>28-118</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
@@ -11391,15 +11557,15 @@
     <row r="357" spans="1:13" ht="15">
       <c r="A357">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B357">
         <f t="shared" si="53"/>
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C357" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-121</v>
+        <v>28-119</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
@@ -11407,15 +11573,15 @@
     <row r="358" spans="1:13" ht="15">
       <c r="A358">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B358">
         <f t="shared" si="53"/>
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C358" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-122</v>
+        <v>28-120</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
@@ -11423,15 +11589,15 @@
     <row r="359" spans="1:13" ht="15">
       <c r="A359">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B359">
         <f t="shared" si="53"/>
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C359" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-123</v>
+        <v>28-121</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
@@ -11439,15 +11605,15 @@
     <row r="360" spans="1:13" ht="15">
       <c r="A360">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B360">
         <f t="shared" si="53"/>
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C360" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-124</v>
+        <v>28-122</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
@@ -11455,15 +11621,15 @@
     <row r="361" spans="1:13" ht="15">
       <c r="A361">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B361">
         <f t="shared" si="53"/>
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C361" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-125</v>
+        <v>28-123</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
@@ -11471,15 +11637,15 @@
     <row r="362" spans="1:13" ht="15">
       <c r="A362">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B362">
         <f t="shared" si="53"/>
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C362" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>27-126</v>
+        <v>28-124</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
@@ -11487,15 +11653,15 @@
     <row r="363" spans="1:13" ht="15">
       <c r="A363">
         <f t="shared" si="55"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B363">
         <f t="shared" ref="B363:B384" si="56">IF(A363=A362,B362+1,1)</f>
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C363" s="3" t="str">
         <f t="shared" ref="C363:C384" si="57">CONCATENATE(A363,"-",B363)</f>
-        <v>27-127</v>
+        <v>28-125</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
@@ -11503,15 +11669,15 @@
     <row r="364" spans="1:13" ht="15">
       <c r="A364">
         <f t="shared" ref="A364:A384" si="58">A363</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B364">
         <f t="shared" si="56"/>
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C364" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-128</v>
+        <v>28-126</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
@@ -11519,15 +11685,15 @@
     <row r="365" spans="1:13" ht="15">
       <c r="A365">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B365">
         <f t="shared" si="56"/>
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C365" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-129</v>
+        <v>28-127</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
@@ -11535,15 +11701,15 @@
     <row r="366" spans="1:13" ht="15">
       <c r="A366">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B366">
         <f t="shared" si="56"/>
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C366" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-130</v>
+        <v>28-128</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
@@ -11551,15 +11717,15 @@
     <row r="367" spans="1:13" ht="15">
       <c r="A367">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B367">
         <f t="shared" si="56"/>
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C367" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-131</v>
+        <v>28-129</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
@@ -11567,15 +11733,15 @@
     <row r="368" spans="1:13" ht="15">
       <c r="A368">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B368">
         <f t="shared" si="56"/>
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C368" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-132</v>
+        <v>28-130</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
@@ -11583,15 +11749,15 @@
     <row r="369" spans="1:13" ht="15">
       <c r="A369">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B369">
         <f t="shared" si="56"/>
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C369" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-133</v>
+        <v>28-131</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
@@ -11599,15 +11765,15 @@
     <row r="370" spans="1:13" ht="15">
       <c r="A370">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B370">
         <f t="shared" si="56"/>
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C370" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-134</v>
+        <v>28-132</v>
       </c>
       <c r="L370" s="6"/>
       <c r="M370" s="6"/>
@@ -11615,15 +11781,15 @@
     <row r="371" spans="1:13" ht="15">
       <c r="A371">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B371">
         <f t="shared" si="56"/>
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C371" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-135</v>
+        <v>28-133</v>
       </c>
       <c r="L371" s="6"/>
       <c r="M371" s="6"/>
@@ -11631,15 +11797,15 @@
     <row r="372" spans="1:13" ht="15">
       <c r="A372">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B372">
         <f t="shared" si="56"/>
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C372" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-136</v>
+        <v>28-134</v>
       </c>
       <c r="L372" s="6"/>
       <c r="M372" s="6"/>
@@ -11647,15 +11813,15 @@
     <row r="373" spans="1:13" ht="15">
       <c r="A373">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B373">
         <f t="shared" si="56"/>
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C373" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-137</v>
+        <v>28-135</v>
       </c>
       <c r="L373" s="6"/>
       <c r="M373" s="6"/>
@@ -11663,15 +11829,15 @@
     <row r="374" spans="1:13" ht="15">
       <c r="A374">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B374">
         <f t="shared" si="56"/>
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C374" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-138</v>
+        <v>28-136</v>
       </c>
       <c r="L374" s="6"/>
       <c r="M374" s="6"/>
@@ -11679,15 +11845,15 @@
     <row r="375" spans="1:13" ht="15">
       <c r="A375">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B375">
         <f t="shared" si="56"/>
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C375" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-139</v>
+        <v>28-137</v>
       </c>
       <c r="L375" s="6"/>
       <c r="M375" s="6"/>
@@ -11695,15 +11861,15 @@
     <row r="376" spans="1:13" ht="15">
       <c r="A376">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B376">
         <f t="shared" si="56"/>
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C376" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-140</v>
+        <v>28-138</v>
       </c>
       <c r="L376" s="6"/>
       <c r="M376" s="6"/>
@@ -11711,15 +11877,15 @@
     <row r="377" spans="1:13" ht="15">
       <c r="A377">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B377">
         <f t="shared" si="56"/>
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C377" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-141</v>
+        <v>28-139</v>
       </c>
       <c r="L377" s="6"/>
       <c r="M377" s="6"/>
@@ -11727,15 +11893,15 @@
     <row r="378" spans="1:13" ht="15">
       <c r="A378">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B378">
         <f t="shared" si="56"/>
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C378" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-142</v>
+        <v>28-140</v>
       </c>
       <c r="L378" s="6"/>
       <c r="M378" s="6"/>
@@ -11743,15 +11909,15 @@
     <row r="379" spans="1:13" ht="15">
       <c r="A379">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B379">
         <f t="shared" si="56"/>
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C379" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-143</v>
+        <v>28-141</v>
       </c>
       <c r="L379" s="6"/>
       <c r="M379" s="6"/>
@@ -11759,15 +11925,15 @@
     <row r="380" spans="1:13" ht="15">
       <c r="A380">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B380">
         <f t="shared" si="56"/>
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C380" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-144</v>
+        <v>28-142</v>
       </c>
       <c r="L380" s="6"/>
       <c r="M380" s="6"/>
@@ -11775,15 +11941,15 @@
     <row r="381" spans="1:13" ht="15">
       <c r="A381">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B381">
         <f t="shared" si="56"/>
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C381" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-145</v>
+        <v>28-143</v>
       </c>
       <c r="L381" s="6"/>
       <c r="M381" s="6"/>
@@ -11791,15 +11957,15 @@
     <row r="382" spans="1:13" ht="15">
       <c r="A382">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B382">
         <f t="shared" si="56"/>
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C382" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-146</v>
+        <v>28-144</v>
       </c>
       <c r="L382" s="6"/>
       <c r="M382" s="6"/>
@@ -11807,15 +11973,15 @@
     <row r="383" spans="1:13" ht="15">
       <c r="A383">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B383">
         <f t="shared" si="56"/>
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C383" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-147</v>
+        <v>28-145</v>
       </c>
       <c r="L383" s="6"/>
       <c r="M383" s="6"/>
@@ -11823,15 +11989,15 @@
     <row r="384" spans="1:13" ht="15">
       <c r="A384">
         <f t="shared" si="58"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B384">
         <f t="shared" si="56"/>
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C384" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>27-148</v>
+        <v>28-146</v>
       </c>
       <c r="L384" s="6"/>
       <c r="M384" s="6"/>
@@ -14589,348 +14755,378 @@
     <mergeCell ref="L188:L191"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsBlanks" dxfId="71" priority="73">
+    <cfRule type="containsBlanks" dxfId="80" priority="79">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsText" dxfId="70" priority="74" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsText" dxfId="69" priority="75" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="78" priority="81" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsBlanks" dxfId="68" priority="70">
+    <cfRule type="containsBlanks" dxfId="77" priority="76">
       <formula>LEN(TRIM(K200))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsBlanks" dxfId="65" priority="64">
+    <cfRule type="containsBlanks" dxfId="74" priority="70">
       <formula>LEN(TRIM(K201))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="73" priority="71" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="72" priority="72" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsBlanks" dxfId="62" priority="61">
+    <cfRule type="containsBlanks" dxfId="71" priority="67">
       <formula>LEN(TRIM(K202))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="70" priority="68" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="69" priority="69" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsBlanks" dxfId="59" priority="58">
+    <cfRule type="containsBlanks" dxfId="68" priority="64">
       <formula>LEN(TRIM(K203))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="56" priority="55">
+    <cfRule type="containsBlanks" dxfId="65" priority="61">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsBlanks" dxfId="55" priority="52">
+    <cfRule type="containsBlanks" dxfId="64" priority="58">
       <formula>LEN(TRIM(K207))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsBlanks" dxfId="54" priority="49">
+    <cfRule type="containsBlanks" dxfId="63" priority="55">
       <formula>LEN(TRIM(K209))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsBlanks" dxfId="53" priority="46">
+    <cfRule type="containsBlanks" dxfId="62" priority="52">
       <formula>LEN(TRIM(K210))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsBlanks" dxfId="52" priority="43">
+    <cfRule type="containsBlanks" dxfId="61" priority="49">
       <formula>LEN(TRIM(K212))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsBlanks" dxfId="51" priority="40">
+    <cfRule type="containsBlanks" dxfId="60" priority="46">
       <formula>LEN(TRIM(K214))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsBlanks" dxfId="50" priority="37">
+    <cfRule type="containsBlanks" dxfId="59" priority="43">
       <formula>LEN(TRIM(K216))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="49" priority="31">
+    <cfRule type="containsBlanks" dxfId="58" priority="37">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="48" priority="56" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="57" priority="62" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="47" priority="57" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="56" priority="63" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsBlanks" dxfId="46" priority="28">
+    <cfRule type="containsBlanks" dxfId="55" priority="34">
       <formula>LEN(TRIM(K208))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="45" priority="53" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="54" priority="59" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="44" priority="54" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="53" priority="60" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="43" priority="25">
+    <cfRule type="containsBlanks" dxfId="52" priority="31">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="42" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="51" priority="56" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="41" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="50" priority="57" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsBlanks" dxfId="40" priority="22">
+    <cfRule type="containsBlanks" dxfId="49" priority="28">
       <formula>LEN(TRIM(K211))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="39" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="48" priority="53" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="38" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="47" priority="54" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsBlanks" dxfId="37" priority="19">
+    <cfRule type="containsBlanks" dxfId="46" priority="25">
       <formula>LEN(TRIM(K213))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="36" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="35" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="44" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsBlanks" dxfId="34" priority="16">
+    <cfRule type="containsBlanks" dxfId="43" priority="22">
       <formula>LEN(TRIM(K215))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="33" priority="41" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="42" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="32" priority="42" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="41" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsText" dxfId="30" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="36" priority="35" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="32" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="31" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="21" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsBlanks" dxfId="17" priority="13">
+    <cfRule type="containsBlanks" dxfId="26" priority="19">
       <formula>LEN(TRIM(K232))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K232))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K232))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsBlanks" dxfId="14" priority="10">
+    <cfRule type="containsBlanks" dxfId="23" priority="16">
       <formula>LEN(TRIM(K217))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsBlanks" dxfId="11" priority="7">
+    <cfRule type="containsBlanks" dxfId="20" priority="13">
       <formula>LEN(TRIM(K218))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsBlanks" dxfId="8" priority="4">
+    <cfRule type="containsBlanks" dxfId="17" priority="10">
       <formula>LEN(TRIM(K235))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="14" priority="7">
       <formula>LEN(TRIM(K236))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K236))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K239">
+    <cfRule type="containsBlanks" dxfId="11" priority="4">
+      <formula>LEN(TRIM(K239))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K239">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K239))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K239">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K239))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K240">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
+      <formula>LEN(TRIM(K240))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K240">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K240))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K240">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K240))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add note about adding hidden perspectives
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="308">
   <si>
     <t>Test Number</t>
   </si>
@@ -938,6 +938,9 @@
   </si>
   <si>
     <t>If target is blank: Error message is shown naming the offending device screen &amp; ok button is disabled</t>
+  </si>
+  <si>
+    <t>Note that if the device screens perspective is not present, use CTRL+ALT+P to access the preferences menu, go to ISIS perspectives and add the device screens. You'll need to restart the GUI</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1010,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1119,11 +1122,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1236,52 +1265,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="81">
+  <dxfs count="75">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF4C7C3"/>
           <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
       <border>
@@ -1322,34 +1329,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFF4C7C3"/>
           <bgColor rgb="FFF4C7C3"/>
         </patternFill>
@@ -1366,34 +1345,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
         </patternFill>
       </fill>
       <border>
@@ -2684,7 +2635,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J232" sqref="J232"/>
+      <selection pane="bottomLeft" activeCell="L239" sqref="L239:L240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -8145,7 +8096,7 @@
       </c>
       <c r="J188" s="8"/>
       <c r="K188" s="7"/>
-      <c r="L188" s="50"/>
+      <c r="L188" s="51"/>
     </row>
     <row r="189" spans="1:13" ht="30">
       <c r="A189">
@@ -8174,7 +8125,7 @@
       </c>
       <c r="J189" s="8"/>
       <c r="K189" s="7"/>
-      <c r="L189" s="51"/>
+      <c r="L189" s="52"/>
       <c r="M189" s="6"/>
     </row>
     <row r="190" spans="1:13" ht="45">
@@ -8204,7 +8155,7 @@
       </c>
       <c r="J190" s="8"/>
       <c r="K190" s="7"/>
-      <c r="L190" s="51"/>
+      <c r="L190" s="52"/>
       <c r="M190" s="6"/>
     </row>
     <row r="191" spans="1:13" ht="30">
@@ -8234,7 +8185,7 @@
       </c>
       <c r="J191" s="8"/>
       <c r="K191" s="7"/>
-      <c r="L191" s="52"/>
+      <c r="L191" s="53"/>
       <c r="M191" s="6"/>
     </row>
     <row r="192" spans="1:13" ht="30">
@@ -9641,7 +9592,7 @@
       <c r="L238" s="26"/>
       <c r="M238" s="6"/>
     </row>
-    <row r="239" spans="1:13" ht="26.25">
+    <row r="239" spans="1:13" ht="39" customHeight="1">
       <c r="A239">
         <v>28</v>
       </c>
@@ -9665,7 +9616,9 @@
       </c>
       <c r="J239" s="23"/>
       <c r="K239" s="21"/>
-      <c r="L239" s="26"/>
+      <c r="L239" s="54" t="s">
+        <v>307</v>
+      </c>
       <c r="M239" s="6"/>
     </row>
     <row r="240" spans="1:13" ht="26.25">
@@ -9691,11 +9644,11 @@
       <c r="I240" s="25" t="s">
         <v>305</v>
       </c>
-      <c r="J240" s="53" t="s">
+      <c r="J240" s="50" t="s">
         <v>306</v>
       </c>
       <c r="K240" s="21"/>
-      <c r="L240" s="26"/>
+      <c r="L240" s="55"/>
       <c r="M240" s="6"/>
     </row>
     <row r="241" spans="1:13" ht="15">
@@ -14751,381 +14704,382 @@
       <c r="M1071" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="L188:L191"/>
+    <mergeCell ref="L239:L240"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsBlanks" dxfId="80" priority="79">
+    <cfRule type="containsBlanks" dxfId="74" priority="79">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="73" priority="80" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsText" dxfId="78" priority="81" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="72" priority="81" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsBlanks" dxfId="77" priority="76">
+    <cfRule type="containsBlanks" dxfId="71" priority="76">
       <formula>LEN(TRIM(K200))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="70" priority="77" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="69" priority="78" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsBlanks" dxfId="74" priority="70">
+    <cfRule type="containsBlanks" dxfId="68" priority="70">
       <formula>LEN(TRIM(K201))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="73" priority="71" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="72" priority="72" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsBlanks" dxfId="71" priority="67">
+    <cfRule type="containsBlanks" dxfId="65" priority="67">
       <formula>LEN(TRIM(K202))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="70" priority="68" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="69" priority="69" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="63" priority="69" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsBlanks" dxfId="68" priority="64">
+    <cfRule type="containsBlanks" dxfId="62" priority="64">
       <formula>LEN(TRIM(K203))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="61" priority="65" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="60" priority="66" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="65" priority="61">
+    <cfRule type="containsBlanks" dxfId="59" priority="61">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsBlanks" dxfId="64" priority="58">
+    <cfRule type="containsBlanks" dxfId="58" priority="58">
       <formula>LEN(TRIM(K207))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsBlanks" dxfId="63" priority="55">
+    <cfRule type="containsBlanks" dxfId="57" priority="55">
       <formula>LEN(TRIM(K209))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsBlanks" dxfId="62" priority="52">
+    <cfRule type="containsBlanks" dxfId="56" priority="52">
       <formula>LEN(TRIM(K210))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsBlanks" dxfId="61" priority="49">
+    <cfRule type="containsBlanks" dxfId="55" priority="49">
       <formula>LEN(TRIM(K212))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsBlanks" dxfId="60" priority="46">
+    <cfRule type="containsBlanks" dxfId="54" priority="46">
       <formula>LEN(TRIM(K214))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsBlanks" dxfId="59" priority="43">
+    <cfRule type="containsBlanks" dxfId="53" priority="43">
       <formula>LEN(TRIM(K216))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="58" priority="37">
+    <cfRule type="containsBlanks" dxfId="52" priority="37">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="57" priority="62" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="51" priority="62" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="56" priority="63" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="50" priority="63" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsBlanks" dxfId="55" priority="34">
+    <cfRule type="containsBlanks" dxfId="49" priority="34">
       <formula>LEN(TRIM(K208))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="54" priority="59" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="48" priority="59" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="53" priority="60" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="47" priority="60" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="52" priority="31">
+    <cfRule type="containsBlanks" dxfId="46" priority="31">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="51" priority="56" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="45" priority="56" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="50" priority="57" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="44" priority="57" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsBlanks" dxfId="49" priority="28">
+    <cfRule type="containsBlanks" dxfId="43" priority="28">
       <formula>LEN(TRIM(K211))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="48" priority="53" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="42" priority="53" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="47" priority="54" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="41" priority="54" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsBlanks" dxfId="46" priority="25">
+    <cfRule type="containsBlanks" dxfId="40" priority="25">
       <formula>LEN(TRIM(K213))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="39" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="44" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="38" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsBlanks" dxfId="43" priority="22">
+    <cfRule type="containsBlanks" dxfId="37" priority="22">
       <formula>LEN(TRIM(K215))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="42" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="36" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="41" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="32" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="31" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="36" priority="35" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="32" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="31" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsBlanks" dxfId="26" priority="19">
+    <cfRule type="containsBlanks" dxfId="20" priority="19">
       <formula>LEN(TRIM(K232))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K232))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K232))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsBlanks" dxfId="23" priority="16">
+    <cfRule type="containsBlanks" dxfId="17" priority="16">
       <formula>LEN(TRIM(K217))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsBlanks" dxfId="20" priority="13">
+    <cfRule type="containsBlanks" dxfId="14" priority="13">
       <formula>LEN(TRIM(K218))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsBlanks" dxfId="17" priority="10">
+    <cfRule type="containsBlanks" dxfId="11" priority="10">
       <formula>LEN(TRIM(K235))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsBlanks" dxfId="14" priority="7">
+    <cfRule type="containsBlanks" dxfId="8" priority="7">
       <formula>LEN(TRIM(K236))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsBlanks" dxfId="11" priority="4">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
       <formula>LEN(TRIM(K239))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(K240))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K240))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K240))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added a manual system test for colour blind option
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="311">
   <si>
     <t>Test Number</t>
   </si>
@@ -941,6 +941,16 @@
   </si>
   <si>
     <t>Note that if the device screens perspective is not present, use CTRL+ALT+P to access the preferences menu, go to ISIS perspectives and add the device screens. You'll need to restart the GUI</t>
+  </si>
+  <si>
+    <t>Colour blind mode in table of motors</t>
+  </si>
+  <si>
+    <t>Check that changing the colour option actually changes the colours in the table of motors. (Change the setting both before and after opening the motors perspective)</t>
+  </si>
+  <si>
+    <t>The colours in the table of motors change to a 
+colour-blind friendly mode.</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1020,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1139,20 +1149,31 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1276,14 +1297,104 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="81">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2634,8 +2745,8 @@
   <dimension ref="A1:N1071"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L239" sqref="L239:L240"/>
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K245" sqref="K245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -9634,24 +9745,24 @@
         <f t="shared" si="51"/>
         <v>28-2</v>
       </c>
-      <c r="D240" s="23"/>
-      <c r="E240" s="23"/>
-      <c r="F240" s="23"/>
-      <c r="G240" s="23"/>
-      <c r="H240" s="24" t="s">
+      <c r="D240" s="36"/>
+      <c r="E240" s="36"/>
+      <c r="F240" s="36"/>
+      <c r="G240" s="36"/>
+      <c r="H240" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="I240" s="25" t="s">
+      <c r="I240" s="37" t="s">
         <v>305</v>
       </c>
-      <c r="J240" s="50" t="s">
+      <c r="J240" s="56" t="s">
         <v>306</v>
       </c>
       <c r="K240" s="21"/>
-      <c r="L240" s="55"/>
+      <c r="L240" s="57"/>
       <c r="M240" s="6"/>
     </row>
-    <row r="241" spans="1:13" ht="15">
+    <row r="241" spans="1:13" ht="51.75">
       <c r="A241">
         <f t="shared" si="52"/>
         <v>28</v>
@@ -9660,11 +9771,31 @@
         <f t="shared" si="50"/>
         <v>3</v>
       </c>
-      <c r="C241" s="3" t="str">
+      <c r="C241" s="55" t="str">
         <f t="shared" si="51"/>
         <v>28-3</v>
       </c>
-      <c r="L241" s="6"/>
+      <c r="D241" s="23">
+        <v>1432</v>
+      </c>
+      <c r="E241" s="23"/>
+      <c r="F241" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="G241" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="H241" s="24" t="s">
+        <v>308</v>
+      </c>
+      <c r="I241" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="J241" s="50" t="s">
+        <v>310</v>
+      </c>
+      <c r="K241" s="21"/>
+      <c r="L241" s="26"/>
       <c r="M241" s="6"/>
     </row>
     <row r="242" spans="1:13" ht="15">
@@ -14709,378 +14840,393 @@
     <mergeCell ref="L239:L240"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsBlanks" dxfId="74" priority="79">
+    <cfRule type="containsBlanks" dxfId="80" priority="82">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsText" dxfId="73" priority="80" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsText" dxfId="72" priority="81" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="78" priority="84" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsBlanks" dxfId="71" priority="76">
+    <cfRule type="containsBlanks" dxfId="77" priority="79">
       <formula>LEN(TRIM(K200))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="70" priority="77" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="76" priority="80" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="69" priority="78" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="75" priority="81" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsBlanks" dxfId="68" priority="70">
+    <cfRule type="containsBlanks" dxfId="74" priority="73">
       <formula>LEN(TRIM(K201))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="72" priority="75" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsBlanks" dxfId="65" priority="67">
+    <cfRule type="containsBlanks" dxfId="71" priority="70">
       <formula>LEN(TRIM(K202))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="63" priority="69" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsBlanks" dxfId="62" priority="64">
+    <cfRule type="containsBlanks" dxfId="68" priority="67">
       <formula>LEN(TRIM(K203))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="61" priority="65" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="60" priority="66" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="59" priority="61">
+    <cfRule type="containsBlanks" dxfId="65" priority="64">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsBlanks" dxfId="58" priority="58">
+    <cfRule type="containsBlanks" dxfId="64" priority="61">
       <formula>LEN(TRIM(K207))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsBlanks" dxfId="57" priority="55">
+    <cfRule type="containsBlanks" dxfId="63" priority="58">
       <formula>LEN(TRIM(K209))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsBlanks" dxfId="56" priority="52">
+    <cfRule type="containsBlanks" dxfId="62" priority="55">
       <formula>LEN(TRIM(K210))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsBlanks" dxfId="55" priority="49">
+    <cfRule type="containsBlanks" dxfId="61" priority="52">
       <formula>LEN(TRIM(K212))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsBlanks" dxfId="54" priority="46">
+    <cfRule type="containsBlanks" dxfId="60" priority="49">
       <formula>LEN(TRIM(K214))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsBlanks" dxfId="53" priority="43">
+    <cfRule type="containsBlanks" dxfId="59" priority="46">
       <formula>LEN(TRIM(K216))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="52" priority="37">
+    <cfRule type="containsBlanks" dxfId="58" priority="40">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="51" priority="62" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="57" priority="65" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="50" priority="63" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="56" priority="66" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsBlanks" dxfId="49" priority="34">
+    <cfRule type="containsBlanks" dxfId="55" priority="37">
       <formula>LEN(TRIM(K208))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="48" priority="59" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="54" priority="62" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="47" priority="60" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="53" priority="63" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="46" priority="31">
+    <cfRule type="containsBlanks" dxfId="52" priority="34">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="45" priority="56" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="51" priority="59" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="44" priority="57" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="50" priority="60" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsBlanks" dxfId="43" priority="28">
+    <cfRule type="containsBlanks" dxfId="49" priority="31">
       <formula>LEN(TRIM(K211))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="42" priority="53" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="48" priority="56" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="41" priority="54" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="47" priority="57" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsBlanks" dxfId="40" priority="25">
+    <cfRule type="containsBlanks" dxfId="46" priority="28">
       <formula>LEN(TRIM(K213))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="39" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="45" priority="53" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="38" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="44" priority="54" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsBlanks" dxfId="37" priority="22">
+    <cfRule type="containsBlanks" dxfId="43" priority="25">
       <formula>LEN(TRIM(K215))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="36" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="42" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="41" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsText" dxfId="34" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="40" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="39" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="32" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="38" priority="41" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="31" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="37" priority="42" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="36" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="35" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="27" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="30" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsBlanks" dxfId="20" priority="19">
+    <cfRule type="containsBlanks" dxfId="26" priority="22">
       <formula>LEN(TRIM(K232))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K232))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K232))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsBlanks" dxfId="17" priority="16">
+    <cfRule type="containsBlanks" dxfId="23" priority="19">
       <formula>LEN(TRIM(K217))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsBlanks" dxfId="14" priority="13">
+    <cfRule type="containsBlanks" dxfId="20" priority="16">
       <formula>LEN(TRIM(K218))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsBlanks" dxfId="11" priority="10">
+    <cfRule type="containsBlanks" dxfId="17" priority="13">
       <formula>LEN(TRIM(K235))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsBlanks" dxfId="8" priority="7">
+    <cfRule type="containsBlanks" dxfId="14" priority="10">
       <formula>LEN(TRIM(K236))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
+    <cfRule type="containsBlanks" dxfId="11" priority="7">
       <formula>LEN(TRIM(K239))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="8" priority="4">
       <formula>LEN(TRIM(K240))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K240))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K240))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K241">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
+      <formula>LEN(TRIM(K241))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K241">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K241))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K241">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K241))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added manual system tests for script generator (Ticket 1567)
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="314">
   <si>
     <t>Test Number</t>
   </si>
@@ -938,6 +938,27 @@
   </si>
   <si>
     <t>If target is blank: Error message is shown naming the offending device screen &amp; ok button is disabled</t>
+  </si>
+  <si>
+    <t>Script Generator</t>
+  </si>
+  <si>
+    <t>Adding a row by setting the sample position to not blank fills the rest of the columns with default values</t>
+  </si>
+  <si>
+    <t>Deleting a row by setting the sample position to blank clears the rest of the columns.</t>
+  </si>
+  <si>
+    <t>Setting the sample geometry to disk links sample width and height parameters; independent otherwise.</t>
+  </si>
+  <si>
+    <t>Preview Script button brings up a popup window with a preview of the generated script.</t>
+  </si>
+  <si>
+    <t>Clear Table button clears all rows from the Table.</t>
+  </si>
+  <si>
+    <t>Write Script button allows User to write python script to a file at a chosen location.</t>
   </si>
 </sst>
 </file>
@@ -1236,24 +1257,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="81">
+  <dxfs count="105">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF4C7C3"/>
           <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
         </patternFill>
       </fill>
       <border>
@@ -1294,8 +1343,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
         </patternFill>
       </fill>
       <border>
@@ -1308,8 +1357,22 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
       <border>
@@ -1350,6 +1413,34 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFF4C7C3"/>
           <bgColor rgb="FFF4C7C3"/>
         </patternFill>
@@ -1378,6 +1469,34 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
@@ -1394,6 +1513,34 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFCE8B2"/>
           <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
       <border>
@@ -2383,6 +2530,216 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2680,11 +3037,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1071"/>
+  <dimension ref="A1:N1072"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J232" sqref="J232"/>
+      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J253" sqref="J253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -8145,7 +8502,7 @@
       </c>
       <c r="J188" s="8"/>
       <c r="K188" s="7"/>
-      <c r="L188" s="50"/>
+      <c r="L188" s="51"/>
     </row>
     <row r="189" spans="1:13" ht="30">
       <c r="A189">
@@ -8174,7 +8531,7 @@
       </c>
       <c r="J189" s="8"/>
       <c r="K189" s="7"/>
-      <c r="L189" s="51"/>
+      <c r="L189" s="52"/>
       <c r="M189" s="6"/>
     </row>
     <row r="190" spans="1:13" ht="45">
@@ -8204,7 +8561,7 @@
       </c>
       <c r="J190" s="8"/>
       <c r="K190" s="7"/>
-      <c r="L190" s="51"/>
+      <c r="L190" s="52"/>
       <c r="M190" s="6"/>
     </row>
     <row r="191" spans="1:13" ht="30">
@@ -8234,7 +8591,7 @@
       </c>
       <c r="J191" s="8"/>
       <c r="K191" s="7"/>
-      <c r="L191" s="52"/>
+      <c r="L191" s="53"/>
       <c r="M191" s="6"/>
     </row>
     <row r="192" spans="1:13" ht="30">
@@ -9537,11 +9894,11 @@
         <v>26</v>
       </c>
       <c r="B235">
-        <f t="shared" ref="B235:B298" si="50">IF(A235=A234,B234+1,1)</f>
+        <f t="shared" ref="B235:B299" si="50">IF(A235=A234,B234+1,1)</f>
         <v>1</v>
       </c>
       <c r="C235" s="3" t="str">
-        <f t="shared" ref="C235:C298" si="51">CONCATENATE(A235,"-",B235)</f>
+        <f t="shared" ref="C235:C299" si="51">CONCATENATE(A235,"-",B235)</f>
         <v>26-1</v>
       </c>
       <c r="D235" s="23"/>
@@ -9561,7 +9918,7 @@
     </row>
     <row r="236" spans="1:13" ht="15">
       <c r="A236">
-        <f t="shared" ref="A236:A299" si="52">A235</f>
+        <f t="shared" ref="A236:A300" si="52">A235</f>
         <v>26</v>
       </c>
       <c r="B236">
@@ -9691,121 +10048,181 @@
       <c r="I240" s="25" t="s">
         <v>305</v>
       </c>
-      <c r="J240" s="53" t="s">
+      <c r="J240" s="50" t="s">
         <v>306</v>
       </c>
       <c r="K240" s="21"/>
       <c r="L240" s="26"/>
       <c r="M240" s="6"/>
     </row>
-    <row r="241" spans="1:13" ht="15">
+    <row r="241" spans="1:13" ht="39">
       <c r="A241">
-        <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B241">
         <f t="shared" si="50"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C241" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-3</v>
-      </c>
-      <c r="L241" s="6"/>
+        <v>29-1</v>
+      </c>
+      <c r="D241" s="23"/>
+      <c r="E241" s="23"/>
+      <c r="F241" s="23"/>
+      <c r="G241" s="23"/>
+      <c r="H241" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="I241" s="25" t="s">
+        <v>308</v>
+      </c>
+      <c r="J241" s="50"/>
+      <c r="K241" s="21"/>
+      <c r="L241" s="26"/>
       <c r="M241" s="6"/>
     </row>
-    <row r="242" spans="1:13" ht="15">
+    <row r="242" spans="1:13" ht="26.25">
       <c r="A242">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B242">
         <f t="shared" si="50"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C242" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-4</v>
-      </c>
-      <c r="L242" s="6"/>
+        <v>29-2</v>
+      </c>
+      <c r="D242" s="23"/>
+      <c r="E242" s="23"/>
+      <c r="F242" s="23"/>
+      <c r="G242" s="23"/>
+      <c r="H242" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="I242" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="J242" s="50"/>
+      <c r="K242" s="21"/>
+      <c r="L242" s="26"/>
       <c r="M242" s="6"/>
     </row>
-    <row r="243" spans="1:13" ht="15">
+    <row r="243" spans="1:13" ht="39">
       <c r="A243">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B243">
         <f t="shared" si="50"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C243" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-5</v>
-      </c>
-      <c r="L243" s="6"/>
+        <v>29-3</v>
+      </c>
+      <c r="D243" s="23"/>
+      <c r="E243" s="23"/>
+      <c r="F243" s="23"/>
+      <c r="G243" s="23"/>
+      <c r="H243" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="I243" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="J243" s="50"/>
+      <c r="K243" s="21"/>
+      <c r="L243" s="26"/>
       <c r="M243" s="6"/>
     </row>
-    <row r="244" spans="1:13" ht="15">
+    <row r="244" spans="1:13" ht="26.25">
       <c r="A244">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B244">
         <f t="shared" si="50"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C244" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-6</v>
-      </c>
-      <c r="L244" s="6"/>
+        <v>29-4</v>
+      </c>
+      <c r="D244" s="23"/>
+      <c r="E244" s="23"/>
+      <c r="F244" s="23"/>
+      <c r="G244" s="23"/>
+      <c r="H244" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="I244" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="J244" s="50"/>
+      <c r="K244" s="21"/>
+      <c r="L244" s="26"/>
       <c r="M244" s="6"/>
     </row>
-    <row r="245" spans="1:13" ht="15">
-      <c r="A245">
-        <f t="shared" si="52"/>
-        <v>28</v>
-      </c>
-      <c r="B245">
-        <f t="shared" si="50"/>
-        <v>7</v>
-      </c>
-      <c r="C245" s="3" t="str">
-        <f t="shared" si="51"/>
-        <v>28-7</v>
-      </c>
-      <c r="L245" s="6"/>
+    <row r="245" spans="1:13" ht="26.25">
+      <c r="C245" s="3"/>
+      <c r="D245" s="23"/>
+      <c r="E245" s="23"/>
+      <c r="F245" s="23"/>
+      <c r="G245" s="23"/>
+      <c r="H245" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="I245" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="J245" s="50"/>
+      <c r="K245" s="21"/>
+      <c r="L245" s="26"/>
       <c r="M245" s="6"/>
     </row>
     <row r="246" spans="1:13" ht="15">
       <c r="A246">
-        <f t="shared" si="52"/>
-        <v>28</v>
+        <f>A244</f>
+        <v>29</v>
       </c>
       <c r="B246">
-        <f t="shared" si="50"/>
-        <v>8</v>
+        <f>IF(A246=A244,B244+1,1)</f>
+        <v>5</v>
       </c>
       <c r="C246" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-8</v>
-      </c>
-      <c r="L246" s="6"/>
+        <v>29-5</v>
+      </c>
+      <c r="D246" s="23"/>
+      <c r="E246" s="23"/>
+      <c r="F246" s="23"/>
+      <c r="G246" s="23"/>
+      <c r="H246" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="I246" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="J246" s="50"/>
+      <c r="K246" s="21"/>
+      <c r="L246" s="26"/>
       <c r="M246" s="6"/>
     </row>
     <row r="247" spans="1:13" ht="15">
       <c r="A247">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B247">
         <f t="shared" si="50"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C247" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-9</v>
+        <v>29-6</v>
       </c>
       <c r="L247" s="6"/>
       <c r="M247" s="6"/>
@@ -9813,15 +10230,15 @@
     <row r="248" spans="1:13" ht="15">
       <c r="A248">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B248">
         <f t="shared" si="50"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C248" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-10</v>
+        <v>29-7</v>
       </c>
       <c r="L248" s="6"/>
       <c r="M248" s="6"/>
@@ -9829,15 +10246,15 @@
     <row r="249" spans="1:13" ht="15">
       <c r="A249">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B249">
         <f t="shared" si="50"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C249" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-11</v>
+        <v>29-8</v>
       </c>
       <c r="L249" s="6"/>
       <c r="M249" s="6"/>
@@ -9845,15 +10262,15 @@
     <row r="250" spans="1:13" ht="15">
       <c r="A250">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B250">
         <f t="shared" si="50"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C250" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-12</v>
+        <v>29-9</v>
       </c>
       <c r="L250" s="6"/>
       <c r="M250" s="6"/>
@@ -9861,15 +10278,15 @@
     <row r="251" spans="1:13" ht="15">
       <c r="A251">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B251">
         <f t="shared" si="50"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C251" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-13</v>
+        <v>29-10</v>
       </c>
       <c r="L251" s="6"/>
       <c r="M251" s="6"/>
@@ -9877,15 +10294,15 @@
     <row r="252" spans="1:13" ht="15">
       <c r="A252">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B252">
         <f t="shared" si="50"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C252" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-14</v>
+        <v>29-11</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
@@ -9893,15 +10310,15 @@
     <row r="253" spans="1:13" ht="15">
       <c r="A253">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B253">
         <f t="shared" si="50"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C253" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-15</v>
+        <v>29-12</v>
       </c>
       <c r="L253" s="6"/>
       <c r="M253" s="6"/>
@@ -9909,15 +10326,15 @@
     <row r="254" spans="1:13" ht="15">
       <c r="A254">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B254">
         <f t="shared" si="50"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C254" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-16</v>
+        <v>29-13</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
@@ -9925,15 +10342,15 @@
     <row r="255" spans="1:13" ht="15">
       <c r="A255">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B255">
         <f t="shared" si="50"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C255" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-17</v>
+        <v>29-14</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
@@ -9941,15 +10358,15 @@
     <row r="256" spans="1:13" ht="15">
       <c r="A256">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B256">
         <f t="shared" si="50"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C256" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-18</v>
+        <v>29-15</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
@@ -9957,15 +10374,15 @@
     <row r="257" spans="1:13" ht="15">
       <c r="A257">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B257">
         <f t="shared" si="50"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C257" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-19</v>
+        <v>29-16</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
@@ -9973,15 +10390,15 @@
     <row r="258" spans="1:13" ht="15">
       <c r="A258">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B258">
         <f t="shared" si="50"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C258" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-20</v>
+        <v>29-17</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
@@ -9989,15 +10406,15 @@
     <row r="259" spans="1:13" ht="15">
       <c r="A259">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B259">
         <f t="shared" si="50"/>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C259" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-21</v>
+        <v>29-18</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
@@ -10005,15 +10422,15 @@
     <row r="260" spans="1:13" ht="15">
       <c r="A260">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B260">
         <f t="shared" si="50"/>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C260" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-22</v>
+        <v>29-19</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
@@ -10021,15 +10438,15 @@
     <row r="261" spans="1:13" ht="15">
       <c r="A261">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B261">
         <f t="shared" si="50"/>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C261" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-23</v>
+        <v>29-20</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
@@ -10037,15 +10454,15 @@
     <row r="262" spans="1:13" ht="15">
       <c r="A262">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B262">
         <f t="shared" si="50"/>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C262" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-24</v>
+        <v>29-21</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
@@ -10053,15 +10470,15 @@
     <row r="263" spans="1:13" ht="15">
       <c r="A263">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B263">
         <f t="shared" si="50"/>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C263" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-25</v>
+        <v>29-22</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
@@ -10069,15 +10486,15 @@
     <row r="264" spans="1:13" ht="15">
       <c r="A264">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B264">
         <f t="shared" si="50"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C264" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-26</v>
+        <v>29-23</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
@@ -10085,15 +10502,15 @@
     <row r="265" spans="1:13" ht="15">
       <c r="A265">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B265">
         <f t="shared" si="50"/>
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C265" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-27</v>
+        <v>29-24</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
@@ -10101,15 +10518,15 @@
     <row r="266" spans="1:13" ht="15">
       <c r="A266">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B266">
         <f t="shared" si="50"/>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C266" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-28</v>
+        <v>29-25</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
@@ -10117,15 +10534,15 @@
     <row r="267" spans="1:13" ht="15">
       <c r="A267">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B267">
         <f t="shared" si="50"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C267" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-29</v>
+        <v>29-26</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
@@ -10133,15 +10550,15 @@
     <row r="268" spans="1:13" ht="15">
       <c r="A268">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B268">
         <f t="shared" si="50"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C268" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-30</v>
+        <v>29-27</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
@@ -10149,15 +10566,15 @@
     <row r="269" spans="1:13" ht="15">
       <c r="A269">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B269">
         <f t="shared" si="50"/>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C269" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-31</v>
+        <v>29-28</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
@@ -10165,15 +10582,15 @@
     <row r="270" spans="1:13" ht="15">
       <c r="A270">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B270">
         <f t="shared" si="50"/>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C270" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-32</v>
+        <v>29-29</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
@@ -10181,15 +10598,15 @@
     <row r="271" spans="1:13" ht="15">
       <c r="A271">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B271">
         <f t="shared" si="50"/>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C271" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-33</v>
+        <v>29-30</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
@@ -10197,15 +10614,15 @@
     <row r="272" spans="1:13" ht="15">
       <c r="A272">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B272">
         <f t="shared" si="50"/>
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C272" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-34</v>
+        <v>29-31</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
@@ -10213,15 +10630,15 @@
     <row r="273" spans="1:13" ht="15">
       <c r="A273">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B273">
         <f t="shared" si="50"/>
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C273" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-35</v>
+        <v>29-32</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
@@ -10229,15 +10646,15 @@
     <row r="274" spans="1:13" ht="15">
       <c r="A274">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B274">
         <f t="shared" si="50"/>
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C274" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-36</v>
+        <v>29-33</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
@@ -10245,15 +10662,15 @@
     <row r="275" spans="1:13" ht="15">
       <c r="A275">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B275">
         <f t="shared" si="50"/>
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C275" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-37</v>
+        <v>29-34</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
@@ -10261,15 +10678,15 @@
     <row r="276" spans="1:13" ht="15">
       <c r="A276">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B276">
         <f t="shared" si="50"/>
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C276" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-38</v>
+        <v>29-35</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
@@ -10277,15 +10694,15 @@
     <row r="277" spans="1:13" ht="15">
       <c r="A277">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B277">
         <f t="shared" si="50"/>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C277" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-39</v>
+        <v>29-36</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
@@ -10293,15 +10710,15 @@
     <row r="278" spans="1:13" ht="15">
       <c r="A278">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B278">
         <f t="shared" si="50"/>
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C278" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-40</v>
+        <v>29-37</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
@@ -10309,15 +10726,15 @@
     <row r="279" spans="1:13" ht="15">
       <c r="A279">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B279">
         <f t="shared" si="50"/>
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C279" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-41</v>
+        <v>29-38</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
@@ -10325,15 +10742,15 @@
     <row r="280" spans="1:13" ht="15">
       <c r="A280">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B280">
         <f t="shared" si="50"/>
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C280" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-42</v>
+        <v>29-39</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
@@ -10341,15 +10758,15 @@
     <row r="281" spans="1:13" ht="15">
       <c r="A281">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B281">
         <f t="shared" si="50"/>
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C281" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-43</v>
+        <v>29-40</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
@@ -10357,15 +10774,15 @@
     <row r="282" spans="1:13" ht="15">
       <c r="A282">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B282">
         <f t="shared" si="50"/>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C282" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-44</v>
+        <v>29-41</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
@@ -10373,15 +10790,15 @@
     <row r="283" spans="1:13" ht="15">
       <c r="A283">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B283">
         <f t="shared" si="50"/>
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C283" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-45</v>
+        <v>29-42</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
@@ -10389,15 +10806,15 @@
     <row r="284" spans="1:13" ht="15">
       <c r="A284">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B284">
         <f t="shared" si="50"/>
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C284" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-46</v>
+        <v>29-43</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
@@ -10405,15 +10822,15 @@
     <row r="285" spans="1:13" ht="15">
       <c r="A285">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B285">
         <f t="shared" si="50"/>
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C285" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-47</v>
+        <v>29-44</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
@@ -10421,15 +10838,15 @@
     <row r="286" spans="1:13" ht="15">
       <c r="A286">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B286">
         <f t="shared" si="50"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C286" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-48</v>
+        <v>29-45</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
@@ -10437,15 +10854,15 @@
     <row r="287" spans="1:13" ht="15">
       <c r="A287">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B287">
         <f t="shared" si="50"/>
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C287" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-49</v>
+        <v>29-46</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
@@ -10453,15 +10870,15 @@
     <row r="288" spans="1:13" ht="15">
       <c r="A288">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B288">
         <f t="shared" si="50"/>
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C288" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-50</v>
+        <v>29-47</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
@@ -10469,15 +10886,15 @@
     <row r="289" spans="1:13" ht="15">
       <c r="A289">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B289">
         <f t="shared" si="50"/>
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C289" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-51</v>
+        <v>29-48</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
@@ -10485,15 +10902,15 @@
     <row r="290" spans="1:13" ht="15">
       <c r="A290">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B290">
         <f t="shared" si="50"/>
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C290" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-52</v>
+        <v>29-49</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
@@ -10501,15 +10918,15 @@
     <row r="291" spans="1:13" ht="15">
       <c r="A291">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B291">
         <f t="shared" si="50"/>
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C291" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-53</v>
+        <v>29-50</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
@@ -10517,15 +10934,15 @@
     <row r="292" spans="1:13" ht="15">
       <c r="A292">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B292">
         <f t="shared" si="50"/>
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C292" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-54</v>
+        <v>29-51</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
@@ -10533,15 +10950,15 @@
     <row r="293" spans="1:13" ht="15">
       <c r="A293">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B293">
         <f t="shared" si="50"/>
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C293" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-55</v>
+        <v>29-52</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
@@ -10549,15 +10966,15 @@
     <row r="294" spans="1:13" ht="15">
       <c r="A294">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B294">
         <f t="shared" si="50"/>
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C294" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-56</v>
+        <v>29-53</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
@@ -10565,15 +10982,15 @@
     <row r="295" spans="1:13" ht="15">
       <c r="A295">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B295">
         <f t="shared" si="50"/>
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C295" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-57</v>
+        <v>29-54</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
@@ -10581,15 +10998,15 @@
     <row r="296" spans="1:13" ht="15">
       <c r="A296">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B296">
         <f t="shared" si="50"/>
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C296" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-58</v>
+        <v>29-55</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
@@ -10597,15 +11014,15 @@
     <row r="297" spans="1:13" ht="15">
       <c r="A297">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B297">
         <f t="shared" si="50"/>
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C297" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-59</v>
+        <v>29-56</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
@@ -10613,15 +11030,15 @@
     <row r="298" spans="1:13" ht="15">
       <c r="A298">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B298">
         <f t="shared" si="50"/>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C298" s="3" t="str">
         <f t="shared" si="51"/>
-        <v>28-60</v>
+        <v>29-57</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
@@ -10629,47 +11046,47 @@
     <row r="299" spans="1:13" ht="15">
       <c r="A299">
         <f t="shared" si="52"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B299">
-        <f t="shared" ref="B299:B362" si="53">IF(A299=A298,B298+1,1)</f>
-        <v>61</v>
+        <f t="shared" si="50"/>
+        <v>58</v>
       </c>
       <c r="C299" s="3" t="str">
-        <f t="shared" ref="C299:C362" si="54">CONCATENATE(A299,"-",B299)</f>
-        <v>28-61</v>
+        <f t="shared" si="51"/>
+        <v>29-58</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
     </row>
     <row r="300" spans="1:13" ht="15">
       <c r="A300">
-        <f t="shared" ref="A300:A363" si="55">A299</f>
-        <v>28</v>
+        <f t="shared" si="52"/>
+        <v>29</v>
       </c>
       <c r="B300">
-        <f t="shared" si="53"/>
-        <v>62</v>
+        <f t="shared" ref="B300:B363" si="53">IF(A300=A299,B299+1,1)</f>
+        <v>59</v>
       </c>
       <c r="C300" s="3" t="str">
-        <f t="shared" si="54"/>
-        <v>28-62</v>
+        <f t="shared" ref="C300:C363" si="54">CONCATENATE(A300,"-",B300)</f>
+        <v>29-59</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
     </row>
     <row r="301" spans="1:13" ht="15">
       <c r="A301">
-        <f t="shared" si="55"/>
-        <v>28</v>
+        <f t="shared" ref="A301:A364" si="55">A300</f>
+        <v>29</v>
       </c>
       <c r="B301">
         <f t="shared" si="53"/>
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C301" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-63</v>
+        <v>29-60</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
@@ -10677,15 +11094,15 @@
     <row r="302" spans="1:13" ht="15">
       <c r="A302">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B302">
         <f t="shared" si="53"/>
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C302" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-64</v>
+        <v>29-61</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
@@ -10693,15 +11110,15 @@
     <row r="303" spans="1:13" ht="15">
       <c r="A303">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B303">
         <f t="shared" si="53"/>
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C303" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-65</v>
+        <v>29-62</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
@@ -10709,15 +11126,15 @@
     <row r="304" spans="1:13" ht="15">
       <c r="A304">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B304">
         <f t="shared" si="53"/>
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C304" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-66</v>
+        <v>29-63</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
@@ -10725,15 +11142,15 @@
     <row r="305" spans="1:13" ht="15">
       <c r="A305">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B305">
         <f t="shared" si="53"/>
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C305" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-67</v>
+        <v>29-64</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
@@ -10741,15 +11158,15 @@
     <row r="306" spans="1:13" ht="15">
       <c r="A306">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B306">
         <f t="shared" si="53"/>
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C306" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-68</v>
+        <v>29-65</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
@@ -10757,15 +11174,15 @@
     <row r="307" spans="1:13" ht="15">
       <c r="A307">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B307">
         <f t="shared" si="53"/>
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C307" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-69</v>
+        <v>29-66</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
@@ -10773,15 +11190,15 @@
     <row r="308" spans="1:13" ht="15">
       <c r="A308">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B308">
         <f t="shared" si="53"/>
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C308" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-70</v>
+        <v>29-67</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
@@ -10789,15 +11206,15 @@
     <row r="309" spans="1:13" ht="15">
       <c r="A309">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B309">
         <f t="shared" si="53"/>
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C309" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-71</v>
+        <v>29-68</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
@@ -10805,15 +11222,15 @@
     <row r="310" spans="1:13" ht="15">
       <c r="A310">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B310">
         <f t="shared" si="53"/>
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C310" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-72</v>
+        <v>29-69</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
@@ -10821,15 +11238,15 @@
     <row r="311" spans="1:13" ht="15">
       <c r="A311">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B311">
         <f t="shared" si="53"/>
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C311" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-73</v>
+        <v>29-70</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
@@ -10837,15 +11254,15 @@
     <row r="312" spans="1:13" ht="15">
       <c r="A312">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B312">
         <f t="shared" si="53"/>
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C312" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-74</v>
+        <v>29-71</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
@@ -10853,15 +11270,15 @@
     <row r="313" spans="1:13" ht="15">
       <c r="A313">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B313">
         <f t="shared" si="53"/>
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C313" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-75</v>
+        <v>29-72</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
@@ -10869,15 +11286,15 @@
     <row r="314" spans="1:13" ht="15">
       <c r="A314">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B314">
         <f t="shared" si="53"/>
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C314" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-76</v>
+        <v>29-73</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
@@ -10885,15 +11302,15 @@
     <row r="315" spans="1:13" ht="15">
       <c r="A315">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B315">
         <f t="shared" si="53"/>
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C315" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-77</v>
+        <v>29-74</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
@@ -10901,15 +11318,15 @@
     <row r="316" spans="1:13" ht="15">
       <c r="A316">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B316">
         <f t="shared" si="53"/>
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C316" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-78</v>
+        <v>29-75</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
@@ -10917,15 +11334,15 @@
     <row r="317" spans="1:13" ht="15">
       <c r="A317">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B317">
         <f t="shared" si="53"/>
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C317" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-79</v>
+        <v>29-76</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
@@ -10933,15 +11350,15 @@
     <row r="318" spans="1:13" ht="15">
       <c r="A318">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B318">
         <f t="shared" si="53"/>
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C318" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-80</v>
+        <v>29-77</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
@@ -10949,15 +11366,15 @@
     <row r="319" spans="1:13" ht="15">
       <c r="A319">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B319">
         <f t="shared" si="53"/>
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C319" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-81</v>
+        <v>29-78</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
@@ -10965,15 +11382,15 @@
     <row r="320" spans="1:13" ht="15">
       <c r="A320">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B320">
         <f t="shared" si="53"/>
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C320" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-82</v>
+        <v>29-79</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
@@ -10981,15 +11398,15 @@
     <row r="321" spans="1:13" ht="15">
       <c r="A321">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B321">
         <f t="shared" si="53"/>
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C321" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-83</v>
+        <v>29-80</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
@@ -10997,15 +11414,15 @@
     <row r="322" spans="1:13" ht="15">
       <c r="A322">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B322">
         <f t="shared" si="53"/>
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C322" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-84</v>
+        <v>29-81</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
@@ -11013,15 +11430,15 @@
     <row r="323" spans="1:13" ht="15">
       <c r="A323">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B323">
         <f t="shared" si="53"/>
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C323" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-85</v>
+        <v>29-82</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
@@ -11029,15 +11446,15 @@
     <row r="324" spans="1:13" ht="15">
       <c r="A324">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B324">
         <f t="shared" si="53"/>
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C324" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-86</v>
+        <v>29-83</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
@@ -11045,15 +11462,15 @@
     <row r="325" spans="1:13" ht="15">
       <c r="A325">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B325">
         <f t="shared" si="53"/>
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C325" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-87</v>
+        <v>29-84</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
@@ -11061,15 +11478,15 @@
     <row r="326" spans="1:13" ht="15">
       <c r="A326">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B326">
         <f t="shared" si="53"/>
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C326" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-88</v>
+        <v>29-85</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
@@ -11077,15 +11494,15 @@
     <row r="327" spans="1:13" ht="15">
       <c r="A327">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B327">
         <f t="shared" si="53"/>
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C327" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-89</v>
+        <v>29-86</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
@@ -11093,15 +11510,15 @@
     <row r="328" spans="1:13" ht="15">
       <c r="A328">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B328">
         <f t="shared" si="53"/>
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C328" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-90</v>
+        <v>29-87</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
@@ -11109,15 +11526,15 @@
     <row r="329" spans="1:13" ht="15">
       <c r="A329">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B329">
         <f t="shared" si="53"/>
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C329" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-91</v>
+        <v>29-88</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
@@ -11125,15 +11542,15 @@
     <row r="330" spans="1:13" ht="15">
       <c r="A330">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B330">
         <f t="shared" si="53"/>
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C330" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-92</v>
+        <v>29-89</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
@@ -11141,15 +11558,15 @@
     <row r="331" spans="1:13" ht="15">
       <c r="A331">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B331">
         <f t="shared" si="53"/>
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C331" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-93</v>
+        <v>29-90</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
@@ -11157,15 +11574,15 @@
     <row r="332" spans="1:13" ht="15">
       <c r="A332">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B332">
         <f t="shared" si="53"/>
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C332" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-94</v>
+        <v>29-91</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
@@ -11173,15 +11590,15 @@
     <row r="333" spans="1:13" ht="15">
       <c r="A333">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B333">
         <f t="shared" si="53"/>
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C333" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-95</v>
+        <v>29-92</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
@@ -11189,15 +11606,15 @@
     <row r="334" spans="1:13" ht="15">
       <c r="A334">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B334">
         <f t="shared" si="53"/>
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C334" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-96</v>
+        <v>29-93</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
@@ -11205,15 +11622,15 @@
     <row r="335" spans="1:13" ht="15">
       <c r="A335">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B335">
         <f t="shared" si="53"/>
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C335" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-97</v>
+        <v>29-94</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
@@ -11221,15 +11638,15 @@
     <row r="336" spans="1:13" ht="15">
       <c r="A336">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B336">
         <f t="shared" si="53"/>
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C336" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-98</v>
+        <v>29-95</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
@@ -11237,15 +11654,15 @@
     <row r="337" spans="1:13" ht="15">
       <c r="A337">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B337">
         <f t="shared" si="53"/>
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C337" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-99</v>
+        <v>29-96</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
@@ -11253,15 +11670,15 @@
     <row r="338" spans="1:13" ht="15">
       <c r="A338">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B338">
         <f t="shared" si="53"/>
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C338" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-100</v>
+        <v>29-97</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
@@ -11269,15 +11686,15 @@
     <row r="339" spans="1:13" ht="15">
       <c r="A339">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B339">
         <f t="shared" si="53"/>
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C339" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-101</v>
+        <v>29-98</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
@@ -11285,15 +11702,15 @@
     <row r="340" spans="1:13" ht="15">
       <c r="A340">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B340">
         <f t="shared" si="53"/>
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C340" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-102</v>
+        <v>29-99</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
@@ -11301,15 +11718,15 @@
     <row r="341" spans="1:13" ht="15">
       <c r="A341">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B341">
         <f t="shared" si="53"/>
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C341" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-103</v>
+        <v>29-100</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
@@ -11317,15 +11734,15 @@
     <row r="342" spans="1:13" ht="15">
       <c r="A342">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B342">
         <f t="shared" si="53"/>
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C342" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-104</v>
+        <v>29-101</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
@@ -11333,15 +11750,15 @@
     <row r="343" spans="1:13" ht="15">
       <c r="A343">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B343">
         <f t="shared" si="53"/>
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C343" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-105</v>
+        <v>29-102</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
@@ -11349,15 +11766,15 @@
     <row r="344" spans="1:13" ht="15">
       <c r="A344">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B344">
         <f t="shared" si="53"/>
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C344" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-106</v>
+        <v>29-103</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
@@ -11365,15 +11782,15 @@
     <row r="345" spans="1:13" ht="15">
       <c r="A345">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B345">
         <f t="shared" si="53"/>
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C345" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-107</v>
+        <v>29-104</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
@@ -11381,15 +11798,15 @@
     <row r="346" spans="1:13" ht="15">
       <c r="A346">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B346">
         <f t="shared" si="53"/>
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C346" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-108</v>
+        <v>29-105</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
@@ -11397,15 +11814,15 @@
     <row r="347" spans="1:13" ht="15">
       <c r="A347">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B347">
         <f t="shared" si="53"/>
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C347" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-109</v>
+        <v>29-106</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
@@ -11413,15 +11830,15 @@
     <row r="348" spans="1:13" ht="15">
       <c r="A348">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B348">
         <f t="shared" si="53"/>
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C348" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-110</v>
+        <v>29-107</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
@@ -11429,15 +11846,15 @@
     <row r="349" spans="1:13" ht="15">
       <c r="A349">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B349">
         <f t="shared" si="53"/>
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C349" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-111</v>
+        <v>29-108</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
@@ -11445,15 +11862,15 @@
     <row r="350" spans="1:13" ht="15">
       <c r="A350">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B350">
         <f t="shared" si="53"/>
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C350" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-112</v>
+        <v>29-109</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
@@ -11461,15 +11878,15 @@
     <row r="351" spans="1:13" ht="15">
       <c r="A351">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B351">
         <f t="shared" si="53"/>
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C351" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-113</v>
+        <v>29-110</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
@@ -11477,15 +11894,15 @@
     <row r="352" spans="1:13" ht="15">
       <c r="A352">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B352">
         <f t="shared" si="53"/>
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C352" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-114</v>
+        <v>29-111</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
@@ -11493,15 +11910,15 @@
     <row r="353" spans="1:13" ht="15">
       <c r="A353">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B353">
         <f t="shared" si="53"/>
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C353" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-115</v>
+        <v>29-112</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
@@ -11509,15 +11926,15 @@
     <row r="354" spans="1:13" ht="15">
       <c r="A354">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B354">
         <f t="shared" si="53"/>
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C354" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-116</v>
+        <v>29-113</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
@@ -11525,15 +11942,15 @@
     <row r="355" spans="1:13" ht="15">
       <c r="A355">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B355">
         <f t="shared" si="53"/>
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C355" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-117</v>
+        <v>29-114</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
@@ -11541,15 +11958,15 @@
     <row r="356" spans="1:13" ht="15">
       <c r="A356">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B356">
         <f t="shared" si="53"/>
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C356" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-118</v>
+        <v>29-115</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
@@ -11557,15 +11974,15 @@
     <row r="357" spans="1:13" ht="15">
       <c r="A357">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B357">
         <f t="shared" si="53"/>
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C357" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-119</v>
+        <v>29-116</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
@@ -11573,15 +11990,15 @@
     <row r="358" spans="1:13" ht="15">
       <c r="A358">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B358">
         <f t="shared" si="53"/>
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C358" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-120</v>
+        <v>29-117</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
@@ -11589,15 +12006,15 @@
     <row r="359" spans="1:13" ht="15">
       <c r="A359">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B359">
         <f t="shared" si="53"/>
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C359" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-121</v>
+        <v>29-118</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
@@ -11605,15 +12022,15 @@
     <row r="360" spans="1:13" ht="15">
       <c r="A360">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B360">
         <f t="shared" si="53"/>
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C360" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-122</v>
+        <v>29-119</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
@@ -11621,15 +12038,15 @@
     <row r="361" spans="1:13" ht="15">
       <c r="A361">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B361">
         <f t="shared" si="53"/>
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C361" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-123</v>
+        <v>29-120</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
@@ -11637,15 +12054,15 @@
     <row r="362" spans="1:13" ht="15">
       <c r="A362">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B362">
         <f t="shared" si="53"/>
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C362" s="3" t="str">
         <f t="shared" si="54"/>
-        <v>28-124</v>
+        <v>29-121</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
@@ -11653,47 +12070,47 @@
     <row r="363" spans="1:13" ht="15">
       <c r="A363">
         <f t="shared" si="55"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B363">
-        <f t="shared" ref="B363:B384" si="56">IF(A363=A362,B362+1,1)</f>
-        <v>125</v>
+        <f t="shared" si="53"/>
+        <v>122</v>
       </c>
       <c r="C363" s="3" t="str">
-        <f t="shared" ref="C363:C384" si="57">CONCATENATE(A363,"-",B363)</f>
-        <v>28-125</v>
+        <f t="shared" si="54"/>
+        <v>29-122</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
     </row>
     <row r="364" spans="1:13" ht="15">
       <c r="A364">
-        <f t="shared" ref="A364:A384" si="58">A363</f>
-        <v>28</v>
+        <f t="shared" si="55"/>
+        <v>29</v>
       </c>
       <c r="B364">
-        <f t="shared" si="56"/>
-        <v>126</v>
+        <f t="shared" ref="B364:B385" si="56">IF(A364=A363,B363+1,1)</f>
+        <v>123</v>
       </c>
       <c r="C364" s="3" t="str">
-        <f t="shared" si="57"/>
-        <v>28-126</v>
+        <f t="shared" ref="C364:C385" si="57">CONCATENATE(A364,"-",B364)</f>
+        <v>29-123</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
     </row>
     <row r="365" spans="1:13" ht="15">
       <c r="A365">
-        <f t="shared" si="58"/>
-        <v>28</v>
+        <f t="shared" ref="A365:A385" si="58">A364</f>
+        <v>29</v>
       </c>
       <c r="B365">
         <f t="shared" si="56"/>
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C365" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-127</v>
+        <v>29-124</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
@@ -11701,15 +12118,15 @@
     <row r="366" spans="1:13" ht="15">
       <c r="A366">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B366">
         <f t="shared" si="56"/>
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C366" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-128</v>
+        <v>29-125</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
@@ -11717,15 +12134,15 @@
     <row r="367" spans="1:13" ht="15">
       <c r="A367">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B367">
         <f t="shared" si="56"/>
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C367" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-129</v>
+        <v>29-126</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
@@ -11733,15 +12150,15 @@
     <row r="368" spans="1:13" ht="15">
       <c r="A368">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B368">
         <f t="shared" si="56"/>
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C368" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-130</v>
+        <v>29-127</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
@@ -11749,15 +12166,15 @@
     <row r="369" spans="1:13" ht="15">
       <c r="A369">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B369">
         <f t="shared" si="56"/>
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C369" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-131</v>
+        <v>29-128</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
@@ -11765,15 +12182,15 @@
     <row r="370" spans="1:13" ht="15">
       <c r="A370">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B370">
         <f t="shared" si="56"/>
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C370" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-132</v>
+        <v>29-129</v>
       </c>
       <c r="L370" s="6"/>
       <c r="M370" s="6"/>
@@ -11781,15 +12198,15 @@
     <row r="371" spans="1:13" ht="15">
       <c r="A371">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B371">
         <f t="shared" si="56"/>
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C371" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-133</v>
+        <v>29-130</v>
       </c>
       <c r="L371" s="6"/>
       <c r="M371" s="6"/>
@@ -11797,15 +12214,15 @@
     <row r="372" spans="1:13" ht="15">
       <c r="A372">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B372">
         <f t="shared" si="56"/>
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C372" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-134</v>
+        <v>29-131</v>
       </c>
       <c r="L372" s="6"/>
       <c r="M372" s="6"/>
@@ -11813,15 +12230,15 @@
     <row r="373" spans="1:13" ht="15">
       <c r="A373">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B373">
         <f t="shared" si="56"/>
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C373" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-135</v>
+        <v>29-132</v>
       </c>
       <c r="L373" s="6"/>
       <c r="M373" s="6"/>
@@ -11829,15 +12246,15 @@
     <row r="374" spans="1:13" ht="15">
       <c r="A374">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B374">
         <f t="shared" si="56"/>
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C374" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-136</v>
+        <v>29-133</v>
       </c>
       <c r="L374" s="6"/>
       <c r="M374" s="6"/>
@@ -11845,15 +12262,15 @@
     <row r="375" spans="1:13" ht="15">
       <c r="A375">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B375">
         <f t="shared" si="56"/>
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C375" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-137</v>
+        <v>29-134</v>
       </c>
       <c r="L375" s="6"/>
       <c r="M375" s="6"/>
@@ -11861,15 +12278,15 @@
     <row r="376" spans="1:13" ht="15">
       <c r="A376">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B376">
         <f t="shared" si="56"/>
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C376" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-138</v>
+        <v>29-135</v>
       </c>
       <c r="L376" s="6"/>
       <c r="M376" s="6"/>
@@ -11877,15 +12294,15 @@
     <row r="377" spans="1:13" ht="15">
       <c r="A377">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B377">
         <f t="shared" si="56"/>
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C377" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-139</v>
+        <v>29-136</v>
       </c>
       <c r="L377" s="6"/>
       <c r="M377" s="6"/>
@@ -11893,15 +12310,15 @@
     <row r="378" spans="1:13" ht="15">
       <c r="A378">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B378">
         <f t="shared" si="56"/>
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C378" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-140</v>
+        <v>29-137</v>
       </c>
       <c r="L378" s="6"/>
       <c r="M378" s="6"/>
@@ -11909,15 +12326,15 @@
     <row r="379" spans="1:13" ht="15">
       <c r="A379">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B379">
         <f t="shared" si="56"/>
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C379" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-141</v>
+        <v>29-138</v>
       </c>
       <c r="L379" s="6"/>
       <c r="M379" s="6"/>
@@ -11925,15 +12342,15 @@
     <row r="380" spans="1:13" ht="15">
       <c r="A380">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B380">
         <f t="shared" si="56"/>
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C380" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-142</v>
+        <v>29-139</v>
       </c>
       <c r="L380" s="6"/>
       <c r="M380" s="6"/>
@@ -11941,15 +12358,15 @@
     <row r="381" spans="1:13" ht="15">
       <c r="A381">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B381">
         <f t="shared" si="56"/>
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C381" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-143</v>
+        <v>29-140</v>
       </c>
       <c r="L381" s="6"/>
       <c r="M381" s="6"/>
@@ -11957,15 +12374,15 @@
     <row r="382" spans="1:13" ht="15">
       <c r="A382">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B382">
         <f t="shared" si="56"/>
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C382" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-144</v>
+        <v>29-141</v>
       </c>
       <c r="L382" s="6"/>
       <c r="M382" s="6"/>
@@ -11973,15 +12390,15 @@
     <row r="383" spans="1:13" ht="15">
       <c r="A383">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B383">
         <f t="shared" si="56"/>
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C383" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-145</v>
+        <v>29-142</v>
       </c>
       <c r="L383" s="6"/>
       <c r="M383" s="6"/>
@@ -11989,80 +12406,92 @@
     <row r="384" spans="1:13" ht="15">
       <c r="A384">
         <f t="shared" si="58"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B384">
         <f t="shared" si="56"/>
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C384" s="3" t="str">
         <f t="shared" si="57"/>
-        <v>28-146</v>
+        <v>29-143</v>
       </c>
       <c r="L384" s="6"/>
       <c r="M384" s="6"/>
     </row>
-    <row r="385" spans="12:13" ht="12.75">
+    <row r="385" spans="1:13" ht="15">
+      <c r="A385">
+        <f t="shared" si="58"/>
+        <v>29</v>
+      </c>
+      <c r="B385">
+        <f t="shared" si="56"/>
+        <v>144</v>
+      </c>
+      <c r="C385" s="3" t="str">
+        <f t="shared" si="57"/>
+        <v>29-144</v>
+      </c>
       <c r="L385" s="6"/>
       <c r="M385" s="6"/>
     </row>
-    <row r="386" spans="12:13" ht="12.75">
+    <row r="386" spans="1:13" ht="12.75">
       <c r="L386" s="6"/>
       <c r="M386" s="6"/>
     </row>
-    <row r="387" spans="12:13" ht="12.75">
+    <row r="387" spans="1:13" ht="12.75">
       <c r="L387" s="6"/>
       <c r="M387" s="6"/>
     </row>
-    <row r="388" spans="12:13" ht="12.75">
+    <row r="388" spans="1:13" ht="12.75">
       <c r="L388" s="6"/>
       <c r="M388" s="6"/>
     </row>
-    <row r="389" spans="12:13" ht="12.75">
+    <row r="389" spans="1:13" ht="12.75">
       <c r="L389" s="6"/>
       <c r="M389" s="6"/>
     </row>
-    <row r="390" spans="12:13" ht="12.75">
+    <row r="390" spans="1:13" ht="12.75">
       <c r="L390" s="6"/>
       <c r="M390" s="6"/>
     </row>
-    <row r="391" spans="12:13" ht="12.75">
+    <row r="391" spans="1:13" ht="12.75">
       <c r="L391" s="6"/>
       <c r="M391" s="6"/>
     </row>
-    <row r="392" spans="12:13" ht="12.75">
+    <row r="392" spans="1:13" ht="12.75">
       <c r="L392" s="6"/>
       <c r="M392" s="6"/>
     </row>
-    <row r="393" spans="12:13" ht="12.75">
+    <row r="393" spans="1:13" ht="12.75">
       <c r="L393" s="6"/>
       <c r="M393" s="6"/>
     </row>
-    <row r="394" spans="12:13" ht="12.75">
+    <row r="394" spans="1:13" ht="12.75">
       <c r="L394" s="6"/>
       <c r="M394" s="6"/>
     </row>
-    <row r="395" spans="12:13" ht="12.75">
+    <row r="395" spans="1:13" ht="12.75">
       <c r="L395" s="6"/>
       <c r="M395" s="6"/>
     </row>
-    <row r="396" spans="12:13" ht="12.75">
+    <row r="396" spans="1:13" ht="12.75">
       <c r="L396" s="6"/>
       <c r="M396" s="6"/>
     </row>
-    <row r="397" spans="12:13" ht="12.75">
+    <row r="397" spans="1:13" ht="12.75">
       <c r="L397" s="6"/>
       <c r="M397" s="6"/>
     </row>
-    <row r="398" spans="12:13" ht="12.75">
+    <row r="398" spans="1:13" ht="12.75">
       <c r="L398" s="6"/>
       <c r="M398" s="6"/>
     </row>
-    <row r="399" spans="12:13" ht="12.75">
+    <row r="399" spans="1:13" ht="12.75">
       <c r="L399" s="6"/>
       <c r="M399" s="6"/>
     </row>
-    <row r="400" spans="12:13" ht="12.75">
+    <row r="400" spans="1:13" ht="12.75">
       <c r="L400" s="6"/>
       <c r="M400" s="6"/>
     </row>
@@ -14749,384 +15178,463 @@
     <row r="1071" spans="12:13" ht="12.75">
       <c r="L1071" s="6"/>
       <c r="M1071" s="6"/>
+    </row>
+    <row r="1072" spans="12:13" ht="12.75">
+      <c r="L1072" s="6"/>
+      <c r="M1072" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="L188:L191"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsBlanks" dxfId="80" priority="79">
+    <cfRule type="containsBlanks" dxfId="89" priority="94">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="88" priority="95" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K199">
-    <cfRule type="containsText" dxfId="78" priority="81" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="87" priority="96" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsBlanks" dxfId="77" priority="76">
+    <cfRule type="containsBlanks" dxfId="86" priority="91">
       <formula>LEN(TRIM(K200))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="85" priority="92" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K200">
-    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="84" priority="93" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K200))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsBlanks" dxfId="74" priority="70">
+    <cfRule type="containsBlanks" dxfId="83" priority="85">
       <formula>LEN(TRIM(K201))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="73" priority="71" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="82" priority="86" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K201">
-    <cfRule type="containsText" dxfId="72" priority="72" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="81" priority="87" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K201))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsBlanks" dxfId="71" priority="67">
+    <cfRule type="containsBlanks" dxfId="80" priority="82">
       <formula>LEN(TRIM(K202))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="70" priority="68" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K202">
-    <cfRule type="containsText" dxfId="69" priority="69" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="78" priority="84" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K202))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsBlanks" dxfId="68" priority="64">
+    <cfRule type="containsBlanks" dxfId="77" priority="79">
       <formula>LEN(TRIM(K203))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="76" priority="80" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="75" priority="81" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="65" priority="61">
+    <cfRule type="containsBlanks" dxfId="74" priority="76">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsBlanks" dxfId="64" priority="58">
+    <cfRule type="containsBlanks" dxfId="73" priority="73">
       <formula>LEN(TRIM(K207))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsBlanks" dxfId="63" priority="55">
+    <cfRule type="containsBlanks" dxfId="72" priority="70">
       <formula>LEN(TRIM(K209))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsBlanks" dxfId="62" priority="52">
+    <cfRule type="containsBlanks" dxfId="71" priority="67">
       <formula>LEN(TRIM(K210))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsBlanks" dxfId="61" priority="49">
+    <cfRule type="containsBlanks" dxfId="70" priority="64">
       <formula>LEN(TRIM(K212))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsBlanks" dxfId="60" priority="46">
+    <cfRule type="containsBlanks" dxfId="69" priority="61">
       <formula>LEN(TRIM(K214))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsBlanks" dxfId="59" priority="43">
+    <cfRule type="containsBlanks" dxfId="68" priority="58">
       <formula>LEN(TRIM(K216))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="58" priority="37">
+    <cfRule type="containsBlanks" dxfId="67" priority="52">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="57" priority="62" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="66" priority="77" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="56" priority="63" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="65" priority="78" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsBlanks" dxfId="55" priority="34">
+    <cfRule type="containsBlanks" dxfId="64" priority="49">
       <formula>LEN(TRIM(K208))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="54" priority="59" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="63" priority="74" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="53" priority="60" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="62" priority="75" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="52" priority="31">
+    <cfRule type="containsBlanks" dxfId="61" priority="46">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="51" priority="56" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="60" priority="71" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="50" priority="57" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="59" priority="72" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsBlanks" dxfId="49" priority="28">
+    <cfRule type="containsBlanks" dxfId="58" priority="43">
       <formula>LEN(TRIM(K211))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="48" priority="53" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="57" priority="68" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="47" priority="54" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="56" priority="69" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsBlanks" dxfId="46" priority="25">
+    <cfRule type="containsBlanks" dxfId="55" priority="40">
       <formula>LEN(TRIM(K213))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="54" priority="65" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="44" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="53" priority="66" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsBlanks" dxfId="43" priority="22">
+    <cfRule type="containsBlanks" dxfId="52" priority="37">
       <formula>LEN(TRIM(K215))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="42" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="51" priority="62" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="41" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="50" priority="63" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="49" priority="59" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216 K233:K234 K221:K231">
-    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="48" priority="60" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="47" priority="53" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="46" priority="54" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="36" priority="35" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="44" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="32" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="41" priority="44" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="31" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="40" priority="45" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="39" priority="41" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="38" priority="42" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsBlanks" dxfId="26" priority="19">
+    <cfRule type="containsBlanks" dxfId="35" priority="34">
       <formula>LEN(TRIM(K232))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K232))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K232">
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K232))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsBlanks" dxfId="23" priority="16">
+    <cfRule type="containsBlanks" dxfId="32" priority="31">
       <formula>LEN(TRIM(K217))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsBlanks" dxfId="20" priority="13">
+    <cfRule type="containsBlanks" dxfId="29" priority="28">
       <formula>LEN(TRIM(K218))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218:K220">
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsBlanks" dxfId="17" priority="10">
+    <cfRule type="containsBlanks" dxfId="26" priority="25">
       <formula>LEN(TRIM(K235))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsBlanks" dxfId="14" priority="7">
+    <cfRule type="containsBlanks" dxfId="23" priority="22">
       <formula>LEN(TRIM(K236))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236:K238">
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsBlanks" dxfId="11" priority="4">
+    <cfRule type="containsBlanks" dxfId="20" priority="19">
       <formula>LEN(TRIM(K239))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="17" priority="16">
       <formula>LEN(TRIM(K240))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K240))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K240))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K241">
+    <cfRule type="containsBlanks" dxfId="14" priority="13">
+      <formula>LEN(TRIM(K241))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K241">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K241))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K241">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K241))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K242">
+    <cfRule type="containsBlanks" dxfId="11" priority="10">
+      <formula>LEN(TRIM(K242))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K242">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K242))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K242">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K242))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K243">
+    <cfRule type="containsBlanks" dxfId="8" priority="7">
+      <formula>LEN(TRIM(K243))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K243">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K243))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K243">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K243))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K244:K245">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
+      <formula>LEN(TRIM(K244))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K244:K245">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K244))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K244:K245">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K244))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K246">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(K246))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K246">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K246))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K246">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K246))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added system test entry for colour options
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="322">
   <si>
     <t>Test Number</t>
   </si>
@@ -974,6 +974,15 @@
   </si>
   <si>
     <t>Cannot add multiple PVs with the same name/IO to the same synoptic component</t>
+  </si>
+  <si>
+    <t>Preferences</t>
+  </si>
+  <si>
+    <t>With the motors perspective open, change the colour scheme in the Preferences menu. Verify that the table of motors background colours have changed.</t>
+  </si>
+  <si>
+    <t>Open the GUI without opening the motors perspective. Change the colour scheme in the Preferences menu. Verify that the table of motors colours background have changed.</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1339,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="93">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2549,132 +2642,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2975,8 +2942,8 @@
   <dimension ref="A1:N1074"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I169" sqref="I169"/>
+      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L254" sqref="L254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10082,16 +10049,15 @@
     </row>
     <row r="244" spans="1:13" ht="39">
       <c r="A244">
-        <f t="shared" si="56"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B244">
         <f t="shared" si="54"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C244" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-3</v>
+        <v>29-1</v>
       </c>
       <c r="D244" s="23"/>
       <c r="E244" s="23"/>
@@ -10113,15 +10079,15 @@
     <row r="245" spans="1:13" ht="39">
       <c r="A245">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B245">
         <f t="shared" si="54"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C245" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-4</v>
+        <v>29-2</v>
       </c>
       <c r="D245" s="23"/>
       <c r="E245" s="23"/>
@@ -10141,15 +10107,15 @@
     <row r="246" spans="1:13" ht="26.25">
       <c r="A246">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B246">
         <f t="shared" si="54"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C246" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-5</v>
+        <v>29-3</v>
       </c>
       <c r="D246" s="23"/>
       <c r="E246" s="23"/>
@@ -10169,15 +10135,15 @@
     <row r="247" spans="1:13" ht="26.25" customHeight="1">
       <c r="A247">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B247">
         <f t="shared" si="54"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C247" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-6</v>
+        <v>29-4</v>
       </c>
       <c r="D247" s="23"/>
       <c r="E247" s="23"/>
@@ -10197,15 +10163,15 @@
     <row r="248" spans="1:13" ht="26.25" customHeight="1">
       <c r="A248">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B248">
         <f t="shared" si="54"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C248" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-7</v>
+        <v>29-5</v>
       </c>
       <c r="D248" s="23"/>
       <c r="E248" s="23"/>
@@ -10225,15 +10191,15 @@
     <row r="249" spans="1:13" ht="39">
       <c r="A249">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B249">
         <f t="shared" si="54"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C249" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-8</v>
+        <v>29-6</v>
       </c>
       <c r="D249" s="23"/>
       <c r="E249" s="23"/>
@@ -10250,50 +10216,81 @@
       <c r="L249" s="55"/>
       <c r="M249" s="6"/>
     </row>
-    <row r="250" spans="1:13" ht="15">
+    <row r="250" spans="1:13" ht="51.75">
       <c r="A250">
-        <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B250">
         <f t="shared" si="54"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C250" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-9</v>
-      </c>
-      <c r="L250" s="6"/>
+        <v>30-1</v>
+      </c>
+      <c r="D250" s="23"/>
+      <c r="E250" s="23"/>
+      <c r="F250" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="G250" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="H250" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="I250" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="J250" s="23"/>
+      <c r="K250" s="21"/>
+      <c r="L250" s="26"/>
       <c r="M250" s="6"/>
     </row>
-    <row r="251" spans="1:13" ht="15">
+    <row r="251" spans="1:13" ht="51.75">
       <c r="A251">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B251">
         <f t="shared" si="54"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C251" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-10</v>
-      </c>
-      <c r="L251" s="6"/>
+        <v>30-2</v>
+      </c>
+      <c r="D251" s="23"/>
+      <c r="E251" s="23"/>
+      <c r="F251" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="G251" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="H251" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="I251" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="J251" s="23"/>
+      <c r="K251" s="21"/>
+      <c r="L251" s="26"/>
       <c r="M251" s="6"/>
     </row>
     <row r="252" spans="1:13" ht="15">
       <c r="A252">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B252">
         <f t="shared" si="54"/>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C252" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-11</v>
+        <v>30-3</v>
       </c>
       <c r="L252" s="6"/>
       <c r="M252" s="6"/>
@@ -10301,15 +10298,15 @@
     <row r="253" spans="1:13" ht="15">
       <c r="A253">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B253">
         <f t="shared" si="54"/>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C253" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-12</v>
+        <v>30-4</v>
       </c>
       <c r="L253" s="6"/>
       <c r="M253" s="6"/>
@@ -10317,15 +10314,15 @@
     <row r="254" spans="1:13" ht="15">
       <c r="A254">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B254">
         <f t="shared" si="54"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C254" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-13</v>
+        <v>30-5</v>
       </c>
       <c r="L254" s="6"/>
       <c r="M254" s="6"/>
@@ -10333,15 +10330,15 @@
     <row r="255" spans="1:13" ht="15">
       <c r="A255">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B255">
         <f t="shared" si="54"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C255" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-14</v>
+        <v>30-6</v>
       </c>
       <c r="L255" s="6"/>
       <c r="M255" s="6"/>
@@ -10349,15 +10346,15 @@
     <row r="256" spans="1:13" ht="15">
       <c r="A256">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B256">
         <f t="shared" si="54"/>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C256" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-15</v>
+        <v>30-7</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
@@ -10365,15 +10362,15 @@
     <row r="257" spans="1:13" ht="15">
       <c r="A257">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B257">
         <f t="shared" si="54"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C257" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-16</v>
+        <v>30-8</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
@@ -10381,15 +10378,15 @@
     <row r="258" spans="1:13" ht="15">
       <c r="A258">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B258">
         <f t="shared" si="54"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C258" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-17</v>
+        <v>30-9</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
@@ -10397,15 +10394,15 @@
     <row r="259" spans="1:13" ht="15">
       <c r="A259">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B259">
         <f t="shared" si="54"/>
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C259" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-18</v>
+        <v>30-10</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
@@ -10413,15 +10410,15 @@
     <row r="260" spans="1:13" ht="15">
       <c r="A260">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B260">
         <f t="shared" si="54"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C260" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-19</v>
+        <v>30-11</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
@@ -10429,15 +10426,15 @@
     <row r="261" spans="1:13" ht="15">
       <c r="A261">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B261">
         <f t="shared" si="54"/>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C261" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-20</v>
+        <v>30-12</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
@@ -10445,15 +10442,15 @@
     <row r="262" spans="1:13" ht="15">
       <c r="A262">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B262">
         <f t="shared" si="54"/>
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C262" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-21</v>
+        <v>30-13</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
@@ -10461,15 +10458,15 @@
     <row r="263" spans="1:13" ht="15">
       <c r="A263">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B263">
         <f t="shared" si="54"/>
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C263" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-22</v>
+        <v>30-14</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
@@ -10477,15 +10474,15 @@
     <row r="264" spans="1:13" ht="15">
       <c r="A264">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B264">
         <f t="shared" si="54"/>
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C264" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-23</v>
+        <v>30-15</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
@@ -10493,15 +10490,15 @@
     <row r="265" spans="1:13" ht="15">
       <c r="A265">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B265">
         <f t="shared" si="54"/>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C265" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-24</v>
+        <v>30-16</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
@@ -10509,15 +10506,15 @@
     <row r="266" spans="1:13" ht="15">
       <c r="A266">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B266">
         <f t="shared" si="54"/>
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C266" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-25</v>
+        <v>30-17</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
@@ -10525,15 +10522,15 @@
     <row r="267" spans="1:13" ht="15">
       <c r="A267">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B267">
         <f t="shared" si="54"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C267" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-26</v>
+        <v>30-18</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
@@ -10541,15 +10538,15 @@
     <row r="268" spans="1:13" ht="15">
       <c r="A268">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B268">
         <f t="shared" si="54"/>
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C268" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-27</v>
+        <v>30-19</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
@@ -10557,15 +10554,15 @@
     <row r="269" spans="1:13" ht="15">
       <c r="A269">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B269">
         <f t="shared" si="54"/>
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C269" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-28</v>
+        <v>30-20</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
@@ -10573,15 +10570,15 @@
     <row r="270" spans="1:13" ht="15">
       <c r="A270">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B270">
         <f t="shared" si="54"/>
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C270" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-29</v>
+        <v>30-21</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
@@ -10589,15 +10586,15 @@
     <row r="271" spans="1:13" ht="15">
       <c r="A271">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B271">
         <f t="shared" si="54"/>
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C271" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-30</v>
+        <v>30-22</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
@@ -10605,15 +10602,15 @@
     <row r="272" spans="1:13" ht="15">
       <c r="A272">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B272">
         <f t="shared" si="54"/>
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C272" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-31</v>
+        <v>30-23</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
@@ -10621,15 +10618,15 @@
     <row r="273" spans="1:13" ht="15">
       <c r="A273">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B273">
         <f t="shared" si="54"/>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C273" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-32</v>
+        <v>30-24</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
@@ -10637,15 +10634,15 @@
     <row r="274" spans="1:13" ht="15">
       <c r="A274">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B274">
         <f t="shared" si="54"/>
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C274" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-33</v>
+        <v>30-25</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
@@ -10653,15 +10650,15 @@
     <row r="275" spans="1:13" ht="15">
       <c r="A275">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B275">
         <f t="shared" si="54"/>
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C275" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-34</v>
+        <v>30-26</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
@@ -10669,15 +10666,15 @@
     <row r="276" spans="1:13" ht="15">
       <c r="A276">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B276">
         <f t="shared" si="54"/>
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C276" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-35</v>
+        <v>30-27</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
@@ -10685,15 +10682,15 @@
     <row r="277" spans="1:13" ht="15">
       <c r="A277">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B277">
         <f t="shared" si="54"/>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C277" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-36</v>
+        <v>30-28</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
@@ -10701,15 +10698,15 @@
     <row r="278" spans="1:13" ht="15">
       <c r="A278">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B278">
         <f t="shared" si="54"/>
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C278" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-37</v>
+        <v>30-29</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
@@ -10717,15 +10714,15 @@
     <row r="279" spans="1:13" ht="15">
       <c r="A279">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B279">
         <f t="shared" si="54"/>
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C279" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-38</v>
+        <v>30-30</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
@@ -10733,15 +10730,15 @@
     <row r="280" spans="1:13" ht="15">
       <c r="A280">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B280">
         <f t="shared" si="54"/>
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C280" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-39</v>
+        <v>30-31</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
@@ -10749,15 +10746,15 @@
     <row r="281" spans="1:13" ht="15">
       <c r="A281">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B281">
         <f t="shared" si="54"/>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C281" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-40</v>
+        <v>30-32</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
@@ -10765,15 +10762,15 @@
     <row r="282" spans="1:13" ht="15">
       <c r="A282">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B282">
         <f t="shared" si="54"/>
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C282" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-41</v>
+        <v>30-33</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
@@ -10781,15 +10778,15 @@
     <row r="283" spans="1:13" ht="15">
       <c r="A283">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B283">
         <f t="shared" si="54"/>
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C283" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-42</v>
+        <v>30-34</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
@@ -10797,15 +10794,15 @@
     <row r="284" spans="1:13" ht="15">
       <c r="A284">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B284">
         <f t="shared" si="54"/>
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C284" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-43</v>
+        <v>30-35</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
@@ -10813,15 +10810,15 @@
     <row r="285" spans="1:13" ht="15">
       <c r="A285">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B285">
         <f t="shared" si="54"/>
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C285" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-44</v>
+        <v>30-36</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
@@ -10829,15 +10826,15 @@
     <row r="286" spans="1:13" ht="15">
       <c r="A286">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B286">
         <f t="shared" si="54"/>
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C286" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-45</v>
+        <v>30-37</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
@@ -10845,15 +10842,15 @@
     <row r="287" spans="1:13" ht="15">
       <c r="A287">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B287">
         <f t="shared" si="54"/>
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C287" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-46</v>
+        <v>30-38</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
@@ -10861,15 +10858,15 @@
     <row r="288" spans="1:13" ht="15">
       <c r="A288">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B288">
         <f t="shared" si="54"/>
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C288" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-47</v>
+        <v>30-39</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
@@ -10877,15 +10874,15 @@
     <row r="289" spans="1:13" ht="15">
       <c r="A289">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B289">
         <f t="shared" si="54"/>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C289" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-48</v>
+        <v>30-40</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
@@ -10893,15 +10890,15 @@
     <row r="290" spans="1:13" ht="15">
       <c r="A290">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B290">
         <f t="shared" si="54"/>
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C290" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-49</v>
+        <v>30-41</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
@@ -10909,15 +10906,15 @@
     <row r="291" spans="1:13" ht="15">
       <c r="A291">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B291">
         <f t="shared" si="54"/>
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C291" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-50</v>
+        <v>30-42</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
@@ -10925,15 +10922,15 @@
     <row r="292" spans="1:13" ht="15">
       <c r="A292">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B292">
         <f t="shared" si="54"/>
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C292" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-51</v>
+        <v>30-43</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
@@ -10941,15 +10938,15 @@
     <row r="293" spans="1:13" ht="15">
       <c r="A293">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B293">
         <f t="shared" si="54"/>
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C293" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-52</v>
+        <v>30-44</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
@@ -10957,15 +10954,15 @@
     <row r="294" spans="1:13" ht="15">
       <c r="A294">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B294">
         <f t="shared" si="54"/>
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C294" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-53</v>
+        <v>30-45</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
@@ -10973,15 +10970,15 @@
     <row r="295" spans="1:13" ht="15">
       <c r="A295">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B295">
         <f t="shared" si="54"/>
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C295" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-54</v>
+        <v>30-46</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
@@ -10989,15 +10986,15 @@
     <row r="296" spans="1:13" ht="15">
       <c r="A296">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B296">
         <f t="shared" si="54"/>
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C296" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-55</v>
+        <v>30-47</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
@@ -11005,15 +11002,15 @@
     <row r="297" spans="1:13" ht="15">
       <c r="A297">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B297">
         <f t="shared" si="54"/>
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C297" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-56</v>
+        <v>30-48</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
@@ -11021,15 +11018,15 @@
     <row r="298" spans="1:13" ht="15">
       <c r="A298">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B298">
         <f t="shared" si="54"/>
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C298" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-57</v>
+        <v>30-49</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
@@ -11037,15 +11034,15 @@
     <row r="299" spans="1:13" ht="15">
       <c r="A299">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B299">
         <f t="shared" si="54"/>
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C299" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-58</v>
+        <v>30-50</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
@@ -11053,15 +11050,15 @@
     <row r="300" spans="1:13" ht="15">
       <c r="A300">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B300">
         <f t="shared" si="54"/>
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C300" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-59</v>
+        <v>30-51</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
@@ -11069,15 +11066,15 @@
     <row r="301" spans="1:13" ht="15">
       <c r="A301">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B301">
         <f t="shared" si="54"/>
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C301" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-60</v>
+        <v>30-52</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
@@ -11085,15 +11082,15 @@
     <row r="302" spans="1:13" ht="15">
       <c r="A302">
         <f t="shared" si="56"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B302">
         <f t="shared" ref="B302:B365" si="57">IF(A302=A301,B301+1,1)</f>
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C302" s="3" t="str">
         <f t="shared" ref="C302:C365" si="58">CONCATENATE(A302,"-",B302)</f>
-        <v>28-61</v>
+        <v>30-53</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
@@ -11101,15 +11098,15 @@
     <row r="303" spans="1:13" ht="15">
       <c r="A303">
         <f t="shared" ref="A303:A366" si="59">A302</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B303">
         <f t="shared" si="57"/>
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C303" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-62</v>
+        <v>30-54</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
@@ -11117,15 +11114,15 @@
     <row r="304" spans="1:13" ht="15">
       <c r="A304">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B304">
         <f t="shared" si="57"/>
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C304" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-63</v>
+        <v>30-55</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
@@ -11133,15 +11130,15 @@
     <row r="305" spans="1:13" ht="15">
       <c r="A305">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B305">
         <f t="shared" si="57"/>
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C305" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-64</v>
+        <v>30-56</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
@@ -11149,15 +11146,15 @@
     <row r="306" spans="1:13" ht="15">
       <c r="A306">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B306">
         <f t="shared" si="57"/>
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C306" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-65</v>
+        <v>30-57</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
@@ -11165,15 +11162,15 @@
     <row r="307" spans="1:13" ht="15">
       <c r="A307">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B307">
         <f t="shared" si="57"/>
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C307" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-66</v>
+        <v>30-58</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
@@ -11181,15 +11178,15 @@
     <row r="308" spans="1:13" ht="15">
       <c r="A308">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B308">
         <f t="shared" si="57"/>
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C308" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-67</v>
+        <v>30-59</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
@@ -11197,15 +11194,15 @@
     <row r="309" spans="1:13" ht="15">
       <c r="A309">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B309">
         <f t="shared" si="57"/>
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C309" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-68</v>
+        <v>30-60</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
@@ -11213,15 +11210,15 @@
     <row r="310" spans="1:13" ht="15">
       <c r="A310">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B310">
         <f t="shared" si="57"/>
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C310" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-69</v>
+        <v>30-61</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
@@ -11229,15 +11226,15 @@
     <row r="311" spans="1:13" ht="15">
       <c r="A311">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B311">
         <f t="shared" si="57"/>
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C311" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-70</v>
+        <v>30-62</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
@@ -11245,15 +11242,15 @@
     <row r="312" spans="1:13" ht="15">
       <c r="A312">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B312">
         <f t="shared" si="57"/>
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C312" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-71</v>
+        <v>30-63</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
@@ -11261,15 +11258,15 @@
     <row r="313" spans="1:13" ht="15">
       <c r="A313">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B313">
         <f t="shared" si="57"/>
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C313" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-72</v>
+        <v>30-64</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
@@ -11277,15 +11274,15 @@
     <row r="314" spans="1:13" ht="15">
       <c r="A314">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B314">
         <f t="shared" si="57"/>
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C314" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-73</v>
+        <v>30-65</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
@@ -11293,15 +11290,15 @@
     <row r="315" spans="1:13" ht="15">
       <c r="A315">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B315">
         <f t="shared" si="57"/>
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C315" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-74</v>
+        <v>30-66</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
@@ -11309,15 +11306,15 @@
     <row r="316" spans="1:13" ht="15">
       <c r="A316">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B316">
         <f t="shared" si="57"/>
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C316" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-75</v>
+        <v>30-67</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
@@ -11325,15 +11322,15 @@
     <row r="317" spans="1:13" ht="15">
       <c r="A317">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B317">
         <f t="shared" si="57"/>
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C317" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-76</v>
+        <v>30-68</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
@@ -11341,15 +11338,15 @@
     <row r="318" spans="1:13" ht="15">
       <c r="A318">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B318">
         <f t="shared" si="57"/>
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C318" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-77</v>
+        <v>30-69</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
@@ -11357,15 +11354,15 @@
     <row r="319" spans="1:13" ht="15">
       <c r="A319">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B319">
         <f t="shared" si="57"/>
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C319" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-78</v>
+        <v>30-70</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
@@ -11373,15 +11370,15 @@
     <row r="320" spans="1:13" ht="15">
       <c r="A320">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B320">
         <f t="shared" si="57"/>
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C320" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-79</v>
+        <v>30-71</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
@@ -11389,15 +11386,15 @@
     <row r="321" spans="1:13" ht="15">
       <c r="A321">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B321">
         <f t="shared" si="57"/>
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C321" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-80</v>
+        <v>30-72</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
@@ -11405,15 +11402,15 @@
     <row r="322" spans="1:13" ht="15">
       <c r="A322">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B322">
         <f t="shared" si="57"/>
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C322" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-81</v>
+        <v>30-73</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
@@ -11421,15 +11418,15 @@
     <row r="323" spans="1:13" ht="15">
       <c r="A323">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B323">
         <f t="shared" si="57"/>
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C323" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-82</v>
+        <v>30-74</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
@@ -11437,15 +11434,15 @@
     <row r="324" spans="1:13" ht="15">
       <c r="A324">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B324">
         <f t="shared" si="57"/>
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C324" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-83</v>
+        <v>30-75</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
@@ -11453,15 +11450,15 @@
     <row r="325" spans="1:13" ht="15">
       <c r="A325">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B325">
         <f t="shared" si="57"/>
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C325" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-84</v>
+        <v>30-76</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
@@ -11469,15 +11466,15 @@
     <row r="326" spans="1:13" ht="15">
       <c r="A326">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B326">
         <f t="shared" si="57"/>
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C326" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-85</v>
+        <v>30-77</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
@@ -11485,15 +11482,15 @@
     <row r="327" spans="1:13" ht="15">
       <c r="A327">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B327">
         <f t="shared" si="57"/>
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C327" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-86</v>
+        <v>30-78</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
@@ -11501,15 +11498,15 @@
     <row r="328" spans="1:13" ht="15">
       <c r="A328">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B328">
         <f t="shared" si="57"/>
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C328" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-87</v>
+        <v>30-79</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
@@ -11517,15 +11514,15 @@
     <row r="329" spans="1:13" ht="15">
       <c r="A329">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B329">
         <f t="shared" si="57"/>
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C329" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-88</v>
+        <v>30-80</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
@@ -11533,15 +11530,15 @@
     <row r="330" spans="1:13" ht="15">
       <c r="A330">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B330">
         <f t="shared" si="57"/>
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C330" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-89</v>
+        <v>30-81</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
@@ -11549,15 +11546,15 @@
     <row r="331" spans="1:13" ht="15">
       <c r="A331">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B331">
         <f t="shared" si="57"/>
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C331" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-90</v>
+        <v>30-82</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
@@ -11565,15 +11562,15 @@
     <row r="332" spans="1:13" ht="15">
       <c r="A332">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B332">
         <f t="shared" si="57"/>
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C332" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-91</v>
+        <v>30-83</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
@@ -11581,15 +11578,15 @@
     <row r="333" spans="1:13" ht="15">
       <c r="A333">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B333">
         <f t="shared" si="57"/>
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C333" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-92</v>
+        <v>30-84</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
@@ -11597,15 +11594,15 @@
     <row r="334" spans="1:13" ht="15">
       <c r="A334">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B334">
         <f t="shared" si="57"/>
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C334" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-93</v>
+        <v>30-85</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
@@ -11613,15 +11610,15 @@
     <row r="335" spans="1:13" ht="15">
       <c r="A335">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B335">
         <f t="shared" si="57"/>
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C335" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-94</v>
+        <v>30-86</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
@@ -11629,15 +11626,15 @@
     <row r="336" spans="1:13" ht="15">
       <c r="A336">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B336">
         <f t="shared" si="57"/>
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C336" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-95</v>
+        <v>30-87</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
@@ -11645,15 +11642,15 @@
     <row r="337" spans="1:13" ht="15">
       <c r="A337">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B337">
         <f t="shared" si="57"/>
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C337" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-96</v>
+        <v>30-88</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
@@ -11661,15 +11658,15 @@
     <row r="338" spans="1:13" ht="15">
       <c r="A338">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B338">
         <f t="shared" si="57"/>
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C338" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-97</v>
+        <v>30-89</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
@@ -11677,15 +11674,15 @@
     <row r="339" spans="1:13" ht="15">
       <c r="A339">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B339">
         <f t="shared" si="57"/>
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C339" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-98</v>
+        <v>30-90</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
@@ -11693,15 +11690,15 @@
     <row r="340" spans="1:13" ht="15">
       <c r="A340">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B340">
         <f t="shared" si="57"/>
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C340" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-99</v>
+        <v>30-91</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
@@ -11709,15 +11706,15 @@
     <row r="341" spans="1:13" ht="15">
       <c r="A341">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B341">
         <f t="shared" si="57"/>
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C341" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-100</v>
+        <v>30-92</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
@@ -11725,15 +11722,15 @@
     <row r="342" spans="1:13" ht="15">
       <c r="A342">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B342">
         <f t="shared" si="57"/>
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C342" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-101</v>
+        <v>30-93</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
@@ -11741,15 +11738,15 @@
     <row r="343" spans="1:13" ht="15">
       <c r="A343">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B343">
         <f t="shared" si="57"/>
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C343" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-102</v>
+        <v>30-94</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
@@ -11757,15 +11754,15 @@
     <row r="344" spans="1:13" ht="15">
       <c r="A344">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B344">
         <f t="shared" si="57"/>
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C344" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-103</v>
+        <v>30-95</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
@@ -11773,15 +11770,15 @@
     <row r="345" spans="1:13" ht="15">
       <c r="A345">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B345">
         <f t="shared" si="57"/>
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C345" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-104</v>
+        <v>30-96</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
@@ -11789,15 +11786,15 @@
     <row r="346" spans="1:13" ht="15">
       <c r="A346">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B346">
         <f t="shared" si="57"/>
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C346" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-105</v>
+        <v>30-97</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
@@ -11805,15 +11802,15 @@
     <row r="347" spans="1:13" ht="15">
       <c r="A347">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B347">
         <f t="shared" si="57"/>
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C347" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-106</v>
+        <v>30-98</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
@@ -11821,15 +11818,15 @@
     <row r="348" spans="1:13" ht="15">
       <c r="A348">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B348">
         <f t="shared" si="57"/>
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C348" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-107</v>
+        <v>30-99</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
@@ -11837,15 +11834,15 @@
     <row r="349" spans="1:13" ht="15">
       <c r="A349">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B349">
         <f t="shared" si="57"/>
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C349" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-108</v>
+        <v>30-100</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
@@ -11853,15 +11850,15 @@
     <row r="350" spans="1:13" ht="15">
       <c r="A350">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B350">
         <f t="shared" si="57"/>
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C350" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-109</v>
+        <v>30-101</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
@@ -11869,15 +11866,15 @@
     <row r="351" spans="1:13" ht="15">
       <c r="A351">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B351">
         <f t="shared" si="57"/>
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C351" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-110</v>
+        <v>30-102</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
@@ -11885,15 +11882,15 @@
     <row r="352" spans="1:13" ht="15">
       <c r="A352">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B352">
         <f t="shared" si="57"/>
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C352" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-111</v>
+        <v>30-103</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
@@ -11901,15 +11898,15 @@
     <row r="353" spans="1:13" ht="15">
       <c r="A353">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B353">
         <f t="shared" si="57"/>
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C353" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-112</v>
+        <v>30-104</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
@@ -11917,15 +11914,15 @@
     <row r="354" spans="1:13" ht="15">
       <c r="A354">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B354">
         <f t="shared" si="57"/>
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C354" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-113</v>
+        <v>30-105</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
@@ -11933,15 +11930,15 @@
     <row r="355" spans="1:13" ht="15">
       <c r="A355">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B355">
         <f t="shared" si="57"/>
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C355" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-114</v>
+        <v>30-106</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
@@ -11949,15 +11946,15 @@
     <row r="356" spans="1:13" ht="15">
       <c r="A356">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B356">
         <f t="shared" si="57"/>
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C356" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-115</v>
+        <v>30-107</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
@@ -11965,15 +11962,15 @@
     <row r="357" spans="1:13" ht="15">
       <c r="A357">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B357">
         <f t="shared" si="57"/>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C357" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-116</v>
+        <v>30-108</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
@@ -11981,15 +11978,15 @@
     <row r="358" spans="1:13" ht="15">
       <c r="A358">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B358">
         <f t="shared" si="57"/>
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C358" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-117</v>
+        <v>30-109</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
@@ -11997,15 +11994,15 @@
     <row r="359" spans="1:13" ht="15">
       <c r="A359">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B359">
         <f t="shared" si="57"/>
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C359" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-118</v>
+        <v>30-110</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
@@ -12013,15 +12010,15 @@
     <row r="360" spans="1:13" ht="15">
       <c r="A360">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B360">
         <f t="shared" si="57"/>
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C360" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-119</v>
+        <v>30-111</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
@@ -12029,15 +12026,15 @@
     <row r="361" spans="1:13" ht="15">
       <c r="A361">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B361">
         <f t="shared" si="57"/>
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C361" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-120</v>
+        <v>30-112</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
@@ -12045,15 +12042,15 @@
     <row r="362" spans="1:13" ht="15">
       <c r="A362">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B362">
         <f t="shared" si="57"/>
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C362" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-121</v>
+        <v>30-113</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
@@ -12061,15 +12058,15 @@
     <row r="363" spans="1:13" ht="15">
       <c r="A363">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B363">
         <f t="shared" si="57"/>
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C363" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-122</v>
+        <v>30-114</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
@@ -12077,15 +12074,15 @@
     <row r="364" spans="1:13" ht="15">
       <c r="A364">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B364">
         <f t="shared" si="57"/>
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C364" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-123</v>
+        <v>30-115</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
@@ -12093,15 +12090,15 @@
     <row r="365" spans="1:13" ht="15">
       <c r="A365">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B365">
         <f t="shared" si="57"/>
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C365" s="3" t="str">
         <f t="shared" si="58"/>
-        <v>28-124</v>
+        <v>30-116</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
@@ -12109,15 +12106,15 @@
     <row r="366" spans="1:13" ht="15">
       <c r="A366">
         <f t="shared" si="59"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B366">
         <f t="shared" ref="B366:B387" si="60">IF(A366=A365,B365+1,1)</f>
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C366" s="3" t="str">
         <f t="shared" ref="C366:C387" si="61">CONCATENATE(A366,"-",B366)</f>
-        <v>28-125</v>
+        <v>30-117</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
@@ -12125,15 +12122,15 @@
     <row r="367" spans="1:13" ht="15">
       <c r="A367">
         <f t="shared" ref="A367:A387" si="62">A366</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B367">
         <f t="shared" si="60"/>
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C367" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-126</v>
+        <v>30-118</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
@@ -12141,15 +12138,15 @@
     <row r="368" spans="1:13" ht="15">
       <c r="A368">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B368">
         <f t="shared" si="60"/>
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C368" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-127</v>
+        <v>30-119</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
@@ -12157,15 +12154,15 @@
     <row r="369" spans="1:13" ht="15">
       <c r="A369">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B369">
         <f t="shared" si="60"/>
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C369" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-128</v>
+        <v>30-120</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
@@ -12173,15 +12170,15 @@
     <row r="370" spans="1:13" ht="15">
       <c r="A370">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B370">
         <f t="shared" si="60"/>
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C370" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-129</v>
+        <v>30-121</v>
       </c>
       <c r="L370" s="6"/>
       <c r="M370" s="6"/>
@@ -12189,15 +12186,15 @@
     <row r="371" spans="1:13" ht="15">
       <c r="A371">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B371">
         <f t="shared" si="60"/>
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C371" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-130</v>
+        <v>30-122</v>
       </c>
       <c r="L371" s="6"/>
       <c r="M371" s="6"/>
@@ -12205,15 +12202,15 @@
     <row r="372" spans="1:13" ht="15">
       <c r="A372">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B372">
         <f t="shared" si="60"/>
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C372" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-131</v>
+        <v>30-123</v>
       </c>
       <c r="L372" s="6"/>
       <c r="M372" s="6"/>
@@ -12221,15 +12218,15 @@
     <row r="373" spans="1:13" ht="15">
       <c r="A373">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B373">
         <f t="shared" si="60"/>
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C373" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-132</v>
+        <v>30-124</v>
       </c>
       <c r="L373" s="6"/>
       <c r="M373" s="6"/>
@@ -12237,15 +12234,15 @@
     <row r="374" spans="1:13" ht="15">
       <c r="A374">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B374">
         <f t="shared" si="60"/>
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C374" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-133</v>
+        <v>30-125</v>
       </c>
       <c r="L374" s="6"/>
       <c r="M374" s="6"/>
@@ -12253,15 +12250,15 @@
     <row r="375" spans="1:13" ht="15">
       <c r="A375">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B375">
         <f t="shared" si="60"/>
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C375" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-134</v>
+        <v>30-126</v>
       </c>
       <c r="L375" s="6"/>
       <c r="M375" s="6"/>
@@ -12269,15 +12266,15 @@
     <row r="376" spans="1:13" ht="15">
       <c r="A376">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B376">
         <f t="shared" si="60"/>
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C376" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-135</v>
+        <v>30-127</v>
       </c>
       <c r="L376" s="6"/>
       <c r="M376" s="6"/>
@@ -12285,15 +12282,15 @@
     <row r="377" spans="1:13" ht="15">
       <c r="A377">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B377">
         <f t="shared" si="60"/>
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C377" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-136</v>
+        <v>30-128</v>
       </c>
       <c r="L377" s="6"/>
       <c r="M377" s="6"/>
@@ -12301,15 +12298,15 @@
     <row r="378" spans="1:13" ht="15">
       <c r="A378">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B378">
         <f t="shared" si="60"/>
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C378" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-137</v>
+        <v>30-129</v>
       </c>
       <c r="L378" s="6"/>
       <c r="M378" s="6"/>
@@ -12317,15 +12314,15 @@
     <row r="379" spans="1:13" ht="15">
       <c r="A379">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B379">
         <f t="shared" si="60"/>
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C379" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-138</v>
+        <v>30-130</v>
       </c>
       <c r="L379" s="6"/>
       <c r="M379" s="6"/>
@@ -12333,15 +12330,15 @@
     <row r="380" spans="1:13" ht="15">
       <c r="A380">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B380">
         <f t="shared" si="60"/>
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C380" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-139</v>
+        <v>30-131</v>
       </c>
       <c r="L380" s="6"/>
       <c r="M380" s="6"/>
@@ -12349,15 +12346,15 @@
     <row r="381" spans="1:13" ht="15">
       <c r="A381">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B381">
         <f t="shared" si="60"/>
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C381" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-140</v>
+        <v>30-132</v>
       </c>
       <c r="L381" s="6"/>
       <c r="M381" s="6"/>
@@ -12365,15 +12362,15 @@
     <row r="382" spans="1:13" ht="15">
       <c r="A382">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B382">
         <f t="shared" si="60"/>
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C382" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-141</v>
+        <v>30-133</v>
       </c>
       <c r="L382" s="6"/>
       <c r="M382" s="6"/>
@@ -12381,15 +12378,15 @@
     <row r="383" spans="1:13" ht="15">
       <c r="A383">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B383">
         <f t="shared" si="60"/>
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C383" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-142</v>
+        <v>30-134</v>
       </c>
       <c r="L383" s="6"/>
       <c r="M383" s="6"/>
@@ -12397,15 +12394,15 @@
     <row r="384" spans="1:13" ht="15">
       <c r="A384">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B384">
         <f t="shared" si="60"/>
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C384" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-143</v>
+        <v>30-135</v>
       </c>
       <c r="L384" s="6"/>
       <c r="M384" s="6"/>
@@ -12413,15 +12410,15 @@
     <row r="385" spans="1:13" ht="15">
       <c r="A385">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B385">
         <f t="shared" si="60"/>
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C385" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-144</v>
+        <v>30-136</v>
       </c>
       <c r="L385" s="6"/>
       <c r="M385" s="6"/>
@@ -12429,15 +12426,15 @@
     <row r="386" spans="1:13" ht="15">
       <c r="A386">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B386">
         <f t="shared" si="60"/>
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C386" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-145</v>
+        <v>30-137</v>
       </c>
       <c r="L386" s="6"/>
       <c r="M386" s="6"/>
@@ -12445,15 +12442,15 @@
     <row r="387" spans="1:13" ht="15">
       <c r="A387">
         <f t="shared" si="62"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B387">
         <f t="shared" si="60"/>
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C387" s="3" t="str">
         <f t="shared" si="61"/>
-        <v>28-146</v>
+        <v>30-138</v>
       </c>
       <c r="L387" s="6"/>
       <c r="M387" s="6"/>
@@ -15213,438 +15210,453 @@
     <mergeCell ref="L244:L249"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K156 K158:K202">
-    <cfRule type="containsBlanks" dxfId="86" priority="91">
+    <cfRule type="containsBlanks" dxfId="92" priority="94">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K156 K158:K202">
-    <cfRule type="containsText" dxfId="85" priority="92" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="91" priority="95" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K156 K158:K202">
-    <cfRule type="containsText" dxfId="84" priority="93" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="90" priority="96" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsBlanks" dxfId="83" priority="88">
+    <cfRule type="containsBlanks" dxfId="89" priority="91">
       <formula>LEN(TRIM(K203))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="82" priority="89" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="88" priority="92" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K203">
-    <cfRule type="containsText" dxfId="81" priority="90" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="87" priority="93" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K203))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="80" priority="82">
+    <cfRule type="containsBlanks" dxfId="86" priority="85">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="78" priority="84" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="77" priority="79">
+    <cfRule type="containsBlanks" dxfId="83" priority="82">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="76" priority="80" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="75" priority="81" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="81" priority="84" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="74" priority="76">
+    <cfRule type="containsBlanks" dxfId="80" priority="79">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="73" priority="77" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="72" priority="78" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="78" priority="81" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsBlanks" dxfId="71" priority="73">
+    <cfRule type="containsBlanks" dxfId="77" priority="76">
       <formula>LEN(TRIM(K208))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsBlanks" dxfId="70" priority="70">
+    <cfRule type="containsBlanks" dxfId="76" priority="73">
       <formula>LEN(TRIM(K210))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsBlanks" dxfId="69" priority="67">
+    <cfRule type="containsBlanks" dxfId="75" priority="70">
       <formula>LEN(TRIM(K212))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsBlanks" dxfId="68" priority="64">
+    <cfRule type="containsBlanks" dxfId="74" priority="67">
       <formula>LEN(TRIM(K213))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsBlanks" dxfId="67" priority="61">
+    <cfRule type="containsBlanks" dxfId="73" priority="64">
       <formula>LEN(TRIM(K215))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsBlanks" dxfId="66" priority="58">
+    <cfRule type="containsBlanks" dxfId="72" priority="61">
       <formula>LEN(TRIM(K217))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219 K236:K237 K224:K234">
-    <cfRule type="containsBlanks" dxfId="65" priority="55">
+    <cfRule type="containsBlanks" dxfId="71" priority="58">
       <formula>LEN(TRIM(K219))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsBlanks" dxfId="64" priority="49">
+    <cfRule type="containsBlanks" dxfId="70" priority="52">
       <formula>LEN(TRIM(K209))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="63" priority="74" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="69" priority="77" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="62" priority="75" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="68" priority="78" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsBlanks" dxfId="61" priority="46">
+    <cfRule type="containsBlanks" dxfId="67" priority="49">
       <formula>LEN(TRIM(K211))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="60" priority="71" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="66" priority="74" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="59" priority="72" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="65" priority="75" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsBlanks" dxfId="58" priority="43">
+    <cfRule type="containsBlanks" dxfId="64" priority="46">
       <formula>LEN(TRIM(K207))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="57" priority="68" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="63" priority="71" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="56" priority="69" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="62" priority="72" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsBlanks" dxfId="55" priority="40">
+    <cfRule type="containsBlanks" dxfId="61" priority="43">
       <formula>LEN(TRIM(K214))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="54" priority="65" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="60" priority="68" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="53" priority="66" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="59" priority="69" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsBlanks" dxfId="52" priority="37">
+    <cfRule type="containsBlanks" dxfId="58" priority="40">
       <formula>LEN(TRIM(K216))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="51" priority="62" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="57" priority="65" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="50" priority="63" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="56" priority="66" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsBlanks" dxfId="49" priority="34">
+    <cfRule type="containsBlanks" dxfId="55" priority="37">
       <formula>LEN(TRIM(K218))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="48" priority="59" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="54" priority="62" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="47" priority="60" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="53" priority="63" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219 K236:K237 K224:K234">
-    <cfRule type="containsText" dxfId="46" priority="56" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K219))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219 K236:K237 K224:K234">
-    <cfRule type="containsText" dxfId="45" priority="57" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="51" priority="60" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K219))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="44" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="50" priority="53" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="43" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="49" priority="54" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="42" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="48" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="41" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="47" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="38" priority="41" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="44" priority="44" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="37" priority="42" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsText" dxfId="36" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="42" priority="41" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsText" dxfId="35" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsBlanks" dxfId="32" priority="31">
+    <cfRule type="containsBlanks" dxfId="38" priority="34">
       <formula>LEN(TRIM(K235))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K235">
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K235))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220">
-    <cfRule type="containsBlanks" dxfId="29" priority="28">
+    <cfRule type="containsBlanks" dxfId="35" priority="31">
       <formula>LEN(TRIM(K220))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220">
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K220))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220">
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K220))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221:K223">
-    <cfRule type="containsBlanks" dxfId="26" priority="25">
+    <cfRule type="containsBlanks" dxfId="32" priority="28">
       <formula>LEN(TRIM(K221))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221:K223">
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K221))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221:K223">
-    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K221))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K238">
-    <cfRule type="containsBlanks" dxfId="23" priority="22">
+    <cfRule type="containsBlanks" dxfId="29" priority="25">
       <formula>LEN(TRIM(K238))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K238">
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K238))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K238">
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K238))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239:K241">
-    <cfRule type="containsBlanks" dxfId="20" priority="19">
+    <cfRule type="containsBlanks" dxfId="26" priority="22">
       <formula>LEN(TRIM(K239))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239:K241">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239:K241">
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K242">
-    <cfRule type="containsBlanks" dxfId="17" priority="16">
+    <cfRule type="containsBlanks" dxfId="23" priority="19">
       <formula>LEN(TRIM(K242))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K242">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K242))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K242">
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K242))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K243">
-    <cfRule type="containsBlanks" dxfId="14" priority="13">
+    <cfRule type="containsBlanks" dxfId="20" priority="16">
       <formula>LEN(TRIM(K243))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K243">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K243))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K243">
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K243))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K157">
-    <cfRule type="containsBlanks" dxfId="11" priority="10">
+    <cfRule type="containsBlanks" dxfId="17" priority="13">
       <formula>LEN(TRIM(K157))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K157">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K157))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K157">
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K157))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K244:K245">
-    <cfRule type="containsBlanks" dxfId="8" priority="7">
+    <cfRule type="containsBlanks" dxfId="14" priority="10">
       <formula>LEN(TRIM(K244))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K244:K245">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K244))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K244:K245">
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K244))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K246">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
+    <cfRule type="containsBlanks" dxfId="11" priority="7">
       <formula>LEN(TRIM(K246))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K246">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K246))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K246">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K246))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247:K249">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="8" priority="4">
       <formula>LEN(TRIM(K247))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247:K249">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K247))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247:K249">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K247))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K250:K251">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
+      <formula>LEN(TRIM(K250))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K250:K251">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K250))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K250:K251">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K250))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added tests for 1870
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -973,9 +973,6 @@
     <t>Cannot add multiple components with the same name to a synoptic</t>
   </si>
   <si>
-    <t>Cannot add multiple PVs with the same name/IO to the same synoptic component</t>
-  </si>
-  <si>
     <t>Preferences</t>
   </si>
   <si>
@@ -989,6 +986,9 @@
   </si>
   <si>
     <t>"Launch maintenance website" is linked to instrument name and will 404 on dev instruments</t>
+  </si>
+  <si>
+    <t>Adding a New PV to a component gives it a unique name to start with</t>
   </si>
 </sst>
 </file>
@@ -1327,6 +1327,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1341,28 +1344,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="93">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1382,34 +1368,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
         </patternFill>
       </fill>
       <border>
@@ -2993,8 +2951,8 @@
   <dimension ref="A1:N1075"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L100" sqref="L100"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J177" sqref="J177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5861,7 +5819,7 @@
         <f>IF(A98=A97,B97+1,1)</f>
         <v>2</v>
       </c>
-      <c r="C98" s="57" t="str">
+      <c r="C98" s="51" t="str">
         <f>CONCATENATE(A98,"-",B98)</f>
         <v>13-2</v>
       </c>
@@ -5873,12 +5831,12 @@
         <v>105</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J98" s="8"/>
       <c r="K98" s="9"/>
       <c r="L98" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="15">
@@ -8093,7 +8051,7 @@
         <v>98</v>
       </c>
       <c r="I176" s="8" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="J176" s="8"/>
       <c r="K176" s="9"/>
@@ -8572,7 +8530,7 @@
       </c>
       <c r="J192" s="8"/>
       <c r="K192" s="7"/>
-      <c r="L192" s="51"/>
+      <c r="L192" s="52"/>
     </row>
     <row r="193" spans="1:13" ht="30">
       <c r="A193">
@@ -8601,7 +8559,7 @@
       </c>
       <c r="J193" s="8"/>
       <c r="K193" s="7"/>
-      <c r="L193" s="52"/>
+      <c r="L193" s="53"/>
       <c r="M193" s="6"/>
     </row>
     <row r="194" spans="1:13" ht="45">
@@ -8631,7 +8589,7 @@
       </c>
       <c r="J194" s="8"/>
       <c r="K194" s="7"/>
-      <c r="L194" s="52"/>
+      <c r="L194" s="53"/>
       <c r="M194" s="6"/>
     </row>
     <row r="195" spans="1:13" ht="30">
@@ -8661,7 +8619,7 @@
       </c>
       <c r="J195" s="8"/>
       <c r="K195" s="7"/>
-      <c r="L195" s="53"/>
+      <c r="L195" s="54"/>
       <c r="M195" s="6"/>
     </row>
     <row r="196" spans="1:13" ht="30">
@@ -10092,7 +10050,7 @@
       </c>
       <c r="J243" s="23"/>
       <c r="K243" s="21"/>
-      <c r="L243" s="54" t="s">
+      <c r="L243" s="55" t="s">
         <v>307</v>
       </c>
       <c r="M243" s="6"/>
@@ -10124,7 +10082,7 @@
         <v>306</v>
       </c>
       <c r="K244" s="21"/>
-      <c r="L244" s="55"/>
+      <c r="L244" s="56"/>
       <c r="M244" s="6"/>
     </row>
     <row r="245" spans="1:13" ht="39">
@@ -10151,7 +10109,7 @@
       </c>
       <c r="J245" s="23"/>
       <c r="K245" s="21"/>
-      <c r="L245" s="54" t="s">
+      <c r="L245" s="55" t="s">
         <v>316</v>
       </c>
       <c r="M245" s="6"/>
@@ -10181,7 +10139,7 @@
       </c>
       <c r="J246" s="23"/>
       <c r="K246" s="21"/>
-      <c r="L246" s="56"/>
+      <c r="L246" s="57"/>
       <c r="M246" s="6"/>
     </row>
     <row r="247" spans="1:13" ht="26.25">
@@ -10209,7 +10167,7 @@
       </c>
       <c r="J247" s="23"/>
       <c r="K247" s="21"/>
-      <c r="L247" s="56"/>
+      <c r="L247" s="57"/>
       <c r="M247" s="6"/>
     </row>
     <row r="248" spans="1:13" ht="26.25" customHeight="1">
@@ -10237,7 +10195,7 @@
       </c>
       <c r="J248" s="23"/>
       <c r="K248" s="21"/>
-      <c r="L248" s="56"/>
+      <c r="L248" s="57"/>
       <c r="M248" s="6"/>
     </row>
     <row r="249" spans="1:13" ht="26.25" customHeight="1">
@@ -10265,7 +10223,7 @@
       </c>
       <c r="J249" s="23"/>
       <c r="K249" s="21"/>
-      <c r="L249" s="56"/>
+      <c r="L249" s="57"/>
       <c r="M249" s="6"/>
     </row>
     <row r="250" spans="1:13" ht="39">
@@ -10293,7 +10251,7 @@
       </c>
       <c r="J250" s="23"/>
       <c r="K250" s="21"/>
-      <c r="L250" s="55"/>
+      <c r="L250" s="56"/>
       <c r="M250" s="6"/>
     </row>
     <row r="251" spans="1:13" ht="51.75">
@@ -10317,10 +10275,10 @@
         <v>177</v>
       </c>
       <c r="H251" s="24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I251" s="25" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J251" s="23"/>
       <c r="K251" s="21"/>
@@ -10349,10 +10307,10 @@
         <v>177</v>
       </c>
       <c r="H252" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="I252" s="25" t="s">
         <v>319</v>
-      </c>
-      <c r="I252" s="25" t="s">
-        <v>320</v>
       </c>
       <c r="J252" s="23"/>
       <c r="K252" s="21"/>
@@ -15290,467 +15248,467 @@
     <mergeCell ref="L245:L250"/>
   </mergeCells>
   <conditionalFormatting sqref="K159:K203 K99:K157 K2:K97">
-    <cfRule type="containsBlanks" dxfId="95" priority="97">
+    <cfRule type="containsBlanks" dxfId="92" priority="97">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K159:K203 K99:K157 K2:K97">
-    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="91" priority="98" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K159:K203 K99:K157 K2:K97">
-    <cfRule type="containsText" dxfId="93" priority="99" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="90" priority="99" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="92" priority="94">
+    <cfRule type="containsBlanks" dxfId="89" priority="94">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="91" priority="95" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="88" priority="95" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="90" priority="96" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="87" priority="96" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="89" priority="88">
+    <cfRule type="containsBlanks" dxfId="86" priority="88">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="85" priority="89" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="87" priority="90" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="84" priority="90" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="86" priority="85">
+    <cfRule type="containsBlanks" dxfId="83" priority="85">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="82" priority="86" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="81" priority="87" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsBlanks" dxfId="83" priority="82">
+    <cfRule type="containsBlanks" dxfId="80" priority="82">
       <formula>LEN(TRIM(K207))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="81" priority="84" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="78" priority="84" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsBlanks" dxfId="80" priority="79">
+    <cfRule type="containsBlanks" dxfId="77" priority="79">
       <formula>LEN(TRIM(K209))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsBlanks" dxfId="79" priority="76">
+    <cfRule type="containsBlanks" dxfId="76" priority="76">
       <formula>LEN(TRIM(K211))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsBlanks" dxfId="78" priority="73">
+    <cfRule type="containsBlanks" dxfId="75" priority="73">
       <formula>LEN(TRIM(K213))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsBlanks" dxfId="77" priority="70">
+    <cfRule type="containsBlanks" dxfId="74" priority="70">
       <formula>LEN(TRIM(K214))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsBlanks" dxfId="76" priority="67">
+    <cfRule type="containsBlanks" dxfId="73" priority="67">
       <formula>LEN(TRIM(K216))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsBlanks" dxfId="75" priority="64">
+    <cfRule type="containsBlanks" dxfId="72" priority="64">
       <formula>LEN(TRIM(K218))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220 K237:K238 K225:K235">
-    <cfRule type="containsBlanks" dxfId="74" priority="61">
+    <cfRule type="containsBlanks" dxfId="71" priority="61">
       <formula>LEN(TRIM(K220))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsBlanks" dxfId="73" priority="55">
+    <cfRule type="containsBlanks" dxfId="70" priority="55">
       <formula>LEN(TRIM(K210))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="72" priority="80" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="69" priority="80" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="71" priority="81" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="68" priority="81" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsBlanks" dxfId="70" priority="52">
+    <cfRule type="containsBlanks" dxfId="67" priority="52">
       <formula>LEN(TRIM(K212))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="69" priority="77" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="66" priority="77" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="68" priority="78" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="65" priority="78" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsBlanks" dxfId="67" priority="49">
+    <cfRule type="containsBlanks" dxfId="64" priority="49">
       <formula>LEN(TRIM(K208))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="66" priority="74" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="63" priority="74" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="65" priority="75" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="62" priority="75" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsBlanks" dxfId="64" priority="46">
+    <cfRule type="containsBlanks" dxfId="61" priority="46">
       <formula>LEN(TRIM(K215))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="63" priority="71" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="60" priority="71" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="62" priority="72" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="59" priority="72" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsBlanks" dxfId="61" priority="43">
+    <cfRule type="containsBlanks" dxfId="58" priority="43">
       <formula>LEN(TRIM(K217))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsText" dxfId="60" priority="68" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="57" priority="68" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsText" dxfId="59" priority="69" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="56" priority="69" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219">
-    <cfRule type="containsBlanks" dxfId="58" priority="40">
+    <cfRule type="containsBlanks" dxfId="55" priority="40">
       <formula>LEN(TRIM(K219))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsText" dxfId="57" priority="65" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="54" priority="65" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsText" dxfId="56" priority="66" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="53" priority="66" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220 K237:K238 K225:K235">
-    <cfRule type="containsText" dxfId="55" priority="62" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="52" priority="62" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K220))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220 K237:K238 K225:K235">
-    <cfRule type="containsText" dxfId="54" priority="63" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="51" priority="63" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K220))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="53" priority="56" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="50" priority="56" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="52" priority="57" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="49" priority="57" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="51" priority="53" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="48" priority="53" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="50" priority="54" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="47" priority="54" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="47" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="44" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="46" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="43" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="45" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="42" priority="44" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="41" priority="45" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219">
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K219))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219">
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K219))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236">
-    <cfRule type="containsBlanks" dxfId="41" priority="37">
+    <cfRule type="containsBlanks" dxfId="38" priority="37">
       <formula>LEN(TRIM(K236))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236">
-    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236">
-    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221">
-    <cfRule type="containsBlanks" dxfId="38" priority="34">
+    <cfRule type="containsBlanks" dxfId="35" priority="34">
       <formula>LEN(TRIM(K221))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221">
-    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K221))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221">
-    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K221))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K222:K224">
-    <cfRule type="containsBlanks" dxfId="35" priority="31">
+    <cfRule type="containsBlanks" dxfId="32" priority="31">
       <formula>LEN(TRIM(K222))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K222:K224">
-    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K222))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K222:K224">
-    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K222))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsBlanks" dxfId="32" priority="28">
+    <cfRule type="containsBlanks" dxfId="29" priority="28">
       <formula>LEN(TRIM(K239))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240:K242">
-    <cfRule type="containsBlanks" dxfId="29" priority="25">
+    <cfRule type="containsBlanks" dxfId="26" priority="25">
       <formula>LEN(TRIM(K240))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240:K242">
-    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K240))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240:K242">
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K240))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K243">
-    <cfRule type="containsBlanks" dxfId="26" priority="22">
+    <cfRule type="containsBlanks" dxfId="23" priority="22">
       <formula>LEN(TRIM(K243))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K243">
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K243))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K243">
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K243))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K244">
-    <cfRule type="containsBlanks" dxfId="23" priority="19">
+    <cfRule type="containsBlanks" dxfId="20" priority="19">
       <formula>LEN(TRIM(K244))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K244">
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K244))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K244">
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K244))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K158">
-    <cfRule type="containsBlanks" dxfId="20" priority="16">
+    <cfRule type="containsBlanks" dxfId="17" priority="16">
       <formula>LEN(TRIM(K158))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K158">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K158))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K158">
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K158))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K245:K246">
-    <cfRule type="containsBlanks" dxfId="17" priority="13">
+    <cfRule type="containsBlanks" dxfId="14" priority="13">
       <formula>LEN(TRIM(K245))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K245:K246">
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K245))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K245:K246">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K245))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247">
-    <cfRule type="containsBlanks" dxfId="14" priority="10">
+    <cfRule type="containsBlanks" dxfId="11" priority="10">
       <formula>LEN(TRIM(K247))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K247))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247">
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K247))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K248:K250">
-    <cfRule type="containsBlanks" dxfId="11" priority="7">
+    <cfRule type="containsBlanks" dxfId="8" priority="7">
       <formula>LEN(TRIM(K248))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K248:K250">
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K248))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K248:K250">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K248))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K251:K252">
-    <cfRule type="containsBlanks" dxfId="8" priority="4">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
       <formula>LEN(TRIM(K251))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K251:K252">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K251))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K251:K252">
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K251))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(K98))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K98))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K98))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added tests for 1932
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="328">
   <si>
     <t>Test Number</t>
   </si>
@@ -989,6 +989,18 @@
   </si>
   <si>
     <t>Adding a New PV to a component gives it a unique name to start with</t>
+  </si>
+  <si>
+    <t>Menu Items</t>
+  </si>
+  <si>
+    <t>Whilst pointing to an instrument that you do not have write permission for (or is offline) the synoptic menu items are greyed out</t>
+  </si>
+  <si>
+    <t>Whilst pointing to an instrument that you do not have write permission for the editing config menu items are greyed out</t>
+  </si>
+  <si>
+    <t>Whilst pointing to an instrument that you do not have write permission for the edit current config menu item becomes view config item</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1360,133 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="93">
+  <dxfs count="102">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2951,8 +3089,8 @@
   <dimension ref="A1:N1075"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J177" sqref="J177"/>
+      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I256" sqref="I256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10317,66 +10455,113 @@
       <c r="L252" s="26"/>
       <c r="M252" s="6"/>
     </row>
-    <row r="253" spans="1:13" ht="15">
+    <row r="253" spans="1:13" ht="39">
       <c r="A253">
+        <v>31</v>
+      </c>
+      <c r="B253">
+        <f t="shared" ref="B253" si="57">IF(A253=A252,B252+1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C253" s="3" t="str">
+        <f t="shared" ref="C253" si="58">CONCATENATE(A253,"-",B253)</f>
+        <v>31-1</v>
+      </c>
+      <c r="D253" s="23"/>
+      <c r="E253" s="23"/>
+      <c r="F253" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="G253" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="H253" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="I253" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="J253" s="23"/>
+      <c r="K253" s="21"/>
+      <c r="L253" s="26"/>
+      <c r="M253" s="6"/>
+    </row>
+    <row r="254" spans="1:13" ht="39">
+      <c r="A254">
         <f t="shared" si="56"/>
-        <v>30</v>
-      </c>
-      <c r="B253">
+        <v>31</v>
+      </c>
+      <c r="B254">
+        <f t="shared" si="54"/>
+        <v>2</v>
+      </c>
+      <c r="C254" s="3" t="str">
+        <f t="shared" si="55"/>
+        <v>31-2</v>
+      </c>
+      <c r="D254" s="23"/>
+      <c r="E254" s="23"/>
+      <c r="F254" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="G254" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="H254" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="I254" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="J254" s="23"/>
+      <c r="K254" s="21"/>
+      <c r="L254" s="26"/>
+      <c r="M254" s="6"/>
+    </row>
+    <row r="255" spans="1:13" ht="39">
+      <c r="A255">
+        <f t="shared" si="56"/>
+        <v>31</v>
+      </c>
+      <c r="B255">
         <f t="shared" si="54"/>
         <v>3</v>
       </c>
-      <c r="C253" s="3" t="str">
-        <f t="shared" si="55"/>
-        <v>30-3</v>
-      </c>
-      <c r="L253" s="6"/>
-      <c r="M253" s="6"/>
-    </row>
-    <row r="254" spans="1:13" ht="15">
-      <c r="A254">
-        <f t="shared" si="56"/>
-        <v>30</v>
-      </c>
-      <c r="B254">
-        <f t="shared" si="54"/>
-        <v>4</v>
-      </c>
-      <c r="C254" s="3" t="str">
-        <f t="shared" si="55"/>
-        <v>30-4</v>
-      </c>
-      <c r="L254" s="6"/>
-      <c r="M254" s="6"/>
-    </row>
-    <row r="255" spans="1:13" ht="15">
-      <c r="A255">
-        <f t="shared" si="56"/>
-        <v>30</v>
-      </c>
-      <c r="B255">
-        <f t="shared" si="54"/>
-        <v>5</v>
-      </c>
       <c r="C255" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-5</v>
-      </c>
-      <c r="L255" s="6"/>
+        <v>31-3</v>
+      </c>
+      <c r="D255" s="23"/>
+      <c r="E255" s="23"/>
+      <c r="F255" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="G255" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="H255" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="I255" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="J255" s="23"/>
+      <c r="K255" s="21"/>
+      <c r="L255" s="26"/>
       <c r="M255" s="6"/>
     </row>
     <row r="256" spans="1:13" ht="15">
       <c r="A256">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B256">
         <f t="shared" si="54"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C256" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-6</v>
+        <v>31-4</v>
       </c>
       <c r="L256" s="6"/>
       <c r="M256" s="6"/>
@@ -10384,15 +10569,15 @@
     <row r="257" spans="1:13" ht="15">
       <c r="A257">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B257">
         <f t="shared" si="54"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C257" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-7</v>
+        <v>31-5</v>
       </c>
       <c r="L257" s="6"/>
       <c r="M257" s="6"/>
@@ -10400,15 +10585,15 @@
     <row r="258" spans="1:13" ht="15">
       <c r="A258">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B258">
         <f t="shared" si="54"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C258" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-8</v>
+        <v>31-6</v>
       </c>
       <c r="L258" s="6"/>
       <c r="M258" s="6"/>
@@ -10416,15 +10601,15 @@
     <row r="259" spans="1:13" ht="15">
       <c r="A259">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B259">
         <f t="shared" si="54"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C259" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-9</v>
+        <v>31-7</v>
       </c>
       <c r="L259" s="6"/>
       <c r="M259" s="6"/>
@@ -10432,15 +10617,15 @@
     <row r="260" spans="1:13" ht="15">
       <c r="A260">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B260">
         <f t="shared" si="54"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C260" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-10</v>
+        <v>31-8</v>
       </c>
       <c r="L260" s="6"/>
       <c r="M260" s="6"/>
@@ -10448,15 +10633,15 @@
     <row r="261" spans="1:13" ht="15">
       <c r="A261">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B261">
         <f t="shared" si="54"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C261" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-11</v>
+        <v>31-9</v>
       </c>
       <c r="L261" s="6"/>
       <c r="M261" s="6"/>
@@ -10464,15 +10649,15 @@
     <row r="262" spans="1:13" ht="15">
       <c r="A262">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B262">
         <f t="shared" si="54"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C262" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-12</v>
+        <v>31-10</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
@@ -10480,15 +10665,15 @@
     <row r="263" spans="1:13" ht="15">
       <c r="A263">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B263">
         <f t="shared" si="54"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C263" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-13</v>
+        <v>31-11</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
@@ -10496,15 +10681,15 @@
     <row r="264" spans="1:13" ht="15">
       <c r="A264">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B264">
         <f t="shared" si="54"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C264" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-14</v>
+        <v>31-12</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
@@ -10512,15 +10697,15 @@
     <row r="265" spans="1:13" ht="15">
       <c r="A265">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B265">
         <f t="shared" si="54"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C265" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-15</v>
+        <v>31-13</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
@@ -10528,15 +10713,15 @@
     <row r="266" spans="1:13" ht="15">
       <c r="A266">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B266">
         <f t="shared" si="54"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C266" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-16</v>
+        <v>31-14</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
@@ -10544,15 +10729,15 @@
     <row r="267" spans="1:13" ht="15">
       <c r="A267">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B267">
         <f t="shared" si="54"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C267" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-17</v>
+        <v>31-15</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
@@ -10560,15 +10745,15 @@
     <row r="268" spans="1:13" ht="15">
       <c r="A268">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B268">
         <f t="shared" si="54"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C268" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-18</v>
+        <v>31-16</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
@@ -10576,15 +10761,15 @@
     <row r="269" spans="1:13" ht="15">
       <c r="A269">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B269">
         <f t="shared" si="54"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C269" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-19</v>
+        <v>31-17</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
@@ -10592,15 +10777,15 @@
     <row r="270" spans="1:13" ht="15">
       <c r="A270">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B270">
         <f t="shared" si="54"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C270" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-20</v>
+        <v>31-18</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
@@ -10608,15 +10793,15 @@
     <row r="271" spans="1:13" ht="15">
       <c r="A271">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B271">
         <f t="shared" si="54"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C271" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-21</v>
+        <v>31-19</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
@@ -10624,15 +10809,15 @@
     <row r="272" spans="1:13" ht="15">
       <c r="A272">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B272">
         <f t="shared" si="54"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C272" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-22</v>
+        <v>31-20</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
@@ -10640,15 +10825,15 @@
     <row r="273" spans="1:13" ht="15">
       <c r="A273">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B273">
         <f t="shared" si="54"/>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C273" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-23</v>
+        <v>31-21</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
@@ -10656,15 +10841,15 @@
     <row r="274" spans="1:13" ht="15">
       <c r="A274">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B274">
         <f t="shared" si="54"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C274" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-24</v>
+        <v>31-22</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
@@ -10672,15 +10857,15 @@
     <row r="275" spans="1:13" ht="15">
       <c r="A275">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B275">
         <f t="shared" si="54"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C275" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-25</v>
+        <v>31-23</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
@@ -10688,15 +10873,15 @@
     <row r="276" spans="1:13" ht="15">
       <c r="A276">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B276">
         <f t="shared" si="54"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C276" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-26</v>
+        <v>31-24</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
@@ -10704,15 +10889,15 @@
     <row r="277" spans="1:13" ht="15">
       <c r="A277">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B277">
         <f t="shared" si="54"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C277" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-27</v>
+        <v>31-25</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
@@ -10720,15 +10905,15 @@
     <row r="278" spans="1:13" ht="15">
       <c r="A278">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B278">
         <f t="shared" si="54"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C278" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-28</v>
+        <v>31-26</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
@@ -10736,15 +10921,15 @@
     <row r="279" spans="1:13" ht="15">
       <c r="A279">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B279">
         <f t="shared" si="54"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C279" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-29</v>
+        <v>31-27</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
@@ -10752,15 +10937,15 @@
     <row r="280" spans="1:13" ht="15">
       <c r="A280">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B280">
         <f t="shared" si="54"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C280" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-30</v>
+        <v>31-28</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
@@ -10768,15 +10953,15 @@
     <row r="281" spans="1:13" ht="15">
       <c r="A281">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B281">
         <f t="shared" si="54"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C281" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-31</v>
+        <v>31-29</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
@@ -10784,15 +10969,15 @@
     <row r="282" spans="1:13" ht="15">
       <c r="A282">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B282">
         <f t="shared" si="54"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C282" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-32</v>
+        <v>31-30</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
@@ -10800,15 +10985,15 @@
     <row r="283" spans="1:13" ht="15">
       <c r="A283">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B283">
         <f t="shared" si="54"/>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C283" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-33</v>
+        <v>31-31</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
@@ -10816,15 +11001,15 @@
     <row r="284" spans="1:13" ht="15">
       <c r="A284">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B284">
         <f t="shared" si="54"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C284" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-34</v>
+        <v>31-32</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
@@ -10832,15 +11017,15 @@
     <row r="285" spans="1:13" ht="15">
       <c r="A285">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B285">
         <f t="shared" si="54"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C285" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-35</v>
+        <v>31-33</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
@@ -10848,15 +11033,15 @@
     <row r="286" spans="1:13" ht="15">
       <c r="A286">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B286">
         <f t="shared" si="54"/>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C286" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-36</v>
+        <v>31-34</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
@@ -10864,15 +11049,15 @@
     <row r="287" spans="1:13" ht="15">
       <c r="A287">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B287">
         <f t="shared" si="54"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C287" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-37</v>
+        <v>31-35</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
@@ -10880,15 +11065,15 @@
     <row r="288" spans="1:13" ht="15">
       <c r="A288">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B288">
         <f t="shared" si="54"/>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C288" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-38</v>
+        <v>31-36</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
@@ -10896,15 +11081,15 @@
     <row r="289" spans="1:13" ht="15">
       <c r="A289">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B289">
         <f t="shared" si="54"/>
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C289" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-39</v>
+        <v>31-37</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
@@ -10912,15 +11097,15 @@
     <row r="290" spans="1:13" ht="15">
       <c r="A290">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B290">
         <f t="shared" si="54"/>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C290" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-40</v>
+        <v>31-38</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
@@ -10928,15 +11113,15 @@
     <row r="291" spans="1:13" ht="15">
       <c r="A291">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B291">
         <f t="shared" si="54"/>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C291" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-41</v>
+        <v>31-39</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
@@ -10944,15 +11129,15 @@
     <row r="292" spans="1:13" ht="15">
       <c r="A292">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B292">
         <f t="shared" si="54"/>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C292" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-42</v>
+        <v>31-40</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
@@ -10960,15 +11145,15 @@
     <row r="293" spans="1:13" ht="15">
       <c r="A293">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B293">
         <f t="shared" si="54"/>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C293" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-43</v>
+        <v>31-41</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
@@ -10976,15 +11161,15 @@
     <row r="294" spans="1:13" ht="15">
       <c r="A294">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B294">
         <f t="shared" si="54"/>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C294" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-44</v>
+        <v>31-42</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
@@ -10992,15 +11177,15 @@
     <row r="295" spans="1:13" ht="15">
       <c r="A295">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B295">
         <f t="shared" si="54"/>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C295" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-45</v>
+        <v>31-43</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
@@ -11008,15 +11193,15 @@
     <row r="296" spans="1:13" ht="15">
       <c r="A296">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B296">
         <f t="shared" si="54"/>
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C296" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-46</v>
+        <v>31-44</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
@@ -11024,15 +11209,15 @@
     <row r="297" spans="1:13" ht="15">
       <c r="A297">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B297">
         <f t="shared" si="54"/>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C297" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-47</v>
+        <v>31-45</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
@@ -11040,15 +11225,15 @@
     <row r="298" spans="1:13" ht="15">
       <c r="A298">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B298">
         <f t="shared" si="54"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C298" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-48</v>
+        <v>31-46</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
@@ -11056,15 +11241,15 @@
     <row r="299" spans="1:13" ht="15">
       <c r="A299">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B299">
         <f t="shared" si="54"/>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C299" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-49</v>
+        <v>31-47</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
@@ -11072,15 +11257,15 @@
     <row r="300" spans="1:13" ht="15">
       <c r="A300">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B300">
         <f t="shared" si="54"/>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C300" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-50</v>
+        <v>31-48</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
@@ -11088,15 +11273,15 @@
     <row r="301" spans="1:13" ht="15">
       <c r="A301">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B301">
         <f t="shared" si="54"/>
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C301" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-51</v>
+        <v>31-49</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
@@ -11104,15 +11289,15 @@
     <row r="302" spans="1:13" ht="15">
       <c r="A302">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B302">
         <f t="shared" si="54"/>
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C302" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-52</v>
+        <v>31-50</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
@@ -11120,1375 +11305,1375 @@
     <row r="303" spans="1:13" ht="15">
       <c r="A303">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B303">
-        <f t="shared" ref="B303:B366" si="57">IF(A303=A302,B302+1,1)</f>
-        <v>53</v>
+        <f t="shared" ref="B303:B366" si="59">IF(A303=A302,B302+1,1)</f>
+        <v>51</v>
       </c>
       <c r="C303" s="3" t="str">
-        <f t="shared" ref="C303:C366" si="58">CONCATENATE(A303,"-",B303)</f>
-        <v>30-53</v>
+        <f t="shared" ref="C303:C366" si="60">CONCATENATE(A303,"-",B303)</f>
+        <v>31-51</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
     </row>
     <row r="304" spans="1:13" ht="15">
       <c r="A304">
-        <f t="shared" ref="A304:A367" si="59">A303</f>
-        <v>30</v>
+        <f t="shared" ref="A304:A367" si="61">A303</f>
+        <v>31</v>
       </c>
       <c r="B304">
-        <f t="shared" si="57"/>
-        <v>54</v>
+        <f t="shared" si="59"/>
+        <v>52</v>
       </c>
       <c r="C304" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-54</v>
+        <f t="shared" si="60"/>
+        <v>31-52</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
     </row>
     <row r="305" spans="1:13" ht="15">
       <c r="A305">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B305">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B305">
-        <f t="shared" si="57"/>
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C305" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-55</v>
+        <f t="shared" si="60"/>
+        <v>31-53</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
     </row>
     <row r="306" spans="1:13" ht="15">
       <c r="A306">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B306">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B306">
-        <f t="shared" si="57"/>
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C306" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-56</v>
+        <f t="shared" si="60"/>
+        <v>31-54</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
     </row>
     <row r="307" spans="1:13" ht="15">
       <c r="A307">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B307">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B307">
-        <f t="shared" si="57"/>
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C307" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-57</v>
+        <f t="shared" si="60"/>
+        <v>31-55</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
     </row>
     <row r="308" spans="1:13" ht="15">
       <c r="A308">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B308">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B308">
-        <f t="shared" si="57"/>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C308" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-58</v>
+        <f t="shared" si="60"/>
+        <v>31-56</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
     </row>
     <row r="309" spans="1:13" ht="15">
       <c r="A309">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B309">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B309">
-        <f t="shared" si="57"/>
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C309" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-59</v>
+        <f t="shared" si="60"/>
+        <v>31-57</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
     </row>
     <row r="310" spans="1:13" ht="15">
       <c r="A310">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B310">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B310">
-        <f t="shared" si="57"/>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C310" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-60</v>
+        <f t="shared" si="60"/>
+        <v>31-58</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
     </row>
     <row r="311" spans="1:13" ht="15">
       <c r="A311">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B311">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B311">
-        <f t="shared" si="57"/>
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C311" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-61</v>
+        <f t="shared" si="60"/>
+        <v>31-59</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
     </row>
     <row r="312" spans="1:13" ht="15">
       <c r="A312">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B312">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B312">
-        <f t="shared" si="57"/>
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C312" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-62</v>
+        <f t="shared" si="60"/>
+        <v>31-60</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
     </row>
     <row r="313" spans="1:13" ht="15">
       <c r="A313">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B313">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B313">
-        <f t="shared" si="57"/>
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C313" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-63</v>
+        <f t="shared" si="60"/>
+        <v>31-61</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
     </row>
     <row r="314" spans="1:13" ht="15">
       <c r="A314">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B314">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B314">
-        <f t="shared" si="57"/>
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C314" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-64</v>
+        <f t="shared" si="60"/>
+        <v>31-62</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
     </row>
     <row r="315" spans="1:13" ht="15">
       <c r="A315">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B315">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B315">
-        <f t="shared" si="57"/>
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C315" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-65</v>
+        <f t="shared" si="60"/>
+        <v>31-63</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
     </row>
     <row r="316" spans="1:13" ht="15">
       <c r="A316">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B316">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B316">
-        <f t="shared" si="57"/>
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C316" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-66</v>
+        <f t="shared" si="60"/>
+        <v>31-64</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
     </row>
     <row r="317" spans="1:13" ht="15">
       <c r="A317">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B317">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B317">
-        <f t="shared" si="57"/>
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C317" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-67</v>
+        <f t="shared" si="60"/>
+        <v>31-65</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
     </row>
     <row r="318" spans="1:13" ht="15">
       <c r="A318">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B318">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B318">
-        <f t="shared" si="57"/>
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C318" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-68</v>
+        <f t="shared" si="60"/>
+        <v>31-66</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
     </row>
     <row r="319" spans="1:13" ht="15">
       <c r="A319">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B319">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B319">
-        <f t="shared" si="57"/>
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C319" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-69</v>
+        <f t="shared" si="60"/>
+        <v>31-67</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
     </row>
     <row r="320" spans="1:13" ht="15">
       <c r="A320">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B320">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B320">
-        <f t="shared" si="57"/>
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C320" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-70</v>
+        <f t="shared" si="60"/>
+        <v>31-68</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
     </row>
     <row r="321" spans="1:13" ht="15">
       <c r="A321">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B321">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B321">
-        <f t="shared" si="57"/>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C321" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-71</v>
+        <f t="shared" si="60"/>
+        <v>31-69</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
     </row>
     <row r="322" spans="1:13" ht="15">
       <c r="A322">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B322">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B322">
-        <f t="shared" si="57"/>
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C322" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-72</v>
+        <f t="shared" si="60"/>
+        <v>31-70</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
     </row>
     <row r="323" spans="1:13" ht="15">
       <c r="A323">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B323">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B323">
-        <f t="shared" si="57"/>
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C323" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-73</v>
+        <f t="shared" si="60"/>
+        <v>31-71</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
     </row>
     <row r="324" spans="1:13" ht="15">
       <c r="A324">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B324">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B324">
-        <f t="shared" si="57"/>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C324" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-74</v>
+        <f t="shared" si="60"/>
+        <v>31-72</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
     </row>
     <row r="325" spans="1:13" ht="15">
       <c r="A325">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B325">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B325">
-        <f t="shared" si="57"/>
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C325" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-75</v>
+        <f t="shared" si="60"/>
+        <v>31-73</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
     </row>
     <row r="326" spans="1:13" ht="15">
       <c r="A326">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B326">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B326">
-        <f t="shared" si="57"/>
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C326" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-76</v>
+        <f t="shared" si="60"/>
+        <v>31-74</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
     </row>
     <row r="327" spans="1:13" ht="15">
       <c r="A327">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B327">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B327">
-        <f t="shared" si="57"/>
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C327" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-77</v>
+        <f t="shared" si="60"/>
+        <v>31-75</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
     </row>
     <row r="328" spans="1:13" ht="15">
       <c r="A328">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B328">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B328">
-        <f t="shared" si="57"/>
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C328" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-78</v>
+        <f t="shared" si="60"/>
+        <v>31-76</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
     </row>
     <row r="329" spans="1:13" ht="15">
       <c r="A329">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B329">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B329">
-        <f t="shared" si="57"/>
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C329" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-79</v>
+        <f t="shared" si="60"/>
+        <v>31-77</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
     </row>
     <row r="330" spans="1:13" ht="15">
       <c r="A330">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B330">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B330">
-        <f t="shared" si="57"/>
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C330" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-80</v>
+        <f t="shared" si="60"/>
+        <v>31-78</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
     </row>
     <row r="331" spans="1:13" ht="15">
       <c r="A331">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B331">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B331">
-        <f t="shared" si="57"/>
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C331" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-81</v>
+        <f t="shared" si="60"/>
+        <v>31-79</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
     </row>
     <row r="332" spans="1:13" ht="15">
       <c r="A332">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B332">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B332">
-        <f t="shared" si="57"/>
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C332" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-82</v>
+        <f t="shared" si="60"/>
+        <v>31-80</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
     </row>
     <row r="333" spans="1:13" ht="15">
       <c r="A333">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B333">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B333">
-        <f t="shared" si="57"/>
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C333" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-83</v>
+        <f t="shared" si="60"/>
+        <v>31-81</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
     </row>
     <row r="334" spans="1:13" ht="15">
       <c r="A334">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B334">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B334">
-        <f t="shared" si="57"/>
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C334" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-84</v>
+        <f t="shared" si="60"/>
+        <v>31-82</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
     </row>
     <row r="335" spans="1:13" ht="15">
       <c r="A335">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B335">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B335">
-        <f t="shared" si="57"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C335" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-85</v>
+        <f t="shared" si="60"/>
+        <v>31-83</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
     </row>
     <row r="336" spans="1:13" ht="15">
       <c r="A336">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B336">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B336">
-        <f t="shared" si="57"/>
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C336" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-86</v>
+        <f t="shared" si="60"/>
+        <v>31-84</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
     </row>
     <row r="337" spans="1:13" ht="15">
       <c r="A337">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B337">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B337">
-        <f t="shared" si="57"/>
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C337" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-87</v>
+        <f t="shared" si="60"/>
+        <v>31-85</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
     </row>
     <row r="338" spans="1:13" ht="15">
       <c r="A338">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B338">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B338">
-        <f t="shared" si="57"/>
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C338" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-88</v>
+        <f t="shared" si="60"/>
+        <v>31-86</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
     </row>
     <row r="339" spans="1:13" ht="15">
       <c r="A339">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B339">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B339">
-        <f t="shared" si="57"/>
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C339" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-89</v>
+        <f t="shared" si="60"/>
+        <v>31-87</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
     </row>
     <row r="340" spans="1:13" ht="15">
       <c r="A340">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B340">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B340">
-        <f t="shared" si="57"/>
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C340" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-90</v>
+        <f t="shared" si="60"/>
+        <v>31-88</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
     </row>
     <row r="341" spans="1:13" ht="15">
       <c r="A341">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B341">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B341">
-        <f t="shared" si="57"/>
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C341" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-91</v>
+        <f t="shared" si="60"/>
+        <v>31-89</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
     </row>
     <row r="342" spans="1:13" ht="15">
       <c r="A342">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B342">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B342">
-        <f t="shared" si="57"/>
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C342" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-92</v>
+        <f t="shared" si="60"/>
+        <v>31-90</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
     </row>
     <row r="343" spans="1:13" ht="15">
       <c r="A343">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B343">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B343">
-        <f t="shared" si="57"/>
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C343" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-93</v>
+        <f t="shared" si="60"/>
+        <v>31-91</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
     </row>
     <row r="344" spans="1:13" ht="15">
       <c r="A344">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B344">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B344">
-        <f t="shared" si="57"/>
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C344" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-94</v>
+        <f t="shared" si="60"/>
+        <v>31-92</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
     </row>
     <row r="345" spans="1:13" ht="15">
       <c r="A345">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B345">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B345">
-        <f t="shared" si="57"/>
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C345" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-95</v>
+        <f t="shared" si="60"/>
+        <v>31-93</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
     </row>
     <row r="346" spans="1:13" ht="15">
       <c r="A346">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B346">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B346">
-        <f t="shared" si="57"/>
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C346" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-96</v>
+        <f t="shared" si="60"/>
+        <v>31-94</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
     </row>
     <row r="347" spans="1:13" ht="15">
       <c r="A347">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B347">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B347">
-        <f t="shared" si="57"/>
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C347" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-97</v>
+        <f t="shared" si="60"/>
+        <v>31-95</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
     </row>
     <row r="348" spans="1:13" ht="15">
       <c r="A348">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B348">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B348">
-        <f t="shared" si="57"/>
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C348" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-98</v>
+        <f t="shared" si="60"/>
+        <v>31-96</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
     </row>
     <row r="349" spans="1:13" ht="15">
       <c r="A349">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B349">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B349">
-        <f t="shared" si="57"/>
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C349" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-99</v>
+        <f t="shared" si="60"/>
+        <v>31-97</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
     </row>
     <row r="350" spans="1:13" ht="15">
       <c r="A350">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B350">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B350">
-        <f t="shared" si="57"/>
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C350" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-100</v>
+        <f t="shared" si="60"/>
+        <v>31-98</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
     </row>
     <row r="351" spans="1:13" ht="15">
       <c r="A351">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B351">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B351">
-        <f t="shared" si="57"/>
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C351" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-101</v>
+        <f t="shared" si="60"/>
+        <v>31-99</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
     </row>
     <row r="352" spans="1:13" ht="15">
       <c r="A352">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B352">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B352">
-        <f t="shared" si="57"/>
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C352" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-102</v>
+        <f t="shared" si="60"/>
+        <v>31-100</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
     </row>
     <row r="353" spans="1:13" ht="15">
       <c r="A353">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B353">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B353">
-        <f t="shared" si="57"/>
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C353" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-103</v>
+        <f t="shared" si="60"/>
+        <v>31-101</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
     </row>
     <row r="354" spans="1:13" ht="15">
       <c r="A354">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B354">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B354">
-        <f t="shared" si="57"/>
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C354" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-104</v>
+        <f t="shared" si="60"/>
+        <v>31-102</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
     </row>
     <row r="355" spans="1:13" ht="15">
       <c r="A355">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B355">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B355">
-        <f t="shared" si="57"/>
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C355" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-105</v>
+        <f t="shared" si="60"/>
+        <v>31-103</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
     </row>
     <row r="356" spans="1:13" ht="15">
       <c r="A356">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B356">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B356">
-        <f t="shared" si="57"/>
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C356" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-106</v>
+        <f t="shared" si="60"/>
+        <v>31-104</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
     </row>
     <row r="357" spans="1:13" ht="15">
       <c r="A357">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B357">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B357">
-        <f t="shared" si="57"/>
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C357" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-107</v>
+        <f t="shared" si="60"/>
+        <v>31-105</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
     </row>
     <row r="358" spans="1:13" ht="15">
       <c r="A358">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B358">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B358">
-        <f t="shared" si="57"/>
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C358" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-108</v>
+        <f t="shared" si="60"/>
+        <v>31-106</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
     </row>
     <row r="359" spans="1:13" ht="15">
       <c r="A359">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B359">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B359">
-        <f t="shared" si="57"/>
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C359" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-109</v>
+        <f t="shared" si="60"/>
+        <v>31-107</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
     </row>
     <row r="360" spans="1:13" ht="15">
       <c r="A360">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B360">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B360">
-        <f t="shared" si="57"/>
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C360" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-110</v>
+        <f t="shared" si="60"/>
+        <v>31-108</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
     </row>
     <row r="361" spans="1:13" ht="15">
       <c r="A361">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B361">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B361">
-        <f t="shared" si="57"/>
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C361" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-111</v>
+        <f t="shared" si="60"/>
+        <v>31-109</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
     </row>
     <row r="362" spans="1:13" ht="15">
       <c r="A362">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B362">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B362">
-        <f t="shared" si="57"/>
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C362" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-112</v>
+        <f t="shared" si="60"/>
+        <v>31-110</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
     </row>
     <row r="363" spans="1:13" ht="15">
       <c r="A363">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B363">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B363">
-        <f t="shared" si="57"/>
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C363" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-113</v>
+        <f t="shared" si="60"/>
+        <v>31-111</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
     </row>
     <row r="364" spans="1:13" ht="15">
       <c r="A364">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B364">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B364">
-        <f t="shared" si="57"/>
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C364" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-114</v>
+        <f t="shared" si="60"/>
+        <v>31-112</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
     </row>
     <row r="365" spans="1:13" ht="15">
       <c r="A365">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B365">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B365">
-        <f t="shared" si="57"/>
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C365" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-115</v>
+        <f t="shared" si="60"/>
+        <v>31-113</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
     </row>
     <row r="366" spans="1:13" ht="15">
       <c r="A366">
+        <f t="shared" si="61"/>
+        <v>31</v>
+      </c>
+      <c r="B366">
         <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="B366">
-        <f t="shared" si="57"/>
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C366" s="3" t="str">
-        <f t="shared" si="58"/>
-        <v>30-116</v>
+        <f t="shared" si="60"/>
+        <v>31-114</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
     </row>
     <row r="367" spans="1:13" ht="15">
       <c r="A367">
-        <f t="shared" si="59"/>
-        <v>30</v>
+        <f t="shared" si="61"/>
+        <v>31</v>
       </c>
       <c r="B367">
-        <f t="shared" ref="B367:B388" si="60">IF(A367=A366,B366+1,1)</f>
-        <v>117</v>
+        <f t="shared" ref="B367:B388" si="62">IF(A367=A366,B366+1,1)</f>
+        <v>115</v>
       </c>
       <c r="C367" s="3" t="str">
-        <f t="shared" ref="C367:C388" si="61">CONCATENATE(A367,"-",B367)</f>
-        <v>30-117</v>
+        <f t="shared" ref="C367:C388" si="63">CONCATENATE(A367,"-",B367)</f>
+        <v>31-115</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
     </row>
     <row r="368" spans="1:13" ht="15">
       <c r="A368">
-        <f t="shared" ref="A368:A388" si="62">A367</f>
-        <v>30</v>
+        <f t="shared" ref="A368:A388" si="64">A367</f>
+        <v>31</v>
       </c>
       <c r="B368">
-        <f t="shared" si="60"/>
-        <v>118</v>
+        <f t="shared" si="62"/>
+        <v>116</v>
       </c>
       <c r="C368" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-118</v>
+        <f t="shared" si="63"/>
+        <v>31-116</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
     </row>
     <row r="369" spans="1:13" ht="15">
       <c r="A369">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B369">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B369">
-        <f t="shared" si="60"/>
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C369" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-119</v>
+        <f t="shared" si="63"/>
+        <v>31-117</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
     </row>
     <row r="370" spans="1:13" ht="15">
       <c r="A370">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B370">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B370">
-        <f t="shared" si="60"/>
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C370" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-120</v>
+        <f t="shared" si="63"/>
+        <v>31-118</v>
       </c>
       <c r="L370" s="6"/>
       <c r="M370" s="6"/>
     </row>
     <row r="371" spans="1:13" ht="15">
       <c r="A371">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B371">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B371">
-        <f t="shared" si="60"/>
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C371" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-121</v>
+        <f t="shared" si="63"/>
+        <v>31-119</v>
       </c>
       <c r="L371" s="6"/>
       <c r="M371" s="6"/>
     </row>
     <row r="372" spans="1:13" ht="15">
       <c r="A372">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B372">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B372">
-        <f t="shared" si="60"/>
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C372" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-122</v>
+        <f t="shared" si="63"/>
+        <v>31-120</v>
       </c>
       <c r="L372" s="6"/>
       <c r="M372" s="6"/>
     </row>
     <row r="373" spans="1:13" ht="15">
       <c r="A373">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B373">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B373">
-        <f t="shared" si="60"/>
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C373" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-123</v>
+        <f t="shared" si="63"/>
+        <v>31-121</v>
       </c>
       <c r="L373" s="6"/>
       <c r="M373" s="6"/>
     </row>
     <row r="374" spans="1:13" ht="15">
       <c r="A374">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B374">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B374">
-        <f t="shared" si="60"/>
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C374" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-124</v>
+        <f t="shared" si="63"/>
+        <v>31-122</v>
       </c>
       <c r="L374" s="6"/>
       <c r="M374" s="6"/>
     </row>
     <row r="375" spans="1:13" ht="15">
       <c r="A375">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B375">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B375">
-        <f t="shared" si="60"/>
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C375" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-125</v>
+        <f t="shared" si="63"/>
+        <v>31-123</v>
       </c>
       <c r="L375" s="6"/>
       <c r="M375" s="6"/>
     </row>
     <row r="376" spans="1:13" ht="15">
       <c r="A376">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B376">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B376">
-        <f t="shared" si="60"/>
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C376" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-126</v>
+        <f t="shared" si="63"/>
+        <v>31-124</v>
       </c>
       <c r="L376" s="6"/>
       <c r="M376" s="6"/>
     </row>
     <row r="377" spans="1:13" ht="15">
       <c r="A377">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B377">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B377">
-        <f t="shared" si="60"/>
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C377" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-127</v>
+        <f t="shared" si="63"/>
+        <v>31-125</v>
       </c>
       <c r="L377" s="6"/>
       <c r="M377" s="6"/>
     </row>
     <row r="378" spans="1:13" ht="15">
       <c r="A378">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B378">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B378">
-        <f t="shared" si="60"/>
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C378" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-128</v>
+        <f t="shared" si="63"/>
+        <v>31-126</v>
       </c>
       <c r="L378" s="6"/>
       <c r="M378" s="6"/>
     </row>
     <row r="379" spans="1:13" ht="15">
       <c r="A379">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B379">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B379">
-        <f t="shared" si="60"/>
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C379" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-129</v>
+        <f t="shared" si="63"/>
+        <v>31-127</v>
       </c>
       <c r="L379" s="6"/>
       <c r="M379" s="6"/>
     </row>
     <row r="380" spans="1:13" ht="15">
       <c r="A380">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B380">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B380">
-        <f t="shared" si="60"/>
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C380" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-130</v>
+        <f t="shared" si="63"/>
+        <v>31-128</v>
       </c>
       <c r="L380" s="6"/>
       <c r="M380" s="6"/>
     </row>
     <row r="381" spans="1:13" ht="15">
       <c r="A381">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B381">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B381">
-        <f t="shared" si="60"/>
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C381" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-131</v>
+        <f t="shared" si="63"/>
+        <v>31-129</v>
       </c>
       <c r="L381" s="6"/>
       <c r="M381" s="6"/>
     </row>
     <row r="382" spans="1:13" ht="15">
       <c r="A382">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B382">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B382">
-        <f t="shared" si="60"/>
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C382" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-132</v>
+        <f t="shared" si="63"/>
+        <v>31-130</v>
       </c>
       <c r="L382" s="6"/>
       <c r="M382" s="6"/>
     </row>
     <row r="383" spans="1:13" ht="15">
       <c r="A383">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B383">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B383">
-        <f t="shared" si="60"/>
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C383" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-133</v>
+        <f t="shared" si="63"/>
+        <v>31-131</v>
       </c>
       <c r="L383" s="6"/>
       <c r="M383" s="6"/>
     </row>
     <row r="384" spans="1:13" ht="15">
       <c r="A384">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B384">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B384">
-        <f t="shared" si="60"/>
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C384" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-134</v>
+        <f t="shared" si="63"/>
+        <v>31-132</v>
       </c>
       <c r="L384" s="6"/>
       <c r="M384" s="6"/>
     </row>
     <row r="385" spans="1:13" ht="15">
       <c r="A385">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B385">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B385">
-        <f t="shared" si="60"/>
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C385" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-135</v>
+        <f t="shared" si="63"/>
+        <v>31-133</v>
       </c>
       <c r="L385" s="6"/>
       <c r="M385" s="6"/>
     </row>
     <row r="386" spans="1:13" ht="15">
       <c r="A386">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B386">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B386">
-        <f t="shared" si="60"/>
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C386" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-136</v>
+        <f t="shared" si="63"/>
+        <v>31-134</v>
       </c>
       <c r="L386" s="6"/>
       <c r="M386" s="6"/>
     </row>
     <row r="387" spans="1:13" ht="15">
       <c r="A387">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B387">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B387">
-        <f t="shared" si="60"/>
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C387" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-137</v>
+        <f t="shared" si="63"/>
+        <v>31-135</v>
       </c>
       <c r="L387" s="6"/>
       <c r="M387" s="6"/>
     </row>
     <row r="388" spans="1:13" ht="15">
       <c r="A388">
+        <f t="shared" si="64"/>
+        <v>31</v>
+      </c>
+      <c r="B388">
         <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="B388">
-        <f t="shared" si="60"/>
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C388" s="3" t="str">
-        <f t="shared" si="61"/>
-        <v>30-138</v>
+        <f t="shared" si="63"/>
+        <v>31-136</v>
       </c>
       <c r="L388" s="6"/>
       <c r="M388" s="6"/>
@@ -15248,467 +15433,467 @@
     <mergeCell ref="L245:L250"/>
   </mergeCells>
   <conditionalFormatting sqref="K159:K203 K99:K157 K2:K97">
-    <cfRule type="containsBlanks" dxfId="92" priority="97">
+    <cfRule type="containsBlanks" dxfId="101" priority="97">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K159:K203 K99:K157 K2:K97">
-    <cfRule type="containsText" dxfId="91" priority="98" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="100" priority="98" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K159:K203 K99:K157 K2:K97">
-    <cfRule type="containsText" dxfId="90" priority="99" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="99" priority="99" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="89" priority="94">
+    <cfRule type="containsBlanks" dxfId="98" priority="94">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="88" priority="95" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="97" priority="95" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="87" priority="96" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="96" priority="96" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="86" priority="88">
+    <cfRule type="containsBlanks" dxfId="95" priority="88">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="85" priority="89" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="94" priority="89" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="84" priority="90" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="93" priority="90" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="83" priority="85">
+    <cfRule type="containsBlanks" dxfId="92" priority="85">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="82" priority="86" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="91" priority="86" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="81" priority="87" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="90" priority="87" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsBlanks" dxfId="80" priority="82">
+    <cfRule type="containsBlanks" dxfId="89" priority="82">
       <formula>LEN(TRIM(K207))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="88" priority="83" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="78" priority="84" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="87" priority="84" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsBlanks" dxfId="77" priority="79">
+    <cfRule type="containsBlanks" dxfId="86" priority="79">
       <formula>LEN(TRIM(K209))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsBlanks" dxfId="76" priority="76">
+    <cfRule type="containsBlanks" dxfId="85" priority="76">
       <formula>LEN(TRIM(K211))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsBlanks" dxfId="75" priority="73">
+    <cfRule type="containsBlanks" dxfId="84" priority="73">
       <formula>LEN(TRIM(K213))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsBlanks" dxfId="74" priority="70">
+    <cfRule type="containsBlanks" dxfId="83" priority="70">
       <formula>LEN(TRIM(K214))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsBlanks" dxfId="73" priority="67">
+    <cfRule type="containsBlanks" dxfId="82" priority="67">
       <formula>LEN(TRIM(K216))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsBlanks" dxfId="72" priority="64">
+    <cfRule type="containsBlanks" dxfId="81" priority="64">
       <formula>LEN(TRIM(K218))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220 K237:K238 K225:K235">
-    <cfRule type="containsBlanks" dxfId="71" priority="61">
+    <cfRule type="containsBlanks" dxfId="80" priority="61">
       <formula>LEN(TRIM(K220))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsBlanks" dxfId="70" priority="55">
+    <cfRule type="containsBlanks" dxfId="79" priority="55">
       <formula>LEN(TRIM(K210))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="69" priority="80" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="78" priority="80" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="68" priority="81" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="77" priority="81" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsBlanks" dxfId="67" priority="52">
+    <cfRule type="containsBlanks" dxfId="76" priority="52">
       <formula>LEN(TRIM(K212))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="66" priority="77" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="75" priority="77" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="65" priority="78" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="74" priority="78" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsBlanks" dxfId="64" priority="49">
+    <cfRule type="containsBlanks" dxfId="73" priority="49">
       <formula>LEN(TRIM(K208))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="63" priority="74" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="72" priority="74" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="62" priority="75" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="71" priority="75" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsBlanks" dxfId="61" priority="46">
+    <cfRule type="containsBlanks" dxfId="70" priority="46">
       <formula>LEN(TRIM(K215))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="60" priority="71" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="69" priority="71" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="59" priority="72" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="68" priority="72" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsBlanks" dxfId="58" priority="43">
+    <cfRule type="containsBlanks" dxfId="67" priority="43">
       <formula>LEN(TRIM(K217))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsText" dxfId="57" priority="68" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="66" priority="68" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsText" dxfId="56" priority="69" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="65" priority="69" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219">
-    <cfRule type="containsBlanks" dxfId="55" priority="40">
+    <cfRule type="containsBlanks" dxfId="64" priority="40">
       <formula>LEN(TRIM(K219))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsText" dxfId="54" priority="65" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="63" priority="65" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsText" dxfId="53" priority="66" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="62" priority="66" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220 K237:K238 K225:K235">
-    <cfRule type="containsText" dxfId="52" priority="62" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K220))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220 K237:K238 K225:K235">
-    <cfRule type="containsText" dxfId="51" priority="63" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K220))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="50" priority="56" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="59" priority="56" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="49" priority="57" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="58" priority="57" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="48" priority="53" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="57" priority="53" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="47" priority="54" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="56" priority="54" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="55" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="54" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="44" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="53" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="43" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="52" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="42" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="51" priority="44" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="41" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="50" priority="45" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219">
-    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="49" priority="41" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K219))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219">
-    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="48" priority="42" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K219))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236">
-    <cfRule type="containsBlanks" dxfId="38" priority="37">
+    <cfRule type="containsBlanks" dxfId="47" priority="37">
       <formula>LEN(TRIM(K236))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236">
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="46" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236">
-    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="45" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221">
-    <cfRule type="containsBlanks" dxfId="35" priority="34">
+    <cfRule type="containsBlanks" dxfId="44" priority="34">
       <formula>LEN(TRIM(K221))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="43" priority="35" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K221))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221">
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="42" priority="36" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K221))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K222:K224">
-    <cfRule type="containsBlanks" dxfId="32" priority="31">
+    <cfRule type="containsBlanks" dxfId="41" priority="31">
       <formula>LEN(TRIM(K222))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K222:K224">
-    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="40" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K222))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K222:K224">
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="39" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K222))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsBlanks" dxfId="29" priority="28">
+    <cfRule type="containsBlanks" dxfId="38" priority="28">
       <formula>LEN(TRIM(K239))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="37" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="36" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240:K242">
-    <cfRule type="containsBlanks" dxfId="26" priority="25">
+    <cfRule type="containsBlanks" dxfId="35" priority="25">
       <formula>LEN(TRIM(K240))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240:K242">
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="34" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K240))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240:K242">
-    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K240))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K243">
-    <cfRule type="containsBlanks" dxfId="23" priority="22">
+    <cfRule type="containsBlanks" dxfId="32" priority="22">
       <formula>LEN(TRIM(K243))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K243">
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="31" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K243))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K243">
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="30" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K243))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K244">
-    <cfRule type="containsBlanks" dxfId="20" priority="19">
+    <cfRule type="containsBlanks" dxfId="29" priority="19">
       <formula>LEN(TRIM(K244))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K244">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="28" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K244))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K244">
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K244))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K158">
-    <cfRule type="containsBlanks" dxfId="17" priority="16">
+    <cfRule type="containsBlanks" dxfId="26" priority="16">
       <formula>LEN(TRIM(K158))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K158">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="25" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K158))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K158">
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="24" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K158))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K245:K246">
-    <cfRule type="containsBlanks" dxfId="14" priority="13">
+    <cfRule type="containsBlanks" dxfId="23" priority="13">
       <formula>LEN(TRIM(K245))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K245:K246">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K245))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K245:K246">
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K245))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247">
-    <cfRule type="containsBlanks" dxfId="11" priority="10">
+    <cfRule type="containsBlanks" dxfId="20" priority="10">
       <formula>LEN(TRIM(K247))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K247))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247">
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K247))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K248:K250">
-    <cfRule type="containsBlanks" dxfId="8" priority="7">
+    <cfRule type="containsBlanks" dxfId="17" priority="7">
       <formula>LEN(TRIM(K248))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K248:K250">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K248))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K248:K250">
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K248))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K251:K252">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
+  <conditionalFormatting sqref="K251:K255">
+    <cfRule type="containsBlanks" dxfId="14" priority="4">
       <formula>LEN(TRIM(K251))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K251:K252">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K251:K255">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K251))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K251:K252">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
+  <conditionalFormatting sqref="K251:K255">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K251))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="11" priority="1">
       <formula>LEN(TRIM(K98))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K98))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K98))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added testing for java version into 3-2
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -108,9 +108,6 @@
     <t>Gui launches</t>
   </si>
   <si>
-    <t>help/about in GUI is expected values (double-check with Jenkins build/commit numbers)</t>
-  </si>
-  <si>
     <t>Dashboard Perspective</t>
   </si>
   <si>
@@ -1007,6 +1004,9 @@
   </si>
   <si>
     <t>Holding SHIFT whilst pressing any key multiple times does not cause changes to perspective switcher text</t>
+  </si>
+  <si>
+    <t>help/about in GUI is expected values (double-check with Jenkins build/commit numbers and java version)</t>
   </si>
 </sst>
 </file>
@@ -1366,49 +1366,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="102">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="96">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2753,48 +2711,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3095,8 +3011,8 @@
   <dimension ref="A1:N1077"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J244" sqref="J244"/>
+      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L265" sqref="L265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3117,10 +3033,10 @@
   <sheetData>
     <row r="1" spans="1:14" ht="57">
       <c r="A1" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>217</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>218</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -3144,7 +3060,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>7</v>
@@ -3174,10 +3090,10 @@
         <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>212</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>213</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="8"/>
@@ -3543,7 +3459,7 @@
       <c r="K15" s="7"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:14" ht="30">
+    <row r="16" spans="1:14" ht="45">
       <c r="A16">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -3564,7 +3480,7 @@
         <v>28</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>30</v>
+        <v>329</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="7"/>
@@ -3588,10 +3504,10 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="7"/>
@@ -3618,7 +3534,7 @@
         <v>17</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="7"/>
@@ -3645,7 +3561,7 @@
         <v>17</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="7"/>
@@ -3669,10 +3585,10 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="7"/>
@@ -3696,10 +3612,10 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="7"/>
@@ -3723,10 +3639,10 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="7"/>
@@ -3749,10 +3665,10 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="7"/>
@@ -3776,10 +3692,10 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="7"/>
@@ -3802,10 +3718,10 @@
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="7"/>
@@ -3830,10 +3746,10 @@
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="7"/>
@@ -3858,10 +3774,10 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="7"/>
@@ -3886,10 +3802,10 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="7"/>
@@ -3913,10 +3829,10 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="7"/>
@@ -3933,28 +3849,28 @@
         <v>2</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K30" s="7"/>
       <c r="L30" s="8"/>
@@ -3977,13 +3893,13 @@
       <c r="E31" s="5"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="J31" s="8"/>
       <c r="K31" s="7"/>
@@ -4007,13 +3923,13 @@
       <c r="E32" s="5"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="7"/>
@@ -4037,13 +3953,13 @@
       <c r="E33" s="5"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="7"/>
@@ -4067,13 +3983,13 @@
       <c r="E34" s="5"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="7"/>
@@ -4097,13 +4013,13 @@
       <c r="E35" s="5"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="7"/>
@@ -4127,13 +4043,13 @@
       <c r="E36" s="5"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="7"/>
@@ -4157,13 +4073,13 @@
       <c r="E37" s="5"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="7"/>
@@ -4187,13 +4103,13 @@
       <c r="E38" s="5"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="7"/>
@@ -4216,14 +4132,14 @@
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="7"/>
@@ -4246,14 +4162,14 @@
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G40" s="7"/>
       <c r="H40" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="7"/>
@@ -4276,13 +4192,13 @@
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="9"/>
@@ -4306,13 +4222,13 @@
       <c r="E42" s="30"/>
       <c r="F42" s="31"/>
       <c r="G42" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H42" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I42" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J42" s="32"/>
       <c r="K42" s="31"/>
@@ -4336,13 +4252,13 @@
       <c r="E43" s="5"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H43" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J43" s="8"/>
       <c r="K43" s="7"/>
@@ -4366,13 +4282,13 @@
       <c r="E44" s="5"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H44" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J44" s="8"/>
       <c r="K44" s="7"/>
@@ -4396,13 +4312,13 @@
       <c r="E45" s="5"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H45" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="7"/>
@@ -4426,13 +4342,13 @@
       <c r="E46" s="5"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H46" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="7"/>
@@ -4456,13 +4372,13 @@
       <c r="E47" s="5"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H47" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="7"/>
@@ -4485,17 +4401,17 @@
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G48" s="9"/>
       <c r="H48" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K48" s="9"/>
       <c r="L48" s="8"/>
@@ -4517,17 +4433,17 @@
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G49" s="9"/>
       <c r="H49" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J49" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K49" s="9"/>
       <c r="L49" s="8"/>
@@ -4548,14 +4464,14 @@
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G50" s="7"/>
       <c r="H50" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J50" s="9"/>
       <c r="K50" s="7"/>
@@ -4579,13 +4495,13 @@
       <c r="E51" s="5"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H51" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H51" s="7" t="s">
+      <c r="I51" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J51" s="8"/>
       <c r="K51" s="7"/>
@@ -4609,13 +4525,13 @@
       <c r="E52" s="5"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H52" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H52" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="I52" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J52" s="8"/>
       <c r="K52" s="7"/>
@@ -4639,13 +4555,13 @@
       <c r="E53" s="5"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H53" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H53" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="I53" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="7"/>
@@ -4668,14 +4584,14 @@
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G54" s="7"/>
       <c r="H54" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J54" s="8"/>
       <c r="K54" s="7"/>
@@ -4699,13 +4615,13 @@
       <c r="E55" s="5"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="J55" s="8"/>
       <c r="K55" s="7"/>
@@ -4730,17 +4646,17 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="I56" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="I56" s="8" t="s">
+      <c r="J56" s="8" t="s">
         <v>280</v>
-      </c>
-      <c r="J56" s="8" t="s">
-        <v>281</v>
       </c>
       <c r="K56" s="9"/>
       <c r="L56" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M56" s="6"/>
     </row>
@@ -4762,17 +4678,17 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J57" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K57" s="9"/>
       <c r="L57" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M57" s="6"/>
     </row>
@@ -4794,17 +4710,17 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J58" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K58" s="9"/>
       <c r="L58" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M58" s="6"/>
     </row>
@@ -4826,17 +4742,17 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J59" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K59" s="9"/>
       <c r="L59" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M59" s="6"/>
     </row>
@@ -4859,7 +4775,7 @@
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
       <c r="I60" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J60" s="8"/>
       <c r="K60" s="9"/>
@@ -4882,13 +4798,13 @@
       <c r="E61" s="5"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J61" s="8"/>
       <c r="K61" s="7"/>
@@ -4912,13 +4828,13 @@
       <c r="E62" s="5"/>
       <c r="F62" s="7"/>
       <c r="G62" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H62" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I62" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="J62" s="8"/>
       <c r="K62" s="7"/>
@@ -4942,13 +4858,13 @@
       <c r="E63" s="5"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J63" s="8"/>
       <c r="K63" s="7"/>
@@ -4972,13 +4888,13 @@
       <c r="E64" s="5"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J64" s="8"/>
       <c r="K64" s="7"/>
@@ -5002,13 +4918,13 @@
       <c r="E65" s="5"/>
       <c r="F65" s="7"/>
       <c r="G65" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J65" s="8"/>
       <c r="K65" s="7"/>
@@ -5032,13 +4948,13 @@
       <c r="E66" s="5"/>
       <c r="F66" s="7"/>
       <c r="G66" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="7"/>
@@ -5062,13 +4978,13 @@
       <c r="E67" s="5"/>
       <c r="F67" s="7"/>
       <c r="G67" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J67" s="8"/>
       <c r="K67" s="7"/>
@@ -5092,13 +5008,13 @@
       <c r="E68" s="5"/>
       <c r="F68" s="7"/>
       <c r="G68" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J68" s="8"/>
       <c r="K68" s="7"/>
@@ -5122,13 +5038,13 @@
       <c r="E69" s="5"/>
       <c r="F69" s="7"/>
       <c r="G69" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J69" s="8"/>
       <c r="K69" s="7"/>
@@ -5152,13 +5068,13 @@
       <c r="E70" s="5"/>
       <c r="F70" s="7"/>
       <c r="G70" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="7"/>
@@ -5175,28 +5091,28 @@
         <v>11</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K71" s="9"/>
       <c r="L71" s="8"/>
@@ -5218,19 +5134,19 @@
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
       <c r="F72" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I72" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="G72" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="H72" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I72" s="8" t="s">
+      <c r="J72" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="J72" s="8" t="s">
-        <v>244</v>
       </c>
       <c r="K72" s="9"/>
       <c r="L72" s="8"/>
@@ -5253,23 +5169,23 @@
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H73" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I73" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="J73" s="8" t="s">
         <v>245</v>
-      </c>
-      <c r="J73" s="8" t="s">
-        <v>246</v>
       </c>
       <c r="K73" s="9"/>
       <c r="L73" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M73" s="6"/>
     </row>
@@ -5289,16 +5205,16 @@
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G74" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G74" s="7" t="s">
+      <c r="H74" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="H74" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="7"/>
@@ -5323,10 +5239,10 @@
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J75" s="8"/>
       <c r="K75" s="7"/>
@@ -5350,10 +5266,10 @@
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
       <c r="H76" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J76" s="8"/>
       <c r="K76" s="7"/>
@@ -5378,10 +5294,10 @@
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
       <c r="H77" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="J77" s="8"/>
       <c r="K77" s="7"/>
@@ -5406,10 +5322,10 @@
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
       <c r="H78" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="7"/>
@@ -5434,10 +5350,10 @@
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
       <c r="H79" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J79" s="8"/>
       <c r="K79" s="7"/>
@@ -5461,10 +5377,10 @@
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
       <c r="H80" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J80" s="8"/>
       <c r="K80" s="7"/>
@@ -5489,10 +5405,10 @@
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
       <c r="H81" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I81" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="J81" s="8"/>
       <c r="K81" s="7"/>
@@ -5517,13 +5433,13 @@
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
       <c r="H82" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I82" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J82" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="J82" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="K82" s="7"/>
       <c r="L82" s="8"/>
@@ -5547,13 +5463,13 @@
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
       <c r="H83" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J83" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K83" s="7"/>
       <c r="L83" s="1"/>
@@ -5577,13 +5493,13 @@
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
       <c r="H84" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I84" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="J84" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="J84" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="K84" s="9"/>
       <c r="L84" s="8"/>
@@ -5604,13 +5520,13 @@
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
       <c r="H85" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J85" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K85" s="9"/>
       <c r="L85" s="8"/>
@@ -5633,16 +5549,16 @@
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
       <c r="G86" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H86" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I86" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="J86" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="J86" s="8" t="s">
-        <v>224</v>
       </c>
       <c r="K86" s="9"/>
       <c r="L86" s="8"/>
@@ -5666,10 +5582,10 @@
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
       <c r="H87" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J87" s="8"/>
       <c r="K87" s="7"/>
@@ -5694,10 +5610,10 @@
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
       <c r="H88" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J88" s="8"/>
       <c r="K88" s="7"/>
@@ -5722,10 +5638,10 @@
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
       <c r="H89" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J89" s="8"/>
       <c r="K89" s="7"/>
@@ -5750,10 +5666,10 @@
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
       <c r="H90" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J90" s="8"/>
       <c r="K90" s="7"/>
@@ -5777,10 +5693,10 @@
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
       <c r="H91" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J91" s="8"/>
       <c r="K91" s="7"/>
@@ -5805,10 +5721,10 @@
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
       <c r="H92" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I92" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="J92" s="8"/>
       <c r="K92" s="7"/>
@@ -5833,10 +5749,10 @@
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
       <c r="H93" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J93" s="8"/>
       <c r="K93" s="7"/>
@@ -5861,10 +5777,10 @@
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
       <c r="H94" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J94" s="8"/>
       <c r="K94" s="7"/>
@@ -5889,10 +5805,10 @@
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
       <c r="H95" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I95" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="J95" s="8"/>
       <c r="K95" s="7"/>
@@ -5917,10 +5833,10 @@
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
       <c r="H96" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J96" s="8"/>
       <c r="K96" s="1"/>
@@ -5944,10 +5860,10 @@
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
       <c r="H97" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J97" s="8"/>
       <c r="K97" s="7"/>
@@ -5972,15 +5888,15 @@
       <c r="F98" s="9"/>
       <c r="G98" s="9"/>
       <c r="H98" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J98" s="8"/>
       <c r="K98" s="9"/>
       <c r="L98" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="15">
@@ -5999,13 +5915,13 @@
       <c r="E99" s="5"/>
       <c r="F99" s="7"/>
       <c r="G99" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H99" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I99" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="J99" s="8"/>
       <c r="K99" s="7"/>
@@ -6029,13 +5945,13 @@
       <c r="E100" s="5"/>
       <c r="F100" s="7"/>
       <c r="G100" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J100" s="8"/>
       <c r="K100" s="7"/>
@@ -6059,10 +5975,10 @@
       <c r="F101" s="7"/>
       <c r="G101" s="7"/>
       <c r="H101" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I101" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="J101" s="8"/>
       <c r="K101" s="7"/>
@@ -6087,10 +6003,10 @@
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
       <c r="H102" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J102" s="8"/>
       <c r="K102" s="7"/>
@@ -6115,10 +6031,10 @@
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
       <c r="H103" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J103" s="8"/>
       <c r="K103" s="7"/>
@@ -6143,10 +6059,10 @@
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
       <c r="H104" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J104" s="8"/>
       <c r="K104" s="7"/>
@@ -6171,10 +6087,10 @@
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
       <c r="H105" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J105" s="8"/>
       <c r="K105" s="7"/>
@@ -6199,10 +6115,10 @@
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
       <c r="H106" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J106" s="8"/>
       <c r="K106" s="7"/>
@@ -6227,10 +6143,10 @@
       <c r="F107" s="7"/>
       <c r="G107" s="7"/>
       <c r="H107" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J107" s="8"/>
       <c r="K107" s="7"/>
@@ -6255,10 +6171,10 @@
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
       <c r="H108" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J108" s="8"/>
       <c r="K108" s="7"/>
@@ -6283,10 +6199,10 @@
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
       <c r="H109" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J109" s="8"/>
       <c r="K109" s="7"/>
@@ -6311,10 +6227,10 @@
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
       <c r="H110" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J110" s="8"/>
       <c r="K110" s="7"/>
@@ -6339,10 +6255,10 @@
       <c r="F111" s="9"/>
       <c r="G111" s="9"/>
       <c r="H111" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I111" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J111" s="8"/>
       <c r="K111" s="9"/>
@@ -6367,10 +6283,10 @@
       <c r="F112" s="9"/>
       <c r="G112" s="9"/>
       <c r="H112" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I112" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J112" s="8"/>
       <c r="K112" s="9"/>
@@ -6395,10 +6311,10 @@
       <c r="F113" s="9"/>
       <c r="G113" s="9"/>
       <c r="H113" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I113" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J113" s="8"/>
       <c r="K113" s="9"/>
@@ -6423,10 +6339,10 @@
       <c r="F114" s="7"/>
       <c r="G114" s="7"/>
       <c r="H114" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J114" s="8"/>
       <c r="K114" s="7"/>
@@ -6451,10 +6367,10 @@
       <c r="F115" s="7"/>
       <c r="G115" s="7"/>
       <c r="H115" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J115" s="8"/>
       <c r="K115" s="7"/>
@@ -6479,10 +6395,10 @@
       <c r="F116" s="7"/>
       <c r="G116" s="7"/>
       <c r="H116" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J116" s="8"/>
       <c r="K116" s="7"/>
@@ -6507,10 +6423,10 @@
       <c r="F117" s="7"/>
       <c r="G117" s="7"/>
       <c r="H117" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J117" s="8"/>
       <c r="K117" s="7"/>
@@ -6535,10 +6451,10 @@
       <c r="F118" s="7"/>
       <c r="G118" s="7"/>
       <c r="H118" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J118" s="8"/>
       <c r="K118" s="7"/>
@@ -6563,10 +6479,10 @@
       <c r="F119" s="7"/>
       <c r="G119" s="7"/>
       <c r="H119" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J119" s="8"/>
       <c r="K119" s="7"/>
@@ -6591,10 +6507,10 @@
       <c r="F120" s="7"/>
       <c r="G120" s="7"/>
       <c r="H120" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J120" s="8"/>
       <c r="K120" s="7"/>
@@ -6619,10 +6535,10 @@
       <c r="F121" s="7"/>
       <c r="G121" s="7"/>
       <c r="H121" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J121" s="8"/>
       <c r="K121" s="7"/>
@@ -6647,10 +6563,10 @@
       <c r="F122" s="7"/>
       <c r="G122" s="7"/>
       <c r="H122" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J122" s="8"/>
       <c r="K122" s="7"/>
@@ -6675,10 +6591,10 @@
       <c r="F123" s="7"/>
       <c r="G123" s="7"/>
       <c r="H123" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J123" s="8"/>
       <c r="K123" s="7"/>
@@ -6703,10 +6619,10 @@
       <c r="F124" s="7"/>
       <c r="G124" s="7"/>
       <c r="H124" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J124" s="8"/>
       <c r="K124" s="7"/>
@@ -6731,10 +6647,10 @@
       <c r="F125" s="7"/>
       <c r="G125" s="7"/>
       <c r="H125" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J125" s="8"/>
       <c r="K125" s="7"/>
@@ -6759,10 +6675,10 @@
       <c r="F126" s="7"/>
       <c r="G126" s="7"/>
       <c r="H126" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J126" s="8"/>
       <c r="K126" s="7"/>
@@ -6787,10 +6703,10 @@
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
       <c r="H127" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J127" s="8"/>
       <c r="K127" s="7"/>
@@ -6815,10 +6731,10 @@
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
       <c r="H128" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J128" s="8"/>
       <c r="K128" s="7"/>
@@ -6843,10 +6759,10 @@
       <c r="F129" s="7"/>
       <c r="G129" s="7"/>
       <c r="H129" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J129" s="8"/>
       <c r="K129" s="7"/>
@@ -6871,10 +6787,10 @@
       <c r="F130" s="7"/>
       <c r="G130" s="7"/>
       <c r="H130" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J130" s="8"/>
       <c r="K130" s="7"/>
@@ -6899,10 +6815,10 @@
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
       <c r="H131" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J131" s="8"/>
       <c r="K131" s="7"/>
@@ -6927,10 +6843,10 @@
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
       <c r="H132" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J132" s="8"/>
       <c r="K132" s="7"/>
@@ -6955,10 +6871,10 @@
       <c r="F133" s="9"/>
       <c r="G133" s="9"/>
       <c r="H133" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I133" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J133" s="8"/>
       <c r="K133" s="9"/>
@@ -6983,10 +6899,10 @@
       <c r="F134" s="7"/>
       <c r="G134" s="7"/>
       <c r="H134" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J134" s="8"/>
       <c r="K134" s="7"/>
@@ -7011,10 +6927,10 @@
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
       <c r="H135" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J135" s="8"/>
       <c r="K135" s="7"/>
@@ -7039,10 +6955,10 @@
       <c r="F136" s="7"/>
       <c r="G136" s="7"/>
       <c r="H136" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J136" s="8"/>
       <c r="K136" s="7"/>
@@ -7067,10 +6983,10 @@
       <c r="F137" s="7"/>
       <c r="G137" s="7"/>
       <c r="H137" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J137" s="8"/>
       <c r="K137" s="7"/>
@@ -7095,10 +7011,10 @@
       <c r="F138" s="7"/>
       <c r="G138" s="7"/>
       <c r="H138" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J138" s="8"/>
       <c r="K138" s="7"/>
@@ -7123,10 +7039,10 @@
       <c r="F139" s="7"/>
       <c r="G139" s="7"/>
       <c r="H139" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J139" s="8"/>
       <c r="K139" s="7"/>
@@ -7151,10 +7067,10 @@
       <c r="F140" s="7"/>
       <c r="G140" s="7"/>
       <c r="H140" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J140" s="8"/>
       <c r="K140" s="7"/>
@@ -7179,10 +7095,10 @@
       <c r="F141" s="7"/>
       <c r="G141" s="7"/>
       <c r="H141" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J141" s="8"/>
       <c r="K141" s="7"/>
@@ -7207,10 +7123,10 @@
       <c r="F142" s="7"/>
       <c r="G142" s="7"/>
       <c r="H142" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J142" s="8"/>
       <c r="K142" s="7"/>
@@ -7235,10 +7151,10 @@
       <c r="F143" s="7"/>
       <c r="G143" s="7"/>
       <c r="H143" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J143" s="8"/>
       <c r="K143" s="7"/>
@@ -7263,10 +7179,10 @@
       <c r="F144" s="7"/>
       <c r="G144" s="7"/>
       <c r="H144" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J144" s="8"/>
       <c r="K144" s="7"/>
@@ -7291,10 +7207,10 @@
       <c r="F145" s="7"/>
       <c r="G145" s="7"/>
       <c r="H145" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J145" s="8"/>
       <c r="K145" s="7"/>
@@ -7319,10 +7235,10 @@
       <c r="F146" s="7"/>
       <c r="G146" s="7"/>
       <c r="H146" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J146" s="8"/>
       <c r="K146" s="7"/>
@@ -7347,10 +7263,10 @@
       <c r="F147" s="7"/>
       <c r="G147" s="7"/>
       <c r="H147" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J147" s="8"/>
       <c r="K147" s="7"/>
@@ -7375,10 +7291,10 @@
       <c r="F148" s="7"/>
       <c r="G148" s="7"/>
       <c r="H148" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J148" s="8"/>
       <c r="K148" s="7"/>
@@ -7403,10 +7319,10 @@
       <c r="F149" s="7"/>
       <c r="G149" s="7"/>
       <c r="H149" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J149" s="8"/>
       <c r="K149" s="7"/>
@@ -7431,10 +7347,10 @@
       <c r="F150" s="7"/>
       <c r="G150" s="7"/>
       <c r="H150" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J150" s="8"/>
       <c r="K150" s="7"/>
@@ -7459,10 +7375,10 @@
       <c r="F151" s="7"/>
       <c r="G151" s="7"/>
       <c r="H151" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J151" s="8"/>
       <c r="K151" s="5"/>
@@ -7487,10 +7403,10 @@
       <c r="F152" s="7"/>
       <c r="G152" s="7"/>
       <c r="H152" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J152" s="8"/>
       <c r="K152" s="7"/>
@@ -7515,10 +7431,10 @@
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
       <c r="H153" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="I153" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="I153" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="J153" s="8"/>
       <c r="K153" s="7"/>
@@ -7543,10 +7459,10 @@
       <c r="F154" s="41"/>
       <c r="G154" s="41"/>
       <c r="H154" s="41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I154" s="42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J154" s="8"/>
       <c r="K154" s="7"/>
@@ -7571,10 +7487,10 @@
       <c r="F155" s="46"/>
       <c r="G155" s="46"/>
       <c r="H155" s="46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I155" s="47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J155" s="40"/>
       <c r="K155" s="7"/>
@@ -7599,10 +7515,10 @@
       <c r="F156" s="46"/>
       <c r="G156" s="46"/>
       <c r="H156" s="46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I156" s="48" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J156" s="40"/>
       <c r="K156" s="9"/>
@@ -7627,10 +7543,10 @@
       <c r="F157" s="46"/>
       <c r="G157" s="46"/>
       <c r="H157" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I157" s="48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J157" s="40"/>
       <c r="K157" s="9"/>
@@ -7655,10 +7571,10 @@
       <c r="F158" s="46"/>
       <c r="G158" s="46"/>
       <c r="H158" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I158" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J158" s="40"/>
       <c r="K158" s="9"/>
@@ -7680,14 +7596,14 @@
       <c r="D159" s="46"/>
       <c r="E159" s="46"/>
       <c r="F159" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G159" s="46"/>
       <c r="H159" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I159" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J159" s="40"/>
       <c r="K159" s="7"/>
@@ -7710,14 +7626,14 @@
       <c r="D160" s="46"/>
       <c r="E160" s="46"/>
       <c r="F160" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G160" s="46"/>
       <c r="H160" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I160" s="47" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J160" s="40"/>
       <c r="K160" s="7"/>
@@ -7740,14 +7656,14 @@
       <c r="D161" s="46"/>
       <c r="E161" s="46"/>
       <c r="F161" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G161" s="46"/>
       <c r="H161" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I161" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J161" s="40"/>
       <c r="K161" s="7"/>
@@ -7769,14 +7685,14 @@
       <c r="D162" s="46"/>
       <c r="E162" s="46"/>
       <c r="F162" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G162" s="46"/>
       <c r="H162" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I162" s="47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J162" s="40"/>
       <c r="K162" s="7"/>
@@ -7800,13 +7716,13 @@
       <c r="E163" s="46"/>
       <c r="F163" s="46"/>
       <c r="G163" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H163" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I163" s="47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J163" s="40"/>
       <c r="K163" s="7"/>
@@ -7830,13 +7746,13 @@
       <c r="E164" s="46"/>
       <c r="F164" s="46"/>
       <c r="G164" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H164" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I164" s="47" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J164" s="40"/>
       <c r="K164" s="7"/>
@@ -7860,13 +7776,13 @@
       <c r="E165" s="44"/>
       <c r="F165" s="44"/>
       <c r="G165" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H165" s="44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I165" s="45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J165" s="8"/>
       <c r="K165" s="7"/>
@@ -7890,13 +7806,13 @@
       <c r="E166" s="5"/>
       <c r="F166" s="7"/>
       <c r="G166" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H166" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J166" s="8"/>
       <c r="K166" s="7"/>
@@ -7919,13 +7835,13 @@
       <c r="E167" s="5"/>
       <c r="F167" s="7"/>
       <c r="G167" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H167" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J167" s="8"/>
       <c r="K167" s="7"/>
@@ -7949,13 +7865,13 @@
       <c r="E168" s="5"/>
       <c r="F168" s="7"/>
       <c r="G168" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H168" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J168" s="8"/>
       <c r="K168" s="7"/>
@@ -7979,13 +7895,13 @@
       <c r="E169" s="5"/>
       <c r="F169" s="7"/>
       <c r="G169" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H169" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J169" s="8"/>
       <c r="K169" s="7"/>
@@ -8009,13 +7925,13 @@
       <c r="E170" s="5"/>
       <c r="F170" s="7"/>
       <c r="G170" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H170" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J170" s="8"/>
       <c r="K170" s="7"/>
@@ -8039,13 +7955,13 @@
       <c r="E171" s="5"/>
       <c r="F171" s="7"/>
       <c r="G171" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H171" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J171" s="8"/>
       <c r="K171" s="7"/>
@@ -8069,13 +7985,13 @@
       <c r="E172" s="5"/>
       <c r="F172" s="7"/>
       <c r="G172" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H172" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J172" s="8"/>
       <c r="K172" s="7"/>
@@ -8099,13 +8015,13 @@
       <c r="E173" s="5"/>
       <c r="F173" s="7"/>
       <c r="G173" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H173" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J173" s="8"/>
       <c r="K173" s="7"/>
@@ -8129,13 +8045,13 @@
       <c r="E174" s="5"/>
       <c r="F174" s="7"/>
       <c r="G174" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H174" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I174" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J174" s="8"/>
       <c r="K174" s="7"/>
@@ -8158,14 +8074,14 @@
       <c r="D175" s="5"/>
       <c r="E175" s="5"/>
       <c r="F175" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G175" s="7"/>
       <c r="H175" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I175" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J175" s="8"/>
       <c r="K175" s="7"/>
@@ -8189,13 +8105,13 @@
       <c r="E176" s="9"/>
       <c r="F176" s="9"/>
       <c r="G176" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H176" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I176" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J176" s="8"/>
       <c r="K176" s="9"/>
@@ -8219,13 +8135,13 @@
       <c r="E177" s="9"/>
       <c r="F177" s="9"/>
       <c r="G177" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H177" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I177" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J177" s="8"/>
       <c r="K177" s="9"/>
@@ -8249,13 +8165,13 @@
       <c r="E178" s="5"/>
       <c r="F178" s="7"/>
       <c r="G178" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="H178" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I178" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="H178" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="I178" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="J178" s="8"/>
       <c r="K178" s="7"/>
@@ -8279,13 +8195,13 @@
       <c r="E179" s="5"/>
       <c r="F179" s="7"/>
       <c r="G179" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H179" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="I179" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="I179" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="J179" s="8"/>
       <c r="K179" s="7"/>
@@ -8309,13 +8225,13 @@
       <c r="E180" s="5"/>
       <c r="F180" s="7"/>
       <c r="G180" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H180" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I180" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J180" s="8"/>
       <c r="K180" s="7"/>
@@ -8339,13 +8255,13 @@
       <c r="E181" s="5"/>
       <c r="F181" s="7"/>
       <c r="G181" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H181" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J181" s="8"/>
       <c r="K181" s="7"/>
@@ -8369,13 +8285,13 @@
       <c r="E182" s="5"/>
       <c r="F182" s="7"/>
       <c r="G182" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H182" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J182" s="8"/>
       <c r="K182" s="7"/>
@@ -8399,13 +8315,13 @@
       <c r="E183" s="9"/>
       <c r="F183" s="9"/>
       <c r="G183" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H183" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I183" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J183" s="8"/>
       <c r="K183" s="9"/>
@@ -8428,13 +8344,13 @@
       <c r="E184" s="5"/>
       <c r="F184" s="7"/>
       <c r="G184" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H184" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="I184" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="I184" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="J184" s="8"/>
       <c r="K184" s="7"/>
@@ -8457,13 +8373,13 @@
       <c r="E185" s="5"/>
       <c r="F185" s="7"/>
       <c r="G185" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H185" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J185" s="8"/>
       <c r="K185" s="7"/>
@@ -8487,13 +8403,13 @@
       <c r="E186" s="5"/>
       <c r="F186" s="7"/>
       <c r="G186" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H186" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J186" s="8"/>
       <c r="K186" s="7"/>
@@ -8517,13 +8433,13 @@
       <c r="E187" s="5"/>
       <c r="F187" s="7"/>
       <c r="G187" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H187" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J187" s="8"/>
       <c r="K187" s="7"/>
@@ -8546,13 +8462,13 @@
       <c r="E188" s="5"/>
       <c r="F188" s="7"/>
       <c r="G188" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H188" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="I188" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="I188" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="J188" s="8"/>
       <c r="K188" s="7"/>
@@ -8575,13 +8491,13 @@
       <c r="E189" s="5"/>
       <c r="F189" s="7"/>
       <c r="G189" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H189" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I189" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J189" s="8"/>
       <c r="K189" s="7"/>
@@ -8605,13 +8521,13 @@
       <c r="E190" s="5"/>
       <c r="F190" s="7"/>
       <c r="G190" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H190" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J190" s="8"/>
       <c r="K190" s="7"/>
@@ -8634,13 +8550,13 @@
       <c r="E191" s="5"/>
       <c r="F191" s="7"/>
       <c r="G191" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H191" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="I191" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="I191" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="J191" s="8"/>
       <c r="K191" s="7"/>
@@ -8664,13 +8580,13 @@
       <c r="E192" s="5"/>
       <c r="F192" s="7"/>
       <c r="G192" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H192" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I192" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J192" s="8"/>
       <c r="K192" s="7"/>
@@ -8693,13 +8609,13 @@
       <c r="E193" s="5"/>
       <c r="F193" s="7"/>
       <c r="G193" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H193" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I193" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J193" s="8"/>
       <c r="K193" s="7"/>
@@ -8723,13 +8639,13 @@
       <c r="E194" s="5"/>
       <c r="F194" s="7"/>
       <c r="G194" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H194" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I194" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J194" s="8"/>
       <c r="K194" s="7"/>
@@ -8753,13 +8669,13 @@
       <c r="E195" s="5"/>
       <c r="F195" s="7"/>
       <c r="G195" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H195" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I195" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J195" s="8"/>
       <c r="K195" s="7"/>
@@ -8782,13 +8698,13 @@
       <c r="E196" s="5"/>
       <c r="F196" s="7"/>
       <c r="G196" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H196" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="I196" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="I196" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="J196" s="8"/>
       <c r="K196" s="7"/>
@@ -8812,13 +8728,13 @@
       <c r="E197" s="5"/>
       <c r="F197" s="7"/>
       <c r="G197" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H197" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I197" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J197" s="8"/>
       <c r="K197" s="7"/>
@@ -8840,14 +8756,14 @@
       <c r="D198" s="15"/>
       <c r="E198" s="15"/>
       <c r="F198" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G198" s="15"/>
       <c r="H198" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I198" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J198" s="12"/>
       <c r="K198" s="10"/>
@@ -8871,13 +8787,13 @@
       <c r="E199" s="15"/>
       <c r="F199" s="15"/>
       <c r="G199" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H199" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I199" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J199" s="12"/>
       <c r="K199" s="10"/>
@@ -8901,13 +8817,13 @@
       <c r="E200" s="15"/>
       <c r="F200" s="15"/>
       <c r="G200" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H200" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I200" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J200" s="12"/>
       <c r="K200" s="10"/>
@@ -8931,13 +8847,13 @@
       <c r="E201" s="15"/>
       <c r="F201" s="15"/>
       <c r="G201" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H201" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I201" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J201" s="12"/>
       <c r="K201" s="10"/>
@@ -8961,13 +8877,13 @@
       <c r="E202" s="15"/>
       <c r="F202" s="15"/>
       <c r="G202" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H202" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I202" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J202" s="12"/>
       <c r="K202" s="10"/>
@@ -8991,13 +8907,13 @@
       <c r="E203" s="15"/>
       <c r="F203" s="15"/>
       <c r="G203" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H203" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I203" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J203" s="12"/>
       <c r="K203" s="10"/>
@@ -9021,18 +8937,18 @@
       <c r="E204" s="15"/>
       <c r="F204" s="15"/>
       <c r="G204" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H204" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I204" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J204" s="12"/>
       <c r="K204" s="10"/>
       <c r="L204" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M204" s="6"/>
     </row>
@@ -9053,18 +8969,18 @@
       <c r="E205" s="15"/>
       <c r="F205" s="15"/>
       <c r="G205" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H205" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I205" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J205" s="12"/>
       <c r="K205" s="10"/>
       <c r="L205" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M205" s="6"/>
     </row>
@@ -9085,18 +9001,18 @@
       <c r="E206" s="15"/>
       <c r="F206" s="15"/>
       <c r="G206" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H206" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I206" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J206" s="12"/>
       <c r="K206" s="10"/>
       <c r="L206" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M206" s="6"/>
     </row>
@@ -9117,18 +9033,18 @@
       <c r="E207" s="15"/>
       <c r="F207" s="15"/>
       <c r="G207" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H207" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I207" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J207" s="12"/>
       <c r="K207" s="10"/>
       <c r="L207" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M207" s="6"/>
     </row>
@@ -9149,18 +9065,18 @@
       <c r="E208" s="15"/>
       <c r="F208" s="15"/>
       <c r="G208" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H208" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I208" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J208" s="12"/>
       <c r="K208" s="10"/>
       <c r="L208" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M208" s="6"/>
     </row>
@@ -9181,18 +9097,18 @@
       <c r="E209" s="15"/>
       <c r="F209" s="15"/>
       <c r="G209" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H209" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I209" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J209" s="12"/>
       <c r="K209" s="10"/>
       <c r="L209" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M209" s="6"/>
     </row>
@@ -9213,18 +9129,18 @@
       <c r="E210" s="15"/>
       <c r="F210" s="15"/>
       <c r="G210" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H210" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I210" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J210" s="12"/>
       <c r="K210" s="10"/>
       <c r="L210" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M210" s="6"/>
     </row>
@@ -9245,18 +9161,18 @@
       <c r="E211" s="15"/>
       <c r="F211" s="15"/>
       <c r="G211" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H211" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I211" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J211" s="12"/>
       <c r="K211" s="10"/>
       <c r="L211" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M211" s="6"/>
     </row>
@@ -9277,18 +9193,18 @@
       <c r="E212" s="15"/>
       <c r="F212" s="15"/>
       <c r="G212" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H212" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I212" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J212" s="12"/>
       <c r="K212" s="10"/>
       <c r="L212" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M212" s="6"/>
     </row>
@@ -9309,18 +9225,18 @@
       <c r="E213" s="15"/>
       <c r="F213" s="15"/>
       <c r="G213" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H213" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I213" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J213" s="12"/>
       <c r="K213" s="10"/>
       <c r="L213" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M213" s="6"/>
     </row>
@@ -9341,18 +9257,18 @@
       <c r="E214" s="15"/>
       <c r="F214" s="15"/>
       <c r="G214" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H214" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I214" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J214" s="12"/>
       <c r="K214" s="10"/>
       <c r="L214" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M214" s="6"/>
     </row>
@@ -9372,18 +9288,18 @@
       <c r="E215" s="15"/>
       <c r="F215" s="15"/>
       <c r="G215" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H215" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I215" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J215" s="12"/>
       <c r="K215" s="10"/>
       <c r="L215" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M215" s="6"/>
     </row>
@@ -9404,18 +9320,18 @@
       <c r="E216" s="15"/>
       <c r="F216" s="15"/>
       <c r="G216" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H216" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I216" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J216" s="12"/>
       <c r="K216" s="10"/>
       <c r="L216" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M216" s="6"/>
     </row>
@@ -9436,18 +9352,18 @@
       <c r="E217" s="15"/>
       <c r="F217" s="15"/>
       <c r="G217" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H217" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I217" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J217" s="12"/>
       <c r="K217" s="10"/>
       <c r="L217" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M217" s="6"/>
     </row>
@@ -9468,18 +9384,18 @@
       <c r="E218" s="15"/>
       <c r="F218" s="15"/>
       <c r="G218" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H218" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I218" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J218" s="12"/>
       <c r="K218" s="10"/>
       <c r="L218" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M218" s="6"/>
     </row>
@@ -9500,18 +9416,18 @@
       <c r="E219" s="15"/>
       <c r="F219" s="15"/>
       <c r="G219" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H219" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I219" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J219" s="12"/>
       <c r="K219" s="10"/>
       <c r="L219" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M219" s="6"/>
     </row>
@@ -9532,18 +9448,18 @@
       <c r="E220" s="20"/>
       <c r="F220" s="20"/>
       <c r="G220" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H220" s="21" t="s">
         <v>15</v>
       </c>
       <c r="I220" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J220" s="18"/>
       <c r="K220" s="21"/>
       <c r="L220" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M220" s="6"/>
     </row>
@@ -9568,7 +9484,7 @@
         <v>15</v>
       </c>
       <c r="I221" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J221" s="39"/>
       <c r="K221" s="21"/>
@@ -9596,7 +9512,7 @@
         <v>15</v>
       </c>
       <c r="I222" s="39" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J222" s="39"/>
       <c r="K222" s="21"/>
@@ -9624,7 +9540,7 @@
         <v>15</v>
       </c>
       <c r="I223" s="49" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J223" s="49"/>
       <c r="K223" s="21"/>
@@ -9652,7 +9568,7 @@
         <v>15</v>
       </c>
       <c r="I224" s="49" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J224" s="49"/>
       <c r="K224" s="21"/>
@@ -9675,10 +9591,10 @@
       <c r="F225" s="23"/>
       <c r="G225" s="24"/>
       <c r="H225" s="24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I225" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J225" s="23"/>
       <c r="K225" s="21"/>
@@ -9703,10 +9619,10 @@
       <c r="F226" s="23"/>
       <c r="G226" s="23"/>
       <c r="H226" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="I226" s="25" t="s">
         <v>249</v>
-      </c>
-      <c r="I226" s="25" t="s">
-        <v>250</v>
       </c>
       <c r="J226" s="23"/>
       <c r="K226" s="21"/>
@@ -9731,10 +9647,10 @@
       <c r="F227" s="23"/>
       <c r="G227" s="23"/>
       <c r="H227" s="24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I227" s="25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J227" s="23"/>
       <c r="K227" s="21"/>
@@ -9759,10 +9675,10 @@
       <c r="F228" s="23"/>
       <c r="G228" s="23"/>
       <c r="H228" s="24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I228" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J228" s="23"/>
       <c r="K228" s="21"/>
@@ -9787,10 +9703,10 @@
       <c r="F229" s="23"/>
       <c r="G229" s="23"/>
       <c r="H229" s="24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I229" s="25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J229" s="23"/>
       <c r="K229" s="21"/>
@@ -9815,10 +9731,10 @@
       <c r="F230" s="36"/>
       <c r="G230" s="36"/>
       <c r="H230" s="27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I230" s="37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J230" s="36"/>
       <c r="K230" s="21"/>
@@ -9841,13 +9757,13 @@
       <c r="E231" s="23"/>
       <c r="F231" s="23"/>
       <c r="G231" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H231" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="I231" s="25" t="s">
         <v>266</v>
-      </c>
-      <c r="I231" s="25" t="s">
-        <v>267</v>
       </c>
       <c r="J231" s="23"/>
       <c r="K231" s="21"/>
@@ -9871,13 +9787,13 @@
       <c r="E232" s="23"/>
       <c r="F232" s="23"/>
       <c r="G232" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H232" s="24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I232" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J232" s="23"/>
       <c r="K232" s="21"/>
@@ -9901,13 +9817,13 @@
       <c r="E233" s="23"/>
       <c r="F233" s="23"/>
       <c r="G233" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H233" s="24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I233" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J233" s="23"/>
       <c r="K233" s="21"/>
@@ -9931,13 +9847,13 @@
       <c r="E234" s="23"/>
       <c r="F234" s="23"/>
       <c r="G234" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H234" s="24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I234" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J234" s="23"/>
       <c r="K234" s="21"/>
@@ -9961,13 +9877,13 @@
       <c r="E235" s="23"/>
       <c r="F235" s="23"/>
       <c r="G235" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H235" s="24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I235" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J235" s="23"/>
       <c r="K235" s="21"/>
@@ -9989,13 +9905,13 @@
       <c r="E236" s="23"/>
       <c r="F236" s="23"/>
       <c r="G236" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H236" s="24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I236" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J236" s="23"/>
       <c r="K236" s="21"/>
@@ -10018,13 +9934,13 @@
       <c r="E237" s="23"/>
       <c r="F237" s="23"/>
       <c r="G237" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H237" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="I237" s="25" t="s">
         <v>272</v>
-      </c>
-      <c r="I237" s="25" t="s">
-        <v>273</v>
       </c>
       <c r="J237" s="23"/>
       <c r="K237" s="21"/>
@@ -10048,13 +9964,13 @@
       <c r="E238" s="23"/>
       <c r="F238" s="23"/>
       <c r="G238" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H238" s="24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I238" s="25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J238" s="23"/>
       <c r="K238" s="21"/>
@@ -10078,10 +9994,10 @@
       <c r="F239" s="23"/>
       <c r="G239" s="23"/>
       <c r="H239" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="I239" s="25" t="s">
         <v>295</v>
-      </c>
-      <c r="I239" s="25" t="s">
-        <v>296</v>
       </c>
       <c r="J239" s="23"/>
       <c r="K239" s="21"/>
@@ -10106,10 +10022,10 @@
       <c r="F240" s="23"/>
       <c r="G240" s="23"/>
       <c r="H240" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I240" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J240" s="23"/>
       <c r="K240" s="21"/>
@@ -10133,10 +10049,10 @@
       <c r="F241" s="23"/>
       <c r="G241" s="23"/>
       <c r="H241" s="24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I241" s="25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J241" s="23"/>
       <c r="K241" s="21"/>
@@ -10161,10 +10077,10 @@
       <c r="F242" s="23"/>
       <c r="G242" s="23"/>
       <c r="H242" s="24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I242" s="25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J242" s="23"/>
       <c r="K242" s="21"/>
@@ -10189,10 +10105,10 @@
       <c r="F243" s="23"/>
       <c r="G243" s="23"/>
       <c r="H243" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="I243" s="25" t="s">
         <v>300</v>
-      </c>
-      <c r="I243" s="25" t="s">
-        <v>301</v>
       </c>
       <c r="J243" s="23"/>
       <c r="K243" s="21"/>
@@ -10217,10 +10133,10 @@
       <c r="F244" s="23"/>
       <c r="G244" s="23"/>
       <c r="H244" s="24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I244" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J244" s="23"/>
       <c r="K244" s="21"/>
@@ -10244,15 +10160,15 @@
       <c r="F245" s="23"/>
       <c r="G245" s="23"/>
       <c r="H245" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="I245" s="25" t="s">
         <v>302</v>
-      </c>
-      <c r="I245" s="25" t="s">
-        <v>303</v>
       </c>
       <c r="J245" s="23"/>
       <c r="K245" s="21"/>
       <c r="L245" s="55" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M245" s="6"/>
     </row>
@@ -10274,13 +10190,13 @@
       <c r="F246" s="23"/>
       <c r="G246" s="23"/>
       <c r="H246" s="24" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I246" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="J246" s="50" t="s">
         <v>304</v>
-      </c>
-      <c r="J246" s="50" t="s">
-        <v>305</v>
       </c>
       <c r="K246" s="21"/>
       <c r="L246" s="56"/>
@@ -10303,15 +10219,15 @@
       <c r="F247" s="23"/>
       <c r="G247" s="23"/>
       <c r="H247" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="I247" s="25" t="s">
         <v>308</v>
-      </c>
-      <c r="I247" s="25" t="s">
-        <v>309</v>
       </c>
       <c r="J247" s="23"/>
       <c r="K247" s="21"/>
       <c r="L247" s="55" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M247" s="6"/>
     </row>
@@ -10333,10 +10249,10 @@
       <c r="F248" s="23"/>
       <c r="G248" s="23"/>
       <c r="H248" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I248" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J248" s="23"/>
       <c r="K248" s="21"/>
@@ -10361,10 +10277,10 @@
       <c r="F249" s="23"/>
       <c r="G249" s="23"/>
       <c r="H249" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I249" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J249" s="23"/>
       <c r="K249" s="21"/>
@@ -10389,10 +10305,10 @@
       <c r="F250" s="23"/>
       <c r="G250" s="23"/>
       <c r="H250" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I250" s="25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J250" s="23"/>
       <c r="K250" s="21"/>
@@ -10417,10 +10333,10 @@
       <c r="F251" s="23"/>
       <c r="G251" s="23"/>
       <c r="H251" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I251" s="25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J251" s="23"/>
       <c r="K251" s="21"/>
@@ -10445,10 +10361,10 @@
       <c r="F252" s="23"/>
       <c r="G252" s="23"/>
       <c r="H252" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I252" s="25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J252" s="23"/>
       <c r="K252" s="21"/>
@@ -10470,16 +10386,16 @@
       <c r="D253" s="23"/>
       <c r="E253" s="23"/>
       <c r="F253" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G253" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H253" s="24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I253" s="25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J253" s="23"/>
       <c r="K253" s="21"/>
@@ -10502,16 +10418,16 @@
       <c r="D254" s="23"/>
       <c r="E254" s="23"/>
       <c r="F254" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G254" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H254" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="I254" s="25" t="s">
         <v>317</v>
-      </c>
-      <c r="I254" s="25" t="s">
-        <v>318</v>
       </c>
       <c r="J254" s="23"/>
       <c r="K254" s="21"/>
@@ -10533,16 +10449,16 @@
       <c r="D255" s="23"/>
       <c r="E255" s="23"/>
       <c r="F255" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G255" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H255" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="I255" s="25" t="s">
         <v>323</v>
-      </c>
-      <c r="I255" s="25" t="s">
-        <v>324</v>
       </c>
       <c r="J255" s="23"/>
       <c r="K255" s="21"/>
@@ -10565,16 +10481,16 @@
       <c r="D256" s="23"/>
       <c r="E256" s="23"/>
       <c r="F256" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G256" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H256" s="24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I256" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J256" s="23"/>
       <c r="K256" s="21"/>
@@ -10597,16 +10513,16 @@
       <c r="D257" s="23"/>
       <c r="E257" s="23"/>
       <c r="F257" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G257" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H257" s="24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I257" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J257" s="23"/>
       <c r="K257" s="21"/>
@@ -10615,7 +10531,6 @@
     </row>
     <row r="258" spans="1:13" ht="15">
       <c r="A258">
-        <f t="shared" si="56"/>
         <v>31</v>
       </c>
       <c r="B258">
@@ -10626,7 +10541,15 @@
         <f t="shared" si="55"/>
         <v>31-4</v>
       </c>
-      <c r="L258" s="6"/>
+      <c r="D258" s="23"/>
+      <c r="E258" s="23"/>
+      <c r="F258" s="23"/>
+      <c r="G258" s="23"/>
+      <c r="H258" s="24"/>
+      <c r="I258" s="25"/>
+      <c r="J258" s="23"/>
+      <c r="K258" s="21"/>
+      <c r="L258" s="26"/>
       <c r="M258" s="6"/>
     </row>
     <row r="259" spans="1:13" ht="15">
@@ -15496,467 +15419,467 @@
     <mergeCell ref="L247:L252"/>
   </mergeCells>
   <conditionalFormatting sqref="K159:K203 K99:K157 K2:K97">
-    <cfRule type="containsBlanks" dxfId="98" priority="97">
+    <cfRule type="containsBlanks" dxfId="95" priority="97">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K159:K203 K99:K157 K2:K97">
-    <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K159:K203 K99:K157 K2:K97">
-    <cfRule type="containsText" dxfId="96" priority="99" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="93" priority="99" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsBlanks" dxfId="95" priority="94">
+    <cfRule type="containsBlanks" dxfId="92" priority="94">
       <formula>LEN(TRIM(K204))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="94" priority="95" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="91" priority="95" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K204">
-    <cfRule type="containsText" dxfId="93" priority="96" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="90" priority="96" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K204))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsBlanks" dxfId="92" priority="88">
+    <cfRule type="containsBlanks" dxfId="89" priority="88">
       <formula>LEN(TRIM(K205))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="91" priority="89" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K205">
-    <cfRule type="containsText" dxfId="90" priority="90" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="87" priority="90" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K205))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsBlanks" dxfId="89" priority="85">
+    <cfRule type="containsBlanks" dxfId="86" priority="85">
       <formula>LEN(TRIM(K206))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="88" priority="86" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K206">
-    <cfRule type="containsText" dxfId="87" priority="87" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K206))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsBlanks" dxfId="86" priority="82">
+    <cfRule type="containsBlanks" dxfId="83" priority="82">
       <formula>LEN(TRIM(K207))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="85" priority="83" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K207">
-    <cfRule type="containsText" dxfId="84" priority="84" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="81" priority="84" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K207))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsBlanks" dxfId="83" priority="79">
+    <cfRule type="containsBlanks" dxfId="80" priority="79">
       <formula>LEN(TRIM(K209))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsBlanks" dxfId="82" priority="76">
+    <cfRule type="containsBlanks" dxfId="79" priority="76">
       <formula>LEN(TRIM(K211))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsBlanks" dxfId="81" priority="73">
+    <cfRule type="containsBlanks" dxfId="78" priority="73">
       <formula>LEN(TRIM(K213))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsBlanks" dxfId="80" priority="70">
+    <cfRule type="containsBlanks" dxfId="77" priority="70">
       <formula>LEN(TRIM(K214))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsBlanks" dxfId="79" priority="67">
+    <cfRule type="containsBlanks" dxfId="76" priority="67">
       <formula>LEN(TRIM(K216))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsBlanks" dxfId="78" priority="64">
+    <cfRule type="containsBlanks" dxfId="75" priority="64">
       <formula>LEN(TRIM(K218))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220 K237:K238 K225:K235">
-    <cfRule type="containsBlanks" dxfId="77" priority="61">
+    <cfRule type="containsBlanks" dxfId="74" priority="61">
       <formula>LEN(TRIM(K220))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsBlanks" dxfId="76" priority="55">
+    <cfRule type="containsBlanks" dxfId="73" priority="55">
       <formula>LEN(TRIM(K210))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="75" priority="80" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="72" priority="80" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K209">
-    <cfRule type="containsText" dxfId="74" priority="81" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="71" priority="81" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K209))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsBlanks" dxfId="73" priority="52">
+    <cfRule type="containsBlanks" dxfId="70" priority="52">
       <formula>LEN(TRIM(K212))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="72" priority="77" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="69" priority="77" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K211">
-    <cfRule type="containsText" dxfId="71" priority="78" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="68" priority="78" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K211))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsBlanks" dxfId="70" priority="49">
+    <cfRule type="containsBlanks" dxfId="67" priority="49">
       <formula>LEN(TRIM(K208))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="69" priority="74" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="66" priority="74" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K213">
-    <cfRule type="containsText" dxfId="68" priority="75" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="65" priority="75" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K213))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsBlanks" dxfId="67" priority="46">
+    <cfRule type="containsBlanks" dxfId="64" priority="46">
       <formula>LEN(TRIM(K215))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="66" priority="71" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="63" priority="71" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K214">
-    <cfRule type="containsText" dxfId="65" priority="72" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="62" priority="72" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsBlanks" dxfId="64" priority="43">
+    <cfRule type="containsBlanks" dxfId="61" priority="43">
       <formula>LEN(TRIM(K217))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsText" dxfId="63" priority="68" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="60" priority="68" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K216">
-    <cfRule type="containsText" dxfId="62" priority="69" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="59" priority="69" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K216))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219">
-    <cfRule type="containsBlanks" dxfId="61" priority="40">
+    <cfRule type="containsBlanks" dxfId="58" priority="40">
       <formula>LEN(TRIM(K219))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsText" dxfId="60" priority="65" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="57" priority="65" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K218">
-    <cfRule type="containsText" dxfId="59" priority="66" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="56" priority="66" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K218))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220 K237:K238 K225:K235">
-    <cfRule type="containsText" dxfId="58" priority="62" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="55" priority="62" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K220))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K220 K237:K238 K225:K235">
-    <cfRule type="containsText" dxfId="57" priority="63" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="54" priority="63" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K220))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="56" priority="56" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="53" priority="56" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210">
-    <cfRule type="containsText" dxfId="55" priority="57" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="52" priority="57" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K210))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="54" priority="53" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="51" priority="53" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K212">
-    <cfRule type="containsText" dxfId="53" priority="54" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="50" priority="54" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K212))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="52" priority="50" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K208">
-    <cfRule type="containsText" dxfId="51" priority="51" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K208))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="50" priority="47" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="47" priority="47" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K215">
-    <cfRule type="containsText" dxfId="49" priority="48" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="46" priority="48" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K215))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="48" priority="44" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="45" priority="44" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K217">
-    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K217))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219">
-    <cfRule type="containsText" dxfId="46" priority="41" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K219))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K219">
-    <cfRule type="containsText" dxfId="45" priority="42" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K219))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236">
-    <cfRule type="containsBlanks" dxfId="44" priority="37">
+    <cfRule type="containsBlanks" dxfId="41" priority="37">
       <formula>LEN(TRIM(K236))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236">
-    <cfRule type="containsText" dxfId="43" priority="38" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K236">
-    <cfRule type="containsText" dxfId="42" priority="39" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K236))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221">
-    <cfRule type="containsBlanks" dxfId="41" priority="34">
+    <cfRule type="containsBlanks" dxfId="38" priority="34">
       <formula>LEN(TRIM(K221))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221">
-    <cfRule type="containsText" dxfId="40" priority="35" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K221))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K221">
-    <cfRule type="containsText" dxfId="39" priority="36" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K221))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K222:K224">
-    <cfRule type="containsBlanks" dxfId="38" priority="31">
+    <cfRule type="containsBlanks" dxfId="35" priority="31">
       <formula>LEN(TRIM(K222))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K222:K224">
-    <cfRule type="containsText" dxfId="37" priority="32" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K222))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K222:K224">
-    <cfRule type="containsText" dxfId="36" priority="33" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K222))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsBlanks" dxfId="35" priority="28">
+    <cfRule type="containsBlanks" dxfId="32" priority="28">
       <formula>LEN(TRIM(K239))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="34" priority="29" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K239">
-    <cfRule type="containsText" dxfId="33" priority="30" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K239))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240:K244">
-    <cfRule type="containsBlanks" dxfId="32" priority="25">
+    <cfRule type="containsBlanks" dxfId="29" priority="25">
       <formula>LEN(TRIM(K240))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240:K244">
-    <cfRule type="containsText" dxfId="31" priority="26" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K240))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K240:K244">
-    <cfRule type="containsText" dxfId="30" priority="27" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K240))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K245">
-    <cfRule type="containsBlanks" dxfId="29" priority="22">
+    <cfRule type="containsBlanks" dxfId="26" priority="22">
       <formula>LEN(TRIM(K245))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K245">
-    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K245))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K245">
-    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K245))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K246">
-    <cfRule type="containsBlanks" dxfId="26" priority="19">
+    <cfRule type="containsBlanks" dxfId="23" priority="19">
       <formula>LEN(TRIM(K246))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K246">
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K246))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K246">
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K246))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K158">
-    <cfRule type="containsBlanks" dxfId="23" priority="16">
+    <cfRule type="containsBlanks" dxfId="20" priority="16">
       <formula>LEN(TRIM(K158))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K158">
-    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K158))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K158">
-    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K158))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247:K248">
-    <cfRule type="containsBlanks" dxfId="20" priority="13">
+    <cfRule type="containsBlanks" dxfId="17" priority="13">
       <formula>LEN(TRIM(K247))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247:K248">
-    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K247))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K247:K248">
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K247))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K249">
-    <cfRule type="containsBlanks" dxfId="17" priority="10">
+    <cfRule type="containsBlanks" dxfId="14" priority="10">
       <formula>LEN(TRIM(K249))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K249">
-    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K249))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K249">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K249))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K250:K252">
-    <cfRule type="containsBlanks" dxfId="14" priority="7">
+    <cfRule type="containsBlanks" dxfId="11" priority="7">
       <formula>LEN(TRIM(K250))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K250:K252">
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K250))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K250:K252">
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K250))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K253:K257">
-    <cfRule type="containsBlanks" dxfId="11" priority="4">
+  <conditionalFormatting sqref="K253:K258">
+    <cfRule type="containsBlanks" dxfId="8" priority="4">
       <formula>LEN(TRIM(K253))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K253:K257">
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K253:K258">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K253))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K253:K257">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="fail">
+  <conditionalFormatting sqref="K253:K258">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K253))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98">
-    <cfRule type="containsBlanks" dxfId="8" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(K98))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K98))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K98))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15985,19 +15908,19 @@
   <sheetData>
     <row r="1" spans="1:28" ht="25.5">
       <c r="A1" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Add manual system tests for log messages switching
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="342">
   <si>
     <t>Test Number</t>
   </si>
@@ -1032,6 +1032,18 @@
   <si>
     <t>[Optional if 15-59 was completed]
 There is an automated system test that will create 40 blank configurations for you. Run this test and check that memory usage is stable, as above.</t>
+  </si>
+  <si>
+    <t>Difficult</t>
+  </si>
+  <si>
+    <t>Switches correctly when instrument is switched</t>
+  </si>
+  <si>
+    <t>The log messages switch correctly when the instrument is switched</t>
+  </si>
+  <si>
+    <t>8-10</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1386,6 +1398,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2994,8 +3009,8 @@
   <dimension ref="A1:N1080"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I162" sqref="I162"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5064,7 +5079,7 @@
       <c r="L70" s="1"/>
       <c r="M70" s="6"/>
     </row>
-    <row r="71" spans="1:13" ht="15">
+    <row r="71" spans="1:13" ht="30">
       <c r="A71">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -5073,8 +5088,8 @@
         <f t="shared" ref="B71" si="7">IF(A71=A70,B70+1,1)</f>
         <v>11</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>263</v>
+      <c r="C71" s="58" t="s">
+        <v>341</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>263</v>
@@ -5086,16 +5101,16 @@
         <v>263</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>263</v>
+        <v>338</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>263</v>
+        <v>70</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>263</v>
+        <v>339</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>263</v>
+        <v>340</v>
       </c>
       <c r="K71" s="9"/>
       <c r="L71" s="8"/>

</xml_diff>

<commit_message>
Correct manual system test number
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -1043,7 +1043,7 @@
     <t>The log messages switch correctly when the instrument is switched</t>
   </si>
   <si>
-    <t>8-10</t>
+    <t>8-11</t>
   </si>
 </sst>
 </file>
@@ -3010,7 +3010,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
+      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add system tests for device screens
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="348">
   <si>
     <t>Test Number</t>
   </si>
@@ -1044,6 +1044,24 @@
   </si>
   <si>
     <t>8-11</t>
+  </si>
+  <si>
+    <t>28-3</t>
+  </si>
+  <si>
+    <t>You can add a local device screen</t>
+  </si>
+  <si>
+    <t>28-4</t>
+  </si>
+  <si>
+    <t>Local device screens disappear when the client is closed and reopened</t>
+  </si>
+  <si>
+    <t>28-5</t>
+  </si>
+  <si>
+    <t>Remote device screens do not disappear when the client is closed and reopened</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1385,6 +1403,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1398,9 +1422,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3006,11 +3027,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1080"/>
+  <dimension ref="A1:N1083"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+      <pane ySplit="1" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G255" sqref="G255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5088,7 +5109,7 @@
         <f t="shared" ref="B71" si="7">IF(A71=A70,B70+1,1)</f>
         <v>11</v>
       </c>
-      <c r="C71" s="58" t="s">
+      <c r="C71" s="53" t="s">
         <v>341</v>
       </c>
       <c r="D71" s="9" t="s">
@@ -8649,7 +8670,7 @@
       </c>
       <c r="J195" s="8"/>
       <c r="K195" s="7"/>
-      <c r="L195" s="52"/>
+      <c r="L195" s="54"/>
     </row>
     <row r="196" spans="1:13" ht="30">
       <c r="A196">
@@ -8678,7 +8699,7 @@
       </c>
       <c r="J196" s="8"/>
       <c r="K196" s="7"/>
-      <c r="L196" s="53"/>
+      <c r="L196" s="55"/>
       <c r="M196" s="6"/>
     </row>
     <row r="197" spans="1:13" ht="45">
@@ -8708,7 +8729,7 @@
       </c>
       <c r="J197" s="8"/>
       <c r="K197" s="7"/>
-      <c r="L197" s="53"/>
+      <c r="L197" s="55"/>
       <c r="M197" s="6"/>
     </row>
     <row r="198" spans="1:13" ht="30">
@@ -8738,7 +8759,7 @@
       </c>
       <c r="J198" s="8"/>
       <c r="K198" s="7"/>
-      <c r="L198" s="54"/>
+      <c r="L198" s="56"/>
       <c r="M198" s="6"/>
     </row>
     <row r="199" spans="1:13" ht="30">
@@ -10041,11 +10062,11 @@
         <v>26</v>
       </c>
       <c r="B242">
-        <f t="shared" ref="B242:B307" si="54">IF(A242=A241,B241+1,1)</f>
+        <f t="shared" ref="B242:B310" si="54">IF(A242=A241,B241+1,1)</f>
         <v>1</v>
       </c>
       <c r="C242" s="3" t="str">
-        <f t="shared" ref="C242:C307" si="55">CONCATENATE(A242,"-",B242)</f>
+        <f t="shared" ref="C242:C310" si="55">CONCATENATE(A242,"-",B242)</f>
         <v>26-1</v>
       </c>
       <c r="D242" s="23"/>
@@ -10065,7 +10086,7 @@
     </row>
     <row r="243" spans="1:13" ht="15">
       <c r="A243">
-        <f t="shared" ref="A243:A308" si="56">A242</f>
+        <f t="shared" ref="A243:A311" si="56">A242</f>
         <v>26</v>
       </c>
       <c r="B243">
@@ -10226,18 +10247,18 @@
       </c>
       <c r="J248" s="23"/>
       <c r="K248" s="21"/>
-      <c r="L248" s="55" t="s">
+      <c r="L248" s="57" t="s">
         <v>305</v>
       </c>
       <c r="M248" s="6"/>
     </row>
     <row r="249" spans="1:13" ht="26.25">
       <c r="A249">
-        <f t="shared" si="56"/>
+        <f>A248</f>
         <v>28</v>
       </c>
       <c r="B249">
-        <f t="shared" si="54"/>
+        <f>IF(A249=A248,B248+1,1)</f>
         <v>2</v>
       </c>
       <c r="C249" s="3" t="str">
@@ -10258,106 +10279,95 @@
         <v>304</v>
       </c>
       <c r="K249" s="21"/>
-      <c r="L249" s="56"/>
+      <c r="L249" s="58"/>
       <c r="M249" s="6"/>
     </row>
-    <row r="250" spans="1:13" ht="39">
+    <row r="250" spans="1:13" ht="15">
       <c r="A250">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B250">
-        <f t="shared" si="54"/>
-        <v>1</v>
-      </c>
-      <c r="C250" s="3" t="str">
-        <f t="shared" si="55"/>
-        <v>29-1</v>
+        <v>3</v>
+      </c>
+      <c r="C250" s="53" t="s">
+        <v>342</v>
       </c>
       <c r="D250" s="23"/>
       <c r="E250" s="23"/>
       <c r="F250" s="23"/>
       <c r="G250" s="23"/>
       <c r="H250" s="24" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="I250" s="25" t="s">
-        <v>308</v>
-      </c>
-      <c r="J250" s="23"/>
+        <v>343</v>
+      </c>
+      <c r="J250" s="50"/>
       <c r="K250" s="21"/>
-      <c r="L250" s="55" t="s">
-        <v>314</v>
-      </c>
+      <c r="L250" s="52"/>
       <c r="M250" s="6"/>
     </row>
-    <row r="251" spans="1:13" ht="39">
+    <row r="251" spans="1:13" ht="26.25">
       <c r="A251">
-        <f t="shared" si="56"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B251">
-        <f t="shared" si="54"/>
-        <v>2</v>
-      </c>
-      <c r="C251" s="3" t="str">
-        <f t="shared" si="55"/>
-        <v>29-2</v>
+        <v>4</v>
+      </c>
+      <c r="C251" s="53" t="s">
+        <v>344</v>
       </c>
       <c r="D251" s="23"/>
       <c r="E251" s="23"/>
       <c r="F251" s="23"/>
       <c r="G251" s="23"/>
       <c r="H251" s="24" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="I251" s="25" t="s">
-        <v>309</v>
-      </c>
-      <c r="J251" s="23"/>
+        <v>345</v>
+      </c>
+      <c r="J251" s="50"/>
       <c r="K251" s="21"/>
-      <c r="L251" s="57"/>
+      <c r="L251" s="52"/>
       <c r="M251" s="6"/>
     </row>
     <row r="252" spans="1:13" ht="26.25">
       <c r="A252">
-        <f t="shared" si="56"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B252">
-        <f t="shared" si="54"/>
-        <v>3</v>
-      </c>
-      <c r="C252" s="3" t="str">
-        <f t="shared" si="55"/>
-        <v>29-3</v>
+        <v>5</v>
+      </c>
+      <c r="C252" s="53" t="s">
+        <v>346</v>
       </c>
       <c r="D252" s="23"/>
       <c r="E252" s="23"/>
       <c r="F252" s="23"/>
       <c r="G252" s="23"/>
       <c r="H252" s="24" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="I252" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="J252" s="23"/>
+        <v>347</v>
+      </c>
+      <c r="J252" s="50"/>
       <c r="K252" s="21"/>
-      <c r="L252" s="57"/>
+      <c r="L252" s="52"/>
       <c r="M252" s="6"/>
     </row>
-    <row r="253" spans="1:13" ht="26.25" customHeight="1">
+    <row r="253" spans="1:13" ht="39">
       <c r="A253">
-        <f t="shared" si="56"/>
         <v>29</v>
       </c>
       <c r="B253">
-        <f t="shared" si="54"/>
-        <v>4</v>
+        <f>IF(A253=A249,B249+1,1)</f>
+        <v>1</v>
       </c>
       <c r="C253" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>29-4</v>
+        <v>29-1</v>
       </c>
       <c r="D253" s="23"/>
       <c r="E253" s="23"/>
@@ -10367,25 +10377,27 @@
         <v>307</v>
       </c>
       <c r="I253" s="25" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="J253" s="23"/>
       <c r="K253" s="21"/>
-      <c r="L253" s="57"/>
+      <c r="L253" s="57" t="s">
+        <v>314</v>
+      </c>
       <c r="M253" s="6"/>
     </row>
-    <row r="254" spans="1:13" ht="26.25" customHeight="1">
+    <row r="254" spans="1:13" ht="39">
       <c r="A254">
         <f t="shared" si="56"/>
         <v>29</v>
       </c>
       <c r="B254">
         <f t="shared" si="54"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C254" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>29-5</v>
+        <v>29-2</v>
       </c>
       <c r="D254" s="23"/>
       <c r="E254" s="23"/>
@@ -10395,25 +10407,25 @@
         <v>307</v>
       </c>
       <c r="I254" s="25" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="J254" s="23"/>
       <c r="K254" s="21"/>
-      <c r="L254" s="57"/>
+      <c r="L254" s="59"/>
       <c r="M254" s="6"/>
     </row>
-    <row r="255" spans="1:13" ht="39">
+    <row r="255" spans="1:13" ht="26.25">
       <c r="A255">
         <f t="shared" si="56"/>
         <v>29</v>
       </c>
       <c r="B255">
         <f t="shared" si="54"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C255" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>29-6</v>
+        <v>29-3</v>
       </c>
       <c r="D255" s="23"/>
       <c r="E255" s="23"/>
@@ -10423,119 +10435,108 @@
         <v>307</v>
       </c>
       <c r="I255" s="25" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="J255" s="23"/>
       <c r="K255" s="21"/>
-      <c r="L255" s="56"/>
+      <c r="L255" s="59"/>
       <c r="M255" s="6"/>
     </row>
-    <row r="256" spans="1:13" ht="51.75">
+    <row r="256" spans="1:13" ht="26.25" customHeight="1">
       <c r="A256">
-        <v>30</v>
+        <f t="shared" si="56"/>
+        <v>29</v>
       </c>
       <c r="B256">
         <f t="shared" si="54"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C256" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-1</v>
+        <v>29-4</v>
       </c>
       <c r="D256" s="23"/>
       <c r="E256" s="23"/>
-      <c r="F256" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="G256" s="23" t="s">
-        <v>176</v>
-      </c>
+      <c r="F256" s="23"/>
+      <c r="G256" s="23"/>
       <c r="H256" s="24" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="I256" s="25" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="J256" s="23"/>
       <c r="K256" s="21"/>
-      <c r="L256" s="26"/>
+      <c r="L256" s="59"/>
       <c r="M256" s="6"/>
     </row>
-    <row r="257" spans="1:13" ht="51.75">
+    <row r="257" spans="1:13" ht="26.25" customHeight="1">
       <c r="A257">
         <f t="shared" si="56"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B257">
         <f t="shared" si="54"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C257" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-2</v>
+        <v>29-5</v>
       </c>
       <c r="D257" s="23"/>
       <c r="E257" s="23"/>
-      <c r="F257" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="G257" s="23" t="s">
-        <v>176</v>
-      </c>
+      <c r="F257" s="23"/>
+      <c r="G257" s="23"/>
       <c r="H257" s="24" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="I257" s="25" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="J257" s="23"/>
       <c r="K257" s="21"/>
-      <c r="L257" s="26"/>
+      <c r="L257" s="59"/>
       <c r="M257" s="6"/>
     </row>
     <row r="258" spans="1:13" ht="39">
       <c r="A258">
-        <v>31</v>
+        <f t="shared" si="56"/>
+        <v>29</v>
       </c>
       <c r="B258">
-        <f t="shared" ref="B258" si="61">IF(A258=A257,B257+1,1)</f>
-        <v>1</v>
+        <f t="shared" si="54"/>
+        <v>6</v>
       </c>
       <c r="C258" s="3" t="str">
-        <f t="shared" ref="C258" si="62">CONCATENATE(A258,"-",B258)</f>
-        <v>31-1</v>
+        <f t="shared" si="55"/>
+        <v>29-6</v>
       </c>
       <c r="D258" s="23"/>
       <c r="E258" s="23"/>
-      <c r="F258" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="G258" s="23" t="s">
-        <v>241</v>
-      </c>
+      <c r="F258" s="23"/>
+      <c r="G258" s="23"/>
       <c r="H258" s="24" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="I258" s="25" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="J258" s="23"/>
       <c r="K258" s="21"/>
-      <c r="L258" s="26"/>
+      <c r="L258" s="58"/>
       <c r="M258" s="6"/>
     </row>
-    <row r="259" spans="1:13" ht="39">
+    <row r="259" spans="1:13" ht="51.75">
       <c r="A259">
-        <f t="shared" si="56"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B259">
         <f t="shared" si="54"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C259" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-2</v>
+        <v>30-1</v>
       </c>
       <c r="D259" s="23"/>
       <c r="E259" s="23"/>
@@ -10543,31 +10544,31 @@
         <v>241</v>
       </c>
       <c r="G259" s="23" t="s">
-        <v>241</v>
+        <v>176</v>
       </c>
       <c r="H259" s="24" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I259" s="25" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="J259" s="23"/>
       <c r="K259" s="21"/>
       <c r="L259" s="26"/>
       <c r="M259" s="6"/>
     </row>
-    <row r="260" spans="1:13" ht="39">
+    <row r="260" spans="1:13" ht="51.75">
       <c r="A260">
         <f t="shared" si="56"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B260">
         <f t="shared" si="54"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C260" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-3</v>
+        <v>30-2</v>
       </c>
       <c r="D260" s="23"/>
       <c r="E260" s="23"/>
@@ -10575,88 +10576,135 @@
         <v>241</v>
       </c>
       <c r="G260" s="23" t="s">
-        <v>241</v>
+        <v>176</v>
       </c>
       <c r="H260" s="24" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I260" s="25" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="J260" s="23"/>
       <c r="K260" s="21"/>
       <c r="L260" s="26"/>
       <c r="M260" s="6"/>
     </row>
-    <row r="261" spans="1:13" ht="15">
+    <row r="261" spans="1:13" ht="39">
       <c r="A261">
         <v>31</v>
       </c>
       <c r="B261">
-        <f t="shared" si="54"/>
-        <v>4</v>
+        <f t="shared" ref="B261" si="61">IF(A261=A260,B260+1,1)</f>
+        <v>1</v>
       </c>
       <c r="C261" s="3" t="str">
-        <f t="shared" si="55"/>
-        <v>31-4</v>
+        <f t="shared" ref="C261" si="62">CONCATENATE(A261,"-",B261)</f>
+        <v>31-1</v>
       </c>
       <c r="D261" s="23"/>
       <c r="E261" s="23"/>
-      <c r="F261" s="23"/>
-      <c r="G261" s="23"/>
-      <c r="H261" s="24"/>
-      <c r="I261" s="25"/>
+      <c r="F261" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="G261" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="H261" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="I261" s="25" t="s">
+        <v>323</v>
+      </c>
       <c r="J261" s="23"/>
       <c r="K261" s="21"/>
       <c r="L261" s="26"/>
       <c r="M261" s="6"/>
     </row>
-    <row r="262" spans="1:13" ht="15">
+    <row r="262" spans="1:13" ht="39">
       <c r="A262">
         <f t="shared" si="56"/>
         <v>31</v>
       </c>
       <c r="B262">
         <f t="shared" si="54"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C262" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-5</v>
-      </c>
-      <c r="L262" s="6"/>
+        <v>31-2</v>
+      </c>
+      <c r="D262" s="23"/>
+      <c r="E262" s="23"/>
+      <c r="F262" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="G262" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="H262" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="I262" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="J262" s="23"/>
+      <c r="K262" s="21"/>
+      <c r="L262" s="26"/>
       <c r="M262" s="6"/>
     </row>
-    <row r="263" spans="1:13" ht="15">
+    <row r="263" spans="1:13" ht="39">
       <c r="A263">
         <f t="shared" si="56"/>
         <v>31</v>
       </c>
       <c r="B263">
         <f t="shared" si="54"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C263" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-6</v>
-      </c>
-      <c r="L263" s="6"/>
+        <v>31-3</v>
+      </c>
+      <c r="D263" s="23"/>
+      <c r="E263" s="23"/>
+      <c r="F263" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="G263" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="H263" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="I263" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="J263" s="23"/>
+      <c r="K263" s="21"/>
+      <c r="L263" s="26"/>
       <c r="M263" s="6"/>
     </row>
     <row r="264" spans="1:13" ht="15">
       <c r="A264">
-        <f t="shared" si="56"/>
         <v>31</v>
       </c>
       <c r="B264">
         <f t="shared" si="54"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C264" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-7</v>
-      </c>
-      <c r="L264" s="6"/>
+        <v>31-4</v>
+      </c>
+      <c r="D264" s="23"/>
+      <c r="E264" s="23"/>
+      <c r="F264" s="23"/>
+      <c r="G264" s="23"/>
+      <c r="H264" s="24"/>
+      <c r="I264" s="25"/>
+      <c r="J264" s="23"/>
+      <c r="K264" s="21"/>
+      <c r="L264" s="26"/>
       <c r="M264" s="6"/>
     </row>
     <row r="265" spans="1:13" ht="15">
@@ -10666,11 +10714,11 @@
       </c>
       <c r="B265">
         <f t="shared" si="54"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C265" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-8</v>
+        <v>31-5</v>
       </c>
       <c r="L265" s="6"/>
       <c r="M265" s="6"/>
@@ -10682,11 +10730,11 @@
       </c>
       <c r="B266">
         <f t="shared" si="54"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C266" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-9</v>
+        <v>31-6</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
@@ -10698,11 +10746,11 @@
       </c>
       <c r="B267">
         <f t="shared" si="54"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C267" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-10</v>
+        <v>31-7</v>
       </c>
       <c r="L267" s="6"/>
       <c r="M267" s="6"/>
@@ -10714,11 +10762,11 @@
       </c>
       <c r="B268">
         <f t="shared" si="54"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C268" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-11</v>
+        <v>31-8</v>
       </c>
       <c r="L268" s="6"/>
       <c r="M268" s="6"/>
@@ -10730,11 +10778,11 @@
       </c>
       <c r="B269">
         <f t="shared" si="54"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C269" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-12</v>
+        <v>31-9</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
@@ -10746,11 +10794,11 @@
       </c>
       <c r="B270">
         <f t="shared" si="54"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C270" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-13</v>
+        <v>31-10</v>
       </c>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
@@ -10762,11 +10810,11 @@
       </c>
       <c r="B271">
         <f t="shared" si="54"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C271" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-14</v>
+        <v>31-11</v>
       </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
@@ -10778,11 +10826,11 @@
       </c>
       <c r="B272">
         <f t="shared" si="54"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C272" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-15</v>
+        <v>31-12</v>
       </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
@@ -10794,11 +10842,11 @@
       </c>
       <c r="B273">
         <f t="shared" si="54"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C273" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-16</v>
+        <v>31-13</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
@@ -10810,11 +10858,11 @@
       </c>
       <c r="B274">
         <f t="shared" si="54"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C274" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-17</v>
+        <v>31-14</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
@@ -10826,11 +10874,11 @@
       </c>
       <c r="B275">
         <f t="shared" si="54"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C275" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-18</v>
+        <v>31-15</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
@@ -10842,11 +10890,11 @@
       </c>
       <c r="B276">
         <f t="shared" si="54"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C276" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-19</v>
+        <v>31-16</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
@@ -10858,11 +10906,11 @@
       </c>
       <c r="B277">
         <f t="shared" si="54"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C277" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-20</v>
+        <v>31-17</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
@@ -10874,11 +10922,11 @@
       </c>
       <c r="B278">
         <f t="shared" si="54"/>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C278" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-21</v>
+        <v>31-18</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
@@ -10890,11 +10938,11 @@
       </c>
       <c r="B279">
         <f t="shared" si="54"/>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C279" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-22</v>
+        <v>31-19</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
@@ -10906,11 +10954,11 @@
       </c>
       <c r="B280">
         <f t="shared" si="54"/>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C280" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-23</v>
+        <v>31-20</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
@@ -10922,11 +10970,11 @@
       </c>
       <c r="B281">
         <f t="shared" si="54"/>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C281" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-24</v>
+        <v>31-21</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
@@ -10938,11 +10986,11 @@
       </c>
       <c r="B282">
         <f t="shared" si="54"/>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C282" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-25</v>
+        <v>31-22</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
@@ -10954,11 +11002,11 @@
       </c>
       <c r="B283">
         <f t="shared" si="54"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C283" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-26</v>
+        <v>31-23</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
@@ -10970,11 +11018,11 @@
       </c>
       <c r="B284">
         <f t="shared" si="54"/>
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C284" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-27</v>
+        <v>31-24</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
@@ -10986,11 +11034,11 @@
       </c>
       <c r="B285">
         <f t="shared" si="54"/>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C285" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-28</v>
+        <v>31-25</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
@@ -11002,11 +11050,11 @@
       </c>
       <c r="B286">
         <f t="shared" si="54"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C286" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-29</v>
+        <v>31-26</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
@@ -11018,11 +11066,11 @@
       </c>
       <c r="B287">
         <f t="shared" si="54"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C287" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-30</v>
+        <v>31-27</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
@@ -11034,11 +11082,11 @@
       </c>
       <c r="B288">
         <f t="shared" si="54"/>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C288" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-31</v>
+        <v>31-28</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
@@ -11050,11 +11098,11 @@
       </c>
       <c r="B289">
         <f t="shared" si="54"/>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C289" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-32</v>
+        <v>31-29</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
@@ -11066,11 +11114,11 @@
       </c>
       <c r="B290">
         <f t="shared" si="54"/>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C290" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-33</v>
+        <v>31-30</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
@@ -11082,11 +11130,11 @@
       </c>
       <c r="B291">
         <f t="shared" si="54"/>
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C291" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-34</v>
+        <v>31-31</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
@@ -11098,11 +11146,11 @@
       </c>
       <c r="B292">
         <f t="shared" si="54"/>
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C292" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-35</v>
+        <v>31-32</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
@@ -11114,11 +11162,11 @@
       </c>
       <c r="B293">
         <f t="shared" si="54"/>
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C293" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-36</v>
+        <v>31-33</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
@@ -11130,11 +11178,11 @@
       </c>
       <c r="B294">
         <f t="shared" si="54"/>
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C294" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-37</v>
+        <v>31-34</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
@@ -11146,11 +11194,11 @@
       </c>
       <c r="B295">
         <f t="shared" si="54"/>
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C295" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-38</v>
+        <v>31-35</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
@@ -11162,11 +11210,11 @@
       </c>
       <c r="B296">
         <f t="shared" si="54"/>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C296" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-39</v>
+        <v>31-36</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
@@ -11178,11 +11226,11 @@
       </c>
       <c r="B297">
         <f t="shared" si="54"/>
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C297" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-40</v>
+        <v>31-37</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
@@ -11194,11 +11242,11 @@
       </c>
       <c r="B298">
         <f t="shared" si="54"/>
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C298" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-41</v>
+        <v>31-38</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
@@ -11210,11 +11258,11 @@
       </c>
       <c r="B299">
         <f t="shared" si="54"/>
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C299" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-42</v>
+        <v>31-39</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
@@ -11226,11 +11274,11 @@
       </c>
       <c r="B300">
         <f t="shared" si="54"/>
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C300" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-43</v>
+        <v>31-40</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
@@ -11242,11 +11290,11 @@
       </c>
       <c r="B301">
         <f t="shared" si="54"/>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C301" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-44</v>
+        <v>31-41</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
@@ -11258,11 +11306,11 @@
       </c>
       <c r="B302">
         <f t="shared" si="54"/>
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C302" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-45</v>
+        <v>31-42</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
@@ -11274,11 +11322,11 @@
       </c>
       <c r="B303">
         <f t="shared" si="54"/>
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C303" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-46</v>
+        <v>31-43</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
@@ -11290,11 +11338,11 @@
       </c>
       <c r="B304">
         <f t="shared" si="54"/>
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C304" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-47</v>
+        <v>31-44</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
@@ -11306,11 +11354,11 @@
       </c>
       <c r="B305">
         <f t="shared" si="54"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C305" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-48</v>
+        <v>31-45</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
@@ -11322,11 +11370,11 @@
       </c>
       <c r="B306">
         <f t="shared" si="54"/>
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C306" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-49</v>
+        <v>31-46</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
@@ -11338,11 +11386,11 @@
       </c>
       <c r="B307">
         <f t="shared" si="54"/>
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C307" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-50</v>
+        <v>31-47</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
@@ -11353,76 +11401,76 @@
         <v>31</v>
       </c>
       <c r="B308">
-        <f t="shared" ref="B308:B371" si="63">IF(A308=A307,B307+1,1)</f>
-        <v>51</v>
+        <f t="shared" si="54"/>
+        <v>48</v>
       </c>
       <c r="C308" s="3" t="str">
-        <f t="shared" ref="C308:C371" si="64">CONCATENATE(A308,"-",B308)</f>
-        <v>31-51</v>
+        <f t="shared" si="55"/>
+        <v>31-48</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
     </row>
     <row r="309" spans="1:13" ht="15">
       <c r="A309">
-        <f t="shared" ref="A309:A372" si="65">A308</f>
+        <f t="shared" si="56"/>
         <v>31</v>
       </c>
       <c r="B309">
+        <f t="shared" si="54"/>
+        <v>49</v>
+      </c>
+      <c r="C309" s="3" t="str">
+        <f t="shared" si="55"/>
+        <v>31-49</v>
+      </c>
+      <c r="L309" s="6"/>
+      <c r="M309" s="6"/>
+    </row>
+    <row r="310" spans="1:13" ht="15">
+      <c r="A310">
+        <f t="shared" si="56"/>
+        <v>31</v>
+      </c>
+      <c r="B310">
+        <f t="shared" si="54"/>
+        <v>50</v>
+      </c>
+      <c r="C310" s="3" t="str">
+        <f t="shared" si="55"/>
+        <v>31-50</v>
+      </c>
+      <c r="L310" s="6"/>
+      <c r="M310" s="6"/>
+    </row>
+    <row r="311" spans="1:13" ht="15">
+      <c r="A311">
+        <f t="shared" si="56"/>
+        <v>31</v>
+      </c>
+      <c r="B311">
+        <f t="shared" ref="B311:B374" si="63">IF(A311=A310,B310+1,1)</f>
+        <v>51</v>
+      </c>
+      <c r="C311" s="3" t="str">
+        <f t="shared" ref="C311:C374" si="64">CONCATENATE(A311,"-",B311)</f>
+        <v>31-51</v>
+      </c>
+      <c r="L311" s="6"/>
+      <c r="M311" s="6"/>
+    </row>
+    <row r="312" spans="1:13" ht="15">
+      <c r="A312">
+        <f t="shared" ref="A312:A375" si="65">A311</f>
+        <v>31</v>
+      </c>
+      <c r="B312">
         <f t="shared" si="63"/>
         <v>52</v>
       </c>
-      <c r="C309" s="3" t="str">
+      <c r="C312" s="3" t="str">
         <f t="shared" si="64"/>
         <v>31-52</v>
-      </c>
-      <c r="L309" s="6"/>
-      <c r="M309" s="6"/>
-    </row>
-    <row r="310" spans="1:13" ht="15">
-      <c r="A310">
-        <f t="shared" si="65"/>
-        <v>31</v>
-      </c>
-      <c r="B310">
-        <f t="shared" si="63"/>
-        <v>53</v>
-      </c>
-      <c r="C310" s="3" t="str">
-        <f t="shared" si="64"/>
-        <v>31-53</v>
-      </c>
-      <c r="L310" s="6"/>
-      <c r="M310" s="6"/>
-    </row>
-    <row r="311" spans="1:13" ht="15">
-      <c r="A311">
-        <f t="shared" si="65"/>
-        <v>31</v>
-      </c>
-      <c r="B311">
-        <f t="shared" si="63"/>
-        <v>54</v>
-      </c>
-      <c r="C311" s="3" t="str">
-        <f t="shared" si="64"/>
-        <v>31-54</v>
-      </c>
-      <c r="L311" s="6"/>
-      <c r="M311" s="6"/>
-    </row>
-    <row r="312" spans="1:13" ht="15">
-      <c r="A312">
-        <f t="shared" si="65"/>
-        <v>31</v>
-      </c>
-      <c r="B312">
-        <f t="shared" si="63"/>
-        <v>55</v>
-      </c>
-      <c r="C312" s="3" t="str">
-        <f t="shared" si="64"/>
-        <v>31-55</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
@@ -11434,11 +11482,11 @@
       </c>
       <c r="B313">
         <f t="shared" si="63"/>
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C313" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-56</v>
+        <v>31-53</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
@@ -11450,11 +11498,11 @@
       </c>
       <c r="B314">
         <f t="shared" si="63"/>
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C314" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-57</v>
+        <v>31-54</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
@@ -11466,11 +11514,11 @@
       </c>
       <c r="B315">
         <f t="shared" si="63"/>
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C315" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-58</v>
+        <v>31-55</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
@@ -11482,11 +11530,11 @@
       </c>
       <c r="B316">
         <f t="shared" si="63"/>
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C316" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-59</v>
+        <v>31-56</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
@@ -11498,11 +11546,11 @@
       </c>
       <c r="B317">
         <f t="shared" si="63"/>
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C317" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-60</v>
+        <v>31-57</v>
       </c>
       <c r="L317" s="6"/>
       <c r="M317" s="6"/>
@@ -11514,11 +11562,11 @@
       </c>
       <c r="B318">
         <f t="shared" si="63"/>
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C318" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-61</v>
+        <v>31-58</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
@@ -11530,11 +11578,11 @@
       </c>
       <c r="B319">
         <f t="shared" si="63"/>
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C319" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-62</v>
+        <v>31-59</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
@@ -11546,11 +11594,11 @@
       </c>
       <c r="B320">
         <f t="shared" si="63"/>
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C320" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-63</v>
+        <v>31-60</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
@@ -11562,11 +11610,11 @@
       </c>
       <c r="B321">
         <f t="shared" si="63"/>
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C321" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-64</v>
+        <v>31-61</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
@@ -11578,11 +11626,11 @@
       </c>
       <c r="B322">
         <f t="shared" si="63"/>
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C322" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-65</v>
+        <v>31-62</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
@@ -11594,11 +11642,11 @@
       </c>
       <c r="B323">
         <f t="shared" si="63"/>
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C323" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-66</v>
+        <v>31-63</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
@@ -11610,11 +11658,11 @@
       </c>
       <c r="B324">
         <f t="shared" si="63"/>
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C324" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-67</v>
+        <v>31-64</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
@@ -11626,11 +11674,11 @@
       </c>
       <c r="B325">
         <f t="shared" si="63"/>
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C325" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-68</v>
+        <v>31-65</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
@@ -11642,11 +11690,11 @@
       </c>
       <c r="B326">
         <f t="shared" si="63"/>
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C326" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-69</v>
+        <v>31-66</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
@@ -11658,11 +11706,11 @@
       </c>
       <c r="B327">
         <f t="shared" si="63"/>
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C327" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-70</v>
+        <v>31-67</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
@@ -11674,11 +11722,11 @@
       </c>
       <c r="B328">
         <f t="shared" si="63"/>
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C328" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-71</v>
+        <v>31-68</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
@@ -11690,11 +11738,11 @@
       </c>
       <c r="B329">
         <f t="shared" si="63"/>
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C329" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-72</v>
+        <v>31-69</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
@@ -11706,11 +11754,11 @@
       </c>
       <c r="B330">
         <f t="shared" si="63"/>
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C330" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-73</v>
+        <v>31-70</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
@@ -11722,11 +11770,11 @@
       </c>
       <c r="B331">
         <f t="shared" si="63"/>
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C331" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-74</v>
+        <v>31-71</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
@@ -11738,11 +11786,11 @@
       </c>
       <c r="B332">
         <f t="shared" si="63"/>
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C332" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-75</v>
+        <v>31-72</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
@@ -11754,11 +11802,11 @@
       </c>
       <c r="B333">
         <f t="shared" si="63"/>
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C333" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-76</v>
+        <v>31-73</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
@@ -11770,11 +11818,11 @@
       </c>
       <c r="B334">
         <f t="shared" si="63"/>
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C334" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-77</v>
+        <v>31-74</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
@@ -11786,11 +11834,11 @@
       </c>
       <c r="B335">
         <f t="shared" si="63"/>
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C335" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-78</v>
+        <v>31-75</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
@@ -11802,11 +11850,11 @@
       </c>
       <c r="B336">
         <f t="shared" si="63"/>
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C336" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-79</v>
+        <v>31-76</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
@@ -11818,11 +11866,11 @@
       </c>
       <c r="B337">
         <f t="shared" si="63"/>
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C337" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-80</v>
+        <v>31-77</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
@@ -11834,11 +11882,11 @@
       </c>
       <c r="B338">
         <f t="shared" si="63"/>
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C338" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-81</v>
+        <v>31-78</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
@@ -11850,11 +11898,11 @@
       </c>
       <c r="B339">
         <f t="shared" si="63"/>
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C339" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-82</v>
+        <v>31-79</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
@@ -11866,11 +11914,11 @@
       </c>
       <c r="B340">
         <f t="shared" si="63"/>
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C340" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-83</v>
+        <v>31-80</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
@@ -11882,11 +11930,11 @@
       </c>
       <c r="B341">
         <f t="shared" si="63"/>
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C341" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-84</v>
+        <v>31-81</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
@@ -11898,11 +11946,11 @@
       </c>
       <c r="B342">
         <f t="shared" si="63"/>
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C342" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-85</v>
+        <v>31-82</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
@@ -11914,11 +11962,11 @@
       </c>
       <c r="B343">
         <f t="shared" si="63"/>
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C343" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-86</v>
+        <v>31-83</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
@@ -11930,11 +11978,11 @@
       </c>
       <c r="B344">
         <f t="shared" si="63"/>
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C344" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-87</v>
+        <v>31-84</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
@@ -11946,11 +11994,11 @@
       </c>
       <c r="B345">
         <f t="shared" si="63"/>
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C345" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-88</v>
+        <v>31-85</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
@@ -11962,11 +12010,11 @@
       </c>
       <c r="B346">
         <f t="shared" si="63"/>
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C346" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-89</v>
+        <v>31-86</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
@@ -11978,11 +12026,11 @@
       </c>
       <c r="B347">
         <f t="shared" si="63"/>
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C347" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-90</v>
+        <v>31-87</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
@@ -11994,11 +12042,11 @@
       </c>
       <c r="B348">
         <f t="shared" si="63"/>
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C348" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-91</v>
+        <v>31-88</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
@@ -12010,11 +12058,11 @@
       </c>
       <c r="B349">
         <f t="shared" si="63"/>
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C349" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-92</v>
+        <v>31-89</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
@@ -12026,11 +12074,11 @@
       </c>
       <c r="B350">
         <f t="shared" si="63"/>
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C350" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-93</v>
+        <v>31-90</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
@@ -12042,11 +12090,11 @@
       </c>
       <c r="B351">
         <f t="shared" si="63"/>
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C351" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-94</v>
+        <v>31-91</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
@@ -12058,11 +12106,11 @@
       </c>
       <c r="B352">
         <f t="shared" si="63"/>
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C352" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-95</v>
+        <v>31-92</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
@@ -12074,11 +12122,11 @@
       </c>
       <c r="B353">
         <f t="shared" si="63"/>
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C353" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-96</v>
+        <v>31-93</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
@@ -12090,11 +12138,11 @@
       </c>
       <c r="B354">
         <f t="shared" si="63"/>
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C354" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-97</v>
+        <v>31-94</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
@@ -12106,11 +12154,11 @@
       </c>
       <c r="B355">
         <f t="shared" si="63"/>
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C355" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-98</v>
+        <v>31-95</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
@@ -12122,11 +12170,11 @@
       </c>
       <c r="B356">
         <f t="shared" si="63"/>
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C356" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-99</v>
+        <v>31-96</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
@@ -12138,11 +12186,11 @@
       </c>
       <c r="B357">
         <f t="shared" si="63"/>
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C357" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-100</v>
+        <v>31-97</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
@@ -12154,11 +12202,11 @@
       </c>
       <c r="B358">
         <f t="shared" si="63"/>
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C358" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-101</v>
+        <v>31-98</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
@@ -12170,11 +12218,11 @@
       </c>
       <c r="B359">
         <f t="shared" si="63"/>
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C359" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-102</v>
+        <v>31-99</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
@@ -12186,11 +12234,11 @@
       </c>
       <c r="B360">
         <f t="shared" si="63"/>
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C360" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-103</v>
+        <v>31-100</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
@@ -12202,11 +12250,11 @@
       </c>
       <c r="B361">
         <f t="shared" si="63"/>
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C361" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-104</v>
+        <v>31-101</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
@@ -12218,11 +12266,11 @@
       </c>
       <c r="B362">
         <f t="shared" si="63"/>
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C362" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-105</v>
+        <v>31-102</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
@@ -12234,11 +12282,11 @@
       </c>
       <c r="B363">
         <f t="shared" si="63"/>
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C363" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-106</v>
+        <v>31-103</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
@@ -12250,11 +12298,11 @@
       </c>
       <c r="B364">
         <f t="shared" si="63"/>
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C364" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-107</v>
+        <v>31-104</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
@@ -12266,11 +12314,11 @@
       </c>
       <c r="B365">
         <f t="shared" si="63"/>
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C365" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-108</v>
+        <v>31-105</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
@@ -12282,11 +12330,11 @@
       </c>
       <c r="B366">
         <f t="shared" si="63"/>
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C366" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-109</v>
+        <v>31-106</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
@@ -12298,11 +12346,11 @@
       </c>
       <c r="B367">
         <f t="shared" si="63"/>
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C367" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-110</v>
+        <v>31-107</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
@@ -12314,11 +12362,11 @@
       </c>
       <c r="B368">
         <f t="shared" si="63"/>
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C368" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-111</v>
+        <v>31-108</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
@@ -12330,11 +12378,11 @@
       </c>
       <c r="B369">
         <f t="shared" si="63"/>
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C369" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-112</v>
+        <v>31-109</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
@@ -12346,11 +12394,11 @@
       </c>
       <c r="B370">
         <f t="shared" si="63"/>
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C370" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-113</v>
+        <v>31-110</v>
       </c>
       <c r="L370" s="6"/>
       <c r="M370" s="6"/>
@@ -12362,11 +12410,11 @@
       </c>
       <c r="B371">
         <f t="shared" si="63"/>
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C371" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-114</v>
+        <v>31-111</v>
       </c>
       <c r="L371" s="6"/>
       <c r="M371" s="6"/>
@@ -12377,76 +12425,76 @@
         <v>31</v>
       </c>
       <c r="B372">
-        <f t="shared" ref="B372:B393" si="66">IF(A372=A371,B371+1,1)</f>
-        <v>115</v>
+        <f t="shared" si="63"/>
+        <v>112</v>
       </c>
       <c r="C372" s="3" t="str">
-        <f t="shared" ref="C372:C393" si="67">CONCATENATE(A372,"-",B372)</f>
-        <v>31-115</v>
+        <f t="shared" si="64"/>
+        <v>31-112</v>
       </c>
       <c r="L372" s="6"/>
       <c r="M372" s="6"/>
     </row>
     <row r="373" spans="1:13" ht="15">
       <c r="A373">
-        <f t="shared" ref="A373:A393" si="68">A372</f>
+        <f t="shared" si="65"/>
         <v>31</v>
       </c>
       <c r="B373">
+        <f t="shared" si="63"/>
+        <v>113</v>
+      </c>
+      <c r="C373" s="3" t="str">
+        <f t="shared" si="64"/>
+        <v>31-113</v>
+      </c>
+      <c r="L373" s="6"/>
+      <c r="M373" s="6"/>
+    </row>
+    <row r="374" spans="1:13" ht="15">
+      <c r="A374">
+        <f t="shared" si="65"/>
+        <v>31</v>
+      </c>
+      <c r="B374">
+        <f t="shared" si="63"/>
+        <v>114</v>
+      </c>
+      <c r="C374" s="3" t="str">
+        <f t="shared" si="64"/>
+        <v>31-114</v>
+      </c>
+      <c r="L374" s="6"/>
+      <c r="M374" s="6"/>
+    </row>
+    <row r="375" spans="1:13" ht="15">
+      <c r="A375">
+        <f t="shared" si="65"/>
+        <v>31</v>
+      </c>
+      <c r="B375">
+        <f t="shared" ref="B375:B396" si="66">IF(A375=A374,B374+1,1)</f>
+        <v>115</v>
+      </c>
+      <c r="C375" s="3" t="str">
+        <f t="shared" ref="C375:C396" si="67">CONCATENATE(A375,"-",B375)</f>
+        <v>31-115</v>
+      </c>
+      <c r="L375" s="6"/>
+      <c r="M375" s="6"/>
+    </row>
+    <row r="376" spans="1:13" ht="15">
+      <c r="A376">
+        <f t="shared" ref="A376:A396" si="68">A375</f>
+        <v>31</v>
+      </c>
+      <c r="B376">
         <f t="shared" si="66"/>
         <v>116</v>
       </c>
-      <c r="C373" s="3" t="str">
+      <c r="C376" s="3" t="str">
         <f t="shared" si="67"/>
         <v>31-116</v>
-      </c>
-      <c r="L373" s="6"/>
-      <c r="M373" s="6"/>
-    </row>
-    <row r="374" spans="1:13" ht="15">
-      <c r="A374">
-        <f t="shared" si="68"/>
-        <v>31</v>
-      </c>
-      <c r="B374">
-        <f t="shared" si="66"/>
-        <v>117</v>
-      </c>
-      <c r="C374" s="3" t="str">
-        <f t="shared" si="67"/>
-        <v>31-117</v>
-      </c>
-      <c r="L374" s="6"/>
-      <c r="M374" s="6"/>
-    </row>
-    <row r="375" spans="1:13" ht="15">
-      <c r="A375">
-        <f t="shared" si="68"/>
-        <v>31</v>
-      </c>
-      <c r="B375">
-        <f t="shared" si="66"/>
-        <v>118</v>
-      </c>
-      <c r="C375" s="3" t="str">
-        <f t="shared" si="67"/>
-        <v>31-118</v>
-      </c>
-      <c r="L375" s="6"/>
-      <c r="M375" s="6"/>
-    </row>
-    <row r="376" spans="1:13" ht="15">
-      <c r="A376">
-        <f t="shared" si="68"/>
-        <v>31</v>
-      </c>
-      <c r="B376">
-        <f t="shared" si="66"/>
-        <v>119</v>
-      </c>
-      <c r="C376" s="3" t="str">
-        <f t="shared" si="67"/>
-        <v>31-119</v>
       </c>
       <c r="L376" s="6"/>
       <c r="M376" s="6"/>
@@ -12458,11 +12506,11 @@
       </c>
       <c r="B377">
         <f t="shared" si="66"/>
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C377" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-120</v>
+        <v>31-117</v>
       </c>
       <c r="L377" s="6"/>
       <c r="M377" s="6"/>
@@ -12474,11 +12522,11 @@
       </c>
       <c r="B378">
         <f t="shared" si="66"/>
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C378" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-121</v>
+        <v>31-118</v>
       </c>
       <c r="L378" s="6"/>
       <c r="M378" s="6"/>
@@ -12490,11 +12538,11 @@
       </c>
       <c r="B379">
         <f t="shared" si="66"/>
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C379" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-122</v>
+        <v>31-119</v>
       </c>
       <c r="L379" s="6"/>
       <c r="M379" s="6"/>
@@ -12506,11 +12554,11 @@
       </c>
       <c r="B380">
         <f t="shared" si="66"/>
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C380" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-123</v>
+        <v>31-120</v>
       </c>
       <c r="L380" s="6"/>
       <c r="M380" s="6"/>
@@ -12522,11 +12570,11 @@
       </c>
       <c r="B381">
         <f t="shared" si="66"/>
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C381" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-124</v>
+        <v>31-121</v>
       </c>
       <c r="L381" s="6"/>
       <c r="M381" s="6"/>
@@ -12538,11 +12586,11 @@
       </c>
       <c r="B382">
         <f t="shared" si="66"/>
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C382" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-125</v>
+        <v>31-122</v>
       </c>
       <c r="L382" s="6"/>
       <c r="M382" s="6"/>
@@ -12554,11 +12602,11 @@
       </c>
       <c r="B383">
         <f t="shared" si="66"/>
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C383" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-126</v>
+        <v>31-123</v>
       </c>
       <c r="L383" s="6"/>
       <c r="M383" s="6"/>
@@ -12570,11 +12618,11 @@
       </c>
       <c r="B384">
         <f t="shared" si="66"/>
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C384" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-127</v>
+        <v>31-124</v>
       </c>
       <c r="L384" s="6"/>
       <c r="M384" s="6"/>
@@ -12586,11 +12634,11 @@
       </c>
       <c r="B385">
         <f t="shared" si="66"/>
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C385" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-128</v>
+        <v>31-125</v>
       </c>
       <c r="L385" s="6"/>
       <c r="M385" s="6"/>
@@ -12602,11 +12650,11 @@
       </c>
       <c r="B386">
         <f t="shared" si="66"/>
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C386" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-129</v>
+        <v>31-126</v>
       </c>
       <c r="L386" s="6"/>
       <c r="M386" s="6"/>
@@ -12618,11 +12666,11 @@
       </c>
       <c r="B387">
         <f t="shared" si="66"/>
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C387" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-130</v>
+        <v>31-127</v>
       </c>
       <c r="L387" s="6"/>
       <c r="M387" s="6"/>
@@ -12634,11 +12682,11 @@
       </c>
       <c r="B388">
         <f t="shared" si="66"/>
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C388" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-131</v>
+        <v>31-128</v>
       </c>
       <c r="L388" s="6"/>
       <c r="M388" s="6"/>
@@ -12650,11 +12698,11 @@
       </c>
       <c r="B389">
         <f t="shared" si="66"/>
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C389" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-132</v>
+        <v>31-129</v>
       </c>
       <c r="L389" s="6"/>
       <c r="M389" s="6"/>
@@ -12666,11 +12714,11 @@
       </c>
       <c r="B390">
         <f t="shared" si="66"/>
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C390" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-133</v>
+        <v>31-130</v>
       </c>
       <c r="L390" s="6"/>
       <c r="M390" s="6"/>
@@ -12682,11 +12730,11 @@
       </c>
       <c r="B391">
         <f t="shared" si="66"/>
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C391" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-134</v>
+        <v>31-131</v>
       </c>
       <c r="L391" s="6"/>
       <c r="M391" s="6"/>
@@ -12698,11 +12746,11 @@
       </c>
       <c r="B392">
         <f t="shared" si="66"/>
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C392" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-135</v>
+        <v>31-132</v>
       </c>
       <c r="L392" s="6"/>
       <c r="M392" s="6"/>
@@ -12714,24 +12762,60 @@
       </c>
       <c r="B393">
         <f t="shared" si="66"/>
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C393" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-136</v>
+        <v>31-133</v>
       </c>
       <c r="L393" s="6"/>
       <c r="M393" s="6"/>
     </row>
-    <row r="394" spans="1:13" ht="12.75">
+    <row r="394" spans="1:13" ht="15">
+      <c r="A394">
+        <f t="shared" si="68"/>
+        <v>31</v>
+      </c>
+      <c r="B394">
+        <f t="shared" si="66"/>
+        <v>134</v>
+      </c>
+      <c r="C394" s="3" t="str">
+        <f t="shared" si="67"/>
+        <v>31-134</v>
+      </c>
       <c r="L394" s="6"/>
       <c r="M394" s="6"/>
     </row>
-    <row r="395" spans="1:13" ht="12.75">
+    <row r="395" spans="1:13" ht="15">
+      <c r="A395">
+        <f t="shared" si="68"/>
+        <v>31</v>
+      </c>
+      <c r="B395">
+        <f t="shared" si="66"/>
+        <v>135</v>
+      </c>
+      <c r="C395" s="3" t="str">
+        <f t="shared" si="67"/>
+        <v>31-135</v>
+      </c>
       <c r="L395" s="6"/>
       <c r="M395" s="6"/>
     </row>
-    <row r="396" spans="1:13" ht="12.75">
+    <row r="396" spans="1:13" ht="15">
+      <c r="A396">
+        <f t="shared" si="68"/>
+        <v>31</v>
+      </c>
+      <c r="B396">
+        <f t="shared" si="66"/>
+        <v>136</v>
+      </c>
+      <c r="C396" s="3" t="str">
+        <f t="shared" si="67"/>
+        <v>31-136</v>
+      </c>
       <c r="L396" s="6"/>
       <c r="M396" s="6"/>
     </row>
@@ -15470,12 +15554,24 @@
     <row r="1080" spans="12:13" ht="12.75">
       <c r="L1080" s="6"/>
       <c r="M1080" s="6"/>
+    </row>
+    <row r="1081" spans="12:13" ht="12.75">
+      <c r="L1081" s="6"/>
+      <c r="M1081" s="6"/>
+    </row>
+    <row r="1082" spans="12:13" ht="12.75">
+      <c r="L1082" s="6"/>
+      <c r="M1082" s="6"/>
+    </row>
+    <row r="1083" spans="12:13" ht="12.75">
+      <c r="L1083" s="6"/>
+      <c r="M1083" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="L195:L198"/>
     <mergeCell ref="L248:L249"/>
-    <mergeCell ref="L250:L255"/>
+    <mergeCell ref="L253:L258"/>
   </mergeCells>
   <conditionalFormatting sqref="K162:K206 K99:K158 K2:K97">
     <cfRule type="containsBlanks" dxfId="92" priority="97">
@@ -15837,17 +15933,17 @@
       <formula>NOT(ISERROR(SEARCH(("fail"),(K248))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K249">
+  <conditionalFormatting sqref="K249:K252">
     <cfRule type="containsBlanks" dxfId="20" priority="19">
       <formula>LEN(TRIM(K249))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K249">
+  <conditionalFormatting sqref="K249:K252">
     <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K249))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K249">
+  <conditionalFormatting sqref="K249:K252">
     <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K249))))</formula>
     </cfRule>
@@ -15867,64 +15963,64 @@
       <formula>NOT(ISERROR(SEARCH(("fail"),(K159))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K250:K251">
+  <conditionalFormatting sqref="K253:K254">
     <cfRule type="containsBlanks" dxfId="14" priority="13">
-      <formula>LEN(TRIM(K250))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K250:K251">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K250))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K250:K251">
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K250))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K252">
-    <cfRule type="containsBlanks" dxfId="11" priority="10">
-      <formula>LEN(TRIM(K252))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K252">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K252))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K252">
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K252))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K253:K255">
-    <cfRule type="containsBlanks" dxfId="8" priority="7">
       <formula>LEN(TRIM(K253))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K253:K255">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K253:K254">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K253))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K253:K255">
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
+  <conditionalFormatting sqref="K253:K254">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K253))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K256:K261">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
+  <conditionalFormatting sqref="K255">
+    <cfRule type="containsBlanks" dxfId="11" priority="10">
+      <formula>LEN(TRIM(K255))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K255">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K255))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K255">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K255))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K256:K258">
+    <cfRule type="containsBlanks" dxfId="8" priority="7">
       <formula>LEN(TRIM(K256))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K256:K261">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K256:K258">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K256))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K256:K261">
+  <conditionalFormatting sqref="K256:K258">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K256))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K259:K264">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
+      <formula>LEN(TRIM(K259))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K259:K264">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K259))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K259:K264">
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K256))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K259))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98">

</xml_diff>

<commit_message>
Update manual system test spreadsheet
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="359">
   <si>
     <t>Test Number</t>
   </si>
@@ -1098,6 +1098,19 @@
   </si>
   <si>
     <t>Spectra Plots: Check that setting the spectra / period number updates the plot on a running instrument</t>
+  </si>
+  <si>
+    <t>Menu items</t>
+  </si>
+  <si>
+    <t>Check that you can login to "manager mode" with the instrument scientist password. (Ibex menu -&gt; manager mode).
+Check that the banner item indicates that you have succesfully entered manager mode (you should see "manager mode: active" in red).</t>
+  </si>
+  <si>
+    <t>Cannot be automated because this test uses a password.</t>
+  </si>
+  <si>
+    <t>Check that you can log out from "manager mode" after performing the above test.</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1316,11 +1329,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1458,6 +1482,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3066,8 +3095,8 @@
   <dimension ref="A1:N1087"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J50" sqref="J50"/>
+      <pane ySplit="1" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F270" sqref="F270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10807,7 +10836,7 @@
       <c r="L267" s="26"/>
       <c r="M267" s="6"/>
     </row>
-    <row r="268" spans="1:13" ht="15">
+    <row r="268" spans="1:13" ht="90">
       <c r="A268">
         <v>31</v>
       </c>
@@ -10821,16 +10850,26 @@
       </c>
       <c r="D268" s="23"/>
       <c r="E268" s="23"/>
-      <c r="F268" s="23"/>
-      <c r="G268" s="23"/>
-      <c r="H268" s="24"/>
-      <c r="I268" s="25"/>
+      <c r="F268" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="G268" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="H268" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="I268" s="25" t="s">
+        <v>356</v>
+      </c>
       <c r="J268" s="23"/>
       <c r="K268" s="21"/>
-      <c r="L268" s="26"/>
+      <c r="L268" s="26" t="s">
+        <v>357</v>
+      </c>
       <c r="M268" s="6"/>
     </row>
-    <row r="269" spans="1:13" ht="15">
+    <row r="269" spans="1:13" ht="26.25">
       <c r="A269">
         <f t="shared" si="56"/>
         <v>31</v>
@@ -10842,6 +10881,18 @@
       <c r="C269" s="3" t="str">
         <f t="shared" si="55"/>
         <v>31-5</v>
+      </c>
+      <c r="F269" s="60" t="s">
+        <v>241</v>
+      </c>
+      <c r="G269" s="60" t="s">
+        <v>241</v>
+      </c>
+      <c r="H269" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="I269" s="62" t="s">
+        <v>358</v>
       </c>
       <c r="L269" s="6"/>
       <c r="M269" s="6"/>
@@ -10859,6 +10910,9 @@
         <f t="shared" si="55"/>
         <v>31-6</v>
       </c>
+      <c r="F270" s="60"/>
+      <c r="G270" s="60"/>
+      <c r="H270" s="61"/>
       <c r="L270" s="6"/>
       <c r="M270" s="6"/>
     </row>

</xml_diff>

<commit_message>
Added test for group with only hidden blocks
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="364">
   <si>
     <t>Test Number</t>
   </si>
@@ -1120,6 +1120,15 @@
 Add the component to a config
 Load the config and run the IOC
 Confirm it has the settings set in component </t>
+  </si>
+  <si>
+    <t>21-27</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Create a group containing ONLY hidden blocks. Verify that the group is NOT shown, except when the right-click option "Shown hidden blocks" is selected</t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1349,11 +1358,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1497,6 +1519,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3101,11 +3137,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1088"/>
+  <dimension ref="A1:N1089"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J165" sqref="J165"/>
+      <pane ySplit="1" topLeftCell="A225" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G235" sqref="G235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -7850,7 +7886,7 @@
         <v>1</v>
       </c>
       <c r="C167" s="22" t="str">
-        <f t="shared" ref="C167:C245" si="27">CONCATENATE(A167,"-",B167)</f>
+        <f t="shared" ref="C167:C246" si="27">CONCATENATE(A167,"-",B167)</f>
         <v>16-1</v>
       </c>
       <c r="D167" s="46"/>
@@ -7872,11 +7908,11 @@
     </row>
     <row r="168" spans="1:13" ht="15">
       <c r="A168">
-        <f t="shared" ref="A168:A246" si="28">A167</f>
+        <f t="shared" ref="A168:A247" si="28">A167</f>
         <v>16</v>
       </c>
       <c r="B168">
-        <f t="shared" ref="B168:B246" si="29">IF(A168=A167,B167+1,1)</f>
+        <f t="shared" ref="B168:B247" si="29">IF(A168=A167,B167+1,1)</f>
         <v>2</v>
       </c>
       <c r="C168" s="22" t="str">
@@ -9835,72 +9871,65 @@
       <c r="L232" s="49"/>
       <c r="M232" s="6"/>
     </row>
-    <row r="233" spans="1:13" ht="26.25">
-      <c r="A233">
+    <row r="233" spans="1:13" s="23" customFormat="1" ht="51.75">
+      <c r="C233" s="22" t="s">
+        <v>361</v>
+      </c>
+      <c r="D233" s="69">
+        <v>1672</v>
+      </c>
+      <c r="E233" s="69"/>
+      <c r="F233" s="69"/>
+      <c r="G233" s="70"/>
+      <c r="H233" s="70" t="s">
+        <v>362</v>
+      </c>
+      <c r="I233" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="J233" s="26"/>
+      <c r="K233" s="70"/>
+      <c r="L233" s="26"/>
+      <c r="M233" s="26"/>
+    </row>
+    <row r="234" spans="1:13" ht="26.25">
+      <c r="A234">
         <v>22</v>
       </c>
-      <c r="B233">
+      <c r="B234">
         <v>1</v>
       </c>
-      <c r="C233" s="22" t="str">
-        <f>CONCATENATE(A233,"-",B233)</f>
+      <c r="C234" s="63" t="str">
+        <f>CONCATENATE(A234,"-",B234)</f>
         <v>22-1</v>
       </c>
-      <c r="D233" s="23"/>
-      <c r="E233" s="23"/>
-      <c r="F233" s="23"/>
-      <c r="G233" s="24"/>
-      <c r="H233" s="24" t="s">
+      <c r="D234" s="64"/>
+      <c r="E234" s="64"/>
+      <c r="F234" s="64"/>
+      <c r="G234" s="65"/>
+      <c r="H234" s="65" t="s">
         <v>248</v>
       </c>
-      <c r="I233" s="25" t="s">
+      <c r="I234" s="66" t="s">
         <v>247</v>
       </c>
-      <c r="J233" s="23"/>
-      <c r="K233" s="21"/>
-      <c r="L233" s="26"/>
-      <c r="M233" s="6"/>
-    </row>
-    <row r="234" spans="1:13" ht="39">
-      <c r="A234">
-        <f>A233</f>
+      <c r="J234" s="64"/>
+      <c r="K234" s="67"/>
+      <c r="L234" s="68"/>
+      <c r="M234" s="6"/>
+    </row>
+    <row r="235" spans="1:13" ht="39">
+      <c r="A235">
+        <f>A234</f>
         <v>22</v>
       </c>
-      <c r="B234">
-        <f>IF(A234=A233,B233+1,1)</f>
+      <c r="B235">
+        <f>IF(A235=A234,B234+1,1)</f>
         <v>2</v>
       </c>
-      <c r="C234" s="22" t="str">
+      <c r="C235" s="22" t="str">
         <f t="shared" si="27"/>
         <v>22-2</v>
-      </c>
-      <c r="D234" s="23"/>
-      <c r="E234" s="23"/>
-      <c r="F234" s="23"/>
-      <c r="G234" s="23"/>
-      <c r="H234" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="I234" s="25" t="s">
-        <v>249</v>
-      </c>
-      <c r="J234" s="23"/>
-      <c r="K234" s="21"/>
-      <c r="L234" s="26"/>
-      <c r="M234" s="6"/>
-    </row>
-    <row r="235" spans="1:13" ht="26.25">
-      <c r="A235">
-        <f t="shared" si="28"/>
-        <v>22</v>
-      </c>
-      <c r="B235">
-        <f t="shared" si="29"/>
-        <v>3</v>
-      </c>
-      <c r="C235" s="22" t="str">
-        <f t="shared" si="27"/>
-        <v>22-3</v>
       </c>
       <c r="D235" s="23"/>
       <c r="E235" s="23"/>
@@ -9910,25 +9939,25 @@
         <v>248</v>
       </c>
       <c r="I235" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J235" s="23"/>
       <c r="K235" s="21"/>
       <c r="L235" s="26"/>
       <c r="M235" s="6"/>
     </row>
-    <row r="236" spans="1:13" ht="15">
+    <row r="236" spans="1:13" ht="26.25">
       <c r="A236">
         <f t="shared" si="28"/>
         <v>22</v>
       </c>
       <c r="B236">
         <f t="shared" si="29"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C236" s="22" t="str">
         <f t="shared" si="27"/>
-        <v>22-4</v>
+        <v>22-3</v>
       </c>
       <c r="D236" s="23"/>
       <c r="E236" s="23"/>
@@ -9938,7 +9967,7 @@
         <v>248</v>
       </c>
       <c r="I236" s="25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J236" s="23"/>
       <c r="K236" s="21"/>
@@ -9952,11 +9981,11 @@
       </c>
       <c r="B237">
         <f t="shared" si="29"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C237" s="22" t="str">
         <f t="shared" si="27"/>
-        <v>22-5</v>
+        <v>22-4</v>
       </c>
       <c r="D237" s="23"/>
       <c r="E237" s="23"/>
@@ -9966,7 +9995,7 @@
         <v>248</v>
       </c>
       <c r="I237" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J237" s="23"/>
       <c r="K237" s="21"/>
@@ -9980,68 +10009,66 @@
       </c>
       <c r="B238">
         <f t="shared" si="29"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C238" s="22" t="str">
         <f t="shared" si="27"/>
-        <v>22-6</v>
-      </c>
-      <c r="D238" s="36"/>
-      <c r="E238" s="36"/>
-      <c r="F238" s="36"/>
-      <c r="G238" s="36"/>
-      <c r="H238" s="27" t="s">
+        <v>22-5</v>
+      </c>
+      <c r="D238" s="23"/>
+      <c r="E238" s="23"/>
+      <c r="F238" s="23"/>
+      <c r="G238" s="23"/>
+      <c r="H238" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="I238" s="37" t="s">
-        <v>253</v>
-      </c>
-      <c r="J238" s="36"/>
+      <c r="I238" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="J238" s="23"/>
       <c r="K238" s="21"/>
-      <c r="L238" s="38"/>
+      <c r="L238" s="26"/>
       <c r="M238" s="6"/>
     </row>
-    <row r="239" spans="1:13" ht="26.25">
+    <row r="239" spans="1:13" ht="15">
       <c r="A239">
-        <v>23</v>
+        <f t="shared" si="28"/>
+        <v>22</v>
       </c>
       <c r="B239">
         <f t="shared" si="29"/>
+        <v>6</v>
+      </c>
+      <c r="C239" s="22" t="str">
+        <f t="shared" si="27"/>
+        <v>22-6</v>
+      </c>
+      <c r="D239" s="36"/>
+      <c r="E239" s="36"/>
+      <c r="F239" s="36"/>
+      <c r="G239" s="36"/>
+      <c r="H239" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="I239" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="J239" s="36"/>
+      <c r="K239" s="21"/>
+      <c r="L239" s="38"/>
+      <c r="M239" s="6"/>
+    </row>
+    <row r="240" spans="1:13" ht="26.25">
+      <c r="A240">
+        <v>23</v>
+      </c>
+      <c r="B240">
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
-      <c r="C239" s="35" t="str">
+      <c r="C240" s="35" t="str">
         <f t="shared" si="27"/>
         <v>23-1</v>
-      </c>
-      <c r="D239" s="23"/>
-      <c r="E239" s="23"/>
-      <c r="F239" s="23"/>
-      <c r="G239" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="H239" s="24" t="s">
-        <v>265</v>
-      </c>
-      <c r="I239" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="J239" s="23"/>
-      <c r="K239" s="21"/>
-      <c r="L239" s="26"/>
-      <c r="M239" s="6"/>
-    </row>
-    <row r="240" spans="1:13" ht="26.25">
-      <c r="A240">
-        <f t="shared" si="28"/>
-        <v>23</v>
-      </c>
-      <c r="B240">
-        <f t="shared" si="29"/>
-        <v>2</v>
-      </c>
-      <c r="C240" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v>23-2</v>
       </c>
       <c r="D240" s="23"/>
       <c r="E240" s="23"/>
@@ -10053,7 +10080,7 @@
         <v>265</v>
       </c>
       <c r="I240" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J240" s="23"/>
       <c r="K240" s="21"/>
@@ -10067,11 +10094,11 @@
       </c>
       <c r="B241">
         <f t="shared" si="29"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C241" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>23-3</v>
+        <v>23-2</v>
       </c>
       <c r="D241" s="23"/>
       <c r="E241" s="23"/>
@@ -10083,25 +10110,25 @@
         <v>265</v>
       </c>
       <c r="I241" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J241" s="23"/>
       <c r="K241" s="21"/>
       <c r="L241" s="26"/>
       <c r="M241" s="6"/>
     </row>
-    <row r="242" spans="1:13" ht="39">
+    <row r="242" spans="1:13" ht="26.25">
       <c r="A242">
         <f t="shared" si="28"/>
         <v>23</v>
       </c>
       <c r="B242">
         <f t="shared" si="29"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C242" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>23-4</v>
+        <v>23-3</v>
       </c>
       <c r="D242" s="23"/>
       <c r="E242" s="23"/>
@@ -10113,25 +10140,25 @@
         <v>265</v>
       </c>
       <c r="I242" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J242" s="23"/>
       <c r="K242" s="21"/>
       <c r="L242" s="26"/>
       <c r="M242" s="6"/>
     </row>
-    <row r="243" spans="1:13" ht="15">
+    <row r="243" spans="1:13" ht="39">
       <c r="A243">
         <f t="shared" si="28"/>
         <v>23</v>
       </c>
       <c r="B243">
         <f t="shared" si="29"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C243" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>23-5</v>
+        <v>23-4</v>
       </c>
       <c r="D243" s="23"/>
       <c r="E243" s="23"/>
@@ -10143,23 +10170,25 @@
         <v>265</v>
       </c>
       <c r="I243" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J243" s="23"/>
       <c r="K243" s="21"/>
       <c r="L243" s="26"/>
       <c r="M243" s="6"/>
     </row>
-    <row r="244" spans="1:13" ht="26.25">
+    <row r="244" spans="1:13" ht="15">
       <c r="A244">
-        <v>24</v>
+        <f t="shared" si="28"/>
+        <v>23</v>
       </c>
       <c r="B244">
-        <v>6</v>
+        <f t="shared" si="29"/>
+        <v>5</v>
       </c>
       <c r="C244" s="3" t="str">
-        <f t="shared" ref="C244" si="52">CONCATENATE(A244,"-",B244)</f>
-        <v>24-6</v>
+        <f t="shared" si="27"/>
+        <v>23-5</v>
       </c>
       <c r="D244" s="23"/>
       <c r="E244" s="23"/>
@@ -10171,7 +10200,7 @@
         <v>265</v>
       </c>
       <c r="I244" s="25" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="J244" s="23"/>
       <c r="K244" s="21"/>
@@ -10180,15 +10209,14 @@
     </row>
     <row r="245" spans="1:13" ht="26.25">
       <c r="A245">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B245">
-        <f>IF(A245=A243,B243+1,1)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C245" s="3" t="str">
-        <f t="shared" si="27"/>
-        <v>25-1</v>
+        <f t="shared" ref="C245" si="52">CONCATENATE(A245,"-",B245)</f>
+        <v>24-6</v>
       </c>
       <c r="D245" s="23"/>
       <c r="E245" s="23"/>
@@ -10197,10 +10225,10 @@
         <v>62</v>
       </c>
       <c r="H245" s="24" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="I245" s="25" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="J245" s="23"/>
       <c r="K245" s="21"/>
@@ -10209,16 +10237,15 @@
     </row>
     <row r="246" spans="1:13" ht="26.25">
       <c r="A246">
-        <f t="shared" si="28"/>
         <v>25</v>
       </c>
       <c r="B246">
-        <f t="shared" si="29"/>
-        <v>2</v>
+        <f>IF(A246=A244,B244+1,1)</f>
+        <v>1</v>
       </c>
       <c r="C246" s="3" t="str">
-        <f t="shared" ref="C246" si="53">CONCATENATE(A246,"-",B246)</f>
-        <v>25-2</v>
+        <f t="shared" si="27"/>
+        <v>25-1</v>
       </c>
       <c r="D246" s="23"/>
       <c r="E246" s="23"/>
@@ -10230,52 +10257,54 @@
         <v>271</v>
       </c>
       <c r="I246" s="25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J246" s="23"/>
       <c r="K246" s="21"/>
       <c r="L246" s="26"/>
       <c r="M246" s="6"/>
     </row>
-    <row r="247" spans="1:13" ht="39">
+    <row r="247" spans="1:13" ht="26.25">
       <c r="A247">
-        <v>26</v>
+        <f t="shared" si="28"/>
+        <v>25</v>
       </c>
       <c r="B247">
-        <f t="shared" ref="B247:B315" si="54">IF(A247=A246,B246+1,1)</f>
-        <v>1</v>
+        <f t="shared" si="29"/>
+        <v>2</v>
       </c>
       <c r="C247" s="3" t="str">
-        <f t="shared" ref="C247:C315" si="55">CONCATENATE(A247,"-",B247)</f>
-        <v>26-1</v>
+        <f t="shared" ref="C247" si="53">CONCATENATE(A247,"-",B247)</f>
+        <v>25-2</v>
       </c>
       <c r="D247" s="23"/>
       <c r="E247" s="23"/>
       <c r="F247" s="23"/>
-      <c r="G247" s="23"/>
+      <c r="G247" s="23" t="s">
+        <v>62</v>
+      </c>
       <c r="H247" s="24" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="I247" s="25" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="J247" s="23"/>
       <c r="K247" s="21"/>
       <c r="L247" s="26"/>
       <c r="M247" s="6"/>
     </row>
-    <row r="248" spans="1:13" ht="15">
+    <row r="248" spans="1:13" ht="39">
       <c r="A248">
-        <f t="shared" ref="A248:A316" si="56">A247</f>
         <v>26</v>
       </c>
       <c r="B248">
-        <f t="shared" si="54"/>
-        <v>2</v>
+        <f t="shared" ref="B248:B316" si="54">IF(A248=A247,B247+1,1)</f>
+        <v>1</v>
       </c>
       <c r="C248" s="3" t="str">
-        <f t="shared" si="55"/>
-        <v>26-2</v>
+        <f t="shared" ref="C248:C316" si="55">CONCATENATE(A248,"-",B248)</f>
+        <v>26-1</v>
       </c>
       <c r="D248" s="23"/>
       <c r="E248" s="23"/>
@@ -10285,34 +10314,35 @@
         <v>294</v>
       </c>
       <c r="I248" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J248" s="23"/>
       <c r="K248" s="21"/>
       <c r="L248" s="26"/>
       <c r="M248" s="6"/>
     </row>
-    <row r="249" spans="1:13" ht="26.25">
+    <row r="249" spans="1:13" ht="15">
       <c r="A249">
-        <v>27</v>
+        <f t="shared" ref="A249:A317" si="56">A248</f>
+        <v>26</v>
       </c>
       <c r="B249">
         <f t="shared" si="54"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C249" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>27-1</v>
+        <v>26-2</v>
       </c>
       <c r="D249" s="23"/>
       <c r="E249" s="23"/>
       <c r="F249" s="23"/>
       <c r="G249" s="23"/>
       <c r="H249" s="24" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="I249" s="25" t="s">
-        <v>327</v>
+        <v>296</v>
       </c>
       <c r="J249" s="23"/>
       <c r="K249" s="21"/>
@@ -10321,16 +10351,15 @@
     </row>
     <row r="250" spans="1:13" ht="26.25">
       <c r="A250">
-        <f>A249</f>
         <v>27</v>
       </c>
       <c r="B250">
         <f t="shared" si="54"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C250" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>27-2</v>
+        <v>27-1</v>
       </c>
       <c r="D250" s="23"/>
       <c r="E250" s="23"/>
@@ -10340,7 +10369,7 @@
         <v>299</v>
       </c>
       <c r="I250" s="25" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="J250" s="23"/>
       <c r="K250" s="21"/>
@@ -10353,12 +10382,12 @@
         <v>27</v>
       </c>
       <c r="B251">
-        <f t="shared" ref="B251" si="57">IF(A251=A250,B250+1,1)</f>
-        <v>3</v>
+        <f t="shared" si="54"/>
+        <v>2</v>
       </c>
       <c r="C251" s="3" t="str">
-        <f t="shared" ref="C251" si="58">CONCATENATE(A251,"-",B251)</f>
-        <v>27-3</v>
+        <f t="shared" si="55"/>
+        <v>27-2</v>
       </c>
       <c r="D251" s="23"/>
       <c r="E251" s="23"/>
@@ -10368,25 +10397,25 @@
         <v>299</v>
       </c>
       <c r="I251" s="25" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
       <c r="J251" s="23"/>
       <c r="K251" s="21"/>
       <c r="L251" s="26"/>
       <c r="M251" s="6"/>
     </row>
-    <row r="252" spans="1:13" ht="39">
+    <row r="252" spans="1:13" ht="26.25">
       <c r="A252">
         <f>A251</f>
         <v>27</v>
       </c>
       <c r="B252">
-        <f t="shared" ref="B252" si="59">IF(A252=A251,B251+1,1)</f>
-        <v>4</v>
+        <f t="shared" ref="B252" si="57">IF(A252=A251,B251+1,1)</f>
+        <v>3</v>
       </c>
       <c r="C252" s="3" t="str">
-        <f t="shared" ref="C252" si="60">CONCATENATE(A252,"-",B252)</f>
-        <v>27-4</v>
+        <f t="shared" ref="C252" si="58">CONCATENATE(A252,"-",B252)</f>
+        <v>27-3</v>
       </c>
       <c r="D252" s="23"/>
       <c r="E252" s="23"/>
@@ -10396,54 +10425,52 @@
         <v>299</v>
       </c>
       <c r="I252" s="25" t="s">
-        <v>328</v>
+        <v>300</v>
       </c>
       <c r="J252" s="23"/>
       <c r="K252" s="21"/>
       <c r="L252" s="26"/>
       <c r="M252" s="6"/>
     </row>
-    <row r="253" spans="1:13" ht="39" customHeight="1">
+    <row r="253" spans="1:13" ht="39">
       <c r="A253">
-        <v>28</v>
+        <f>A252</f>
+        <v>27</v>
       </c>
       <c r="B253">
-        <f t="shared" si="54"/>
-        <v>1</v>
+        <f t="shared" ref="B253" si="59">IF(A253=A252,B252+1,1)</f>
+        <v>4</v>
       </c>
       <c r="C253" s="3" t="str">
-        <f t="shared" si="55"/>
-        <v>28-1</v>
+        <f t="shared" ref="C253" si="60">CONCATENATE(A253,"-",B253)</f>
+        <v>27-4</v>
       </c>
       <c r="D253" s="23"/>
       <c r="E253" s="23"/>
       <c r="F253" s="23"/>
       <c r="G253" s="23"/>
       <c r="H253" s="24" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I253" s="25" t="s">
-        <v>302</v>
+        <v>328</v>
       </c>
       <c r="J253" s="23"/>
       <c r="K253" s="21"/>
-      <c r="L253" s="60" t="s">
-        <v>305</v>
-      </c>
+      <c r="L253" s="26"/>
       <c r="M253" s="6"/>
     </row>
-    <row r="254" spans="1:13" ht="26.25">
+    <row r="254" spans="1:13" ht="39" customHeight="1">
       <c r="A254">
-        <f>A253</f>
         <v>28</v>
       </c>
       <c r="B254">
-        <f>IF(A254=A253,B253+1,1)</f>
-        <v>2</v>
+        <f t="shared" si="54"/>
+        <v>1</v>
       </c>
       <c r="C254" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>28-2</v>
+        <v>28-1</v>
       </c>
       <c r="D254" s="23"/>
       <c r="E254" s="23"/>
@@ -10453,24 +10480,27 @@
         <v>301</v>
       </c>
       <c r="I254" s="25" t="s">
-        <v>303</v>
-      </c>
-      <c r="J254" s="50" t="s">
-        <v>304</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="J254" s="23"/>
       <c r="K254" s="21"/>
-      <c r="L254" s="61"/>
+      <c r="L254" s="60" t="s">
+        <v>305</v>
+      </c>
       <c r="M254" s="6"/>
     </row>
-    <row r="255" spans="1:13" ht="15">
+    <row r="255" spans="1:13" ht="26.25">
       <c r="A255">
+        <f>A254</f>
         <v>28</v>
       </c>
       <c r="B255">
-        <v>3</v>
-      </c>
-      <c r="C255" s="53" t="s">
-        <v>342</v>
+        <f>IF(A255=A254,B254+1,1)</f>
+        <v>2</v>
+      </c>
+      <c r="C255" s="3" t="str">
+        <f t="shared" si="55"/>
+        <v>28-2</v>
       </c>
       <c r="D255" s="23"/>
       <c r="E255" s="23"/>
@@ -10480,22 +10510,24 @@
         <v>301</v>
       </c>
       <c r="I255" s="25" t="s">
-        <v>343</v>
-      </c>
-      <c r="J255" s="50"/>
+        <v>303</v>
+      </c>
+      <c r="J255" s="50" t="s">
+        <v>304</v>
+      </c>
       <c r="K255" s="21"/>
-      <c r="L255" s="52"/>
+      <c r="L255" s="61"/>
       <c r="M255" s="6"/>
     </row>
-    <row r="256" spans="1:13" ht="26.25">
+    <row r="256" spans="1:13" ht="15">
       <c r="A256">
         <v>28</v>
       </c>
       <c r="B256">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C256" s="53" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D256" s="23"/>
       <c r="E256" s="23"/>
@@ -10505,7 +10537,7 @@
         <v>301</v>
       </c>
       <c r="I256" s="25" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J256" s="50"/>
       <c r="K256" s="21"/>
@@ -10517,10 +10549,10 @@
         <v>28</v>
       </c>
       <c r="B257">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C257" s="53" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D257" s="23"/>
       <c r="E257" s="23"/>
@@ -10530,54 +10562,49 @@
         <v>301</v>
       </c>
       <c r="I257" s="25" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="J257" s="50"/>
       <c r="K257" s="21"/>
       <c r="L257" s="52"/>
       <c r="M257" s="6"/>
     </row>
-    <row r="258" spans="1:13" ht="39">
+    <row r="258" spans="1:13" ht="26.25">
       <c r="A258">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B258">
-        <f>IF(A258=A254,B254+1,1)</f>
-        <v>1</v>
-      </c>
-      <c r="C258" s="3" t="str">
-        <f t="shared" si="55"/>
-        <v>29-1</v>
+        <v>5</v>
+      </c>
+      <c r="C258" s="53" t="s">
+        <v>346</v>
       </c>
       <c r="D258" s="23"/>
       <c r="E258" s="23"/>
       <c r="F258" s="23"/>
       <c r="G258" s="23"/>
       <c r="H258" s="24" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="I258" s="25" t="s">
-        <v>308</v>
-      </c>
-      <c r="J258" s="23"/>
+        <v>347</v>
+      </c>
+      <c r="J258" s="50"/>
       <c r="K258" s="21"/>
-      <c r="L258" s="60" t="s">
-        <v>314</v>
-      </c>
+      <c r="L258" s="52"/>
       <c r="M258" s="6"/>
     </row>
     <row r="259" spans="1:13" ht="39">
       <c r="A259">
-        <f t="shared" si="56"/>
         <v>29</v>
       </c>
       <c r="B259">
-        <f t="shared" si="54"/>
-        <v>2</v>
+        <f>IF(A259=A255,B255+1,1)</f>
+        <v>1</v>
       </c>
       <c r="C259" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>29-2</v>
+        <v>29-1</v>
       </c>
       <c r="D259" s="23"/>
       <c r="E259" s="23"/>
@@ -10587,25 +10614,27 @@
         <v>307</v>
       </c>
       <c r="I259" s="25" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J259" s="23"/>
       <c r="K259" s="21"/>
-      <c r="L259" s="62"/>
+      <c r="L259" s="60" t="s">
+        <v>314</v>
+      </c>
       <c r="M259" s="6"/>
     </row>
-    <row r="260" spans="1:13" ht="26.25">
+    <row r="260" spans="1:13" ht="39">
       <c r="A260">
         <f t="shared" si="56"/>
         <v>29</v>
       </c>
       <c r="B260">
         <f t="shared" si="54"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C260" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>29-3</v>
+        <v>29-2</v>
       </c>
       <c r="D260" s="23"/>
       <c r="E260" s="23"/>
@@ -10615,25 +10644,25 @@
         <v>307</v>
       </c>
       <c r="I260" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J260" s="23"/>
       <c r="K260" s="21"/>
       <c r="L260" s="62"/>
       <c r="M260" s="6"/>
     </row>
-    <row r="261" spans="1:13" ht="26.25" customHeight="1">
+    <row r="261" spans="1:13" ht="26.25">
       <c r="A261">
         <f t="shared" si="56"/>
         <v>29</v>
       </c>
       <c r="B261">
         <f t="shared" si="54"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C261" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>29-4</v>
+        <v>29-3</v>
       </c>
       <c r="D261" s="23"/>
       <c r="E261" s="23"/>
@@ -10643,7 +10672,7 @@
         <v>307</v>
       </c>
       <c r="I261" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J261" s="23"/>
       <c r="K261" s="21"/>
@@ -10657,11 +10686,11 @@
       </c>
       <c r="B262">
         <f t="shared" si="54"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C262" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>29-5</v>
+        <v>29-4</v>
       </c>
       <c r="D262" s="23"/>
       <c r="E262" s="23"/>
@@ -10671,25 +10700,25 @@
         <v>307</v>
       </c>
       <c r="I262" s="25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J262" s="23"/>
       <c r="K262" s="21"/>
       <c r="L262" s="62"/>
       <c r="M262" s="6"/>
     </row>
-    <row r="263" spans="1:13" ht="39">
+    <row r="263" spans="1:13" ht="26.25" customHeight="1">
       <c r="A263">
         <f t="shared" si="56"/>
         <v>29</v>
       </c>
       <c r="B263">
         <f t="shared" si="54"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C263" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>29-6</v>
+        <v>29-5</v>
       </c>
       <c r="D263" s="23"/>
       <c r="E263" s="23"/>
@@ -10699,56 +10728,52 @@
         <v>307</v>
       </c>
       <c r="I263" s="25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J263" s="23"/>
       <c r="K263" s="21"/>
-      <c r="L263" s="61"/>
+      <c r="L263" s="62"/>
       <c r="M263" s="6"/>
     </row>
-    <row r="264" spans="1:13" ht="51.75">
+    <row r="264" spans="1:13" ht="39">
       <c r="A264">
-        <v>30</v>
+        <f t="shared" si="56"/>
+        <v>29</v>
       </c>
       <c r="B264">
         <f t="shared" si="54"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C264" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-1</v>
+        <v>29-6</v>
       </c>
       <c r="D264" s="23"/>
       <c r="E264" s="23"/>
-      <c r="F264" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="G264" s="23" t="s">
-        <v>176</v>
-      </c>
+      <c r="F264" s="23"/>
+      <c r="G264" s="23"/>
       <c r="H264" s="24" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="I264" s="25" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="J264" s="23"/>
       <c r="K264" s="21"/>
-      <c r="L264" s="26"/>
+      <c r="L264" s="61"/>
       <c r="M264" s="6"/>
     </row>
     <row r="265" spans="1:13" ht="51.75">
       <c r="A265">
-        <f t="shared" si="56"/>
         <v>30</v>
       </c>
       <c r="B265">
         <f t="shared" si="54"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C265" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>30-2</v>
+        <v>30-1</v>
       </c>
       <c r="D265" s="23"/>
       <c r="E265" s="23"/>
@@ -10762,24 +10787,25 @@
         <v>316</v>
       </c>
       <c r="I265" s="25" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="J265" s="23"/>
       <c r="K265" s="21"/>
       <c r="L265" s="26"/>
       <c r="M265" s="6"/>
     </row>
-    <row r="266" spans="1:13" ht="39">
+    <row r="266" spans="1:13" ht="51.75">
       <c r="A266">
-        <v>31</v>
+        <f t="shared" si="56"/>
+        <v>30</v>
       </c>
       <c r="B266">
-        <f t="shared" ref="B266" si="61">IF(A266=A265,B265+1,1)</f>
-        <v>1</v>
+        <f t="shared" si="54"/>
+        <v>2</v>
       </c>
       <c r="C266" s="3" t="str">
-        <f t="shared" ref="C266" si="62">CONCATENATE(A266,"-",B266)</f>
-        <v>31-1</v>
+        <f t="shared" si="55"/>
+        <v>30-2</v>
       </c>
       <c r="D266" s="23"/>
       <c r="E266" s="23"/>
@@ -10787,13 +10813,13 @@
         <v>241</v>
       </c>
       <c r="G266" s="23" t="s">
-        <v>241</v>
+        <v>176</v>
       </c>
       <c r="H266" s="24" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I266" s="25" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="J266" s="23"/>
       <c r="K266" s="21"/>
@@ -10802,16 +10828,15 @@
     </row>
     <row r="267" spans="1:13" ht="39">
       <c r="A267">
-        <f t="shared" si="56"/>
         <v>31</v>
       </c>
       <c r="B267">
-        <f t="shared" si="54"/>
-        <v>2</v>
+        <f t="shared" ref="B267" si="61">IF(A267=A266,B266+1,1)</f>
+        <v>1</v>
       </c>
       <c r="C267" s="3" t="str">
-        <f t="shared" si="55"/>
-        <v>31-2</v>
+        <f t="shared" ref="C267" si="62">CONCATENATE(A267,"-",B267)</f>
+        <v>31-1</v>
       </c>
       <c r="D267" s="23"/>
       <c r="E267" s="23"/>
@@ -10825,7 +10850,7 @@
         <v>322</v>
       </c>
       <c r="I267" s="25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J267" s="23"/>
       <c r="K267" s="21"/>
@@ -10839,11 +10864,11 @@
       </c>
       <c r="B268">
         <f t="shared" si="54"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C268" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-3</v>
+        <v>31-2</v>
       </c>
       <c r="D268" s="23"/>
       <c r="E268" s="23"/>
@@ -10857,24 +10882,25 @@
         <v>322</v>
       </c>
       <c r="I268" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J268" s="23"/>
       <c r="K268" s="21"/>
       <c r="L268" s="26"/>
       <c r="M268" s="6"/>
     </row>
-    <row r="269" spans="1:13" ht="90">
+    <row r="269" spans="1:13" ht="39">
       <c r="A269">
+        <f t="shared" si="56"/>
         <v>31</v>
       </c>
       <c r="B269">
         <f t="shared" si="54"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C269" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-4</v>
+        <v>31-3</v>
       </c>
       <c r="D269" s="23"/>
       <c r="E269" s="23"/>
@@ -10885,62 +10911,74 @@
         <v>241</v>
       </c>
       <c r="H269" s="24" t="s">
-        <v>355</v>
+        <v>322</v>
       </c>
       <c r="I269" s="25" t="s">
-        <v>356</v>
+        <v>325</v>
       </c>
       <c r="J269" s="23"/>
       <c r="K269" s="21"/>
-      <c r="L269" s="26" t="s">
-        <v>357</v>
-      </c>
+      <c r="L269" s="26"/>
       <c r="M269" s="6"/>
     </row>
-    <row r="270" spans="1:13" ht="26.25">
+    <row r="270" spans="1:13" ht="90">
       <c r="A270">
-        <f t="shared" si="56"/>
         <v>31</v>
       </c>
       <c r="B270">
         <f t="shared" si="54"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C270" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-5</v>
-      </c>
-      <c r="F270" s="54" t="s">
+        <v>31-4</v>
+      </c>
+      <c r="D270" s="23"/>
+      <c r="E270" s="23"/>
+      <c r="F270" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="G270" s="54" t="s">
+      <c r="G270" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="H270" s="55" t="s">
-        <v>322</v>
-      </c>
-      <c r="I270" s="56" t="s">
-        <v>358</v>
-      </c>
-      <c r="L270" s="6"/>
+      <c r="H270" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="I270" s="25" t="s">
+        <v>356</v>
+      </c>
+      <c r="J270" s="23"/>
+      <c r="K270" s="21"/>
+      <c r="L270" s="26" t="s">
+        <v>357</v>
+      </c>
       <c r="M270" s="6"/>
     </row>
-    <row r="271" spans="1:13" ht="15">
+    <row r="271" spans="1:13" ht="26.25">
       <c r="A271">
         <f t="shared" si="56"/>
         <v>31</v>
       </c>
       <c r="B271">
         <f t="shared" si="54"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C271" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-6</v>
-      </c>
-      <c r="F271" s="54"/>
-      <c r="G271" s="54"/>
-      <c r="H271" s="55"/>
+        <v>31-5</v>
+      </c>
+      <c r="F271" s="54" t="s">
+        <v>241</v>
+      </c>
+      <c r="G271" s="54" t="s">
+        <v>241</v>
+      </c>
+      <c r="H271" s="55" t="s">
+        <v>322</v>
+      </c>
+      <c r="I271" s="56" t="s">
+        <v>358</v>
+      </c>
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
     </row>
@@ -10951,12 +10989,15 @@
       </c>
       <c r="B272">
         <f t="shared" si="54"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C272" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-7</v>
-      </c>
+        <v>31-6</v>
+      </c>
+      <c r="F272" s="54"/>
+      <c r="G272" s="54"/>
+      <c r="H272" s="55"/>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
     </row>
@@ -10967,11 +11008,11 @@
       </c>
       <c r="B273">
         <f t="shared" si="54"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C273" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-8</v>
+        <v>31-7</v>
       </c>
       <c r="L273" s="6"/>
       <c r="M273" s="6"/>
@@ -10983,11 +11024,11 @@
       </c>
       <c r="B274">
         <f t="shared" si="54"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C274" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-9</v>
+        <v>31-8</v>
       </c>
       <c r="L274" s="6"/>
       <c r="M274" s="6"/>
@@ -10999,11 +11040,11 @@
       </c>
       <c r="B275">
         <f t="shared" si="54"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C275" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-10</v>
+        <v>31-9</v>
       </c>
       <c r="L275" s="6"/>
       <c r="M275" s="6"/>
@@ -11015,11 +11056,11 @@
       </c>
       <c r="B276">
         <f t="shared" si="54"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C276" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-11</v>
+        <v>31-10</v>
       </c>
       <c r="L276" s="6"/>
       <c r="M276" s="6"/>
@@ -11031,11 +11072,11 @@
       </c>
       <c r="B277">
         <f t="shared" si="54"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C277" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-12</v>
+        <v>31-11</v>
       </c>
       <c r="L277" s="6"/>
       <c r="M277" s="6"/>
@@ -11047,11 +11088,11 @@
       </c>
       <c r="B278">
         <f t="shared" si="54"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C278" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-13</v>
+        <v>31-12</v>
       </c>
       <c r="L278" s="6"/>
       <c r="M278" s="6"/>
@@ -11063,11 +11104,11 @@
       </c>
       <c r="B279">
         <f t="shared" si="54"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C279" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-14</v>
+        <v>31-13</v>
       </c>
       <c r="L279" s="6"/>
       <c r="M279" s="6"/>
@@ -11079,11 +11120,11 @@
       </c>
       <c r="B280">
         <f t="shared" si="54"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C280" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-15</v>
+        <v>31-14</v>
       </c>
       <c r="L280" s="6"/>
       <c r="M280" s="6"/>
@@ -11095,11 +11136,11 @@
       </c>
       <c r="B281">
         <f t="shared" si="54"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C281" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-16</v>
+        <v>31-15</v>
       </c>
       <c r="L281" s="6"/>
       <c r="M281" s="6"/>
@@ -11111,11 +11152,11 @@
       </c>
       <c r="B282">
         <f t="shared" si="54"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C282" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-17</v>
+        <v>31-16</v>
       </c>
       <c r="L282" s="6"/>
       <c r="M282" s="6"/>
@@ -11127,11 +11168,11 @@
       </c>
       <c r="B283">
         <f t="shared" si="54"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C283" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-18</v>
+        <v>31-17</v>
       </c>
       <c r="L283" s="6"/>
       <c r="M283" s="6"/>
@@ -11143,11 +11184,11 @@
       </c>
       <c r="B284">
         <f t="shared" si="54"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C284" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-19</v>
+        <v>31-18</v>
       </c>
       <c r="L284" s="6"/>
       <c r="M284" s="6"/>
@@ -11159,11 +11200,11 @@
       </c>
       <c r="B285">
         <f t="shared" si="54"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C285" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-20</v>
+        <v>31-19</v>
       </c>
       <c r="L285" s="6"/>
       <c r="M285" s="6"/>
@@ -11175,11 +11216,11 @@
       </c>
       <c r="B286">
         <f t="shared" si="54"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C286" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-21</v>
+        <v>31-20</v>
       </c>
       <c r="L286" s="6"/>
       <c r="M286" s="6"/>
@@ -11191,11 +11232,11 @@
       </c>
       <c r="B287">
         <f t="shared" si="54"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C287" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-22</v>
+        <v>31-21</v>
       </c>
       <c r="L287" s="6"/>
       <c r="M287" s="6"/>
@@ -11207,11 +11248,11 @@
       </c>
       <c r="B288">
         <f t="shared" si="54"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C288" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-23</v>
+        <v>31-22</v>
       </c>
       <c r="L288" s="6"/>
       <c r="M288" s="6"/>
@@ -11223,11 +11264,11 @@
       </c>
       <c r="B289">
         <f t="shared" si="54"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C289" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-24</v>
+        <v>31-23</v>
       </c>
       <c r="L289" s="6"/>
       <c r="M289" s="6"/>
@@ -11239,11 +11280,11 @@
       </c>
       <c r="B290">
         <f t="shared" si="54"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C290" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-25</v>
+        <v>31-24</v>
       </c>
       <c r="L290" s="6"/>
       <c r="M290" s="6"/>
@@ -11255,11 +11296,11 @@
       </c>
       <c r="B291">
         <f t="shared" si="54"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C291" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-26</v>
+        <v>31-25</v>
       </c>
       <c r="L291" s="6"/>
       <c r="M291" s="6"/>
@@ -11271,11 +11312,11 @@
       </c>
       <c r="B292">
         <f t="shared" si="54"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C292" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-27</v>
+        <v>31-26</v>
       </c>
       <c r="L292" s="6"/>
       <c r="M292" s="6"/>
@@ -11287,11 +11328,11 @@
       </c>
       <c r="B293">
         <f t="shared" si="54"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C293" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-28</v>
+        <v>31-27</v>
       </c>
       <c r="L293" s="6"/>
       <c r="M293" s="6"/>
@@ -11303,11 +11344,11 @@
       </c>
       <c r="B294">
         <f t="shared" si="54"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C294" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-29</v>
+        <v>31-28</v>
       </c>
       <c r="L294" s="6"/>
       <c r="M294" s="6"/>
@@ -11319,11 +11360,11 @@
       </c>
       <c r="B295">
         <f t="shared" si="54"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C295" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-30</v>
+        <v>31-29</v>
       </c>
       <c r="L295" s="6"/>
       <c r="M295" s="6"/>
@@ -11335,11 +11376,11 @@
       </c>
       <c r="B296">
         <f t="shared" si="54"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C296" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-31</v>
+        <v>31-30</v>
       </c>
       <c r="L296" s="6"/>
       <c r="M296" s="6"/>
@@ -11351,11 +11392,11 @@
       </c>
       <c r="B297">
         <f t="shared" si="54"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C297" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-32</v>
+        <v>31-31</v>
       </c>
       <c r="L297" s="6"/>
       <c r="M297" s="6"/>
@@ -11367,11 +11408,11 @@
       </c>
       <c r="B298">
         <f t="shared" si="54"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C298" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-33</v>
+        <v>31-32</v>
       </c>
       <c r="L298" s="6"/>
       <c r="M298" s="6"/>
@@ -11383,11 +11424,11 @@
       </c>
       <c r="B299">
         <f t="shared" si="54"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C299" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-34</v>
+        <v>31-33</v>
       </c>
       <c r="L299" s="6"/>
       <c r="M299" s="6"/>
@@ -11399,11 +11440,11 @@
       </c>
       <c r="B300">
         <f t="shared" si="54"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C300" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-35</v>
+        <v>31-34</v>
       </c>
       <c r="L300" s="6"/>
       <c r="M300" s="6"/>
@@ -11415,11 +11456,11 @@
       </c>
       <c r="B301">
         <f t="shared" si="54"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C301" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-36</v>
+        <v>31-35</v>
       </c>
       <c r="L301" s="6"/>
       <c r="M301" s="6"/>
@@ -11431,11 +11472,11 @@
       </c>
       <c r="B302">
         <f t="shared" si="54"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C302" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-37</v>
+        <v>31-36</v>
       </c>
       <c r="L302" s="6"/>
       <c r="M302" s="6"/>
@@ -11447,11 +11488,11 @@
       </c>
       <c r="B303">
         <f t="shared" si="54"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C303" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-38</v>
+        <v>31-37</v>
       </c>
       <c r="L303" s="6"/>
       <c r="M303" s="6"/>
@@ -11463,11 +11504,11 @@
       </c>
       <c r="B304">
         <f t="shared" si="54"/>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C304" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-39</v>
+        <v>31-38</v>
       </c>
       <c r="L304" s="6"/>
       <c r="M304" s="6"/>
@@ -11479,11 +11520,11 @@
       </c>
       <c r="B305">
         <f t="shared" si="54"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C305" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-40</v>
+        <v>31-39</v>
       </c>
       <c r="L305" s="6"/>
       <c r="M305" s="6"/>
@@ -11495,11 +11536,11 @@
       </c>
       <c r="B306">
         <f t="shared" si="54"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C306" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-41</v>
+        <v>31-40</v>
       </c>
       <c r="L306" s="6"/>
       <c r="M306" s="6"/>
@@ -11511,11 +11552,11 @@
       </c>
       <c r="B307">
         <f t="shared" si="54"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C307" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-42</v>
+        <v>31-41</v>
       </c>
       <c r="L307" s="6"/>
       <c r="M307" s="6"/>
@@ -11527,11 +11568,11 @@
       </c>
       <c r="B308">
         <f t="shared" si="54"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C308" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-43</v>
+        <v>31-42</v>
       </c>
       <c r="L308" s="6"/>
       <c r="M308" s="6"/>
@@ -11543,11 +11584,11 @@
       </c>
       <c r="B309">
         <f t="shared" si="54"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C309" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-44</v>
+        <v>31-43</v>
       </c>
       <c r="L309" s="6"/>
       <c r="M309" s="6"/>
@@ -11559,11 +11600,11 @@
       </c>
       <c r="B310">
         <f t="shared" si="54"/>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C310" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-45</v>
+        <v>31-44</v>
       </c>
       <c r="L310" s="6"/>
       <c r="M310" s="6"/>
@@ -11575,11 +11616,11 @@
       </c>
       <c r="B311">
         <f t="shared" si="54"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C311" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-46</v>
+        <v>31-45</v>
       </c>
       <c r="L311" s="6"/>
       <c r="M311" s="6"/>
@@ -11591,11 +11632,11 @@
       </c>
       <c r="B312">
         <f t="shared" si="54"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C312" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-47</v>
+        <v>31-46</v>
       </c>
       <c r="L312" s="6"/>
       <c r="M312" s="6"/>
@@ -11607,11 +11648,11 @@
       </c>
       <c r="B313">
         <f t="shared" si="54"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C313" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-48</v>
+        <v>31-47</v>
       </c>
       <c r="L313" s="6"/>
       <c r="M313" s="6"/>
@@ -11623,11 +11664,11 @@
       </c>
       <c r="B314">
         <f t="shared" si="54"/>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C314" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-49</v>
+        <v>31-48</v>
       </c>
       <c r="L314" s="6"/>
       <c r="M314" s="6"/>
@@ -11639,11 +11680,11 @@
       </c>
       <c r="B315">
         <f t="shared" si="54"/>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C315" s="3" t="str">
         <f t="shared" si="55"/>
-        <v>31-50</v>
+        <v>31-49</v>
       </c>
       <c r="L315" s="6"/>
       <c r="M315" s="6"/>
@@ -11654,44 +11695,44 @@
         <v>31</v>
       </c>
       <c r="B316">
-        <f t="shared" ref="B316:B379" si="63">IF(A316=A315,B315+1,1)</f>
-        <v>51</v>
+        <f t="shared" si="54"/>
+        <v>50</v>
       </c>
       <c r="C316" s="3" t="str">
-        <f t="shared" ref="C316:C379" si="64">CONCATENATE(A316,"-",B316)</f>
-        <v>31-51</v>
+        <f t="shared" si="55"/>
+        <v>31-50</v>
       </c>
       <c r="L316" s="6"/>
       <c r="M316" s="6"/>
     </row>
     <row r="317" spans="1:13" ht="15">
       <c r="A317">
-        <f t="shared" ref="A317:A380" si="65">A316</f>
+        <f t="shared" si="56"/>
         <v>31</v>
       </c>
       <c r="B317">
+        <f t="shared" ref="B317:B380" si="63">IF(A317=A316,B316+1,1)</f>
+        <v>51</v>
+      </c>
+      <c r="C317" s="3" t="str">
+        <f t="shared" ref="C317:C380" si="64">CONCATENATE(A317,"-",B317)</f>
+        <v>31-51</v>
+      </c>
+      <c r="L317" s="6"/>
+      <c r="M317" s="6"/>
+    </row>
+    <row r="318" spans="1:13" ht="15">
+      <c r="A318">
+        <f t="shared" ref="A318:A381" si="65">A317</f>
+        <v>31</v>
+      </c>
+      <c r="B318">
         <f t="shared" si="63"/>
         <v>52</v>
       </c>
-      <c r="C317" s="3" t="str">
+      <c r="C318" s="3" t="str">
         <f t="shared" si="64"/>
         <v>31-52</v>
-      </c>
-      <c r="L317" s="6"/>
-      <c r="M317" s="6"/>
-    </row>
-    <row r="318" spans="1:13" ht="15">
-      <c r="A318">
-        <f t="shared" si="65"/>
-        <v>31</v>
-      </c>
-      <c r="B318">
-        <f t="shared" si="63"/>
-        <v>53</v>
-      </c>
-      <c r="C318" s="3" t="str">
-        <f t="shared" si="64"/>
-        <v>31-53</v>
       </c>
       <c r="L318" s="6"/>
       <c r="M318" s="6"/>
@@ -11703,11 +11744,11 @@
       </c>
       <c r="B319">
         <f t="shared" si="63"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C319" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-54</v>
+        <v>31-53</v>
       </c>
       <c r="L319" s="6"/>
       <c r="M319" s="6"/>
@@ -11719,11 +11760,11 @@
       </c>
       <c r="B320">
         <f t="shared" si="63"/>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C320" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-55</v>
+        <v>31-54</v>
       </c>
       <c r="L320" s="6"/>
       <c r="M320" s="6"/>
@@ -11735,11 +11776,11 @@
       </c>
       <c r="B321">
         <f t="shared" si="63"/>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C321" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-56</v>
+        <v>31-55</v>
       </c>
       <c r="L321" s="6"/>
       <c r="M321" s="6"/>
@@ -11751,11 +11792,11 @@
       </c>
       <c r="B322">
         <f t="shared" si="63"/>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C322" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-57</v>
+        <v>31-56</v>
       </c>
       <c r="L322" s="6"/>
       <c r="M322" s="6"/>
@@ -11767,11 +11808,11 @@
       </c>
       <c r="B323">
         <f t="shared" si="63"/>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C323" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-58</v>
+        <v>31-57</v>
       </c>
       <c r="L323" s="6"/>
       <c r="M323" s="6"/>
@@ -11783,11 +11824,11 @@
       </c>
       <c r="B324">
         <f t="shared" si="63"/>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C324" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-59</v>
+        <v>31-58</v>
       </c>
       <c r="L324" s="6"/>
       <c r="M324" s="6"/>
@@ -11799,11 +11840,11 @@
       </c>
       <c r="B325">
         <f t="shared" si="63"/>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C325" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-60</v>
+        <v>31-59</v>
       </c>
       <c r="L325" s="6"/>
       <c r="M325" s="6"/>
@@ -11815,11 +11856,11 @@
       </c>
       <c r="B326">
         <f t="shared" si="63"/>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C326" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-61</v>
+        <v>31-60</v>
       </c>
       <c r="L326" s="6"/>
       <c r="M326" s="6"/>
@@ -11831,11 +11872,11 @@
       </c>
       <c r="B327">
         <f t="shared" si="63"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C327" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-62</v>
+        <v>31-61</v>
       </c>
       <c r="L327" s="6"/>
       <c r="M327" s="6"/>
@@ -11847,11 +11888,11 @@
       </c>
       <c r="B328">
         <f t="shared" si="63"/>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C328" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-63</v>
+        <v>31-62</v>
       </c>
       <c r="L328" s="6"/>
       <c r="M328" s="6"/>
@@ -11863,11 +11904,11 @@
       </c>
       <c r="B329">
         <f t="shared" si="63"/>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C329" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-64</v>
+        <v>31-63</v>
       </c>
       <c r="L329" s="6"/>
       <c r="M329" s="6"/>
@@ -11879,11 +11920,11 @@
       </c>
       <c r="B330">
         <f t="shared" si="63"/>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C330" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-65</v>
+        <v>31-64</v>
       </c>
       <c r="L330" s="6"/>
       <c r="M330" s="6"/>
@@ -11895,11 +11936,11 @@
       </c>
       <c r="B331">
         <f t="shared" si="63"/>
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C331" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-66</v>
+        <v>31-65</v>
       </c>
       <c r="L331" s="6"/>
       <c r="M331" s="6"/>
@@ -11911,11 +11952,11 @@
       </c>
       <c r="B332">
         <f t="shared" si="63"/>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C332" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-67</v>
+        <v>31-66</v>
       </c>
       <c r="L332" s="6"/>
       <c r="M332" s="6"/>
@@ -11927,11 +11968,11 @@
       </c>
       <c r="B333">
         <f t="shared" si="63"/>
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C333" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-68</v>
+        <v>31-67</v>
       </c>
       <c r="L333" s="6"/>
       <c r="M333" s="6"/>
@@ -11943,11 +11984,11 @@
       </c>
       <c r="B334">
         <f t="shared" si="63"/>
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C334" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-69</v>
+        <v>31-68</v>
       </c>
       <c r="L334" s="6"/>
       <c r="M334" s="6"/>
@@ -11959,11 +12000,11 @@
       </c>
       <c r="B335">
         <f t="shared" si="63"/>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C335" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-70</v>
+        <v>31-69</v>
       </c>
       <c r="L335" s="6"/>
       <c r="M335" s="6"/>
@@ -11975,11 +12016,11 @@
       </c>
       <c r="B336">
         <f t="shared" si="63"/>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C336" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-71</v>
+        <v>31-70</v>
       </c>
       <c r="L336" s="6"/>
       <c r="M336" s="6"/>
@@ -11991,11 +12032,11 @@
       </c>
       <c r="B337">
         <f t="shared" si="63"/>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C337" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-72</v>
+        <v>31-71</v>
       </c>
       <c r="L337" s="6"/>
       <c r="M337" s="6"/>
@@ -12007,11 +12048,11 @@
       </c>
       <c r="B338">
         <f t="shared" si="63"/>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C338" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-73</v>
+        <v>31-72</v>
       </c>
       <c r="L338" s="6"/>
       <c r="M338" s="6"/>
@@ -12023,11 +12064,11 @@
       </c>
       <c r="B339">
         <f t="shared" si="63"/>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C339" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-74</v>
+        <v>31-73</v>
       </c>
       <c r="L339" s="6"/>
       <c r="M339" s="6"/>
@@ -12039,11 +12080,11 @@
       </c>
       <c r="B340">
         <f t="shared" si="63"/>
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C340" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-75</v>
+        <v>31-74</v>
       </c>
       <c r="L340" s="6"/>
       <c r="M340" s="6"/>
@@ -12055,11 +12096,11 @@
       </c>
       <c r="B341">
         <f t="shared" si="63"/>
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C341" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-76</v>
+        <v>31-75</v>
       </c>
       <c r="L341" s="6"/>
       <c r="M341" s="6"/>
@@ -12071,11 +12112,11 @@
       </c>
       <c r="B342">
         <f t="shared" si="63"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C342" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-77</v>
+        <v>31-76</v>
       </c>
       <c r="L342" s="6"/>
       <c r="M342" s="6"/>
@@ -12087,11 +12128,11 @@
       </c>
       <c r="B343">
         <f t="shared" si="63"/>
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C343" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-78</v>
+        <v>31-77</v>
       </c>
       <c r="L343" s="6"/>
       <c r="M343" s="6"/>
@@ -12103,11 +12144,11 @@
       </c>
       <c r="B344">
         <f t="shared" si="63"/>
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C344" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-79</v>
+        <v>31-78</v>
       </c>
       <c r="L344" s="6"/>
       <c r="M344" s="6"/>
@@ -12119,11 +12160,11 @@
       </c>
       <c r="B345">
         <f t="shared" si="63"/>
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C345" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-80</v>
+        <v>31-79</v>
       </c>
       <c r="L345" s="6"/>
       <c r="M345" s="6"/>
@@ -12135,11 +12176,11 @@
       </c>
       <c r="B346">
         <f t="shared" si="63"/>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C346" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-81</v>
+        <v>31-80</v>
       </c>
       <c r="L346" s="6"/>
       <c r="M346" s="6"/>
@@ -12151,11 +12192,11 @@
       </c>
       <c r="B347">
         <f t="shared" si="63"/>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C347" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-82</v>
+        <v>31-81</v>
       </c>
       <c r="L347" s="6"/>
       <c r="M347" s="6"/>
@@ -12167,11 +12208,11 @@
       </c>
       <c r="B348">
         <f t="shared" si="63"/>
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C348" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-83</v>
+        <v>31-82</v>
       </c>
       <c r="L348" s="6"/>
       <c r="M348" s="6"/>
@@ -12183,11 +12224,11 @@
       </c>
       <c r="B349">
         <f t="shared" si="63"/>
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C349" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-84</v>
+        <v>31-83</v>
       </c>
       <c r="L349" s="6"/>
       <c r="M349" s="6"/>
@@ -12199,11 +12240,11 @@
       </c>
       <c r="B350">
         <f t="shared" si="63"/>
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C350" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-85</v>
+        <v>31-84</v>
       </c>
       <c r="L350" s="6"/>
       <c r="M350" s="6"/>
@@ -12215,11 +12256,11 @@
       </c>
       <c r="B351">
         <f t="shared" si="63"/>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C351" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-86</v>
+        <v>31-85</v>
       </c>
       <c r="L351" s="6"/>
       <c r="M351" s="6"/>
@@ -12231,11 +12272,11 @@
       </c>
       <c r="B352">
         <f t="shared" si="63"/>
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C352" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-87</v>
+        <v>31-86</v>
       </c>
       <c r="L352" s="6"/>
       <c r="M352" s="6"/>
@@ -12247,11 +12288,11 @@
       </c>
       <c r="B353">
         <f t="shared" si="63"/>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C353" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-88</v>
+        <v>31-87</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
@@ -12263,11 +12304,11 @@
       </c>
       <c r="B354">
         <f t="shared" si="63"/>
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C354" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-89</v>
+        <v>31-88</v>
       </c>
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
@@ -12279,11 +12320,11 @@
       </c>
       <c r="B355">
         <f t="shared" si="63"/>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C355" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-90</v>
+        <v>31-89</v>
       </c>
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
@@ -12295,11 +12336,11 @@
       </c>
       <c r="B356">
         <f t="shared" si="63"/>
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C356" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-91</v>
+        <v>31-90</v>
       </c>
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
@@ -12311,11 +12352,11 @@
       </c>
       <c r="B357">
         <f t="shared" si="63"/>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C357" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-92</v>
+        <v>31-91</v>
       </c>
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
@@ -12327,11 +12368,11 @@
       </c>
       <c r="B358">
         <f t="shared" si="63"/>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C358" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-93</v>
+        <v>31-92</v>
       </c>
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
@@ -12343,11 +12384,11 @@
       </c>
       <c r="B359">
         <f t="shared" si="63"/>
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C359" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-94</v>
+        <v>31-93</v>
       </c>
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
@@ -12359,11 +12400,11 @@
       </c>
       <c r="B360">
         <f t="shared" si="63"/>
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C360" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-95</v>
+        <v>31-94</v>
       </c>
       <c r="L360" s="6"/>
       <c r="M360" s="6"/>
@@ -12375,11 +12416,11 @@
       </c>
       <c r="B361">
         <f t="shared" si="63"/>
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C361" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-96</v>
+        <v>31-95</v>
       </c>
       <c r="L361" s="6"/>
       <c r="M361" s="6"/>
@@ -12391,11 +12432,11 @@
       </c>
       <c r="B362">
         <f t="shared" si="63"/>
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C362" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-97</v>
+        <v>31-96</v>
       </c>
       <c r="L362" s="6"/>
       <c r="M362" s="6"/>
@@ -12407,11 +12448,11 @@
       </c>
       <c r="B363">
         <f t="shared" si="63"/>
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C363" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-98</v>
+        <v>31-97</v>
       </c>
       <c r="L363" s="6"/>
       <c r="M363" s="6"/>
@@ -12423,11 +12464,11 @@
       </c>
       <c r="B364">
         <f t="shared" si="63"/>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C364" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-99</v>
+        <v>31-98</v>
       </c>
       <c r="L364" s="6"/>
       <c r="M364" s="6"/>
@@ -12439,11 +12480,11 @@
       </c>
       <c r="B365">
         <f t="shared" si="63"/>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C365" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-100</v>
+        <v>31-99</v>
       </c>
       <c r="L365" s="6"/>
       <c r="M365" s="6"/>
@@ -12455,11 +12496,11 @@
       </c>
       <c r="B366">
         <f t="shared" si="63"/>
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C366" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-101</v>
+        <v>31-100</v>
       </c>
       <c r="L366" s="6"/>
       <c r="M366" s="6"/>
@@ -12471,11 +12512,11 @@
       </c>
       <c r="B367">
         <f t="shared" si="63"/>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C367" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-102</v>
+        <v>31-101</v>
       </c>
       <c r="L367" s="6"/>
       <c r="M367" s="6"/>
@@ -12487,11 +12528,11 @@
       </c>
       <c r="B368">
         <f t="shared" si="63"/>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C368" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-103</v>
+        <v>31-102</v>
       </c>
       <c r="L368" s="6"/>
       <c r="M368" s="6"/>
@@ -12503,11 +12544,11 @@
       </c>
       <c r="B369">
         <f t="shared" si="63"/>
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C369" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-104</v>
+        <v>31-103</v>
       </c>
       <c r="L369" s="6"/>
       <c r="M369" s="6"/>
@@ -12519,11 +12560,11 @@
       </c>
       <c r="B370">
         <f t="shared" si="63"/>
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C370" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-105</v>
+        <v>31-104</v>
       </c>
       <c r="L370" s="6"/>
       <c r="M370" s="6"/>
@@ -12535,11 +12576,11 @@
       </c>
       <c r="B371">
         <f t="shared" si="63"/>
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C371" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-106</v>
+        <v>31-105</v>
       </c>
       <c r="L371" s="6"/>
       <c r="M371" s="6"/>
@@ -12551,11 +12592,11 @@
       </c>
       <c r="B372">
         <f t="shared" si="63"/>
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C372" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-107</v>
+        <v>31-106</v>
       </c>
       <c r="L372" s="6"/>
       <c r="M372" s="6"/>
@@ -12567,11 +12608,11 @@
       </c>
       <c r="B373">
         <f t="shared" si="63"/>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C373" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-108</v>
+        <v>31-107</v>
       </c>
       <c r="L373" s="6"/>
       <c r="M373" s="6"/>
@@ -12583,11 +12624,11 @@
       </c>
       <c r="B374">
         <f t="shared" si="63"/>
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C374" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-109</v>
+        <v>31-108</v>
       </c>
       <c r="L374" s="6"/>
       <c r="M374" s="6"/>
@@ -12599,11 +12640,11 @@
       </c>
       <c r="B375">
         <f t="shared" si="63"/>
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C375" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-110</v>
+        <v>31-109</v>
       </c>
       <c r="L375" s="6"/>
       <c r="M375" s="6"/>
@@ -12615,11 +12656,11 @@
       </c>
       <c r="B376">
         <f t="shared" si="63"/>
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C376" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-111</v>
+        <v>31-110</v>
       </c>
       <c r="L376" s="6"/>
       <c r="M376" s="6"/>
@@ -12631,11 +12672,11 @@
       </c>
       <c r="B377">
         <f t="shared" si="63"/>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C377" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-112</v>
+        <v>31-111</v>
       </c>
       <c r="L377" s="6"/>
       <c r="M377" s="6"/>
@@ -12647,11 +12688,11 @@
       </c>
       <c r="B378">
         <f t="shared" si="63"/>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C378" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-113</v>
+        <v>31-112</v>
       </c>
       <c r="L378" s="6"/>
       <c r="M378" s="6"/>
@@ -12663,11 +12704,11 @@
       </c>
       <c r="B379">
         <f t="shared" si="63"/>
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C379" s="3" t="str">
         <f t="shared" si="64"/>
-        <v>31-114</v>
+        <v>31-113</v>
       </c>
       <c r="L379" s="6"/>
       <c r="M379" s="6"/>
@@ -12678,44 +12719,44 @@
         <v>31</v>
       </c>
       <c r="B380">
-        <f t="shared" ref="B380:B401" si="66">IF(A380=A379,B379+1,1)</f>
-        <v>115</v>
+        <f t="shared" si="63"/>
+        <v>114</v>
       </c>
       <c r="C380" s="3" t="str">
-        <f t="shared" ref="C380:C401" si="67">CONCATENATE(A380,"-",B380)</f>
-        <v>31-115</v>
+        <f t="shared" si="64"/>
+        <v>31-114</v>
       </c>
       <c r="L380" s="6"/>
       <c r="M380" s="6"/>
     </row>
     <row r="381" spans="1:13" ht="15">
       <c r="A381">
-        <f t="shared" ref="A381:A401" si="68">A380</f>
+        <f t="shared" si="65"/>
         <v>31</v>
       </c>
       <c r="B381">
+        <f t="shared" ref="B381:B402" si="66">IF(A381=A380,B380+1,1)</f>
+        <v>115</v>
+      </c>
+      <c r="C381" s="3" t="str">
+        <f t="shared" ref="C381:C402" si="67">CONCATENATE(A381,"-",B381)</f>
+        <v>31-115</v>
+      </c>
+      <c r="L381" s="6"/>
+      <c r="M381" s="6"/>
+    </row>
+    <row r="382" spans="1:13" ht="15">
+      <c r="A382">
+        <f t="shared" ref="A382:A402" si="68">A381</f>
+        <v>31</v>
+      </c>
+      <c r="B382">
         <f t="shared" si="66"/>
         <v>116</v>
       </c>
-      <c r="C381" s="3" t="str">
+      <c r="C382" s="3" t="str">
         <f t="shared" si="67"/>
         <v>31-116</v>
-      </c>
-      <c r="L381" s="6"/>
-      <c r="M381" s="6"/>
-    </row>
-    <row r="382" spans="1:13" ht="15">
-      <c r="A382">
-        <f t="shared" si="68"/>
-        <v>31</v>
-      </c>
-      <c r="B382">
-        <f t="shared" si="66"/>
-        <v>117</v>
-      </c>
-      <c r="C382" s="3" t="str">
-        <f t="shared" si="67"/>
-        <v>31-117</v>
       </c>
       <c r="L382" s="6"/>
       <c r="M382" s="6"/>
@@ -12727,11 +12768,11 @@
       </c>
       <c r="B383">
         <f t="shared" si="66"/>
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C383" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-118</v>
+        <v>31-117</v>
       </c>
       <c r="L383" s="6"/>
       <c r="M383" s="6"/>
@@ -12743,11 +12784,11 @@
       </c>
       <c r="B384">
         <f t="shared" si="66"/>
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C384" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-119</v>
+        <v>31-118</v>
       </c>
       <c r="L384" s="6"/>
       <c r="M384" s="6"/>
@@ -12759,11 +12800,11 @@
       </c>
       <c r="B385">
         <f t="shared" si="66"/>
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C385" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-120</v>
+        <v>31-119</v>
       </c>
       <c r="L385" s="6"/>
       <c r="M385" s="6"/>
@@ -12775,11 +12816,11 @@
       </c>
       <c r="B386">
         <f t="shared" si="66"/>
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C386" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-121</v>
+        <v>31-120</v>
       </c>
       <c r="L386" s="6"/>
       <c r="M386" s="6"/>
@@ -12791,11 +12832,11 @@
       </c>
       <c r="B387">
         <f t="shared" si="66"/>
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C387" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-122</v>
+        <v>31-121</v>
       </c>
       <c r="L387" s="6"/>
       <c r="M387" s="6"/>
@@ -12807,11 +12848,11 @@
       </c>
       <c r="B388">
         <f t="shared" si="66"/>
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C388" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-123</v>
+        <v>31-122</v>
       </c>
       <c r="L388" s="6"/>
       <c r="M388" s="6"/>
@@ -12823,11 +12864,11 @@
       </c>
       <c r="B389">
         <f t="shared" si="66"/>
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C389" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-124</v>
+        <v>31-123</v>
       </c>
       <c r="L389" s="6"/>
       <c r="M389" s="6"/>
@@ -12839,11 +12880,11 @@
       </c>
       <c r="B390">
         <f t="shared" si="66"/>
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C390" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-125</v>
+        <v>31-124</v>
       </c>
       <c r="L390" s="6"/>
       <c r="M390" s="6"/>
@@ -12855,11 +12896,11 @@
       </c>
       <c r="B391">
         <f t="shared" si="66"/>
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C391" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-126</v>
+        <v>31-125</v>
       </c>
       <c r="L391" s="6"/>
       <c r="M391" s="6"/>
@@ -12871,11 +12912,11 @@
       </c>
       <c r="B392">
         <f t="shared" si="66"/>
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C392" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-127</v>
+        <v>31-126</v>
       </c>
       <c r="L392" s="6"/>
       <c r="M392" s="6"/>
@@ -12887,11 +12928,11 @@
       </c>
       <c r="B393">
         <f t="shared" si="66"/>
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C393" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-128</v>
+        <v>31-127</v>
       </c>
       <c r="L393" s="6"/>
       <c r="M393" s="6"/>
@@ -12903,11 +12944,11 @@
       </c>
       <c r="B394">
         <f t="shared" si="66"/>
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C394" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-129</v>
+        <v>31-128</v>
       </c>
       <c r="L394" s="6"/>
       <c r="M394" s="6"/>
@@ -12919,11 +12960,11 @@
       </c>
       <c r="B395">
         <f t="shared" si="66"/>
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C395" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-130</v>
+        <v>31-129</v>
       </c>
       <c r="L395" s="6"/>
       <c r="M395" s="6"/>
@@ -12935,11 +12976,11 @@
       </c>
       <c r="B396">
         <f t="shared" si="66"/>
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C396" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-131</v>
+        <v>31-130</v>
       </c>
       <c r="L396" s="6"/>
       <c r="M396" s="6"/>
@@ -12951,11 +12992,11 @@
       </c>
       <c r="B397">
         <f t="shared" si="66"/>
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C397" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-132</v>
+        <v>31-131</v>
       </c>
       <c r="L397" s="6"/>
       <c r="M397" s="6"/>
@@ -12967,11 +13008,11 @@
       </c>
       <c r="B398">
         <f t="shared" si="66"/>
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C398" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-133</v>
+        <v>31-132</v>
       </c>
       <c r="L398" s="6"/>
       <c r="M398" s="6"/>
@@ -12983,11 +13024,11 @@
       </c>
       <c r="B399">
         <f t="shared" si="66"/>
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C399" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-134</v>
+        <v>31-133</v>
       </c>
       <c r="L399" s="6"/>
       <c r="M399" s="6"/>
@@ -12999,11 +13040,11 @@
       </c>
       <c r="B400">
         <f t="shared" si="66"/>
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C400" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-135</v>
+        <v>31-134</v>
       </c>
       <c r="L400" s="6"/>
       <c r="M400" s="6"/>
@@ -13015,16 +13056,28 @@
       </c>
       <c r="B401">
         <f t="shared" si="66"/>
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C401" s="3" t="str">
         <f t="shared" si="67"/>
-        <v>31-136</v>
+        <v>31-135</v>
       </c>
       <c r="L401" s="6"/>
       <c r="M401" s="6"/>
     </row>
-    <row r="402" spans="1:13" ht="12.75">
+    <row r="402" spans="1:13" ht="15">
+      <c r="A402">
+        <f t="shared" si="68"/>
+        <v>31</v>
+      </c>
+      <c r="B402">
+        <f t="shared" si="66"/>
+        <v>136</v>
+      </c>
+      <c r="C402" s="3" t="str">
+        <f t="shared" si="67"/>
+        <v>31-136</v>
+      </c>
       <c r="L402" s="6"/>
       <c r="M402" s="6"/>
     </row>
@@ -15772,11 +15825,15 @@
       <c r="L1088" s="6"/>
       <c r="M1088" s="6"/>
     </row>
+    <row r="1089" spans="12:13" ht="12.75">
+      <c r="L1089" s="6"/>
+      <c r="M1089" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="L200:L203"/>
-    <mergeCell ref="L253:L254"/>
-    <mergeCell ref="L258:L263"/>
+    <mergeCell ref="L254:L255"/>
+    <mergeCell ref="L259:L264"/>
   </mergeCells>
   <conditionalFormatting sqref="K167:K211 K100:K159 K2:K98">
     <cfRule type="containsBlanks" dxfId="92" priority="97">
@@ -15883,7 +15940,7 @@
       <formula>LEN(TRIM(K226))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K228 K245:K246 K233:K243">
+  <conditionalFormatting sqref="K228 K246:K247 K234:K244">
     <cfRule type="containsBlanks" dxfId="71" priority="61">
       <formula>LEN(TRIM(K228))=0</formula>
     </cfRule>
@@ -15978,12 +16035,12 @@
       <formula>NOT(ISERROR(SEARCH(("fail"),(K226))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K228 K245:K246 K233:K243">
+  <conditionalFormatting sqref="K228 K246:K247 K234:K244">
     <cfRule type="containsText" dxfId="52" priority="62" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K228))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K228 K245:K246 K233:K243">
+  <conditionalFormatting sqref="K228 K246:K247 K234:K244">
     <cfRule type="containsText" dxfId="51" priority="63" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K228))))</formula>
     </cfRule>
@@ -16048,19 +16105,19 @@
       <formula>NOT(ISERROR(SEARCH(("fail"),(K227))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K244">
+  <conditionalFormatting sqref="K245">
     <cfRule type="containsBlanks" dxfId="38" priority="37">
-      <formula>LEN(TRIM(K244))=0</formula>
+      <formula>LEN(TRIM(K245))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K244">
+  <conditionalFormatting sqref="K245">
     <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K244))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K245))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K244">
+  <conditionalFormatting sqref="K245">
     <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K244))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K245))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K229">
@@ -16078,79 +16135,79 @@
       <formula>NOT(ISERROR(SEARCH(("fail"),(K229))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K230:K232">
+  <conditionalFormatting sqref="K230:K233">
     <cfRule type="containsBlanks" dxfId="32" priority="31">
       <formula>LEN(TRIM(K230))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K230:K232">
+  <conditionalFormatting sqref="K230:K233">
     <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K230))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K230:K232">
+  <conditionalFormatting sqref="K230:K233">
     <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K230))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K247">
+  <conditionalFormatting sqref="K248">
     <cfRule type="containsBlanks" dxfId="29" priority="28">
-      <formula>LEN(TRIM(K247))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K247">
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K247))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K247">
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K247))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K248:K252">
-    <cfRule type="containsBlanks" dxfId="26" priority="25">
       <formula>LEN(TRIM(K248))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K248:K252">
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K248">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K248))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K248:K252">
-    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="fail">
+  <conditionalFormatting sqref="K248">
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K248))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K253">
-    <cfRule type="containsBlanks" dxfId="23" priority="22">
-      <formula>LEN(TRIM(K253))=0</formula>
+  <conditionalFormatting sqref="K249:K253">
+    <cfRule type="containsBlanks" dxfId="26" priority="25">
+      <formula>LEN(TRIM(K249))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K253">
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K253))))</formula>
+  <conditionalFormatting sqref="K249:K253">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K249))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K253">
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K253))))</formula>
+  <conditionalFormatting sqref="K249:K253">
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K249))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K254:K257">
-    <cfRule type="containsBlanks" dxfId="20" priority="19">
+  <conditionalFormatting sqref="K254">
+    <cfRule type="containsBlanks" dxfId="23" priority="22">
       <formula>LEN(TRIM(K254))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K254:K257">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K254">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K254))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K254:K257">
+  <conditionalFormatting sqref="K254">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K254))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K255:K258">
+    <cfRule type="containsBlanks" dxfId="20" priority="19">
+      <formula>LEN(TRIM(K255))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K255:K258">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K255))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K255:K258">
     <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K254))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K255))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K160:K166">
@@ -16168,64 +16225,64 @@
       <formula>NOT(ISERROR(SEARCH(("fail"),(K160))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K258:K259">
+  <conditionalFormatting sqref="K259:K260">
     <cfRule type="containsBlanks" dxfId="14" priority="13">
-      <formula>LEN(TRIM(K258))=0</formula>
+      <formula>LEN(TRIM(K259))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K258:K259">
+  <conditionalFormatting sqref="K259:K260">
     <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K258))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K259))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K258:K259">
+  <conditionalFormatting sqref="K259:K260">
     <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K258))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K259))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K260">
+  <conditionalFormatting sqref="K261">
     <cfRule type="containsBlanks" dxfId="11" priority="10">
-      <formula>LEN(TRIM(K260))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K260">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K260))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K260">
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K260))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K261:K263">
-    <cfRule type="containsBlanks" dxfId="8" priority="7">
       <formula>LEN(TRIM(K261))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K261:K263">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K261">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K261))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K261:K263">
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
+  <conditionalFormatting sqref="K261">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K261))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K264:K269">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
-      <formula>LEN(TRIM(K264))=0</formula>
+  <conditionalFormatting sqref="K262:K264">
+    <cfRule type="containsBlanks" dxfId="8" priority="7">
+      <formula>LEN(TRIM(K262))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K264:K269">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K264))))</formula>
+  <conditionalFormatting sqref="K262:K264">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K262))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K264:K269">
+  <conditionalFormatting sqref="K262:K264">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K262))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K265:K270">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
+      <formula>LEN(TRIM(K265))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K265:K270">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K265))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K265:K270">
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K264))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K265))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K99">

</xml_diff>

<commit_message>
Add run diagnostics test
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="367">
   <si>
     <t>Test Number</t>
   </si>
@@ -1129,6 +1129,15 @@
   </si>
   <si>
     <t>Create a group containing ONLY hidden blocks. Verify that the group is NOT shown, except when the right-click option "Shown hidden blocks" is selected</t>
+  </si>
+  <si>
+    <t>32-1</t>
+  </si>
+  <si>
+    <t>Rin diagnostics</t>
+  </si>
+  <si>
+    <t>Start a run in simulation mode, check that spectra 2,4 and 6 are counting on the run diagnostics page</t>
   </si>
 </sst>
 </file>
@@ -1505,6 +1514,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1519,20 +1542,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3140,8 +3149,8 @@
   <dimension ref="A1:N1089"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A225" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G235" sqref="G235"/>
+      <pane ySplit="1" topLeftCell="A264" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I276" sqref="I276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -8886,7 +8895,7 @@
       </c>
       <c r="J200" s="8"/>
       <c r="K200" s="7"/>
-      <c r="L200" s="57"/>
+      <c r="L200" s="65"/>
     </row>
     <row r="201" spans="1:13" ht="30">
       <c r="A201">
@@ -8915,7 +8924,7 @@
       </c>
       <c r="J201" s="8"/>
       <c r="K201" s="7"/>
-      <c r="L201" s="58"/>
+      <c r="L201" s="66"/>
       <c r="M201" s="6"/>
     </row>
     <row r="202" spans="1:13" ht="45">
@@ -8945,7 +8954,7 @@
       </c>
       <c r="J202" s="8"/>
       <c r="K202" s="7"/>
-      <c r="L202" s="58"/>
+      <c r="L202" s="66"/>
       <c r="M202" s="6"/>
     </row>
     <row r="203" spans="1:13" ht="30">
@@ -8975,7 +8984,7 @@
       </c>
       <c r="J203" s="8"/>
       <c r="K203" s="7"/>
-      <c r="L203" s="59"/>
+      <c r="L203" s="67"/>
       <c r="M203" s="6"/>
     </row>
     <row r="204" spans="1:13" ht="30">
@@ -9875,20 +9884,20 @@
       <c r="C233" s="22" t="s">
         <v>361</v>
       </c>
-      <c r="D233" s="69">
+      <c r="D233" s="63">
         <v>1672</v>
       </c>
-      <c r="E233" s="69"/>
-      <c r="F233" s="69"/>
-      <c r="G233" s="70"/>
-      <c r="H233" s="70" t="s">
+      <c r="E233" s="63"/>
+      <c r="F233" s="63"/>
+      <c r="G233" s="64"/>
+      <c r="H233" s="64" t="s">
         <v>362</v>
       </c>
       <c r="I233" s="26" t="s">
         <v>363</v>
       </c>
       <c r="J233" s="26"/>
-      <c r="K233" s="70"/>
+      <c r="K233" s="64"/>
       <c r="L233" s="26"/>
       <c r="M233" s="26"/>
     </row>
@@ -9899,23 +9908,23 @@
       <c r="B234">
         <v>1</v>
       </c>
-      <c r="C234" s="63" t="str">
+      <c r="C234" s="57" t="str">
         <f>CONCATENATE(A234,"-",B234)</f>
         <v>22-1</v>
       </c>
-      <c r="D234" s="64"/>
-      <c r="E234" s="64"/>
-      <c r="F234" s="64"/>
-      <c r="G234" s="65"/>
-      <c r="H234" s="65" t="s">
+      <c r="D234" s="58"/>
+      <c r="E234" s="58"/>
+      <c r="F234" s="58"/>
+      <c r="G234" s="59"/>
+      <c r="H234" s="59" t="s">
         <v>248</v>
       </c>
-      <c r="I234" s="66" t="s">
+      <c r="I234" s="60" t="s">
         <v>247</v>
       </c>
-      <c r="J234" s="64"/>
-      <c r="K234" s="67"/>
-      <c r="L234" s="68"/>
+      <c r="J234" s="58"/>
+      <c r="K234" s="61"/>
+      <c r="L234" s="62"/>
       <c r="M234" s="6"/>
     </row>
     <row r="235" spans="1:13" ht="39">
@@ -10484,7 +10493,7 @@
       </c>
       <c r="J254" s="23"/>
       <c r="K254" s="21"/>
-      <c r="L254" s="60" t="s">
+      <c r="L254" s="68" t="s">
         <v>305</v>
       </c>
       <c r="M254" s="6"/>
@@ -10516,7 +10525,7 @@
         <v>304</v>
       </c>
       <c r="K255" s="21"/>
-      <c r="L255" s="61"/>
+      <c r="L255" s="69"/>
       <c r="M255" s="6"/>
     </row>
     <row r="256" spans="1:13" ht="15">
@@ -10618,7 +10627,7 @@
       </c>
       <c r="J259" s="23"/>
       <c r="K259" s="21"/>
-      <c r="L259" s="60" t="s">
+      <c r="L259" s="68" t="s">
         <v>314</v>
       </c>
       <c r="M259" s="6"/>
@@ -10648,7 +10657,7 @@
       </c>
       <c r="J260" s="23"/>
       <c r="K260" s="21"/>
-      <c r="L260" s="62"/>
+      <c r="L260" s="70"/>
       <c r="M260" s="6"/>
     </row>
     <row r="261" spans="1:13" ht="26.25">
@@ -10676,7 +10685,7 @@
       </c>
       <c r="J261" s="23"/>
       <c r="K261" s="21"/>
-      <c r="L261" s="62"/>
+      <c r="L261" s="70"/>
       <c r="M261" s="6"/>
     </row>
     <row r="262" spans="1:13" ht="26.25" customHeight="1">
@@ -10704,7 +10713,7 @@
       </c>
       <c r="J262" s="23"/>
       <c r="K262" s="21"/>
-      <c r="L262" s="62"/>
+      <c r="L262" s="70"/>
       <c r="M262" s="6"/>
     </row>
     <row r="263" spans="1:13" ht="26.25" customHeight="1">
@@ -10732,7 +10741,7 @@
       </c>
       <c r="J263" s="23"/>
       <c r="K263" s="21"/>
-      <c r="L263" s="62"/>
+      <c r="L263" s="70"/>
       <c r="M263" s="6"/>
     </row>
     <row r="264" spans="1:13" ht="39">
@@ -10760,7 +10769,7 @@
       </c>
       <c r="J264" s="23"/>
       <c r="K264" s="21"/>
-      <c r="L264" s="61"/>
+      <c r="L264" s="69"/>
       <c r="M264" s="6"/>
     </row>
     <row r="265" spans="1:13" ht="51.75">
@@ -10982,7 +10991,7 @@
       <c r="L271" s="6"/>
       <c r="M271" s="6"/>
     </row>
-    <row r="272" spans="1:13" ht="15">
+    <row r="272" spans="1:13" ht="26.25">
       <c r="A272">
         <f t="shared" si="56"/>
         <v>31</v>
@@ -10991,13 +11000,21 @@
         <f t="shared" si="54"/>
         <v>6</v>
       </c>
-      <c r="C272" s="3" t="str">
-        <f t="shared" si="55"/>
-        <v>31-6</v>
-      </c>
-      <c r="F272" s="54"/>
-      <c r="G272" s="54"/>
-      <c r="H272" s="55"/>
+      <c r="C272" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="F272" s="54" t="s">
+        <v>241</v>
+      </c>
+      <c r="G272" s="54" t="s">
+        <v>241</v>
+      </c>
+      <c r="H272" s="55" t="s">
+        <v>365</v>
+      </c>
+      <c r="I272" s="56" t="s">
+        <v>366</v>
+      </c>
       <c r="L272" s="6"/>
       <c r="M272" s="6"/>
     </row>

</xml_diff>

<commit_message>
Entries for manual system tests relating to alarm state indicators
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="361">
   <si>
     <t>Test Number</t>
   </si>
@@ -1125,6 +1125,15 @@
   </si>
   <si>
     <t>Create a config with SIMPLE IOC and blocks TEST_BLOCK_INT (SIMPLE:VALUE:P5) and TEST_BLOCK_STR (SIMPLE:HELLO). Run script "genie_python_blocks.py" from the testing area of the developer manual. Check that no assertions are violated and prompted behaviours are observed</t>
+  </si>
+  <si>
+    <t>Verify that a purple border appears around blocks in an INVALID-alarm state (.SEVR field)</t>
+  </si>
+  <si>
+    <t>Verify that an orange border appears around blocks in a MINOR-alarm state (.SEVR field)</t>
+  </si>
+  <si>
+    <t>Verify that a red border appears around blocks in an MAJOR-alarm state (.SEVR field)</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1553,6 +1562,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3985,11 +4000,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M796"/>
+  <dimension ref="A1:M799"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I115" sqref="I115"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J106" sqref="J106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -6651,7 +6666,7 @@
         <v>25</v>
       </c>
       <c r="C94" s="3" t="str">
-        <f t="shared" ref="C94:C110" si="3">CONCATENATE(A94,"-",B94)</f>
+        <f t="shared" ref="C94:C113" si="3">CONCATENATE(A94,"-",B94)</f>
         <v>16-25</v>
       </c>
       <c r="D94" s="9"/>
@@ -6780,7 +6795,7 @@
       </c>
       <c r="J98" s="8"/>
       <c r="K98" s="7"/>
-      <c r="L98" s="78"/>
+      <c r="L98" s="80"/>
     </row>
     <row r="99" spans="1:13" ht="30">
       <c r="A99">
@@ -6807,7 +6822,7 @@
       </c>
       <c r="J99" s="8"/>
       <c r="K99" s="7"/>
-      <c r="L99" s="79"/>
+      <c r="L99" s="81"/>
       <c r="M99" s="6"/>
     </row>
     <row r="100" spans="1:13" ht="45">
@@ -6835,7 +6850,7 @@
       </c>
       <c r="J100" s="8"/>
       <c r="K100" s="7"/>
-      <c r="L100" s="79"/>
+      <c r="L100" s="81"/>
       <c r="M100" s="6"/>
     </row>
     <row r="101" spans="1:13" ht="30">
@@ -6863,7 +6878,7 @@
       </c>
       <c r="J101" s="8"/>
       <c r="K101" s="7"/>
-      <c r="L101" s="80"/>
+      <c r="L101" s="82"/>
       <c r="M101" s="6"/>
     </row>
     <row r="102" spans="1:13" ht="26.25">
@@ -6978,156 +6993,150 @@
       <c r="L105" s="12"/>
       <c r="M105" s="6"/>
     </row>
-    <row r="106" spans="1:13" ht="39">
+    <row r="106" spans="1:13" ht="26.25">
       <c r="A106">
         <v>21</v>
       </c>
       <c r="B106">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C106" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-26</v>
+        <v>21-6</v>
       </c>
       <c r="D106" s="18"/>
       <c r="E106" s="18"/>
       <c r="F106" s="18"/>
-      <c r="G106" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="G106" s="19"/>
       <c r="H106" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I106" s="42" t="s">
-        <v>295</v>
-      </c>
-      <c r="J106" s="42"/>
+      <c r="I106" s="79" t="s">
+        <v>359</v>
+      </c>
+      <c r="J106" s="79"/>
       <c r="K106" s="19"/>
-      <c r="L106" s="42"/>
+      <c r="L106" s="79"/>
       <c r="M106" s="6"/>
     </row>
-    <row r="107" spans="1:13" ht="39">
+    <row r="107" spans="1:13" ht="26.25">
       <c r="A107">
         <v>21</v>
       </c>
       <c r="B107">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C107" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-27</v>
+        <v>21-7</v>
       </c>
       <c r="D107" s="18"/>
       <c r="E107" s="18"/>
       <c r="F107" s="18"/>
-      <c r="G107" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="G107" s="19"/>
       <c r="H107" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I107" s="42" t="s">
-        <v>296</v>
-      </c>
-      <c r="J107" s="42"/>
+      <c r="I107" s="79" t="s">
+        <v>360</v>
+      </c>
+      <c r="J107" s="79"/>
       <c r="K107" s="19"/>
-      <c r="L107" s="42"/>
+      <c r="L107" s="79"/>
       <c r="M107" s="6"/>
     </row>
-    <row r="108" spans="1:13" ht="39">
+    <row r="108" spans="1:13" ht="26.25">
       <c r="A108">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B108">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C108" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>22-2</v>
-      </c>
-      <c r="D108" s="20"/>
-      <c r="E108" s="20"/>
-      <c r="F108" s="20"/>
-      <c r="G108" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H108" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="I108" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="J108" s="20"/>
+        <v>21-8</v>
+      </c>
+      <c r="D108" s="18"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="18"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I108" s="78" t="s">
+        <v>358</v>
+      </c>
+      <c r="J108" s="78"/>
       <c r="K108" s="19"/>
-      <c r="L108" s="23"/>
+      <c r="L108" s="78"/>
       <c r="M108" s="6"/>
     </row>
-    <row r="109" spans="1:13" ht="26.25">
+    <row r="109" spans="1:13" ht="39">
       <c r="A109">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B109">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C109" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>22-3</v>
-      </c>
-      <c r="D109" s="20"/>
-      <c r="E109" s="20"/>
-      <c r="F109" s="20"/>
-      <c r="G109" s="20" t="s">
+        <v>21-26</v>
+      </c>
+      <c r="D109" s="18"/>
+      <c r="E109" s="18"/>
+      <c r="F109" s="18"/>
+      <c r="G109" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H109" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="I109" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="J109" s="20"/>
+      <c r="H109" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I109" s="42" t="s">
+        <v>295</v>
+      </c>
+      <c r="J109" s="42"/>
       <c r="K109" s="19"/>
-      <c r="L109" s="23"/>
+      <c r="L109" s="42"/>
       <c r="M109" s="6"/>
     </row>
     <row r="110" spans="1:13" ht="39">
       <c r="A110">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C110" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>26-1</v>
-      </c>
-      <c r="D110" s="20"/>
-      <c r="E110" s="20"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="20" t="s">
+        <v>21-27</v>
+      </c>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="18"/>
+      <c r="G110" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H110" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="I110" s="22" t="s">
-        <v>293</v>
-      </c>
-      <c r="J110" s="20"/>
+      <c r="H110" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I110" s="42" t="s">
+        <v>296</v>
+      </c>
+      <c r="J110" s="42"/>
       <c r="K110" s="19"/>
-      <c r="L110" s="23"/>
+      <c r="L110" s="42"/>
       <c r="M110" s="6"/>
     </row>
     <row r="111" spans="1:13" ht="39">
       <c r="A111">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C111" s="3" t="str">
-        <f t="shared" ref="C111:C112" si="4">CONCATENATE(A111,"-",B111)</f>
-        <v>26-1</v>
+        <f t="shared" si="3"/>
+        <v>22-2</v>
       </c>
       <c r="D111" s="20"/>
       <c r="E111" s="20"/>
@@ -7136,115 +7145,110 @@
         <v>62</v>
       </c>
       <c r="H111" s="21" t="s">
-        <v>292</v>
+        <v>247</v>
       </c>
       <c r="I111" s="22" t="s">
-        <v>293</v>
+        <v>248</v>
       </c>
       <c r="J111" s="20"/>
       <c r="K111" s="19"/>
       <c r="L111" s="23"/>
       <c r="M111" s="6"/>
     </row>
-    <row r="112" spans="1:13" ht="64.5">
+    <row r="112" spans="1:13" ht="26.25">
       <c r="A112">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C112" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>27-1</v>
+        <f t="shared" si="3"/>
+        <v>22-3</v>
       </c>
       <c r="D112" s="20"/>
       <c r="E112" s="20"/>
-      <c r="F112" s="77" t="s">
-        <v>240</v>
-      </c>
+      <c r="F112" s="20"/>
       <c r="G112" s="20" t="s">
         <v>62</v>
       </c>
       <c r="H112" s="21" t="s">
-        <v>354</v>
+        <v>247</v>
       </c>
       <c r="I112" s="22" t="s">
-        <v>356</v>
+        <v>249</v>
       </c>
       <c r="J112" s="20"/>
       <c r="K112" s="19"/>
       <c r="L112" s="23"/>
       <c r="M112" s="6"/>
     </row>
-    <row r="113" spans="1:13" ht="15.75" customHeight="1">
+    <row r="113" spans="1:13" ht="39">
       <c r="A113">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C113" s="3" t="str">
-        <f t="shared" ref="C113" si="5">CONCATENATE(A113,"-",B113)</f>
-        <v>27-2</v>
+        <f t="shared" si="3"/>
+        <v>26-1</v>
       </c>
       <c r="D113" s="20"/>
       <c r="E113" s="20"/>
-      <c r="F113" s="77" t="s">
-        <v>240</v>
-      </c>
+      <c r="F113" s="20"/>
       <c r="G113" s="20" t="s">
         <v>62</v>
       </c>
       <c r="H113" s="21" t="s">
-        <v>354</v>
+        <v>292</v>
       </c>
       <c r="I113" s="22" t="s">
-        <v>355</v>
+        <v>293</v>
       </c>
       <c r="J113" s="20"/>
       <c r="K113" s="19"/>
       <c r="L113" s="23"/>
-    </row>
-    <row r="114" spans="1:13" ht="77.25">
+      <c r="M113" s="6"/>
+    </row>
+    <row r="114" spans="1:13" ht="39">
       <c r="A114">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C114" s="3" t="str">
-        <f>CONCATENATE(A114,"-",B114)</f>
-        <v>27-3</v>
+        <f t="shared" ref="C114:C115" si="4">CONCATENATE(A114,"-",B114)</f>
+        <v>26-1</v>
       </c>
       <c r="D114" s="20"/>
       <c r="E114" s="20"/>
-      <c r="F114" s="77" t="s">
-        <v>240</v>
-      </c>
+      <c r="F114" s="20"/>
       <c r="G114" s="20" t="s">
         <v>62</v>
       </c>
       <c r="H114" s="21" t="s">
-        <v>354</v>
+        <v>292</v>
       </c>
       <c r="I114" s="22" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="J114" s="20"/>
       <c r="K114" s="19"/>
       <c r="L114" s="23"/>
       <c r="M114" s="6"/>
     </row>
-    <row r="115" spans="1:13" ht="15">
+    <row r="115" spans="1:13" ht="64.5">
       <c r="A115">
         <v>27</v>
       </c>
       <c r="B115">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C115" s="3" t="str">
-        <f>CONCATENATE(A115,"-",B115)</f>
-        <v>27-4</v>
+        <f t="shared" si="4"/>
+        <v>27-1</v>
       </c>
       <c r="D115" s="20"/>
       <c r="E115" s="20"/>
@@ -7258,23 +7262,100 @@
         <v>354</v>
       </c>
       <c r="I115" s="22" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="J115" s="20"/>
       <c r="K115" s="19"/>
       <c r="L115" s="23"/>
       <c r="M115" s="6"/>
     </row>
-    <row r="116" spans="1:13" ht="12.75">
-      <c r="L116" s="6"/>
-      <c r="M116" s="6"/>
-    </row>
-    <row r="117" spans="1:13" ht="12.75">
-      <c r="L117" s="6"/>
+    <row r="116" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A116">
+        <v>27</v>
+      </c>
+      <c r="B116">
+        <v>2</v>
+      </c>
+      <c r="C116" s="3" t="str">
+        <f t="shared" ref="C116" si="5">CONCATENATE(A116,"-",B116)</f>
+        <v>27-2</v>
+      </c>
+      <c r="D116" s="20"/>
+      <c r="E116" s="20"/>
+      <c r="F116" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G116" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H116" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I116" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="J116" s="20"/>
+      <c r="K116" s="19"/>
+      <c r="L116" s="23"/>
+    </row>
+    <row r="117" spans="1:13" ht="77.25">
+      <c r="A117">
+        <v>27</v>
+      </c>
+      <c r="B117">
+        <v>3</v>
+      </c>
+      <c r="C117" s="3" t="str">
+        <f>CONCATENATE(A117,"-",B117)</f>
+        <v>27-3</v>
+      </c>
+      <c r="D117" s="20"/>
+      <c r="E117" s="20"/>
+      <c r="F117" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G117" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H117" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I117" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="J117" s="20"/>
+      <c r="K117" s="19"/>
+      <c r="L117" s="23"/>
       <c r="M117" s="6"/>
     </row>
-    <row r="118" spans="1:13" ht="12.75">
-      <c r="L118" s="6"/>
+    <row r="118" spans="1:13" ht="15">
+      <c r="A118">
+        <v>27</v>
+      </c>
+      <c r="B118">
+        <v>4</v>
+      </c>
+      <c r="C118" s="3" t="str">
+        <f>CONCATENATE(A118,"-",B118)</f>
+        <v>27-4</v>
+      </c>
+      <c r="D118" s="20"/>
+      <c r="E118" s="20"/>
+      <c r="F118" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G118" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H118" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I118" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="J118" s="20"/>
+      <c r="K118" s="19"/>
+      <c r="L118" s="23"/>
       <c r="M118" s="6"/>
     </row>
     <row r="119" spans="1:13" ht="12.75">
@@ -9988,6 +10069,18 @@
     <row r="796" spans="12:13" ht="12.75">
       <c r="L796" s="6"/>
       <c r="M796" s="6"/>
+    </row>
+    <row r="797" spans="12:13" ht="12.75">
+      <c r="L797" s="6"/>
+      <c r="M797" s="6"/>
+    </row>
+    <row r="798" spans="12:13" ht="12.75">
+      <c r="L798" s="6"/>
+      <c r="M798" s="6"/>
+    </row>
+    <row r="799" spans="12:13" ht="12.75">
+      <c r="L799" s="6"/>
+      <c r="M799" s="6"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -10049,17 +10142,17 @@
   <mergeCells count="1">
     <mergeCell ref="L98:L101"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:K25 K27:K112 K114">
+  <conditionalFormatting sqref="K2:K25 K27:K115 K117">
     <cfRule type="containsBlanks" dxfId="11" priority="103">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K25 K27:K112 K114">
+  <conditionalFormatting sqref="K2:K25 K27:K115 K117">
     <cfRule type="containsText" dxfId="10" priority="104" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K25 K27:K112 K114">
+  <conditionalFormatting sqref="K2:K25 K27:K115 K117">
     <cfRule type="containsText" dxfId="9" priority="105" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
@@ -10079,34 +10172,34 @@
       <formula>NOT(ISERROR(SEARCH(("fail"),(K26))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K113">
+  <conditionalFormatting sqref="K116">
     <cfRule type="containsBlanks" dxfId="5" priority="4">
-      <formula>LEN(TRIM(K113))=0</formula>
+      <formula>LEN(TRIM(K116))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K113">
+  <conditionalFormatting sqref="K116">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K113))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K116))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K113">
+  <conditionalFormatting sqref="K116">
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K113))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K116))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K115">
+  <conditionalFormatting sqref="K118">
     <cfRule type="containsBlanks" dxfId="2" priority="1">
-      <formula>LEN(TRIM(K115))=0</formula>
+      <formula>LEN(TRIM(K118))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K115">
+  <conditionalFormatting sqref="K118">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K115))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K118))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K115">
+  <conditionalFormatting sqref="K118">
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K115))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K118))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update system test spreadsheet
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Instrument\Dev\dev_manual\testing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="8505" activeTab="1"/>
   </bookViews>
@@ -13,23 +18,23 @@
     <sheet name="Automated" sheetId="3" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Baker, Kathryn (STFC,RAL,ISIS) - Personal View" guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Kathryn Baker - Personal View" guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="1"/>
+    <customWorkbookView name="Clarke, Matt (STFC,RAL,ISIS) - Personal View" guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" mergeInterval="0" personalView="1" xWindow="75" yWindow="75" windowWidth="1707" windowHeight="1032" activeSheetId="1"/>
+    <customWorkbookView name="Willemsen, Thomas (Tessella,RAL,ISIS) - Personal View" guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="David Keymer - Personal View" guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1789" windowHeight="772" activeSheetId="1"/>
+    <customWorkbookView name="Akeroyd, Freddie (STFC,RAL,ISIS) - Personal View" guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1667" windowHeight="917" activeSheetId="1"/>
+    <customWorkbookView name="Holt, John (Tessella,RAL,ISIS) - Personal View" guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1186" activeSheetId="1"/>
+    <customWorkbookView name="Oram, Dominic (STFC,RAL,ISIS) - Personal View" guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="894" activeSheetId="1"/>
     <customWorkbookView name="Potter, Adrian (Tessella,RAL,ISIS) - Personal View" guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1014" activeSheetId="1"/>
-    <customWorkbookView name="Oram, Dominic (STFC,RAL,ISIS) - Personal View" guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="894" activeSheetId="1"/>
-    <customWorkbookView name="Holt, John (Tessella,RAL,ISIS) - Personal View" guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1186" activeSheetId="1"/>
-    <customWorkbookView name="Akeroyd, Freddie (STFC,RAL,ISIS) - Personal View" guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1667" windowHeight="917" activeSheetId="1"/>
-    <customWorkbookView name="David Keymer - Personal View" guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1789" windowHeight="772" activeSheetId="1"/>
-    <customWorkbookView name="Willemsen, Thomas (Tessella,RAL,ISIS) - Personal View" guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Clarke, Matt (STFC,RAL,ISIS) - Personal View" guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" mergeInterval="0" personalView="1" xWindow="75" yWindow="75" windowWidth="1707" windowHeight="1032" activeSheetId="1"/>
-    <customWorkbookView name="Kathryn Baker - Personal View" guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="1"/>
-    <customWorkbookView name="Baker, Kathryn (STFC,RAL,ISIS) - Personal View" guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="363">
   <si>
     <t>Test Number</t>
   </si>
@@ -1135,11 +1140,17 @@
   <si>
     <t>Verify that a red border appears around blocks in an MAJOR-alarm state (.SEVR field)</t>
   </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Check that spectra plots appear. Check that you can change the Y axis type and that this is reflected in the graph's Y axis.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11">
     <font>
       <sz val="10"/>
@@ -1395,7 +1406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1573,6 +1584,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1802,7 +1814,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1837,7 +1849,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4000,11 +4012,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M799"/>
+  <dimension ref="A1:M800"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J106" sqref="J106"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4070,7 +4082,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f t="shared" ref="C2:C29" si="0">CONCATENATE(A2,"-",B2)</f>
+        <f t="shared" ref="C2:C30" si="0">CONCATENATE(A2,"-",B2)</f>
         <v>4-1</v>
       </c>
       <c r="D2" s="5"/>
@@ -4229,30 +4241,31 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="15">
+    <row r="8" spans="1:13" ht="45">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>7-2</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="G8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>64</v>
+        <v>6-20</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>362</v>
       </c>
       <c r="J8" s="8"/>
-      <c r="K8" s="7"/>
+      <c r="K8" s="9"/>
       <c r="L8" s="8"/>
       <c r="M8" s="6"/>
     </row>
@@ -4261,15 +4274,14 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>7-4</v>
+        <v>7-2</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
         <v>62</v>
       </c>
@@ -4277,43 +4289,39 @@
         <v>63</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="7"/>
       <c r="L9" s="8"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:13" ht="45">
+    <row r="10" spans="1:13" ht="15">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>7-9</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="H10" s="9" t="s">
+        <v>7-4</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="8" t="s">
-        <v>285</v>
-      </c>
+      <c r="I10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="8"/>
       <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" ht="45">
@@ -4321,11 +4329,11 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>7-10</v>
+        <v>7-9</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -4337,10 +4345,10 @@
         <v>63</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="8" t="s">
@@ -4348,16 +4356,16 @@
       </c>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13" ht="30">
+    <row r="12" spans="1:13" ht="45">
       <c r="A12">
         <v>7</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>7-11</v>
+        <v>7-10</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -4369,10 +4377,10 @@
         <v>63</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="8" t="s">
@@ -4380,32 +4388,36 @@
       </c>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13" ht="15">
+    <row r="13" spans="1:13" ht="30">
       <c r="A13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-1</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="8"/>
+        <v>7-11</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="8" t="s">
+        <v>285</v>
+      </c>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" ht="15">
@@ -4413,11 +4425,11 @@
         <v>8</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-2</v>
+        <v>8-1</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -4429,11 +4441,11 @@
         <v>70</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="1"/>
+      <c r="L14" s="8"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" ht="15">
@@ -4441,11 +4453,11 @@
         <v>8</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-3</v>
+        <v>8-2</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -4457,11 +4469,11 @@
         <v>70</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="8"/>
+      <c r="L15" s="1"/>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:13" ht="15">
@@ -4469,11 +4481,11 @@
         <v>8</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-4</v>
+        <v>8-3</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -4485,11 +4497,11 @@
         <v>70</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="1"/>
+      <c r="L16" s="8"/>
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:13" ht="15">
@@ -4497,11 +4509,11 @@
         <v>8</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-5</v>
+        <v>8-4</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -4513,11 +4525,11 @@
         <v>70</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="8"/>
+      <c r="L17" s="1"/>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" ht="15">
@@ -4525,11 +4537,11 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-6</v>
+        <v>8-5</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -4541,7 +4553,7 @@
         <v>70</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="7"/>
@@ -4553,11 +4565,11 @@
         <v>8</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-7</v>
+        <v>8-6</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -4569,11 +4581,11 @@
         <v>70</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="1"/>
+      <c r="L19" s="8"/>
       <c r="M19" s="6"/>
     </row>
     <row r="20" spans="1:13" ht="15">
@@ -4581,11 +4593,11 @@
         <v>8</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-8</v>
+        <v>8-7</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -4597,7 +4609,7 @@
         <v>70</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="7"/>
@@ -4609,11 +4621,11 @@
         <v>8</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-9</v>
+        <v>8-8</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -4625,11 +4637,11 @@
         <v>70</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
+      <c r="L21" s="1"/>
       <c r="M21" s="6"/>
     </row>
     <row r="22" spans="1:13" ht="15">
@@ -4637,11 +4649,11 @@
         <v>8</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-10</v>
+        <v>8-9</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -4653,43 +4665,39 @@
         <v>70</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="1"/>
+      <c r="L22" s="8"/>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="1:13" ht="30">
+    <row r="23" spans="1:13" ht="15">
       <c r="A23">
         <v>8</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-12</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="G23" s="9" t="s">
+        <v>8-10</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="H23" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I23" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="K23" s="9"/>
-      <c r="L23" s="8"/>
+      <c r="I23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J23" s="8"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="1"/>
       <c r="M23" s="6"/>
     </row>
     <row r="24" spans="1:13" ht="30">
@@ -4697,61 +4705,61 @@
         <v>8</v>
       </c>
       <c r="B24">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-14</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J24" s="8"/>
-      <c r="K24" s="7"/>
+        <v>8-12</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="K24" s="9"/>
       <c r="L24" s="8"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:13" ht="15">
+    <row r="25" spans="1:13" ht="30">
       <c r="A25">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>13-1</v>
+        <v>8-14</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="64" t="s">
-        <v>62</v>
+      <c r="F25" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="7"/>
-      <c r="L25" s="8" t="s">
-        <v>352</v>
-      </c>
+      <c r="L25" s="8"/>
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" ht="15">
@@ -4759,67 +4767,71 @@
         <v>13</v>
       </c>
       <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>13-1</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" s="8"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="M26" s="6"/>
+    </row>
+    <row r="27" spans="1:13" ht="15">
+      <c r="A27">
+        <v>13</v>
+      </c>
+      <c r="B27">
         <v>2</v>
       </c>
-      <c r="C26" s="60" t="str">
+      <c r="C27" s="60" t="str">
         <f t="shared" si="0"/>
         <v>13-2</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="64" t="s">
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G27" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I27" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="J26" s="8"/>
-      <c r="K26" s="9"/>
-    </row>
-    <row r="27" spans="1:13" ht="30">
-      <c r="A27">
-        <v>15</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>15-1</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="J27" s="8"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="6"/>
+      <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:13" ht="30">
       <c r="A28">
         <v>15</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>15-2</v>
+        <v>15-1</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -4831,7 +4843,7 @@
         <v>108</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="7"/>
@@ -4843,11 +4855,11 @@
         <v>15</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>15-3</v>
+        <v>15-2</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -4859,7 +4871,7 @@
         <v>108</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="7"/>
@@ -4871,23 +4883,23 @@
         <v>15</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3" t="str">
-        <f t="shared" ref="C30:C61" si="1">CONCATENATE(A30,"-",B30)</f>
-        <v>15-4</v>
+        <f t="shared" si="0"/>
+        <v>15-3</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="7"/>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="7" t="s">
         <v>62</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="7"/>
@@ -4899,11 +4911,11 @@
         <v>15</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>15-5</v>
+        <f t="shared" ref="C31:C62" si="1">CONCATENATE(A31,"-",B31)</f>
+        <v>15-4</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -4915,7 +4927,7 @@
         <v>108</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J31" s="8"/>
       <c r="K31" s="7"/>
@@ -4927,11 +4939,11 @@
         <v>15</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-6</v>
+        <v>15-5</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -4943,7 +4955,7 @@
         <v>108</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="7"/>
@@ -4955,11 +4967,11 @@
         <v>15</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-7</v>
+        <v>15-6</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -4971,7 +4983,7 @@
         <v>108</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="7"/>
@@ -4983,11 +4995,11 @@
         <v>15</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-8</v>
+        <v>15-7</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -4999,23 +5011,23 @@
         <v>108</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="7"/>
       <c r="L34" s="8"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="1:13" ht="45">
+    <row r="35" spans="1:13" ht="30">
       <c r="A35">
         <v>15</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C35" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-9</v>
+        <v>15-8</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -5027,23 +5039,23 @@
         <v>108</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>273</v>
+        <v>116</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="7"/>
       <c r="L35" s="8"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="1:13" ht="30">
+    <row r="36" spans="1:13" ht="45">
       <c r="A36">
         <v>15</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-10</v>
+        <v>15-9</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -5055,38 +5067,38 @@
         <v>108</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>117</v>
+        <v>273</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="7"/>
       <c r="L36" s="8"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="1:13" ht="60">
+    <row r="37" spans="1:13" ht="30">
       <c r="A37">
         <v>15</v>
       </c>
       <c r="B37">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-11</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
+        <v>15-10</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H37" s="9" t="s">
+      <c r="H37" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I37" s="8" t="s">
-        <v>287</v>
+      <c r="I37" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="J37" s="8"/>
-      <c r="K37" s="9"/>
+      <c r="K37" s="7"/>
       <c r="L37" s="8"/>
       <c r="M37" s="6"/>
     </row>
@@ -5095,11 +5107,11 @@
         <v>15</v>
       </c>
       <c r="B38">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-12</v>
+        <v>15-11</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -5111,7 +5123,7 @@
         <v>108</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="9"/>
@@ -5123,11 +5135,11 @@
         <v>15</v>
       </c>
       <c r="B39">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C39" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-13</v>
+        <v>15-12</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -5139,38 +5151,38 @@
         <v>108</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="9"/>
       <c r="L39" s="8"/>
       <c r="M39" s="6"/>
     </row>
-    <row r="40" spans="1:13" ht="30">
+    <row r="40" spans="1:13" ht="60">
       <c r="A40">
         <v>15</v>
       </c>
       <c r="B40">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C40" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-14</v>
-      </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="7"/>
+        <v>15-13</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
       <c r="G40" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H40" s="7" t="s">
+      <c r="H40" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="I40" s="1" t="s">
-        <v>118</v>
+      <c r="I40" s="8" t="s">
+        <v>274</v>
       </c>
       <c r="J40" s="8"/>
-      <c r="K40" s="7"/>
+      <c r="K40" s="9"/>
       <c r="L40" s="8"/>
       <c r="M40" s="6"/>
     </row>
@@ -5179,11 +5191,11 @@
         <v>15</v>
       </c>
       <c r="B41">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-15</v>
+        <v>15-14</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -5195,7 +5207,7 @@
         <v>108</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="7"/>
@@ -5207,11 +5219,11 @@
         <v>15</v>
       </c>
       <c r="B42">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C42" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-16</v>
+        <v>15-15</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -5223,11 +5235,11 @@
         <v>108</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="7"/>
-      <c r="L42" s="1"/>
+      <c r="L42" s="8"/>
       <c r="M42" s="6"/>
     </row>
     <row r="43" spans="1:13" ht="30">
@@ -5235,11 +5247,11 @@
         <v>15</v>
       </c>
       <c r="B43">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C43" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-17</v>
+        <v>15-16</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -5251,11 +5263,11 @@
         <v>108</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J43" s="8"/>
       <c r="K43" s="7"/>
-      <c r="L43" s="8"/>
+      <c r="L43" s="1"/>
       <c r="M43" s="6"/>
     </row>
     <row r="44" spans="1:13" ht="30">
@@ -5263,11 +5275,11 @@
         <v>15</v>
       </c>
       <c r="B44">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-18</v>
+        <v>15-17</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
@@ -5279,7 +5291,7 @@
         <v>108</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J44" s="8"/>
       <c r="K44" s="7"/>
@@ -5291,11 +5303,11 @@
         <v>15</v>
       </c>
       <c r="B45">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C45" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-19</v>
+        <v>15-18</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -5307,23 +5319,23 @@
         <v>108</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="7"/>
       <c r="L45" s="8"/>
       <c r="M45" s="6"/>
     </row>
-    <row r="46" spans="1:13" ht="15">
+    <row r="46" spans="1:13" ht="30">
       <c r="A46">
         <v>15</v>
       </c>
       <c r="B46">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C46" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-20</v>
+        <v>15-19</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -5335,7 +5347,7 @@
         <v>108</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="7"/>
@@ -5347,11 +5359,11 @@
         <v>15</v>
       </c>
       <c r="B47">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C47" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-21</v>
+        <v>15-20</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -5363,7 +5375,7 @@
         <v>108</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="7"/>
@@ -5375,11 +5387,11 @@
         <v>15</v>
       </c>
       <c r="B48">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C48" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-22</v>
+        <v>15-21</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -5391,7 +5403,7 @@
         <v>108</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J48" s="8"/>
       <c r="K48" s="7"/>
@@ -5403,11 +5415,11 @@
         <v>15</v>
       </c>
       <c r="B49">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C49" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-23</v>
+        <v>15-22</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -5419,7 +5431,7 @@
         <v>108</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J49" s="8"/>
       <c r="K49" s="7"/>
@@ -5431,11 +5443,11 @@
         <v>15</v>
       </c>
       <c r="B50">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C50" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-24</v>
+        <v>15-23</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -5447,7 +5459,7 @@
         <v>108</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J50" s="8"/>
       <c r="K50" s="7"/>
@@ -5459,11 +5471,11 @@
         <v>15</v>
       </c>
       <c r="B51">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C51" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-25</v>
+        <v>15-24</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -5475,7 +5487,7 @@
         <v>108</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J51" s="8"/>
       <c r="K51" s="7"/>
@@ -5487,11 +5499,11 @@
         <v>15</v>
       </c>
       <c r="B52">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C52" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-26</v>
+        <v>15-25</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
@@ -5503,7 +5515,7 @@
         <v>108</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J52" s="8"/>
       <c r="K52" s="7"/>
@@ -5515,11 +5527,11 @@
         <v>15</v>
       </c>
       <c r="B53">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C53" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-27</v>
+        <v>15-26</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -5531,7 +5543,7 @@
         <v>108</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="7"/>
@@ -5543,11 +5555,11 @@
         <v>15</v>
       </c>
       <c r="B54">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C54" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-28</v>
+        <v>15-27</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
@@ -5559,7 +5571,7 @@
         <v>108</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J54" s="8"/>
       <c r="K54" s="7"/>
@@ -5571,11 +5583,11 @@
         <v>15</v>
       </c>
       <c r="B55">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C55" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-29</v>
+        <v>15-28</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
@@ -5587,7 +5599,7 @@
         <v>108</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J55" s="8"/>
       <c r="K55" s="7"/>
@@ -5599,11 +5611,11 @@
         <v>15</v>
       </c>
       <c r="B56">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C56" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-30</v>
+        <v>15-29</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
@@ -5615,7 +5627,7 @@
         <v>108</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J56" s="8"/>
       <c r="K56" s="7"/>
@@ -5627,11 +5639,11 @@
         <v>15</v>
       </c>
       <c r="B57">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C57" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-31</v>
+        <v>15-30</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
@@ -5643,7 +5655,7 @@
         <v>108</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J57" s="8"/>
       <c r="K57" s="7"/>
@@ -5655,11 +5667,11 @@
         <v>15</v>
       </c>
       <c r="B58">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-32</v>
+        <v>15-31</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
@@ -5671,79 +5683,79 @@
         <v>108</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J58" s="8"/>
       <c r="K58" s="7"/>
       <c r="L58" s="8"/>
       <c r="M58" s="6"/>
     </row>
-    <row r="59" spans="1:13" ht="30">
+    <row r="59" spans="1:13" ht="15">
       <c r="A59">
         <v>15</v>
       </c>
       <c r="B59">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C59" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-33</v>
-      </c>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
+        <v>15-32</v>
+      </c>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="7"/>
       <c r="G59" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H59" s="9" t="s">
+      <c r="H59" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I59" s="8" t="s">
-        <v>223</v>
+      <c r="I59" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="J59" s="8"/>
-      <c r="K59" s="9"/>
+      <c r="K59" s="7"/>
       <c r="L59" s="8"/>
       <c r="M59" s="6"/>
     </row>
-    <row r="60" spans="1:13" ht="15">
+    <row r="60" spans="1:13" ht="30">
       <c r="A60">
         <v>15</v>
       </c>
       <c r="B60">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C60" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-34</v>
-      </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="7"/>
+        <v>15-33</v>
+      </c>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
       <c r="G60" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H60" s="7" t="s">
+      <c r="H60" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="I60" s="1" t="s">
-        <v>137</v>
+      <c r="I60" s="8" t="s">
+        <v>223</v>
       </c>
       <c r="J60" s="8"/>
-      <c r="K60" s="7"/>
+      <c r="K60" s="9"/>
       <c r="L60" s="8"/>
       <c r="M60" s="6"/>
     </row>
-    <row r="61" spans="1:13" ht="30">
+    <row r="61" spans="1:13" ht="15">
       <c r="A61">
         <v>15</v>
       </c>
       <c r="B61">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C61" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-35</v>
+        <v>15-34</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -5755,23 +5767,23 @@
         <v>108</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J61" s="8"/>
       <c r="K61" s="7"/>
-      <c r="L61" s="1"/>
+      <c r="L61" s="8"/>
       <c r="M61" s="6"/>
     </row>
-    <row r="62" spans="1:13" ht="15">
+    <row r="62" spans="1:13" ht="30">
       <c r="A62">
         <v>15</v>
       </c>
       <c r="B62">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C62" s="3" t="str">
-        <f t="shared" ref="C62:C93" si="2">CONCATENATE(A62,"-",B62)</f>
-        <v>15-36</v>
+        <f t="shared" si="1"/>
+        <v>15-35</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
@@ -5783,23 +5795,23 @@
         <v>108</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J62" s="8"/>
       <c r="K62" s="7"/>
-      <c r="L62" s="8"/>
+      <c r="L62" s="1"/>
       <c r="M62" s="6"/>
     </row>
-    <row r="63" spans="1:13" ht="30">
+    <row r="63" spans="1:13" ht="15">
       <c r="A63">
         <v>15</v>
       </c>
       <c r="B63">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C63" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>15-37</v>
+        <f t="shared" ref="C63:C94" si="2">CONCATENATE(A63,"-",B63)</f>
+        <v>15-36</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
@@ -5811,7 +5823,7 @@
         <v>108</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J63" s="8"/>
       <c r="K63" s="7"/>
@@ -5823,11 +5835,11 @@
         <v>15</v>
       </c>
       <c r="B64">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C64" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-38</v>
+        <v>15-37</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
@@ -5839,23 +5851,23 @@
         <v>108</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J64" s="8"/>
       <c r="K64" s="7"/>
       <c r="L64" s="8"/>
       <c r="M64" s="6"/>
     </row>
-    <row r="65" spans="1:13" ht="15">
+    <row r="65" spans="1:13" ht="30">
       <c r="A65">
         <v>15</v>
       </c>
       <c r="B65">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C65" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-41</v>
+        <v>15-38</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
@@ -5867,7 +5879,7 @@
         <v>108</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J65" s="8"/>
       <c r="K65" s="7"/>
@@ -5879,11 +5891,11 @@
         <v>15</v>
       </c>
       <c r="B66">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C66" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-42</v>
+        <v>15-41</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
@@ -5895,7 +5907,7 @@
         <v>108</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="7"/>
@@ -5907,11 +5919,11 @@
         <v>15</v>
       </c>
       <c r="B67">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C67" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-45</v>
+        <v>15-42</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
@@ -5923,7 +5935,7 @@
         <v>108</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J67" s="8"/>
       <c r="K67" s="7"/>
@@ -5935,11 +5947,11 @@
         <v>15</v>
       </c>
       <c r="B68">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C68" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-46</v>
+        <v>15-45</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
@@ -5951,7 +5963,7 @@
         <v>108</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J68" s="8"/>
       <c r="K68" s="7"/>
@@ -5963,11 +5975,11 @@
         <v>15</v>
       </c>
       <c r="B69">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C69" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-47</v>
+        <v>15-46</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
@@ -5979,7 +5991,7 @@
         <v>108</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J69" s="8"/>
       <c r="K69" s="7"/>
@@ -5991,11 +6003,11 @@
         <v>15</v>
       </c>
       <c r="B70">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C70" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-48</v>
+        <v>15-47</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
@@ -6007,7 +6019,7 @@
         <v>108</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="7"/>
@@ -6019,11 +6031,11 @@
         <v>15</v>
       </c>
       <c r="B71">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C71" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-49</v>
+        <v>15-48</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
@@ -6035,51 +6047,51 @@
         <v>108</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J71" s="8"/>
       <c r="K71" s="7"/>
       <c r="L71" s="8"/>
       <c r="M71" s="6"/>
     </row>
-    <row r="72" spans="1:13" ht="30">
+    <row r="72" spans="1:13" ht="15">
       <c r="A72">
         <v>15</v>
       </c>
       <c r="B72">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C72" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-51</v>
+        <v>15-49</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="7"/>
-      <c r="G72" s="7" t="s">
+      <c r="G72" s="9" t="s">
         <v>62</v>
       </c>
       <c r="H72" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J72" s="8"/>
-      <c r="K72" s="5"/>
-      <c r="L72" s="16"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="8"/>
       <c r="M72" s="6"/>
     </row>
-    <row r="73" spans="1:13" ht="60">
+    <row r="73" spans="1:13" ht="30">
       <c r="A73">
         <v>15</v>
       </c>
       <c r="B73">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C73" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-52</v>
+        <v>15-51</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
@@ -6088,26 +6100,26 @@
         <v>62</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>260</v>
+        <v>154</v>
       </c>
       <c r="J73" s="8"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="8"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="16"/>
       <c r="M73" s="6"/>
     </row>
-    <row r="74" spans="1:13" ht="30">
+    <row r="74" spans="1:13" ht="60">
       <c r="A74">
         <v>15</v>
       </c>
       <c r="B74">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C74" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-53</v>
+        <v>15-52</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
@@ -6119,51 +6131,51 @@
         <v>155</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>156</v>
+        <v>260</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="7"/>
-      <c r="L74" s="1"/>
+      <c r="L74" s="8"/>
       <c r="M74" s="6"/>
     </row>
-    <row r="75" spans="1:13" ht="50.25" customHeight="1">
+    <row r="75" spans="1:13" ht="30">
       <c r="A75">
         <v>15</v>
       </c>
       <c r="B75">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C75" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-56</v>
-      </c>
-      <c r="D75" s="39"/>
-      <c r="E75" s="39"/>
-      <c r="F75" s="39"/>
-      <c r="G75" s="39" t="s">
+        <v>15-53</v>
+      </c>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H75" s="39" t="s">
+      <c r="H75" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="I75" s="41" t="s">
-        <v>261</v>
-      </c>
-      <c r="J75" s="34"/>
-      <c r="K75" s="9"/>
-      <c r="L75" s="8"/>
+      <c r="I75" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J75" s="8"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="1"/>
       <c r="M75" s="6"/>
     </row>
-    <row r="76" spans="1:13" ht="64.5">
+    <row r="76" spans="1:13" ht="50.25" customHeight="1">
       <c r="A76">
         <v>15</v>
       </c>
       <c r="B76">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C76" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-57</v>
+        <v>15-56</v>
       </c>
       <c r="D76" s="39"/>
       <c r="E76" s="39"/>
@@ -6172,10 +6184,10 @@
         <v>62</v>
       </c>
       <c r="H76" s="39" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="I76" s="41" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
       <c r="J76" s="34"/>
       <c r="K76" s="9"/>
@@ -6187,11 +6199,11 @@
         <v>15</v>
       </c>
       <c r="B77">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C77" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-58</v>
+        <v>15-57</v>
       </c>
       <c r="D77" s="39"/>
       <c r="E77" s="39"/>
@@ -6203,7 +6215,7 @@
         <v>108</v>
       </c>
       <c r="I77" s="41" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="J77" s="34"/>
       <c r="K77" s="9"/>
@@ -6215,11 +6227,11 @@
         <v>15</v>
       </c>
       <c r="B78">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C78" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-63</v>
+        <v>15-58</v>
       </c>
       <c r="D78" s="39"/>
       <c r="E78" s="39"/>
@@ -6231,7 +6243,7 @@
         <v>108</v>
       </c>
       <c r="I78" s="41" t="s">
-        <v>340</v>
+        <v>303</v>
       </c>
       <c r="J78" s="34"/>
       <c r="K78" s="9"/>
@@ -6243,11 +6255,11 @@
         <v>15</v>
       </c>
       <c r="B79">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C79" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-64</v>
+        <v>15-63</v>
       </c>
       <c r="D79" s="39"/>
       <c r="E79" s="39"/>
@@ -6259,51 +6271,51 @@
         <v>108</v>
       </c>
       <c r="I79" s="41" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="J79" s="34"/>
       <c r="K79" s="9"/>
       <c r="L79" s="8"/>
       <c r="M79" s="6"/>
     </row>
-    <row r="80" spans="1:13" ht="30">
+    <row r="80" spans="1:13" ht="64.5">
       <c r="A80">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B80">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="C80" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-9</v>
-      </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="7"/>
-      <c r="G80" s="7" t="s">
+        <v>15-64</v>
+      </c>
+      <c r="D80" s="39"/>
+      <c r="E80" s="39"/>
+      <c r="F80" s="39"/>
+      <c r="G80" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H80" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="J80" s="8"/>
-      <c r="K80" s="7"/>
-      <c r="L80" s="1"/>
+      <c r="H80" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="I80" s="41" t="s">
+        <v>346</v>
+      </c>
+      <c r="J80" s="34"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="8"/>
       <c r="M80" s="6"/>
     </row>
-    <row r="81" spans="1:13" ht="45">
+    <row r="81" spans="1:13" ht="30">
       <c r="A81">
         <v>16</v>
       </c>
       <c r="B81">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C81" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-10</v>
+        <v>16-9</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
@@ -6315,23 +6327,23 @@
         <v>97</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J81" s="8"/>
       <c r="K81" s="7"/>
-      <c r="L81" s="8"/>
+      <c r="L81" s="1"/>
       <c r="M81" s="6"/>
     </row>
-    <row r="82" spans="1:13" ht="30">
+    <row r="82" spans="1:13" ht="45">
       <c r="A82">
         <v>16</v>
       </c>
       <c r="B82">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C82" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-11</v>
+        <v>16-10</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
@@ -6343,23 +6355,23 @@
         <v>97</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J82" s="8"/>
       <c r="K82" s="7"/>
       <c r="L82" s="8"/>
       <c r="M82" s="6"/>
     </row>
-    <row r="83" spans="1:13" ht="45">
+    <row r="83" spans="1:13" ht="30">
       <c r="A83">
         <v>16</v>
       </c>
       <c r="B83">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C83" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-12</v>
+        <v>16-11</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
@@ -6371,7 +6383,7 @@
         <v>97</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J83" s="8"/>
       <c r="K83" s="7"/>
@@ -6383,11 +6395,11 @@
         <v>16</v>
       </c>
       <c r="B84">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C84" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-13</v>
+        <v>16-12</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
@@ -6399,23 +6411,23 @@
         <v>97</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J84" s="8"/>
       <c r="K84" s="7"/>
       <c r="L84" s="8"/>
       <c r="M84" s="6"/>
     </row>
-    <row r="85" spans="1:13" ht="60">
+    <row r="85" spans="1:13" ht="45">
       <c r="A85">
         <v>16</v>
       </c>
       <c r="B85">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C85" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-14</v>
+        <v>16-13</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
@@ -6427,23 +6439,23 @@
         <v>97</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J85" s="8"/>
       <c r="K85" s="7"/>
       <c r="L85" s="8"/>
       <c r="M85" s="6"/>
     </row>
-    <row r="86" spans="1:13" ht="15">
+    <row r="86" spans="1:13" ht="60">
       <c r="A86">
         <v>16</v>
       </c>
       <c r="B86">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C86" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-15</v>
+        <v>16-14</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
@@ -6455,7 +6467,7 @@
         <v>97</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J86" s="8"/>
       <c r="K86" s="7"/>
@@ -6467,11 +6479,11 @@
         <v>16</v>
       </c>
       <c r="B87">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C87" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-16</v>
+        <v>16-15</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
@@ -6483,38 +6495,38 @@
         <v>97</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J87" s="8"/>
       <c r="K87" s="7"/>
       <c r="L87" s="8"/>
       <c r="M87" s="6"/>
     </row>
-    <row r="88" spans="1:13" ht="30">
+    <row r="88" spans="1:13" ht="15">
       <c r="A88">
         <v>16</v>
       </c>
       <c r="B88">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C88" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-18</v>
-      </c>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
-      <c r="G88" s="9" t="s">
+        <v>16-16</v>
+      </c>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H88" s="9" t="s">
+      <c r="H88" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="I88" s="8" t="s">
-        <v>318</v>
+      <c r="I88" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="J88" s="8"/>
-      <c r="K88" s="9"/>
+      <c r="K88" s="7"/>
       <c r="L88" s="8"/>
       <c r="M88" s="6"/>
     </row>
@@ -6523,11 +6535,11 @@
         <v>16</v>
       </c>
       <c r="B89">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C89" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-19</v>
+        <v>16-18</v>
       </c>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
@@ -6539,7 +6551,7 @@
         <v>97</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="J89" s="8"/>
       <c r="K89" s="9"/>
@@ -6551,26 +6563,26 @@
         <v>16</v>
       </c>
       <c r="B90">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C90" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-21</v>
-      </c>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="7"/>
-      <c r="G90" s="7" t="s">
+        <v>16-19</v>
+      </c>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H90" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>179</v>
+      <c r="H90" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I90" s="8" t="s">
+        <v>312</v>
       </c>
       <c r="J90" s="8"/>
-      <c r="K90" s="7"/>
+      <c r="K90" s="9"/>
       <c r="L90" s="8"/>
       <c r="M90" s="6"/>
     </row>
@@ -6579,11 +6591,11 @@
         <v>16</v>
       </c>
       <c r="B91">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C91" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-22</v>
+        <v>16-21</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -6595,23 +6607,23 @@
         <v>178</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J91" s="8"/>
       <c r="K91" s="7"/>
       <c r="L91" s="8"/>
       <c r="M91" s="6"/>
     </row>
-    <row r="92" spans="1:13" ht="15">
+    <row r="92" spans="1:13" ht="30">
       <c r="A92">
         <v>16</v>
       </c>
       <c r="B92">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C92" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-23</v>
+        <v>16-22</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -6623,7 +6635,7 @@
         <v>178</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J92" s="8"/>
       <c r="K92" s="7"/>
@@ -6635,11 +6647,11 @@
         <v>16</v>
       </c>
       <c r="B93">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C93" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-24</v>
+        <v>16-23</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
@@ -6651,79 +6663,79 @@
         <v>178</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J93" s="8"/>
       <c r="K93" s="7"/>
       <c r="L93" s="8"/>
       <c r="M93" s="6"/>
     </row>
-    <row r="94" spans="1:13" ht="60">
+    <row r="94" spans="1:13" ht="15">
       <c r="A94">
         <v>16</v>
       </c>
       <c r="B94">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C94" s="3" t="str">
-        <f t="shared" ref="C94:C113" si="3">CONCATENATE(A94,"-",B94)</f>
-        <v>16-25</v>
-      </c>
-      <c r="D94" s="9"/>
-      <c r="E94" s="9"/>
-      <c r="F94" s="9"/>
-      <c r="G94" s="9" t="s">
+        <f t="shared" si="2"/>
+        <v>16-24</v>
+      </c>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H94" s="9" t="s">
+      <c r="H94" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="I94" s="8" t="s">
-        <v>291</v>
+      <c r="I94" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="J94" s="8"/>
-      <c r="K94" s="9"/>
+      <c r="K94" s="7"/>
       <c r="L94" s="8"/>
       <c r="M94" s="6"/>
     </row>
-    <row r="95" spans="1:13" ht="30">
+    <row r="95" spans="1:13" ht="60">
       <c r="A95">
+        <v>16</v>
+      </c>
+      <c r="B95">
+        <v>25</v>
+      </c>
+      <c r="C95" s="3" t="str">
+        <f t="shared" ref="C95:C114" si="3">CONCATENATE(A95,"-",B95)</f>
+        <v>16-25</v>
+      </c>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H95" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="I95" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="J95" s="8"/>
+      <c r="K95" s="9"/>
+      <c r="L95" s="8"/>
+      <c r="M95" s="6"/>
+    </row>
+    <row r="96" spans="1:13" ht="30">
+      <c r="A96">
         <v>17</v>
       </c>
-      <c r="B95">
+      <c r="B96">
         <v>2</v>
       </c>
-      <c r="C95" s="3" t="str">
+      <c r="C96" s="3" t="str">
         <f t="shared" si="3"/>
         <v>17-2</v>
-      </c>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="7"/>
-      <c r="G95" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H95" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="J95" s="8"/>
-      <c r="K95" s="7"/>
-      <c r="L95" s="1"/>
-      <c r="M95" s="6"/>
-    </row>
-    <row r="96" spans="1:13" ht="15">
-      <c r="A96">
-        <v>17</v>
-      </c>
-      <c r="B96">
-        <v>4</v>
-      </c>
-      <c r="C96" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>17-4</v>
       </c>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
@@ -6735,23 +6747,23 @@
         <v>183</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J96" s="8"/>
       <c r="K96" s="7"/>
-      <c r="L96" s="8"/>
+      <c r="L96" s="1"/>
       <c r="M96" s="6"/>
     </row>
-    <row r="97" spans="1:13" ht="30">
+    <row r="97" spans="1:13" ht="15">
       <c r="A97">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B97">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C97" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>19-1</v>
+        <v>17-4</v>
       </c>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
@@ -6760,10 +6772,10 @@
         <v>62</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="J97" s="8"/>
       <c r="K97" s="7"/>
@@ -6775,11 +6787,11 @@
         <v>19</v>
       </c>
       <c r="B98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C98" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>19-2</v>
+        <v>19-1</v>
       </c>
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
@@ -6791,22 +6803,23 @@
         <v>192</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J98" s="8"/>
       <c r="K98" s="7"/>
-      <c r="L98" s="80"/>
+      <c r="L98" s="8"/>
+      <c r="M98" s="6"/>
     </row>
     <row r="99" spans="1:13" ht="30">
       <c r="A99">
         <v>19</v>
       </c>
       <c r="B99">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C99" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>19-3</v>
+        <v>19-2</v>
       </c>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
@@ -6818,23 +6831,22 @@
         <v>192</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J99" s="8"/>
       <c r="K99" s="7"/>
-      <c r="L99" s="81"/>
-      <c r="M99" s="6"/>
-    </row>
-    <row r="100" spans="1:13" ht="45">
+      <c r="L99" s="80"/>
+    </row>
+    <row r="100" spans="1:13" ht="30">
       <c r="A100">
         <v>19</v>
       </c>
       <c r="B100">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C100" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>19-4</v>
+        <v>19-3</v>
       </c>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
@@ -6846,23 +6858,23 @@
         <v>192</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J100" s="8"/>
       <c r="K100" s="7"/>
       <c r="L100" s="81"/>
       <c r="M100" s="6"/>
     </row>
-    <row r="101" spans="1:13" ht="30">
+    <row r="101" spans="1:13" ht="45">
       <c r="A101">
         <v>19</v>
       </c>
       <c r="B101">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C101" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>19-5</v>
+        <v>19-4</v>
       </c>
       <c r="D101" s="5"/>
       <c r="E101" s="5"/>
@@ -6874,51 +6886,51 @@
         <v>192</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J101" s="8"/>
       <c r="K101" s="7"/>
-      <c r="L101" s="82"/>
+      <c r="L101" s="81"/>
       <c r="M101" s="6"/>
     </row>
-    <row r="102" spans="1:13" ht="26.25">
+    <row r="102" spans="1:13" ht="30">
       <c r="A102">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B102">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C102" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-2</v>
-      </c>
-      <c r="D102" s="15"/>
-      <c r="E102" s="15"/>
-      <c r="F102" s="15"/>
-      <c r="G102" s="10" t="s">
+        <v>19-5</v>
+      </c>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H102" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I102" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="J102" s="12"/>
-      <c r="K102" s="10"/>
-      <c r="L102" s="12"/>
+      <c r="H102" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J102" s="8"/>
+      <c r="K102" s="7"/>
+      <c r="L102" s="82"/>
       <c r="M102" s="6"/>
     </row>
-    <row r="103" spans="1:13" ht="39">
+    <row r="103" spans="1:13" ht="26.25">
       <c r="A103">
         <v>21</v>
       </c>
       <c r="B103">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C103" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-3</v>
+        <v>21-2</v>
       </c>
       <c r="D103" s="15"/>
       <c r="E103" s="15"/>
@@ -6930,11 +6942,11 @@
         <v>15</v>
       </c>
       <c r="I103" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J103" s="12"/>
       <c r="K103" s="10"/>
-      <c r="L103" s="11"/>
+      <c r="L103" s="12"/>
       <c r="M103" s="6"/>
     </row>
     <row r="104" spans="1:13" ht="39">
@@ -6942,11 +6954,11 @@
         <v>21</v>
       </c>
       <c r="B104">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C104" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-4</v>
+        <v>21-3</v>
       </c>
       <c r="D104" s="15"/>
       <c r="E104" s="15"/>
@@ -6957,24 +6969,24 @@
       <c r="H104" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I104" s="12" t="s">
-        <v>203</v>
+      <c r="I104" s="11" t="s">
+        <v>202</v>
       </c>
       <c r="J104" s="12"/>
       <c r="K104" s="10"/>
-      <c r="L104" s="12"/>
+      <c r="L104" s="11"/>
       <c r="M104" s="6"/>
     </row>
-    <row r="105" spans="1:13" ht="51.75">
+    <row r="105" spans="1:13" ht="39">
       <c r="A105">
         <v>21</v>
       </c>
       <c r="B105">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C105" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-5</v>
+        <v>21-4</v>
       </c>
       <c r="D105" s="15"/>
       <c r="E105" s="15"/>
@@ -6986,37 +6998,39 @@
         <v>15</v>
       </c>
       <c r="I105" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J105" s="12"/>
       <c r="K105" s="10"/>
       <c r="L105" s="12"/>
       <c r="M105" s="6"/>
     </row>
-    <row r="106" spans="1:13" ht="26.25">
+    <row r="106" spans="1:13" ht="51.75">
       <c r="A106">
         <v>21</v>
       </c>
       <c r="B106">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C106" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-6</v>
-      </c>
-      <c r="D106" s="18"/>
-      <c r="E106" s="18"/>
-      <c r="F106" s="18"/>
-      <c r="G106" s="19"/>
-      <c r="H106" s="19" t="s">
+        <v>21-5</v>
+      </c>
+      <c r="D106" s="15"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="15"/>
+      <c r="G106" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H106" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I106" s="79" t="s">
-        <v>359</v>
-      </c>
-      <c r="J106" s="79"/>
-      <c r="K106" s="19"/>
-      <c r="L106" s="79"/>
+      <c r="I106" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="J106" s="12"/>
+      <c r="K106" s="10"/>
+      <c r="L106" s="12"/>
       <c r="M106" s="6"/>
     </row>
     <row r="107" spans="1:13" ht="26.25">
@@ -7024,11 +7038,11 @@
         <v>21</v>
       </c>
       <c r="B107">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C107" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-7</v>
+        <v>21-6</v>
       </c>
       <c r="D107" s="18"/>
       <c r="E107" s="18"/>
@@ -7038,7 +7052,7 @@
         <v>15</v>
       </c>
       <c r="I107" s="79" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J107" s="79"/>
       <c r="K107" s="19"/>
@@ -7050,11 +7064,11 @@
         <v>21</v>
       </c>
       <c r="B108">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C108" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-8</v>
+        <v>21-7</v>
       </c>
       <c r="D108" s="18"/>
       <c r="E108" s="18"/>
@@ -7063,40 +7077,38 @@
       <c r="H108" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I108" s="78" t="s">
-        <v>358</v>
-      </c>
-      <c r="J108" s="78"/>
+      <c r="I108" s="79" t="s">
+        <v>360</v>
+      </c>
+      <c r="J108" s="79"/>
       <c r="K108" s="19"/>
-      <c r="L108" s="78"/>
+      <c r="L108" s="79"/>
       <c r="M108" s="6"/>
     </row>
-    <row r="109" spans="1:13" ht="39">
+    <row r="109" spans="1:13" ht="26.25">
       <c r="A109">
         <v>21</v>
       </c>
       <c r="B109">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C109" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-26</v>
+        <v>21-8</v>
       </c>
       <c r="D109" s="18"/>
       <c r="E109" s="18"/>
       <c r="F109" s="18"/>
-      <c r="G109" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="G109" s="19"/>
       <c r="H109" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I109" s="42" t="s">
-        <v>295</v>
-      </c>
-      <c r="J109" s="42"/>
+      <c r="I109" s="78" t="s">
+        <v>358</v>
+      </c>
+      <c r="J109" s="78"/>
       <c r="K109" s="19"/>
-      <c r="L109" s="42"/>
+      <c r="L109" s="78"/>
       <c r="M109" s="6"/>
     </row>
     <row r="110" spans="1:13" ht="39">
@@ -7104,11 +7116,11 @@
         <v>21</v>
       </c>
       <c r="B110">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C110" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-27</v>
+        <v>21-26</v>
       </c>
       <c r="D110" s="18"/>
       <c r="E110" s="18"/>
@@ -7120,7 +7132,7 @@
         <v>15</v>
       </c>
       <c r="I110" s="42" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J110" s="42"/>
       <c r="K110" s="19"/>
@@ -7129,42 +7141,42 @@
     </row>
     <row r="111" spans="1:13" ht="39">
       <c r="A111">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B111">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C111" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>22-2</v>
-      </c>
-      <c r="D111" s="20"/>
-      <c r="E111" s="20"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="20" t="s">
+        <v>21-27</v>
+      </c>
+      <c r="D111" s="18"/>
+      <c r="E111" s="18"/>
+      <c r="F111" s="18"/>
+      <c r="G111" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H111" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="I111" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="J111" s="20"/>
+      <c r="H111" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I111" s="42" t="s">
+        <v>296</v>
+      </c>
+      <c r="J111" s="42"/>
       <c r="K111" s="19"/>
-      <c r="L111" s="23"/>
+      <c r="L111" s="42"/>
       <c r="M111" s="6"/>
     </row>
-    <row r="112" spans="1:13" ht="26.25">
+    <row r="112" spans="1:13" ht="39">
       <c r="A112">
         <v>22</v>
       </c>
       <c r="B112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C112" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>22-3</v>
+        <v>22-2</v>
       </c>
       <c r="D112" s="20"/>
       <c r="E112" s="20"/>
@@ -7176,23 +7188,23 @@
         <v>247</v>
       </c>
       <c r="I112" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J112" s="20"/>
       <c r="K112" s="19"/>
       <c r="L112" s="23"/>
       <c r="M112" s="6"/>
     </row>
-    <row r="113" spans="1:13" ht="39">
+    <row r="113" spans="1:13" ht="26.25">
       <c r="A113">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C113" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>26-1</v>
+        <v>22-3</v>
       </c>
       <c r="D113" s="20"/>
       <c r="E113" s="20"/>
@@ -7201,10 +7213,10 @@
         <v>62</v>
       </c>
       <c r="H113" s="21" t="s">
-        <v>292</v>
+        <v>247</v>
       </c>
       <c r="I113" s="22" t="s">
-        <v>293</v>
+        <v>249</v>
       </c>
       <c r="J113" s="20"/>
       <c r="K113" s="19"/>
@@ -7219,7 +7231,7 @@
         <v>1</v>
       </c>
       <c r="C114" s="3" t="str">
-        <f t="shared" ref="C114:C115" si="4">CONCATENATE(A114,"-",B114)</f>
+        <f t="shared" si="3"/>
         <v>26-1</v>
       </c>
       <c r="D114" s="20"/>
@@ -7239,46 +7251,44 @@
       <c r="L114" s="23"/>
       <c r="M114" s="6"/>
     </row>
-    <row r="115" spans="1:13" ht="64.5">
+    <row r="115" spans="1:13" ht="39">
       <c r="A115">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B115">
         <v>1</v>
       </c>
       <c r="C115" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>27-1</v>
+        <f t="shared" ref="C115:C116" si="4">CONCATENATE(A115,"-",B115)</f>
+        <v>26-1</v>
       </c>
       <c r="D115" s="20"/>
       <c r="E115" s="20"/>
-      <c r="F115" s="77" t="s">
-        <v>240</v>
-      </c>
+      <c r="F115" s="20"/>
       <c r="G115" s="20" t="s">
         <v>62</v>
       </c>
       <c r="H115" s="21" t="s">
-        <v>354</v>
+        <v>292</v>
       </c>
       <c r="I115" s="22" t="s">
-        <v>356</v>
+        <v>293</v>
       </c>
       <c r="J115" s="20"/>
       <c r="K115" s="19"/>
       <c r="L115" s="23"/>
       <c r="M115" s="6"/>
     </row>
-    <row r="116" spans="1:13" ht="15.75" customHeight="1">
+    <row r="116" spans="1:13" ht="64.5">
       <c r="A116">
         <v>27</v>
       </c>
       <c r="B116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C116" s="3" t="str">
-        <f t="shared" ref="C116" si="5">CONCATENATE(A116,"-",B116)</f>
-        <v>27-2</v>
+        <f t="shared" si="4"/>
+        <v>27-1</v>
       </c>
       <c r="D116" s="20"/>
       <c r="E116" s="20"/>
@@ -7292,22 +7302,23 @@
         <v>354</v>
       </c>
       <c r="I116" s="22" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="J116" s="20"/>
       <c r="K116" s="19"/>
       <c r="L116" s="23"/>
-    </row>
-    <row r="117" spans="1:13" ht="77.25">
+      <c r="M116" s="6"/>
+    </row>
+    <row r="117" spans="1:13" ht="15.75" customHeight="1">
       <c r="A117">
         <v>27</v>
       </c>
       <c r="B117">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C117" s="3" t="str">
-        <f>CONCATENATE(A117,"-",B117)</f>
-        <v>27-3</v>
+        <f t="shared" ref="C117" si="5">CONCATENATE(A117,"-",B117)</f>
+        <v>27-2</v>
       </c>
       <c r="D117" s="20"/>
       <c r="E117" s="20"/>
@@ -7321,23 +7332,22 @@
         <v>354</v>
       </c>
       <c r="I117" s="22" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J117" s="20"/>
       <c r="K117" s="19"/>
       <c r="L117" s="23"/>
-      <c r="M117" s="6"/>
-    </row>
-    <row r="118" spans="1:13" ht="15">
+    </row>
+    <row r="118" spans="1:13" ht="77.25">
       <c r="A118">
         <v>27</v>
       </c>
       <c r="B118">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C118" s="3" t="str">
         <f>CONCATENATE(A118,"-",B118)</f>
-        <v>27-4</v>
+        <v>27-3</v>
       </c>
       <c r="D118" s="20"/>
       <c r="E118" s="20"/>
@@ -7351,15 +7361,41 @@
         <v>354</v>
       </c>
       <c r="I118" s="22" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="J118" s="20"/>
       <c r="K118" s="19"/>
       <c r="L118" s="23"/>
       <c r="M118" s="6"/>
     </row>
-    <row r="119" spans="1:13" ht="12.75">
-      <c r="L119" s="6"/>
+    <row r="119" spans="1:13" ht="15">
+      <c r="A119">
+        <v>27</v>
+      </c>
+      <c r="B119">
+        <v>4</v>
+      </c>
+      <c r="C119" s="3" t="str">
+        <f>CONCATENATE(A119,"-",B119)</f>
+        <v>27-4</v>
+      </c>
+      <c r="D119" s="20"/>
+      <c r="E119" s="20"/>
+      <c r="F119" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G119" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H119" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I119" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="J119" s="20"/>
+      <c r="K119" s="19"/>
+      <c r="L119" s="23"/>
       <c r="M119" s="6"/>
     </row>
     <row r="120" spans="1:13" ht="12.75">
@@ -10082,29 +10118,33 @@
       <c r="L799" s="6"/>
       <c r="M799" s="6"/>
     </row>
+    <row r="800" spans="12:13" ht="12.75">
+      <c r="L800" s="6"/>
+      <c r="M800" s="6"/>
+    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" scale="115">
+    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" scale="115">
-      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
+    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" scale="115">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -10114,92 +10154,92 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" scale="115">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
     </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
     </customSheetView>
-    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" scale="115">
+      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
     </customSheetView>
-    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" scale="115">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
-    <mergeCell ref="L98:L101"/>
+    <mergeCell ref="L99:L102"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:K25 K27:K115 K117">
+  <conditionalFormatting sqref="K2:K26 K28:K116 K118">
     <cfRule type="containsBlanks" dxfId="11" priority="103">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K25 K27:K115 K117">
+  <conditionalFormatting sqref="K2:K26 K28:K116 K118">
     <cfRule type="containsText" dxfId="10" priority="104" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K25 K27:K115 K117">
+  <conditionalFormatting sqref="K2:K26 K28:K116 K118">
     <cfRule type="containsText" dxfId="9" priority="105" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="K27">
     <cfRule type="containsBlanks" dxfId="8" priority="7">
-      <formula>LEN(TRIM(K26))=0</formula>
+      <formula>LEN(TRIM(K27))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="K27">
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K26))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K27))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="K27">
     <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K26))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K27))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K116">
+  <conditionalFormatting sqref="K117">
     <cfRule type="containsBlanks" dxfId="5" priority="4">
-      <formula>LEN(TRIM(K116))=0</formula>
+      <formula>LEN(TRIM(K117))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K116">
+  <conditionalFormatting sqref="K117">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K116))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K117))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K116">
+  <conditionalFormatting sqref="K117">
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K116))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K117))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K118">
+  <conditionalFormatting sqref="K119">
     <cfRule type="containsBlanks" dxfId="2" priority="1">
-      <formula>LEN(TRIM(K118))=0</formula>
+      <formula>LEN(TRIM(K119))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K118">
+  <conditionalFormatting sqref="K119">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K118))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K119))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K118">
+  <conditionalFormatting sqref="K119">
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K118))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K119))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11561,7 +11601,37 @@
     <row r="45" spans="1:28" ht="38.25" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
+    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11571,37 +11641,7 @@
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13893,19 +13933,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" topLeftCell="A82">
-      <selection activeCell="F113" sqref="F113"/>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" topLeftCell="A4">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" topLeftCell="A13">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" topLeftCell="A43">
-      <selection activeCell="D85" sqref="D85"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" topLeftCell="A4">
       <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13913,12 +13945,20 @@
       <selection activeCell="A10" sqref="A10:XFD10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" topLeftCell="A4">
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
       <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" topLeftCell="A4">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" topLeftCell="A43">
+      <selection activeCell="D85" sqref="D85"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" topLeftCell="A13">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" topLeftCell="A82">
+      <selection activeCell="F113" sqref="F113"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -13935,25 +13975,25 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <customSheetViews>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Add plot_spectrum test to manual system tests
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Instrument\Dev\dev_manual\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Instrument\Docs\developers_manual\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,21 +20,21 @@
   </sheets>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Potter, Adrian (Tessella,RAL,ISIS) - Personal View" guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1014" activeSheetId="1"/>
+    <customWorkbookView name="Oram, Dominic (STFC,RAL,ISIS) - Personal View" guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="894" activeSheetId="1"/>
+    <customWorkbookView name="Holt, John (Tessella,RAL,ISIS) - Personal View" guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1186" activeSheetId="1"/>
+    <customWorkbookView name="Akeroyd, Freddie (STFC,RAL,ISIS) - Personal View" guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1667" windowHeight="917" activeSheetId="1"/>
+    <customWorkbookView name="David Keymer - Personal View" guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1789" windowHeight="772" activeSheetId="1"/>
+    <customWorkbookView name="Willemsen, Thomas (Tessella,RAL,ISIS) - Personal View" guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Clarke, Matt (STFC,RAL,ISIS) - Personal View" guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" mergeInterval="0" personalView="1" xWindow="75" yWindow="75" windowWidth="1707" windowHeight="1032" activeSheetId="1"/>
+    <customWorkbookView name="Kathryn Baker - Personal View" guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="1"/>
     <customWorkbookView name="Baker, Kathryn (STFC,RAL,ISIS) - Personal View" guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Kathryn Baker - Personal View" guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="1"/>
-    <customWorkbookView name="Clarke, Matt (STFC,RAL,ISIS) - Personal View" guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" mergeInterval="0" personalView="1" xWindow="75" yWindow="75" windowWidth="1707" windowHeight="1032" activeSheetId="1"/>
-    <customWorkbookView name="Willemsen, Thomas (Tessella,RAL,ISIS) - Personal View" guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="David Keymer - Personal View" guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1789" windowHeight="772" activeSheetId="1"/>
-    <customWorkbookView name="Akeroyd, Freddie (STFC,RAL,ISIS) - Personal View" guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1667" windowHeight="917" activeSheetId="1"/>
-    <customWorkbookView name="Holt, John (Tessella,RAL,ISIS) - Personal View" guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1186" activeSheetId="1"/>
-    <customWorkbookView name="Oram, Dominic (STFC,RAL,ISIS) - Personal View" guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="894" activeSheetId="1"/>
-    <customWorkbookView name="Potter, Adrian (Tessella,RAL,ISIS) - Personal View" guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1014" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="365">
   <si>
     <t>Test Number</t>
   </si>
@@ -1145,6 +1145,12 @@
   </si>
   <si>
     <t>Check that spectra plots appear. Check that you can change the Y axis type and that this is reflected in the graph's Y axis.</t>
+  </si>
+  <si>
+    <t>From a genie_python console (i.e. from the GUI) run `g.plot_spectrum(1)`</t>
+  </si>
+  <si>
+    <t>A matplotlib window should appear with a sensible plot (probably a flat line for a simulated instrument). No error message should appear in the scripting window</t>
   </si>
 </sst>
 </file>
@@ -1579,17 +1585,59 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -4015,8 +4063,8 @@
   <dimension ref="A1:M800"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J126" sqref="J126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4254,7 +4302,7 @@
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="83"/>
+      <c r="F8" s="80"/>
       <c r="G8" s="9" t="s">
         <v>361</v>
       </c>
@@ -6110,7 +6158,7 @@
       <c r="L73" s="16"/>
       <c r="M73" s="6"/>
     </row>
-    <row r="74" spans="1:13" ht="60">
+    <row r="74" spans="1:13" ht="45">
       <c r="A74">
         <v>15</v>
       </c>
@@ -6835,7 +6883,7 @@
       </c>
       <c r="J99" s="8"/>
       <c r="K99" s="7"/>
-      <c r="L99" s="80"/>
+      <c r="L99" s="81"/>
     </row>
     <row r="100" spans="1:13" ht="30">
       <c r="A100">
@@ -6862,7 +6910,7 @@
       </c>
       <c r="J100" s="8"/>
       <c r="K100" s="7"/>
-      <c r="L100" s="81"/>
+      <c r="L100" s="82"/>
       <c r="M100" s="6"/>
     </row>
     <row r="101" spans="1:13" ht="45">
@@ -6890,7 +6938,7 @@
       </c>
       <c r="J101" s="8"/>
       <c r="K101" s="7"/>
-      <c r="L101" s="81"/>
+      <c r="L101" s="82"/>
       <c r="M101" s="6"/>
     </row>
     <row r="102" spans="1:13" ht="30">
@@ -6918,7 +6966,7 @@
       </c>
       <c r="J102" s="8"/>
       <c r="K102" s="7"/>
-      <c r="L102" s="82"/>
+      <c r="L102" s="83"/>
       <c r="M102" s="6"/>
     </row>
     <row r="103" spans="1:13" ht="26.25">
@@ -7398,8 +7446,36 @@
       <c r="L119" s="23"/>
       <c r="M119" s="6"/>
     </row>
-    <row r="120" spans="1:13" ht="12.75">
-      <c r="L120" s="6"/>
+    <row r="120" spans="1:13" ht="51.75">
+      <c r="A120">
+        <v>27</v>
+      </c>
+      <c r="B120">
+        <v>5</v>
+      </c>
+      <c r="C120" s="3" t="str">
+        <f>CONCATENATE(A120,"-",B120)</f>
+        <v>27-5</v>
+      </c>
+      <c r="D120" s="20"/>
+      <c r="E120" s="20"/>
+      <c r="F120" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G120" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="H120" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I120" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="J120" s="43" t="s">
+        <v>364</v>
+      </c>
+      <c r="K120" s="19"/>
+      <c r="L120" s="23"/>
       <c r="M120" s="6"/>
     </row>
     <row r="121" spans="1:13" ht="12.75">
@@ -10124,27 +10200,27 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" scale="115">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" scale="115">
+      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" scale="115">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -10154,27 +10230,27 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" scale="115">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
     </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
     </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" scale="115">
-      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
+    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
     </customSheetView>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" scale="115">
+    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
     </customSheetView>
@@ -10183,63 +10259,78 @@
     <mergeCell ref="L99:L102"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K26 K28:K116 K118">
-    <cfRule type="containsBlanks" dxfId="11" priority="103">
+    <cfRule type="containsBlanks" dxfId="14" priority="106">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K26 K28:K116 K118">
-    <cfRule type="containsText" dxfId="10" priority="104" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="13" priority="107" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K26 K28:K116 K118">
-    <cfRule type="containsText" dxfId="9" priority="105" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="12" priority="108" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="containsBlanks" dxfId="8" priority="7">
+    <cfRule type="containsBlanks" dxfId="11" priority="10">
       <formula>LEN(TRIM(K27))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K27))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K117">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
+    <cfRule type="containsBlanks" dxfId="8" priority="7">
       <formula>LEN(TRIM(K117))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K117">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K117))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K117">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K117))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K119">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
       <formula>LEN(TRIM(K119))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K119">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K119))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K119">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K119))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K120">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(K120))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K120">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K120))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K120">
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K119))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K120))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11601,7 +11692,37 @@
     <row r="45" spans="1:28" ht="38.25" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11611,37 +11732,7 @@
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
+    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13933,11 +14024,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" topLeftCell="A4">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" topLeftCell="A82">
+      <selection activeCell="F113" sqref="F113"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" topLeftCell="A4">
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" topLeftCell="A13">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" topLeftCell="A43">
+      <selection activeCell="D85" sqref="D85"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
       <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13945,20 +14044,12 @@
       <selection activeCell="A10" sqref="A10:XFD10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" topLeftCell="A4">
       <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" topLeftCell="A43">
-      <selection activeCell="D85" sqref="D85"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" topLeftCell="A13">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" topLeftCell="A82">
-      <selection activeCell="F113" sqref="F113"/>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" topLeftCell="A4">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -13975,25 +14066,25 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <customSheetViews>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Add manual system tests for no tables paths
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -20,21 +20,21 @@
   </sheets>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Baker, Kathryn (STFC,RAL,ISIS) - Personal View" guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Kathryn Baker - Personal View" guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="1"/>
+    <customWorkbookView name="Clarke, Matt (STFC,RAL,ISIS) - Personal View" guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" mergeInterval="0" personalView="1" xWindow="75" yWindow="75" windowWidth="1707" windowHeight="1032" activeSheetId="1"/>
+    <customWorkbookView name="Willemsen, Thomas (Tessella,RAL,ISIS) - Personal View" guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="David Keymer - Personal View" guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1789" windowHeight="772" activeSheetId="1"/>
+    <customWorkbookView name="Akeroyd, Freddie (STFC,RAL,ISIS) - Personal View" guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1667" windowHeight="917" activeSheetId="1"/>
+    <customWorkbookView name="Holt, John (Tessella,RAL,ISIS) - Personal View" guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1186" activeSheetId="1"/>
+    <customWorkbookView name="Oram, Dominic (STFC,RAL,ISIS) - Personal View" guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="894" activeSheetId="1"/>
     <customWorkbookView name="Potter, Adrian (Tessella,RAL,ISIS) - Personal View" guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1014" activeSheetId="1"/>
-    <customWorkbookView name="Oram, Dominic (STFC,RAL,ISIS) - Personal View" guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="894" activeSheetId="1"/>
-    <customWorkbookView name="Holt, John (Tessella,RAL,ISIS) - Personal View" guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1186" activeSheetId="1"/>
-    <customWorkbookView name="Akeroyd, Freddie (STFC,RAL,ISIS) - Personal View" guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1667" windowHeight="917" activeSheetId="1"/>
-    <customWorkbookView name="David Keymer - Personal View" guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1789" windowHeight="772" activeSheetId="1"/>
-    <customWorkbookView name="Willemsen, Thomas (Tessella,RAL,ISIS) - Personal View" guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Clarke, Matt (STFC,RAL,ISIS) - Personal View" guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" mergeInterval="0" personalView="1" xWindow="75" yWindow="75" windowWidth="1707" windowHeight="1032" activeSheetId="1"/>
-    <customWorkbookView name="Kathryn Baker - Personal View" guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="1"/>
-    <customWorkbookView name="Baker, Kathryn (STFC,RAL,ISIS) - Personal View" guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="371">
   <si>
     <t>Test Number</t>
   </si>
@@ -1151,6 +1151,24 @@
   </si>
   <si>
     <t>A matplotlib window should appear with a sensible plot (probably a flat line for a simulated instrument). No error message should appear in the scripting window</t>
+  </si>
+  <si>
+    <t>When you have no TCB files in your settings then the error message in the TCB file dropdown points to the correct location to place files</t>
+  </si>
+  <si>
+    <t>As above for spectra tables</t>
+  </si>
+  <si>
+    <t>As above for wiring tables</t>
+  </si>
+  <si>
+    <t>As above for detector tables</t>
+  </si>
+  <si>
+    <t>As above for period files</t>
+  </si>
+  <si>
+    <t>Fixed at ticket 2825 for NDX machines</t>
   </si>
 </sst>
 </file>
@@ -1412,7 +1430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1591,6 +1609,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4060,11 +4087,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M800"/>
+  <dimension ref="A1:M805"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J126" sqref="J126"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4130,7 +4157,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f t="shared" ref="C2:C30" si="0">CONCATENATE(A2,"-",B2)</f>
+        <f t="shared" ref="C2:C35" si="0">CONCATENATE(A2,"-",B2)</f>
         <v>4-1</v>
       </c>
       <c r="D2" s="5"/>
@@ -4317,195 +4344,186 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13" ht="15">
+    <row r="9" spans="1:13" ht="60">
       <c r="A9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>7-2</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="G9" s="7" t="s">
+        <v>6-21</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>64</v>
+      <c r="H9" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>365</v>
       </c>
       <c r="J9" s="8"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="8"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="84" t="s">
+        <v>370</v>
+      </c>
       <c r="M9" s="6"/>
     </row>
     <row r="10" spans="1:13" ht="15">
       <c r="A10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>7-4</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7" t="s">
+        <v>6-22</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>66</v>
+      <c r="H10" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>367</v>
       </c>
       <c r="J10" s="8"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="8"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="85"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13" ht="45">
+    <row r="11" spans="1:13" ht="15">
       <c r="A11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>7-9</v>
+        <v>6-23</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>279</v>
-      </c>
+        <v>368</v>
+      </c>
+      <c r="J11" s="8"/>
       <c r="K11" s="9"/>
-      <c r="L11" s="8" t="s">
-        <v>285</v>
-      </c>
+      <c r="L11" s="85"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13" ht="45">
+    <row r="12" spans="1:13" ht="15">
       <c r="A12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>7-10</v>
+        <v>6-24</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>280</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="J12" s="8"/>
       <c r="K12" s="9"/>
-      <c r="L12" s="8" t="s">
-        <v>285</v>
-      </c>
+      <c r="L12" s="85"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13" ht="30">
+    <row r="13" spans="1:13" ht="15">
       <c r="A13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>7-11</v>
+        <v>6-25</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>281</v>
-      </c>
+        <v>369</v>
+      </c>
+      <c r="J13" s="8"/>
       <c r="K13" s="9"/>
-      <c r="L13" s="8" t="s">
-        <v>285</v>
-      </c>
+      <c r="L13" s="85"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" ht="15">
       <c r="A14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-1</v>
+        <v>7-2</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="9"/>
       <c r="G14" s="7" t="s">
         <v>62</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="8"/>
+      <c r="L14" s="86"/>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:13" ht="15">
       <c r="A15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-2</v>
+        <v>7-4</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -4514,98 +4532,110 @@
         <v>62</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="1"/>
+      <c r="L15" s="8"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:13" ht="15">
+    <row r="16" spans="1:13" ht="45">
       <c r="A16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-3</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J16" s="8"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="8"/>
+        <v>7-9</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16" s="8" t="s">
+        <v>285</v>
+      </c>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" ht="15">
+    <row r="17" spans="1:13" ht="45">
       <c r="A17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-4</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="1"/>
+        <v>7-10</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="8" t="s">
+        <v>285</v>
+      </c>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:13" ht="15">
+    <row r="18" spans="1:13" ht="30">
       <c r="A18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-5</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="8"/>
+        <v>7-11</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="K18" s="9"/>
+      <c r="L18" s="8" t="s">
+        <v>285</v>
+      </c>
       <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:13" ht="15">
@@ -4613,11 +4643,11 @@
         <v>8</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-6</v>
+        <v>8-1</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -4629,7 +4659,7 @@
         <v>70</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="7"/>
@@ -4641,11 +4671,11 @@
         <v>8</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-7</v>
+        <v>8-2</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -4657,7 +4687,7 @@
         <v>70</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="7"/>
@@ -4669,11 +4699,11 @@
         <v>8</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-8</v>
+        <v>8-3</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -4685,11 +4715,11 @@
         <v>70</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="7"/>
-      <c r="L21" s="1"/>
+      <c r="L21" s="8"/>
       <c r="M21" s="6"/>
     </row>
     <row r="22" spans="1:13" ht="15">
@@ -4697,11 +4727,11 @@
         <v>8</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-9</v>
+        <v>8-4</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -4713,11 +4743,11 @@
         <v>70</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="7"/>
-      <c r="L22" s="8"/>
+      <c r="L22" s="1"/>
       <c r="M22" s="6"/>
     </row>
     <row r="23" spans="1:13" ht="15">
@@ -4725,11 +4755,11 @@
         <v>8</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-10</v>
+        <v>8-5</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -4741,145 +4771,135 @@
         <v>70</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="1"/>
+      <c r="L23" s="8"/>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:13" ht="30">
+    <row r="24" spans="1:13" ht="15">
       <c r="A24">
         <v>8</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-12</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="G24" s="9" t="s">
+        <v>8-6</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I24" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="K24" s="9"/>
+      <c r="I24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J24" s="8"/>
+      <c r="K24" s="7"/>
       <c r="L24" s="8"/>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:13" ht="30">
+    <row r="25" spans="1:13" ht="15">
       <c r="A25">
         <v>8</v>
       </c>
       <c r="B25">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>8-14</v>
+        <v>8-7</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="7" t="s">
-        <v>81</v>
-      </c>
+      <c r="F25" s="7"/>
       <c r="G25" s="7" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="7"/>
-      <c r="L25" s="8"/>
+      <c r="L25" s="1"/>
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" ht="15">
       <c r="A26">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>13-1</v>
+        <v>8-8</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="64" t="s">
-        <v>62</v>
-      </c>
+      <c r="F26" s="7"/>
       <c r="G26" s="7" t="s">
         <v>62</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="7"/>
-      <c r="L26" s="8" t="s">
-        <v>352</v>
-      </c>
+      <c r="L26" s="1"/>
       <c r="M26" s="6"/>
     </row>
     <row r="27" spans="1:13" ht="15">
       <c r="A27">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" s="60" t="str">
+        <v>9</v>
+      </c>
+      <c r="C27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>13-2</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="64" t="s">
+        <v>8-9</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>316</v>
+      <c r="H27" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="J27" s="8"/>
-      <c r="K27" s="9"/>
-    </row>
-    <row r="28" spans="1:13" ht="30">
+      <c r="K27" s="7"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="6"/>
+    </row>
+    <row r="28" spans="1:13" ht="15">
       <c r="A28">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>15-1</v>
+        <v>8-10</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -4888,150 +4908,160 @@
         <v>62</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="J28" s="8"/>
       <c r="K28" s="7"/>
-      <c r="L28" s="8"/>
+      <c r="L28" s="1"/>
       <c r="M28" s="6"/>
     </row>
     <row r="29" spans="1:13" ht="30">
       <c r="A29">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>15-2</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7" t="s">
+        <v>8-12</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="G29" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H29" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="7"/>
+      <c r="H29" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="K29" s="9"/>
       <c r="L29" s="8"/>
       <c r="M29" s="6"/>
     </row>
     <row r="30" spans="1:13" ht="30">
       <c r="A30">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>15-3</v>
+        <v>8-14</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="G30" s="7" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="7"/>
       <c r="L30" s="8"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="1:13" ht="30">
+    <row r="31" spans="1:13" ht="15">
       <c r="A31">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C31" s="3" t="str">
-        <f t="shared" ref="C31:C62" si="1">CONCATENATE(A31,"-",B31)</f>
-        <v>15-4</v>
+        <f t="shared" si="0"/>
+        <v>13-1</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="9" t="s">
+      <c r="F31" s="64" t="s">
         <v>62</v>
       </c>
+      <c r="G31" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="H31" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="J31" s="8"/>
       <c r="K31" s="7"/>
-      <c r="L31" s="8"/>
+      <c r="L31" s="8" t="s">
+        <v>352</v>
+      </c>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="1:13" ht="30">
+    <row r="32" spans="1:13" ht="15">
       <c r="A32">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B32">
-        <v>5</v>
-      </c>
-      <c r="C32" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>15-5</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="C32" s="60" t="str">
+        <f t="shared" si="0"/>
+        <v>13-2</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="64" t="s">
+        <v>62</v>
+      </c>
       <c r="G32" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H32" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>113</v>
+      <c r="H32" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>316</v>
       </c>
       <c r="J32" s="8"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="6"/>
+      <c r="K32" s="9"/>
     </row>
     <row r="33" spans="1:13" ht="30">
       <c r="A33">
         <v>15</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C33" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>15-6</v>
+        <f t="shared" si="0"/>
+        <v>15-1</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="7" t="s">
         <v>62</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="7"/>
@@ -5043,23 +5073,23 @@
         <v>15</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C34" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>15-7</v>
+        <f t="shared" si="0"/>
+        <v>15-2</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="7" t="s">
         <v>62</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="7"/>
@@ -5071,39 +5101,39 @@
         <v>15</v>
       </c>
       <c r="B35">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C35" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>15-8</v>
+        <f t="shared" si="0"/>
+        <v>15-3</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="9" t="s">
+      <c r="G35" s="7" t="s">
         <v>62</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="7"/>
       <c r="L35" s="8"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="1:13" ht="45">
+    <row r="36" spans="1:13" ht="30">
       <c r="A36">
         <v>15</v>
       </c>
       <c r="B36">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C36" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>15-9</v>
+        <f t="shared" ref="C36:C67" si="1">CONCATENATE(A36,"-",B36)</f>
+        <v>15-4</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -5115,7 +5145,7 @@
         <v>108</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>273</v>
+        <v>112</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="7"/>
@@ -5127,11 +5157,11 @@
         <v>15</v>
       </c>
       <c r="B37">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-10</v>
+        <v>15-5</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -5143,107 +5173,107 @@
         <v>108</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="7"/>
       <c r="L37" s="8"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="1:13" ht="60">
+    <row r="38" spans="1:13" ht="30">
       <c r="A38">
         <v>15</v>
       </c>
       <c r="B38">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-11</v>
-      </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
+        <v>15-6</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H38" s="9" t="s">
+      <c r="H38" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I38" s="8" t="s">
-        <v>287</v>
+      <c r="I38" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="J38" s="8"/>
-      <c r="K38" s="9"/>
+      <c r="K38" s="7"/>
       <c r="L38" s="8"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="1:13" ht="60">
+    <row r="39" spans="1:13" ht="30">
       <c r="A39">
         <v>15</v>
       </c>
       <c r="B39">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C39" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-12</v>
-      </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
+        <v>15-7</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H39" s="9" t="s">
+      <c r="H39" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I39" s="8" t="s">
-        <v>286</v>
+      <c r="I39" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="J39" s="8"/>
-      <c r="K39" s="9"/>
+      <c r="K39" s="7"/>
       <c r="L39" s="8"/>
       <c r="M39" s="6"/>
     </row>
-    <row r="40" spans="1:13" ht="60">
+    <row r="40" spans="1:13" ht="30">
       <c r="A40">
         <v>15</v>
       </c>
       <c r="B40">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C40" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-13</v>
-      </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
+        <v>15-8</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="7"/>
       <c r="G40" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="H40" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I40" s="8" t="s">
-        <v>274</v>
+      <c r="I40" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="J40" s="8"/>
-      <c r="K40" s="9"/>
+      <c r="K40" s="7"/>
       <c r="L40" s="8"/>
       <c r="M40" s="6"/>
     </row>
-    <row r="41" spans="1:13" ht="30">
+    <row r="41" spans="1:13" ht="45">
       <c r="A41">
         <v>15</v>
       </c>
       <c r="B41">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C41" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-14</v>
+        <v>15-9</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -5255,7 +5285,7 @@
         <v>108</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>118</v>
+        <v>273</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="7"/>
@@ -5267,11 +5297,11 @@
         <v>15</v>
       </c>
       <c r="B42">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C42" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-15</v>
+        <v>15-10</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -5283,94 +5313,94 @@
         <v>108</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="7"/>
       <c r="L42" s="8"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="1:13" ht="30">
+    <row r="43" spans="1:13" ht="60">
       <c r="A43">
         <v>15</v>
       </c>
       <c r="B43">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C43" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-16</v>
-      </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="7"/>
+        <v>15-11</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
       <c r="G43" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H43" s="7" t="s">
+      <c r="H43" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="I43" s="1" t="s">
-        <v>120</v>
+      <c r="I43" s="8" t="s">
+        <v>287</v>
       </c>
       <c r="J43" s="8"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="1"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="8"/>
       <c r="M43" s="6"/>
     </row>
-    <row r="44" spans="1:13" ht="30">
+    <row r="44" spans="1:13" ht="60">
       <c r="A44">
         <v>15</v>
       </c>
       <c r="B44">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C44" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-17</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="7"/>
+        <v>15-12</v>
+      </c>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
       <c r="G44" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H44" s="7" t="s">
+      <c r="H44" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="I44" s="1" t="s">
-        <v>121</v>
+      <c r="I44" s="8" t="s">
+        <v>286</v>
       </c>
       <c r="J44" s="8"/>
-      <c r="K44" s="7"/>
+      <c r="K44" s="9"/>
       <c r="L44" s="8"/>
       <c r="M44" s="6"/>
     </row>
-    <row r="45" spans="1:13" ht="30">
+    <row r="45" spans="1:13" ht="60">
       <c r="A45">
         <v>15</v>
       </c>
       <c r="B45">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C45" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-18</v>
-      </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="7"/>
+        <v>15-13</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
       <c r="G45" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H45" s="7" t="s">
+      <c r="H45" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="I45" s="1" t="s">
-        <v>122</v>
+      <c r="I45" s="8" t="s">
+        <v>274</v>
       </c>
       <c r="J45" s="8"/>
-      <c r="K45" s="7"/>
+      <c r="K45" s="9"/>
       <c r="L45" s="8"/>
       <c r="M45" s="6"/>
     </row>
@@ -5379,11 +5409,11 @@
         <v>15</v>
       </c>
       <c r="B46">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C46" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-19</v>
+        <v>15-14</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -5395,23 +5425,23 @@
         <v>108</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="7"/>
       <c r="L46" s="8"/>
       <c r="M46" s="6"/>
     </row>
-    <row r="47" spans="1:13" ht="15">
+    <row r="47" spans="1:13" ht="30">
       <c r="A47">
         <v>15</v>
       </c>
       <c r="B47">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C47" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-20</v>
+        <v>15-15</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -5423,23 +5453,23 @@
         <v>108</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="7"/>
       <c r="L47" s="8"/>
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="1:13" ht="15">
+    <row r="48" spans="1:13" ht="30">
       <c r="A48">
         <v>15</v>
       </c>
       <c r="B48">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C48" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-21</v>
+        <v>15-16</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -5451,23 +5481,23 @@
         <v>108</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J48" s="8"/>
       <c r="K48" s="7"/>
-      <c r="L48" s="8"/>
+      <c r="L48" s="1"/>
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="1:13" ht="15">
+    <row r="49" spans="1:13" ht="30">
       <c r="A49">
         <v>15</v>
       </c>
       <c r="B49">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C49" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-22</v>
+        <v>15-17</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -5479,23 +5509,23 @@
         <v>108</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J49" s="8"/>
       <c r="K49" s="7"/>
       <c r="L49" s="8"/>
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="1:13" ht="15">
+    <row r="50" spans="1:13" ht="30">
       <c r="A50">
         <v>15</v>
       </c>
       <c r="B50">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C50" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-23</v>
+        <v>15-18</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -5507,23 +5537,23 @@
         <v>108</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J50" s="8"/>
       <c r="K50" s="7"/>
       <c r="L50" s="8"/>
       <c r="M50" s="6"/>
     </row>
-    <row r="51" spans="1:13" ht="15">
+    <row r="51" spans="1:13" ht="30">
       <c r="A51">
         <v>15</v>
       </c>
       <c r="B51">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C51" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-24</v>
+        <v>15-19</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -5535,7 +5565,7 @@
         <v>108</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J51" s="8"/>
       <c r="K51" s="7"/>
@@ -5547,11 +5577,11 @@
         <v>15</v>
       </c>
       <c r="B52">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C52" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-25</v>
+        <v>15-20</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
@@ -5563,7 +5593,7 @@
         <v>108</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="J52" s="8"/>
       <c r="K52" s="7"/>
@@ -5575,11 +5605,11 @@
         <v>15</v>
       </c>
       <c r="B53">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C53" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-26</v>
+        <v>15-21</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -5591,7 +5621,7 @@
         <v>108</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="7"/>
@@ -5603,11 +5633,11 @@
         <v>15</v>
       </c>
       <c r="B54">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C54" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-27</v>
+        <v>15-22</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
@@ -5619,7 +5649,7 @@
         <v>108</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="J54" s="8"/>
       <c r="K54" s="7"/>
@@ -5631,11 +5661,11 @@
         <v>15</v>
       </c>
       <c r="B55">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C55" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-28</v>
+        <v>15-23</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
@@ -5647,7 +5677,7 @@
         <v>108</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J55" s="8"/>
       <c r="K55" s="7"/>
@@ -5659,11 +5689,11 @@
         <v>15</v>
       </c>
       <c r="B56">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C56" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-29</v>
+        <v>15-24</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
@@ -5675,7 +5705,7 @@
         <v>108</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="J56" s="8"/>
       <c r="K56" s="7"/>
@@ -5687,11 +5717,11 @@
         <v>15</v>
       </c>
       <c r="B57">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C57" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-30</v>
+        <v>15-25</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
@@ -5703,7 +5733,7 @@
         <v>108</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J57" s="8"/>
       <c r="K57" s="7"/>
@@ -5715,11 +5745,11 @@
         <v>15</v>
       </c>
       <c r="B58">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C58" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-31</v>
+        <v>15-26</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
@@ -5731,7 +5761,7 @@
         <v>108</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J58" s="8"/>
       <c r="K58" s="7"/>
@@ -5743,11 +5773,11 @@
         <v>15</v>
       </c>
       <c r="B59">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C59" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-32</v>
+        <v>15-27</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
@@ -5759,38 +5789,38 @@
         <v>108</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J59" s="8"/>
       <c r="K59" s="7"/>
       <c r="L59" s="8"/>
       <c r="M59" s="6"/>
     </row>
-    <row r="60" spans="1:13" ht="30">
+    <row r="60" spans="1:13" ht="15">
       <c r="A60">
         <v>15</v>
       </c>
       <c r="B60">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C60" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-33</v>
-      </c>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
+        <v>15-28</v>
+      </c>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="7"/>
       <c r="G60" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H60" s="9" t="s">
+      <c r="H60" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I60" s="8" t="s">
-        <v>223</v>
+      <c r="I60" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="J60" s="8"/>
-      <c r="K60" s="9"/>
+      <c r="K60" s="7"/>
       <c r="L60" s="8"/>
       <c r="M60" s="6"/>
     </row>
@@ -5799,11 +5829,11 @@
         <v>15</v>
       </c>
       <c r="B61">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C61" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-34</v>
+        <v>15-29</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -5815,23 +5845,23 @@
         <v>108</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J61" s="8"/>
       <c r="K61" s="7"/>
       <c r="L61" s="8"/>
       <c r="M61" s="6"/>
     </row>
-    <row r="62" spans="1:13" ht="30">
+    <row r="62" spans="1:13" ht="15">
       <c r="A62">
         <v>15</v>
       </c>
       <c r="B62">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C62" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>15-35</v>
+        <v>15-30</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
@@ -5843,11 +5873,11 @@
         <v>108</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J62" s="8"/>
       <c r="K62" s="7"/>
-      <c r="L62" s="1"/>
+      <c r="L62" s="8"/>
       <c r="M62" s="6"/>
     </row>
     <row r="63" spans="1:13" ht="15">
@@ -5855,11 +5885,11 @@
         <v>15</v>
       </c>
       <c r="B63">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C63" s="3" t="str">
-        <f t="shared" ref="C63:C94" si="2">CONCATENATE(A63,"-",B63)</f>
-        <v>15-36</v>
+        <f t="shared" si="1"/>
+        <v>15-31</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
@@ -5871,23 +5901,23 @@
         <v>108</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J63" s="8"/>
       <c r="K63" s="7"/>
       <c r="L63" s="8"/>
       <c r="M63" s="6"/>
     </row>
-    <row r="64" spans="1:13" ht="30">
+    <row r="64" spans="1:13" ht="15">
       <c r="A64">
         <v>15</v>
       </c>
       <c r="B64">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C64" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>15-37</v>
+        <f t="shared" si="1"/>
+        <v>15-32</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
@@ -5899,7 +5929,7 @@
         <v>108</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J64" s="8"/>
       <c r="K64" s="7"/>
@@ -5911,26 +5941,26 @@
         <v>15</v>
       </c>
       <c r="B65">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C65" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>15-38</v>
-      </c>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="7"/>
+        <f t="shared" si="1"/>
+        <v>15-33</v>
+      </c>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
       <c r="G65" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H65" s="7" t="s">
+      <c r="H65" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="I65" s="1" t="s">
-        <v>141</v>
+      <c r="I65" s="8" t="s">
+        <v>223</v>
       </c>
       <c r="J65" s="8"/>
-      <c r="K65" s="7"/>
+      <c r="K65" s="9"/>
       <c r="L65" s="8"/>
       <c r="M65" s="6"/>
     </row>
@@ -5939,11 +5969,11 @@
         <v>15</v>
       </c>
       <c r="B66">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C66" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>15-41</v>
+        <f t="shared" si="1"/>
+        <v>15-34</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
@@ -5955,23 +5985,23 @@
         <v>108</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="7"/>
       <c r="L66" s="8"/>
       <c r="M66" s="6"/>
     </row>
-    <row r="67" spans="1:13" ht="15">
+    <row r="67" spans="1:13" ht="30">
       <c r="A67">
         <v>15</v>
       </c>
       <c r="B67">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C67" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>15-42</v>
+        <f t="shared" si="1"/>
+        <v>15-35</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
@@ -5983,11 +6013,11 @@
         <v>108</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="J67" s="8"/>
       <c r="K67" s="7"/>
-      <c r="L67" s="8"/>
+      <c r="L67" s="1"/>
       <c r="M67" s="6"/>
     </row>
     <row r="68" spans="1:13" ht="15">
@@ -5995,11 +6025,11 @@
         <v>15</v>
       </c>
       <c r="B68">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C68" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>15-45</v>
+        <f t="shared" ref="C68:C99" si="2">CONCATENATE(A68,"-",B68)</f>
+        <v>15-36</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
@@ -6011,23 +6041,23 @@
         <v>108</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J68" s="8"/>
       <c r="K68" s="7"/>
       <c r="L68" s="8"/>
       <c r="M68" s="6"/>
     </row>
-    <row r="69" spans="1:13" ht="15">
+    <row r="69" spans="1:13" ht="30">
       <c r="A69">
         <v>15</v>
       </c>
       <c r="B69">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C69" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-46</v>
+        <v>15-37</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
@@ -6039,23 +6069,23 @@
         <v>108</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="J69" s="8"/>
       <c r="K69" s="7"/>
       <c r="L69" s="8"/>
       <c r="M69" s="6"/>
     </row>
-    <row r="70" spans="1:13" ht="15">
+    <row r="70" spans="1:13" ht="30">
       <c r="A70">
         <v>15</v>
       </c>
       <c r="B70">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C70" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-47</v>
+        <v>15-38</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
@@ -6067,7 +6097,7 @@
         <v>108</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="7"/>
@@ -6079,11 +6109,11 @@
         <v>15</v>
       </c>
       <c r="B71">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C71" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-48</v>
+        <v>15-41</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
@@ -6095,7 +6125,7 @@
         <v>108</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="J71" s="8"/>
       <c r="K71" s="7"/>
@@ -6107,11 +6137,11 @@
         <v>15</v>
       </c>
       <c r="B72">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C72" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-49</v>
+        <v>15-42</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -6123,387 +6153,387 @@
         <v>108</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="J72" s="8"/>
       <c r="K72" s="7"/>
       <c r="L72" s="8"/>
       <c r="M72" s="6"/>
     </row>
-    <row r="73" spans="1:13" ht="30">
+    <row r="73" spans="1:13" ht="15">
       <c r="A73">
         <v>15</v>
       </c>
       <c r="B73">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C73" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-51</v>
+        <v>15-45</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="7"/>
-      <c r="G73" s="7" t="s">
+      <c r="G73" s="9" t="s">
         <v>62</v>
       </c>
       <c r="H73" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J73" s="8"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="16"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="8"/>
       <c r="M73" s="6"/>
     </row>
-    <row r="74" spans="1:13" ht="45">
+    <row r="74" spans="1:13" ht="15">
       <c r="A74">
         <v>15</v>
       </c>
       <c r="B74">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C74" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-52</v>
+        <v>15-46</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="7"/>
-      <c r="G74" s="7" t="s">
+      <c r="G74" s="9" t="s">
         <v>62</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>260</v>
+        <v>149</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="7"/>
       <c r="L74" s="8"/>
       <c r="M74" s="6"/>
     </row>
-    <row r="75" spans="1:13" ht="30">
+    <row r="75" spans="1:13" ht="15">
       <c r="A75">
         <v>15</v>
       </c>
       <c r="B75">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C75" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-53</v>
+        <v>15-47</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="7"/>
-      <c r="G75" s="7" t="s">
+      <c r="G75" s="9" t="s">
         <v>62</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="J75" s="8"/>
       <c r="K75" s="7"/>
-      <c r="L75" s="1"/>
+      <c r="L75" s="8"/>
       <c r="M75" s="6"/>
     </row>
-    <row r="76" spans="1:13" ht="50.25" customHeight="1">
+    <row r="76" spans="1:13" ht="15">
       <c r="A76">
         <v>15</v>
       </c>
       <c r="B76">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C76" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-56</v>
-      </c>
-      <c r="D76" s="39"/>
-      <c r="E76" s="39"/>
-      <c r="F76" s="39"/>
-      <c r="G76" s="39" t="s">
+        <v>15-48</v>
+      </c>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H76" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="I76" s="41" t="s">
-        <v>261</v>
-      </c>
-      <c r="J76" s="34"/>
-      <c r="K76" s="9"/>
+      <c r="H76" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J76" s="8"/>
+      <c r="K76" s="7"/>
       <c r="L76" s="8"/>
       <c r="M76" s="6"/>
     </row>
-    <row r="77" spans="1:13" ht="64.5">
+    <row r="77" spans="1:13" ht="15">
       <c r="A77">
         <v>15</v>
       </c>
       <c r="B77">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C77" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-57</v>
-      </c>
-      <c r="D77" s="39"/>
-      <c r="E77" s="39"/>
-      <c r="F77" s="39"/>
-      <c r="G77" s="39" t="s">
+        <v>15-49</v>
+      </c>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H77" s="39" t="s">
+      <c r="H77" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I77" s="41" t="s">
-        <v>288</v>
-      </c>
-      <c r="J77" s="34"/>
-      <c r="K77" s="9"/>
+      <c r="I77" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J77" s="8"/>
+      <c r="K77" s="7"/>
       <c r="L77" s="8"/>
       <c r="M77" s="6"/>
     </row>
-    <row r="78" spans="1:13" ht="64.5">
+    <row r="78" spans="1:13" ht="30">
       <c r="A78">
         <v>15</v>
       </c>
       <c r="B78">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C78" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-58</v>
-      </c>
-      <c r="D78" s="39"/>
-      <c r="E78" s="39"/>
-      <c r="F78" s="39"/>
-      <c r="G78" s="39" t="s">
+        <v>15-51</v>
+      </c>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H78" s="39" t="s">
+      <c r="H78" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I78" s="41" t="s">
-        <v>303</v>
-      </c>
-      <c r="J78" s="34"/>
-      <c r="K78" s="9"/>
-      <c r="L78" s="8"/>
+      <c r="I78" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J78" s="8"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="16"/>
       <c r="M78" s="6"/>
     </row>
-    <row r="79" spans="1:13" ht="64.5">
+    <row r="79" spans="1:13" ht="60">
       <c r="A79">
         <v>15</v>
       </c>
       <c r="B79">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C79" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-63</v>
-      </c>
-      <c r="D79" s="39"/>
-      <c r="E79" s="39"/>
-      <c r="F79" s="39"/>
-      <c r="G79" s="39" t="s">
+        <v>15-52</v>
+      </c>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H79" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="I79" s="41" t="s">
-        <v>340</v>
-      </c>
-      <c r="J79" s="34"/>
-      <c r="K79" s="9"/>
+      <c r="H79" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J79" s="8"/>
+      <c r="K79" s="7"/>
       <c r="L79" s="8"/>
       <c r="M79" s="6"/>
     </row>
-    <row r="80" spans="1:13" ht="64.5">
+    <row r="80" spans="1:13" ht="30">
       <c r="A80">
         <v>15</v>
       </c>
       <c r="B80">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C80" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>15-64</v>
-      </c>
-      <c r="D80" s="39"/>
-      <c r="E80" s="39"/>
-      <c r="F80" s="39"/>
-      <c r="G80" s="39" t="s">
+        <v>15-53</v>
+      </c>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H80" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="I80" s="41" t="s">
-        <v>346</v>
-      </c>
-      <c r="J80" s="34"/>
-      <c r="K80" s="9"/>
-      <c r="L80" s="8"/>
+      <c r="H80" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J80" s="8"/>
+      <c r="K80" s="7"/>
+      <c r="L80" s="1"/>
       <c r="M80" s="6"/>
     </row>
-    <row r="81" spans="1:13" ht="30">
+    <row r="81" spans="1:13" ht="50.25" customHeight="1">
       <c r="A81">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B81">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C81" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-9</v>
-      </c>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7" t="s">
+        <v>15-56</v>
+      </c>
+      <c r="D81" s="39"/>
+      <c r="E81" s="39"/>
+      <c r="F81" s="39"/>
+      <c r="G81" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H81" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="J81" s="8"/>
-      <c r="K81" s="7"/>
-      <c r="L81" s="1"/>
+      <c r="H81" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="I81" s="41" t="s">
+        <v>261</v>
+      </c>
+      <c r="J81" s="34"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="8"/>
       <c r="M81" s="6"/>
     </row>
-    <row r="82" spans="1:13" ht="45">
+    <row r="82" spans="1:13" ht="64.5">
       <c r="A82">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B82">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C82" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-10</v>
-      </c>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7" t="s">
+        <v>15-57</v>
+      </c>
+      <c r="D82" s="39"/>
+      <c r="E82" s="39"/>
+      <c r="F82" s="39"/>
+      <c r="G82" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H82" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="J82" s="8"/>
-      <c r="K82" s="7"/>
+      <c r="H82" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="I82" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="J82" s="34"/>
+      <c r="K82" s="9"/>
       <c r="L82" s="8"/>
       <c r="M82" s="6"/>
     </row>
-    <row r="83" spans="1:13" ht="30">
+    <row r="83" spans="1:13" ht="64.5">
       <c r="A83">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B83">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="C83" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-11</v>
-      </c>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="7"/>
-      <c r="G83" s="7" t="s">
+        <v>15-58</v>
+      </c>
+      <c r="D83" s="39"/>
+      <c r="E83" s="39"/>
+      <c r="F83" s="39"/>
+      <c r="G83" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H83" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J83" s="8"/>
-      <c r="K83" s="7"/>
+      <c r="H83" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="I83" s="41" t="s">
+        <v>303</v>
+      </c>
+      <c r="J83" s="34"/>
+      <c r="K83" s="9"/>
       <c r="L83" s="8"/>
       <c r="M83" s="6"/>
     </row>
-    <row r="84" spans="1:13" ht="45">
+    <row r="84" spans="1:13" ht="64.5">
       <c r="A84">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B84">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="C84" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-12</v>
-      </c>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="7"/>
-      <c r="G84" s="7" t="s">
+        <v>15-63</v>
+      </c>
+      <c r="D84" s="39"/>
+      <c r="E84" s="39"/>
+      <c r="F84" s="39"/>
+      <c r="G84" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H84" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I84" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J84" s="8"/>
-      <c r="K84" s="7"/>
+      <c r="H84" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="I84" s="41" t="s">
+        <v>340</v>
+      </c>
+      <c r="J84" s="34"/>
+      <c r="K84" s="9"/>
       <c r="L84" s="8"/>
       <c r="M84" s="6"/>
     </row>
-    <row r="85" spans="1:13" ht="45">
+    <row r="85" spans="1:13" ht="64.5">
       <c r="A85">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B85">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="C85" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-13</v>
-      </c>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="7"/>
-      <c r="G85" s="7" t="s">
+        <v>15-64</v>
+      </c>
+      <c r="D85" s="39"/>
+      <c r="E85" s="39"/>
+      <c r="F85" s="39"/>
+      <c r="G85" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H85" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="J85" s="8"/>
-      <c r="K85" s="7"/>
+      <c r="H85" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="I85" s="41" t="s">
+        <v>346</v>
+      </c>
+      <c r="J85" s="34"/>
+      <c r="K85" s="9"/>
       <c r="L85" s="8"/>
       <c r="M85" s="6"/>
     </row>
-    <row r="86" spans="1:13" ht="60">
+    <row r="86" spans="1:13" ht="30">
       <c r="A86">
         <v>16</v>
       </c>
       <c r="B86">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C86" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-14</v>
+        <v>16-9</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
@@ -6515,23 +6545,23 @@
         <v>97</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="J86" s="8"/>
       <c r="K86" s="7"/>
-      <c r="L86" s="8"/>
+      <c r="L86" s="1"/>
       <c r="M86" s="6"/>
     </row>
-    <row r="87" spans="1:13" ht="15">
+    <row r="87" spans="1:13" ht="45">
       <c r="A87">
         <v>16</v>
       </c>
       <c r="B87">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C87" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-15</v>
+        <v>16-10</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
@@ -6543,23 +6573,23 @@
         <v>97</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="J87" s="8"/>
       <c r="K87" s="7"/>
       <c r="L87" s="8"/>
       <c r="M87" s="6"/>
     </row>
-    <row r="88" spans="1:13" ht="15">
+    <row r="88" spans="1:13" ht="30">
       <c r="A88">
         <v>16</v>
       </c>
       <c r="B88">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C88" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-16</v>
+        <v>16-11</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
@@ -6571,79 +6601,79 @@
         <v>97</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="J88" s="8"/>
       <c r="K88" s="7"/>
       <c r="L88" s="8"/>
       <c r="M88" s="6"/>
     </row>
-    <row r="89" spans="1:13" ht="30">
+    <row r="89" spans="1:13" ht="45">
       <c r="A89">
         <v>16</v>
       </c>
       <c r="B89">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C89" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-18</v>
-      </c>
-      <c r="D89" s="9"/>
-      <c r="E89" s="9"/>
-      <c r="F89" s="9"/>
-      <c r="G89" s="9" t="s">
+        <v>16-12</v>
+      </c>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H89" s="9" t="s">
+      <c r="H89" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="I89" s="8" t="s">
-        <v>318</v>
+      <c r="I89" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="J89" s="8"/>
-      <c r="K89" s="9"/>
+      <c r="K89" s="7"/>
       <c r="L89" s="8"/>
       <c r="M89" s="6"/>
     </row>
-    <row r="90" spans="1:13" ht="30">
+    <row r="90" spans="1:13" ht="45">
       <c r="A90">
         <v>16</v>
       </c>
       <c r="B90">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C90" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-19</v>
-      </c>
-      <c r="D90" s="9"/>
-      <c r="E90" s="9"/>
-      <c r="F90" s="9"/>
-      <c r="G90" s="9" t="s">
+        <v>16-13</v>
+      </c>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H90" s="9" t="s">
+      <c r="H90" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="I90" s="8" t="s">
-        <v>312</v>
+      <c r="I90" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="J90" s="8"/>
-      <c r="K90" s="9"/>
+      <c r="K90" s="7"/>
       <c r="L90" s="8"/>
       <c r="M90" s="6"/>
     </row>
-    <row r="91" spans="1:13" ht="30">
+    <row r="91" spans="1:13" ht="60">
       <c r="A91">
         <v>16</v>
       </c>
       <c r="B91">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C91" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-21</v>
+        <v>16-14</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -6652,26 +6682,26 @@
         <v>62</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>178</v>
+        <v>97</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="J91" s="8"/>
       <c r="K91" s="7"/>
       <c r="L91" s="8"/>
       <c r="M91" s="6"/>
     </row>
-    <row r="92" spans="1:13" ht="30">
+    <row r="92" spans="1:13" ht="15">
       <c r="A92">
         <v>16</v>
       </c>
       <c r="B92">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C92" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-22</v>
+        <v>16-15</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -6680,10 +6710,10 @@
         <v>62</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>178</v>
+        <v>97</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="J92" s="8"/>
       <c r="K92" s="7"/>
@@ -6695,11 +6725,11 @@
         <v>16</v>
       </c>
       <c r="B93">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C93" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-23</v>
+        <v>16-16</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
@@ -6708,54 +6738,54 @@
         <v>62</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>178</v>
+        <v>97</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="J93" s="8"/>
       <c r="K93" s="7"/>
       <c r="L93" s="8"/>
       <c r="M93" s="6"/>
     </row>
-    <row r="94" spans="1:13" ht="15">
+    <row r="94" spans="1:13" ht="30">
       <c r="A94">
         <v>16</v>
       </c>
       <c r="B94">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C94" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-24</v>
-      </c>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7" t="s">
+        <v>16-18</v>
+      </c>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H94" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>182</v>
+      <c r="H94" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I94" s="8" t="s">
+        <v>318</v>
       </c>
       <c r="J94" s="8"/>
-      <c r="K94" s="7"/>
+      <c r="K94" s="9"/>
       <c r="L94" s="8"/>
       <c r="M94" s="6"/>
     </row>
-    <row r="95" spans="1:13" ht="60">
+    <row r="95" spans="1:13" ht="30">
       <c r="A95">
         <v>16</v>
       </c>
       <c r="B95">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C95" s="3" t="str">
-        <f t="shared" ref="C95:C114" si="3">CONCATENATE(A95,"-",B95)</f>
-        <v>16-25</v>
+        <f t="shared" si="2"/>
+        <v>16-19</v>
       </c>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
@@ -6764,10 +6794,10 @@
         <v>62</v>
       </c>
       <c r="H95" s="9" t="s">
-        <v>178</v>
+        <v>97</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="J95" s="8"/>
       <c r="K95" s="9"/>
@@ -6776,14 +6806,14 @@
     </row>
     <row r="96" spans="1:13" ht="30">
       <c r="A96">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B96">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C96" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>17-2</v>
+        <f t="shared" si="2"/>
+        <v>16-21</v>
       </c>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
@@ -6792,26 +6822,26 @@
         <v>62</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J96" s="8"/>
       <c r="K96" s="7"/>
-      <c r="L96" s="1"/>
+      <c r="L96" s="8"/>
       <c r="M96" s="6"/>
     </row>
-    <row r="97" spans="1:13" ht="15">
+    <row r="97" spans="1:13" ht="30">
       <c r="A97">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B97">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C97" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>17-4</v>
+        <f t="shared" si="2"/>
+        <v>16-22</v>
       </c>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
@@ -6820,26 +6850,26 @@
         <v>62</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="J97" s="8"/>
       <c r="K97" s="7"/>
       <c r="L97" s="8"/>
       <c r="M97" s="6"/>
     </row>
-    <row r="98" spans="1:13" ht="30">
+    <row r="98" spans="1:13" ht="15">
       <c r="A98">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C98" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>19-1</v>
+        <f t="shared" si="2"/>
+        <v>16-23</v>
       </c>
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
@@ -6848,26 +6878,26 @@
         <v>62</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="J98" s="8"/>
       <c r="K98" s="7"/>
       <c r="L98" s="8"/>
       <c r="M98" s="6"/>
     </row>
-    <row r="99" spans="1:13" ht="30">
+    <row r="99" spans="1:13" ht="15">
       <c r="A99">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B99">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C99" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>19-2</v>
+        <f t="shared" si="2"/>
+        <v>16-24</v>
       </c>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
@@ -6876,53 +6906,54 @@
         <v>62</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J99" s="8"/>
       <c r="K99" s="7"/>
-      <c r="L99" s="81"/>
-    </row>
-    <row r="100" spans="1:13" ht="30">
+      <c r="L99" s="8"/>
+      <c r="M99" s="6"/>
+    </row>
+    <row r="100" spans="1:13" ht="60">
       <c r="A100">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B100">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C100" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>19-3</v>
-      </c>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="7"/>
-      <c r="G100" s="7" t="s">
+        <f t="shared" ref="C100:C119" si="3">CONCATENATE(A100,"-",B100)</f>
+        <v>16-25</v>
+      </c>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H100" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>195</v>
+      <c r="H100" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="I100" s="8" t="s">
+        <v>291</v>
       </c>
       <c r="J100" s="8"/>
-      <c r="K100" s="7"/>
-      <c r="L100" s="82"/>
+      <c r="K100" s="9"/>
+      <c r="L100" s="8"/>
       <c r="M100" s="6"/>
     </row>
-    <row r="101" spans="1:13" ht="45">
+    <row r="101" spans="1:13" ht="30">
       <c r="A101">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B101">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C101" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>19-4</v>
+        <v>17-2</v>
       </c>
       <c r="D101" s="5"/>
       <c r="E101" s="5"/>
@@ -6931,26 +6962,26 @@
         <v>62</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="J101" s="8"/>
       <c r="K101" s="7"/>
-      <c r="L101" s="82"/>
+      <c r="L101" s="1"/>
       <c r="M101" s="6"/>
     </row>
-    <row r="102" spans="1:13" ht="30">
+    <row r="102" spans="1:13" ht="15">
       <c r="A102">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B102">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C102" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>19-5</v>
+        <v>17-4</v>
       </c>
       <c r="D102" s="5"/>
       <c r="E102" s="5"/>
@@ -6959,152 +6990,153 @@
         <v>62</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="J102" s="8"/>
       <c r="K102" s="7"/>
-      <c r="L102" s="83"/>
+      <c r="L102" s="8"/>
       <c r="M102" s="6"/>
     </row>
-    <row r="103" spans="1:13" ht="26.25">
+    <row r="103" spans="1:13" ht="30">
       <c r="A103">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C103" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-2</v>
-      </c>
-      <c r="D103" s="15"/>
-      <c r="E103" s="15"/>
-      <c r="F103" s="15"/>
-      <c r="G103" s="10" t="s">
+        <v>19-1</v>
+      </c>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H103" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I103" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="J103" s="12"/>
-      <c r="K103" s="10"/>
-      <c r="L103" s="12"/>
+      <c r="H103" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J103" s="8"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="8"/>
       <c r="M103" s="6"/>
     </row>
-    <row r="104" spans="1:13" ht="39">
+    <row r="104" spans="1:13" ht="30">
       <c r="A104">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B104">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C104" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-3</v>
-      </c>
-      <c r="D104" s="15"/>
-      <c r="E104" s="15"/>
-      <c r="F104" s="15"/>
-      <c r="G104" s="10" t="s">
+        <v>19-2</v>
+      </c>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="7"/>
+      <c r="G104" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H104" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I104" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="J104" s="12"/>
-      <c r="K104" s="10"/>
-      <c r="L104" s="11"/>
-      <c r="M104" s="6"/>
-    </row>
-    <row r="105" spans="1:13" ht="39">
+      <c r="H104" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J104" s="8"/>
+      <c r="K104" s="7"/>
+      <c r="L104" s="81"/>
+    </row>
+    <row r="105" spans="1:13" ht="30">
       <c r="A105">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B105">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C105" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-4</v>
-      </c>
-      <c r="D105" s="15"/>
-      <c r="E105" s="15"/>
-      <c r="F105" s="15"/>
-      <c r="G105" s="10" t="s">
+        <v>19-3</v>
+      </c>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="7"/>
+      <c r="G105" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H105" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I105" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="J105" s="12"/>
-      <c r="K105" s="10"/>
-      <c r="L105" s="12"/>
+      <c r="H105" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J105" s="8"/>
+      <c r="K105" s="7"/>
+      <c r="L105" s="82"/>
       <c r="M105" s="6"/>
     </row>
-    <row r="106" spans="1:13" ht="51.75">
+    <row r="106" spans="1:13" ht="45">
       <c r="A106">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B106">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C106" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-5</v>
-      </c>
-      <c r="D106" s="15"/>
-      <c r="E106" s="15"/>
-      <c r="F106" s="15"/>
-      <c r="G106" s="10" t="s">
+        <v>19-4</v>
+      </c>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="7"/>
+      <c r="G106" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H106" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I106" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="J106" s="12"/>
-      <c r="K106" s="10"/>
-      <c r="L106" s="12"/>
+      <c r="H106" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="J106" s="8"/>
+      <c r="K106" s="7"/>
+      <c r="L106" s="82"/>
       <c r="M106" s="6"/>
     </row>
-    <row r="107" spans="1:13" ht="26.25">
+    <row r="107" spans="1:13" ht="30">
       <c r="A107">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B107">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C107" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-6</v>
-      </c>
-      <c r="D107" s="18"/>
-      <c r="E107" s="18"/>
-      <c r="F107" s="18"/>
-      <c r="G107" s="19"/>
-      <c r="H107" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I107" s="79" t="s">
-        <v>359</v>
-      </c>
-      <c r="J107" s="79"/>
-      <c r="K107" s="19"/>
-      <c r="L107" s="79"/>
+        <v>19-5</v>
+      </c>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="7"/>
+      <c r="G107" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J107" s="8"/>
+      <c r="K107" s="7"/>
+      <c r="L107" s="83"/>
       <c r="M107" s="6"/>
     </row>
     <row r="108" spans="1:13" ht="26.25">
@@ -7112,51 +7144,55 @@
         <v>21</v>
       </c>
       <c r="B108">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C108" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-7</v>
-      </c>
-      <c r="D108" s="18"/>
-      <c r="E108" s="18"/>
-      <c r="F108" s="18"/>
-      <c r="G108" s="19"/>
-      <c r="H108" s="19" t="s">
+        <v>21-2</v>
+      </c>
+      <c r="D108" s="15"/>
+      <c r="E108" s="15"/>
+      <c r="F108" s="15"/>
+      <c r="G108" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H108" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I108" s="79" t="s">
-        <v>360</v>
-      </c>
-      <c r="J108" s="79"/>
-      <c r="K108" s="19"/>
-      <c r="L108" s="79"/>
+      <c r="I108" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="J108" s="12"/>
+      <c r="K108" s="10"/>
+      <c r="L108" s="12"/>
       <c r="M108" s="6"/>
     </row>
-    <row r="109" spans="1:13" ht="26.25">
+    <row r="109" spans="1:13" ht="39">
       <c r="A109">
         <v>21</v>
       </c>
       <c r="B109">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C109" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-8</v>
-      </c>
-      <c r="D109" s="18"/>
-      <c r="E109" s="18"/>
-      <c r="F109" s="18"/>
-      <c r="G109" s="19"/>
-      <c r="H109" s="19" t="s">
+        <v>21-3</v>
+      </c>
+      <c r="D109" s="15"/>
+      <c r="E109" s="15"/>
+      <c r="F109" s="15"/>
+      <c r="G109" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H109" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I109" s="78" t="s">
-        <v>358</v>
-      </c>
-      <c r="J109" s="78"/>
-      <c r="K109" s="19"/>
-      <c r="L109" s="78"/>
+      <c r="I109" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="J109" s="12"/>
+      <c r="K109" s="10"/>
+      <c r="L109" s="11"/>
       <c r="M109" s="6"/>
     </row>
     <row r="110" spans="1:13" ht="39">
@@ -7164,338 +7200,452 @@
         <v>21</v>
       </c>
       <c r="B110">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C110" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-26</v>
-      </c>
-      <c r="D110" s="18"/>
-      <c r="E110" s="18"/>
-      <c r="F110" s="18"/>
-      <c r="G110" s="19" t="s">
+        <v>21-4</v>
+      </c>
+      <c r="D110" s="15"/>
+      <c r="E110" s="15"/>
+      <c r="F110" s="15"/>
+      <c r="G110" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H110" s="19" t="s">
+      <c r="H110" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I110" s="42" t="s">
-        <v>295</v>
-      </c>
-      <c r="J110" s="42"/>
-      <c r="K110" s="19"/>
-      <c r="L110" s="42"/>
+      <c r="I110" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="J110" s="12"/>
+      <c r="K110" s="10"/>
+      <c r="L110" s="12"/>
       <c r="M110" s="6"/>
     </row>
-    <row r="111" spans="1:13" ht="39">
+    <row r="111" spans="1:13" ht="51.75">
       <c r="A111">
         <v>21</v>
       </c>
       <c r="B111">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C111" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-27</v>
-      </c>
-      <c r="D111" s="18"/>
-      <c r="E111" s="18"/>
-      <c r="F111" s="18"/>
-      <c r="G111" s="19" t="s">
+        <v>21-5</v>
+      </c>
+      <c r="D111" s="15"/>
+      <c r="E111" s="15"/>
+      <c r="F111" s="15"/>
+      <c r="G111" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H111" s="19" t="s">
+      <c r="H111" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I111" s="42" t="s">
-        <v>296</v>
-      </c>
-      <c r="J111" s="42"/>
-      <c r="K111" s="19"/>
-      <c r="L111" s="42"/>
+      <c r="I111" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="J111" s="12"/>
+      <c r="K111" s="10"/>
+      <c r="L111" s="12"/>
       <c r="M111" s="6"/>
     </row>
-    <row r="112" spans="1:13" ht="39">
+    <row r="112" spans="1:13" ht="26.25">
       <c r="A112">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B112">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C112" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>22-2</v>
-      </c>
-      <c r="D112" s="20"/>
-      <c r="E112" s="20"/>
-      <c r="F112" s="20"/>
-      <c r="G112" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H112" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="I112" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="J112" s="20"/>
+        <v>21-6</v>
+      </c>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="19"/>
+      <c r="H112" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I112" s="79" t="s">
+        <v>359</v>
+      </c>
+      <c r="J112" s="79"/>
       <c r="K112" s="19"/>
-      <c r="L112" s="23"/>
+      <c r="L112" s="79"/>
       <c r="M112" s="6"/>
     </row>
     <row r="113" spans="1:13" ht="26.25">
       <c r="A113">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C113" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>22-3</v>
-      </c>
-      <c r="D113" s="20"/>
-      <c r="E113" s="20"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H113" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="I113" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="J113" s="20"/>
+        <v>21-7</v>
+      </c>
+      <c r="D113" s="18"/>
+      <c r="E113" s="18"/>
+      <c r="F113" s="18"/>
+      <c r="G113" s="19"/>
+      <c r="H113" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I113" s="79" t="s">
+        <v>360</v>
+      </c>
+      <c r="J113" s="79"/>
       <c r="K113" s="19"/>
-      <c r="L113" s="23"/>
+      <c r="L113" s="79"/>
       <c r="M113" s="6"/>
     </row>
-    <row r="114" spans="1:13" ht="39">
+    <row r="114" spans="1:13" ht="26.25">
       <c r="A114">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C114" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>26-1</v>
-      </c>
-      <c r="D114" s="20"/>
-      <c r="E114" s="20"/>
-      <c r="F114" s="20"/>
-      <c r="G114" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H114" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="I114" s="22" t="s">
-        <v>293</v>
-      </c>
-      <c r="J114" s="20"/>
+        <v>21-8</v>
+      </c>
+      <c r="D114" s="18"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="19"/>
+      <c r="H114" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I114" s="78" t="s">
+        <v>358</v>
+      </c>
+      <c r="J114" s="78"/>
       <c r="K114" s="19"/>
-      <c r="L114" s="23"/>
+      <c r="L114" s="78"/>
       <c r="M114" s="6"/>
     </row>
     <row r="115" spans="1:13" ht="39">
       <c r="A115">
+        <v>21</v>
+      </c>
+      <c r="B115">
         <v>26</v>
       </c>
-      <c r="B115">
-        <v>1</v>
-      </c>
       <c r="C115" s="3" t="str">
-        <f t="shared" ref="C115:C116" si="4">CONCATENATE(A115,"-",B115)</f>
-        <v>26-1</v>
-      </c>
-      <c r="D115" s="20"/>
-      <c r="E115" s="20"/>
-      <c r="F115" s="20"/>
-      <c r="G115" s="20" t="s">
+        <f t="shared" si="3"/>
+        <v>21-26</v>
+      </c>
+      <c r="D115" s="18"/>
+      <c r="E115" s="18"/>
+      <c r="F115" s="18"/>
+      <c r="G115" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H115" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="I115" s="22" t="s">
-        <v>293</v>
-      </c>
-      <c r="J115" s="20"/>
+      <c r="H115" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I115" s="42" t="s">
+        <v>295</v>
+      </c>
+      <c r="J115" s="42"/>
       <c r="K115" s="19"/>
-      <c r="L115" s="23"/>
+      <c r="L115" s="42"/>
       <c r="M115" s="6"/>
     </row>
-    <row r="116" spans="1:13" ht="64.5">
+    <row r="116" spans="1:13" ht="39">
       <c r="A116">
+        <v>21</v>
+      </c>
+      <c r="B116">
         <v>27</v>
       </c>
-      <c r="B116">
-        <v>1</v>
-      </c>
       <c r="C116" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>27-1</v>
-      </c>
-      <c r="D116" s="20"/>
-      <c r="E116" s="20"/>
-      <c r="F116" s="77" t="s">
-        <v>240</v>
-      </c>
-      <c r="G116" s="20" t="s">
+        <f t="shared" si="3"/>
+        <v>21-27</v>
+      </c>
+      <c r="D116" s="18"/>
+      <c r="E116" s="18"/>
+      <c r="F116" s="18"/>
+      <c r="G116" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H116" s="21" t="s">
-        <v>354</v>
-      </c>
-      <c r="I116" s="22" t="s">
-        <v>356</v>
-      </c>
-      <c r="J116" s="20"/>
+      <c r="H116" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I116" s="42" t="s">
+        <v>296</v>
+      </c>
+      <c r="J116" s="42"/>
       <c r="K116" s="19"/>
-      <c r="L116" s="23"/>
+      <c r="L116" s="42"/>
       <c r="M116" s="6"/>
     </row>
-    <row r="117" spans="1:13" ht="15.75" customHeight="1">
+    <row r="117" spans="1:13" ht="39">
       <c r="A117">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B117">
         <v>2</v>
       </c>
       <c r="C117" s="3" t="str">
-        <f t="shared" ref="C117" si="5">CONCATENATE(A117,"-",B117)</f>
-        <v>27-2</v>
+        <f t="shared" si="3"/>
+        <v>22-2</v>
       </c>
       <c r="D117" s="20"/>
       <c r="E117" s="20"/>
-      <c r="F117" s="77" t="s">
-        <v>240</v>
-      </c>
+      <c r="F117" s="20"/>
       <c r="G117" s="20" t="s">
         <v>62</v>
       </c>
       <c r="H117" s="21" t="s">
-        <v>354</v>
+        <v>247</v>
       </c>
       <c r="I117" s="22" t="s">
-        <v>355</v>
+        <v>248</v>
       </c>
       <c r="J117" s="20"/>
       <c r="K117" s="19"/>
       <c r="L117" s="23"/>
-    </row>
-    <row r="118" spans="1:13" ht="77.25">
+      <c r="M117" s="6"/>
+    </row>
+    <row r="118" spans="1:13" ht="26.25">
       <c r="A118">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B118">
         <v>3</v>
       </c>
       <c r="C118" s="3" t="str">
-        <f>CONCATENATE(A118,"-",B118)</f>
-        <v>27-3</v>
+        <f t="shared" si="3"/>
+        <v>22-3</v>
       </c>
       <c r="D118" s="20"/>
       <c r="E118" s="20"/>
-      <c r="F118" s="77" t="s">
-        <v>240</v>
-      </c>
+      <c r="F118" s="20"/>
       <c r="G118" s="20" t="s">
         <v>62</v>
       </c>
       <c r="H118" s="21" t="s">
-        <v>354</v>
+        <v>247</v>
       </c>
       <c r="I118" s="22" t="s">
-        <v>357</v>
+        <v>249</v>
       </c>
       <c r="J118" s="20"/>
       <c r="K118" s="19"/>
       <c r="L118" s="23"/>
       <c r="M118" s="6"/>
     </row>
-    <row r="119" spans="1:13" ht="15">
+    <row r="119" spans="1:13" ht="39">
       <c r="A119">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B119">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C119" s="3" t="str">
-        <f>CONCATENATE(A119,"-",B119)</f>
-        <v>27-4</v>
+        <f t="shared" si="3"/>
+        <v>26-1</v>
       </c>
       <c r="D119" s="20"/>
       <c r="E119" s="20"/>
-      <c r="F119" s="77" t="s">
-        <v>240</v>
-      </c>
+      <c r="F119" s="20"/>
       <c r="G119" s="20" t="s">
         <v>62</v>
       </c>
       <c r="H119" s="21" t="s">
-        <v>354</v>
+        <v>292</v>
       </c>
       <c r="I119" s="22" t="s">
-        <v>355</v>
+        <v>293</v>
       </c>
       <c r="J119" s="20"/>
       <c r="K119" s="19"/>
       <c r="L119" s="23"/>
       <c r="M119" s="6"/>
     </row>
-    <row r="120" spans="1:13" ht="51.75">
+    <row r="120" spans="1:13" ht="39">
       <c r="A120">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B120">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C120" s="3" t="str">
-        <f>CONCATENATE(A120,"-",B120)</f>
-        <v>27-5</v>
+        <f t="shared" ref="C120:C121" si="4">CONCATENATE(A120,"-",B120)</f>
+        <v>26-1</v>
       </c>
       <c r="D120" s="20"/>
       <c r="E120" s="20"/>
-      <c r="F120" s="77" t="s">
-        <v>240</v>
-      </c>
+      <c r="F120" s="20"/>
       <c r="G120" s="20" t="s">
-        <v>240</v>
+        <v>62</v>
       </c>
       <c r="H120" s="21" t="s">
-        <v>354</v>
+        <v>292</v>
       </c>
       <c r="I120" s="22" t="s">
-        <v>363</v>
-      </c>
-      <c r="J120" s="43" t="s">
-        <v>364</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="J120" s="20"/>
       <c r="K120" s="19"/>
       <c r="L120" s="23"/>
       <c r="M120" s="6"/>
     </row>
-    <row r="121" spans="1:13" ht="12.75">
-      <c r="L121" s="6"/>
+    <row r="121" spans="1:13" ht="64.5">
+      <c r="A121">
+        <v>27</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+      <c r="C121" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>27-1</v>
+      </c>
+      <c r="D121" s="20"/>
+      <c r="E121" s="20"/>
+      <c r="F121" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G121" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H121" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I121" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="J121" s="20"/>
+      <c r="K121" s="19"/>
+      <c r="L121" s="23"/>
       <c r="M121" s="6"/>
     </row>
-    <row r="122" spans="1:13" ht="12.75">
-      <c r="L122" s="6"/>
-      <c r="M122" s="6"/>
-    </row>
-    <row r="123" spans="1:13" ht="12.75">
-      <c r="L123" s="6"/>
+    <row r="122" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A122">
+        <v>27</v>
+      </c>
+      <c r="B122">
+        <v>2</v>
+      </c>
+      <c r="C122" s="3" t="str">
+        <f t="shared" ref="C122" si="5">CONCATENATE(A122,"-",B122)</f>
+        <v>27-2</v>
+      </c>
+      <c r="D122" s="20"/>
+      <c r="E122" s="20"/>
+      <c r="F122" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G122" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H122" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I122" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="J122" s="20"/>
+      <c r="K122" s="19"/>
+      <c r="L122" s="23"/>
+    </row>
+    <row r="123" spans="1:13" ht="77.25">
+      <c r="A123">
+        <v>27</v>
+      </c>
+      <c r="B123">
+        <v>3</v>
+      </c>
+      <c r="C123" s="3" t="str">
+        <f>CONCATENATE(A123,"-",B123)</f>
+        <v>27-3</v>
+      </c>
+      <c r="D123" s="20"/>
+      <c r="E123" s="20"/>
+      <c r="F123" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G123" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H123" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I123" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="J123" s="20"/>
+      <c r="K123" s="19"/>
+      <c r="L123" s="23"/>
       <c r="M123" s="6"/>
     </row>
-    <row r="124" spans="1:13" ht="12.75">
-      <c r="L124" s="6"/>
+    <row r="124" spans="1:13" ht="15">
+      <c r="A124">
+        <v>27</v>
+      </c>
+      <c r="B124">
+        <v>4</v>
+      </c>
+      <c r="C124" s="3" t="str">
+        <f>CONCATENATE(A124,"-",B124)</f>
+        <v>27-4</v>
+      </c>
+      <c r="D124" s="20"/>
+      <c r="E124" s="20"/>
+      <c r="F124" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G124" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H124" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I124" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="J124" s="20"/>
+      <c r="K124" s="19"/>
+      <c r="L124" s="23"/>
       <c r="M124" s="6"/>
     </row>
-    <row r="125" spans="1:13" ht="12.75">
-      <c r="L125" s="6"/>
+    <row r="125" spans="1:13" ht="51.75">
+      <c r="A125">
+        <v>27</v>
+      </c>
+      <c r="B125">
+        <v>5</v>
+      </c>
+      <c r="C125" s="3" t="str">
+        <f>CONCATENATE(A125,"-",B125)</f>
+        <v>27-5</v>
+      </c>
+      <c r="D125" s="20"/>
+      <c r="E125" s="20"/>
+      <c r="F125" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G125" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="H125" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I125" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="J125" s="43" t="s">
+        <v>364</v>
+      </c>
+      <c r="K125" s="19"/>
+      <c r="L125" s="23"/>
       <c r="M125" s="6"/>
     </row>
     <row r="126" spans="1:13" ht="12.75">
@@ -10198,29 +10348,49 @@
       <c r="L800" s="6"/>
       <c r="M800" s="6"/>
     </row>
+    <row r="801" spans="12:13" ht="12.75">
+      <c r="L801" s="6"/>
+      <c r="M801" s="6"/>
+    </row>
+    <row r="802" spans="12:13" ht="12.75">
+      <c r="L802" s="6"/>
+      <c r="M802" s="6"/>
+    </row>
+    <row r="803" spans="12:13" ht="12.75">
+      <c r="L803" s="6"/>
+      <c r="M803" s="6"/>
+    </row>
+    <row r="804" spans="12:13" ht="12.75">
+      <c r="L804" s="6"/>
+      <c r="M804" s="6"/>
+    </row>
+    <row r="805" spans="12:13" ht="12.75">
+      <c r="L805" s="6"/>
+      <c r="M805" s="6"/>
+    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" scale="115">
+    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" scale="115">
-      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
+    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" scale="115">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -10230,107 +10400,108 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" scale="115">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
     </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
     </customSheetView>
-    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" scale="115">
+      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
     </customSheetView>
-    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" scale="115">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="1">
-    <mergeCell ref="L99:L102"/>
+  <mergeCells count="2">
+    <mergeCell ref="L104:L107"/>
+    <mergeCell ref="L9:L14"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:K26 K28:K116 K118">
+  <conditionalFormatting sqref="K2:K31 K33:K121 K123">
     <cfRule type="containsBlanks" dxfId="14" priority="106">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K26 K28:K116 K118">
+  <conditionalFormatting sqref="K2:K31 K33:K121 K123">
     <cfRule type="containsText" dxfId="13" priority="107" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K26 K28:K116 K118">
+  <conditionalFormatting sqref="K2:K31 K33:K121 K123">
     <cfRule type="containsText" dxfId="12" priority="108" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
+  <conditionalFormatting sqref="K32">
     <cfRule type="containsBlanks" dxfId="11" priority="10">
-      <formula>LEN(TRIM(K27))=0</formula>
+      <formula>LEN(TRIM(K32))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
+  <conditionalFormatting sqref="K32">
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K27))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K32))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
+  <conditionalFormatting sqref="K32">
     <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K27))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K32))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K117">
+  <conditionalFormatting sqref="K122">
     <cfRule type="containsBlanks" dxfId="8" priority="7">
-      <formula>LEN(TRIM(K117))=0</formula>
+      <formula>LEN(TRIM(K122))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K117">
+  <conditionalFormatting sqref="K122">
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K117))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K122))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K117">
+  <conditionalFormatting sqref="K122">
     <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K117))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K122))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K119">
+  <conditionalFormatting sqref="K124">
     <cfRule type="containsBlanks" dxfId="5" priority="4">
-      <formula>LEN(TRIM(K119))=0</formula>
+      <formula>LEN(TRIM(K124))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K119">
+  <conditionalFormatting sqref="K124">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K119))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K124))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K119">
+  <conditionalFormatting sqref="K124">
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K119))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K124))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K120">
+  <conditionalFormatting sqref="K125">
     <cfRule type="containsBlanks" dxfId="2" priority="1">
-      <formula>LEN(TRIM(K120))=0</formula>
+      <formula>LEN(TRIM(K125))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K120">
+  <conditionalFormatting sqref="K125">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K120))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K125))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K120">
+  <conditionalFormatting sqref="K125">
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K120))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K125))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11692,7 +11863,37 @@
     <row r="45" spans="1:28" ht="38.25" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
+    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11702,37 +11903,7 @@
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14024,19 +14195,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" topLeftCell="A82">
-      <selection activeCell="F113" sqref="F113"/>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" topLeftCell="A4">
+      <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" topLeftCell="A13">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" topLeftCell="A43">
-      <selection activeCell="D85" sqref="D85"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" topLeftCell="A4">
       <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -14044,12 +14207,20 @@
       <selection activeCell="A10" sqref="A10:XFD10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" topLeftCell="A4">
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
       <selection activeCell="F24" sqref="F24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" topLeftCell="A4">
-      <selection activeCell="F24" sqref="F24"/>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" topLeftCell="A43">
+      <selection activeCell="D85" sqref="D85"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" topLeftCell="A13">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" topLeftCell="A82">
+      <selection activeCell="F113" sqref="F113"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -14066,25 +14237,25 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <customSheetViews>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Manual system tests for Ticket #2527
</commit_message>
<xml_diff>
--- a/testing/manual_system_tests_template.xlsx
+++ b/testing/manual_system_tests_template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Instrument\Docs\developers_manual\testing\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21885" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28005" windowHeight="14610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cannot be automated tests" sheetId="5" r:id="rId1"/>
@@ -18,23 +13,23 @@
     <sheet name="Automated" sheetId="3" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Baker, Kathryn (STFC,RAL,ISIS) - Personal View" guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Kathryn Baker - Personal View" guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="1"/>
+    <customWorkbookView name="Clarke, Matt (STFC,RAL,ISIS) - Personal View" guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" mergeInterval="0" personalView="1" xWindow="75" yWindow="75" windowWidth="1707" windowHeight="1032" activeSheetId="1"/>
+    <customWorkbookView name="Willemsen, Thomas (Tessella,RAL,ISIS) - Personal View" guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="David Keymer - Personal View" guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1789" windowHeight="772" activeSheetId="1"/>
+    <customWorkbookView name="Akeroyd, Freddie (STFC,RAL,ISIS) - Personal View" guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1667" windowHeight="917" activeSheetId="1"/>
+    <customWorkbookView name="Holt, John (Tessella,RAL,ISIS) - Personal View" guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1186" activeSheetId="1"/>
+    <customWorkbookView name="Oram, Dominic (STFC,RAL,ISIS) - Personal View" guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="894" activeSheetId="1"/>
     <customWorkbookView name="Potter, Adrian (Tessella,RAL,ISIS) - Personal View" guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="1014" activeSheetId="1"/>
-    <customWorkbookView name="Oram, Dominic (STFC,RAL,ISIS) - Personal View" guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="894" activeSheetId="1"/>
-    <customWorkbookView name="Holt, John (Tessella,RAL,ISIS) - Personal View" guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1186" activeSheetId="1"/>
-    <customWorkbookView name="Akeroyd, Freddie (STFC,RAL,ISIS) - Personal View" guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1667" windowHeight="917" activeSheetId="1"/>
-    <customWorkbookView name="David Keymer - Personal View" guid="{7D900B46-42CB-4AD7-89CF-8A6BDE7583C7}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1789" windowHeight="772" activeSheetId="1"/>
-    <customWorkbookView name="Willemsen, Thomas (Tessella,RAL,ISIS) - Personal View" guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Clarke, Matt (STFC,RAL,ISIS) - Personal View" guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}" mergeInterval="0" personalView="1" xWindow="75" yWindow="75" windowWidth="1707" windowHeight="1032" activeSheetId="1"/>
-    <customWorkbookView name="Kathryn Baker - Personal View" guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="975" activeSheetId="1"/>
-    <customWorkbookView name="Baker, Kathryn (STFC,RAL,ISIS) - Personal View" guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="382">
   <si>
     <t>Test Number</t>
   </si>
@@ -1194,11 +1189,23 @@
   <si>
     <t>Create a block called [PVPREFIX]:DAE:TITLE:DISPLAY. Check its value when the "Show DAE title on web dashboard" box is ticked/unticked in the DAE run summary</t>
   </si>
+  <si>
+    <t>Create a configuration. 
+Set a default synoptic and save
+Verify the previously selected synoptic is set as this configuration's default synoptic. 
+Verify this works when the default synoptic of the configuration being edited is different from the default synoptic in the currently active configuration</t>
+  </si>
+  <si>
+    <t>Open the Synoptic perspective. Verify the synoptic selected in the drop down menu by default is the current configuration's default synoptic</t>
+  </si>
+  <si>
+    <t>In the synoptic perspective, verify that pushing the "Load Default" button selects the current configurations default synoptic in the adjacent drop down menu.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11">
     <font>
       <sz val="10"/>
@@ -1628,17 +1635,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1663,6 +1659,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2060,7 +2067,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2095,7 +2102,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4258,11 +4265,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M806"/>
+  <dimension ref="A1:M809"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I105" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4540,7 +4547,7 @@
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="84" t="s">
+      <c r="L9" s="89" t="s">
         <v>370</v>
       </c>
       <c r="M9" s="6"/>
@@ -4570,7 +4577,7 @@
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="9"/>
-      <c r="L10" s="85"/>
+      <c r="L10" s="90"/>
       <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:13" ht="15">
@@ -4598,7 +4605,7 @@
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="9"/>
-      <c r="L11" s="85"/>
+      <c r="L11" s="90"/>
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" ht="15">
@@ -4626,7 +4633,7 @@
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="9"/>
-      <c r="L12" s="85"/>
+      <c r="L12" s="90"/>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" ht="15">
@@ -4654,7 +4661,7 @@
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="9"/>
-      <c r="L13" s="85"/>
+      <c r="L13" s="90"/>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" ht="60">
@@ -6231,7 +6238,7 @@
         <v>36</v>
       </c>
       <c r="C69" s="3" t="str">
-        <f t="shared" ref="C69:C100" si="2">CONCATENATE(A69,"-",B69)</f>
+        <f t="shared" ref="C69:C101" si="2">CONCATENATE(A69,"-",B69)</f>
         <v>15-36</v>
       </c>
       <c r="D69" s="5"/>
@@ -6727,44 +6734,44 @@
       <c r="L86" s="8"/>
       <c r="M86" s="6"/>
     </row>
-    <row r="87" spans="1:13" ht="30">
+    <row r="87" spans="1:13" ht="102.75">
       <c r="A87">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B87">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="C87" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-9</v>
-      </c>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="7"/>
-      <c r="G87" s="7" t="s">
+        <v>15-65</v>
+      </c>
+      <c r="D87" s="39"/>
+      <c r="E87" s="39"/>
+      <c r="F87" s="39"/>
+      <c r="G87" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H87" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="J87" s="8"/>
-      <c r="K87" s="7"/>
-      <c r="L87" s="1"/>
+      <c r="H87" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="I87" s="41" t="s">
+        <v>379</v>
+      </c>
+      <c r="J87" s="34"/>
+      <c r="K87" s="9"/>
+      <c r="L87" s="8"/>
       <c r="M87" s="6"/>
     </row>
-    <row r="88" spans="1:13" ht="45">
+    <row r="88" spans="1:13" ht="30">
       <c r="A88">
         <v>16</v>
       </c>
       <c r="B88">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C88" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-10</v>
+        <v>16-9</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
@@ -6776,23 +6783,23 @@
         <v>97</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J88" s="8"/>
       <c r="K88" s="7"/>
-      <c r="L88" s="8"/>
+      <c r="L88" s="1"/>
       <c r="M88" s="6"/>
     </row>
-    <row r="89" spans="1:13" ht="30">
+    <row r="89" spans="1:13" ht="45">
       <c r="A89">
         <v>16</v>
       </c>
       <c r="B89">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C89" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-11</v>
+        <v>16-10</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
@@ -6804,23 +6811,23 @@
         <v>97</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J89" s="8"/>
       <c r="K89" s="7"/>
       <c r="L89" s="8"/>
       <c r="M89" s="6"/>
     </row>
-    <row r="90" spans="1:13" ht="45">
+    <row r="90" spans="1:13" ht="30">
       <c r="A90">
         <v>16</v>
       </c>
       <c r="B90">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C90" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-12</v>
+        <v>16-11</v>
       </c>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
@@ -6832,7 +6839,7 @@
         <v>97</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J90" s="8"/>
       <c r="K90" s="7"/>
@@ -6844,11 +6851,11 @@
         <v>16</v>
       </c>
       <c r="B91">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C91" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-13</v>
+        <v>16-12</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -6860,23 +6867,23 @@
         <v>97</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J91" s="8"/>
       <c r="K91" s="7"/>
       <c r="L91" s="8"/>
       <c r="M91" s="6"/>
     </row>
-    <row r="92" spans="1:13" ht="60">
+    <row r="92" spans="1:13" ht="45">
       <c r="A92">
         <v>16</v>
       </c>
       <c r="B92">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C92" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-14</v>
+        <v>16-13</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -6888,23 +6895,23 @@
         <v>97</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J92" s="8"/>
       <c r="K92" s="7"/>
       <c r="L92" s="8"/>
       <c r="M92" s="6"/>
     </row>
-    <row r="93" spans="1:13" ht="15">
+    <row r="93" spans="1:13" ht="60">
       <c r="A93">
         <v>16</v>
       </c>
       <c r="B93">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C93" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-15</v>
+        <v>16-14</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
@@ -6916,7 +6923,7 @@
         <v>97</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J93" s="8"/>
       <c r="K93" s="7"/>
@@ -6928,11 +6935,11 @@
         <v>16</v>
       </c>
       <c r="B94">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C94" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-16</v>
+        <v>16-15</v>
       </c>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
@@ -6944,38 +6951,38 @@
         <v>97</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J94" s="8"/>
       <c r="K94" s="7"/>
       <c r="L94" s="8"/>
       <c r="M94" s="6"/>
     </row>
-    <row r="95" spans="1:13" ht="30">
+    <row r="95" spans="1:13" ht="15">
       <c r="A95">
         <v>16</v>
       </c>
       <c r="B95">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C95" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-18</v>
-      </c>
-      <c r="D95" s="9"/>
-      <c r="E95" s="9"/>
-      <c r="F95" s="9"/>
-      <c r="G95" s="9" t="s">
+        <v>16-16</v>
+      </c>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="7"/>
+      <c r="G95" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H95" s="9" t="s">
+      <c r="H95" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="I95" s="8" t="s">
-        <v>318</v>
+      <c r="I95" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="J95" s="8"/>
-      <c r="K95" s="9"/>
+      <c r="K95" s="7"/>
       <c r="L95" s="8"/>
       <c r="M95" s="6"/>
     </row>
@@ -6984,11 +6991,11 @@
         <v>16</v>
       </c>
       <c r="B96">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C96" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-19</v>
+        <v>16-18</v>
       </c>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
@@ -7000,7 +7007,7 @@
         <v>97</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="J96" s="8"/>
       <c r="K96" s="9"/>
@@ -7012,26 +7019,26 @@
         <v>16</v>
       </c>
       <c r="B97">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C97" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-21</v>
-      </c>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="7"/>
-      <c r="G97" s="7" t="s">
+        <v>16-19</v>
+      </c>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H97" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>179</v>
+      <c r="H97" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I97" s="8" t="s">
+        <v>312</v>
       </c>
       <c r="J97" s="8"/>
-      <c r="K97" s="7"/>
+      <c r="K97" s="9"/>
       <c r="L97" s="8"/>
       <c r="M97" s="6"/>
     </row>
@@ -7040,11 +7047,11 @@
         <v>16</v>
       </c>
       <c r="B98">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C98" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-22</v>
+        <v>16-21</v>
       </c>
       <c r="D98" s="5"/>
       <c r="E98" s="5"/>
@@ -7056,23 +7063,23 @@
         <v>178</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J98" s="8"/>
       <c r="K98" s="7"/>
       <c r="L98" s="8"/>
       <c r="M98" s="6"/>
     </row>
-    <row r="99" spans="1:13" ht="15">
+    <row r="99" spans="1:13" ht="30">
       <c r="A99">
         <v>16</v>
       </c>
       <c r="B99">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C99" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-23</v>
+        <v>16-22</v>
       </c>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
@@ -7084,7 +7091,7 @@
         <v>178</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J99" s="8"/>
       <c r="K99" s="7"/>
@@ -7096,11 +7103,11 @@
         <v>16</v>
       </c>
       <c r="B100">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C100" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>16-24</v>
+        <v>16-23</v>
       </c>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
@@ -7112,135 +7119,135 @@
         <v>178</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J100" s="8"/>
       <c r="K100" s="7"/>
       <c r="L100" s="8"/>
       <c r="M100" s="6"/>
     </row>
-    <row r="101" spans="1:13" ht="60">
+    <row r="101" spans="1:13" ht="15">
       <c r="A101">
         <v>16</v>
       </c>
       <c r="B101">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C101" s="3" t="str">
-        <f t="shared" ref="C101:C120" si="3">CONCATENATE(A101,"-",B101)</f>
-        <v>16-25</v>
-      </c>
-      <c r="D101" s="9"/>
-      <c r="E101" s="9"/>
-      <c r="F101" s="9"/>
-      <c r="G101" s="9" t="s">
+        <f t="shared" si="2"/>
+        <v>16-24</v>
+      </c>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H101" s="9" t="s">
+      <c r="H101" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="I101" s="8" t="s">
-        <v>291</v>
+      <c r="I101" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="J101" s="8"/>
-      <c r="K101" s="9"/>
+      <c r="K101" s="7"/>
       <c r="L101" s="8"/>
       <c r="M101" s="6"/>
     </row>
-    <row r="102" spans="1:13" ht="30">
+    <row r="102" spans="1:13" ht="60">
       <c r="A102">
+        <v>16</v>
+      </c>
+      <c r="B102">
+        <v>25</v>
+      </c>
+      <c r="C102" s="3" t="str">
+        <f t="shared" ref="C102:C123" si="3">CONCATENATE(A102,"-",B102)</f>
+        <v>16-25</v>
+      </c>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H102" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="I102" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="J102" s="8"/>
+      <c r="K102" s="9"/>
+      <c r="L102" s="8"/>
+      <c r="M102" s="6"/>
+    </row>
+    <row r="103" spans="1:13" ht="60">
+      <c r="A103">
+        <v>16</v>
+      </c>
+      <c r="B103">
+        <v>26</v>
+      </c>
+      <c r="C103" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>16-26</v>
+      </c>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H103" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I103" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="J103" s="8"/>
+      <c r="K103" s="9"/>
+      <c r="L103" s="8"/>
+      <c r="M103" s="6"/>
+    </row>
+    <row r="104" spans="1:13" ht="60">
+      <c r="A104">
+        <v>16</v>
+      </c>
+      <c r="B104">
+        <v>27</v>
+      </c>
+      <c r="C104" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>16-27</v>
+      </c>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H104" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I104" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="J104" s="8"/>
+      <c r="K104" s="9"/>
+      <c r="L104" s="8"/>
+      <c r="M104" s="6"/>
+    </row>
+    <row r="105" spans="1:13" ht="30">
+      <c r="A105">
         <v>17</v>
       </c>
-      <c r="B102">
+      <c r="B105">
         <v>2</v>
       </c>
-      <c r="C102" s="3" t="str">
+      <c r="C105" s="3" t="str">
         <f t="shared" si="3"/>
         <v>17-2</v>
-      </c>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="7"/>
-      <c r="G102" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H102" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="I102" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="J102" s="8"/>
-      <c r="K102" s="7"/>
-      <c r="L102" s="1"/>
-      <c r="M102" s="6"/>
-    </row>
-    <row r="103" spans="1:13" ht="15">
-      <c r="A103">
-        <v>17</v>
-      </c>
-      <c r="B103">
-        <v>4</v>
-      </c>
-      <c r="C103" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>17-4</v>
-      </c>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="7"/>
-      <c r="G103" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H103" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="I103" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="J103" s="8"/>
-      <c r="K103" s="7"/>
-      <c r="L103" s="8"/>
-      <c r="M103" s="6"/>
-    </row>
-    <row r="104" spans="1:13" ht="30">
-      <c r="A104">
-        <v>19</v>
-      </c>
-      <c r="B104">
-        <v>1</v>
-      </c>
-      <c r="C104" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>19-1</v>
-      </c>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="7"/>
-      <c r="G104" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H104" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="I104" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="J104" s="8"/>
-      <c r="K104" s="7"/>
-      <c r="L104" s="8"/>
-      <c r="M104" s="6"/>
-    </row>
-    <row r="105" spans="1:13" ht="30">
-      <c r="A105">
-        <v>19</v>
-      </c>
-      <c r="B105">
-        <v>2</v>
-      </c>
-      <c r="C105" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>19-2</v>
       </c>
       <c r="D105" s="5"/>
       <c r="E105" s="5"/>
@@ -7249,25 +7256,26 @@
         <v>62</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="J105" s="8"/>
       <c r="K105" s="7"/>
-      <c r="L105" s="81"/>
-    </row>
-    <row r="106" spans="1:13" ht="30">
+      <c r="L105" s="1"/>
+      <c r="M105" s="6"/>
+    </row>
+    <row r="106" spans="1:13" ht="15">
       <c r="A106">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B106">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C106" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>19-3</v>
+        <v>17-4</v>
       </c>
       <c r="D106" s="5"/>
       <c r="E106" s="5"/>
@@ -7276,26 +7284,26 @@
         <v>62</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="J106" s="8"/>
       <c r="K106" s="7"/>
-      <c r="L106" s="82"/>
+      <c r="L106" s="8"/>
       <c r="M106" s="6"/>
     </row>
-    <row r="107" spans="1:13" ht="45">
+    <row r="107" spans="1:13" ht="30">
       <c r="A107">
         <v>19</v>
       </c>
       <c r="B107">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C107" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>19-4</v>
+        <v>19-1</v>
       </c>
       <c r="D107" s="5"/>
       <c r="E107" s="5"/>
@@ -7307,11 +7315,11 @@
         <v>192</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J107" s="8"/>
       <c r="K107" s="7"/>
-      <c r="L107" s="82"/>
+      <c r="L107" s="8"/>
       <c r="M107" s="6"/>
     </row>
     <row r="108" spans="1:13" ht="30">
@@ -7319,11 +7327,11 @@
         <v>19</v>
       </c>
       <c r="B108">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C108" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>19-5</v>
+        <v>19-2</v>
       </c>
       <c r="D108" s="5"/>
       <c r="E108" s="5"/>
@@ -7335,107 +7343,106 @@
         <v>192</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J108" s="8"/>
       <c r="K108" s="7"/>
-      <c r="L108" s="83"/>
-      <c r="M108" s="6"/>
-    </row>
-    <row r="109" spans="1:13" ht="26.25">
+      <c r="L108" s="91"/>
+    </row>
+    <row r="109" spans="1:13" ht="30">
       <c r="A109">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C109" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-2</v>
-      </c>
-      <c r="D109" s="15"/>
-      <c r="E109" s="15"/>
-      <c r="F109" s="15"/>
-      <c r="G109" s="10" t="s">
+        <v>19-3</v>
+      </c>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H109" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I109" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="J109" s="12"/>
-      <c r="K109" s="10"/>
-      <c r="L109" s="12"/>
+      <c r="H109" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J109" s="8"/>
+      <c r="K109" s="7"/>
+      <c r="L109" s="92"/>
       <c r="M109" s="6"/>
     </row>
-    <row r="110" spans="1:13" ht="39">
+    <row r="110" spans="1:13" ht="45">
       <c r="A110">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C110" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-3</v>
-      </c>
-      <c r="D110" s="15"/>
-      <c r="E110" s="15"/>
-      <c r="F110" s="15"/>
-      <c r="G110" s="10" t="s">
+        <v>19-4</v>
+      </c>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="7"/>
+      <c r="G110" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H110" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I110" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="J110" s="12"/>
-      <c r="K110" s="10"/>
-      <c r="L110" s="11"/>
+      <c r="H110" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="J110" s="8"/>
+      <c r="K110" s="7"/>
+      <c r="L110" s="92"/>
       <c r="M110" s="6"/>
     </row>
-    <row r="111" spans="1:13" ht="39">
+    <row r="111" spans="1:13" ht="30">
       <c r="A111">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B111">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C111" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-4</v>
-      </c>
-      <c r="D111" s="15"/>
-      <c r="E111" s="15"/>
-      <c r="F111" s="15"/>
-      <c r="G111" s="10" t="s">
+        <v>19-5</v>
+      </c>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="7"/>
+      <c r="G111" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H111" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I111" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="J111" s="12"/>
-      <c r="K111" s="10"/>
-      <c r="L111" s="12"/>
+      <c r="H111" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J111" s="8"/>
+      <c r="K111" s="7"/>
+      <c r="L111" s="93"/>
       <c r="M111" s="6"/>
     </row>
-    <row r="112" spans="1:13" ht="51.75">
+    <row r="112" spans="1:13" ht="26.25">
       <c r="A112">
         <v>21</v>
       </c>
       <c r="B112">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C112" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-5</v>
+        <v>21-2</v>
       </c>
       <c r="D112" s="15"/>
       <c r="E112" s="15"/>
@@ -7446,242 +7453,242 @@
       <c r="H112" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I112" s="12" t="s">
-        <v>204</v>
+      <c r="I112" s="11" t="s">
+        <v>201</v>
       </c>
       <c r="J112" s="12"/>
       <c r="K112" s="10"/>
       <c r="L112" s="12"/>
       <c r="M112" s="6"/>
     </row>
-    <row r="113" spans="1:13" ht="26.25">
+    <row r="113" spans="1:13" ht="39">
       <c r="A113">
         <v>21</v>
       </c>
       <c r="B113">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C113" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-6</v>
-      </c>
-      <c r="D113" s="18"/>
-      <c r="E113" s="18"/>
-      <c r="F113" s="18"/>
-      <c r="G113" s="19"/>
-      <c r="H113" s="19" t="s">
+        <v>21-3</v>
+      </c>
+      <c r="D113" s="15"/>
+      <c r="E113" s="15"/>
+      <c r="F113" s="15"/>
+      <c r="G113" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H113" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I113" s="79" t="s">
-        <v>359</v>
-      </c>
-      <c r="J113" s="79"/>
-      <c r="K113" s="19"/>
-      <c r="L113" s="79"/>
+      <c r="I113" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="J113" s="12"/>
+      <c r="K113" s="10"/>
+      <c r="L113" s="11"/>
       <c r="M113" s="6"/>
     </row>
-    <row r="114" spans="1:13" ht="26.25">
+    <row r="114" spans="1:13" ht="39">
       <c r="A114">
         <v>21</v>
       </c>
       <c r="B114">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C114" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-7</v>
-      </c>
-      <c r="D114" s="18"/>
-      <c r="E114" s="18"/>
-      <c r="F114" s="18"/>
-      <c r="G114" s="19"/>
-      <c r="H114" s="19" t="s">
+        <v>21-4</v>
+      </c>
+      <c r="D114" s="15"/>
+      <c r="E114" s="15"/>
+      <c r="F114" s="15"/>
+      <c r="G114" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H114" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I114" s="79" t="s">
-        <v>360</v>
-      </c>
-      <c r="J114" s="79"/>
-      <c r="K114" s="19"/>
-      <c r="L114" s="79"/>
+      <c r="I114" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="J114" s="12"/>
+      <c r="K114" s="10"/>
+      <c r="L114" s="12"/>
       <c r="M114" s="6"/>
     </row>
-    <row r="115" spans="1:13" ht="26.25">
+    <row r="115" spans="1:13" ht="51.75">
       <c r="A115">
         <v>21</v>
       </c>
       <c r="B115">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C115" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-8</v>
-      </c>
-      <c r="D115" s="18"/>
-      <c r="E115" s="18"/>
-      <c r="F115" s="18"/>
-      <c r="G115" s="19"/>
-      <c r="H115" s="19" t="s">
+        <v>21-5</v>
+      </c>
+      <c r="D115" s="15"/>
+      <c r="E115" s="15"/>
+      <c r="F115" s="15"/>
+      <c r="G115" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H115" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I115" s="78" t="s">
-        <v>358</v>
-      </c>
-      <c r="J115" s="78"/>
-      <c r="K115" s="19"/>
-      <c r="L115" s="78"/>
+      <c r="I115" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="J115" s="12"/>
+      <c r="K115" s="10"/>
+      <c r="L115" s="12"/>
       <c r="M115" s="6"/>
     </row>
-    <row r="116" spans="1:13" ht="39">
+    <row r="116" spans="1:13" ht="26.25">
       <c r="A116">
         <v>21</v>
       </c>
       <c r="B116">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C116" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-26</v>
+        <v>21-6</v>
       </c>
       <c r="D116" s="18"/>
       <c r="E116" s="18"/>
       <c r="F116" s="18"/>
-      <c r="G116" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="G116" s="19"/>
       <c r="H116" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I116" s="42" t="s">
-        <v>295</v>
-      </c>
-      <c r="J116" s="42"/>
+      <c r="I116" s="79" t="s">
+        <v>359</v>
+      </c>
+      <c r="J116" s="79"/>
       <c r="K116" s="19"/>
-      <c r="L116" s="42"/>
+      <c r="L116" s="79"/>
       <c r="M116" s="6"/>
     </row>
-    <row r="117" spans="1:13" ht="39">
+    <row r="117" spans="1:13" ht="26.25">
       <c r="A117">
         <v>21</v>
       </c>
       <c r="B117">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C117" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>21-27</v>
+        <v>21-7</v>
       </c>
       <c r="D117" s="18"/>
       <c r="E117" s="18"/>
       <c r="F117" s="18"/>
-      <c r="G117" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="G117" s="19"/>
       <c r="H117" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I117" s="42" t="s">
-        <v>296</v>
-      </c>
-      <c r="J117" s="42"/>
+      <c r="I117" s="79" t="s">
+        <v>360</v>
+      </c>
+      <c r="J117" s="79"/>
       <c r="K117" s="19"/>
-      <c r="L117" s="42"/>
+      <c r="L117" s="79"/>
       <c r="M117" s="6"/>
     </row>
-    <row r="118" spans="1:13" ht="39">
+    <row r="118" spans="1:13" ht="26.25">
       <c r="A118">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B118">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C118" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>22-2</v>
-      </c>
-      <c r="D118" s="20"/>
-      <c r="E118" s="20"/>
-      <c r="F118" s="20"/>
-      <c r="G118" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H118" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="I118" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="J118" s="20"/>
+        <v>21-8</v>
+      </c>
+      <c r="D118" s="18"/>
+      <c r="E118" s="18"/>
+      <c r="F118" s="18"/>
+      <c r="G118" s="19"/>
+      <c r="H118" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I118" s="78" t="s">
+        <v>358</v>
+      </c>
+      <c r="J118" s="78"/>
       <c r="K118" s="19"/>
-      <c r="L118" s="23"/>
+      <c r="L118" s="78"/>
       <c r="M118" s="6"/>
     </row>
-    <row r="119" spans="1:13" ht="26.25">
+    <row r="119" spans="1:13" ht="39">
       <c r="A119">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B119">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C119" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>22-3</v>
-      </c>
-      <c r="D119" s="20"/>
-      <c r="E119" s="20"/>
-      <c r="F119" s="20"/>
-      <c r="G119" s="20" t="s">
+        <v>21-26</v>
+      </c>
+      <c r="D119" s="18"/>
+      <c r="E119" s="18"/>
+      <c r="F119" s="18"/>
+      <c r="G119" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H119" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="I119" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="J119" s="20"/>
+      <c r="H119" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I119" s="42" t="s">
+        <v>295</v>
+      </c>
+      <c r="J119" s="42"/>
       <c r="K119" s="19"/>
-      <c r="L119" s="23"/>
+      <c r="L119" s="42"/>
       <c r="M119" s="6"/>
     </row>
     <row r="120" spans="1:13" ht="39">
       <c r="A120">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C120" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>26-1</v>
-      </c>
-      <c r="D120" s="20"/>
-      <c r="E120" s="20"/>
-      <c r="F120" s="20"/>
-      <c r="G120" s="20" t="s">
+        <v>21-27</v>
+      </c>
+      <c r="D120" s="18"/>
+      <c r="E120" s="18"/>
+      <c r="F120" s="18"/>
+      <c r="G120" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H120" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="I120" s="22" t="s">
-        <v>293</v>
-      </c>
-      <c r="J120" s="20"/>
+      <c r="H120" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I120" s="42" t="s">
+        <v>296</v>
+      </c>
+      <c r="J120" s="42"/>
       <c r="K120" s="19"/>
-      <c r="L120" s="23"/>
+      <c r="L120" s="42"/>
       <c r="M120" s="6"/>
     </row>
     <row r="121" spans="1:13" ht="39">
       <c r="A121">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C121" s="3" t="str">
-        <f t="shared" ref="C121:C122" si="4">CONCATENATE(A121,"-",B121)</f>
-        <v>26-1</v>
+        <f t="shared" si="3"/>
+        <v>22-2</v>
       </c>
       <c r="D121" s="20"/>
       <c r="E121" s="20"/>
@@ -7690,115 +7697,110 @@
         <v>62</v>
       </c>
       <c r="H121" s="21" t="s">
-        <v>292</v>
+        <v>247</v>
       </c>
       <c r="I121" s="22" t="s">
-        <v>293</v>
+        <v>248</v>
       </c>
       <c r="J121" s="20"/>
       <c r="K121" s="19"/>
       <c r="L121" s="23"/>
       <c r="M121" s="6"/>
     </row>
-    <row r="122" spans="1:13" ht="64.5">
+    <row r="122" spans="1:13" ht="26.25">
       <c r="A122">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B122">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C122" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>27-1</v>
+        <f t="shared" si="3"/>
+        <v>22-3</v>
       </c>
       <c r="D122" s="20"/>
       <c r="E122" s="20"/>
-      <c r="F122" s="77" t="s">
-        <v>240</v>
-      </c>
+      <c r="F122" s="20"/>
       <c r="G122" s="20" t="s">
         <v>62</v>
       </c>
       <c r="H122" s="21" t="s">
-        <v>354</v>
+        <v>247</v>
       </c>
       <c r="I122" s="22" t="s">
-        <v>356</v>
+        <v>249</v>
       </c>
       <c r="J122" s="20"/>
       <c r="K122" s="19"/>
       <c r="L122" s="23"/>
       <c r="M122" s="6"/>
     </row>
-    <row r="123" spans="1:13" ht="15.75" customHeight="1">
+    <row r="123" spans="1:13" ht="39">
       <c r="A123">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C123" s="3" t="str">
-        <f t="shared" ref="C123" si="5">CONCATENATE(A123,"-",B123)</f>
-        <v>27-2</v>
+        <f t="shared" si="3"/>
+        <v>26-1</v>
       </c>
       <c r="D123" s="20"/>
       <c r="E123" s="20"/>
-      <c r="F123" s="77" t="s">
-        <v>240</v>
-      </c>
+      <c r="F123" s="20"/>
       <c r="G123" s="20" t="s">
         <v>62</v>
       </c>
       <c r="H123" s="21" t="s">
-        <v>354</v>
+        <v>292</v>
       </c>
       <c r="I123" s="22" t="s">
-        <v>355</v>
+        <v>293</v>
       </c>
       <c r="J123" s="20"/>
       <c r="K123" s="19"/>
       <c r="L123" s="23"/>
-    </row>
-    <row r="124" spans="1:13" ht="77.25">
+      <c r="M123" s="6"/>
+    </row>
+    <row r="124" spans="1:13" ht="39">
       <c r="A124">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C124" s="3" t="str">
-        <f>CONCATENATE(A124,"-",B124)</f>
-        <v>27-3</v>
+        <f t="shared" ref="C124:C125" si="4">CONCATENATE(A124,"-",B124)</f>
+        <v>26-1</v>
       </c>
       <c r="D124" s="20"/>
       <c r="E124" s="20"/>
-      <c r="F124" s="77" t="s">
-        <v>240</v>
-      </c>
+      <c r="F124" s="20"/>
       <c r="G124" s="20" t="s">
         <v>62</v>
       </c>
       <c r="H124" s="21" t="s">
-        <v>354</v>
+        <v>292</v>
       </c>
       <c r="I124" s="22" t="s">
-        <v>357</v>
+        <v>293</v>
       </c>
       <c r="J124" s="20"/>
       <c r="K124" s="19"/>
       <c r="L124" s="23"/>
       <c r="M124" s="6"/>
     </row>
-    <row r="125" spans="1:13" ht="15">
+    <row r="125" spans="1:13" ht="64.5">
       <c r="A125">
         <v>27</v>
       </c>
       <c r="B125">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C125" s="3" t="str">
-        <f>CONCATENATE(A125,"-",B125)</f>
-        <v>27-4</v>
+        <f t="shared" si="4"/>
+        <v>27-1</v>
       </c>
       <c r="D125" s="20"/>
       <c r="E125" s="20"/>
@@ -7812,23 +7814,23 @@
         <v>354</v>
       </c>
       <c r="I125" s="22" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="J125" s="20"/>
       <c r="K125" s="19"/>
       <c r="L125" s="23"/>
       <c r="M125" s="6"/>
     </row>
-    <row r="126" spans="1:13" ht="51.75">
+    <row r="126" spans="1:13" ht="15.75" customHeight="1">
       <c r="A126">
         <v>27</v>
       </c>
       <c r="B126">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C126" s="3" t="str">
-        <f>CONCATENATE(A126,"-",B126)</f>
-        <v>27-5</v>
+        <f t="shared" ref="C126" si="5">CONCATENATE(A126,"-",B126)</f>
+        <v>27-2</v>
       </c>
       <c r="D126" s="20"/>
       <c r="E126" s="20"/>
@@ -7836,142 +7838,219 @@
         <v>240</v>
       </c>
       <c r="G126" s="20" t="s">
-        <v>240</v>
+        <v>62</v>
       </c>
       <c r="H126" s="21" t="s">
         <v>354</v>
       </c>
       <c r="I126" s="22" t="s">
-        <v>363</v>
-      </c>
-      <c r="J126" s="43" t="s">
-        <v>364</v>
-      </c>
+        <v>355</v>
+      </c>
+      <c r="J126" s="20"/>
       <c r="K126" s="19"/>
       <c r="L126" s="23"/>
-      <c r="M126" s="6"/>
-    </row>
-    <row r="127" spans="1:13" ht="26.25">
+    </row>
+    <row r="127" spans="1:13" ht="77.25">
       <c r="A127">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B127">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C127" s="3" t="str">
         <f>CONCATENATE(A127,"-",B127)</f>
-        <v>28-1</v>
+        <v>27-3</v>
       </c>
       <c r="D127" s="20"/>
       <c r="E127" s="20"/>
-      <c r="F127" s="92" t="s">
+      <c r="F127" s="77" t="s">
         <v>240</v>
       </c>
-      <c r="G127" s="90" t="s">
+      <c r="G127" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="H127" s="88" t="s">
-        <v>376</v>
+      <c r="H127" s="21" t="s">
+        <v>354</v>
       </c>
       <c r="I127" s="22" t="s">
-        <v>372</v>
-      </c>
-      <c r="J127" s="43" t="s">
-        <v>373</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="J127" s="20"/>
       <c r="K127" s="19"/>
-      <c r="L127" s="86" t="s">
-        <v>371</v>
-      </c>
+      <c r="L127" s="23"/>
       <c r="M127" s="6"/>
     </row>
-    <row r="128" spans="1:13" ht="26.25">
+    <row r="128" spans="1:13" ht="15">
       <c r="A128">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B128">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C128" s="3" t="str">
         <f>CONCATENATE(A128,"-",B128)</f>
-        <v>28-2</v>
+        <v>27-4</v>
       </c>
       <c r="D128" s="20"/>
       <c r="E128" s="20"/>
-      <c r="F128" s="93"/>
-      <c r="G128" s="91"/>
-      <c r="H128" s="89"/>
+      <c r="F128" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G128" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H128" s="21" t="s">
+        <v>354</v>
+      </c>
       <c r="I128" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="J128" s="20"/>
+      <c r="K128" s="19"/>
+      <c r="L128" s="23"/>
+      <c r="M128" s="6"/>
+    </row>
+    <row r="129" spans="1:13" ht="51.75">
+      <c r="A129">
+        <v>27</v>
+      </c>
+      <c r="B129">
+        <v>5</v>
+      </c>
+      <c r="C129" s="3" t="str">
+        <f>CONCATENATE(A129,"-",B129)</f>
+        <v>27-5</v>
+      </c>
+      <c r="D129" s="20"/>
+      <c r="E129" s="20"/>
+      <c r="F129" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="G129" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="H129" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="I129" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="J129" s="43" t="s">
+        <v>364</v>
+      </c>
+      <c r="K129" s="19"/>
+      <c r="L129" s="23"/>
+      <c r="M129" s="6"/>
+    </row>
+    <row r="130" spans="1:13" ht="26.25">
+      <c r="A130">
+        <v>28</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130" s="3" t="str">
+        <f>CONCATENATE(A130,"-",B130)</f>
+        <v>28-1</v>
+      </c>
+      <c r="D130" s="20"/>
+      <c r="E130" s="20"/>
+      <c r="F130" s="87" t="s">
+        <v>240</v>
+      </c>
+      <c r="G130" s="85" t="s">
+        <v>62</v>
+      </c>
+      <c r="H130" s="83" t="s">
+        <v>376</v>
+      </c>
+      <c r="I130" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="J130" s="43" t="s">
+        <v>373</v>
+      </c>
+      <c r="K130" s="19"/>
+      <c r="L130" s="81" t="s">
+        <v>371</v>
+      </c>
+      <c r="M130" s="6"/>
+    </row>
+    <row r="131" spans="1:13" ht="26.25">
+      <c r="A131">
+        <v>28</v>
+      </c>
+      <c r="B131">
+        <v>2</v>
+      </c>
+      <c r="C131" s="3" t="str">
+        <f>CONCATENATE(A131,"-",B131)</f>
+        <v>28-2</v>
+      </c>
+      <c r="D131" s="20"/>
+      <c r="E131" s="20"/>
+      <c r="F131" s="88"/>
+      <c r="G131" s="86"/>
+      <c r="H131" s="84"/>
+      <c r="I131" s="22" t="s">
         <v>374</v>
       </c>
-      <c r="J128" s="43" t="s">
+      <c r="J131" s="43" t="s">
         <v>375</v>
       </c>
-      <c r="K128" s="19"/>
-      <c r="L128" s="87"/>
-      <c r="M128" s="6"/>
-    </row>
-    <row r="129" spans="12:13" ht="12.75">
-      <c r="L129" s="6"/>
-      <c r="M129" s="6"/>
-    </row>
-    <row r="130" spans="12:13" ht="12.75">
-      <c r="L130" s="6"/>
-      <c r="M130" s="6"/>
-    </row>
-    <row r="131" spans="12:13" ht="12.75">
-      <c r="L131" s="6"/>
+      <c r="K131" s="19"/>
+      <c r="L131" s="82"/>
       <c r="M131" s="6"/>
     </row>
-    <row r="132" spans="12:13" ht="12.75">
+    <row r="132" spans="1:13" ht="12.75">
       <c r="L132" s="6"/>
       <c r="M132" s="6"/>
     </row>
-    <row r="133" spans="12:13" ht="12.75">
+    <row r="133" spans="1:13" ht="12.75">
       <c r="L133" s="6"/>
       <c r="M133" s="6"/>
     </row>
-    <row r="134" spans="12:13" ht="12.75">
+    <row r="134" spans="1:13" ht="12.75">
       <c r="L134" s="6"/>
       <c r="M134" s="6"/>
     </row>
-    <row r="135" spans="12:13" ht="12.75">
+    <row r="135" spans="1:13" ht="12.75">
       <c r="L135" s="6"/>
       <c r="M135" s="6"/>
     </row>
-    <row r="136" spans="12:13" ht="12.75">
+    <row r="136" spans="1:13" ht="12.75">
       <c r="L136" s="6"/>
       <c r="M136" s="6"/>
     </row>
-    <row r="137" spans="12:13" ht="12.75">
+    <row r="137" spans="1:13" ht="12.75">
       <c r="L137" s="6"/>
       <c r="M137" s="6"/>
     </row>
-    <row r="138" spans="12:13" ht="12.75">
+    <row r="138" spans="1:13" ht="12.75">
       <c r="L138" s="6"/>
       <c r="M138" s="6"/>
     </row>
-    <row r="139" spans="12:13" ht="12.75">
+    <row r="139" spans="1:13" ht="12.75">
       <c r="L139" s="6"/>
       <c r="M139" s="6"/>
     </row>
-    <row r="140" spans="12:13" ht="12.75">
+    <row r="140" spans="1:13" ht="12.75">
       <c r="L140" s="6"/>
       <c r="M140" s="6"/>
     </row>
-    <row r="141" spans="12:13" ht="12.75">
+    <row r="141" spans="1:13" ht="12.75">
       <c r="L141" s="6"/>
       <c r="M141" s="6"/>
     </row>
-    <row r="142" spans="12:13" ht="12.75">
+    <row r="142" spans="1:13" ht="12.75">
       <c r="L142" s="6"/>
       <c r="M142" s="6"/>
     </row>
-    <row r="143" spans="12:13" ht="12.75">
+    <row r="143" spans="1:13" ht="12.75">
       <c r="L143" s="6"/>
       <c r="M143" s="6"/>
     </row>
-    <row r="144" spans="12:13" ht="12.75">
+    <row r="144" spans="1:13" ht="12.75">
       <c r="L144" s="6"/>
       <c r="M144" s="6"/>
     </row>
@@ -10623,29 +10702,41 @@
       <c r="L806" s="6"/>
       <c r="M806" s="6"/>
     </row>
+    <row r="807" spans="12:13" ht="12.75">
+      <c r="L807" s="6"/>
+      <c r="M807" s="6"/>
+    </row>
+    <row r="808" spans="12:13" ht="12.75">
+      <c r="L808" s="6"/>
+      <c r="M808" s="6"/>
+    </row>
+    <row r="809" spans="12:13" ht="12.75">
+      <c r="L809" s="6"/>
+      <c r="M809" s="6"/>
+    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" scale="115">
+    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" scale="115">
-      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
+    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" scale="115">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -10655,127 +10746,142 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>
-    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}" scale="115">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
+    <customSheetView guid="{A261AA16-395A-4133-AC57-0EAB9A6305EB}">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
     </customSheetView>
-    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+    <customSheetView guid="{CEDC8F8C-0552-41C2-BFFD-AE6167E9BA48}">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
     </customSheetView>
-    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+    <customSheetView guid="{684D6F67-3A9F-42B8-B57C-B09D2BC01A42}" scale="115">
+      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
     </customSheetView>
-    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}" scale="115">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="6">
-    <mergeCell ref="L127:L128"/>
-    <mergeCell ref="H127:H128"/>
-    <mergeCell ref="G127:G128"/>
-    <mergeCell ref="F127:F128"/>
+    <mergeCell ref="L130:L131"/>
+    <mergeCell ref="H130:H131"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="F130:F131"/>
     <mergeCell ref="L9:L13"/>
-    <mergeCell ref="L105:L108"/>
+    <mergeCell ref="L108:L111"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:K32 K34:K122 K124">
-    <cfRule type="containsBlanks" dxfId="23" priority="115">
+  <conditionalFormatting sqref="K2:K32 K34:K86 K127 K88:K125">
+    <cfRule type="containsBlanks" dxfId="20" priority="118">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K32 K34:K122 K124">
-    <cfRule type="containsText" dxfId="22" priority="116" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K2:K32 K34:K86 K127 K88:K125">
+    <cfRule type="containsText" dxfId="19" priority="119" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K32 K34:K122 K124">
-    <cfRule type="containsText" dxfId="21" priority="117" operator="containsText" text="fail">
+  <conditionalFormatting sqref="K2:K32 K34:K86 K127 K88:K125">
+    <cfRule type="containsText" dxfId="18" priority="120" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33">
-    <cfRule type="containsBlanks" dxfId="20" priority="19">
+    <cfRule type="containsBlanks" dxfId="17" priority="22">
       <formula>LEN(TRIM(K33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K33))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33">
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="15" priority="24" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K33))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K123">
-    <cfRule type="containsBlanks" dxfId="17" priority="16">
-      <formula>LEN(TRIM(K123))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K123">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K123))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K123">
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K123))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K125">
-    <cfRule type="containsBlanks" dxfId="14" priority="13">
-      <formula>LEN(TRIM(K125))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K125">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K125))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K125">
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K125))))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K126">
-    <cfRule type="containsBlanks" dxfId="11" priority="10">
+    <cfRule type="containsBlanks" dxfId="14" priority="19">
       <formula>LEN(TRIM(K126))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K126">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="13" priority="20" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH(("pass"),(K126))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K126">
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="12" priority="21" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH(("fail"),(K126))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K127:K128">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
-      <formula>LEN(TRIM(K127))=0</formula>
+  <conditionalFormatting sqref="K128">
+    <cfRule type="containsBlanks" dxfId="11" priority="16">
+      <formula>LEN(TRIM(K128))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K127:K128">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH(("pass"),(K127))))</formula>
+  <conditionalFormatting sqref="K128">
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K128))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K127:K128">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH(("fail"),(K127))))</formula>
+  <conditionalFormatting sqref="K128">
+    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K128))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K129">
+    <cfRule type="containsBlanks" dxfId="8" priority="13">
+      <formula>LEN(TRIM(K129))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K129">
+    <cfRule type="containsText" dxfId="7" priority="14" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K129))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K129">
+    <cfRule type="containsText" dxfId="6" priority="15" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K129))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K130:K131">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
+      <formula>LEN(TRIM(K130))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K130:K131">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K130))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K130:K131">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K130))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K87">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(K87))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K87">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH(("pass"),(K87))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K87">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH(("fail"),(K87))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12137,7 +12243,37 @@
     <row r="45" spans="1:28" ht="38.25" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{85F3695B-032A-4A88-B2A8-7589EA4BF272}">
+    <customSheetView guid="{0E9ACB5E-D990-4F66-9FAE-4A09EE1669DA}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{FF7CD254-0CE8-4FC9-AF55-6D042EF01199}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{8BFFCA10-A97E-43DB-A10A-DB0A21E06383}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{2FD27013-34EA-408F-80D9-9AE4DD52D5A3}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" f